<commit_message>
Update threading: threading is working this version
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="31">
   <si>
     <t>1.Average (mA)</t>
   </si>
@@ -32,13 +32,82 @@
     <t>5.Count</t>
   </si>
   <si>
-    <t>Deep Sleep</t>
-  </si>
-  <si>
-    <t>BT Idle</t>
-  </si>
-  <si>
-    <t>BT Pscan</t>
+    <t>deep_sleep</t>
+  </si>
+  <si>
+    <t>bt_idle</t>
+  </si>
+  <si>
+    <t>bt_pscan</t>
+  </si>
+  <si>
+    <t>bt_iscan</t>
+  </si>
+  <si>
+    <t>bt_piscan</t>
+  </si>
+  <si>
+    <t>bt_acl_sniff_1dot28s_master_0dbm</t>
+  </si>
+  <si>
+    <t>bt_acl_sniff_1dot28s_master_4dbm</t>
+  </si>
+  <si>
+    <t>bt_acl_sniff_1dot28s_master_12dot5dbm</t>
+  </si>
+  <si>
+    <t>bt_acl_sniff_dot5s_master_0dbm</t>
+  </si>
+  <si>
+    <t>bt_acl_sniff_dot5s_master_4dbm</t>
+  </si>
+  <si>
+    <t>bt_acl_sniff_dot5s_master_12dot5dbm</t>
+  </si>
+  <si>
+    <t>bt_sco_hv3_master_0dbm</t>
+  </si>
+  <si>
+    <t>bt_sco_hv3_master_4dbm</t>
+  </si>
+  <si>
+    <t>bt_sco_hv3_master_12dot5dbm</t>
+  </si>
+  <si>
+    <t>bt_sco_ev3_master_0dbm</t>
+  </si>
+  <si>
+    <t>bt_sco_ev3_master_4dbm</t>
+  </si>
+  <si>
+    <t>bt_sco_ev3_master_12dot5dbm</t>
+  </si>
+  <si>
+    <t>BLE_Adv_1dot28s_3Channel_0dbm</t>
+  </si>
+  <si>
+    <t>BLE_Adv_1dot28s_3Channel_4dbm</t>
+  </si>
+  <si>
+    <t>BLE_Adv_1dot28s_3Channel_12dot5dbm</t>
+  </si>
+  <si>
+    <t>BLE_scan_1dot28s</t>
+  </si>
+  <si>
+    <t>BLE_scan_1s</t>
+  </si>
+  <si>
+    <t>BLE_scan_10ms</t>
+  </si>
+  <si>
+    <t>BLE_Conn_1dot28s_0dbm</t>
+  </si>
+  <si>
+    <t>BLE_Conn_1dot28s_4dbm</t>
+  </si>
+  <si>
+    <t>BLE_Conn_1dot28s_12dot5dbm</t>
   </si>
 </sst>
 </file>
@@ -396,7 +465,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -424,19 +493,19 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>-0.2374</v>
+        <v>-0.0072</v>
       </c>
       <c r="C2">
-        <v>-0.2244</v>
+        <v>-0.0072</v>
       </c>
       <c r="D2">
-        <v>-0.2455</v>
+        <v>-0.0072</v>
       </c>
       <c r="E2">
-        <v>0.004</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -444,19 +513,19 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>5.4964</v>
+        <v>0.0026</v>
       </c>
       <c r="C3">
-        <v>5.5087</v>
+        <v>0.0026</v>
       </c>
       <c r="D3">
-        <v>5.4834</v>
+        <v>0.0026</v>
       </c>
       <c r="E3">
-        <v>0.0052</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -464,19 +533,479 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>0.3033</v>
+        <v>0.0018</v>
       </c>
       <c r="C4">
-        <v>6.8126</v>
+        <v>0.0018</v>
       </c>
       <c r="D4">
-        <v>0.0679</v>
+        <v>0.0018</v>
       </c>
       <c r="E4">
-        <v>1.0382</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>100</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>0.0016</v>
+      </c>
+      <c r="C5">
+        <v>0.0016</v>
+      </c>
+      <c r="D5">
+        <v>0.0016</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>0.0024</v>
+      </c>
+      <c r="C6">
+        <v>0.0024</v>
+      </c>
+      <c r="D6">
+        <v>0.0024</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>0.0004</v>
+      </c>
+      <c r="C7">
+        <v>0.0004</v>
+      </c>
+      <c r="D7">
+        <v>0.0004</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>0.0002</v>
+      </c>
+      <c r="C8">
+        <v>0.0002</v>
+      </c>
+      <c r="D8">
+        <v>0.0002</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>-0.0032</v>
+      </c>
+      <c r="C9">
+        <v>-0.0032</v>
+      </c>
+      <c r="D9">
+        <v>-0.0032</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>-0.0029</v>
+      </c>
+      <c r="C10">
+        <v>-0.0029</v>
+      </c>
+      <c r="D10">
+        <v>-0.0029</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>-0.0034</v>
+      </c>
+      <c r="C11">
+        <v>-0.0034</v>
+      </c>
+      <c r="D11">
+        <v>-0.0034</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>0.0038</v>
+      </c>
+      <c r="C12">
+        <v>0.0038</v>
+      </c>
+      <c r="D12">
+        <v>0.0038</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13">
+        <v>0.0045</v>
+      </c>
+      <c r="C13">
+        <v>0.0045</v>
+      </c>
+      <c r="D13">
+        <v>0.0045</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14">
+        <v>0.0065</v>
+      </c>
+      <c r="C14">
+        <v>0.0065</v>
+      </c>
+      <c r="D14">
+        <v>0.0065</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15">
+        <v>-0.003</v>
+      </c>
+      <c r="C15">
+        <v>-0.003</v>
+      </c>
+      <c r="D15">
+        <v>-0.003</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16">
+        <v>0.0011</v>
+      </c>
+      <c r="C16">
+        <v>0.0011</v>
+      </c>
+      <c r="D16">
+        <v>0.0011</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17">
+        <v>-0.0002</v>
+      </c>
+      <c r="C17">
+        <v>-0.0002</v>
+      </c>
+      <c r="D17">
+        <v>-0.0002</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18">
+        <v>-0.0093</v>
+      </c>
+      <c r="C18">
+        <v>-0.0093</v>
+      </c>
+      <c r="D18">
+        <v>-0.0093</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19">
+        <v>0.0024</v>
+      </c>
+      <c r="C19">
+        <v>0.0024</v>
+      </c>
+      <c r="D19">
+        <v>0.0024</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20">
+        <v>0.0046</v>
+      </c>
+      <c r="C20">
+        <v>0.0046</v>
+      </c>
+      <c r="D20">
+        <v>0.0046</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21">
+        <v>-0.0066</v>
+      </c>
+      <c r="C21">
+        <v>-0.0066</v>
+      </c>
+      <c r="D21">
+        <v>-0.0066</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22">
+        <v>-0.0014</v>
+      </c>
+      <c r="C22">
+        <v>-0.0014</v>
+      </c>
+      <c r="D22">
+        <v>-0.0014</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23">
+        <v>0.0042</v>
+      </c>
+      <c r="C23">
+        <v>0.0042</v>
+      </c>
+      <c r="D23">
+        <v>0.0042</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24">
+        <v>-0.0037</v>
+      </c>
+      <c r="C24">
+        <v>-0.0037</v>
+      </c>
+      <c r="D24">
+        <v>-0.0037</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25">
+        <v>-0.0012</v>
+      </c>
+      <c r="C25">
+        <v>-0.0012</v>
+      </c>
+      <c r="D25">
+        <v>-0.0012</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26">
+        <v>0.0059</v>
+      </c>
+      <c r="C26">
+        <v>0.0059</v>
+      </c>
+      <c r="D26">
+        <v>0.0059</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27">
+        <v>0.0012</v>
+      </c>
+      <c r="C27">
+        <v>0.0012</v>
+      </c>
+      <c r="D27">
+        <v>0.0012</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -486,7 +1015,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -514,19 +1043,19 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>0.1019</v>
+        <v>0.0054</v>
       </c>
       <c r="C2">
-        <v>0.1393</v>
+        <v>0.0054</v>
       </c>
       <c r="D2">
-        <v>0.079</v>
+        <v>0.0054</v>
       </c>
       <c r="E2">
-        <v>0.018</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -534,19 +1063,19 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>-8.341</v>
+        <v>0.0007</v>
       </c>
       <c r="C3">
-        <v>-8.3186</v>
+        <v>0.0007</v>
       </c>
       <c r="D3">
-        <v>-8.3595</v>
+        <v>0.0007</v>
       </c>
       <c r="E3">
-        <v>0.0102</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -554,19 +1083,479 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>-0.3887</v>
+        <v>0.0001</v>
       </c>
       <c r="C4">
-        <v>-0.2289</v>
+        <v>0.0001</v>
       </c>
       <c r="D4">
-        <v>-4.7185</v>
+        <v>0.0001</v>
       </c>
       <c r="E4">
-        <v>0.7386</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>100</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>0.0007</v>
+      </c>
+      <c r="C5">
+        <v>0.0007</v>
+      </c>
+      <c r="D5">
+        <v>0.0007</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>0.0026</v>
+      </c>
+      <c r="C6">
+        <v>0.0026</v>
+      </c>
+      <c r="D6">
+        <v>0.0026</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>-0.006</v>
+      </c>
+      <c r="C7">
+        <v>-0.006</v>
+      </c>
+      <c r="D7">
+        <v>-0.006</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>0.0032</v>
+      </c>
+      <c r="C8">
+        <v>0.0032</v>
+      </c>
+      <c r="D8">
+        <v>0.0032</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>0.0046</v>
+      </c>
+      <c r="C9">
+        <v>0.0046</v>
+      </c>
+      <c r="D9">
+        <v>0.0046</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>0.0049</v>
+      </c>
+      <c r="C10">
+        <v>0.0049</v>
+      </c>
+      <c r="D10">
+        <v>0.0049</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>-0.0018</v>
+      </c>
+      <c r="C11">
+        <v>-0.0018</v>
+      </c>
+      <c r="D11">
+        <v>-0.0018</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>0.0087</v>
+      </c>
+      <c r="C12">
+        <v>0.0087</v>
+      </c>
+      <c r="D12">
+        <v>0.0087</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13">
+        <v>0.0071</v>
+      </c>
+      <c r="C13">
+        <v>0.0071</v>
+      </c>
+      <c r="D13">
+        <v>0.0071</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14">
+        <v>0.0065</v>
+      </c>
+      <c r="C14">
+        <v>0.0065</v>
+      </c>
+      <c r="D14">
+        <v>0.0065</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15">
+        <v>0.0001</v>
+      </c>
+      <c r="C15">
+        <v>0.0001</v>
+      </c>
+      <c r="D15">
+        <v>0.0001</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16">
+        <v>-0.0085</v>
+      </c>
+      <c r="C16">
+        <v>-0.0085</v>
+      </c>
+      <c r="D16">
+        <v>-0.0085</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17">
+        <v>-0.0071</v>
+      </c>
+      <c r="C17">
+        <v>-0.0071</v>
+      </c>
+      <c r="D17">
+        <v>-0.0071</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18">
+        <v>0.0046</v>
+      </c>
+      <c r="C18">
+        <v>0.0046</v>
+      </c>
+      <c r="D18">
+        <v>0.0046</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19">
+        <v>0.0018</v>
+      </c>
+      <c r="C19">
+        <v>0.0018</v>
+      </c>
+      <c r="D19">
+        <v>0.0018</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20">
+        <v>0.0024</v>
+      </c>
+      <c r="C20">
+        <v>0.0024</v>
+      </c>
+      <c r="D20">
+        <v>0.0024</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21">
+        <v>0.0029</v>
+      </c>
+      <c r="C21">
+        <v>0.0029</v>
+      </c>
+      <c r="D21">
+        <v>0.0029</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22">
+        <v>0.001</v>
+      </c>
+      <c r="C22">
+        <v>0.001</v>
+      </c>
+      <c r="D22">
+        <v>0.001</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23">
+        <v>0.0004</v>
+      </c>
+      <c r="C23">
+        <v>0.0004</v>
+      </c>
+      <c r="D23">
+        <v>0.0004</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24">
+        <v>0.0054</v>
+      </c>
+      <c r="C24">
+        <v>0.0054</v>
+      </c>
+      <c r="D24">
+        <v>0.0054</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25">
+        <v>0.0032</v>
+      </c>
+      <c r="C25">
+        <v>0.0032</v>
+      </c>
+      <c r="D25">
+        <v>0.0032</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26">
+        <v>-0.0043</v>
+      </c>
+      <c r="C26">
+        <v>-0.0043</v>
+      </c>
+      <c r="D26">
+        <v>-0.0043</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27">
+        <v>-0.0004</v>
+      </c>
+      <c r="C27">
+        <v>-0.0004</v>
+      </c>
+      <c r="D27">
+        <v>-0.0004</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix threading issue, functional version
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="30">
   <si>
     <t>1.Average (mA)</t>
   </si>
@@ -32,82 +32,79 @@
     <t>5.Count</t>
   </si>
   <si>
-    <t>deep_sleep</t>
-  </si>
-  <si>
-    <t>bt_idle</t>
-  </si>
-  <si>
-    <t>bt_pscan</t>
-  </si>
-  <si>
-    <t>bt_iscan</t>
-  </si>
-  <si>
-    <t>bt_piscan</t>
-  </si>
-  <si>
-    <t>bt_acl_sniff_1dot28s_master_0dbm</t>
-  </si>
-  <si>
-    <t>bt_acl_sniff_1dot28s_master_4dbm</t>
-  </si>
-  <si>
-    <t>bt_acl_sniff_1dot28s_master_12dot5dbm</t>
-  </si>
-  <si>
-    <t>bt_acl_sniff_dot5s_master_0dbm</t>
-  </si>
-  <si>
-    <t>bt_acl_sniff_dot5s_master_4dbm</t>
-  </si>
-  <si>
-    <t>bt_acl_sniff_dot5s_master_12dot5dbm</t>
-  </si>
-  <si>
-    <t>bt_sco_hv3_master_0dbm</t>
-  </si>
-  <si>
-    <t>bt_sco_hv3_master_4dbm</t>
-  </si>
-  <si>
-    <t>bt_sco_hv3_master_12dot5dbm</t>
-  </si>
-  <si>
-    <t>bt_sco_ev3_master_0dbm</t>
-  </si>
-  <si>
-    <t>bt_sco_ev3_master_4dbm</t>
-  </si>
-  <si>
-    <t>bt_sco_ev3_master_12dot5dbm</t>
-  </si>
-  <si>
-    <t>BLE_Adv_1dot28s_3Channel_0dbm</t>
-  </si>
-  <si>
-    <t>BLE_Adv_1dot28s_3Channel_4dbm</t>
-  </si>
-  <si>
-    <t>BLE_Adv_1dot28s_3Channel_12dot5dbm</t>
-  </si>
-  <si>
-    <t>BLE_scan_1dot28s</t>
-  </si>
-  <si>
-    <t>BLE_scan_1s</t>
-  </si>
-  <si>
-    <t>BLE_scan_10ms</t>
-  </si>
-  <si>
-    <t>BLE_Conn_1dot28s_0dbm</t>
-  </si>
-  <si>
-    <t>BLE_Conn_1dot28s_4dbm</t>
-  </si>
-  <si>
-    <t>BLE_Conn_1dot28s_12dot5dbm</t>
+    <t>Deep_Sleep</t>
+  </si>
+  <si>
+    <t>BT_Idle</t>
+  </si>
+  <si>
+    <t>BT_Pscan</t>
+  </si>
+  <si>
+    <t>bt_Iscan</t>
+  </si>
+  <si>
+    <t>bt_PIscan</t>
+  </si>
+  <si>
+    <t>BT_ACL_Sniff_1dot28s_Master_0dBm</t>
+  </si>
+  <si>
+    <t>BT_ACL_Sniff_1dot28s_Master_4dBm</t>
+  </si>
+  <si>
+    <t>BT_ACL_Sniff_1dot28s_Master_12dot5dBm</t>
+  </si>
+  <si>
+    <t>BT_ACL_Sniff_0dot5s_Master_0dBm</t>
+  </si>
+  <si>
+    <t>BT_ACL_Sniff_0dot5s_Master_4dBm</t>
+  </si>
+  <si>
+    <t>BT_SCO_HV3_Master_0dBm</t>
+  </si>
+  <si>
+    <t>BT_SCO_HV3_Master_4dBm</t>
+  </si>
+  <si>
+    <t>BT_SCO_HV3_Master_12dot5dBm</t>
+  </si>
+  <si>
+    <t>BT_SCO_EV3_Master_0dBm</t>
+  </si>
+  <si>
+    <t>BT_SCO_EV3_Master_4dBm</t>
+  </si>
+  <si>
+    <t>BT_SCO_EV3_Master_12dot5dBm</t>
+  </si>
+  <si>
+    <t>BLE_Adv_1dot28s_3Channel_0dBm</t>
+  </si>
+  <si>
+    <t>BLE_Adv_1dot28s_3Channel_4dBm</t>
+  </si>
+  <si>
+    <t>BLE_Adv_1dot28s_3Channel_12dot5dBm</t>
+  </si>
+  <si>
+    <t>BLE_Scan_1dot28s</t>
+  </si>
+  <si>
+    <t>BLE_Scan_1s</t>
+  </si>
+  <si>
+    <t>BLE_Scan_10ms</t>
+  </si>
+  <si>
+    <t>BLE_Conn_1dot28s_0dBm</t>
+  </si>
+  <si>
+    <t>BLE_Conn_1dot28s_4dBm</t>
+  </si>
+  <si>
+    <t>BLE_Conn_1dot28s_12dot5dBm</t>
   </si>
 </sst>
 </file>
@@ -465,7 +462,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -493,19 +490,19 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>-0.0072</v>
+        <v>0.0994</v>
       </c>
       <c r="C2">
-        <v>-0.0072</v>
+        <v>0.1334</v>
       </c>
       <c r="D2">
-        <v>-0.0072</v>
+        <v>0.075</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>0.0179</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -513,19 +510,19 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>0.0026</v>
+        <v>5.4892</v>
       </c>
       <c r="C3">
-        <v>0.0026</v>
+        <v>5.4989</v>
       </c>
       <c r="D3">
-        <v>0.0026</v>
+        <v>5.4768</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>0.0045</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -533,19 +530,19 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>0.0018</v>
+        <v>0.1454</v>
       </c>
       <c r="C4">
-        <v>0.0018</v>
+        <v>1.3266</v>
       </c>
       <c r="D4">
-        <v>0.0018</v>
+        <v>0.0623</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>0.2012</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -553,19 +550,19 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>0.0016</v>
+        <v>0.4484</v>
       </c>
       <c r="C5">
-        <v>0.0016</v>
+        <v>11.0226</v>
       </c>
       <c r="D5">
-        <v>0.0016</v>
+        <v>0.0793</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1.8486</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -573,19 +570,19 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>0.0024</v>
+        <v>0.564</v>
       </c>
       <c r="C6">
-        <v>0.0024</v>
+        <v>14.8009</v>
       </c>
       <c r="D6">
-        <v>0.0024</v>
+        <v>0.0753</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>2.5077</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -593,19 +590,19 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>0.0004</v>
+        <v>0.2675</v>
       </c>
       <c r="C7">
-        <v>0.0004</v>
+        <v>3.546</v>
       </c>
       <c r="D7">
-        <v>0.0004</v>
+        <v>0.0709</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>0.6367</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -613,19 +610,19 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>0.0002</v>
+        <v>0.442</v>
       </c>
       <c r="C8">
-        <v>0.0002</v>
+        <v>4.5064</v>
       </c>
       <c r="D8">
-        <v>0.0002</v>
+        <v>0.0786</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>1.0099</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -633,19 +630,19 @@
         <v>12</v>
       </c>
       <c r="B9">
-        <v>-0.0032</v>
+        <v>0.3904</v>
       </c>
       <c r="C9">
-        <v>-0.0032</v>
+        <v>5.9808</v>
       </c>
       <c r="D9">
-        <v>-0.0032</v>
+        <v>0.0772</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>1.1282</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -653,19 +650,19 @@
         <v>13</v>
       </c>
       <c r="B10">
-        <v>-0.0029</v>
+        <v>0.4586</v>
       </c>
       <c r="C10">
-        <v>-0.0029</v>
+        <v>6.1246</v>
       </c>
       <c r="D10">
-        <v>-0.0029</v>
+        <v>0.0636</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>1.1492</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -673,19 +670,19 @@
         <v>14</v>
       </c>
       <c r="B11">
-        <v>-0.0034</v>
+        <v>0.3735</v>
       </c>
       <c r="C11">
-        <v>-0.0034</v>
+        <v>6.0667</v>
       </c>
       <c r="D11">
-        <v>-0.0034</v>
+        <v>0.0708</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>1.0571</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -693,19 +690,19 @@
         <v>15</v>
       </c>
       <c r="B12">
-        <v>0.0038</v>
+        <v>8.1549</v>
       </c>
       <c r="C12">
-        <v>0.0038</v>
+        <v>9.4889</v>
       </c>
       <c r="D12">
-        <v>0.0038</v>
+        <v>7.8679</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>0.2858</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -713,19 +710,19 @@
         <v>16</v>
       </c>
       <c r="B13">
-        <v>0.0045</v>
+        <v>8.5943</v>
       </c>
       <c r="C13">
-        <v>0.0045</v>
+        <v>9.8775</v>
       </c>
       <c r="D13">
-        <v>0.0045</v>
+        <v>8.1714</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>0.3251</v>
       </c>
       <c r="F13">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -733,19 +730,19 @@
         <v>17</v>
       </c>
       <c r="B14">
-        <v>0.0065</v>
+        <v>13.2779</v>
       </c>
       <c r="C14">
-        <v>0.0065</v>
+        <v>14.9539</v>
       </c>
       <c r="D14">
-        <v>0.0065</v>
+        <v>12.0784</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>0.8209</v>
       </c>
       <c r="F14">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -753,19 +750,19 @@
         <v>18</v>
       </c>
       <c r="B15">
-        <v>-0.003</v>
+        <v>8.131</v>
       </c>
       <c r="C15">
-        <v>-0.003</v>
+        <v>9.3553</v>
       </c>
       <c r="D15">
-        <v>-0.003</v>
+        <v>7.8354</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>0.2682</v>
       </c>
       <c r="F15">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -773,19 +770,19 @@
         <v>19</v>
       </c>
       <c r="B16">
-        <v>0.0011</v>
+        <v>8.6443</v>
       </c>
       <c r="C16">
-        <v>0.0011</v>
+        <v>9.4952</v>
       </c>
       <c r="D16">
-        <v>0.0011</v>
+        <v>8.1934</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>0.3136</v>
       </c>
       <c r="F16">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -793,19 +790,19 @@
         <v>20</v>
       </c>
       <c r="B17">
-        <v>-0.0002</v>
+        <v>13.4639</v>
       </c>
       <c r="C17">
-        <v>-0.0002</v>
+        <v>15.4356</v>
       </c>
       <c r="D17">
-        <v>-0.0002</v>
+        <v>12.3822</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>0.7764</v>
       </c>
       <c r="F17">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -813,19 +810,19 @@
         <v>21</v>
       </c>
       <c r="B18">
-        <v>-0.0093</v>
+        <v>0.1119</v>
       </c>
       <c r="C18">
-        <v>-0.0093</v>
+        <v>1.2701</v>
       </c>
       <c r="D18">
-        <v>-0.0093</v>
+        <v>0.0779</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>0.1177</v>
       </c>
       <c r="F18">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -833,19 +830,19 @@
         <v>22</v>
       </c>
       <c r="B19">
-        <v>0.0024</v>
+        <v>0.1006</v>
       </c>
       <c r="C19">
-        <v>0.0024</v>
+        <v>0.1796</v>
       </c>
       <c r="D19">
-        <v>0.0024</v>
+        <v>0.0765</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>0.0183</v>
       </c>
       <c r="F19">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -853,19 +850,19 @@
         <v>23</v>
       </c>
       <c r="B20">
-        <v>0.0046</v>
+        <v>0.2259</v>
       </c>
       <c r="C20">
-        <v>0.0046</v>
+        <v>6.5985</v>
       </c>
       <c r="D20">
-        <v>0.0046</v>
+        <v>0.0765</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>0.8808</v>
       </c>
       <c r="F20">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -873,19 +870,19 @@
         <v>24</v>
       </c>
       <c r="B21">
-        <v>-0.0066</v>
+        <v>0.3211</v>
       </c>
       <c r="C21">
-        <v>-0.0066</v>
+        <v>11.2443</v>
       </c>
       <c r="D21">
-        <v>-0.0066</v>
+        <v>0.0798</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>1.5545</v>
       </c>
       <c r="F21">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -893,19 +890,19 @@
         <v>25</v>
       </c>
       <c r="B22">
-        <v>-0.0014</v>
+        <v>0.2528</v>
       </c>
       <c r="C22">
-        <v>-0.0014</v>
+        <v>11.2629</v>
       </c>
       <c r="D22">
-        <v>-0.0014</v>
+        <v>0.0786</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>1.1493</v>
       </c>
       <c r="F22">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -913,19 +910,19 @@
         <v>26</v>
       </c>
       <c r="B23">
-        <v>0.0042</v>
+        <v>9.5751</v>
       </c>
       <c r="C23">
-        <v>0.0042</v>
+        <v>14.1172</v>
       </c>
       <c r="D23">
-        <v>0.0042</v>
+        <v>2.2144</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>3.0326</v>
       </c>
       <c r="F23">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -933,19 +930,19 @@
         <v>27</v>
       </c>
       <c r="B24">
-        <v>-0.0037</v>
+        <v>0.2144</v>
       </c>
       <c r="C24">
-        <v>-0.0037</v>
+        <v>3.2109</v>
       </c>
       <c r="D24">
-        <v>-0.0037</v>
+        <v>0.056</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>0.5131</v>
       </c>
       <c r="F24">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -953,19 +950,19 @@
         <v>28</v>
       </c>
       <c r="B25">
-        <v>-0.0012</v>
+        <v>0.1844</v>
       </c>
       <c r="C25">
-        <v>-0.0012</v>
+        <v>2.7666</v>
       </c>
       <c r="D25">
-        <v>-0.0012</v>
+        <v>0.0806</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>0.4136</v>
       </c>
       <c r="F25">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -973,39 +970,19 @@
         <v>29</v>
       </c>
       <c r="B26">
-        <v>0.0059</v>
+        <v>0.1867</v>
       </c>
       <c r="C26">
-        <v>0.0059</v>
+        <v>2.8814</v>
       </c>
       <c r="D26">
-        <v>0.0059</v>
+        <v>0.0608</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>0.4286</v>
       </c>
       <c r="F26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B27">
-        <v>0.0012</v>
-      </c>
-      <c r="C27">
-        <v>0.0012</v>
-      </c>
-      <c r="D27">
-        <v>0.0012</v>
-      </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-      <c r="F27">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1015,7 +992,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1043,19 +1020,19 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>0.0054</v>
+        <v>0.2344</v>
       </c>
       <c r="C2">
-        <v>0.0054</v>
+        <v>0.2444</v>
       </c>
       <c r="D2">
-        <v>0.0054</v>
+        <v>0.2211</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>0.004</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1063,19 +1040,19 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>0.0007</v>
+        <v>8.328</v>
       </c>
       <c r="C3">
-        <v>0.0007</v>
+        <v>8.3428</v>
       </c>
       <c r="D3">
-        <v>0.0007</v>
+        <v>8.3072</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>0.0096</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1083,19 +1060,19 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>0.0001</v>
+        <v>0.3182</v>
       </c>
       <c r="C4">
-        <v>0.0001</v>
+        <v>3.2812</v>
       </c>
       <c r="D4">
-        <v>0.0001</v>
+        <v>0.2235</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>0.4204</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1103,19 +1080,19 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>0.0007</v>
+        <v>0.469</v>
       </c>
       <c r="C5">
-        <v>0.0007</v>
+        <v>6.1327</v>
       </c>
       <c r="D5">
-        <v>0.0007</v>
+        <v>0.22</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1.0239</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1123,19 +1100,19 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>0.0026</v>
+        <v>0.5286</v>
       </c>
       <c r="C6">
-        <v>0.0026</v>
+        <v>8.2569</v>
       </c>
       <c r="D6">
-        <v>0.0026</v>
+        <v>0.2238</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>1.4053</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1143,19 +1120,19 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>-0.006</v>
+        <v>0.6602</v>
       </c>
       <c r="C7">
-        <v>-0.006</v>
+        <v>8.1711</v>
       </c>
       <c r="D7">
-        <v>-0.006</v>
+        <v>0.2224</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>1.4835</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1163,19 +1140,19 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>0.0032</v>
+        <v>0.562</v>
       </c>
       <c r="C8">
-        <v>0.0032</v>
+        <v>9.7773</v>
       </c>
       <c r="D8">
-        <v>0.0032</v>
+        <v>0.2233</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>1.5503</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1183,19 +1160,19 @@
         <v>12</v>
       </c>
       <c r="B9">
-        <v>0.0046</v>
+        <v>0.3384</v>
       </c>
       <c r="C9">
-        <v>0.0046</v>
+        <v>4.0969</v>
       </c>
       <c r="D9">
-        <v>0.0046</v>
+        <v>0.2244</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>0.4439</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1203,19 +1180,19 @@
         <v>13</v>
       </c>
       <c r="B10">
-        <v>0.0049</v>
+        <v>0.5448</v>
       </c>
       <c r="C10">
-        <v>0.0049</v>
+        <v>7.8059</v>
       </c>
       <c r="D10">
-        <v>0.0049</v>
+        <v>0.2233</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>1.2319</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1223,19 +1200,19 @@
         <v>14</v>
       </c>
       <c r="B11">
-        <v>-0.0018</v>
+        <v>0.5593</v>
       </c>
       <c r="C11">
-        <v>-0.0018</v>
+        <v>7.7425</v>
       </c>
       <c r="D11">
-        <v>-0.0018</v>
+        <v>0.2208</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>1.2682</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1243,19 +1220,19 @@
         <v>15</v>
       </c>
       <c r="B12">
-        <v>0.0087</v>
+        <v>11.3549</v>
       </c>
       <c r="C12">
-        <v>0.0087</v>
+        <v>12.1485</v>
       </c>
       <c r="D12">
-        <v>0.0087</v>
+        <v>10.9978</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>0.2769</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1263,19 +1240,19 @@
         <v>16</v>
       </c>
       <c r="B13">
-        <v>0.0071</v>
+        <v>12.3031</v>
       </c>
       <c r="C13">
-        <v>0.0071</v>
+        <v>13.2164</v>
       </c>
       <c r="D13">
-        <v>0.0071</v>
+        <v>11.8003</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>0.342</v>
       </c>
       <c r="F13">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1283,19 +1260,19 @@
         <v>17</v>
       </c>
       <c r="B14">
-        <v>0.0065</v>
+        <v>9.7492</v>
       </c>
       <c r="C14">
-        <v>0.0065</v>
+        <v>10.2441</v>
       </c>
       <c r="D14">
-        <v>0.0065</v>
+        <v>9.6097</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>0.0886</v>
       </c>
       <c r="F14">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1303,19 +1280,19 @@
         <v>18</v>
       </c>
       <c r="B15">
-        <v>0.0001</v>
+        <v>11.4917</v>
       </c>
       <c r="C15">
-        <v>0.0001</v>
+        <v>12.3767</v>
       </c>
       <c r="D15">
-        <v>0.0001</v>
+        <v>11.0183</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>0.2732</v>
       </c>
       <c r="F15">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1323,19 +1300,19 @@
         <v>19</v>
       </c>
       <c r="B16">
-        <v>-0.0085</v>
+        <v>12.2369</v>
       </c>
       <c r="C16">
-        <v>-0.0085</v>
+        <v>13.0403</v>
       </c>
       <c r="D16">
-        <v>-0.0085</v>
+        <v>11.7453</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>0.3438</v>
       </c>
       <c r="F16">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1343,19 +1320,19 @@
         <v>20</v>
       </c>
       <c r="B17">
-        <v>-0.0071</v>
+        <v>9.7411</v>
       </c>
       <c r="C17">
-        <v>-0.0071</v>
+        <v>10.2708</v>
       </c>
       <c r="D17">
-        <v>-0.0071</v>
+        <v>9.5933</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>0.1114</v>
       </c>
       <c r="F17">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1363,19 +1340,19 @@
         <v>21</v>
       </c>
       <c r="B18">
-        <v>0.0046</v>
+        <v>0.307</v>
       </c>
       <c r="C18">
-        <v>0.0046</v>
+        <v>3.9448</v>
       </c>
       <c r="D18">
-        <v>0.0046</v>
+        <v>0.2244</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>0.5197</v>
       </c>
       <c r="F18">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1383,19 +1360,19 @@
         <v>22</v>
       </c>
       <c r="B19">
-        <v>0.0018</v>
+        <v>0.2754</v>
       </c>
       <c r="C19">
-        <v>0.0018</v>
+        <v>4.3856</v>
       </c>
       <c r="D19">
-        <v>0.0018</v>
+        <v>0.2172</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>0.414</v>
       </c>
       <c r="F19">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1403,19 +1380,19 @@
         <v>23</v>
       </c>
       <c r="B20">
-        <v>0.0024</v>
+        <v>0.2323</v>
       </c>
       <c r="C20">
-        <v>0.0024</v>
+        <v>0.3128</v>
       </c>
       <c r="D20">
-        <v>0.0024</v>
+        <v>0.218</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>0.0089</v>
       </c>
       <c r="F20">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1423,19 +1400,19 @@
         <v>24</v>
       </c>
       <c r="B21">
-        <v>0.0029</v>
+        <v>0.2546</v>
       </c>
       <c r="C21">
-        <v>0.0029</v>
+        <v>1.7978</v>
       </c>
       <c r="D21">
-        <v>0.0029</v>
+        <v>0.2183</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>0.176</v>
       </c>
       <c r="F21">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1443,19 +1420,19 @@
         <v>25</v>
       </c>
       <c r="B22">
-        <v>0.001</v>
+        <v>0.3905</v>
       </c>
       <c r="C22">
-        <v>0.001</v>
+        <v>9.3187</v>
       </c>
       <c r="D22">
-        <v>0.001</v>
+        <v>0.2214</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>1.0629</v>
       </c>
       <c r="F22">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1463,19 +1440,19 @@
         <v>26</v>
       </c>
       <c r="B23">
-        <v>0.0004</v>
+        <v>8.0462</v>
       </c>
       <c r="C23">
-        <v>0.0004</v>
+        <v>12.7251</v>
       </c>
       <c r="D23">
-        <v>0.0004</v>
+        <v>0.8369</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>2.8992</v>
       </c>
       <c r="F23">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1483,19 +1460,19 @@
         <v>27</v>
       </c>
       <c r="B24">
-        <v>0.0054</v>
+        <v>0.2832</v>
       </c>
       <c r="C24">
-        <v>0.0054</v>
+        <v>2.7502</v>
       </c>
       <c r="D24">
-        <v>0.0054</v>
+        <v>0.2202</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>0.3437</v>
       </c>
       <c r="F24">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1503,19 +1480,19 @@
         <v>28</v>
       </c>
       <c r="B25">
-        <v>0.0032</v>
+        <v>0.2906</v>
       </c>
       <c r="C25">
-        <v>0.0032</v>
+        <v>3.2073</v>
       </c>
       <c r="D25">
-        <v>0.0032</v>
+        <v>0.2205</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>0.4142</v>
       </c>
       <c r="F25">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1523,39 +1500,19 @@
         <v>29</v>
       </c>
       <c r="B26">
-        <v>-0.0043</v>
+        <v>0.2806</v>
       </c>
       <c r="C26">
-        <v>-0.0043</v>
+        <v>3.0164</v>
       </c>
       <c r="D26">
-        <v>-0.0043</v>
+        <v>0.2169</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>0.3526</v>
       </c>
       <c r="F26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B27">
-        <v>-0.0004</v>
-      </c>
-      <c r="C27">
-        <v>-0.0004</v>
-      </c>
-      <c r="D27">
-        <v>-0.0004</v>
-      </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-      <c r="F27">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Threading tested as Pass - Add ToDo.md
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -9,13 +9,14 @@
   <sheets>
     <sheet name="3_3" sheetId="1" r:id="rId1"/>
     <sheet name="1_8" sheetId="2" r:id="rId2"/>
+    <sheet name="1_1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="30">
   <si>
     <t>1.Average (mA)</t>
   </si>
@@ -490,19 +491,19 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>0.0994</v>
+        <v>0.2318</v>
       </c>
       <c r="C2">
-        <v>0.1334</v>
+        <v>0.2494</v>
       </c>
       <c r="D2">
-        <v>0.075</v>
+        <v>0.2177</v>
       </c>
       <c r="E2">
-        <v>0.0179</v>
+        <v>0.004</v>
       </c>
       <c r="F2">
-        <v>100</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -510,19 +511,19 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>5.4892</v>
+        <v>8.3145</v>
       </c>
       <c r="C3">
-        <v>5.4989</v>
+        <v>8.3389</v>
       </c>
       <c r="D3">
-        <v>5.4768</v>
+        <v>8.283</v>
       </c>
       <c r="E3">
-        <v>0.0045</v>
+        <v>0.01</v>
       </c>
       <c r="F3">
-        <v>100</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -530,19 +531,19 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>0.1454</v>
+        <v>0.3197</v>
       </c>
       <c r="C4">
-        <v>1.3266</v>
+        <v>6.7671</v>
       </c>
       <c r="D4">
-        <v>0.0623</v>
+        <v>0.2188</v>
       </c>
       <c r="E4">
-        <v>0.2012</v>
+        <v>0.6325</v>
       </c>
       <c r="F4">
-        <v>100</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -550,19 +551,19 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>0.4484</v>
+        <v>0.3252</v>
       </c>
       <c r="C5">
-        <v>11.0226</v>
+        <v>6.7785</v>
       </c>
       <c r="D5">
-        <v>0.0793</v>
+        <v>0.2172</v>
       </c>
       <c r="E5">
-        <v>1.8486</v>
+        <v>0.6503</v>
       </c>
       <c r="F5">
-        <v>100</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -570,19 +571,19 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>0.564</v>
+        <v>0.392</v>
       </c>
       <c r="C6">
-        <v>14.8009</v>
+        <v>8.549</v>
       </c>
       <c r="D6">
-        <v>0.0753</v>
+        <v>0.2169</v>
       </c>
       <c r="E6">
-        <v>2.5077</v>
+        <v>0.9844</v>
       </c>
       <c r="F6">
-        <v>100</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -590,19 +591,19 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>0.2675</v>
+        <v>0.4555</v>
       </c>
       <c r="C7">
-        <v>3.546</v>
+        <v>9.1831</v>
       </c>
       <c r="D7">
-        <v>0.0709</v>
+        <v>0.2138</v>
       </c>
       <c r="E7">
-        <v>0.6367</v>
+        <v>0.9902</v>
       </c>
       <c r="F7">
-        <v>100</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -610,19 +611,19 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>0.442</v>
+        <v>0.4585</v>
       </c>
       <c r="C8">
-        <v>4.5064</v>
+        <v>9.3812</v>
       </c>
       <c r="D8">
-        <v>0.0786</v>
+        <v>0.2149</v>
       </c>
       <c r="E8">
-        <v>1.0099</v>
+        <v>1.0022</v>
       </c>
       <c r="F8">
-        <v>100</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -630,19 +631,19 @@
         <v>12</v>
       </c>
       <c r="B9">
-        <v>0.3904</v>
+        <v>0.453</v>
       </c>
       <c r="C9">
-        <v>5.9808</v>
+        <v>9.07</v>
       </c>
       <c r="D9">
-        <v>0.0772</v>
+        <v>0.2163</v>
       </c>
       <c r="E9">
-        <v>1.1282</v>
+        <v>0.9718</v>
       </c>
       <c r="F9">
-        <v>100</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -650,19 +651,19 @@
         <v>13</v>
       </c>
       <c r="B10">
-        <v>0.4586</v>
+        <v>0.6158</v>
       </c>
       <c r="C10">
-        <v>6.1246</v>
+        <v>9.3599</v>
       </c>
       <c r="D10">
-        <v>0.0636</v>
+        <v>0.2138</v>
       </c>
       <c r="E10">
-        <v>1.1492</v>
+        <v>1.3238</v>
       </c>
       <c r="F10">
-        <v>100</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -670,19 +671,19 @@
         <v>14</v>
       </c>
       <c r="B11">
-        <v>0.3735</v>
+        <v>0.6173</v>
       </c>
       <c r="C11">
-        <v>6.0667</v>
+        <v>9.2673</v>
       </c>
       <c r="D11">
-        <v>0.0708</v>
+        <v>0.213</v>
       </c>
       <c r="E11">
-        <v>1.0571</v>
+        <v>1.3362</v>
       </c>
       <c r="F11">
-        <v>100</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -690,19 +691,19 @@
         <v>15</v>
       </c>
       <c r="B12">
-        <v>8.1549</v>
+        <v>11.3096</v>
       </c>
       <c r="C12">
-        <v>9.4889</v>
+        <v>12.8049</v>
       </c>
       <c r="D12">
-        <v>7.8679</v>
+        <v>10.8796</v>
       </c>
       <c r="E12">
-        <v>0.2858</v>
+        <v>0.262</v>
       </c>
       <c r="F12">
-        <v>100</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -710,19 +711,19 @@
         <v>16</v>
       </c>
       <c r="B13">
-        <v>8.5943</v>
+        <v>11.7143</v>
       </c>
       <c r="C13">
-        <v>9.8775</v>
+        <v>13.4163</v>
       </c>
       <c r="D13">
-        <v>8.1714</v>
+        <v>0.221</v>
       </c>
       <c r="E13">
-        <v>0.3251</v>
+        <v>2.0736</v>
       </c>
       <c r="F13">
-        <v>100</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -730,19 +731,19 @@
         <v>17</v>
       </c>
       <c r="B14">
-        <v>13.2779</v>
+        <v>9.7154</v>
       </c>
       <c r="C14">
-        <v>14.9539</v>
+        <v>10.5281</v>
       </c>
       <c r="D14">
-        <v>12.0784</v>
+        <v>9.5227</v>
       </c>
       <c r="E14">
-        <v>0.8209</v>
+        <v>0.1179</v>
       </c>
       <c r="F14">
-        <v>100</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -750,19 +751,19 @@
         <v>18</v>
       </c>
       <c r="B15">
-        <v>8.131</v>
+        <v>11.3949</v>
       </c>
       <c r="C15">
-        <v>9.3553</v>
+        <v>12.3931</v>
       </c>
       <c r="D15">
-        <v>7.8354</v>
+        <v>10.9491</v>
       </c>
       <c r="E15">
-        <v>0.2682</v>
+        <v>0.2641</v>
       </c>
       <c r="F15">
-        <v>100</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -770,19 +771,19 @@
         <v>19</v>
       </c>
       <c r="B16">
-        <v>8.6443</v>
+        <v>7.3326</v>
       </c>
       <c r="C16">
-        <v>9.4952</v>
+        <v>13.4557</v>
       </c>
       <c r="D16">
-        <v>8.1934</v>
+        <v>0.2133</v>
       </c>
       <c r="E16">
-        <v>0.3136</v>
+        <v>5.8741</v>
       </c>
       <c r="F16">
-        <v>100</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -790,19 +791,19 @@
         <v>20</v>
       </c>
       <c r="B17">
-        <v>13.4639</v>
+        <v>9.7324</v>
       </c>
       <c r="C17">
-        <v>15.4356</v>
+        <v>10.5098</v>
       </c>
       <c r="D17">
-        <v>12.3822</v>
+        <v>9.5233</v>
       </c>
       <c r="E17">
-        <v>0.7764</v>
+        <v>0.1176</v>
       </c>
       <c r="F17">
-        <v>100</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -810,19 +811,19 @@
         <v>21</v>
       </c>
       <c r="B18">
-        <v>0.1119</v>
+        <v>0.2724</v>
       </c>
       <c r="C18">
-        <v>1.2701</v>
+        <v>3.9579</v>
       </c>
       <c r="D18">
-        <v>0.0779</v>
+        <v>0.2119</v>
       </c>
       <c r="E18">
-        <v>0.1177</v>
+        <v>0.3899</v>
       </c>
       <c r="F18">
-        <v>100</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -830,19 +831,19 @@
         <v>22</v>
       </c>
       <c r="B19">
-        <v>0.1006</v>
+        <v>0.277</v>
       </c>
       <c r="C19">
-        <v>0.1796</v>
+        <v>4.4614</v>
       </c>
       <c r="D19">
-        <v>0.0765</v>
+        <v>0.2097</v>
       </c>
       <c r="E19">
-        <v>0.0183</v>
+        <v>0.4435</v>
       </c>
       <c r="F19">
-        <v>100</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -850,19 +851,19 @@
         <v>23</v>
       </c>
       <c r="B20">
-        <v>0.2259</v>
+        <v>0.2561</v>
       </c>
       <c r="C20">
-        <v>6.5985</v>
+        <v>2.8896</v>
       </c>
       <c r="D20">
-        <v>0.0765</v>
+        <v>0.2088</v>
       </c>
       <c r="E20">
-        <v>0.8808</v>
+        <v>0.2703</v>
       </c>
       <c r="F20">
-        <v>100</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -870,19 +871,19 @@
         <v>24</v>
       </c>
       <c r="B21">
-        <v>0.3211</v>
+        <v>0.353</v>
       </c>
       <c r="C21">
-        <v>11.2443</v>
+        <v>9.7689</v>
       </c>
       <c r="D21">
-        <v>0.0798</v>
+        <v>0.2091</v>
       </c>
       <c r="E21">
-        <v>1.5545</v>
+        <v>0.9451</v>
       </c>
       <c r="F21">
-        <v>100</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -890,19 +891,19 @@
         <v>25</v>
       </c>
       <c r="B22">
-        <v>0.2528</v>
+        <v>0.394</v>
       </c>
       <c r="C22">
-        <v>11.2629</v>
+        <v>11.9248</v>
       </c>
       <c r="D22">
-        <v>0.0786</v>
+        <v>0.208</v>
       </c>
       <c r="E22">
-        <v>1.1493</v>
+        <v>1.1047</v>
       </c>
       <c r="F22">
-        <v>100</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -910,19 +911,19 @@
         <v>26</v>
       </c>
       <c r="B23">
-        <v>9.5751</v>
+        <v>8.5255</v>
       </c>
       <c r="C23">
-        <v>14.1172</v>
+        <v>13.157</v>
       </c>
       <c r="D23">
-        <v>2.2144</v>
+        <v>0.9936</v>
       </c>
       <c r="E23">
-        <v>3.0326</v>
+        <v>2.7766</v>
       </c>
       <c r="F23">
-        <v>100</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -930,19 +931,19 @@
         <v>27</v>
       </c>
       <c r="B24">
-        <v>0.2144</v>
+        <v>0.2953</v>
       </c>
       <c r="C24">
-        <v>3.2109</v>
+        <v>4.2241</v>
       </c>
       <c r="D24">
-        <v>0.056</v>
+        <v>0.2119</v>
       </c>
       <c r="E24">
-        <v>0.5131</v>
+        <v>0.3889</v>
       </c>
       <c r="F24">
-        <v>100</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -950,19 +951,19 @@
         <v>28</v>
       </c>
       <c r="B25">
-        <v>0.1844</v>
+        <v>0.2964</v>
       </c>
       <c r="C25">
-        <v>2.7666</v>
+        <v>3.7945</v>
       </c>
       <c r="D25">
-        <v>0.0806</v>
+        <v>0.2108</v>
       </c>
       <c r="E25">
-        <v>0.4136</v>
+        <v>0.3906</v>
       </c>
       <c r="F25">
-        <v>100</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -970,19 +971,19 @@
         <v>29</v>
       </c>
       <c r="B26">
-        <v>0.1867</v>
+        <v>0.2966</v>
       </c>
       <c r="C26">
-        <v>2.8814</v>
+        <v>4.5323</v>
       </c>
       <c r="D26">
-        <v>0.0608</v>
+        <v>0.2099</v>
       </c>
       <c r="E26">
-        <v>0.4286</v>
+        <v>0.3892</v>
       </c>
       <c r="F26">
-        <v>100</v>
+        <v>6000</v>
       </c>
     </row>
   </sheetData>
@@ -1020,19 +1021,19 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>0.2344</v>
+        <v>0.0103</v>
       </c>
       <c r="C2">
-        <v>0.2444</v>
+        <v>0.0364</v>
       </c>
       <c r="D2">
-        <v>0.2211</v>
+        <v>-0.0088</v>
       </c>
       <c r="E2">
-        <v>0.004</v>
+        <v>0.009</v>
       </c>
       <c r="F2">
-        <v>100</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1040,19 +1041,19 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>8.328</v>
+        <v>4.3892</v>
       </c>
       <c r="C3">
-        <v>8.3428</v>
+        <v>4.4023</v>
       </c>
       <c r="D3">
-        <v>8.3072</v>
+        <v>4.3755</v>
       </c>
       <c r="E3">
-        <v>0.0096</v>
+        <v>0.0037</v>
       </c>
       <c r="F3">
-        <v>100</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1060,19 +1061,19 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>0.3182</v>
+        <v>0.1724</v>
       </c>
       <c r="C4">
-        <v>3.2812</v>
+        <v>11.8944</v>
       </c>
       <c r="D4">
-        <v>0.2235</v>
+        <v>-0.0101</v>
       </c>
       <c r="E4">
-        <v>0.4204</v>
+        <v>1.1714</v>
       </c>
       <c r="F4">
-        <v>100</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1080,19 +1081,19 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>0.469</v>
+        <v>0.1696</v>
       </c>
       <c r="C5">
-        <v>6.1327</v>
+        <v>11.8393</v>
       </c>
       <c r="D5">
-        <v>0.22</v>
+        <v>-0.009</v>
       </c>
       <c r="E5">
-        <v>1.0239</v>
+        <v>1.156</v>
       </c>
       <c r="F5">
-        <v>100</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1100,19 +1101,19 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>0.5286</v>
+        <v>0.3128</v>
       </c>
       <c r="C6">
-        <v>8.2569</v>
+        <v>16.1558</v>
       </c>
       <c r="D6">
-        <v>0.2238</v>
+        <v>-0.0099</v>
       </c>
       <c r="E6">
-        <v>1.4053</v>
+        <v>1.8789</v>
       </c>
       <c r="F6">
-        <v>100</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1120,19 +1121,19 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>0.6602</v>
+        <v>0.1638</v>
       </c>
       <c r="C7">
-        <v>8.1711</v>
+        <v>4.4102</v>
       </c>
       <c r="D7">
-        <v>0.2224</v>
+        <v>-0.0098</v>
       </c>
       <c r="E7">
-        <v>1.4835</v>
+        <v>0.5891</v>
       </c>
       <c r="F7">
-        <v>100</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1140,19 +1141,19 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>0.562</v>
+        <v>0.1565</v>
       </c>
       <c r="C8">
-        <v>9.7773</v>
+        <v>4.4241</v>
       </c>
       <c r="D8">
-        <v>0.2233</v>
+        <v>-0.0097</v>
       </c>
       <c r="E8">
-        <v>1.5503</v>
+        <v>0.575</v>
       </c>
       <c r="F8">
-        <v>100</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1160,19 +1161,19 @@
         <v>12</v>
       </c>
       <c r="B9">
-        <v>0.3384</v>
+        <v>0.1689</v>
       </c>
       <c r="C9">
-        <v>4.0969</v>
+        <v>5.118</v>
       </c>
       <c r="D9">
-        <v>0.2244</v>
+        <v>-0.0099</v>
       </c>
       <c r="E9">
-        <v>0.4439</v>
+        <v>0.635</v>
       </c>
       <c r="F9">
-        <v>100</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1180,19 +1181,19 @@
         <v>13</v>
       </c>
       <c r="B10">
-        <v>0.5448</v>
+        <v>0.2413</v>
       </c>
       <c r="C10">
-        <v>7.8059</v>
+        <v>4.4414</v>
       </c>
       <c r="D10">
-        <v>0.2233</v>
+        <v>-0.0088</v>
       </c>
       <c r="E10">
-        <v>1.2319</v>
+        <v>0.7185</v>
       </c>
       <c r="F10">
-        <v>100</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1200,19 +1201,19 @@
         <v>14</v>
       </c>
       <c r="B11">
-        <v>0.5593</v>
+        <v>0.2416</v>
       </c>
       <c r="C11">
-        <v>7.7425</v>
+        <v>4.4196</v>
       </c>
       <c r="D11">
-        <v>0.2208</v>
+        <v>-0.0092</v>
       </c>
       <c r="E11">
-        <v>1.2682</v>
+        <v>0.7186</v>
       </c>
       <c r="F11">
-        <v>100</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1220,19 +1221,19 @@
         <v>15</v>
       </c>
       <c r="B12">
-        <v>11.3549</v>
+        <v>5.1388</v>
       </c>
       <c r="C12">
-        <v>12.1485</v>
+        <v>6.5294</v>
       </c>
       <c r="D12">
-        <v>10.9978</v>
+        <v>4.7801</v>
       </c>
       <c r="E12">
-        <v>0.2769</v>
+        <v>0.2616</v>
       </c>
       <c r="F12">
-        <v>100</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1240,19 +1241,19 @@
         <v>16</v>
       </c>
       <c r="B13">
-        <v>12.3031</v>
+        <v>0.0103</v>
       </c>
       <c r="C13">
-        <v>13.2164</v>
+        <v>0.0319</v>
       </c>
       <c r="D13">
-        <v>11.8003</v>
+        <v>-0.0127</v>
       </c>
       <c r="E13">
-        <v>0.342</v>
+        <v>0.0091</v>
       </c>
       <c r="F13">
-        <v>100</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1260,19 +1261,19 @@
         <v>17</v>
       </c>
       <c r="B14">
-        <v>9.7492</v>
+        <v>12.6908</v>
       </c>
       <c r="C14">
-        <v>10.2441</v>
+        <v>16.8267</v>
       </c>
       <c r="D14">
-        <v>9.6097</v>
+        <v>10.7125</v>
       </c>
       <c r="E14">
-        <v>0.0886</v>
+        <v>1.0643</v>
       </c>
       <c r="F14">
-        <v>100</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1280,19 +1281,19 @@
         <v>18</v>
       </c>
       <c r="B15">
-        <v>11.4917</v>
+        <v>5.2462</v>
       </c>
       <c r="C15">
-        <v>12.3767</v>
+        <v>6.5931</v>
       </c>
       <c r="D15">
-        <v>11.0183</v>
+        <v>4.8417</v>
       </c>
       <c r="E15">
-        <v>0.2732</v>
+        <v>0.255</v>
       </c>
       <c r="F15">
-        <v>100</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1300,19 +1301,19 @@
         <v>19</v>
       </c>
       <c r="B16">
-        <v>12.2369</v>
+        <v>0.0102</v>
       </c>
       <c r="C16">
-        <v>13.0403</v>
+        <v>0.0313</v>
       </c>
       <c r="D16">
-        <v>11.7453</v>
+        <v>-0.0097</v>
       </c>
       <c r="E16">
-        <v>0.3438</v>
+        <v>0.009</v>
       </c>
       <c r="F16">
-        <v>100</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1320,19 +1321,19 @@
         <v>20</v>
       </c>
       <c r="B17">
-        <v>9.7411</v>
+        <v>13.1336</v>
       </c>
       <c r="C17">
-        <v>10.2708</v>
+        <v>17.3444</v>
       </c>
       <c r="D17">
-        <v>9.5933</v>
+        <v>11.2425</v>
       </c>
       <c r="E17">
-        <v>0.1114</v>
+        <v>1.0751</v>
       </c>
       <c r="F17">
-        <v>100</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1340,19 +1341,19 @@
         <v>21</v>
       </c>
       <c r="B18">
-        <v>0.307</v>
+        <v>0.0429</v>
       </c>
       <c r="C18">
-        <v>3.9448</v>
+        <v>2.5405</v>
       </c>
       <c r="D18">
-        <v>0.2244</v>
+        <v>-0.01</v>
       </c>
       <c r="E18">
-        <v>0.5197</v>
+        <v>0.2623</v>
       </c>
       <c r="F18">
-        <v>100</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1360,19 +1361,19 @@
         <v>22</v>
       </c>
       <c r="B19">
-        <v>0.2754</v>
+        <v>0.0419</v>
       </c>
       <c r="C19">
-        <v>4.3856</v>
+        <v>2.6189</v>
       </c>
       <c r="D19">
-        <v>0.2172</v>
+        <v>-0.0126</v>
       </c>
       <c r="E19">
-        <v>0.414</v>
+        <v>0.2615</v>
       </c>
       <c r="F19">
-        <v>100</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1380,19 +1381,19 @@
         <v>23</v>
       </c>
       <c r="B20">
-        <v>0.2323</v>
+        <v>0.1114</v>
       </c>
       <c r="C20">
-        <v>0.3128</v>
+        <v>7.5731</v>
       </c>
       <c r="D20">
-        <v>0.218</v>
+        <v>-0.0099</v>
       </c>
       <c r="E20">
-        <v>0.0089</v>
+        <v>0.8396</v>
       </c>
       <c r="F20">
-        <v>100</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1400,19 +1401,19 @@
         <v>24</v>
       </c>
       <c r="B21">
-        <v>0.2546</v>
+        <v>0.148</v>
       </c>
       <c r="C21">
-        <v>1.7978</v>
+        <v>10.5908</v>
       </c>
       <c r="D21">
-        <v>0.2183</v>
+        <v>-0.0098</v>
       </c>
       <c r="E21">
-        <v>0.176</v>
+        <v>1.0389</v>
       </c>
       <c r="F21">
-        <v>100</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1420,19 +1421,19 @@
         <v>25</v>
       </c>
       <c r="B22">
-        <v>0.3905</v>
+        <v>0.1922</v>
       </c>
       <c r="C22">
-        <v>9.3187</v>
+        <v>10.5995</v>
       </c>
       <c r="D22">
-        <v>0.2214</v>
+        <v>-0.0099</v>
       </c>
       <c r="E22">
-        <v>1.0629</v>
+        <v>1.1952</v>
       </c>
       <c r="F22">
-        <v>100</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1440,19 +1441,19 @@
         <v>26</v>
       </c>
       <c r="B23">
-        <v>8.0462</v>
+        <v>8.7978</v>
       </c>
       <c r="C23">
-        <v>12.7251</v>
+        <v>13.0455</v>
       </c>
       <c r="D23">
-        <v>0.8369</v>
+        <v>0.6659</v>
       </c>
       <c r="E23">
-        <v>2.8992</v>
+        <v>3.0013</v>
       </c>
       <c r="F23">
-        <v>100</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1460,19 +1461,19 @@
         <v>27</v>
       </c>
       <c r="B24">
-        <v>0.2832</v>
+        <v>0.0693</v>
       </c>
       <c r="C24">
-        <v>2.7502</v>
+        <v>3.5055</v>
       </c>
       <c r="D24">
-        <v>0.2202</v>
+        <v>-0.0129</v>
       </c>
       <c r="E24">
-        <v>0.3437</v>
+        <v>0.3271</v>
       </c>
       <c r="F24">
-        <v>100</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1480,19 +1481,19 @@
         <v>28</v>
       </c>
       <c r="B25">
-        <v>0.2906</v>
+        <v>0.0849</v>
       </c>
       <c r="C25">
-        <v>3.2073</v>
+        <v>3.6275</v>
       </c>
       <c r="D25">
-        <v>0.2205</v>
+        <v>-0.008</v>
       </c>
       <c r="E25">
-        <v>0.4142</v>
+        <v>0.3924</v>
       </c>
       <c r="F25">
-        <v>100</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1500,19 +1501,549 @@
         <v>29</v>
       </c>
       <c r="B26">
-        <v>0.2806</v>
+        <v>-0.5525</v>
       </c>
       <c r="C26">
-        <v>3.0164</v>
+        <v>3.3158</v>
       </c>
       <c r="D26">
-        <v>0.2169</v>
+        <v>-0.6531</v>
       </c>
       <c r="E26">
-        <v>0.3526</v>
+        <v>0.4088</v>
       </c>
       <c r="F26">
-        <v>100</v>
+        <v>6000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>0.1016</v>
+      </c>
+      <c r="C2">
+        <v>0.139</v>
+      </c>
+      <c r="D2">
+        <v>0.0744</v>
+      </c>
+      <c r="E2">
+        <v>0.0143</v>
+      </c>
+      <c r="F2">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>6.4537</v>
+      </c>
+      <c r="C3">
+        <v>6.4727</v>
+      </c>
+      <c r="D3">
+        <v>6.4363</v>
+      </c>
+      <c r="E3">
+        <v>0.0055</v>
+      </c>
+      <c r="F3">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>0.2484</v>
+      </c>
+      <c r="C4">
+        <v>11.1387</v>
+      </c>
+      <c r="D4">
+        <v>0.0575</v>
+      </c>
+      <c r="E4">
+        <v>1.0721</v>
+      </c>
+      <c r="F4">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>0.2586</v>
+      </c>
+      <c r="C5">
+        <v>11.1337</v>
+      </c>
+      <c r="D5">
+        <v>0.0581</v>
+      </c>
+      <c r="E5">
+        <v>1.1231</v>
+      </c>
+      <c r="F5">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>0.3783</v>
+      </c>
+      <c r="C6">
+        <v>14.873</v>
+      </c>
+      <c r="D6">
+        <v>0.0612</v>
+      </c>
+      <c r="E6">
+        <v>1.7125</v>
+      </c>
+      <c r="F6">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>0.2965</v>
+      </c>
+      <c r="C7">
+        <v>6.8557</v>
+      </c>
+      <c r="D7">
+        <v>0.0576</v>
+      </c>
+      <c r="E7">
+        <v>0.794</v>
+      </c>
+      <c r="F7">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>0.2971</v>
+      </c>
+      <c r="C8">
+        <v>6.7271</v>
+      </c>
+      <c r="D8">
+        <v>0.0547</v>
+      </c>
+      <c r="E8">
+        <v>0.8034</v>
+      </c>
+      <c r="F8">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>0.3052</v>
+      </c>
+      <c r="C9">
+        <v>7.4401</v>
+      </c>
+      <c r="D9">
+        <v>0.0524</v>
+      </c>
+      <c r="E9">
+        <v>0.8479</v>
+      </c>
+      <c r="F9">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>0.4235</v>
+      </c>
+      <c r="C10">
+        <v>6.8736</v>
+      </c>
+      <c r="D10">
+        <v>0.0575</v>
+      </c>
+      <c r="E10">
+        <v>1.0375</v>
+      </c>
+      <c r="F10">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>0.4247</v>
+      </c>
+      <c r="C11">
+        <v>6.8663</v>
+      </c>
+      <c r="D11">
+        <v>0.0573</v>
+      </c>
+      <c r="E11">
+        <v>1.047</v>
+      </c>
+      <c r="F11">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>8.0895</v>
+      </c>
+      <c r="C12">
+        <v>9.5125</v>
+      </c>
+      <c r="D12">
+        <v>7.7</v>
+      </c>
+      <c r="E12">
+        <v>0.2782</v>
+      </c>
+      <c r="F12">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13">
+        <v>0.0994</v>
+      </c>
+      <c r="C13">
+        <v>0.1326</v>
+      </c>
+      <c r="D13">
+        <v>0.073</v>
+      </c>
+      <c r="E13">
+        <v>0.0142</v>
+      </c>
+      <c r="F13">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14">
+        <v>12.92</v>
+      </c>
+      <c r="C14">
+        <v>16.4131</v>
+      </c>
+      <c r="D14">
+        <v>11.4807</v>
+      </c>
+      <c r="E14">
+        <v>0.798</v>
+      </c>
+      <c r="F14">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15">
+        <v>1.9265</v>
+      </c>
+      <c r="C15">
+        <v>10.0655</v>
+      </c>
+      <c r="D15">
+        <v>0.0729</v>
+      </c>
+      <c r="E15">
+        <v>3.3866</v>
+      </c>
+      <c r="F15">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16">
+        <v>0.099</v>
+      </c>
+      <c r="C16">
+        <v>0.1317</v>
+      </c>
+      <c r="D16">
+        <v>0.073</v>
+      </c>
+      <c r="E16">
+        <v>0.0143</v>
+      </c>
+      <c r="F16">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17">
+        <v>13.249</v>
+      </c>
+      <c r="C17">
+        <v>16.2012</v>
+      </c>
+      <c r="D17">
+        <v>11.8697</v>
+      </c>
+      <c r="E17">
+        <v>0.7947</v>
+      </c>
+      <c r="F17">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18">
+        <v>0.1382</v>
+      </c>
+      <c r="C18">
+        <v>3.4664</v>
+      </c>
+      <c r="D18">
+        <v>0.0627</v>
+      </c>
+      <c r="E18">
+        <v>0.3311</v>
+      </c>
+      <c r="F18">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19">
+        <v>0.1447</v>
+      </c>
+      <c r="C19">
+        <v>3.7092</v>
+      </c>
+      <c r="D19">
+        <v>0.0543</v>
+      </c>
+      <c r="E19">
+        <v>0.3751</v>
+      </c>
+      <c r="F19">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20">
+        <v>0.1861</v>
+      </c>
+      <c r="C20">
+        <v>6.6838</v>
+      </c>
+      <c r="D20">
+        <v>0.0568</v>
+      </c>
+      <c r="E20">
+        <v>0.7144</v>
+      </c>
+      <c r="F20">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21">
+        <v>0.2478</v>
+      </c>
+      <c r="C21">
+        <v>11.4393</v>
+      </c>
+      <c r="D21">
+        <v>0.062</v>
+      </c>
+      <c r="E21">
+        <v>1.1113</v>
+      </c>
+      <c r="F21">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22">
+        <v>0.2917</v>
+      </c>
+      <c r="C22">
+        <v>11.9323</v>
+      </c>
+      <c r="D22">
+        <v>0.0555</v>
+      </c>
+      <c r="E22">
+        <v>1.2738</v>
+      </c>
+      <c r="F22">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23">
+        <v>9.6927</v>
+      </c>
+      <c r="C23">
+        <v>14.3653</v>
+      </c>
+      <c r="D23">
+        <v>0.9721</v>
+      </c>
+      <c r="E23">
+        <v>3.19</v>
+      </c>
+      <c r="F23">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24">
+        <v>0.1713</v>
+      </c>
+      <c r="C24">
+        <v>3.7361</v>
+      </c>
+      <c r="D24">
+        <v>0.06</v>
+      </c>
+      <c r="E24">
+        <v>0.3965</v>
+      </c>
+      <c r="F24">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25">
+        <v>0.1736</v>
+      </c>
+      <c r="C25">
+        <v>3.9579</v>
+      </c>
+      <c r="D25">
+        <v>0.0581</v>
+      </c>
+      <c r="E25">
+        <v>0.4071</v>
+      </c>
+      <c r="F25">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26">
+        <v>0.1758</v>
+      </c>
+      <c r="C26">
+        <v>4.9522</v>
+      </c>
+      <c r="D26">
+        <v>0.0568</v>
+      </c>
+      <c r="E26">
+        <v>0.4192</v>
+      </c>
+      <c r="F26">
+        <v>6000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sync up for DMM capture
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -7,15 +7,14 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="3_3" sheetId="1" r:id="rId1"/>
-    <sheet name="1_8" sheetId="2" r:id="rId2"/>
+    <sheet name="test" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
   <si>
     <t>1.Average (mA)</t>
   </si>
@@ -32,10 +31,16 @@
     <t>5.Count</t>
   </si>
   <si>
-    <t>Deep_Sleep</t>
-  </si>
-  <si>
-    <t>BT_Idle</t>
+    <t>6.Raw</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>-0.009826,-0.012998,-0.010111,-0.00806,-0.009181,-0.008067,-0.006314,-0.015587,-0.012808,-0.012802</t>
+  </si>
+  <si>
+    <t>-7.836767,-7.83968,-7.841563,-7.833445,-7.825357,-7.831563,-7.82865,-7.837141,-7.837677,-7.829997</t>
   </si>
 </sst>
 </file>
@@ -393,13 +398,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -415,115 +420,31 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2">
-        <v>0.2424</v>
+        <v>-7.8342</v>
       </c>
       <c r="C2">
-        <v>0.2527</v>
+        <v>-7.8254</v>
       </c>
       <c r="D2">
-        <v>0.2314</v>
+        <v>-7.8416</v>
       </c>
       <c r="E2">
-        <v>0.0036</v>
+        <v>0.005</v>
       </c>
       <c r="F2">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3">
-        <v>8.5867</v>
-      </c>
-      <c r="C3">
-        <v>8.6106</v>
-      </c>
-      <c r="D3">
-        <v>8.5626</v>
-      </c>
-      <c r="E3">
-        <v>0.0108</v>
-      </c>
-      <c r="F3">
-        <v>600</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2">
-        <v>-0.1014</v>
-      </c>
-      <c r="C2">
-        <v>-0.0754</v>
-      </c>
-      <c r="D2">
-        <v>-0.1391</v>
-      </c>
-      <c r="E2">
-        <v>0.0178</v>
-      </c>
-      <c r="F2">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3">
-        <v>-6.5543</v>
-      </c>
-      <c r="C3">
-        <v>-6.5384</v>
-      </c>
-      <c r="D3">
-        <v>-6.5704</v>
-      </c>
-      <c r="E3">
-        <v>0.0056</v>
-      </c>
-      <c r="F3">
-        <v>600</v>
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sync up for main test flow
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -7,14 +7,15 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="test" sheetId="1" r:id="rId1"/>
+    <sheet name="3_3" sheetId="1" r:id="rId1"/>
+    <sheet name="1_8" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t>1.Average (mA)</t>
   </si>
@@ -34,13 +35,22 @@
     <t>6.Raw</t>
   </si>
   <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>-0.009826,-0.012998,-0.010111,-0.00806,-0.009181,-0.008067,-0.006314,-0.015587,-0.012808,-0.012802</t>
-  </si>
-  <si>
-    <t>-7.836767,-7.83968,-7.841563,-7.833445,-7.825357,-7.831563,-7.82865,-7.837141,-7.837677,-7.829997</t>
+    <t>case_0</t>
+  </si>
+  <si>
+    <t>case_1</t>
+  </si>
+  <si>
+    <t>-0.011314,-0.010668,-0.011504,-0.011599,-0.014935,-0.005098,-0.00825,-0.008896,-0.013175,-0.013909</t>
+  </si>
+  <si>
+    <t>-0.017625,-0.017897,-0.008338,-0.007231,-0.016144,-0.004629,-0.01808,-0.007319,-0.018359,-0.002679</t>
+  </si>
+  <si>
+    <t>-7.852064,-7.847924,-7.857142,-7.854257,-7.85059,-7.850463,-7.847953,-7.852409,-7.847798,-7.849398</t>
+  </si>
+  <si>
+    <t>-7.855414,-7.860365,-7.868426,-7.850682,-7.860527,-7.85363,-7.865979,-7.850026,-7.856169,-7.859462</t>
   </si>
 </sst>
 </file>
@@ -398,7 +408,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -429,22 +439,124 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>-7.8342</v>
+        <v>-0.0109</v>
       </c>
       <c r="C2">
-        <v>-7.8254</v>
+        <v>-0.0051</v>
       </c>
       <c r="D2">
-        <v>-7.8416</v>
+        <v>-0.0149</v>
       </c>
       <c r="E2">
-        <v>0.005</v>
+        <v>0.0028</v>
       </c>
       <c r="F2">
         <v>10</v>
       </c>
       <c r="G2" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>-0.0118</v>
+      </c>
+      <c r="C3">
+        <v>-0.0027</v>
+      </c>
+      <c r="D3">
+        <v>-0.0184</v>
+      </c>
+      <c r="E3">
+        <v>0.006</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>-7.851</v>
+      </c>
+      <c r="C2">
+        <v>-7.8478</v>
+      </c>
+      <c r="D2">
+        <v>-7.8571</v>
+      </c>
+      <c r="E2">
+        <v>0.0029</v>
+      </c>
+      <c r="F2">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>-7.8581</v>
+      </c>
+      <c r="C3">
+        <v>-7.85</v>
+      </c>
+      <c r="D3">
+        <v>-7.8684</v>
+      </c>
+      <c r="E3">
+        <v>0.0058</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Call BT func working
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
   <si>
     <t>1.Average (mA)</t>
   </si>
@@ -35,22 +35,31 @@
     <t>6.Raw</t>
   </si>
   <si>
-    <t>case_0</t>
+    <t>Deep_Sleep</t>
   </si>
   <si>
     <t>case_1</t>
   </si>
   <si>
-    <t>0.007461,0.008858,0.00271,-0.005052,-0.00168,-0.002879,-0.00132,-0.004096,0.008002,0.001853</t>
-  </si>
-  <si>
-    <t>-0.000842,-0.002221,0.002971,-0.002519,0.001214,0.006586,0.00389,-0.002879,-3e-06,0.001773</t>
-  </si>
-  <si>
-    <t>-0.242436,-0.242757,-0.244714,-0.242738,-0.246368,-0.243856,-0.243275,-0.241367,-0.246905,-0.236632</t>
-  </si>
-  <si>
-    <t>-0.239373,-0.238855,-0.23854,-0.239972,-0.236651,-0.242466,-0.240509,-0.245794,-0.241621,-0.245529</t>
+    <t>case_3</t>
+  </si>
+  <si>
+    <t>-0.002798,-0.001482,-0.010965,0.009219,-0.001184,-0.000364,-0.000382,-0.005754,0.002791,-0.000463</t>
+  </si>
+  <si>
+    <t>-0.004854,0.000177,-0.009424,-0.002978,-0.004835,0.005325,0.006064,0.002431,0.000673,0.008281</t>
+  </si>
+  <si>
+    <t>-0.002699,-0.00178,0.008858,0.004188,0.000456,-0.00178,-0.002618,-0.003618,0.002133,0.006126</t>
+  </si>
+  <si>
+    <t>-0.240528,-0.244695,-0.240515,-0.244961,-0.236367,-0.235231,-0.240503,-0.241621,-0.239108,-0.241059</t>
+  </si>
+  <si>
+    <t>-0.247745,-0.238861,-0.240509,-0.241349,-0.23799,-0.241102,-0.249684,-0.237737,-0.239682,-0.241355</t>
+  </si>
+  <si>
+    <t>-0.239694,-0.239991,-0.247473,-0.240225,-0.240799,-0.244992,-0.236644,-0.248295,-0.23996,-0.245251</t>
   </si>
 </sst>
 </file>
@@ -408,7 +417,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -439,22 +448,22 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>0.0014</v>
+        <v>-0.0011</v>
       </c>
       <c r="C2">
-        <v>0.0089</v>
+        <v>0.0092</v>
       </c>
       <c r="D2">
-        <v>-0.0051</v>
+        <v>-0.011</v>
       </c>
       <c r="E2">
-        <v>0.0049</v>
+        <v>0.005</v>
       </c>
       <c r="F2">
         <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -462,22 +471,45 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>0.0008</v>
+        <v>0.0001</v>
       </c>
       <c r="C3">
-        <v>0.0066</v>
+        <v>0.0083</v>
       </c>
       <c r="D3">
-        <v>-0.0029</v>
+        <v>-0.0094</v>
       </c>
       <c r="E3">
-        <v>0.0029</v>
+        <v>0.0053</v>
       </c>
       <c r="F3">
         <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>0.0009</v>
+      </c>
+      <c r="C4">
+        <v>0.0089</v>
+      </c>
+      <c r="D4">
+        <v>-0.0036</v>
+      </c>
+      <c r="E4">
+        <v>0.004</v>
+      </c>
+      <c r="F4">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -487,7 +519,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -518,22 +550,22 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>-0.2431</v>
+        <v>-0.2405</v>
       </c>
       <c r="C2">
-        <v>-0.2366</v>
+        <v>-0.2352</v>
       </c>
       <c r="D2">
-        <v>-0.2469</v>
+        <v>-0.245</v>
       </c>
       <c r="E2">
-        <v>0.0027</v>
+        <v>0.0029</v>
       </c>
       <c r="F2">
         <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -541,22 +573,45 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>-0.2409</v>
+        <v>-0.2416</v>
       </c>
       <c r="C3">
-        <v>-0.2367</v>
+        <v>-0.2377</v>
       </c>
       <c r="D3">
-        <v>-0.2458</v>
+        <v>-0.2497</v>
       </c>
       <c r="E3">
-        <v>0.0028</v>
+        <v>0.0038</v>
       </c>
       <c r="F3">
         <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>-0.2423</v>
+      </c>
+      <c r="C4">
+        <v>-0.2366</v>
+      </c>
+      <c r="D4">
+        <v>-0.2483</v>
+      </c>
+      <c r="E4">
+        <v>0.0037</v>
+      </c>
+      <c r="F4">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BD address get from ssh working
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
     <t>1.Average (mA)</t>
   </si>
@@ -44,22 +44,31 @@
     <t>BT_I_Scan</t>
   </si>
   <si>
-    <t>0.238239,0.235705,0.24335,0.23686,0.245387,0.2374,0.247623,0.236842,0.234507,0.242493</t>
-  </si>
-  <si>
-    <t>8.361353,8.365427,8.383853,8.387523,8.366563,8.351752,8.370377,8.38453,8.375848,8.358701</t>
-  </si>
-  <si>
-    <t>0.230954,0.23822,0.244188,0.243151,0.235724,0.240655,0.242294,0.24189,0.237978,0.242331</t>
-  </si>
-  <si>
-    <t>-0.091836,-0.088261,-0.086551,-0.127434,-0.097417,-0.087403,-0.122409,-0.086822,-0.086014,-0.128823</t>
-  </si>
-  <si>
-    <t>-5.506857,-5.5191,-5.511889,-5.503017,-5.502147,-5.516316,-5.519082,-5.511321,-5.49688,-5.504369</t>
-  </si>
-  <si>
-    <t>-4.43255,-0.082661,-0.094892,-0.124082,-0.088526,-0.084347,-0.125175,-0.086841,-0.087958,-0.091298</t>
+    <t>BT_ACL_Sniff_1dot28s_Master_0dBm</t>
+  </si>
+  <si>
+    <t>0.234209,0.242412,0.239419,0.246225,0.239158,0.231252,0.233389,0.239798,0.246523,0.240357</t>
+  </si>
+  <si>
+    <t>8.39487,8.380977,8.361055,8.371432,8.382853,8.398062,8.383132,8.355366,8.372432,8.384548</t>
+  </si>
+  <si>
+    <t>0.23722,0.236363,0.245604,0.236003,0.243648,0.240177,0.236363,0.241015,0.240294,0.240835</t>
+  </si>
+  <si>
+    <t>0.24353,0.237699,0.249219,0.243151,0.237959,0.239996,0.244008,3.433437,0.242214,0.241971</t>
+  </si>
+  <si>
+    <t>-0.086304,-0.08936,-0.127971,-0.094632,-0.087705,-0.130206,-0.08739,-0.123502,-0.089366,-0.08573</t>
+  </si>
+  <si>
+    <t>-5.507963,-5.519113,-5.506302,-5.511062,-5.506042,-5.510759,-5.516316,-5.510482,-5.509951,-5.507975</t>
+  </si>
+  <si>
+    <t>-0.127706,-0.089903,-0.085433,-0.129373,-0.080741,-3.445201,-0.086267,-0.123823,-0.084063,-0.091589</t>
+  </si>
+  <si>
+    <t>-0.08965,-0.125502,-0.092681,-0.082958,-0.126292,-0.085186,-0.094614,-0.131867,-0.092947,-0.088502</t>
   </si>
 </sst>
 </file>
@@ -417,7 +426,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -448,22 +457,22 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>0.2398</v>
+        <v>0.2393</v>
       </c>
       <c r="C2">
-        <v>0.2476</v>
+        <v>0.2465</v>
       </c>
       <c r="D2">
-        <v>0.2345</v>
+        <v>0.2313</v>
       </c>
       <c r="E2">
-        <v>0.0043</v>
+        <v>0.0049</v>
       </c>
       <c r="F2">
         <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -471,22 +480,22 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>8.3706</v>
+        <v>8.3785</v>
       </c>
       <c r="C3">
-        <v>8.387499999999999</v>
+        <v>8.3981</v>
       </c>
       <c r="D3">
-        <v>8.351800000000001</v>
+        <v>8.3554</v>
       </c>
       <c r="E3">
-        <v>0.0114</v>
+        <v>0.0129</v>
       </c>
       <c r="F3">
         <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -494,22 +503,45 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>0.2397</v>
+        <v>0.2398</v>
       </c>
       <c r="C4">
-        <v>0.2442</v>
+        <v>0.2456</v>
       </c>
       <c r="D4">
-        <v>0.231</v>
+        <v>0.236</v>
       </c>
       <c r="E4">
-        <v>0.0039</v>
+        <v>0.0031</v>
       </c>
       <c r="F4">
         <v>10</v>
       </c>
       <c r="G4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>0.5613</v>
+      </c>
+      <c r="C5">
+        <v>3.4334</v>
+      </c>
+      <c r="D5">
+        <v>0.2377</v>
+      </c>
+      <c r="E5">
+        <v>0.9574</v>
+      </c>
+      <c r="F5">
+        <v>10</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -519,7 +551,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -550,22 +582,22 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>-0.1003</v>
+        <v>-0.1002</v>
       </c>
       <c r="C2">
-        <v>-0.08599999999999999</v>
+        <v>-0.0857</v>
       </c>
       <c r="D2">
-        <v>-0.1288</v>
+        <v>-0.1302</v>
       </c>
       <c r="E2">
-        <v>0.0173</v>
+        <v>0.0179</v>
       </c>
       <c r="F2">
         <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -573,22 +605,22 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>-5.5091</v>
+        <v>-5.5106</v>
       </c>
       <c r="C3">
-        <v>-5.4969</v>
+        <v>-5.506</v>
       </c>
       <c r="D3">
         <v>-5.5191</v>
       </c>
       <c r="E3">
-        <v>0.0073</v>
+        <v>0.004</v>
       </c>
       <c r="F3">
         <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -596,22 +628,45 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>-0.5298</v>
+        <v>-0.4344</v>
       </c>
       <c r="C4">
-        <v>-0.0827</v>
+        <v>-0.0807</v>
       </c>
       <c r="D4">
-        <v>-4.4325</v>
+        <v>-3.4452</v>
       </c>
       <c r="E4">
-        <v>1.301</v>
+        <v>1.0038</v>
       </c>
       <c r="F4">
         <v>10</v>
       </c>
       <c r="G4" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>-0.101</v>
+      </c>
+      <c r="C5">
+        <v>-0.083</v>
+      </c>
+      <c r="D5">
+        <v>-0.1319</v>
+      </c>
+      <c r="E5">
+        <v>0.018</v>
+      </c>
+      <c r="F5">
+        <v>10</v>
+      </c>
+      <c r="G5" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BT Tx @ max power may have issue, need to debug
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
   <si>
     <t>1.Average (mA)</t>
   </si>
@@ -35,40 +35,76 @@
     <t>6.Raw</t>
   </si>
   <si>
-    <t>Deep_Sleep</t>
-  </si>
-  <si>
-    <t>BT_Idle</t>
-  </si>
-  <si>
-    <t>BT_I_Scan</t>
-  </si>
-  <si>
-    <t>BT_ACL_Sniff_1dot28s_Master_0dBm</t>
-  </si>
-  <si>
-    <t>0.234209,0.242412,0.239419,0.246225,0.239158,0.231252,0.233389,0.239798,0.246523,0.240357</t>
-  </si>
-  <si>
-    <t>8.39487,8.380977,8.361055,8.371432,8.382853,8.398062,8.383132,8.355366,8.372432,8.384548</t>
-  </si>
-  <si>
-    <t>0.23722,0.236363,0.245604,0.236003,0.243648,0.240177,0.236363,0.241015,0.240294,0.240835</t>
-  </si>
-  <si>
-    <t>0.24353,0.237699,0.249219,0.243151,0.237959,0.239996,0.244008,3.433437,0.242214,0.241971</t>
-  </si>
-  <si>
-    <t>-0.086304,-0.08936,-0.127971,-0.094632,-0.087705,-0.130206,-0.08739,-0.123502,-0.089366,-0.08573</t>
-  </si>
-  <si>
-    <t>-5.507963,-5.519113,-5.506302,-5.511062,-5.506042,-5.510759,-5.516316,-5.510482,-5.509951,-5.507975</t>
-  </si>
-  <si>
-    <t>-0.127706,-0.089903,-0.085433,-0.129373,-0.080741,-3.445201,-0.086267,-0.123823,-0.084063,-0.091589</t>
-  </si>
-  <si>
-    <t>-0.08965,-0.125502,-0.092681,-0.082958,-0.126292,-0.085186,-0.094614,-0.131867,-0.092947,-0.088502</t>
+    <t>Deep Sleep</t>
+  </si>
+  <si>
+    <t>BT Idle</t>
+  </si>
+  <si>
+    <t>BT SCO HV3 Master @ 0 dBm at Pin</t>
+  </si>
+  <si>
+    <t>BT SCO HV3 Master @ 4 dBm at Pin</t>
+  </si>
+  <si>
+    <t>BT SCO HV3 Master @ Max dBm at Pin</t>
+  </si>
+  <si>
+    <t>BT SCO EV3 Master @ 0 dBm at Pin</t>
+  </si>
+  <si>
+    <t>BT SCO EV3 Master @ 4 dBm at Pin</t>
+  </si>
+  <si>
+    <t>BT SCO EV3 Master @ Max dBm at Pin</t>
+  </si>
+  <si>
+    <t>0.249976,0.249777,0.246623,0.252112,0.24848,0.259378,0.254609,0.25451,0.249796,0.249535</t>
+  </si>
+  <si>
+    <t>8.460822,8.444135,8.43082,8.450085,8.453736,8.45332,8.44144,8.432199,8.455953,8.466014,8.453096,8.436689,8.439006,8.451283,8.455612,8.442179,8.428125,8.448886,8.459009,8.464716,8.44116,8.436012,8.450923,8.462679,8.454277,8.438825,8.445054,8.449346,8.463138,8.448426,8.418704,8.442278,8.462778,8.459785,8.443856,8.435373,8.448408,8.46248,8.452022,8.440223,8.436969,8.454078,8.472802,8.44757,8.430541,8.447687,8.458829,8.455854,8.443477,8.436969,8.45224,8.458748,8.45214,8.44116,8.444613,8.454773,8.465374,8.45178,8.429603,8.4418,8.45781,8.461083,8.442639,8.442837,8.450644,8.464175,8.457152,8.445812,8.436112,8.4526,8.460704,8.444514,8.428287,8.445595,8.456431,8.463138,8.448389,8.43659,8.450644,8.464076,8.452059,8.44144,8.446911,8.452699,8.459884,8.450103,8.437248,8.447948,8.459965,8.460325,8.442937,8.44244,8.455096,8.462021,8.45763,8.432777,8.443278,8.455773,8.468169,8.448607,8.442458,8.441539,8.46294,8.461164,8.439863,8.433876,8.44757,8.464815,8.453159,8.435751,8.442241,8.456512,8.466672,8.448128,8.435292,8.45232,8.464455,8.456891,8.439267,8.430802,8.455574,8.467051,8.454835,8.438565,8.436571,8.452339,8.465175,8.446948,8.436671,8.450364,8.460462,8.459884,8.44144,8.433137,8.437906,8.463877,8.451221,8.436788,8.437509,8.451482,8.460505,8.444216,8.436689,8.440602,8.46348,8.455872,8.447868,8.432218,8.446948,8.465815,8.452898,8.431659,8.440161,8.450923,8.464256,8.44747,8.434273,8.448128,8.458766,8.455953,8.442458,8.43128,8.448426,8.461542,8.45314,8.441241,8.439881,8.450761,8.460027,8.443955,8.43641,8.443197,8.467051,8.462282,8.439447,8.43092,8.45124,8.464418,8.445433,8.431839,8.438267,8.452482,8.464058,8.450022,8.43577,8.446191,8.468709,8.460686,8.443937,8.430864,8.451383,8.46176,8.453078,8.442061,8.436211,8.456711,8.464896,8.452861,8.433615,8.449463,8.463058,8.457829,8.445514,8.42643,8.447389,8.459487,8.455494,8.436689,8.441043,8.458487,8.465635,8.44693,8.439465,8.446334,8.46258,8.464716,8.440502,8.439267,8.453556,8.461903,8.453997,8.442278,8.438465,8.459307,8.465095,8.448066,8.432938,8.439186,8.452681,8.464436,8.446011,8.438825,8.454935,8.460344,8.450482,8.440484,8.430622,8.458766,8.460425,8.453637,8.435652,8.448066,8.46312,8.458487,8.446849,8.436751,8.448128,8.460226,8.452699,8.433615,8.438645,8.453879,8.463958,8.446389,8.434932,8.44875,8.456692,8.458388,8.449985,8.431578,8.451122,8.46276,8.453277,8.435571,8.443216,8.455655,8.454277,8.4515,8.435354,8.440862,8.455115,8.462958,8.440421,8.438745,8.446073,8.465194,8.453898,8.440223,8.440204,8.458748,8.461182,8.444775,8.439763,8.44126,8.468448,8.453258,8.442458,8.434615,8.45314,8.463778,8.451879,8.438447,8.438006,8.460623,8.466194,8.45178,8.438366,8.439546,8.454475,8.460984,8.442918,8.433634,8.444235,8.465374,8.455792,8.437608,8.439186,8.458208,8.461921,8.453817,8.429802,8.44262,8.459108,8.458127,8.44244,8.436049,8.449507,8.464175,8.454935,8.435652,8.435472,8.449886,8.463138,8.442701,8.437689,8.455574,8.462201,8.45681,8.436509,8.435373,8.445713,8.461344,8.458748,8.44298,8.439645,8.464238,8.460605,8.456891,8.426132,8.43595,8.46258,8.46248,8.442477,8.431361,8.448327,8.470845,8.453755,8.43677,8.434553,8.451202,8.455612,8.448489,8.438167,8.439502,8.459127,8.45799,8.451041,8.435932,8.44711,8.466113,8.461822,8.439745,8.435869,8.453537,8.465734,8.454016,8.433236,8.447967,8.462561,8.461083,8.441061,8.433416,8.449265,8.467628,8.451302,8.441521,8.437627,8.450265,8.465536,8.446172,8.434453,8.44198,8.45745,8.462201,8.448526,8.435851,8.449743,8.460686,8.457829,8.439962,8.443937,8.451482,8.464058,8.455214,8.43174,8.443017,8.455016,8.461903,8.447029,8.429982,8.450383,8.456233,8.457332,8.437807,8.432435,8.452519,8.461263,8.446551,8.431119,8.442738,8.457152,8.456692,8.448426,8.432299,8.450383,8.46258,8.459307,8.438627,8.43559,8.458468,8.46384,8.444974,8.430063,8.444297,8.454537,8.465734,8.448147,8.436869,8.457009,8.461542,8.453817,8.434634,8.43641,8.453817,8.454537,8.449644,8.434093,8.450644,8.45727,8.463337,8.444676,8.438285,8.452339,8.46715,8.453618,8.439186,8.433137,8.456332,8.458288,8.453655,8.431839,8.439645,8.460064,8.463958,8.447209,8.429901,8.454494,8.461803,8.455792,8.434435,8.432398,8.454394,8.466411,8.448905,8.434895,8.444533,8.461524,8.45799,8.443117,8.425511,8.440223,8.4623,8.448246,8.438186,8.443378,8.45232,8.461443,8.444154,8.436888,8.447408,8.461344,8.451202,8.443216,8.440862,8.448724,8.457431,8.449426,8.431181,8.431218,8.4526,8.463977,8.446551,8.435193,8.43613,8.4623,8.45691,8.443576,8.435851,8.450283,8.459605,8.455773,8.435652,8.434994,8.455854,8.461083,8.435553,8.432038,8.450302,8.46212,8.461561,8.439844,8.43128,8.452401,8.461282,8.456413,8.44226,8.438745,8.460164,8.464995,8.443216,8.432038,8.440204,8.464815,8.455935,8.443477,8.43064,8.452699,8.460245,8.444216,8.439006,8.433516,8.454935,8.464797,8.44793,8.431379,8.448526,8.455494,8.46294,8.440602,8.432435,8.449805,8.466455,8.453537,8.440881,8.437248,8.459686,8.464815,8.455053,8.425033,8.439465,8.455115,8.456251,8.442539,8.434913,8.448309,8.467908,8.455953,8.43623,8.443738,8.446731,8.462039,8.448147,8.431361,8.443278,8.460704,8.459866,8.441061,8.432019,8.452699,8.466293,8.45114,8.429107,8.438546,8.456612,8.463138,8.449644,8.429442,8.441502,8.465455,8.460704,8.440862,8.430063,8.450563,8.461741,8.449526,8.441962,8.434336,8.456152,8.459704,8.450103,8.44198,8.449706,8.45242,8.45663,8.44847,8.435453,8.450581,8.45727,8.455755,8.439925,8.438167,8.460623,8.464536,8.44793,8.428746,8.442017,8.456332,8.453618,8.43531,8.430342,8.446371,8.458866,8.453339,8.441341,8.436012,8.451842,8.461263,8.445433,8.430802,8.438844,8.45745,8.458307,8.448166,8.429324,8.450265,8.460443,8.449265,8.442657,8.441999,8.457351,8.462201,8.44675,8.435751,8.437869,8.466275,8.45142,8.445073,8.434994,8.452401,8.459984,8.453258,8.434255,8.433634,8.448607,8.457909,8.4525,8.433696,8.443216,8.45745,8.46258,8.4408,8.436671,8.448905,8.463138,8.452519,8.434336,8.437608,8.459803,8.462958,8.450022,8.437888,8.443415,8.457928,8.45242,8.438546,8.434075,8.450265,8.470647,8.453519,8.439204,8.442179,8.456872,8.459686,8.44711,8.431479,8.443216,8.455214,8.459027,8.436969,8.431758,8.444713,8.460443,8.454357,8.442458,8.443117,8.456351,8.461064,8.450085,8.433416,8.447011,8.451761,8.451681,8.438366,8.431181,8.450482,8.460704,8.460605,8.437627,8.43649,8.453637,8.468088,8.450085,8.434193,8.435453,8.459667,8.459505,8.439465,8.437608,8.45096,8.464039,8.448985,8.437329,8.429864,8.453537,8.453159,8.448327,8.433876,8.442521,8.458388,8.457053,8.450283,8.440061,8.445452,8.460524,8.450283,8.44144,8.437329,8.457909,8.4633,8.451122,8.435453,8.449066,8.459207,8.460543,8.445073,8.431839,8.447948,8.46725,8.445893,8.438465,8.435671,8.462021,8.458568,8.455332,8.43064,8.442539,8.462083,8.454394,8.448408,8.429225,8.443676,8.45709,8.449463,8.436689,8.437987,8.451761,8.459009,8.449228,8.438447,8.443036,8.460064,8.454854,8.443197,8.433354,8.437788,8.465834,8.453817,8.430442,8.437428,8.451022,8.463679,8.445234,8.433218,8.442179,8.465175,8.454835,8.437807,8.435751,8.446849,8.460605,8.448687,8.434615,8.442856,8.448886,8.458487,8.441241,8.429864,8.446632,8.455872,8.454196,8.443036,8.431019,8.446433,8.454537,8.456431,8.435932,8.441701,8.456593,8.453817,8.43723,8.436428,8.436869,8.462741,8.45727,8.432677,8.42625,8.454755,8.469287,8.458009,8.432858,8.44144,8.448265,8.461002,8.448967,8.428927,8.444415,8.462101,8.455214,8.44747,8.424474,8.449346,8.464815,8.459586,8.431379,8.443179,8.450743,8.459686,8.444477,8.437149,8.444017,8.455792,8.455394,8.442179,8.434516,8.443955,8.457431,8.4525,8.438447,8.434093,8.45232,8.46248,8.451041,8.439465,8.444974,8.46276,8.458549,8.44098,8.429982,8.451184,8.461983,8.451581,8.436689,8.436888,8.456295,8.466591,8.450923,8.427927,8.444054,8.461145,8.455854,8.439664,8.425411,8.44683,8.460704,8.455351,8.429044,8.437528,8.458947,8.459686,8.453357,8.43128,8.436292,8.454295,8.454916,8.443477,8.428585,8.450122,8.459425,8.447489,8.437049,8.432299,8.447228,8.46725,8.441359,8.433516,8.44693,8.463896,8.457568,8.438627,8.431262,8.446433,8.459785,8.443856,8.4419,8.437528,8.45727,8.461164,8.445911,8.433137,8.445253,8.463039,8.457369,8.432199,8.430361,8.451463,8.460425,8.450004,8.435193,8.433236,8.461101,8.459164,8.442937,8.433994,8.436671,8.461822,8.455016,8.438384,8.426989,8.451022,8.459425,8.452718,8.432019,8.44126,8.456612,8.462561,8.445154,8.432858,8.4409,8.458009,8.455295,8.443396,8.437689,8.448507,8.471063,8.450383,8.433038,8.436192,8.452401,8.462021,8.440403,8.430541,8.442918,8.467231,8.459667,8.44775,8.43649,8.448706,8.468529,8.45178,8.434435,8.445234,8.450103,8.461822,8.444856,8.432038,8.444297,8.456431,8.460127,8.443595,8.432597,8.448246,8.462101,8.451022,8.438844,8.441341,8.451761,8.460642,8.440862,8.431839,8.438167,8.458866,8.45232,8.4419,8.438726,8.448706,8.462182,8.45178,8.436969,8.429225,8.457531,8.455034,8.452041,8.436192,8.442819,8.459847,8.457431,8.441061,8.429802,8.43759,8.460226,8.452699,8.432299,8.438888,8.455053,8.461244,8.449445,8.432416,8.439906,8.460822,8.462499,8.450203,8.438366,8.450743,8.453339,8.44775,8.433156,8.437788,8.451563,8.45178,8.442657,8.433714,8.446911,8.461822,8.460704,8.443955,8.434553,8.448128,8.46248,8.455935,8.436049,8.444495,8.454394,8.460543,8.449625,8.436292,8.445613,8.46166,8.457729,8.442918,8.434895,8.442719,8.460524,8.451879,8.432118,8.435571,8.455295,8.461064,8.445632,8.430342,8.445551,8.459568,8.45781,8.449886,8.433416,8.448787,8.466672,8.449985,8.436031,8.433137,8.456612,8.46212,8.443396,8.438384,8.440602,8.459425,8.460406,8.442937,8.43082,8.449165,8.464716,8.455314,8.438149,8.440682,8.455773,8.462219,8.444036,8.432218,8.45296,8.459325,8.449526,8.440943,8.428964,8.457549,8.465654,8.451383,8.436671,8.43613,8.455053,8.456531,8.452979,8.440024,8.440322,8.465473,8.461182,8.444154,8.435012,8.452718,8.458829,8.455972,8.433137,8.442098,8.459884,8.453718,8.443378,8.435832,8.436329,8.459667,8.454475,8.447687,8.431361,8.450302,8.456512,8.449644,8.43156,8.439925,8.456233,8.461002,8.44062,8.434733,8.44208,8.453916,8.457928,8.441738,8.43677,8.452041,8.465256,8.45278,8.433336,8.432336,8.455494,8.459388,8.443378,8.431442,8.44144,8.464418,8.449165,8.444334,8.433416,8.444694,8.457909,8.445632,8.433336,8.430081,8.45214,8.458108,8.448967,8.43146,8.443918,8.460145,8.464039,8.440881,8.433895,8.446191,8.464797,8.446272,8.436012,8.428548,8.453736,8.459903,8.446371,8.4321,8.443558,8.460046,8.458847,8.444676,8.429324,8.442558,8.455016,8.449706,8.436292,8.444235,8.454196,8.457729,8.450383,8.431379,8.447607,8.461362,8.453997,8.430703,8.43513,8.444595,8.464995,8.448687,8.439943,8.437608,8.460307,8.461244,8.449048,8.432696,8.440682,8.46212,8.459127,8.444613,8.430423,8.443856,8.459667,8.452997,8.435174,8.438068,8.455935,8.454817,8.444533,8.431578,8.44611,8.466473,8.460325,8.438844,8.432858,8.444775,8.450004,8.45178,8.438844,8.43677,8.456034,8.458947,8.445154,8.439583,8.442937,8.45709,8.459425,8.432479,8.430721,8.439546,8.466374,8.450526,8.435174,8.437788,8.455295,8.464238,8.442819,8.43156,8.446669,8.454214,8.454177,8.440502,8.436031,8.447408,8.45681,8.45296,8.436292,8.433795,8.449706,8.458189,8.446532,8.431659,8.44665,8.460704,8.458468,8.437329,8.438149,8.453258,8.465256,8.451581,8.434255,8.439204,8.456351,8.46751,8.443278,8.433118,8.445371,8.461282,8.46258,8.437807,8.437788,8.446452,8.463399,8.45242,8.438267,8.43731,8.456512,8.460723,8.443738,8.424492,8.439024,8.458766,8.461282,8.443197,8.432659,8.454935,8.463319,8.445992,8.435472,8.440421,8.455034,8.46266,8.443775,8.429523,8.442458,8.459127,8.452041,8.439285,8.438447,8.448607,8.468367,8.455972,8.431541,8.442098,8.454475,8.468926,8.446731,8.429423,8.447489,8.45809,8.454196,8.440602,8.430144,8.438608,8.463877,8.45232,8.438708,8.440502,8.452979,8.464815,8.443856,8.432938,8.439825,8.464175,8.452718,8.442539,8.432975,8.445812,8.462679,8.44711,8.432299,8.437608,8.458748,8.459425,8.44208,8.430423,8.439682,8.463877,8.452941,8.439664,8.432938,8.449246,8.459965,8.4535,8.431659,8.43613,8.446352,8.462921,8.439465,8.434913,8.451041,8.460704,8.459388,8.438347,8.425331,8.439863,8.461064,8.451103,8.440602,8.431479,8.459847,8.46184,8.442359,8.438366,8.44262,8.465672,8.459884,8.435751,8.423815,8.452177,8.454854,8.452997,8.43659,8.434453,8.456612,8.461282,8.444135,8.432118,8.437906,8.460226,8.451879,8.441701,8.435193,8.450842,8.454475,8.448029,8.438546,8.440701,8.454618,8.458766,8.451202,8.435174,8.440763,8.465095,8.452041,8.440943,8.432777,8.444992,8.4623,8.453817,8.434354,8.439204,8.456494,8.460704,8.443874,8.427026,8.43631,8.464256,8.451979,8.439267,8.433814,8.444775,8.45817,8.448886,8.430802,8.445234,8.452718,8.463617,8.442378,8.434354,8.443036,8.457152,8.452538,8.433497,8.429063,8.447209,8.461381,8.444216,8.428026,8.439366,8.453618,8.465852,8.445812,8.432795,8.449842,8.465095,8.453979,8.440304,8.427827,8.450743,8.464337,8.449905,8.436851,8.434534,8.457649,8.46376,8.443477,8.430938,8.442639,8.457667,8.450283,8.435832,8.431199,8.452699,8.459946,8.448048,8.437546,8.436391,8.45809,8.454593,8.444117,8.431758,8.439204,8.458549,8.460965,8.434075,8.43046,8.446073,8.456251,8.451202,8.436751,8.434155,8.450364,8.463679,8.445533,8.43156,8.437167,8.460425,8.453997,8.431541,8.433156,8.447191,8.459524,8.451842,8.437689,8.437708,8.451041,8.460443,8.446371,8.432659,8.435174,8.459027,8.461623,8.440682,8.43182,8.443837,8.458468,8.454835,8.439366,8.436211,8.453339,8.46843,8.44162,8.427188,8.43723,8.46166,8.464995,8.444793,8.427368,8.449724,8.458108,8.454196,8.439204,8.440682,8.454258,8.463039,8.439384,8.429982,8.444495,8.455872,8.450463,8.442819,8.431938,8.454935,8.463778,8.446731,8.432218,8.437068,8.457388,8.459984,8.441602,8.43174,8.448985,8.452618,8.456431,8.438006,8.436329,8.448905,8.456152,8.442179,8.434913,8.433317,8.452997,8.459046,8.44575,8.427268,8.439583,8.460245,8.463138,8.437068,8.433137,8.439664,8.453537,8.447029,8.429703,8.434453,8.454854,8.457152,8.445452,8.430162,8.444216,8.458009,8.454637,8.437049,8.427846,8.45178,8.458369,8.456351,8.437211,8.440304,8.4516,8.461921,8.447948,8.437546,8.440304,8.458667,8.452357,8.440322,8.440999,8.448408,8.455773,8.448787,8.430522,8.437627,8.449606,8.451581,8.448867,8.430181,8.451842,8.463319,8.455133,8.436969,8.429783,8.456512,8.463281,8.449805,8.422735,8.434751,8.450203,8.459884,8.442278,8.436969,8.444595,8.45717,8.460543,8.43695,8.432876,8.444315,8.455872,8.450184,8.441602,8.445713,8.456133,8.458009,8.44126,8.430125,8.444415,8.460723,8.45278,8.444533,8.437608,8.447209,8.46258,8.443278,8.432858,8.440682,8.455196,8.462499,8.443937,8.429361,8.443378,8.463778,8.456593,8.439943,8.43082,8.4525,8.460623,8.454196,8.435932,8.435634,8.454475,8.457847,8.443756,8.430262,8.440583,8.465194,8.456152,8.438726,8.431758,8.450942,8.455034,8.458649,8.429342,8.437509,8.445713,8.463679,8.442837,8.427927,8.44647,8.453177,8.458307,8.435571,8.428945,8.445352,8.456152,8.449724,8.43659,8.437167,8.452438,8.459785,8.438807,8.431081,8.444694,8.461182,8.45196,8.434553,8.434516,8.446452,8.458468,8.456351,8.423455,8.437726,8.453078,8.462201,8.449445,8.440204,8.442837,8.459505,8.460704,8.446172,8.439844,8.444676,8.45809,8.454258,8.428647,8.432497,8.460325,8.459127,8.444793,8.433056,8.44062,8.462201,8.458568,8.438825,8.437906,8.448985,8.456233,8.447768,8.434255,8.43649,8.451842,8.463517,8.443297,8.434534,8.448327,8.46276,8.454096,8.438347,8.434534,8.448507,8.456152,8.446389,8.432677,8.434317,8.456413,8.458829,8.447029,8.438347,8.446532,8.466473,8.453177,8.434615,8.437906,8.451041,8.462201,8.450463,8.424772,8.4418,8.449886,8.459307,8.444036,8.429603,8.433218,8.462859,8.449066,8.443756,8.43613,8.449346,8.4525,8.450165,8.433038,8.435869,8.455854,8.456431,8.444495,8.434255,8.445514,8.458189,8.457729,8.435112,8.425113,8.451401,8.465473,8.449526,8.437347,8.439863,8.449985,8.462741,8.448644,8.439465,8.441521,8.460064,8.452898,8.439384,8.430839,8.446452,8.455556,8.451202,8.434075,8.437608,8.457512,8.462362,8.448029,8.429405,8.453836,8.464716,8.459605,8.442899,8.434714,8.448687,8.452997,8.449085,8.429703,8.438546,8.456512,8.45681,8.446948,8.435391,8.437248,8.460524,8.450923,8.442396,8.437627,8.450283,8.460921,8.450463,8.428846,8.435671,8.457251,8.456314,8.446191,8.425871,8.443576,8.459686,8.455773,8.434615,8.440421,8.449327,8.458568,8.449985,8.431199,8.435292,8.452401,8.455972,8.44683,8.433516,8.445713,8.45781,8.450004,8.433795,8.435491,8.448569,8.463058,8.452438,8.435851,8.437528,8.459127,8.460704,8.443955,8.440061,8.434236,8.463157,8.455016,8.438186,8.43156,8.451761,8.455494,8.446011,8.43074,8.438086,8.44711,8.464238,8.446551,8.425691,8.441682,8.462101,8.455773,8.443117,8.425051,8.453159,8.459605,8.445253,8.437546,8.439763,8.451283,8.464697,8.444352,8.435292,8.442378,8.460903,8.461803,8.438329,8.432019,8.454556,8.457909,8.451302,8.429144,8.435292,8.451761,8.459928,8.439844,8.429783,8.439664,8.460524,8.458847,8.433795,8.43723,8.443477,8.461741,8.445812,8.434733,8.436689,8.454096,8.456431,8.444576,8.432957,8.447768,8.460803,8.453935,8.443197,8.441241,8.449004,8.458928,8.445694,8.428305,8.435391,8.457251,8.452916,8.449004,8.434895,8.443955,8.468007,8.460307,8.441421,8.430361,8.450103,8.457909,8.446669,8.43174,8.440322,8.454556,8.456711,8.445154,8.429504,8.444415,8.456531,8.452618,8.44198,8.442359,8.450463,8.465076,8.455953,8.439546,8.436869,8.453556,8.466672,8.447886,8.428945,8.449426,8.454475,8.456891,8.43613,8.432218,8.445632,8.465014,8.451463,8.43146,8.437428,8.458829,8.463679,8.443297,8.434336,8.441223,8.454997,8.457369,8.435273,8.434795,8.457909,8.457729,8.452618,8.443856,8.433615,8.451842,8.464536,8.43677,8.43595,8.447191,8.466492,8.454115,8.442278,8.427088,8.454854,8.459785,8.453239,8.435571,8.438049,8.45599,8.457189,8.449346,8.431001,8.445272,8.463281,8.453817,8.429703,8.435211,8.450681,8.454916,8.457053,8.434435,8.443576,8.45232,8.454034,8.446272,8.430324,8.439863,8.461822,8.463157,8.434913,8.434932,8.443775,8.461542,8.450942,8.435255,8.438627,8.457549,8.45745,8.445154,8.430541,8.4418,8.461803,8.456152,8.43595,8.438366,8.448048,8.463021,8.443458,8.43759,8.439204,8.450743,8.462561,8.444415,8.430342,8.440862,8.464455,8.45599,8.435571,8.436211,8.450283,8.461101,8.447967,8.439465,8.432299,8.457071,8.454637,8.446731,8.433895,8.449346,8.464436,8.459866,8.439583,8.438167,8.445911,8.460686,8.450165,8.434652,8.444253,8.455133,8.459226,8.440682,8.43046,8.446992,8.452997,8.459965,8.43613,8.423834,8.445793,8.458829,8.452059,8.433336,8.439384,8.454096,8.465914,8.448147,8.427566,8.445713,8.461425,8.454457,8.43713,8.432199,8.456233,8.466374,8.445253,8.439745,8.448607,8.461344,8.461164,8.441241,8.431299,8.444216,8.464536,8.458766,8.443017,8.435733,8.450085,8.460064,8.451103,8.431081,8.44108,8.454556,8.458667,8.437149,8.424672,8.446948,8.458847,8.4526,8.43713,8.436391,8.444992,8.465455,8.454277,8.439844,8.438086,8.454854,8.458208,8.448128,8.434373,8.438906,8.459245,8.452997,8.436391,8.435534,8.44711,8.456332,8.452898,8.434652,8.440322,8.453916,8.458568,8.439645,8.442198,8.442216,8.455593,8.450644,8.442701,8.429287,8.451022,8.455177,8.448228,8.437149,8.436969,8.459487,8.457288,8.444315,8.436851,8.433795,8.458568,8.453258,8.433038,8.4321,8.450265,8.46166,8.450563,8.440204,8.444054,8.453258,8.458928,8.447309,8.428305,8.443359,8.45709,8.454755,8.44657,8.422238,8.449544,8.465455,8.457369,8.435273,8.437528,8.448607,8.459127,8.452699,8.436093,8.444117,8.469448,8.454475,8.443576,8.434255,8.448228,8.459487,8.449364,8.429622,8.439863,8.456711,8.455692,8.446154,8.428125,8.447948,8.455295,8.461182,8.437267,8.429504,8.449706,8.462282,8.44647,8.436211,8.435851,8.456332,8.456891,8.44208,8.436149,8.445551,8.461642,8.449327,8.439304,8.433056,8.450383,8.467889,8.451519,8.432597,8.440024,8.456152,8.451581,8.443396,8.434814,8.449886,8.456133,8.453817,8.437248,8.444154,8.442539,8.460903,8.452699,8.43577,8.446551,8.459406,8.456314,8.442278,8.43046,8.447489,8.464455,8.448886,8.446793,8.433814,8.454196,8.457909,8.451122,8.433038,8.442061,8.450644,8.465734,8.439186,8.429342,8.440502,8.459307,8.455133,8.437807,8.432758,8.451122,8.465554,8.453537,8.433975,8.433354,8.459766,8.461679,8.446371,8.434534,8.448408,8.460704,8.45717,8.440421,8.430262,8.451401,8.462282,8.449606,8.426728,8.438167,8.465095,8.46258,8.44208,8.430802,8.440962,8.459667,8.45691,8.441819,8.430162,8.442856,8.455692,8.457233,8.429982,8.436788,8.453817,8.45745,8.437049,8.434155,8.44675,8.460984,8.454637,8.442899,8.429603,8.449327,8.462679,8.442918,8.437888,8.434273,8.449563,8.459127,8.442539,8.433137,8.438664,8.464455,8.459667,8.441521,8.428964,8.445154,8.460803,8.448787,8.435832,8.433553,8.459207,8.460226,8.444135,8.434832,8.442359,8.458288,8.44765,8.443458,8.429585,8.447091,8.466275,8.448526,8.428206,8.440583,8.456711,8.464175,8.445731,8.426169,8.446948,8.465275,8.456711,8.446452,8.433336,8.448408,8.454556,8.446054,8.426709,8.434453,8.455196,8.455115,8.44665,8.440043,8.445595,8.458847,8.448147,8.433714,8.43577,8.447489,8.458549,8.450203,8.433957,8.434255,8.457431,8.459568,8.451122,8.43631,8.446632,8.457611,8.459884,8.44098,8.437906,8.449526,8.454115,8.451122,8.432118,8.433336,8.460263,8.464797,8.447588,8.429603,8.448967,8.459568,8.455593,8.434336,8.434814,8.446073,8.460245,8.455133,8.433975,8.434453,8.450265,8.457928,8.445234,8.429603,8.44693,8.466852,8.45763,8.437267,8.431379,8.44693,8.463896,8.455016,8.434112,8.436528,8.460803,8.456792,8.445694,8.429622,8.44793,8.45681,8.458766,8.437826,8.429703,8.447687,8.455792,8.447209,8.433497,8.443117,8.450644,8.455475,8.452438,8.432038,8.442576,8.459307,8.456891,8.438664,8.437149,8.458108,8.459866,8.444874,8.437049,8.44244,8.455295,8.458847,8.441278,8.432777,8.435913,8.459505,8.45827,8.436509,8.437068,8.448967,8.46284,8.446849,8.434895,8.440043,8.453637,8.456792,8.454016,8.433516,8.44765,8.462921,8.454637,8.442198,8.434634,8.451581,8.457108,8.450581,8.429125,8.438527,8.447669,8.465473,8.445992,8.430982,8.445812,8.459127,8.459344,8.435851,8.433534,8.450184,8.455593,8.452979,8.432975,8.433677,8.450184,8.463517,8.445551,8.431361,8.435453,8.456233,8.452861,8.439484,8.43046,8.450184,8.46312,8.45332,8.437969,8.439546,8.456332,8.460903,8.439366,8.434354,8.446091,8.458649,8.455655,8.443415,8.436689,8.45242,8.468871,8.444036,8.436391,8.438428,8.452718,8.462282,8.448687,8.435553,8.437969,8.458071,8.453718,8.436689,8.437987,8.451122,8.460524,8.452879,8.43613,8.435652,8.457351,8.457549,8.451942,8.432137,8.443396,8.45845,8.45132,8.443738,8.430883,8.446011,8.463238,8.443197,8.422536,8.439682,8.453637,8.459406,8.450861,8.427529,8.444676,8.455295,8.45132,8.442477,8.431578,8.451581,8.460145,8.453817,8.432677,8.431001,8.453916,8.460182,8.450743,8.428107,8.443117,8.466194,8.457288,8.44216,8.429504,8.450625,8.466852,8.455214,8.427728,8.443297,8.450942,8.454096,8.445533,8.430721,8.445054,8.458369,8.457251,8.437807,8.434273,8.449265,8.459226,8.447669,8.435273,8.435851,8.452798,8.46843,8.449165,8.427287,8.446948,8.45278,8.456612,8.434354,8.437608,8.453916,8.458667,8.44747,8.432858,8.436329,8.459425,8.450085,8.441241,8.431199,8.444514,8.468169,8.458667,8.437528,8.434273,8.444396,8.459406,8.445893,8.436112,8.440962,8.456152,8.466095,8.444955,8.43613,8.442756,8.456891,8.45817,8.437869,8.432497,8.444235,8.460803,8.450842,8.436888,8.439484,8.450085,8.465635,8.446371,8.43192,8.444135,8.464256,8.453637,8.438726,8.437347,8.449228,8.457549,8.447687,8.437329,8.435832,8.466952,8.470845,8.443694,8.427566,8.443235,8.460462,8.458388,8.435491,8.434553,8.454854,8.453258,8.455053,8.433236,8.440322,8.450283,8.462778,8.440384,8.434155,8.441701,8.45809,8.454674,8.435012,8.440782,8.447967,8.46312,8.455674,8.428044,8.43659,8.450923,8.460164,8.446272,8.431541,8.44657,8.463319,8.449265,8.445433,8.433516,8.443937,8.451022,8.448029,8.437049,8.443676,8.459866,8.458369,8.446551,8.428187,8.444334,8.45599,8.456413,8.434615,8.434895,8.450625,8.456612,8.445036,8.432019,8.438267,8.454835,8.452302,8.442999,8.436987,8.445812,8.46384,8.450383,8.43082,8.430044,8.451581,8.464778,8.444297,8.434093,8.439384,8.456053,8.456332,8.444235,8.424194,8.440682,8.460425,8.45214,8.438329,8.430721,8.450923,8.458009,8.447948,8.43759,8.439583,8.45817,8.46861,8.438825,8.428647,8.437888,8.458369,8.450482,8.429982,8.433137,8.445154,8.465194,8.445234,8.433336,8.441539,8.453357,8.459127,8.434534,8.429324,8.445893,8.465095,8.454755,8.432895,8.431119,8.447948,8.460307,8.450824,8.438807,8.433634,8.453798,8.45709,8.442017,8.43631,8.44629,8.457549,8.453277,8.434354,8.432975,8.445533,8.460822,8.458406,8.425989,8.439863,8.456773,8.458766,8.440701,8.429783,8.447967,8.46366,8.457251,8.440521,8.433814,8.455494,8.4526,8.450563,8.433156,8.448706,8.457531,8.45178,8.444793,8.436509,8.439745,8.457531,8.456053,8.440341,8.429423,8.455773,8.451401,8.446849,8.42992,8.441539,8.458208,8.455196,8.443955,8.435093,8.4409,8.45717,8.451519,8.43595,8.439186,8.445613,8.456233,8.450544,8.434354,8.440123,8.458208,8.464256,8.444315,8.437627,8.439285,8.454177,8.452122,8.437528,8.428504,8.450842,8.464598,8.452519,8.428585,8.440123,8.453239,8.45763,8.444396,8.434615,8.439204,8.453718,8.452879,8.441999,8.433777,8.453059,8.456729,8.453059,8.430181,8.437447,8.454196,8.457251,8.437167,8.434453,8.443477,8.452041,8.459406,8.434137,8.431218,8.447551,8.45745,8.441881,8.434634,8.435689,8.455674,8.45799,8.44683,8.432497,8.447967,8.457251,8.458071,8.438465,8.434553,8.449085,8.455214,8.446272,8.43623,8.437708,8.45681,8.456891,8.443477,8.436211,8.439484,8.457829,8.452159,8.444433,8.434634,8.451563,8.460623,8.449426,8.432659,8.438068,8.449985,8.464517,8.442458,8.425989,8.44683,8.463399,8.459884,8.435553,8.432218,8.446209,8.455413,8.444974,8.435671,8.448805,8.451861,8.456332,8.439484,8.431199,8.442458,8.46312,8.459207,8.438186,8.434814,8.452997,8.453078,8.444495,8.432137,8.43531,8.454637,8.466871,8.443216,8.431081,8.446433,8.448228,8.455115,8.437987,8.435571,8.453618,8.459505,8.44683,8.428964,8.44262,8.460524,8.460145,8.448905,8.433038,8.437807,8.459586,8.453916,8.439844,8.437708,8.449724,8.457568,8.457909,8.43559,8.44108,8.447911,8.460884,8.432516,8.433398,8.446551,8.461362,8.457909,8.443576,8.434795,8.445812,8.456053,8.450923,8.434696,8.4419,8.457251,8.464517,8.44657,8.428107,8.439105,8.456593,8.451681,8.431442,8.429324,8.452041,8.463219,8.44657,8.433156,8.438167,8.455233,8.457649,8.452699,8.438546,8.444694,8.456152,8.451221,8.436112,8.426529,8.447489,8.467989,8.45314,8.430982,8.444315,8.456612,8.461064,8.446371,8.429901,8.4419,8.463958,8.450463,8.439223,8.434255,8.448967,8.466573,8.448228,8.427448,8.438384,8.451302,8.454835,8.450103,8.433416,8.444197,8.454295,8.456351,8.434571,8.428485,8.448985,8.459226,8.448867,8.432597,8.435652,8.456214,8.463039,8.442999,8.431019,8.44747,8.455674,8.454755,8.445154,8.432118,8.448246,8.464716,8.446172,8.43659,8.440763,8.45214,8.455152,8.44098,8.429901,8.447271,8.455413,8.455574,8.437969,8.430081,8.452339,8.4623,8.44208,8.434056,8.441241,8.456792,8.466393,8.449805,8.431442,8.448985,8.46266,8.447011,8.435751,8.440682,8.445054,8.460443,8.45681,8.442918,8.440241,8.459487,8.45699,8.4428,8.431839,8.443315,8.457388,8.453277,8.441043,8.437428,8.4526,8.456972,8.439105,8.431162,8.43623,8.454835,8.460145,8.445632,8.427188,8.444694,8.46276,8.457251,8.436093,8.434832,8.449724,8.460822,8.450364,8.433137,8.439223,8.45232,8.459505,8.444514,8.428864,8.448588,8.462021,8.454494,8.439645,8.431199,8.4419,8.457729,8.448327,8.429504,8.435472,8.455692,8.454755,8.44611,8.436112,8.445694,8.463995,8.455674,8.442539,8.426529,8.450165,8.457431,8.441881,8.433255,8.435193,8.454438,8.45717,8.445433,8.429783,8.447489,8.460822,8.457288,8.44144,8.436391,8.449346,8.455692,8.451122,8.426846,8.43146,8.458127,8.467231,8.436888,8.428225,8.443297,8.45727,8.454078,8.440602,8.44226,8.447209,8.460245,8.44783,8.43146,8.431659,8.453159,8.459046,8.443856,8.429783,8.442918,8.458406,8.453177,8.434354,8.432199,8.446452,8.457531,8.453177,8.429423,8.440024,8.452979,8.463877,8.44308,8.431578,8.44693,8.447389,8.453916,8.436608,8.434236,8.44729,8.46166,8.448147,8.431758,8.440763,8.455016,8.457152,8.445731,8.427746,8.442458,8.456593,8.454196,8.432559,8.43146,8.44757,8.455214,8.454277,8.426132,8.44226,8.459027,8.452519,8.440285,8.43174,8.444216,8.464256,8.454196,8.439384,8.433156,8.450184,8.460884,8.445911,8.428107,8.443676,8.449165,8.454177,8.440782,8.436192,8.445334,8.464238,8.455034,8.434814,8.43659,8.44711,8.45863,8.446209,8.433994,8.439304,8.456711,8.459027,8.449246,8.429964,8.445352,8.458766,8.453357,8.441341,8.432479,8.447489,8.46715,8.443937,8.429262,8.439664,8.454674,8.461263,8.438906,8.432876,8.441819,8.462362,8.456692,8.439006,8.434913,8.444415,8.457847,8.453357,8.427368,8.437788,8.463138,8.466095,8.436751,8.432858,8.443856,8.461083,8.451482,8.439484,8.436211,8.454214,8.459406,8.444775,8.429523,8.438105,8.45717,8.461344,8.444893,8.429225,8.444098,8.461642,8.460741,8.447489,8.433975,8.442819,8.455972,8.447408,8.435391,8.433516,8.45232,8.458748,8.444197,8.425753,8.44198,8.460046,8.454134,8.432659,8.427709,8.443955,8.456593,8.442837,8.434832,8.435093,8.450184,8.464076,8.443017,8.435851,8.441179,8.455332,8.459965,8.437068,8.434814,8.447849,8.460046,8.452202,8.424474,8.438906,8.46312,8.462381,8.443135,8.434814,8.434634,8.459866,8.451681,8.43649,8.433677,8.451482,8.460803,8.444017,8.433795,8.437347,8.455295,8.460642,8.443117,8.426908,8.437807,8.4623,8.456711,8.439943,8.439043,8.449588,8.451861,8.449147,8.429982,8.438167,8.456531,8.45809,8.448948,8.42992,8.448228,8.460263,8.460965,8.432677,8.43723,8.447389,8.461064,8.45096,8.436888,8.440881,8.454475,8.460226,8.443197,8.426051,8.450743,8.456792,8.458009,8.437969,8.428864,8.445514,8.464977,8.4525,8.429305,8.438347,8.460505,8.462381,8.435832,8.433218,8.447029,8.457649,8.45278,8.44216,8.430243,8.451979,8.461921,8.44711,8.42625,8.437167,8.45224,8.459226,8.441701,8.434932,8.45232,8.459406,8.452357,8.435193,8.426989,8.454295,8.461561,8.448147,8.436689,8.434534,8.458108,8.46212,8.443719,8.427287,8.442999,8.461182,8.46312,8.437546,8.434255,8.44647,8.462282,8.447849,8.434714,8.439024,8.453537,8.465014,8.444694,8.430901,8.444694,8.461263,8.450923,8.434733,8.428125,8.454755,8.452339,8.44565,8.429703,8.446091,8.450103,8.456972,8.438366,8.42625,8.442539,8.46258,8.450184,8.434416,8.434913,8.445613,8.453016,8.450383,8.436689,8.435851,8.453618,8.461822,8.443378,8.427927,8.4516,8.455674,8.4525,8.44198,8.438825,8.451662,8.454556,8.448309,8.435913,8.441819,8.462201,8.459586,8.447389,8.432597,8.450482,8.465113,8.460704,8.437627,8.425871,8.450004,8.450463,8.44729,8.432497,8.440241,8.456071,8.4623,8.445272,8.432677,8.441341,8.460723,8.456053,8.439565,8.44198,8.444334,8.45763,8.437329,8.434453,8.443576,8.461822,8.459226,8.44226,8.42579,8.44683,8.465374,8.451085,8.440142,8.434932,8.451122,8.463058,8.453339,8.433416,8.436571,8.459406,8.458226,8.445613,8.429206,8.442198,8.460524,8.455475,8.433398,8.427846,8.445595,8.457568,8.451842,8.429603,8.436211,8.458667,8.456314,8.446272,8.432317,8.448029,8.459425,8.451302,8.433814,8.434634,8.449923,8.461921,8.451879,8.437509,8.444396,8.451004,8.461263,8.439745,8.432938,8.444216,8.462462,8.452339,8.436671,8.435112,8.448128,8.466312,8.448967,8.434056,8.443576,8.455494,8.459388,8.440502,8.427548,8.445992,8.463319,8.45296,8.431262,8.434174,8.45717,8.459505,8.450463,8.430622,8.437149,8.457909,8.45709,8.442098,8.430063,8.445073,8.460282,8.444415,8.4321,8.433156,8.455034,8.457288,8.441241,8.434174,8.442639,8.456593,8.466374,8.441819,8.436689,8.441341,8.460425,8.455332,8.44126,8.429324,8.445533,8.458729,8.44747,8.426169,8.440384,8.456413,8.453277,8.441179,8.434255,8.442639,8.458947,8.45178,8.432758,8.431541,8.451202,8.459307,8.449184,8.433516,8.442322,8.460164,8.464896,8.443396,8.429883,8.446191,8.459487,8.457531,8.435012,8.434634,8.449563,8.456133,8.449905,8.429964,8.446352,8.468349,8.456972,8.441521,8.427088,8.439583,8.455295,8.455214,8.440123,8.44116,8.456332,8.459406,8.450662,8.432038,8.434056,8.461083,8.462878,8.441819,8.432578,8.433156,8.462021,8.451761,8.439565,8.435193,8.458189,8.459605,8.445992,8.436788,8.440484,8.456829,8.463877,8.442676,8.43082,8.440819,8.455773,8.459984,8.439006,8.440204,8.451761,8.454376,8.443396,8.429206,8.438086,8.458568,8.460164,8.443676,8.428287,8.450463,8.460884,8.447805,8.431199,8.432118,8.455196,8.458369,8.452798,8.423294,8.436112,8.455034,8.458487,8.440521,8.436851,8.442179,8.455755,8.456133,8.439285,8.434075,8.454277,8.46194,8.449625,8.428964,8.437347,8.456332,8.456332,8.435913,8.431659,8.449724,8.455034,8.449743,8.440583,8.433696,8.45278,8.458729,8.450743,8.426231,8.441142,8.459307,8.457947,8.448246,8.429063,8.44144,8.457909,8.449184,8.436031,8.430423,8.452457,8.46266,8.45196,8.433634,8.444135,8.458288,8.460623,8.443595,8.429684,8.444036,8.460462,8.450165,8.434453,8.432199,8.445073,8.459207,8.44747,8.428783,8.434255,8.460145,8.458108,8.442918,8.428927,8.445533,8.45096,8.452618,8.434596,8.440322,8.449327,8.464039,8.44675,8.432858,8.439763,8.45178,8.44693,8.444036,8.435093,8.44216,8.461362,8.450563,8.440043,8.439484,8.451122,8.456214,8.452059,8.431199,8.435472,8.459803,8.462958,8.442539,8.429225,8.442639,8.461542,8.44565,8.439565,8.441701,8.452438,8.462958,8.45178,8.432938,8.443937,8.457531,8.456512,8.447489,8.430162,8.448029,8.45699,8.448687,8.43623,8</t>
+  </si>
+  <si>
+    <t>11.525513,11.417976,11.315812,11.314216,11.36909,11.309366,11.376418,11.382584,11.355558,11.355198,11.276409,11.384541,11.313496,11.360905,11.356297,11.367512,11.330226,11.378753,11.388633,11.996066,11.423286,11.468143,11.564656,11.662808,11.762476,11.889114,11.863125,11.844581,11.901789,11.900311,11.850847,11.911931,11.905323,11.846997,12.334641,12.319091,11.754893,11.722973,11.773555,11.753253,11.663249,11.481134,11.432508,11.378355,11.297846,11.303597,11.276868,11.352819,11.323178,11.813778,11.344497,11.214306,11.335834,11.348851,11.347832,11.323141,11.25553,11.278185,11.24904,11.359309,11.363122,11.356874,11.408773,11.459498,11.5723,11.650909,11.716644,11.874185,11.848133,11.839408,11.804575,11.809586,11.822442,11.85045,11.809307,11.806873,11.793179,11.833638,11.787546,11.727506,11.757905,11.749621,11.6261,11.535772,11.455964,11.369748,11.310782,11.296169,11.285829,11.257865,11.256287,11.245606,11.311179,11.24904,11.305311,11.31108,11.306472,11.290382,11.292338,11.318147,11.290661,11.331742,11.394881,11.343479,11.370649,11.453828,11.510881,11.566991,11.66215,11.813201,11.85402,12.030682,11.809487,11.880929,11.89117,11.862945,11.862864,11.914644,11.833583,11.845699,11.866335,11.767046,11.840426,11.823181,11.607214,11.604438,11.398594,11.374101,11.260597,11.233291,11.249779,11.256784,11.300442,11.293915,11.243352,11.223131,11.288587,11.318129,11.321662,11.274732,11.275191,11.262355,11.340684,11.32214,11.346273,11.335654,11.293158,11.415163,11.512614,11.642327,11.700075,11.822442,11.796831,11.814337,11.844121,11.856436,11.757787,11.795235,11.810505,11.829608,11.843103,11.807233,11.732474,11.730481,11.747006,11.704808,11.652928,11.589509,11.726686,11.359191,11.393583,11.384441,11.372903,11.325755,11.352502,11.390552,11.306472,11.332102,11.35847,11.323935,11.30138,11.298765,11.283575,11.353278,11.358191,11.436682,11.423007,11.361445,11.356235,11.466683,11.523855,11.612244,11.717582,11.831266,11.783019,11.829807,11.811642,11.789664,12.314818,11.798787,11.784597,11.826851,11.822522,11.794955,11.760321,11.722494,11.705187,11.751477,11.627975,11.548348,11.433924,11.292716,11.317849,11.81276,11.262734,11.328848,11.30605,11.294493,11.267367,11.293897,11.332021,11.325656,11.293654,11.261498,11.251655,11.309925,11.357713,11.398234,11.85961,11.356794,11.428199,11.538765,11.544417,11.708341,11.775033,11.883904,11.882047,11.875998,11.820746,11.879812,11.878017,11.857275,11.867975,11.893766,11.874322,11.883084,11.749341,11.723252,11.778684,11.727624,11.639253,11.546652,11.421492,11.303939,11.287227,11.261634,11.274912,11.256946,11.792837,11.348391,11.241035,11.252574,11.301461,11.33879,11.297908,11.294754,11.318588,11.278383,11.320364,11.348031,11.328829,11.345417,11.390589,11.408854,11.519663,11.655362,11.68337,11.835116,11.84378,11.773536,11.801681,11.776809,11.809388,11.835179,11.8241,11.80781,11.832682,11.790664,11.747087,11.784534,11.753316,11.78174,11.748025,11.555235,11.438557,11.378231,11.294834,11.312856,11.373822,11.314253,11.315992,11.275272,11.263752,11.250698,11.279122,11.242134,11.24922,11.277806,11.208121,11.294493,11.312838,11.267186,11.337312,11.346733,11.325612,11.421852,11.479259,11.620448,11.705006,11.808947,11.797849,11.830627,11.74972,11.763674,11.761339,11.761439,11.765991,11.747205,11.820106,11.765233,11.762476,11.799625,11.710154,11.696821,11.61384,11.495468,11.442929,11.289425,11.267006,11.307789,11.244569,11.288425,11.289543,11.275651,11.276048,11.269323,11.402724,11.365258,11.38528,11.361346,11.301858,11.334356,11.377238,11.400911,11.443768,11.357154,11.470875,11.549186,11.656281,11.684687,11.810425,11.906602,11.959637,11.851325,11.881786,11.872067,11.864242,11.893964,11.87067,11.872744,11.889971,11.902789,11.8338,11.899734,11.804538,11.833701,11.717601,11.962774,11.474229,11.436818,11.367314,11.396278,11.329705,11.362644,11.378573,11.425683,11.375039,11.321681,11.288245,11.403724,11.358452,11.353701,11.898597,11.302237,11.336275,11.320843,11.34392,11.356794,11.392366,11.428857,11.573201,11.689816,11.791161,11.826913,11.815554,11.777331,11.868832,12.355619,11.865118,11.837874,11.856995,11.92173,11.847512,11.850207,11.763376,11.716166,11.796694,11.780144,11.654524,11.551819,11.474688,11.39013,11.357911,11.337952,11.295033,11.279582,11.382305,11.313117,11.279284,11.326215,11.268323,11.341945,11.280483,11.278744,11.279961,11.265808,11.283774,11.803059,11.264851,11.28088,11.330326,11.461697,11.48904,11.559905,11.66682,11.791422,11.823559,11.858951,11.767189,11.735368,11.767469,11.7412,11.810505,11.738622,11.781082,11.727922,11.747105,11.719998,11.721495,11.706602,11.63516,11.449537,11.401308,11.283935,11.290021,11.272595,11.288624,11.778504,11.19752,11.363482,11.237023,11.267447,11.255449,11.314595,11.243631,11.253412,11.246345,11.265547,11.29122,11.299585,11.333896,11.328469,11.727624,11.383603,11.519743,11.587453,11.736486,11.726723,11.802898,11.78092,11.803159,11.727543,11.780262,11.706205,11.742615,11.751558,11.767307,11.763215,11.733195,11.764314,11.777268,11.751099,11.601346,11.52042,11.333201,11.320023,11.290382,11.257505,11.249761,11.278104,11.253294,11.271919,11.275589,11.237781,11.23331,11.260399,11.283376,11.291437,11.249239,11.24437,11.247183,11.329208,11.25902,11.315992,11.294033,11.448618,11.45884,11.612325,11.677079,11.853803,11.774654,11.70826,11.778846,11.851605,11.788546,11.764351,11.791223,11.776449,11.767686,11.770661,11.783895,11.787248,11.701193,11.747366,11.629372,11.538467,11.366295,11.255927,11.221454,11.211512,11.240439,11.247345,11.280979,11.271478,11.261318,11.292816,11.281358,11.275111,11.272676,11.260678,11.219895,11.273813,11.262653,11.262138,11.279383,11.272993,11.321004,11.479079,11.424286,11.546869,11.69253,11.77679,11.813499,11.753353,11.879812,11.757048,11.793757,11.85879,11.773636,11.802041,11.78605,11.743075,11.706205,11.728183,11.675564,11.754812,11.64065,11.486904,11.431211,11.337213,11.281638,11.271279,11.239836,11.250897,11.187938,11.226944,11.280222,11.20329,11.282277,11.210096,11.278563,11.291419,11.239358,11.240439,11.272695,11.241675,11.413586,11.409674,11.409953,11.464466,11.560824,11.684885,11.716644,11.863783,11.839209,11.808947,12.357197,11.874682,11.81248,11.819926,11.858293,11.753514,11.823199,11.792378,11.749621,11.748584,11.780802,11.831682,11.663907,11.518265,11.475328,11.357172,11.302479,11.307789,11.351763,11.28645,11.272676,11.299865,11.272776,11.339827,11.30138,11.352863,11.282277,11.302417,11.341982,11.369288,11.861566,11.346615,11.40999,11.297107,11.300703,11.336374,11.436862,11.604221,11.69307,11.691394,11.778386,11.743174,11.732834,11.78695,11.738983,12.28268,11.746249,11.682072,11.733393,11.807748,11.696523,11.746168,11.656381,11.651369,11.562302,11.531599,11.336672,11.262075,11.263311,11.21317,11.742038,11.245668,11.228441,11.231695,11.20796,11.200333,11.296971,11.355017,11.313838,11.289841,11.238501,11.271478,11.237582,11.293474,11.31154,11.341243,11.346453,11.438936,11.515291,11.585075,11.678458,11.801221,11.808667,11.809686,11.777728,11.762656,11.816933,11.778188,11.788329,11.777927,11.788528,11.765531,11.731779,11.715346,11.691195,11.748025,11.591943,11.47367,11.380268,11.344795,11.275589,11.274831,11.210754,11.229298,11.288326,11.306112,11.245966,11.271378,11.258343,11.285612,11.275409,11.346814,11.345255,11.341784,11.331245,11.324656,11.338088,11.374381,11.41035,11.485208,11.514272,11.664845,11.777088,11.817014,11.864721,11.871347,11.827174,11.837712,11.889475,11.84532,11.866497,11.842823,11.787149,11.833881,11.782137,11.759961,11.747385,11.737685,11.583938,11.52078,11.393266,11.348708,11.318787,11.299225,11.328009,11.290599,11.332841,11.267367,11.31236,11.322718,11.305752,11.313415,11.331742,11.28509,11.260858,11.326053,11.334536,11.323078,11.335834,11.394403,11.40668,11.500759,11.548546,11.692971,11.776151,11.83334,11.865081,11.868236,11.802898,11.901789,11.842842,11.865379,11.8445,11.814598,11.854921,11.81312,11.837731,11.757824,11.77543,12.005513,11.729382,11.645643,11.47924,11.417635,11.444426,11.338989,11.295791,11.2904,11.334518,11.267584,11.253953,11.294294,11.328928,11.351006,11.355856,11.27154,11.328829,11.351645,11.342342,11.295232,11.363879,11.400029,11.367413,11.496648,11.574418,11.633222,11.742715,11.840948,11.820026,12.395644,11.815275,11.848251,11.814058,11.838191,11.899057,11.822063,11.852424,11.828292,12.13217,11.800923,11.853983,11.851307,11.711875,11.600408,12.013374,11.451394,11.355576,11.359849,11.360985,11.324755,11.388354,11.392366,11.370847,11.373344,11.368351,11.334356,11.402786,11.381007,11.364059,11.878874,11.393943,11.378852,11.448618,11.409034,11.451692,11.547248,11.639352,11.721836,11.83911,11.91139,11.899274,11.928319,11.925506,11.870012,11.968841,11.90151,11.897417,11.892828,11.945385,11.904242,11.850946,11.793216,11.809208,11.768046,11.699895,11.552738,11.429795,11.367494,11.324836,11.836154,11.294114,11.328108,11.324954,11.312242,11.292437,11.335157,11.347751,11.303137,11.344677,11.346336,11.298647,11.312099,11.342162,11.329965,11.344677,11.336853,11.424224,11.494909,11.59362,11.671949,11.802401,11.857554,11.860808,11.878135,12.421913,11.842445,11.94387,11.780324,11.914148,11.896182,11.888276,11.910434,11.848071,11.766829,11.835216,11.821883,11.725568,11.595216,11.492096,11.392546,11.368053,11.354999,11.360669,11.322402,11.309385,11.298846,11.299703,11.285053,11.266069,11.395601,11.341442,11.300361,11.300442,11.300641,11.303895,11.356874,11.315272,11.346814,11.405283,11.469757,11.5529,11.658815,12.384484,11.843121,11.856797,11.853822,11.888853,11.8757,11.881929,11.839551,11.878495,11.889114,11.819827,11.868174,11.795533,11.779063,11.811362,11.779026,11.701914,11.563997,11.418896,11.340846,11.324898,11.302976,11.402966,11.288966,11.326972,11.403345,11.344038,11.367115,11.367214,11.391266,11.360129,11.360228,11.344218,11.379511,11.330524,11.421988,11.420094,11.461175,11.427019,11.491835,11.584038,11.659256,11.785932,11.86428,11.89656,11.867615,11.875042,11.88622,11.912688,11.875303,11.85584,11.840029,11.884444,11.844239,11.790204,11.700634,12.167959,11.782659,11.67239,11.571903,11.473968,11.371406,11.360768,11.345975,11.361824,11.325656,11.304435,11.365059,11.324674,11.335474,11.298206,11.875998,11.3538,11.303814,11.339927,11.349788,11.963451,11.410133,11.439936,11.446444,11.481016,11.514471,11.597135,11.69207,11.815176,11.908136,12.437321,11.911869,11.924488,11.896759,11.877017,11.795992,11.854281,11.834899,11.830086,11.83408,11.814977,11.774853,11.790024,11.790043,11.699399,11.581504,11.429695,11.379691,11.335555,11.339846,11.323438,11.281439,11.346733,11.264951,11.315974,11.300163,11.31693,11.336374,11.907261,11.293474,11.87552,11.331263,11.354558,11.38033,11.399352,11.380647,11.412387,11.481414,11.603103,11.681911,11.801923,11.847313,11.873365,11.888295,11.860069,11.931077,11.939976,11.923848,11.857057,11.893145,11.851325,11.82895,11.791142,11.750062,11.76124,11.793937,11.624063,11.531338,11.456902,11.31162,11.76645,11.307609,11.309826,11.257902,11.304435,11.342442,11.341802,11.284612,11.352123,11.350726,11.322519,11.324917,11.303914,11.340144,11.27539,11.737225,11.407258,11.376697,11.356874,11.497865,11.564575,11.668478,11.744292,11.846276,11.835216,11.797191,11.879929,11.848233,11.884724,11.905702,11.847872,11.821746,11.849928,11.844401,11.794415,11.74944,11.780721,11.75988,11.674284,11.564395,11.423647,11.387714,11.358371,11.325475,11.89153,11.373623,11.34392,11.364637,11.367034,11.323078,11.367413,11.39616,11.379871,11.364799,11.383342,11.366575,11.421672,11.413027,11.445643,11.39626,11.479321,11.54723,11.627596,11.702554,11.827012,11.909695,11.899933,11.906341,11.923587,11.921811,11.937063,11.912229,11.842904,11.914347,11.913347,11.863504,11.845916,11.810884,11.824398,11.809009,11.695784,11.608531,11.733871,11.394999,11.382206,11.403327,11.335455,11.388273,11.38967,11.351565,11.318327,11.369189,11.396079,11.40596,11.340026,11.382467,11.334039,11.430732,11.300883,11.326215,11.381827,11.417318,11.353421,11.464628,11.591484,11.664224,11.751937,11.881631,11.885202,11.878216,11.868236,11.857635,11.845754,11.881768,11.80242,11.854002,11.881768,11.826255,11.808351,11.789484,11.757526,11.789844,11.70305,11.530705,11.433986,11.383143,11.349528,11.297846,11.250518,11.354738,11.347373,11.339827,11.335635,11.342883,11.370288,11.339088,11.319905,11.344615,11.337511,11.300821,11.322979,11.256027,11.335393,11.300802,11.295331,11.422349,11.54146,11.635881,11.759923,12.367059,11.789105,11.773896,11.847574,11.761538,11.805314,11.774213,11.753415,11.793856,12.307931,11.791521,11.734989,11.766767,11.719656,11.721377,11.642227,11.490139,11.408935,11.316912,11.374679,11.306671,11.296449,11.258163,11.298486,11.242594,11.256946,11.28152,11.285351,11.244749,11.27018,11.857815,11.276769,11.243153,11.294493,11.2592,11.322023,11.303336,11.385298,11.389968,11.460796,11.649114,11.730058,11.804656,11.805593,11.810822,12.273756,11.808071,12.44573,11.934306,11.887258,11.888493,11.881606,11.864503,11.81861,11.818889,11.814617,11.814517,11.676781,11.566071,11.427838,11.836297,11.326115,11.324755,11.300262,11.277166,11.294573,11.292139,11.304535,11.314216,11.332859,11.308087,11.295151,11.303994,11.335176,11.355595,11.307292,11.338051,11.379132,11.35398,11.37045,11.514912,11.570605,11.644742,11.733791,11.868534,11.843121,11.825994,11.872825,11.892387,11.861845,11.84386,11.831285,11.892387,11.867137,11.803898,11.812462,11.808829,11.800364,11.762296,11.691673,11.543137,11.440414,11.388552,11.345038,11.312341,11.326891,11.30641,11.337871,11.347112,11.305572,11.302578,11.342901,11.31739,11.310962,11.330704,11.321861,11.345895,11.363681,11.346453,11.395539,11.372524,11.367873,11.487426,12.154986,11.71942,11.832223,11.922289,11.912409,11.834819,11.84963,11.876818,11.858293,11.861088,11.871707,11.857293,11.814058,11.868813,11.826354,11.750459,11.788844,11.824777,11.668795,11.536132,11.44814,11.373182,11.313937,11.344398,11.319166,11.335194,11.297747,11.283954,11.359128,11.315713,11.307149,11.349149,11.374921,11.317731,11.313018,11.310403,11.33825,11.369711,11.914247,11.407438,11.435924,11.50002,11.606276,11.680333,11.811524,11.882569,11.883283,11.85997,11.874862,11.907838,11.887158,11.917601,11.893406,11.862647,11.897778,11.922587,12.076955,11.818926,11.868931,11.820647,11.727984,11.637017,11.524811,11.421889,11.401209,11.325395,11.380448,11.365618,11.371766,11.37412,11.302939,11.347671,11.371325,11.406699,11.336213,11.365935,11.320824,11.287668,11.315514,11.341802,11.354837,11.411909,11.406438,11.507925,11.589509,11.675402,12.34005,11.847854,11.907161,11.847394,11.842904,11.8757,11.858753,11.869912,11.839352,11.860808,11.852524,11.852344,11.784876,11.769922,11.748863,12.395762,11.691151,11.526009,11.502336,11.379871,11.356297,11.347751,11.322122,11.316272,11.288804,11.373462,11.321762,11.332779,11.879072,11.329947,11.858094,11.326252,11.312658,11.349888,11.358731,11.317949,11.396837,11.386894,11.392465,11.495269,11.601066,11.638414,11.755489,11.852965,11.903709,11.924506,11.819548,11.889512,11.893884,11.879911,11.875719,11.892468,11.867857,11.813499,11.794676,11.799265,11.805034,11.80242,11.73471,11.520998,11.976846,11.382324,11.293276,11.291419,11.308925,11.289084,11.895064,11.383802,11.379231,11.345516,11.383342,11.384522,11.413288,11.412928,11.366395,11.375995,11.387317,11.405941,11.395999,11.466304,11.500957,11.536232,11.647817,11.736548,11.831546,11.914744,11.939218,11.943789,11.882029,11.947385,11.987006,11.868273,11.885301,11.942951,11.968524,11.923308,11.89163,11.830627,11.810046,11.84927,11.737685,11.577511,11.40999,11.334735,11.292977,11.294393,11.282476,11.315154,11.321582,11.357613,11.273452,11.253772,11.289742,11.310503,11.254331,11.23303,11.258505,11.333499,11.312297,11.357253,11.309745,11.325475,11.377815,11.450835,11.530642,11.684606,11.769425,11.824398,11.81212,11.83783,11.750919,11.826534,11.794496,11.795172,11.775095,11.849972,11.900374,11.861349,11.757346,11.774853,11.717744,11.736946,11.615797,11.559507,11.392167,11.308149,11.367115,11.279222,11.278365,11.316651,11.297567,11.292158,11.274074,11.315334,11.326332,11.293095,11.353539,11.329127,11.251096,11.269503,11.309844,11.32288,11.309565,11.349049,11.36332,11.450736,11.478942,11.636918,11.748962,11.790683,11.798389,11.773816,11.810344,11.8026,11.783199,11.810127,11.790664,11.840029,11.862125,12.098094,11.69766,11.755508,11.756769,11.778007,11.62061,11.524972,11.469099,11.428677,11.346354,11.36991,11.356135,11.365376,11.38959,11.349149,11.85412,11.314632,11.344299,11.327332,11.269621,11.292158,11.325935,11.314136,11.387335,11.344975,11.324935,11.326494,11.333238,11.425603,11.531878,12.169878,11.760501,11.848574,11.806711,11.793657,11.780423,11.808388,11.763215,11.795433,11.789745,11.813977,11.779945,11.739541,11.807829,11.697622,11.776231,11.703149,11.65684,11.585634,11.417778,11.303354,11.295611,11.287488,11.302876,11.305354,11.331922,11.293996,11.2699,11.230416,11.205345,11.82913,11.231155,11.267087,11.257225,11.252114,11.228938,11.263473,11.299883,11.283656,11.277707,11.44704,11.482352,11.595017,11.805494,11.750801,11.797911,11.785112,11.787726,11.858132,11.775231,11.765351,11.773257,11.743373,11.68786,11.770282,11.72876,11.750919,11.715446,11.682271,11.555713,11.834179,11.298883,11.265528,11.244209,11.258803,11.225124,11.232372,11.269702,11.211133,11.246525,11.200072,11.19698,11.2914,11.234192,11.233012,11.703988,11.24337,11.243333,11.269341,11.261796,11.306472,11.339566,11.428019,11.533437,11.584118,11.683289,11.836234,11.787888,11.773834,11.734511,11.787807,11.757166,11.744472,11.762178,11.77104,11.710776,11.750621,11.685444,11.663628,11.707062,11.625037,11.550962,11.488003,11.379411,11.266609,11.216163,11.230478,11.235508,11.209537,11.227683,11.253294,11.211593,11.200234,11.199495,11.313955,11.234887,11.26523,11.261138,11.261995,11.297349,11.26469,11.318029,11.262274,11.330524,11.39159,11.50433,11.568369,11.660013,11.719979,11.749223,11.746546,11.795253,11.805376,11.720917,11.733052,11.67221,11.775673,11.770543,11.745491,11.690655,11.718942,11.650773,11.69838,11.56809,11.47403,11.390012,11.296169,11.195645,11.259281,11.25004,11.223529,11.25453,11.269801,11.229298,11.288786,11.28088,11.259461,11.31236,11.220715,11.28655,11.325295,11.242612,11.298666,11.328947,11.316353,11.292257,11.3958,11.439594,11.630211,11.726047,11.761159,11.716166,11.750856,11.69866,11.747385,11.796911,11.73489,11.74441,11.709298,11.741057,11.740759,11.726624,11.685525,11.695946,11.665423,11.574238,11.460256,11.324196,11.288506,11.265168,11.253611,11.211214,11.235049,11.251437,11.272993,11.23339,11.262814,11.215325,11.278744,11.288425,11.322402,11.248841,11.229099,11.28491,11.238601,11.233291,11.2806,11.353999,11.372325,12.064497,11.590745,11.65584,11.735467,11.819467,11.745907,11.765748,11.758545,11.717762,11.783137,11.749981,11.729978,11.774933,11.807171,11.686643,11.702013,11.703609,11.701355,11.54695,11.503094,11.371388,11.27988,11.293754,11.273893,11.232732,11.240576,11.244749,11.269223,11.271099,11.264373,11.804277,11.226025,11.288363,11.230956,11.256207,11.236725,11.292977,11.21848,11.258523,11.265249,11.350366,11.423727,11.459498,11.584019,11.729319,12.346478,11.718961,11.819926,11.791782,11.759942,11.785913,11.763917,11.736405,11.767407,11.79272,11.749962,11.732934,11.705267,11.756327,11.72904,12.122966,11.479799,11.373741,11.351925,11.290642,11.251375,11.267404,11.278924,11.219417,11.253971,11.236266,11.201054,11.212431,11.272856,11.219498,11.175362,11.162228,11.22836,11.204885,11.298784,11.26459,11.248022,11.323699,11.340585,11.462373,11.607314,11.677619,11.759041,11.771319,11.751775,11.762457,11.759122,11.798209,11.738163,11.742336,11.779523,11.798129,11.754732,11.695766,11.708739,11.697641,11.659194,11.589987,11.519942,11.417418,11.309546,11.234887,11.227422,11.180753,11.204345,11.24483,11.274533,11.193509,11.215126,11.26487,11.182249,11.17063,11.20704,11.214586,11.205246,11.241197,11.268385,11.270937,11.27036,11.301641,11.383522,11.492375,11.629031,11.720836,11.828012,11.748962,11.729518,11.751216,11.764891,11.835377,11.755787,11.701814,11.727345,11.790304,11.789105,11.77058,11.734511,11.706286,11.681911,11.632248,11.47834,11.395657,11.303994,11.237005,11.285252,11.185044,11.247823,11.248121,11.289046,11.223628,11.257405,11.260939,11.201054,11.237843,11.276607,11.235608,11.261237,11.297648,11.26559,11.27639,11.299144,11.342342,11.424025,11.425801,11.582243,11.724109,11.775231,11.801302,11.78156,11.846674,11.72473,11.78146,11.74972,11.861268,12.087574,11.731356,11.747826,11.753694,11.626776,11.657057,11.656939,11.568226,11.452394,11.360309,11.281917,11.183746,11.251096,11.2289,11.223808,11.248481,11.255188,11.208121,11.252493,11.219157,11.275092,11.295033,11.226665,11.216939,11.264888,11.257884,11.260498,11.269341,11.278383,11.376058,11.976467,11.53607,11.644941,11.660554,11.789881,11.737964,11.82346,11.762395,11.787987,11.794657,11.751477,11.69884,11.707602,11.739659,11.756508,12.292921,11.659672,11.710136,11.736548,11.552918,11.454089,11.386876,11.261138,11.217623,11.243252,11.199613,11.22269,11.213008,11.220554,11.241656,11.756048,11.229018,11.250717,11.30587,11.217461,11.271838,11.310024,11.263733,11.277365,11.291878,11.3021,11.340324,11.338827,11.498902,11.55721,11.81879,11.90115,11.808866,11.683687,11.733114,11.732853,11.776629,11.81348,11.711415,11.733294,11.780821,11.761339,11.643128,11.663665,11.746447,12.19339,11.532257,11.526351,11.365718,11.261318,11.197818,11.238501,11.276707,11.257343,11.282575,11.245128,11.248841,11.2904,11.264212,11.299964,11.24383,11.292419,11.298126,11.238042,11.252574,11.251338,11.266547,11.263771,11.276328,11.453387,11.465547,11.768767,11.766928,11.864242,11.840886,11.822063,11.813859,11.82292,11.835495,11.810586,11.823181,11.885103,11.858852,11.823298,11.761817,11.779784,11.774654,11.779964,11.660852,11.510701,11.414722,11.32106,11.310764,11.326612,11.277787,11.329605,11.302876,11.30605,11.325215,11.310503,11.288605,11.283873,11.313018,11.31747,11.261237,11.338231,11.35326,11.348112,11.340107,11.463411,11.425702,11.510757,11.631167,11.765811,11.82867,11.856995,11.857734,11.895461,11.903168,11.891909,11.882308,11.843221,11.799706,11.851946,11.884562,11.797092,11.73956,11.73443,11.740659,11.722811,11.610909,11.541082,11.386019,11.26074,11.307689,11.356694,11.315812,11.298585,11.329903,11.31657,11.324854,11.241892,11.311223,11.357812,11.290003,11.317427,11.264131,11.272397,11.333977,11.372425,11.362662,11.398712,11.331363,11.524432,11.543895,11.630689,11.759184,11.8963,11.818989,11.796191,11.834458,11.8348,11.802861,11.83883,12.313421,11.819548,11.810027,11.795694,11.738063,11.6875,11.781019,11.608711,11.593819,11.555831,11.316831,11.273136,11.273154,11.256107,11.201929,11.792359,11.310801,11.277166,11.270441,11.215567,11.249419,11.776629,11.194285,11.277346,11.237402,11.266926,11.289941,11.267925,11.286009,11.335455,11.837514,11.433347,11.487922,11.627515,11.711434,11.722494,11.735809,11.72473,11.834738,11.741057,11.828391,11.761917,11.734449,11.793937,11.768984,11.751819,11.729282,11.760339,11.669813,11.702851,11.524072,11.440135,11.36927,11.2387,11.280402,11.190795,11.23906,11.201451,11.24383,11.775871,11.787608,11.268323,11.31236,11.242532,11.264851,11.308168,11.215424,11.257505,11.254052,11.203569,11.230975,11.262336,11.315353,11.413126,11.546869,11.672869,11.713813,11.771878,11.726444,11.761439,11.804277,11.755769,11.733014,11.788087,11.73938,11.762755,11.771959,11.733853,11.711254,11.729121,12.131368,11.629571,11.570586,11.47,11.398992,11.277085,11.278284,11.252114,11.247804,11.235067,11.179734,11.244351,11.19798,11.22287,11.212071,11.675663,11.250158,11.216182,11.226224,11.279464,11.273173,11.270459,11.28501,11.297107,11.307168,11.421889,11.466764,11.64478,11.747664,11.747447,11.765072,11.767326,11.768065,11.728481,11.841047,11.782976,11.780703,11.741796,11.831925,11.792459,11.743075,11.700274,11.755849,11.691313,11.525631,12.081705,11.498622,11.390589,11.378231,11.317949,11.338728,11.382467,11.369829,11.376436,11.343541,11.339188,11.370189,11.380069,11.27539,11.308826,11.23934,11.278545,11.274074,11.345696,11.308267,11.298945,11.311701,11.415083,11.56727,11.630211,11.784056,11.804357,11.793819,11.762376,11.886897,11.782516,11.852064,11.812021,11.818349,11.745311,11.794974,11.797849,11.790943,12.337635,11.778368,11.738262,11.62079,11.516589,11.475328,11.379548,11.363122,11.316831,11.29176,11.262833,11.341305,11.329289,11.250698,11.281178,11.336871,11.321221,11.340305,11.29671,11.33294,11.327829,11.361563,11.293654,11.348192,11.376517,11.388192,11.474111,11.515688,11.634583,11.725028,11.813418,11.761718,11.86995,11.806214,11.799364,11.861647,11.949018,11.834179,11.858871,11.871409,11.81879,11.774492,11.739541,11.807692,11.754154,11.637657,11.480638,11.438954,11.290102,11.311142,11.308907,11.35947,11.240836,11.310024,11.280321,11.315632,11.309664,11.292499,11.33312,11.299424,11.253971,11.275632,11.277707,11.285252,11.303237,11.400172,11.809947,11.358272,11.416561,11.58931,11.686183,11.751099,11.794775,11.872744,11.78741,11.788149,12.469881,11.903106,11.874384,11.86382,11.855579,11.901591,11.920954,11.850866,11.799066,11.830546,11.805736,11.709937,11.591825,11.538008,11.389472,11.364339,11.321203,11.36396,11.341305,11.340107,11.873185,11.369053,11.318129,11.312279,11.343199,11.273434,11.331444,11.404463,11.377256,11.373443,11.31172,11.39983,11.406159,11.44814,11.459778,12.108353,11.57412,11.772418,12.396824,11.852126,11.8543,11.952055,11.872067,11.902889,11.848512,11.873663,11.847593,11.924786,11.864162,11.789726,12.265913,11.833999,11.826056,11.750179,11.554216,11.46954,11.378473,11.354999,11.340684,11.334058,11.386515,11.35426,11.370108,11.33204,11.363563,11.34246,11.367773,11.342144,11.304516,11.292698,11.326513,11.370586,11.354918,11.422168,11.401327,11.413685,11.521358,11.589671,11.722134,11.797352,11.870428,11.885463,11.907478,11.884264,11.907938,11.948242,11.899355,11.850766,11.859212,11.859411,11.900491,11.798967,11.805873,11.743652,11.721277,11.622845,11.529903,11.394403,11.366953,11.334536,11.319725,11.249698,11.316371,11.31811,11.329506,11.296368,11.278582,11.261138,11.285811,11.292257,11.281718,11.293853,11.313577,11.330624,11.904665,11.347851,11.330245,11.425919,11.443488,11.544975,11.663286,11.792521,11.885761,11.867975,11.818771,11.824957,11.857473,11.792837,11.875241,11.854561,11.863721,11.825714,11.806314,11.777449,11.752496,11.814157,11.707882,11.618113,11.461932,11.365177,11.251195,11.328487,11.274254,11.292617,11.271776,11.242873,11.281818,11.273235,11.325395,11.366836,11.288723,11.227602,11.81843,11.273912,11.317949,11.285153,11.331822,11.335356,11.366736,11.44301,11.477123,11.567351,11.697921,11.767388,11.843103,11.84945,11.827111,11.884544,11.858392,12.157501,11.826894,11.847494,11.799327,11.878675,11.819709,11.818349,11.823261,11.780423,11.724929,11.635719,11.52106,11.454946,11.406997,11.33358,11.356315,11.335437,11.331183,11.350167,11.316073,11.338548,11.300343,11.306689,11.282457,11.345975,11.315235,11.286929,11.267565,11.288506,11.304733,11.968003,11.394502,11.389372,11.491356,11.561401,11.657976,11.807568,11.883426,11.807711,11.842004,11.844121,11.892946,11.751918,11.825894,11.820485,12.441376,11.819368,11.718439,11.757725,11.7295,11.761439,11.744671,11.645581,11.492195,11.378753,11.286009,11.344957,11.284531,11.278483,11.807351,11.813977,11.298666,11.293276,11.360805,11.276626,11.278346,11.300262,11.28555,11.315533,11.341703,11.330624,11.324097,11.360886,11.37933,11.41712,11.468261,11.534952,11.726307,11.77643,11.863323,11.803159,11.830167,11.828112,11.820007,11.822063,11.841886,11.832123,11.867037,11.885401,11.832204,12.260342,11.80314,11.780603,11.739939,11.623963,11.547311,11.44914,11.59362,11.351285,11.304156,11.347193,11.311142,11.359569,11.316011,11.305454,11.392285,11.348112,11.36432,11.32306,11.316812,11.335492,11.351645,11.423665,11.384441,11.439656,11.382106,11.454567,11.508863,11.596613,11.744329,11.810108,11.930375,11.922451,11.910074,11.866397,11.88047,11.883625,11.83452,11.867695,11.863025,11.900653,11.828689,11.841165,11.838172,11.783416,11.682252,11.634303,11.474346,11.389751,11.323917,11.318768,11.292058,11.30695,11.292276,11.329028,11.305112,11.263373,11.312918,11.283855,11.333661,11.290462,11.319824,11.235986,11.373083,11.342262,11.336555,11.374282,11.414244,11.410512,11.497424,11.561401,11.707304,11.719501,11.869111,11.797309,11.818908,11.794775,11.843084,11.825155,11.776132,11.889232,11.845239,11.819268,12.020144,11.824758,11.788248,11.820703,11.736188,11.658355,11.582243,11.481656,11.339368,11.353341,11.300063,11.329487,11.284215,11.381908,11.35344,11.366376,11.302678,11.380908,11.313396,11.383622,11.409034,11.367773,11.381746,11.369071,11.436204,11.435943,11.477141,11.464808,11.534474,11.6045,11.711794,11.828292,11.933729,11.827111,11.889754,11.858312,12.320768,11.913148,12.206965,11.849531,11.867615,11.839569,11.838091,11.824379,11.77076,11.775312,11.686643,11.613182,11.484252,11.369251,11.30138,11.889015,11.360445,11.230298,11.322501,11.270801,11.297467,11.332841,11.339467,11.305391,11.340964,11.310422,11.334275,11.298386,11.290282,11.325134,11.832204,11.360787,11.29743,11.422709,11.476564,11.618753,11.640091,11.772896,11.837253,11.798787,11.760861,11.849413,11.847754,11.815275,11.840029,11.828391,11.800464,11.817654,11.799426,11.752036,11.760321,11.739641,11.76655,11.594539,11.412766,11.374399,11.292977,11.300641,11.232912,11.239358,11.784534,11.294356,11.254368,11.288984,11.263355,11.26936,11.290121,11.276489,11.284053,11.19634,11.278085,11.294213,11.253033,11.301461,11.348329,11.339188,11.418833,11.508043,12.080246,11.777629,11.737486,11.736368,11.771002,11.722314,11.794135,11.802122,11.718303,11.743013,11.726127,11.842544,12.061765,11.68732,11.705745,11.747186,11.72409,11.537449,11.451773,11.355775,11.231794,11.243911,11.211493,11.235229,11.257604,11.220175,11.244587,11.500659,11.243072,11.26451,11.341901,11.285252,11.257884,11.26487,11.260759,11.234688,11.282575,11.262237,11.234906,11.267826,11.359886,11.4904,11.570767,11.734629,11.809388,11.771959,11.7294,11.747764,11.764333,11.809686,11.758545,11.761737,11.720656,11.693052,11.739821,11.671012,11.739063,11.717383,11.69399,11.58282,11.48419,11.426081,11.314136,11.307149,11.240656,11.239638,11.189534,11.220156,11.242693,11.273695,11.20301,11.247904,11.225646,11.236123,11.28609,11.234968,11.255368,11.240377,11.221473,11.321221,11.34474,11.32278,11.405581,11.519402,11.640253,11.679215,11.813958,11.729959,11.814399,11.758942,11.825174,11.748962,11.772238,11.842085,11.824118,11.788447,11.76463,11.74056,11.731754,11.746006,11.716526,11.56781,11.416579,11.289543,11.221932,11.296989,11.246984,11.246128,11.260219,11.263373,11.283594,11.272397,11.276967,11.285848,11.306131,11.274173,11.323737,11.245569,11.260516,11.288444,11.266069,11.366177,11.310683,11.340107,11.382963,11.51593,11.650071,11.710515,11.833918,11.785273,11.738424,11.998545,11.738622,11.780784,11.767028,11.748105,11.80827,11.762314,11.732456,11.694368,11.713949,11.680855,11.706503,11.619951,11.425261,11.366078,11.350267,11.260939,11.273775,11.211512,11.229677,11.270397,11.173325,11.213828,11.169593,11.27603,11.25389,11.30723,11.281935,11.234868,11.237303,11.809947,11.246885,11.254611,11.318247,11.334058,11.397955,11.58346,11.605339,11.674365,11.793179,11.720917,11.74487,11.693089,11.812462,11.843184,11.788267,11.726425,11.779666,11.757048,11.749602,11.70918,11.70369,11.743355,11.68786,11.55757,11.46269,11.376157,11.293437,11.287686,11.21253,11.799085,11.307348,11.320923,11.23403,11.220535,11.257784,11.277346,11.27485,11.301839,11.230875,11.263951,11.260697,11.239439,11.256188,11.319706,11.85969,11.337691,11.425404,11.492474,11.652748,11.675005,11.750341,11.802501,11.760302,11.7402,11.778765,11.796551,11.744752,11.80881,11.721016,12.257908,11.77725,11.650152,11.817852,11.745329,11.67752,11.554496,11.511397,11.328289,11.254629,11.264032,11.216343,11.236005,11.174722,11.224367,11.212269,11.207202,11.235645,11.295132,11.351304,11.240756,11.416679,11.239123,11.248382,11.247444,11.326531,11.308646,11.282277,11.270441,11.403364,11.485947,11.628993,11.68291,11.759302,11.808947,11.810804,11.855958,11.809307,11.759464,11.831123,11.73453,11.761718,11.761041,11.731437,11.701075,11.718762,11.658815,11.646519,11.561861,11.441072,11.363979,11.277247,11.246326,11.205985,11.224466,11.228242,11.248363,11.23349,11.193788,11.258641,11.301722,11.217101,11.326972,11.239719,11.182945,11.244569,11.240675,11.258623,11.336592,11.254412,11.29094,11.440315,11.508664,11.604798,11.733294,11.741895,11.781262,11.69299,11.717284,11.731176,11.778927,11.790124,11.693809,11.763755,11.789223,11.777747,11.765252,11.717085,11.672788,11.709937,11.597054,11.488282,11.381647,11.285351,11.283376,11.289643,11.273334,11.255188,11.251096,11.291878,11.21263,11.250978,11.231173,11.303137,11.292536,11.174642,11.188577,11.273154,11.272875,11.281718,11.329289,11.250158,11.345317,11.410872,11.447419,11.615039,11.72968,11.819846,11.840308,12.224652,11.769624,11.755272,11.781001,11.726326,11.7606,11.733114,11.812021,11.728183,11.668577,11.6</t>
+  </si>
+  <si>
+    <t>12.638358,12.567015,12.51665,12.34051,12.319172,12.137219,11.952334,11.862684,11.910993,11.951533,11.941914,11.901311,11.872806,12.046773,11.968841,11.931133,11.900752,11.914924,11.915086,11.974151,11.931474,11.962693,11.909596,12.006108,11.99539,12.013536,12.111328,12.340528,12.453294,12.571468,12.531307,12.636483,12.647201,12.640972,12.590868,12.611089,12.615082,12.571207,12.654349,12.546633,12.696187,12.497069,12.54913,12.515775,12.478607,12.406481,12.256989,12.064379,11.95385,11.875222,11.85412,11.938001,11.800283,11.971716,11.964829,11.921432,11.936604,11.970021,11.980578,11.926022,11.885463,11.933089,11.865658,11.867615,11.979001,12.057573,11.994073,11.946105,12.111167,12.31416,12.358712,12.689499,12.576896,12.582205,12.552123,12.713017,12.619734,12.702534,12.614045,12.579212,12.564121,12.638277,12.520904,12.596619,12.55919,12.554502,12.529667,12.404227,12.222336,12.024354,11.970021,11.898156,11.941535,11.912968,11.880929,11.881488,12.035172,11.958321,11.907938,11.908695,11.904069,12.376362,11.952912,11.846096,11.84468,11.89684,11.915762,12.006407,11.943131,12.002917,12.121929,12.246152,12.314179,12.491381,12.619075,12.664987,12.725829,12.590968,12.558072,12.673272,12.567294,12.647301,12.551365,12.607978,12.586198,12.605959,12.64227,12.633328,12.515514,12.387639,12.215151,12.624025,11.862088,11.923469,11.960737,11.919576,11.930356,11.909136,11.845239,11.92237,11.921234,11.992875,11.949838,12.023534,11.955148,11.896318,12.47447,11.980001,11.985031,11.960637,11.954949,11.98944,12.114384,12.248785,12.409617,12.522419,12.661913,12.661472,12.718246,12.666683,12.633067,13.138262,12.557694,12.593825,12.669378,12.640935,12.565518,12.531424,12.566096,12.569394,12.518588,12.290505,12.262839,12.154644,11.909794,11.928139,11.956663,11.899914,11.95924,11.931474,11.85484,11.979541,11.881029,11.934306,11.957762,11.938659,11.933548,12.040644,11.87562,11.982615,12.031701,12.093083,11.96373,12.078091,12.233055,12.208903,12.455268,12.48142,12.562202,12.649077,12.59588,12.595439,12.567934,12.565798,12.720122,12.659498,12.545776,12.656423,12.56999,12.542801,12.563662,12.575498,12.460858,12.420615,12.180796,12.140311,11.915303,11.909217,11.968282,11.901131,11.84927,11.85484,12.030962,12.013356,11.955986,11.877955,11.909975,11.919476,12.015672,11.928996,11.859672,11.953831,11.948441,12.004072,12.004034,11.910695,12.081625,12.295076,12.349651,12.525754,12.618535,12.675949,12.631011,12.59634,12.561165,12.632011,12.602109,12.623267,12.560786,12.584702,12.560886,12.588235,12.584242,12.470061,12.527052,12.369592,12.232657,12.081705,11.930574,11.877737,11.922171,11.9586,11.883165,11.971157,11.914825,12.007208,11.917241,11.93253,11.900193,11.986348,11.89199,11.925525,11.890512,11.974132,11.925922,11.976287,12.007848,11.950037,12.114483,12.20994,12.839973,12.62718,12.568313,12.61656,12.604165,12.563382,12.578914,12.665348,12.510862,12.660516,12.561705,12.582367,12.573884,12.520643,12.495175,12.598656,12.489443,12.354222,12.195427,12.105578,11.918017,11.923867,11.929655,11.952794,11.969201,11.949919,11.89666,11.93335,11.893946,11.984131,12.418939,11.955986,11.902746,11.96912,11.847394,11.957265,11.994253,12.035495,11.965109,11.99511,12.060106,12.286015,12.444891,12.680618,12.594501,13.155687,12.55388,12.602587,12.565419,12.602606,12.640594,12.587217,12.623888,12.653232,12.539069,12.515135,12.573741,12.493815,12.464932,12.416523,12.778529,12.079551,11.954129,11.992316,11.824118,11.947664,11.857095,11.894722,11.916924,11.931692,11.919557,11.91275,11.869093,11.940995,11.883146,11.993496,11.8758,11.947882,11.992577,12.007226,12.015294,11.909416,12.046512,12.23054,12.408319,12.569449,12.603345,12.594564,12.646462,12.662093,12.868956,12.616957,12.631291,12.635402,12.626161,12.610791,12.582187,12.563103,12.603506,12.58041,12.515172,12.595799,12.275532,12.119793,11.96912,11.929077,11.966885,12.038029,11.907242,11.987466,11.930772,11.966245,11.974809,11.99693,11.908794,12.017629,11.961097,12.014275,12.017088,11.967245,11.993974,12.135262,11.987205,12.03811,12.175585,12.309869,12.405723,12.564221,12.567916,12.770226,12.689741,12.621212,12.63139,12.625521,12.659057,12.752241,12.616641,12.605084,12.567375,12.555458,12.523438,12.555458,12.569089,12.374902,12.263777,12.103323,11.91185,11.928698,11.880731,11.904863,11.907459,11.952912,11.899535,11.93838,11.919035,11.885022,11.998085,11.917141,11.913626,11.938678,11.948999,11.937063,11.945087,11.977784,12.006369,12.001699,12.127555,12.296293,12.392409,12.467546,12.615181,12.714514,12.609673,12.620851,12.570549,12.585018,12.638718,12.737349,12.655666,12.569629,12.608952,12.606158,12.568872,12.601109,12.565996,12.477905,12.291362,12.077352,11.991558,11.935008,11.873564,12.014654,12.004016,11.951794,12.045736,11.894343,11.936523,11.933008,11.965227,11.978703,12.003674,12.013834,11.949838,11.977504,12.024056,12.108093,12.039787,11.970238,12.12596,12.828074,12.431974,12.639917,12.688462,12.63321,12.66459,12.680799,12.671514,12.665907,12.667024,12.604804,12.607617,12.756712,12.613045,12.630713,13.193216,12.637222,12.519867,12.362687,12.307832,12.099591,11.971716,11.881488,11.947782,11.962494,11.918278,11.970499,11.888593,11.898454,11.963513,12.367934,11.922171,11.921414,11.935026,11.903087,11.890133,11.930176,11.958159,12.092325,12.001619,11.988683,12.121488,12.259044,12.434272,12.592707,12.675489,12.620473,12.656045,12.577175,12.627819,12.576877,12.67878,12.624845,12.658361,12.568313,12.667385,12.630695,12.57566,12.564779,12.571586,12.91411,12.309608,12.106938,12.006829,11.939237,12.007947,11.960917,11.9489,11.99054,11.918619,11.997886,12.01076,11.979721,11.951974,12.024795,12.061504,11.920793,12.029825,12.002395,11.939957,11.989503,11.998743,11.989521,12.077892,12.314079,12.43375,12.541963,12.634924,12.617777,12.702895,12.803283,12.625701,12.534219,12.626819,12.600892,12.71044,12.636483,12.615424,12.543,12.541485,12.597575,12.539628,12.38672,12.317153,12.080985,12.10921,11.891331,11.902528,12.056834,11.963712,11.932151,11.884444,11.997147,11.931493,11.950614,11.951515,11.987167,12.613207,11.892089,11.908099,11.987385,11.978622,12.081886,12.075216,12.01048,12.071844,12.330189,12.386621,12.610313,12.584882,12.612846,12.632092,12.669918,12.654846,12.661156,12.587018,12.64273,12.57017,12.660535,12.594644,12.617119,12.606878,12.534418,12.538131,12.460001,12.206965,12.165065,11.955067,12.013536,11.989043,12.037489,12.020262,12.130791,12.007388,11.954669,12.284295,12.054219,11.956445,12.023497,12.020504,12.057032,11.871689,11.981398,11.973772,12.057312,11.985528,12.030583,12.078892,12.264975,12.356321,12.586217,12.567655,12.637141,12.568512,12.644785,12.730741,12.593744,12.606698,12.654728,12.607139,12.611287,12.628757,12.629316,12.58436,12.629713,12.487027,12.332586,12.286512,12.148378,11.956247,11.996949,11.84935,11.949099,11.93289,12.033676,11.865441,11.904646,11.974449,11.945646,11.973853,12.057492,11.985689,11.931114,11.933648,11.976765,12.081507,12.01661,12.08971,12.012058,12.441196,12.248027,12.516731,12.524357,12.63257,12.645425,12.646146,12.650934,12.600053,12.595663,12.6796,12.638737,12.654567,12.624826,12.677122,12.679122,12.608276,12.603867,12.581348,12.415225,12.281941,12.122948,12.826838,11.963531,12.005351,12.004873,12.003773,11.923128,11.981398,11.955309,12.547335,11.919656,11.946385,11.899355,11.988583,11.92183,11.936262,11.939119,11.872067,12.033756,12.05815,12.000861,12.126239,12.29815,12.495852,12.568512,12.64722,12.672812,12.632669,12.721879,12.615703,12.650816,12.692915,12.571685,12.646903,12.643767,12.615523,12.610872,12.552781,12.60622,13.786459,12.398377,12.221497,12.142348,11.973132,11.935225,11.996588,11.99529,12.005928,11.971897,12.032539,11.960954,12.00563,11.944727,12.007928,12.001556,11.961296,11.943032,12.000699,11.952533,12.003215,12.031601,12.034197,12.025913,12.186683,12.314818,12.474371,12.642711,12.680438,12.660435,13.034619,12.586838,12.595042,12.627279,12.591328,12.579193,12.591688,12.577156,12.564798,12.581267,12.514495,12.567294,12.502578,12.321047,12.241501,12.079209,11.934586,11.882209,11.922947,11.956626,11.971139,12.013257,11.950117,11.913986,11.918377,11.882109,11.905683,11.940075,11.894406,11.890232,11.950179,11.892207,11.960998,11.993235,11.989683,12.031881,12.12622,12.261677,12.461677,12.607257,12.544199,12.628956,12.631949,12.588415,12.555178,12.614343,13.354986,12.746291,12.764916,12.655666,12.656045,12.655883,12.626683,12.640494,12.521941,12.500522,12.275793,12.21489,12.040842,11.9596,12.02777,12.040762,12.073601,11.945385,11.99529,12.005351,12.082246,11.924525,12.005072,12.011058,12.043879,12.0016,12.04278,12.070446,12.009903,12.098473,12.036054,12.036253,12.177063,12.390074,12.373126,12.570927,12.703615,12.673371,13.039171,12.748248,12.70541,12.636483,12.665807,12.712937,12.779069,12.618715,12.668061,12.683792,12.628856,12.728325,12.574262,12.376262,12.391912,12.114024,11.95339,12.01058,11.997886,12.009363,12.333604,11.966028,11.931294,11.963792,12.024814,11.945006,11.966624,11.92237,11.900932,11.971456,11.949558,11.966127,12.032819,12.010381,12.116539,12.493337,12.163308,12.287351,12.596042,12.488984,12.516632,12.647481,12.707645,12.643109,12.735014,12.61684,12.687686,12.632769,12.734536,12.667782,12.589335,12.670757,12.478464,12.573244,12.587236,12.348236,12.230341,12.162749,11.938616,11.911751,11.979343,11.978523,11.899734,12.038868,11.919576,12.502857,11.850406,11.889195,11.923867,11.946962,11.965488,11.811859,11.811263,11.910155,11.925426,11.989583,12.651772,11.966624,12.10564,12.188521,12.447587,12.592067,12.546416,12.589372,12.551763,12.527233,12.651772,12.558271,12.529145,12.497628,12.571424,12.553682,12.603345,12.462416,12.442811,12.994098,12.476309,12.316973,12.206208,12.027248,11.828652,11.945944,11.951813,11.898417,11.869291,11.810605,11.888574,11.888115,11.865839,11.82849,12.434588,11.926941,11.915545,11.836216,12.616939,11.960917,11.95842,12.024777,12.066633,12.031701,12.065615,12.212294,12.410474,12.523258,12.66962,13.145347,12.68948,12.627658,12.639836,12.636141,12.682755,12.667583,12.581628,12.61135,12.625882,12.558631,12.698342,12.518948,12.480401,12.36165,12.212474,12.09494,12.025193,11.967344,11.914266,11.979982,12.013418,11.956265,12.034378,11.901852,11.916284,11.991179,11.931754,11.932269,11.920793,11.904764,11.985131,11.956626,11.988925,11.979461,11.911173,11.920153,12.096995,12.191235,12.346838,12.544317,12.557035,12.574461,12.589074,12.563401,12.544118,12.526953,12.681656,12.563581,12.543261,12.558271,12.540845,12.580771,12.651654,12.46523,12.495691,12.295933,12.2514,12.081066,11.925543,11.856157,11.897778,11.86436,11.892928,11.88029,12.614324,11.948919,12.043457,12.015952,11.981255,12.032738,12.006829,11.944447,11.998066,11.969679,12.000699,12.058908,12.009903,11.997787,12.109372,12.19503,12.481122,12.546416,12.615262,12.564519,12.735952,12.565618,12.587037,12.604183,12.605202,12.593725,12.671036,12.578193,12.675868,12.563662,12.475091,12.571126,12.536833,12.302243,12.266633,12.061963,11.918718,11.903628,12.687046,11.891729,11.955526,11.976728,11.950595,11.992676,11.903385,11.870012,11.980019,11.889953,11.915806,12.004413,11.925742,11.877216,12.032999,12.098933,12.601407,12.029124,12.18323,12.378237,12.482935,12.514936,12.695709,12.722618,12.672272,12.718526,12.789129,12.590931,12.738963,12.735573,12.600712,12.74092,12.761581,12.558631,12.624106,12.716867,12.585559,12.435626,12.303162,12.019784,12.007866,11.953949,11.931692,11.970716,11.939318,11.898337,12.526413,11.957383,11.951217,11.966146,11.984373,11.903727,11.948441,11.960557,11.939498,11.977386,12.024894,12.031782,12.02777,11.989701,12.171375,12.84219,12.437923,12.537212,12.589831,12.588533,12.678203,12.62187,12.601289,12.572045,12.620491,12.586279,12.624764,12.691337,12.610989,12.610052,13.779491,12.500783,12.586676,12.438122,12.1879,12.048549,11.975188,11.904385,11.994173,11.936225,11.965749,11.971816,11.939858,11.894263,11.944826,11.893523,11.92173,11.935045,11.847295,11.934729,12.02174,11.873483,12.019883,12.050145,12.067733,11.962016,12.212654,12.254753,12.576038,12.593663,12.990663,12.761562,12.733076,12.754756,12.805878,12.644407,12.715669,12.864087,12.988049,12.590092,12.600072,12.640954,12.720302,12.729263,12.724854,12.534877,12.463975,12.274955,12.078352,11.988304,12.135343,12.012815,12.061684,12.020423,12.016529,12.132927,12.042004,12.00106,11.981976,11.963351,12.066633,11.954887,12.023336,12.05861,12.093921,12.069049,12.052201,12.071862,12.231117,12.366779,12.537572,12.705031,12.688623,12.754098,12.80468,12.692735,12.591427,12.565618,12.707825,12.725792,12.667322,12.581367,12.740063,12.675868,12.68006,12.624863,12.597954,12.38187,12.256268,12.212716,12.065615,11.942112,11.908037,12.009425,12.019423,11.930754,11.907099,12.081246,11.959619,12.033937,11.977026,12.035893,12.058051,12.055734,11.987863,11.981994,12.010164,12.020523,12.16858,12.05258,12.233055,12.317911,12.541684,12.49212,13.313085,12.7527,12.746571,12.707447,12.633309,12.806996,12.792763,12.770443,12.717607,12.743497,12.679358,12.710459,12.733654,12.595042,12.687443,12.545037,12.259125,12.106279,11.990918,12.071763,12.055734,12.092722,11.983274,11.998166,12.027149,12.054318,12.082445,11.943212,11.98523,12.055734,12.055616,12.077613,12.038246,12.090909,12.150434,12.65389,12.142149,12.019585,12.336796,12.461137,12.623447,12.722457,12.749825,12.839954,12.781485,12.839793,12.745633,12.823882,12.669279,12.728388,13.307775,12.720699,12.715731,12.578914,12.705931,12.523997,12.64273,12.417604,12.379436,12.105677,11.980839,11.971996,12.087773,11.939777,11.992577,12.492617,12.066813,12.086276,12.038669,11.97992,11.975548,11.913707,11.973753,12.034676,11.992875,11.998725,12.045574,12.120613,12.016331,12.097635,12.102386,12.340528,12.46541,12.620932,12.750701,12.763158,12.809232,12.584522,12.732877,12.625863,12.748906,12.753098,12.756669,12.635744,12.472955,13.130753,12.53166,12.564121,12.447705,12.249363,12.337175,12.147341,11.885581,11.895443,11.898175,11.916123,11.925146,11.87095,11.937181,11.943032,11.902087,11.912968,11.849711,11.851965,11.961494,11.908577,11.873943,11.95924,11.965388,11.951732,11.982336,11.950577,12.166823,12.253896,12.310825,12.651195,12.50659,12.578355,12.609393,12.608735,12.509546,12.610989,12.690319,12.626701,12.607915,12.630334,12.59506,12.580448,12.59616,12.543261,12.63175,12.377976,12.153247,12.082643,11.815834,11.844041,11.92786,11.974828,11.811245,11.914247,11.992875,11.927742,11.895461,11.802401,11.905783,11.913148,12.007587,11.850909,11.909136,11.788447,11.95934,11.965668,11.991738,11.898237,12.210977,12.248903,12.340429,12.492617,12.526791,12.602128,12.699299,12.665285,12.562643,12.487866,12.62223,12.568953,12.514576,12.604984,12.655865,12.597656,12.506751,12.506031,12.442053,12.323581,12.173089,11.994173,11.896182,11.882867,11.900411,11.876657,11.8231,11.798489,11.883345,11.971176,11.991937,11.937722,12.030186,11.958619,11.980839,11.810245,11.931114,11.921252,11.934287,12.046512,11.983056,12.046295,12.08486,12.265671,12.415865,12.610493,12.546912,12.632408,12.555476,12.493455,12.572225,12.592446,12.630154,12.648779,12.609114,12.572604,12.600153,12.588254,12.581944,12.5343,12.431334,12.36073,12.223273,12.051903,11.956626,11.991198,11.903746,11.982156,11.95942,11.954508,11.951695,11.877035,12.0006,11.914564,11.981001,11.921252,11.945367,11.968562,11.964469,12.006829,12.386621,12.076756,12.020162,12.036551,12.166363,12.379075,12.431496,12.576796,12.669161,12.652052,12.643568,12.675048,12.636302,12.695448,12.615803,12.681016,12.584602,12.648139,12.651312,12.5743,12.526773,12.636781,12.536274,12.41335,12.244034,12.080209,12.053778,11.89584,11.910552,11.985429,12.531722,11.936225,11.992055,12.056374,11.927941,11.999762,11.991819,11.988745,12.013356,11.935585,11.931791,11.964649,11.955247,11.929835,12.079551,12.036352,12.113645,12.35506,12.451418,12.53751,12.668999,12.760264,12.692014,12.599594,12.597575,12.70962,12.670098,12.647462,12.589552,12.728785,13.228608,12.589272,12.499665,12.630651,12.538709,12.40319,12.288189,12.099591,11.95906,12.060007,11.96024,12.019784,11.90297,11.912868,11.898337,12.458883,11.977703,11.890611,11.916899,11.962233,11.944727,11.968841,11.847015,11.960457,12.015312,12.031999,11.926301,12.076216,12.165922,12.256231,12.884965,12.523537,12.525376,12.674507,12.581547,12.708086,12.648499,12.658821,12.667801,12.82472,12.661472,12.694132,12.676805,12.680538,12.586838,12.649275,12.577796,12.456504,12.343603,12.202233,12.055455,11.992775,12.080128,12.016529,12.059448,11.9898,12.053977,12.075936,11.975188,12.033856,11.956247,11.965009,11.969922,11.935585,11.916601,11.990179,11.956284,11.99044,12.042699,11.99126,12.121569,12.291822,12.448742,12.629036,12.727568,12.678581,12.607319,12.630794,12.646282,12.685947,12.644028,12.699442,12.574939,12.594483,12.62736,12.660796,12.530244,12.59606,12.528549,12.422671,12.311943,12.093461,11.910254,12.000401,11.908857,11.899734,11.894424,11.976287,11.965109,11.944429,11.899933,11.958979,11.961215,12.030024,12.122047,12.022597,11.979622,12.072862,12.121109,12.031943,12.078091,12.047251,12.249704,12.328313,12.466546,12.604202,12.757072,12.671595,12.718345,12.706527,12.698703,12.718265,12.812145,12.708223,12.574722,12.78354,12.604742,12.725711,12.504894,12.688462,12.602947,12.451679,12.335002,12.139634,12.051164,12.00088,11.981578,12.009804,11.937461,11.976666,11.989602,11.982398,11.918197,11.940336,12.097455,11.993775,12.048568,11.972375,11.971419,12.505733,11.891071,12.02741,11.942293,12.100249,12.243196,12.400774,12.553502,12.779845,12.737728,12.784956,12.815939,12.685767,12.677942,12.788111,12.784099,12.678861,12.716452,12.729605,12.697566,12.713036,12.680718,12.643929,12.625404,12.445326,12.29284,12.210679,11.99062,12.031403,12.053381,12.57456,12.025112,12.020144,11.90151,11.983354,12.007109,11.872086,11.979262,11.961035,11.988962,11.989782,11.914545,11.978902,12.133207,12.128574,12.655964,12.06931,12.316315,12.351049,12.518209,12.615064,12.735852,12.797433,12.739106,12.729803,12.73166,12.637041,12.741919,12.705652,12.728226,13.205692,12.668801,12.692257,12.643009,12.691238,12.562444,12.524177,12.380094,12.129592,12.051741,12.111688,11.962414,11.978641,12.01176,11.998526,12.020523,12.04324,12.010878,12.014834,11.889332,12.028825,12.077433,11.970679,11.978063,12.068931,11.997408,12.076657,12.103243,12.072763,12.155266,12.574461,12.451536,12.688741,12.683432,12.64155,12.738647,12.657703,12.669099,12.687245,12.708304,12.690778,12.668521,12.698703,12.659876,12.645046,12.600929,12.65828,12.50228,12.328593,12.232036,12.099392,11.907261,11.936784,12.009164,12.007667,11.939759,11.948999,11.856039,11.912092,11.98541,11.944826,11.969301,11.882091,11.956427,11.891971,11.961855,11.864522,11.851865,12.027149,11.960439,11.998563,12.105478,12.150813,12.441376,12.542981,12.656144,12.701118,12.614424,12.551104,12.592725,12.605301,12.671533,12.57402,12.635843,12.626882,12.519047,12.551663,12.584242,12.599693,12.394526,12.339411,12.174828,12.068788,11.903168,11.905224,11.86464,11.988683,11.986627,11.906621,11.904385,11.946404,11.930195,11.940318,11.843761,11.954968,11.880929,11.970617,11.905981,11.944006,11.967885,11.987664,12.014095,11.973132,12.1879,12.268546,12.482898,12.479463,12.609754,12.624006,12.628478,12.655566,12.607276,12.587577,12.566934,12.699063,12.620752,12.640693,12.544379,12.598855,12.613567,12.541044,12.435607,12.3976,12.219243,12.059367,11.956526,11.936523,11.909118,11.891611,11.905503,11.878396,11.968543,11.892847,11.874303,11.882327,11.895542,12.005811,11.932232,11.925786,11.918917,11.988024,11.912968,12.000799,11.903087,11.96894,12.137877,12.280184,12.341926,12.635203,12.536374,12.632967,12.674967,12.656045,12.639476,12.614405,12.668521,12.571486,12.55919,12.608394,12.571306,12.692014,12.645146,12.502118,12.512719,12.360072,12.220858,12.136741,11.926823,11.891331,12.443252,11.925426,11.925426,11.920017,11.786211,11.869291,11.898796,11.960259,11.957203,11.974151,11.979343,12.026671,11.991937,11.898237,11.954968,12.021839,12.003891,11.97004,12.111608,12.217864,12.345441,12.56432,12.644885,12.660858,12.609474,12.640594,12.573082,12.699839,12.594104,12.703373,13.153731,12.754675,12.552266,12.666204,12.596439,12.61025,12.466627,12.340187,12.334119,12.112788,11.979461,11.90297,11.934666,11.92273,11.907559,12.48791,11.881109,11.902988,11.986708,11.974114,11.866857,11.913148,11.877594,11.927319,11.998625,11.971257,11.90115,11.898597,11.950037,12.01222,12.638619,12.275793,12.385304,12.475849,12.602028,12.56414,12.655865,12.661634,12.624845,12.651114,12.632669,12.688922,12.643009,12.635203,12.6591,12.624925,12.597557,12.654728,12.463634,12.337057,12.217883,12.063938,11.925904,12.036253,12.02264,11.89181,11.852785,11.85512,11.960755,12.012996,12.109372,11.98908,11.832601,12.00114,12.014294,11.873446,11.885481,11.90764,11.967705,12.024056,11.998824,11.884941,12.096977,12.29302,12.394104,12.555737,12.609574,13.235594,12.648518,12.650636,12.614244,12.597197,12.596259,12.626323,12.598855,12.593365,12.586577,12.551067,12.575138,12.536094,12.493896,12.468682,12.207705,12.015871,11.934548,11.959079,11.941274,11.937703,11.999482,11.9069,11.89163,11.89189,11.963631,11.928021,11.85448,11.901709,11.940175,11.944888,11.915402,11.910055,12.017827,12.067174,12.028627,11.996768,12.146043,12.959022,12.391633,12.675607,12.590011,12.710322,12.67375,12.624782,12.675408,12.593564,12.676986,12.614324,12.58051,12.550546,12.583584,12.623385,12.45525,12.50795,12.502758,12.347875,12.242159,12.033477,11.969102,11.869633,11.954949,11.965227,11.917241,11.934188,11.960376,11.874961,11.998247,11.910713,11.867317,11.975548,11.997228,12.071185,11.857014,11.88047,11.929456,11.945925,11.99108,12.011878,12.139175,12.208822,12.450319,12.530766,12.677402,12.686884,12.614064,12.685289,12.576579,12.657659,12.619274,12.62836,12.580367,12.624124,12.623429,12.514595,12.536871,12.620473,12.527052,12.347776,12.211896,12.107316,11.990061,12.520184,11.88586,11.971176,11.982895,11.862827,11.887338,11.927183,11.981299,11.945087,11.928698,11.951235,12.029347,12.553061,11.983833,11.971338,12.47539,11.978423,11.985031,12.027248,12.10033,12.337157,12.434408,12.546273,12.623609,12.641432,12.599134,12.61025,12.551924,12.660715,12.578833,13.083605,12.635663,12.641414,12.690139,12.561985,12.656361,12.524177,12.488884,12.393688,12.102683,12.122525,11.983814,11.902547,11.94954,12.03711,12.020603,11.887015,11.979019,11.961395,11.901491,12.620013,11.921054,11.988782,11.916942,11.936722,11.877855,11.855679,11.941752,12.029105,11.996029,12.479364,12.138038,12.322805,12.436905,12.574001,12.54236,12.610431,12.6484,12.713396,12.579752,12.597458,12.586441,12.626621,12.575498,12.546552,12.566997,12.612449,12.503776,12.562643,12.467844,12.372747,12.295356,12.091325,11.978883,11.944186,11.906981,11.899914,12.04314,11.981299,11.982354,11.952931,11.955048,11.914607,11.88165,11.930195,11.989422,11.989403,11.887518,11.905224,11.933548,11.920495,11.983454,12.029943,12.092704,12.223056,12.483196,12.603525,12.709223,12.688263,12.62636,12.611269,12.653349,12.630912,12.60686,12.683233,12.617318,12.632011,12.608555,12.5957,12.596998,12.595321,12.562463,12.347515,12.280662,12.062622,11.946124,12.696287,11.964351,11.92283,11.972952,11.917638,11.936324,11.946782,11.825975,11.883066,11.922929,11.994632,11.935225,11.894604,11.96391,11.931772,12.009822,11.939759,11.898436,12.086158,12.180994,12.16776,12.466906,12.524897,12.649238,12.575958,12.634744,12.678861,12.677284,12.683612,12.661634,12.632949,12.505913,12.696088,12.612946,12.629136,12.61738,12.573561,12.440457,13.054641,12.317694,12.046692,11.922072,11.842345,11.967264,11.977424,11.836613,11.917222,11.890692,11.881849,11.954148,11.980019,11.890394,11.893225,12.27244,11.972834,11.96912,11.935585,11.953291,12.078091,11.990701,11.966208,12.097374,12.358774,12.5323,12.645245,12.58051,12.634887,12.62708,12.915805,12.541386,12.668142,12.653467,12.60119,12.618355,12.567574,12.553322,12.594203,12.587037,12.526512,12.496132,12.356737,12.260802,12.084997,12.444171,11.925227,11.876278,11.968822,11.920333,11.996588,11.881289,11.923208,11.92273,11.91157,11.919756,11.937461,11.968841,11.924804,11.915104,11.942013,12.012896,11.938759,12.070285,11.891331,12.135343,12.1997,12.427999,12.638538,12.643451,12.629695,12.686028,12.558712,12.666024,12.659119,13.161655,13.377504,12.582106,12.595421,12.599911,12.596079,12.518948,12.546534,12.494256,12.419678,12.273179,12.056014,11.989322,11.91734,11.964649,11.911453,11.932449,11.87534,12.057231,12.015672,11.871806,11.937181,11.971139,11.864721,11.948757,11.858492,11.840787,11.843202,11.95824,11.977386,12.555458,11.97453,12.195147,12.243755,12.436147,12.526556,12.636663,12.63706,12.620932,13.427645,12.586676,12.512521,12.603227,12.634508,12.636762,13.142211,12.571704,12.543838,12.607419,12.521084,12.466906,12.318613,12.206164,12.000619,11.896678,11.818231,11.992676,12.035911,11.937163,11.911192,12.295716,11.936623,11.981976,11.852406,11.943888,11.959917,11.927301,11.949378,11.873626,11.898635,11.994471,12.024516,12.031223,11.983572,12.150055,12.312005,12.398557,12.548093,12.603804,12.562184,12.665186,12.640935,12.536653,12.677861,12.658659,12.598755,12.588813,12.6591,12.643109,12.624385,12.555756,12.563481,12.445748,12.330747,12.246667,12.05851,11.959159,11.892369,12.003575,11.942752,11.962972,11.945745,11.970518,11.961395,11.919097,11.985348,11.94936,11.934946,11.930195,11.928139,11.944249,11.907739,11.930655,11.932493,11.990242,12.680898,12.126698,12.264155,12.537131,12.576976,12.602668,12.633688,12.608816,12.558911,12.706329,12.628117,12.641233,12.508329,12.633408,12.593483,12.54831,12.483016,12.576796,12.542125,12.571964,12.387279,12.264218,12.101926,11.890512,11.93371,11.92237,11.836775,11.892449,12.013337,11.883904,11.932989,11.983274,11.908478,11.908217,11.952154,12.035334,11.989304,11.873583,12.705869,12.11698,12.058989,12.119911,12.073241,12.23996,12.341727,12.446028,12.613685,12.754837,12.700361,12.784099,12.754315,12.718923,12.76763,12.732337,12.670297,12.677824,12.668981,12.715687,12.615821,12.634247,12.623547,12.606158,12.489325,12.238228,12.704391,11.985491,12.039147,12.019784,12.007307,11.986807,11.992396,11.991738,11.992316,11.997545,11.93207,12.024994,12.005891,12.011381,12.050965,12.0319,12.041383,12.007767,12.019603,12.0415,12.142249,12.251841,12.39706,12.48627,12.692617,12.701317,12.683071,12.788111,12.655865,12.606978,13.25769,12.665465,12.737367,12.669018,12.733995,12.654548,12.752259,12.62708,12.64273,12.602469,12.378237,12.292281,12.127419,12.033955,11.951154,12.608853,12.031539,11.961377,12.090928,11.909794,12.549608,11.986267,11.992477,11.981299,12.031322,11.986168,12.058691,12.001736,11.986826,12.135182,12.497349,12.073899,12.00709,12.257989,12.381988,12.592924,12.700659,12.655206,12.652871,12.751123,12.74685,12.712216,12.725233,12.708384,12.800768,12.706627,12.832644,12.76268,12.66295,12.606338,12.640873,12.573082,12.476688,12.309391,12.123767,12.020622,12.030844,12.012996,12.852548,11.995651,12.113483,12.043817,12.048189,12.034856,12.007947,12.055157,12.032819,12.041122,12.077793,12.065037,12.051723,12.017449,12.090946,12.139535,12.07829,12.187403,12.378995,12.539069,12.620932,12.753818,12.699181,12.645785,12.767071,12.763438,12.772263,12.831427,12.6484,12.673533,12.662472,12.623547,12.64255,12.672055,12.644227,12.555837,12.425186,12.296753,12.155825,12.024075,11.961414,12.044096,11.943627,11.997364,11.960637,11.965966,12.038309,12.087512,12.005991,12.024155,11.921811,11.974393,11.964929,12.009903,11.884463,12.040724,11.965307,11.958942,12.003575,12.124742,12.362867,12.4493,12.646444,12.740063,12.608195,12.687642,12.635563,12.551365,12.674011,12.567574,12.656604,12.658721,12.66313,12.665907,12.662671,12.691797,12.576417,12.545695,12.369133,12.262379,12.155365,12.043339,11.942833,11.969021,11.968084,11.962153,11.924065,11.99008,11.904503,12.005811,11.933828,12.145702,11.967245,11.966966,11.976828,11.926481,12.001718,11.986429,12.090251,11.987646,12.023317,12.206506,12.393508,12.386441,12.62187,12.683711,12.619274,12.702137,12.693474,12.629515,12.645705,12.666006,12.701677,12.672055,12.683134,12.792365,12.772623,12.676066,12.639575,12.623944,12.41371,12.776635,12.16201,12.062044,11.997247,11.998526,12.055157,12.021243,12.029863,11.981119,12.035154,12.020982,12.003972,12.049288,12.004811,12.063578,12.599395,11.964829,12.039905,12.029664,12.143249,12.090928,12.061864,12.263777,12.428179,12.4708,12.564519,12.729164,12.674669,12.781963,12.722898,13.243698,12.775455,12.757172,12.700839,12.75601,12.780584,12.767593,12.663609,12.666944,12.541864,12.473235,12.441115,12.244034,12.133666,11.940075,11.961494,11.968841,11.978243,12.009065,12.04817,11.979442,11.977045,11.960178,12.045016,11.999681,11.933611,12.049325,11.957302,12.015132,11.875998,12.47475,12.070527,12.055418,12.068111,12.21507,12.365382,12.44391,12.640395,12.638079,12.694772,12.629875,12.701379,12.637439,12.671912,12.674191,12.740342,12.710142,12.597439,12.492418,12.627838,12.589894,12.60622,12.604444,12.388459,12.28727,12.101448,12.095002,11.969679,11.977026,12.034315,11.97489,11.967444,11.904882,11.934027,12.008785,11.967462,11.904665,12.04232,11.946584,11.970977,12.009263,11.916321,12.017827,12.07426,12.017051,12.094318,12.235651,12.235731,12.574461,12.647201,12.756153,12.821988,12.655504,12.79434,12.670297,12.71629,12.668583,12.6796,12.782441,12.770064,12.627838,12.720519,12.618895,12.632589,12.566177,12.497908,12.317911,12.082445,12.000898,12.004134,12.061423,12.065155,12.05184,12.010164,12.0114,12.116178,12.008046,12.010841,11.99429,11.977045,12.018107,11.966525,12.042681,12.073222,12.053778,12.03775,12.139094,12.07416,12.16822,12.418361,12.524736,12.70495,12.711458,12.745372,12.710999,12.732797,12.679538,12.797135,12.754017,12.715172,12.738684,12.701398,12.764276,12.757849,12.667645,12.596097,12.546093,12.485531,12.307832,12.137579,12.078253,12.0328,11.988763,11.966767,11.97004,12.02246,12.007109,12.05725,11.989981,12.311546,12.069689,12.075576,12.109931,12.020243,12.100988,12.116917,12.196265,12.164028,12.10087,12.093002,12.214331,12.403947,12.516812,12.620969,13.043823,12.790266,12.724953,12.711179,12.751583,12.753837,12.767332,12.722798,12.812405,12.766394,12.713793,12.700578,12.754675,12.577094,12.59021,12.972002,12.261622,12.160594,11.987167,11.986348,12.01743,12.067192,11.958799,12.016151,12.019864,12.041022,11.991577,12.022938,12.016331,12.071123,12.11598,12.002358,12.025112,12.088729,12.084103,11.994533,12.067292,12.135623,12.354141,12.459063,12.590111,12.707266,12.684071,12.790247,12.817256,13.318476,12.707447,12.807773,12.782981,12.829092,12.789949,12.771704,12.75234,12.792023,12.695268,12.691635,12.59588,12.512377,12.388776,12.171872,12.11488,12.096436,12.085158,12.096436,12.082544,12.08468,11.938659,12.039787,12.086475,11.91139,12.030024,12.069031,12.181914,12.02695,11.958799,12.651934,12.104,12.048468,12.076414,12.130872,12.312781,12.396582,12.56981,12.654728,12.64712,12.703571,12.669459,12.770524,12.667385,12.724674,13.226751,12.755657,12.71116,12.773399,12.755594,12.69076,12.642929,12.597737,12.59167,12.507608,12.280842,12.176144,12.003854,12.088512,12.060287,12.237246,12.057032,11.935964,11.985248,12.064118,12.022299,12.078569,12.03857,12.0631,12.058808,12.004873,11.895244,12.032043,12.107875,12.14151,12.057771,12.093145,12.206785,12.38618,12.600532,12.747391,12.71026,12.77366,12.776337,12.736709,12.743416,12.7732,12.768009,12.801065,12.668422,12.725512,12.676346,12.662572,12.62169,12.616479,12.489263,12.346596,12.292741,12.177542,12.015014,12.029763,11.985248,12.081724,12.034378,12.026373,12.015393,12.042041,12.012878,12.008245,12.039905,11.986987,12.023895,11.968065,12.024534,12.050226,12.1362,12.055995,12.077892,12.092623,12.247748,12.473054,12.541206,12.670838,12.698703,12.811747,12.713613,12.687363,12.730443,12.712794,12.730561,12.71675,12.656423,12.751682,12.661516,12.576318,12.593005,12.563401,12.483314,12.348875,12.226807,12.060665,11.960178,12.018585,12.015772,11.935604,12.036172,12.036893,11.934089,12.009046,11.924326,11.99593,12.02723,11.946764,11.963631,12.023398,11.933809,11.944789,12.003196,12.047152,12.028627,12.020162,12.269745,12.350608,12.500802,12.665348,12.706248,12.668242,12.612188,12.686208,12.58472,12.629217,12.659119,12.674986,12.586478,12.637861,12.681115,12.629595,12.590011,12.522221,13.144329,12.464472,12.351067,12.143845,12.024174,11.980858,12.070428,12.068788,12.012337,12.023416,11.966903,12.076036,11.98495,12.042258,12.034936,12.039246,11.99557,11.962035,12.029366,12.060367,12.071664,12.137778,12.116656,12.126879,12.246568,12.414089,12.590931,12.654765,12.732399,12.798271,13.342987,12.697107,12.821168,12.726189,12.827596,12.845841,12.817156,12.753899,12.823584,12.76268,12.774157,12.71126,12.605841,12.483016,12.335877,12.749185,11.981696,12.040762,12.053579,11.992775,11.892288,12.069689,11.992775,11.965307,12.007369,12.001619,12.049847,11.998166,11.958321,12.017368,12.518569,11.995769,12.123165,12.138075,12.066677,12.101466,12.233433,12.462416,12.463174,12.676445,12.69415,12.651033,12.708925,12.721618,12.714334,12.740901,12.717588</t>
+  </si>
+  <si>
+    <t>10.037601,10.01209,9.993447,9.965762,9.962166,9.94474,9.941946,9.957875,9.983268,9.965159,9.952925,9.948373,9.949509,9.958912,9.963923,9.940368,9.977896,9.947833,9.968954,9.986119,10.012829,10.035546,10.031714,10.05335,10.053251,10.063591,10.091419,10.160148,10.144038,10.092338,10.071199,10.050159,10.084973,10.081079,10.07467,10.049121,10.340064,10.132301,10.087606,10.060679,10.065746,10.06964,10.044849,9.997459,9.99131,9.989795,9.966556,9.969333,9.951807,9.951286,9.966358,9.980573,9.954242,9.959073,9.946814,9.973705,9.970829,9.944641,9.951149,9.969314,9.98161,10.001831,10.030019,10.009916,10.024088,10.062554,10.073832,10.072074,10.100424,10.125035,10.137133,10.149528,10.116111,10.136511,10.152025,10.136952,10.145417,10.105212,10.14292,10.138331,10.089724,10.056406,10.041793,10.071677,10.060436,10.014406,9.992329,9.987218,10.01758,9.960669,9.953323,9.943703,9.952565,9.965159,9.947715,9.942685,9.974363,9.966041,9.972965,9.951727,9.950329,9.975381,9.982206,10.490953,10.013748,10.022691,10.035645,10.063231,10.075211,10.08501,10.100399,10.146311,10.277682,10.128488,10.136654,10.146373,10.140685,10.132959,10.643221,10.125054,10.146373,10.117608,10.084433,10.053133,10.053233,10.060697,10.043731,10.014226,9.981548,9.988516,9.962725,9.967917,9.948112,10.448395,9.932922,9.95993,9.95472,9.944659,9.940747,9.959732,9.962166,9.953062,9.943424,9.973804,9.976201,9.986721,10.009556,10.019617,10.045228,10.044867,10.184641,10.075012,10.085091,10.133319,10.13871,10.123917,10.11821,10.129326,10.146653,10.137989,10.134257,10.149348,10.130841,10.682147,10.086109,10.058381,10.050177,10.066007,10.036465,10.008997,9.983684,9.984784,9.965979,9.949491,9.943163,9.939971,9.953025,9.964843,9.999533,9.949329,9.935077,9.947597,9.964482,9.945858,9.942144,9.966258,9.973885,9.989534,10.016083,10.022511,10.032174,10.086569,10.065448,10.265007,10.108268,10.140306,10.14787,10.134357,10.124476,10.153999,10.163042,10.182684,10.136033,10.126072,10.139325,10.141759,10.091537,10.038682,10.056288,10.071758,10.055269,10.014884,9.987019,9.990932,10.006519,9.965501,9.937213,9.945957,9.964861,9.972208,9.973425,9.953863,9.958893,9.972785,9.98107,9.962147,10.095611,9.962545,9.968954,9.992112,10.003768,10.023908,10.013649,10.05563,10.065268,10.069,10.094052,10.136394,10.142281,10.113217,10.117608,10.147671,10.151006,10.147013,10.130264,10.112658,10.131102,10.128649,10.112919,10.049519,10.047743,10.062933,10.049401,9.998316,9.987218,9.983088,9.962545,9.955161,9.963464,9.953242,9.952403,9.964023,9.953403,9.937474,10.093556,9.970829,9.956937,9.948472,9.937114,9.960868,9.977455,9.981151,10.011512,10.013388,10.030814,10.047941,10.065429,10.075211,10.098306,10.135257,10.155676,10.13158,10.141424,10.146454,10.130724,10.147851,10.121998,10.126631,10.130742,10.123458,10.082936,10.04301,10.051015,10.055288,10.035266,10.010457,9.99259,10.05445,9.857766,9.904057,9.885874,9.901163,9.889426,9.924898,9.90356,9.900784,9.891102,9.916974,9.929848,9.900107,9.910205,9.921464,10.340921,9.946994,9.964464,9.961986,9.977996,9.98546,10.032931,10.02828,10.042911,10.079862,10.092636,10.091618,10.072876,10.072993,10.099821,10.113875,10.077167,10.081439,10.085091,10.082837,10.034888,10.015145,10.011674,10.006699,9.997179,9.981449,9.93404,9.879104,10.142343,9.960949,10.536828,9.950969,9.98079,9.973922,9.955161,9.941008,9.947994,9.967556,9.960967,9.950491,9.944262,9.952447,9.974263,9.997179,10.002011,10.042433,10.036303,10.067504,10.075148,10.077626,10.099064,10.135114,10.154676,10.132761,10.129506,10.139325,10.155235,10.14302,10.13268,10.13817,10.651965,10.12701,10.076247,10.047463,10.055009,10.055568,10.13232,10.01794,9.984585,9.973164,9.963824,9.959471,9.947255,9.949292,9.969215,10.489096,9.913459,9.897791,9.908528,9.903678,9.913937,9.89835,9.880601,9.897971,9.924159,9.948174,9.954801,9.958334,9.969035,10.014686,10.516384,10.042532,10.052791,10.083116,10.111739,10.086029,10.078104,10.050475,10.087606,10.09114,10.07403,10.045066,10.074732,10.077266,10.040278,10.004246,10.035527,10.019877,9.997719,9.96596,9.957676,9.926333,9.879564,9.915614,9.905877,9.901144,9.881582,9.926414,9.898648,9.873379,9.836987,9.852997,9.886811,9.890463,9.861859,9.878725,9.882042,9.896971,9.904138,9.897971,9.92937,9.920346,9.993826,9.962166,10.021691,10.04942,10.060039,10.050457,10.00714,10.035366,10.069062,10.035546,10.24193,10.124774,10.141244,10.117409,10.092357,10.069441,10.061896,10.062554,10.053071,10.007401,9.9861,9.967854,9.969333,9.963824,9.952627,9.938691,9.947156,9.980213,9.959253,9.9452,9.895754,9.914459,9.915117,9.897151,9.909565,9.899188,9.874614,9.934319,9.957713,9.963563,9.948653,10.011413,10.009097,10.01766,10.043712,10.093953,10.087488,10.080042,10.285128,10.084892,10.105193,10.10633,10.083855,10.073714,10.090401,10.078645,10.047265,10.01748,10.004445,10.01345,9.998017,9.957036,9.948851,9.920545,9.925439,9.910025,9.912602,9.901343,9.916037,9.927693,9.913819,9.902461,9.854754,9.905814,9.907293,9.896953,9.913801,10.427913,9.917552,9.935536,9.988137,9.960849,9.968395,9.995583,10.004445,10.076527,10.041793,10.087445,10.079024,10.118843,10.076527,10.055269,10.124395,10.093214,10.1119,10.068044,10.093754,10.081278,10.025846,10.002272,10.025324,10.009394,9.995602,9.961427,9.985361,9.927594,9.875173,10.455561,9.892959,9.925917,9.872757,9.915875,9.908789,9.884675,9.898909,9.883079,9.863697,9.858145,9.845849,9.897971,9.875552,9.879825,10.469056,9.916397,10.088823,9.947895,9.982827,9.966718,10.008059,10.052394,10.026404,10.0485,10.006482,10.013829,10.027982,10.020157,10.058623,10.538343,10.022312,10.045128,9.975201,9.987236,9.983467,9.981349,9.935338,9.925457,9.895673,9.831677,9.875751,9.882222,9.870981,9.847625,9.863896,9.882241,9.892661,9.86679,9.883458,9.891363,9.864635,9.858226,9.89699,9.842477,9.86597,9.904858,9.926594,9.896971,9.933959,10.264386,9.94502,9.997359,9.991391,10.038837,10.071019,10.027504,10.025026,10.049978,10.056586,10.0496,10.034329,10.043849,10.067125,9.993068,10.013009,10.014487,9.975381,9.981231,9.948031,9.918589,9.91272,9.917092,9.87639,9.915335,9.872379,9.84052,9.83018,9.912801,9.848904,9.868746,9.870261,9.868864,9.865175,9.884855,9.845551,9.837546,9.896033,9.919688,9.921545,9.953583,9.915018,9.967376,9.978437,9.958614,10.030497,10.084613,10.057605,10.039278,10.065311,10.002768,10.044389,10.063293,10.028938,10.029596,10.012829,10.056307,10.00732,9.996043,9.974642,10.031633,9.972767,9.916353,9.921564,9.919968,9.923501,9.885252,9.865113,9.848923,9.902181,9.915117,9.927991,9.879384,9.846209,9.863976,9.888209,9.858325,9.848283,9.868187,9.88216,9.898089,9.922601,9.916434,9.907734,9.986001,9.931624,10.003048,9.99123,10.074453,10.038719,10.079421,9.995763,10.055648,10.079402,10.020474,10.011332,10.005662,10.021771,10.026901,9.988336,9.956279,9.989013,9.999632,9.932804,9.988435,9.925035,9.89799,9.826051,9.895555,9.858226,9.941747,9.952105,9.966159,9.960272,9.960471,9.940331,9.957695,9.957856,9.963563,10.453866,9.951646,9.978257,9.99213,10.005743,10.021033,10.030155,10.061995,10.060201,10.07998,10.097288,10.086488,10.10102,10.073056,10.091338,10.615095,10.046265,10.08519,10.074571,10.073552,10.057903,10.072136,10.031453,10.011593,10.004166,10.010214,10.01299,9.957695,9.932841,9.94456,10.433322,9.916633,9.899865,9.902461,9.919787,9.899946,9.916813,9.907988,9.894077,9.907572,9.929407,9.892761,9.879266,9.896692,9.93476,9.979213,9.963762,9.97173,9.984324,10.008556,10.012847,10.052791,10.056027,10.096089,10.101579,10.106231,10.084892,10.057803,10.109702,10.105473,10.627392,10.057344,10.10248,10.093313,10.041973,10.034527,10.019797,10.075869,10.052773,10.01327,9.989752,9.985082,9.975841,9.972885,9.957757,9.976959,9.954142,9.974822,9.968972,9.964582,9.954521,9.964644,9.967196,9.954602,9.938629,9.950609,9.972407,10.003768,10.019337,10.012171,10.197875,10.064951,10.066268,10.105392,10.101101,10.156136,10.145597,10.127271,10.131742,10.144318,10.154279,10.155496,10.083973,10.128587,10.132941,10.102697,10.039819,10.000812,10.030335,10.026423,9.995763,9.966556,9.950708,9.927532,9.870162,9.902939,9.896493,9.896151,9.878347,9.919247,9.895772,9.901983,9.889624,9.912441,9.91821,9.901163,9.887289,9.912341,9.937294,9.944181,9.945299,9.971388,9.978095,10.03349,10.031615,10.031733,10.050339,10.089345,10.094295,10.046724,10.060399,10.076266,10.102337,10.099865,10.080918,10.08116,10.091419,10.098505,10.025405,10.032292,10.00257,10.042073,10.004526,9.982188,9.945839,9.899927,9.919806,9.925755,9.901163,9.886631,9.924439,9.930885,9.921284,9.926575,9.922483,9.926016,9.930109,9.914676,9.920005,9.908609,9.889227,9.957856,9.97494,9.978337,9.962427,10.041793,10.03816,10.04311,10.064312,10.113316,10.093636,10.149547,10.141343,10.145833,10.161644,10.149627,10.134717,10.145218,10.145715,10.145138,10.09535,10.059958,10.066187,10.073453,10.129264,9.951987,9.926954,9.941287,9.937834,9.916074,9.888948,9.8827,9.902461,9.895555,9.920409,9.902101,9.910025,9.937393,9.917111,10.360862,9.889345,9.906752,9.921383,9.952105,9.947814,9.964843,10.000334,10.005743,10.003309,10.06479,10.080141,10.062175,10.108727,10.093195,10.120644,10.068423,10.110242,10.105752,10.089742,10.097747,10.089643,10.089022,10.041495,10.013649,10.070839,9.988696,10.000794,10.014046,9.990553,10.475502,9.976238,9.963203,9.960769,9.936816,9.898269,9.917813,9.895015,9.925097,9.899306,9.908708,9.904616,9.912043,9.891941,9.880762,9.95041,9.94061,9.967358,9.969531,9.98189,10.025467,10.0173,10.035726,10.076328,10.093853,10.102399,10.087308,10.089084,10.0808,10.056884,10.632602,10.093295,10.081855,10.067864,10.09168,10.052711,10.021312,10.014766,10.023889,10.01199,9.960949,9.938232,9.94969,9.919589,9.913739,10.4251,9.901983,9.911484,9.908789,9.908032,9.909826,9.900586,9.92316,9.934698,9.911683,9.89735,9.891102,9.937971,9.957136,9.95554,10.463386,9.971289,10.017021,9.999496,10.060418,10.040638,10.096648,10.096828,10.085389,10.131562,10.048419,10.095828,10.104355,10.079682,10.05866,10.087966,10.083296,10.02792,10.005004,10.031453,10.021293,9.9979,9.952105,9.961607,9.931245,9.874515,9.903101,9.888128,9.890823,9.888848,9.925936,9.910447,9.903181,9.879284,9.918191,9.936536,9.926377,9.949851,9.946597,9.977356,10.0066,10.016344,10.028777,10.028721,10.059201,10.076608,10.076428,10.110044,10.126911,10.151205,10.136493,10.132978,10.139387,10.155496,10.154198,10.135015,10.131922,10.150484,10.139846,10.092736,10.055648,10.054972,10.057344,10.035049,10.028677,9.993987,9.985361,9.972046,9.979375,9.946715,9.948733,9.962886,9.973146,9.966935,9.950068,9.89753,9.908708,9.917533,9.920986,9.912503,9.875552,9.926675,9.957415,9.967737,9.943541,9.981529,10.013009,10.027901,10.035266,10.083874,10.107727,10.095232,10.088003,10.106311,10.085749,10.062852,10.099983,10.086966,10.076409,10.07467,10.088345,10.055568,10.002948,9.996422,10.029659,10.00265,9.974003,9.957955,9.946299,9.926395,9.922104,9.907473,9.900766,9.914658,9.921067,9.91318,9.899107,9.941946,9.98089,10.511894,9.953484,9.942387,9.95426,9.984125,10.003408,10.017002,10.016642,10.034527,10.069901,10.058281,10.071397,10.105852,10.134717,10.14841,10.159408,10.126153,10.140523,10.14823,10.144299,10.072354,10.069621,10.086271,10.04832,10.049519,9.998757,10.008159,10.010295,10.00147,10.024107,10.55082,9.994645,9.981629,9.971189,9.969513,9.948211,9.949031,9.986622,9.964681,9.977176,9.958993,9.979412,9.982386,9.958695,9.957415,10.516086,9.983188,10.00157,10.040377,10.030534,10.037303,10.077005,10.084054,10.090518,10.104815,10.154658,10.15939,10.14266,10.146814,10.157353,10.671465,10.074173,10.078384,10.085749,10.087047,10.04914,10.042532,10.014406,10.013027,10.019598,10.001489,9.972785,9.938132,9.921446,9.91803,9.939412,9.895772,9.900107,9.903777,9.937853,9.911043,9.923042,9.900045,9.913279,9.914496,9.910845,9.892581,9.875372,9.933723,9.967873,10.281153,9.957316,9.9861,10.02343,10.028,10.031453,10.076067,10.092997,10.107168,10.087165,10.103318,10.089481,10.063293,10.079402,10.054729,10.154658,10.140703,10.129569,10.085569,10.064051,10.074534,10.063672,10.041054,10.008159,9.990671,9.985342,9.980033,9.963166,9.945417,9.941548,9.967575,9.968215,9.961787,9.946174,9.960651,9.964383,9.975381,9.963365,9.953403,9.945318,9.977039,10.000694,10.015903,10.024467,10.050059,10.020635,10.015704,10.034329,10.071335,10.099902,10.095412,10.072615,10.081899,10.120203,10.114335,10.102498,10.093475,10.078365,10.091798,10.094493,10.047941,10.013767,10.026224,10.023448,10.010953,9.978176,9.957415,9.932742,9.884476,9.919247,9.902958,9.913422,9.930388,9.932624,9.905175,9.909187,9.906094,9.91867,9.920626,9.909249,9.898449,9.914577,9.937853,9.956496,9.978077,9.977518,9.984784,10.01876,10.062672,10.075589,10.099163,10.095133,10.096828,10.081837,10.133419,10.088904,10.109963,10.087488,10.091239,10.074832,10.097505,10.083694,10.039837,10.01327,10.029677,10.005526,10.00247,9.971171,9.947634,9.927973,9.91867,9.9237,9.904976,9.902623,9.906473,9.915875,9.899946,9.901082,9.906094,10.46207,9.929929,9.902281,9.90366,9.910006,9.945939,9.952186,9.973326,9.963104,9.991391,10.147131,10.069541,10.069,10.102119,10.138809,10.663442,10.125693,10.055568,10.081756,10.094773,10.088624,10.056785,10.069739,10.082098,10.074869,10.020176,10.01263,9.997161,10.011792,9.984964,10.473447,9.929848,9.891761,9.911006,9.910267,9.900964,9.880943,9.89789,9.916894,9.89232,9.895096,9.921806,9.909447,9.924638,9.891301,9.985442,9.905995,9.877589,10.210351,10.021393,10.028379,10.036844,10.066268,10.073434,10.085172,10.104634,10.138666,10.169072,10.145156,10.134276,10.696958,10.152341,10.148131,10.130282,10.145237,10.149429,10.127848,10.087146,10.068125,10.064231,10.072515,10.057524,10.030776,9.991211,9.983864,9.996999,9.964563,9.950708,9.929929,9.958732,9.96588,9.964743,9.946796,9.950509,9.958154,9.972487,9.955062,9.908808,9.920166,9.943461,10.128885,9.98161,9.973245,9.99726,10.019319,10.041675,10.037241,10.064411,10.0905,10.108746,10.111702,10.13807,10.141964,10.165259,10.158191,10.128388,10.084694,10.099263,10.083116,10.036366,10.03926,10.020635,10.014884,10.007159,10.018139,9.939971,9.895474,9.923439,9.915956,9.921924,9.890544,9.919011,9.926196,9.911602,10.110963,9.904616,9.919787,9.918452,9.899648,9.910963,9.90869,9.938971,9.954801,9.981691,9.984045,9.981051,10.029975,10.034807,10.03844,10.065286,10.109006,10.109944,10.100362,10.089463,10.095791,10.107466,10.104076,10.117328,10.140306,10.134798,10.1325,10.087966,10.068584,10.068044,10.065249,10.052034,10.008997,9.988354,9.969531,9.970891,9.96578,9.970711,10.084072,9.967556,9.981349,9.961129,9.950888,9.95344,9.974462,9.975183,9.957235,9.966519,9.953503,9.989354,10.009935,10.033248,10.024088,10.02764,10.070541,10.114055,10.075869,10.10084,10.145237,10.157191,10.139387,10.126234,10.137393,10.154639,10.143361,10.15408,10.135574,10.152999,10.143958,10.123936,10.151565,10.008097,10.015046,9.985144,9.974642,9.93486,9.89304,9.921284,9.91857,9.901325,9.889065,9.919409,9.934301,9.917372,9.904057,10.428832,9.929668,9.923601,9.906554,9.929929,9.908547,9.890444,9.953683,9.97622,9.982088,9.966998,10.025026,10.028938,10.0486,10.069423,10.131003,10.09681,10.080818,10.084712,10.117409,10.110242,10.096369,10.081737,10.087507,10.09763,10.058921,10.066926,10.015046,9.983405,10.27431,10.634918,10.013847,9.986758,9.982088,9.963923,9.963085,9.942703,9.956459,9.958614,9.973624,9.96103,9.948472,9.973524,9.964861,9.972208,9.95554,9.952068,9.957875,9.983964,10.009916,10.020176,10.023709,10.030335,10.071677,10.078384,10.089662,10.133878,10.135375,10.139846,10.130922,10.682265,10.135096,10.116651,10.152161,10.123097,10.126929,10.145156,10.219735,10.083234,10.067224,10.078365,10.071515,10.042812,10.009115,9.980194,10.532655,9.909628,9.904895,9.889805,9.891202,9.907653,9.927116,9.896114,9.930109,9.891463,9.915757,9.912702,9.898468,9.899424,9.870901,10.402961,9.953701,9.95536,9.951807,9.973804,10.020058,10.013748,10.028677,10.062833,10.09122,10.108826,10.077645,10.097369,10.086687,10.062653,10.093015,10.088066,10.087786,10.079042,10.0915,10.043731,10.013369,10.013487,10.030516,10.001731,9.971947,9.93971,9.946119,9.912242,9.870224,9.880943,9.858045,9.849482,9.839241,9.922582,9.86202,9.860759,9.892798,9.900685,9.847904,9.816425,9.881619,9.927513,9.878247,9.93019,9.969991,9.935238,9.977319,9.966439,9.997061,10.017102,10.030236,10.060058,10.212407,10.013108,10.000054,10.067125,10.051674,10.008358,10.017921,10.050717,10.021393,10.033968,9.969891,9.972487,9.968774,9.96442,9.885134,9.912242,9.881682,9.824411,9.852817,9.865672,9.869981,9.83549,9.872658,9.877328,9.846786,9.853854,9.862157,9.875236,9.86687,9.880961,9.87136,9.879564,9.861182,9.898729,9.932903,9.924619,9.961147,9.993347,10.25794,10.040855,10.082017,10.105833,10.137548,10.064212,10.075589,10.145436,10.090401,10.072037,10.075012,10.084333,10.073832,10.035844,10.030354,10.009935,10.006383,9.996142,9.966358,9.945299,9.895772,9.91318,9.911323,9.898629,9.875372,9.905796,9.924079,9.953422,10.436359,9.910926,9.912522,9.897747,9.894357,9.907212,9.905833,9.886811,9.950211,9.969413,9.978735,9.971009,10.018517,10.029975,10.047004,10.004507,10.016164,10.055928,10.017381,10.05499,10.054009,10.025125,10.010016,10.042812,10.03808,10.055766,10.034229,9.99223,9.976617,9.96506,10.508199,9.960589,9.920048,9.894555,9.885315,9.901902,9.885991,9.856008,9.890345,9.904318,9.877589,9.877788,9.893139,9.859306,9.885414,10.466261,9.891562,9.864274,10.056884,10.007501,10.000054,10.049519,10.019797,10.033571,10.056983,10.073614,10.081458,10.109025,10.14859,10.14338,10.604016,10.079421,10.046985,10.097288,10.103156,10.081259,10.065808,10.105591,10.081141,10.037043,10.014947,10.035807,10.009494,9.999235,9.952006,9.989336,9.91903,9.873236,9.916055,9.900865,9.909348,9.891102,9.92242,9.908069,9.896872,9.874732,10.134239,9.986361,9.963824,9.95005,10.213028,9.994763,10.022989,10.0281,10.030155,10.051096,10.087569,10.085631,10.094754,10.115831,10.160247,10.164439,10.139666,10.144777,10.15903,10.160545,10.147292,10.134257,10.123259,10.145156,10.14202,10.075788,10.066907,10.06982,10.065709,10.041775,10.020952,9.993068,9.99259,9.974804,9.970649,9.955341,9.956378,9.943181,9.998017,9.976779,9.969152,9.961048,9.985144,9.97073,9.969413,9.965259,9.994285,10.009575,10.018021,9.974363,9.98546,9.969432,10.029298,10.038142,10.039359,10.060859,10.104554,10.110025,10.090202,10.093754,10.124756,10.123358,10.094853,10.09068,10.093475,10.099542,10.068143,10.062833,10.0193,10.018319,10.027261,10.008059,9.974183,9.936617,9.926954,9.92919,10.136133,9.902181,9.911944,9.923781,9.926414,9.918111,9.933462,9.885035,9.927414,9.92388,9.916335,9.904895,9.916974,9.94474,9.956459,9.990273,10.018958,10.048401,10.083215,10.084793,10.030894,10.074869,10.088283,10.094673,10.085631,10.095791,10.094313,10.061318,10.077744,10.070298,10.087029,10.065889,10.111441,10.03934,10.009556,10.003805,10.029957,10.0066,10.155496,9.954422,9.939151,9.939052,9.923203,9.913378,9.915378,9.938871,9.935419,10.469714,9.916713,9.908808,9.929749,9.927513,9.910547,9.908889,9.918291,9.938971,9.963563,9.978257,9.978816,10.008618,10.024107,10.040855,10.632782,10.054189,10.102119,10.108727,10.083135,10.07531,10.107429,10.145355,10.084252,10.084172,10.076987,10.083955,10.051276,10.048302,10.063374,10.527184,10.020455,10.013568,9.963545,9.92855,9.926855,9.931345,9.922085,9.894555,9.899648,9.921365,9.93422,9.915117,9.937654,9.903958,9.951267,9.92434,9.915974,9.912801,9.881141,9.936276,9.965141,9.975002,9.970531,9.99708,10.017462,10.026324,10.047084,10.09132,10.111341,10.650146,10.09517,10.109845,10.103156,10.076707,10.107087,10.103697,10.103815,10.140225,10.13158,10.084252,10.067386,10.056487,10.083116,10.047724,10.044327,10.000632,9.983026,9.982169,9.9754,9.952105,9.960651,9.965122,9.974363,9.956577,9.954981,9.958334,9.977176,9.978077,9.959191,10.067187,9.961408,9.985821,10.003607,10.024846,10.018598,10.031975,10.075012,10.076825,10.040495,10.103635,10.157813,10.158607,10.12619,10.134636,10.130724,10.105212,10.152701,10.096089,10.090301,10.093816,10.09086,10.040495,10.042911,9.985523,10.022032,10.010512,9.969233,9.951447,9.930947,9.935518,9.921104,9.910304,9.90841,9.921824,9.936915,9.928171,9.937095,9.880564,9.925656,9.918552,9.912043,9.906094,9.907274,9.941685,9.957875,9.980114,9.99141,9.995204,10.028181,10.03834,10.06533,10.046227,10.126911,10.121222,10.106249,10.109242,10.104454,10.123675,10.105193,10.098486,10.082296,10.097549,10.088761,10.04365,10.042973,9.979772,10.0173,9.996521,9.966339,9.941927,9.937213,9.932543,9.919309,9.900865,9.917372,9.927053,9.920787,9.911782,9.92901,9.885712,9.927973,9.927233,9.913378,9.898449,9.930966,9.940548,9.975363,9.979114,10.087146,9.992149,10.022952,10.077663,10.118166,10.113217,10.144715,10.146572,10.128407,10.126271,10.136412,10.163023,10.147292,10.131562,10.131841,10.25209,10.06469,10.040936,10.004066,10.009078,10.023989,9.991652,9.963923,9.947814,9.940629,9.918291,9.90723,9.881439,9.899486,9.910646,10.403961,9.92406,9.896872,9.901225,9.918471,9.919346,9.905417,9.872776,9.906814,9.923979,9.948572,10.032372,10.026703,10.041973,10.083135,10.117192,10.100759,10.123557,10.168171,10.158651,10.147951,10.160067,10.137692,10.175418,10.149988,10.136673,10.145554,10.144516,10.118607,10.09114,10.563954,10.062933,10.066926,10.047103,10.021132,10.012071,9.980672,9.977275,9.96103,9.969233,9.942126,9.963365,9.992031,9.967836,9.962644,9.974804,9.972947,9.974804,9.97127,9.984405,9.97091,9.997918,10.006041,10.020256,10.031931,10.053152,10.086886,10.085551,10.093114,10.11172,10.655679,10.157632,10.151782,10.161644,10.149627,10.172903,10.160589,10.151981,10.139027,10.155297,10.143759,10.105411,10.070857,10.098604,10.024548,10.526227,9.97127,9.938033,9.952223,9.925457,9.92406,9.901225,9.908988,9.928351,9.910124,9.932264,9.910069,9.881719,9.921383,9.934779,10.357191,9.910745,9.916415,9.942045,9.966277,9.982827,9.987678,10.002948,10.036484,10.028361,10.075589,10.042731,10.101759,10.113857,10.089481,10.084153,10.103256,10.104815,10.110621,10.097288,10.147032,10.100561,10.081377,10.050798,10.037862,10.071497,10.020356,10.00714,9.943442,9.952826,9.91875,9.879167,9.910205,9.889805,9.9032,9.937735,9.943722,9.920048,9.903101,9.91354,9.928892,9.931525,9.918173,9.90851,9.914558,9.951646,9.958831,9.972686,9.989273,10.002209,10.083495,10.032273,10.047364,10.072317,10.100561,10.113136,10.09717,10.100939,10.093934,10.119148,10.100759,10.099461,10.090879,10.118067,10.080899,10.047482,10.031534,10.019716,10.06918,10.051674,10.009295,9.988255,9.984026,9.927035,9.92855,9.902262,9.887171,9.933462,9.932624,9.919707,9.911584,9.906833,9.923321,9.924917,9.905256,9.90869,9.912323,9.940169,9.962806,10.111143,9.971748,9.9969,10.028857,10.021852,10.05994,10.061238,10.10569,10.094791,10.100759,10.080241,10.061275,10.110304,10.09517,10.084072,10.191826,10.096946,10.102039,10.047463,10.027162,10.043948,10.023908,9.96624,9.964302,10.010314,9.936195,9.935058,9.927973,9.901225,9.919887,9.947615,9.938592,9.913198,9.901604,9.908069,9.936176,9.897449,9.917651,9.906355,9.918291,9.95005,9.964482,9.979853,10.020915,10.037043,10.566091,10.070578,10.086966,10.114236,10.158111,10.155415,10.13853,10.136493,10.138747,10.150646,10.152602,10.128289,10.13789,10.14877,10.132798,10.128506,10.06002,10.060859,10.063951,10.04886,10.01309,9.979592,9.969693,9.974642,9.97155,9.944541,9.939809,9.969792,9.967556,9.959949,10.500796,9.952267,9.963725,9.964023,9.965519,9.948274,9.961228,9.996502,10.006879,10.021293,10.01794,10.042551,10.079241,10.079402,10.09168,10.622063,10.087606,10.088923,10.089742,10.080818,10.060219,10.097685,10.0905,10.084091,10.06551,10.092438,10.092835,10.044209,10.014487,10.047482,10.541616,9.997421,9.957316,9.957595,9.930028,9.88901,9.916235,9.900405,9.914018,9.892581,9.930767,9.911106,9.899405,9.909628,9.928414,9.926873,9.908609,9.896872,9.922601,9.928712,9.956099,9.971748,9.967997,9.997639,10.000235,10.054648,10.04301,10.066547,10.028559,10.06918,10.025864,9.998819,10.038521,10.05445,10.051376,9.993645,10.033968,10.033888,10.030435,9.976959,9.976499,9.964221,9.971848,9.930028,9.931065,9.901362,9.841197,9.852177,9.841116,9.855412,9.818921,9.86697,9.896592,9.844594,9.850221,9.892382,9.878148,9.870143,9.850482,9.85104,9.849084,9.814251,9.900306,9.915298,9.99141,9.91857,9.954782,9.97594,9.998415,10.136133,10.14841,10.153558,10.138188,10.146634,10.140207,10.097207,10.100082,10.082098,10.082116,10.104833,10.045066,10.056406,10.004129,10.021672,10.06497,10.007103,9.942802,9.929929,9.923141,9.926973,9.908032,9.898089,9.894077,9.912062,9.934978,9.951627,9.920166,9.900865,9.916912,9.919148,9.908808,9.901442,9.88134,9.936195,9.958253,9.978257,9.95069,9.98646,10.028857,10.021771,10.047463,10.091916,10.100082,10.108547,10.097468,10.1002,10.105311,10.031652,10.054152,10.320899,10.034608,10.014686,10.046706,9.994447,9.984405,9.991509,9.997558,9.933382,9.919806,9.884476,9.89835,9.881222,9.879545,9.882917,9.926414,9.873055,9.873037,9.890363,9.870323,9.878446,9.878968,9.870603,9.871261,9.861598,9.864274,9.992509,10.008438,10.024169,10.031832,10.593856,10.088345,10.094394,10.083973,10.105212,10.135592,10.14302,10.131022,10.13322,10.134375,10.160365,10.102796,10.08483,10.080439,10.091059,10.615654,10.061517,10.011512,10.012531,10.006681,9.998937,9.954322,9.920968,9.923861,9.924159,9.912782,9.899747,9.898747,9.907032,9.925557,10.41394,9.915794,9.899207,9.924961,9.918949,9.912441,9.907473,9.921725,9.947435,9.964843,9.982647,9.986938,9.996738,10.021194,10.032553,10.089283,10.069342,10.11218,10.108727,10.093195,10.089345,10.099244,10.108727,10.083116,10.072534,10.088624,10.08547,10.056027,10.058642,10.005283,10.48201,10.013108,9.982765,9.960471,9.92424,9.923979,9.919328,9.911404,9.895934,9.894934,9.923899,9.926395,9.902921,9.932903,9.914776,9.926395,9.938971,9.92452,9.905734,9.886911,9.953863,9.962067,9.979194,9.963923,9.995484,10.018778,10.040197,10.043154,10.090121,10.098424,10.115372,10.084973,10.106609,10.09635,10.069342,10.097387,10.096189,10.089003,10.091158,10.100262,10.04365,10.033229,10.023349,10.033292,10.016182,9.977996,9.955918,9.944442,9.931326,9.935878,10.026883,9.95554,9.955819,9.975599,9.946137,9.983883,9.962445,9.964762,9.978555,9.961508,9.95544,9.964762,9.991869,10.026044,10.028199,10.023448,10.04868,10.075328,10.09086,10.117806,10.103598,10.157794,10.149907,10.13825,10.138368,10.14959,10.156235,10.158328,10.132021,10.137431,10.154459,10.076167,10.030516,10.005842,10.025386,10.017002,9.997241,9.95993,10.136313,9.939548,9.927973,9.926973,9.91372,9.901362,9.93386,9.926016,9.913937,9.908708,9.91839,9.911963,9.931668,9.91839,9.908249,9.923979,9.962247,9.964284,9.981088,9.974804,10.015984,10.03359,10.031714,10.046886,10.075869,10.102138,10.112459,10.094295,10.099542,10.103156,10.107348,10.551658,10.089761,10.088345,10.101219,10.131742,10.08455,10.060778,10.023628,10.03395,10.009736,9.964861,9.948491,9.935158,9.932084,9.922483,10.503051,9.894816,9.926476,9.922762,9.910006,9.896195,9.926656,9.930786,9.921644,9.902641,9.92927,9.919489,9.906653,9.968494,9.968593,10.551118,9.983368,10.028559,10.032111,10.045507,10.072416,10.102896,10.108764,10.11154,10.088047,10.115453,10.10084,10.11054,10.087047,10.081458,10.910229,10.135276,10.10048,10.068125,10.073453,10.075968,10.055766,10.026783,10.018039,9.989075,9.989932,9.977598,9.96129,9.958173,9.970612,10.536704,9.966339,9.927612,9.959812,9.974381,9.987479,9.974344,9.981592,9.965681,9.985144,10.002489,10.032832,10.030696,10.042153,10.076167,10.086867,10.087426,10.103535,10.154378,10.158111,10.145436,10.153341,10.139567,10.289438,10.14338,10.130804,10.136853,10.152962,10.137133,10.081657,10.594856,10.019436,10.014704,9.992329,9.968035,9.936356,9.896772,9.927873,9.909845,9.906454,9.876589,9.902623,9.92506,9.906373,9.899927,10.466442,9.927991,9.922762,9.909267,9.915018,9.909628,9.889065,9.97055,9.980989,9.961849,9.967656,10.011972,10.027442,10.038918,10.060977,10.133978,10.103175,10.090003,10.088544,10.104194,10.110062,10.110422,10.081918,10.087625,10.103337,10.066945,10.070739,10.021753,9.971388,9.972127,9.972009,9.922582,9.904138,9.864392,9.877347,9.873316,9.877229,9.839961,9.876471,9.88719,9.887948,9.894257,9.871062,9.873956,9.877428,9.868566,9.881042,9.845451,9.886134,9.936257,9.94492,9.891003,9.942902,9.962806,10.129345,9.956279,10.034546,10.04896,10.062734,10.035744,10.051357,10.019176,10.016803,10.007898,10.049717,10.018238,9.999415,10.061914,10.008177,9.96488,9.983026,9.974183,9.94456,9.906454,9.912323,9.907193,9.893537,9.859722,9.827783,9.87649,9.906653,9.843694,9.878167,9.860921,9.877949,9.889047,9.878446,9.920626,9.860263,9.842296,9.88188,9.920526,10.181846,9.966718,9.984442,10.028361,10.014804,10.066088,10.063951,10.098567,10.097567,10.08601,10.081458,10.051574,10.099244,10.093673,10.086109,10.059399,10.089183,10.088742,10.024386,10.005861,10.037583,10.014307,9.99213,9.955161,9.95041,9.919986,9.870162,10.130264,9.904678,9.908491,9.885613,9.928829,9.910646,9.904815,9.907951,9.922365,9.916434,9.89853,9.906256,9.927513,9.945479,9.96057,9.999595,9.930127,9.936717,9.928892,10.032968,9.982088,9.99662,10.032869,10.051475,10.065349,10.026883,10.03349,10.043632,10.046706,10.011531,10.592459,10.03459,10.037223,10.003246,9.996422,10.036943,9.982169,9.931345,9.931723,9.917931,9.863517,9.898008,9.8818,9.846507,9.834652,10.446718,9.873316,9.878825,9.884377,10.068684,9.852537,9.855909,9.850202,9.891742,9.858387,9.831137,9.889724,9.920409,9.926314,9.890562,10.472888,9.962427,10.103138,9.995682,10.021933,10.028199,10.006283,10.015623,10.045209,10.056307,10.029516,10.039421,10.057344,10.045886,9.99672,10.014947,9.946876,9.963166,9.963725,9.933922,9.902001,9.857089,9.871242,9.856251,9.854754,9.868746,9.85553,10.101101,9.974425,9.973425,10.508839,9.957316,9.967277,9.919968,9.900225,9.900244,9.940548,9.939989,9.954322,9.964762,9.975561,9.969152,9.991112,10.058064,10.045967,10.046265,10.105374,10.098406,10.090301,10.060939,10.115732,10.100443,10.09653,10.085109,10.091618,10.092438,10.071397,10.015723,10.042414,10.009755,10.020834,9.995602,9.972009,9.94043,9.893357,9.934779,9.915397,9.901461,9.889985,9.924538,9.928991,9.926016,9.899288,9.931922,9.927215,9.926016,9.88737,9.886513,9.851158,9.857567,9.89232,9.945498,9.943063,9.919309,9.966898,9.964824,9.968376,10.017182,10.063014,10.030236,10.027423,10.041532,10.019797,10.066827,10.032472,10.012171,10.023908,10.052953,9.990292,10.070541,10.018021,10.022871,10.010494,10.145814,9.896971,9.849643,9.857369,9.898747,9.88252,9.836707,9.835887,9.870323,9.873875,9.849581,9.846507,9.842675,9.868367,9.875832,9.868348,9.867789,9.847445,9.881682,9.981169,9.941306,9.864212,9.928351,9.983784,9.96139,9.996241,10.019238,10.048743,10.047662,10.026143,10.038936,10.029218,10.003967,10.026541,10.029218,10.021591,9.98179,10.067746,10.188274,9.9452,9.981728,10.014667,9.999955,9.958073,9.899027,9.898188,10.248357,9.857549,9.87585,9.894257,9.898909,9.853655,9.895195,9.835807,9.905616,9.875552,9.88206,9.837049,9.846786,9.858045,9.887091,10.39226,9.90823,9.930984,9.942883,9.957216,9.963563,10.004184,9.997719,10.028758,10.05445,10.02343,10.021014,10.011674,10.038999,10.013388,10.532015,10.0388,10.062355,10.052872,9.987497,9.962824,10.039936,9.971848,9.969053,9.951068,9.926675,9.911323,9.873497,9.878229,9.884675,9.893357,9.837546,9.874155,9.862057,9.846786,9.867889,9.889985,9.880843,9.856729,9.864473,9.898089,9.917272,9.904219,9.942144,9.949491,10.485283,9.96524,9.979393,9.983945,10.00742,10.061157,10.031913,10.024846,10.206258,10.035906,10.056785,10.038719,10.013369,10.034987,10.034509,10.055406,9.991211,9.960191,9.972785,9.992428,10.001893,9.908429,9.86633,9.851798,9.895195,9.896853,9.909727,9.832056,9.884874,9.89735,10.418412,9.898449,9.860722,9.859983,9.871621,9.842116,9.874136,9.862318,9.823753,9.888047,9.942685,9.906373,9.906932,9.96542,9.958713,10.450071,10.214462,10.047004,10.071938,10.035266,10.00596,10.034888,10.034906,10.029659,10.051475,10.03908,10.029559,10.056567,10.012729,9.940107,10.089922,9.952286,9.92973,9.919409,9.855828,9.853854,9.87667,9.87136,9.852239,9.86687,9.926016,9.928631,9.853971,9.893419,9.86112,9.86697,9.909069,9.849562,9.879806,9.808022,9.886811,9.935437,9.905535,9.865473,9.956676,9.988174,9.984721,10.017679,10.027721,10.067504,10.085172,10.045426,10.051935,10.061554,9.999893,10.025206,10.09032,10.021654,10.029038,10.041477,9.969612,9.976859,10.018021,9.991608,9.967575,9.931885,9.890643,9.913143,9.91354,9.852556,9.885432,9.880384,9.888867,9.886333,9.941368,9.886072,9.89122,9.889606,9.851158,9.858126,9.847507,9.856748,10.060517,9.90805,9.924259,9.920508,9.940927,9.987398,9.96542,10.000632,10.002886,10.050357,10.031832,10.013469,10.062194,9.997837,10.102119,10.03862,10.026622,10.009575,10.050935,10.049041,10.009935,9.986839,9.981449,9.953962,9.941567,9.902821,9.920148,9.907491,9.811376,9.842315,9.874975,9.857189,9.891922,9.86715,9.867429,9.864933,9.88252,9.907889,10.010873,9.853295,9.856468,9.921266,9.926973,9.895474,9.901703,9.924898,9.936077,9.945957,9.9861,9.991211,10.046724,10.060436,10.064492,10.044967,10.00614,10.02874,10.06415,10.594713,10.01345,10.023511,10.026243,10.015723,10.011531,9.995701,9.957235,9.96578,9.931164,9.921744,9.921427,9.847687,9.880762,9.885594,9.87713,9.863697,9.847886,9.8592</t>
+  </si>
+  <si>
+    <t>11.720755,11.820945,11.944808,11.924047,11.948161,11.931276,11.896101,11.955508,11.946484,11.960998,11.917899,11.924146,11.884066,11.915942,11.915663,11.847233,11.850189,11.765631,11.64632,11.633005,11.498424,11.388931,11.397595,11.391608,11.37027,11.3636,11.37458,11.371505,11.414362,11.406519,11.433589,11.360246,11.376436,11.383882,11.366376,11.402966,11.412766,11.462752,11.445904,11.446301,11.481873,11.589906,11.73343,11.83398,11.895821,11.927319,11.891611,11.919557,11.913508,11.928878,11.868633,11.950217,11.91734,11.885562,11.851189,11.836756,11.782299,11.826832,11.88622,11.700075,11.612704,11.544634,11.407556,11.301181,11.370947,11.34356,11.299343,11.353161,11.316011,11.358893,11.338231,11.33312,11.345597,11.872806,11.327469,11.360526,11.306671,11.328767,11.339864,11.411648,11.432049,11.372207,11.470155,11.561203,11.667478,11.770922,11.905242,11.883724,11.901032,11.921153,11.905422,11.879631,11.831086,11.8865,11.867236,11.917241,11.877259,11.833322,11.836396,11.865739,11.769822,11.733772,11.61466,12.063379,11.440613,11.331642,11.306671,11.337411,11.361824,11.310503,11.328009,11.321104,11.340026,11.372841,11.329009,11.287047,11.390589,11.337231,11.365736,11.359868,11.34328,11.388652,11.38061,11.45199,11.43798,11.518824,11.608332,11.794856,11.820467,11.884923,11.862963,11.886879,11.881109,12.427304,11.892586,11.861808,11.871328,11.900212,11.887978,11.846475,11.866056,11.794297,11.783255,11.688077,11.578349,11.554235,11.441992,11.302839,11.874601,11.349267,11.35408,11.377536,11.349329,11.335933,11.383882,11.37558,11.377654,11.457461,11.383802,11.399253,11.383982,11.29625,11.335014,11.923109,11.353278,11.401029,11.458182,11.568767,11.650152,11.786608,11.837371,11.894983,11.948919,11.885103,11.850847,11.859429,11.894343,11.856256,11.951036,11.845717,11.852983,11.811182,11.816033,11.798607,11.85502,11.695225,11.614958,11.513254,11.403364,11.36442,11.342622,11.297026,11.326314,11.37961,11.29707,11.428677,11.376356,11.303057,11.386578,11.343541,11.318228,11.338709,11.335555,11.334139,11.359607,11.34356,11.414505,11.487543,11.421032,11.529903,11.653604,11.727363,11.83462,11.90133,11.926065,11.903628,11.900193,11.912688,11.863404,11.880532,11.829527,11.911173,11.909695,11.798228,11.768705,11.856517,11.856697,11.753632,11.658436,11.545112,11.446562,11.448239,11.360066,11.412828,11.441892,11.351304,11.359967,11.420293,11.298126,11.391329,11.332859,11.288984,11.348509,11.350528,11.319545,11.305274,11.344218,11.366575,11.453729,11.387615,11.470695,11.531698,11.643264,11.734592,11.875899,11.84396,11.867993,11.909496,11.871788,11.894722,11.843202,11.893685,11.871148,11.849531,11.883066,11.846475,11.817952,11.836396,11.785093,11.716247,11.614281,11.566811,11.409295,11.311981,11.323078,11.359588,11.340107,11.369829,11.35326,11.32745,11.44301,11.396558,11.902709,11.462311,11.369928,11.389571,11.364979,11.366115,11.424503,11.485146,11.440594,11.430751,11.489121,11.620908,11.699219,11.807053,11.856157,11.92273,11.988105,11.959979,11.91221,11.877197,11.825714,11.917123,11.860069,11.887717,11.846078,11.842004,11.803059,11.841426,11.795415,11.691313,12.151713,11.522376,11.393465,11.348211,11.350024,11.347534,11.334536,11.395918,11.341324,11.347689,11.37466,11.319545,11.330406,11.301082,11.314496,11.911012,11.321023,11.295791,11.343001,11.386677,11.396477,11.426919,11.425702,11.57761,11.678719,11.791502,11.81925,11.9285,11.931493,11.92265,12.398898,11.896399,11.822342,11.878234,11.850766,11.901131,11.863702,11.810325,11.760122,11.830068,11.762277,11.704429,11.636539,11.552937,11.398712,11.360588,11.288146,11.337592,11.340684,11.307509,11.36396,11.358551,11.315514,11.302957,11.402687,11.30787,11.315614,11.367295,11.367953,11.381187,11.66215,11.370468,11.390509,11.407177,11.442668,11.647158,11.753316,11.814896,11.920873,11.985509,11.900473,11.976089,11.999725,11.904845,11.934846,11.965127,11.912949,11.977125,11.891847,11.893306,11.893884,11.944826,11.808351,11.741796,11.627633,11.599569,11.474129,11.392906,11.372406,11.412586,11.359588,11.41227,11.40568,11.344777,11.393086,11.41584,11.391148,11.392366,11.392626,11.379032,11.378032,11.355974,11.390031,11.484966,11.411928,11.390409,11.497126,11.581305,11.683209,11.785571,11.827093,11.851126,11.911688,11.902907,11.910173,11.88586,11.909217,11.933052,11.878396,11.877197,11.838172,11.836675,11.838271,11.832583,11.810984,11.675545,11.631608,11.57789,11.438557,11.354458,11.346814,11.318967,11.363879,11.379411,11.362302,11.326593,11.353819,11.321184,11.346435,11.317787,11.32791,11.371388,11.41117,11.29589,11.382783,11.432508,11.456244,11.492195,11.549646,11.589527,11.730617,11.805773,11.866037,11.945006,11.879054,11.934846,11.904882,12.002935,11.915185,11.963991,11.900473,11.905602,11.910695,11.929655,11.892946,11.839967,11.782659,11.72309,11.626118,11.550024,11.379511,11.314297,11.286749,11.361426,11.349987,11.272875,11.353719,11.329885,11.315794,11.374399,11.320762,11.322321,11.296331,11.374381,11.334878,11.314117,11.368531,11.399433,11.429434,11.393844,11.431291,11.576772,11.671192,11.773654,11.904783,11.905062,11.81797,11.94323,11.887798,11.877576,11.919675,11.89666,11.892946,11.872266,11.835377,11.855679,11.805376,11.856076,11.830807,12.336697,11.686165,11.601047,11.446823,11.399532,11.389689,11.419175,11.427298,11.433347,11.360408,11.315415,11.320545,11.353421,11.366177,11.384342,11.329885,11.325016,11.324718,11.375039,11.351546,11.409295,11.440215,11.376815,11.481855,11.586453,11.654604,11.762358,11.887438,11.905143,11.852325,12.455169,11.870111,11.908099,11.852803,11.914446,11.926984,11.90682,11.876837,11.858473,11.784975,11.802699,11.817691,11.760861,11.550881,11.532238,11.947422,11.350627,11.381945,11.407078,11.387435,11.413064,11.351484,11.387553,11.396856,11.424864,11.3529,11.422168,11.383125,11.42297,11.383143,11.877576,11.387615,11.442948,11.51072,11.446382,11.519942,11.588671,11.749981,11.867975,11.887574,11.97992,11.88532,11.934766,11.919774,11.926003,11.913527,11.975206,11.989124,11.92804,11.944069,11.912589,11.828372,11.910192,11.815275,11.769642,11.677259,11.579529,11.471713,11.367972,11.373542,11.456523,11.361364,11.271478,11.331841,11.329208,11.39077,11.31162,11.335095,11.297828,11.356396,11.359948,11.359327,11.326991,11.350347,11.363581,11.417157,11.393881,11.443128,11.647475,11.643823,11.745131,11.809785,11.946863,11.847773,11.961116,11.900293,11.873024,11.888655,11.911912,11.910875,11.863982,11.832502,11.802041,11.797011,11.883444,11.750999,11.691493,11.65566,11.554874,11.387236,11.350204,11.320085,11.390292,11.298685,11.364159,11.308627,11.371226,11.277526,11.351447,11.293816,11.358272,11.367475,11.350645,11.333859,11.322582,11.330704,11.389553,11.433347,11.365817,11.494412,11.565034,11.666478,11.784075,11.820206,11.845438,11.885401,11.889512,11.874601,11.911192,11.786969,11.834638,11.889574,11.90736,11.817511,11.882066,11.853424,11.784534,11.791043,11.698399,11.601526,11.521637,11.427081,11.347751,11.373263,11.319365,11.304913,11.329208,11.357713,11.310403,11.514073,11.331003,11.345156,11.325215,11.403625,11.389273,11.376617,11.281737,11.372443,11.409493,11.407916,11.447102,11.473949,11.553117,11.65602,11.792061,11.839768,11.884842,11.864541,11.849909,11.977026,11.91249,11.940554,11.981615,11.915384,11.902087,11.981957,11.820367,11.809506,11.842544,12.316116,11.700995,11.60514,11.510738,11.406898,11.308708,11.306392,11.339945,11.313117,11.298685,11.336294,11.312279,11.363501,11.336672,11.384839,11.907559,11.35408,11.386398,11.362563,11.355396,11.322519,11.352664,11.426982,11.431931,11.417598,11.632266,11.673707,11.752875,11.876477,11.924885,12.353564,11.905143,11.911192,11.860871,11.89648,11.902069,11.886338,11.86582,11.87534,11.767028,11.844239,11.8553,11.861187,11.702671,11.616256,11.547348,11.459219,11.375058,11.344777,11.378871,11.346634,11.341063,11.368692,11.305174,11.320004,11.392366,11.337672,11.326215,11.365339,11.32773,11.9177,11.347112,11.339827,11.403345,11.425242,11.373083,12.137001,11.589987,11.708062,11.746807,11.886338,11.892108,11.866199,11.940696,11.863801,11.861249,11.867894,11.899355,11.883426,11.888177,11.786652,11.875601,11.82182,11.785373,11.815437,11.699678,11.598669,11.539604,11.406041,11.306311,11.349428,11.344317,11.344758,11.329388,11.329406,11.307348,11.356253,11.366736,11.295493,11.313279,11.40093,11.334878,11.371866,11.309484,11.905522,11.410431,11.409972,11.385479,11.497622,11.5509,11.727444,11.820585,11.909155,11.929158,11.955328,11.919017,11.913409,11.95906,11.913806,11.934846,11.893306,11.841525,11.824876,11.876557,11.849369,11.809468,11.78046,11.706565,11.626956,11.509801,11.435123,11.312242,11.328208,11.302678,11.375157,11.379312,11.323159,11.306149,11.362563,11.337691,11.41153,11.282873,11.368115,11.322439,11.352701,11.323637,11.3539,11.378113,11.422547,11.475166,11.507186,11.554154,11.642507,11.815095,11.858194,11.929816,11.897715,11.8436,11.873924,11.845159,11.898896,11.917123,11.890151,11.837135,11.912012,11.803078,11.864342,11.789086,11.828273,11.718961,11.606574,11.496467,11.449798,11.363501,11.283494,11.330841,11.382007,11.328108,11.349888,11.711055,11.98962,11.380889,11.366854,11.360886,11.430173,11.433465,11.376617,11.353881,11.410332,11.427099,11.516048,11.45189,11.498343,11.6143,12.088692,11.77122,11.913508,11.859392,11.898734,11.869931,11.860429,11.860746,11.821702,11.873365,11.902348,11.865497,11.845357,11.830086,11.806674,12.30895,11.792918,11.721675,11.609288,11.514173,11.402966,11.311322,11.361544,11.329425,11.977045,11.340883,11.317949,11.31308,11.370847,11.321501,11.355856,11.329127,11.347012,11.35893,11.307807,11.336672,11.337213,11.428298,11.435862,11.397216,11.51108,11.563718,11.689437,11.852145,11.927021,12.433669,11.968183,11.940616,11.955427,11.982553,11.873546,11.902727,11.969021,11.875222,11.919756,11.84899,11.870093,11.85969,11.877955,11.746329,11.704429,11.611145,11.358191,11.336113,11.328009,11.337231,11.391148,11.389472,11.305472,11.393906,11.361426,11.378293,11.354819,11.372145,11.317688,11.944609,11.326531,11.298008,11.413505,11.372083,11.414064,11.376256,11.509819,11.533555,11.69217,11.758346,11.885562,11.899156,11.899933,11.887158,12.37071,11.868074,11.867857,11.898156,11.90251,11.903584,11.893108,11.836874,11.879252,11.82292,12.378535,11.666621,11.613741,11.502914,11.418517,11.570903,11.382268,11.355477,11.380051,11.341784,11.31739,11.378852,11.350987,11.360905,11.312179,11.373263,11.360507,11.346273,11.331624,11.316812,11.414983,11.356135,11.472714,11.445724,11.44732,11.567991,11.68722,11.744671,11.876377,11.848972,11.895722,11.907658,11.853362,11.824,11.896101,11.869751,11.835638,11.905882,12.422653,11.899355,11.900392,11.875259,11.871067,11.776871,11.670092,11.623802,11.493213,11.363761,11.430651,11.443109,11.396756,11.379051,11.36927,11.383901,11.448239,11.384361,11.345056,11.362743,11.406879,11.359309,11.409493,11.393726,11.39444,11.444985,11.571344,11.454784,11.527227,11.599191,11.741038,11.869534,11.908596,11.897877,11.947782,11.983435,11.953191,11.918017,11.920234,11.905981,11.994974,11.916681,11.917619,11.8328,11.834819,11.80817,11.823398,11.69171,11.625801,11.526829,11.395079,11.340485,11.320923,11.316912,11.358632,11.371108,11.324078,11.371487,11.392825,11.320563,11.358191,11.353719,11.363103,11.366755,11.336275,11.32845,11.431633,11.418175,11.429056,11.402588,11.502175,11.53771,11.732915,11.774853,11.851884,11.868894,12.470142,11.829509,11.904485,11.881389,11.925463,11.952055,11.901709,11.845618,11.908235,11.903466,12.457125,11.889313,11.890232,11.724289,11.665305,11.575654,11.478321,11.392726,11.347391,11.38015,11.418237,11.349428,11.414244,11.383522,11.361464,11.392744,11.355613,11.383342,11.4368,11.389553,11.428236,11.382206,11.429695,11.455207,11.444966,11.480737,11.489941,11.615859,11.95321,11.809586,12.478607,11.936424,11.947341,11.976567,11.907099,11.871906,11.948142,11.91706,11.940318,11.90808,11.901609,11.8552,11.908577,11.899653,11.86436,12.311825,11.605835,11.47888,11.438719,11.299504,11.346652,11.33797,11.306031,11.307348,11.325034,11.370866,11.363681,11.323898,11.303634,11.329965,11.864938,11.315632,11.350546,11.363761,11.37915,11.391446,11.462491,11.379808,11.478862,11.542082,11.666658,11.78723,11.903187,11.882209,11.929239,11.959799,11.899635,11.894524,11.846935,11.847034,11.865379,11.872924,11.850189,11.839308,11.77697,11.811263,11.826615,11.730139,11.627118,11.506907,11.462113,11.345497,11.338511,11.360905,11.409214,11.330146,11.341523,11.317688,11.365556,11.365078,11.397657,11.340268,11.322582,11.334959,11.888537,11.408655,11.450475,11.439197,11.447301,11.478222,11.547888,11.572102,11.71367,11.80709,11.928617,11.933828,11.916942,11.929338,11.972356,11.885401,11.900491,11.974033,11.961116,11.953831,11.924867,11.913067,11.897877,11.864603,11.811903,11.70918,11.67221,11.553297,11.493114,11.35911,11.344218,11.32791,11.360209,11.311801,11.409052,11.306274,11.318607,11.347454,11.894126,11.33779,11.345777,11.375716,11.352043,11.364041,11.365979,11.37063,11.448699,11.437439,11.465187,11.548726,11.711794,11.795911,11.8757,11.91752,11.867813,11.914744,11.887618,11.84927,11.904963,11.903286,11.904746,11.849071,11.92722,11.796651,11.868894,11.844898,11.792539,11.746348,11.603401,11.524711,11.449456,11.402706,11.363861,11.422007,11.368314,11.563637,11.325755,11.366078,11.38528,11.352782,11.313018,11.355558,11.359948,11.377455,11.358172,11.371785,11.334635,11.413604,11.420113,11.449257,11.534294,11.539802,11.693828,11.762817,11.882668,11.897598,11.880749,11.895002,11.87534,11.925363,11.928996,11.891747,11.918259,11.886761,11.865658,12.409717,11.835675,11.767388,11.800203,11.669056,11.646239,11.498622,11.396756,11.330524,11.649133,11.38482,11.378952,11.382684,11.407177,11.358911,11.932412,11.429217,11.382206,11.355495,11.358253,11.410972,11.375877,11.406978,11.467279,11.448239,11.461013,11.44319,11.503112,11.673328,11.725047,12.353402,11.916421,11.917321,11.980137,11.899833,11.917719,11.939939,11.906043,11.950297,11.950316,11.909813,11.978442,11.922569,11.811164,11.902367,11.816492,11.783156,11.885382,11.606096,11.460517,11.393105,11.378032,11.34805,11.401768,11.396918,11.394403,11.34795,11.423746,11.399433,11.431192,11.913247,11.414064,11.436781,11.356514,11.459138,11.417579,11.475924,11.488562,11.454207,11.495089,11.622286,11.699877,11.814697,11.917421,11.936244,11.934784,11.961954,11.925426,11.939697,11.919197,11.906242,11.880253,11.945627,11.948801,11.872167,11.811903,11.849909,11.79657,11.748124,11.611505,11.57276,11.434148,11.397638,11.373841,11.329009,11.360886,11.312639,11.33258,11.357452,11.363761,11.355595,11.299523,11.346553,11.356433,11.376995,11.348788,11.347689,11.341622,11.418796,11.473409,11.455766,11.470298,11.574778,11.67221,11.786031,11.824578,11.908198,11.912111,11.894604,11.870012,11.881172,11.886959,11.949378,11.921631,11.871608,11.847394,11.829608,11.803979,11.827273,11.804817,11.693847,11.627335,11.542001,11.395403,11.335635,11.330344,11.348491,11.346093,11.352161,11.328829,11.347491,11.391887,11.405103,11.353881,11.361066,11.304715,11.343181,11.354179,11.377474,11.357334,11.357632,11.413865,11.403426,11.470975,11.523873,11.685407,11.757806,11.813778,11.866578,11.901789,11.904646,11.877017,11.879433,11.942609,12.000221,11.945447,11.95906,11.951055,11.910813,11.896821,11.874682,11.889673,11.816374,11.681252,11.591123,11.44832,11.384423,11.371965,11.385497,11.798309,11.392086,11.377275,11.377915,11.448537,11.38546,11.352863,11.394682,11.3851,11.401488,11.426261,11.364898,11.406258,11.435924,11.47421,11.858572,11.505988,11.742454,11.707882,11.83408,11.859672,11.899535,11.861268,11.91139,11.880749,11.862243,11.890611,11.923271,11.877017,11.904485,12.404028,11.819728,11.816194,11.85017,11.781082,11.721358,11.644742,11.506808,11.430651,11.372164,11.302119,11.386497,11.358632,11.386578,11.329866,11.400191,11.329767,11.413406,11.33322,11.379889,11.377374,11.379529,11.352043,11.34831,11.319824,11.406419,11.460237,11.388453,11.529146,11.614101,12.288729,11.855579,11.965966,11.897138,11.890052,11.930474,11.940175,11.906422,12.012996,11.885562,11.926661,11.936784,11.875899,11.906801,11.865956,11.866118,11.819069,11.741678,11.62464,11.589049,11.440793,11.392229,11.385938,11.406239,11.394881,11.439557,11.373561,11.393366,11.393763,11.396936,11.927319,11.401308,11.335375,11.414921,11.374201,11.433986,11.447158,11.464988,11.44265,11.458299,11.532716,11.675663,11.72922,11.857995,11.903808,12.365841,11.939616,11.934107,11.930294,11.951074,11.881029,11.940616,11.951974,11.901771,11.889114,11.910416,11.869471,11.843562,11.865739,11.79226,11.777747,11.592123,11.413785,11.412567,11.373245,11.404445,11.416381,11.358731,11.351186,11.416859,11.319706,11.425062,11.35847,11.388534,11.397837,11.345354,11.346416,11.344975,11.394403,11.433428,11.482495,11.458299,11.451133,11.570822,11.664305,11.758743,11.854859,11.852163,11.853182,11.886779,11.871825,11.879035,11.880551,11.901032,11.894045,11.924146,11.861647,11.86015,11.835297,11.829211,11.795893,11.730617,11.621187,11.506547,11.395918,11.346913,11.351123,11.374778,11.362644,11.35875,11.322159,11.355117,11.355117,11.428298,11.34823,11.422168,11.424926,11.424125,11.411729,11.389453,11.409313,11.434384,11.455964,11.439675,11.482234,11.639072,11.724109,11.849251,11.884444,11.949838,11.915284,11.907279,11.916402,11.964829,11.923289,11.887357,11.910173,11.9392,11.890692,11.973294,11.899094,11.917799,11.806133,11.762078,11.621467,11.57294,11.401867,11.388354,11.369369,11.393763,11.340703,11.400209,11.404761,11.372425,11.404842,11.407338,11.361265,11.381647,11.396458,11.396999,11.411648,11.443209,11.40101,11.484469,11.532536,11.494151,11.531499,11.60891,11.705628,11.816095,11.867155,11.936703,11.955446,11.905683,11.972474,11.97004,11.913825,11.931033,11.925444,12.426006,11.89071,11.85969,11.87662,11.898896,11.868497,11.737144,11.669614,11.564097,11.458958,11.355378,11.316452,11.348012,11.34841,11.318588,11.336654,11.365059,11.425783,11.33789,11.351763,11.311503,11.346894,11.4163,11.311602,11.322501,11.340187,11.413325,11.434347,11.431471,11.529264,12.15221,11.720836,11.805115,11.856076,11.894163,11.871608,11.95924,11.884742,11.88137,11.853921,11.895884,11.894623,11.938579,11.893325,11.899355,12.351589,11.824938,11.798228,11.765233,11.664205,11.559625,11.45902,11.41063,11.356235,11.439098,11.40029,11.334058,11.347112,11.377356,11.424224,11.896082,11.356955,11.367196,11.410133,11.412288,11.378132,11.469279,11.41153,11.479439,11.469261,11.507087,11.495169,11.648872,11.740877,11.852505,11.94323,11.925065,11.914328,12.013654,11.947422,11.918998,11.950018,11.926301,11.925084,11.924308,11.872365,11.915123,11.893406,11.861845,11.836098,11.777765,11.611307,11.584559,11.45271,11.401371,11.362265,11.433527,11.429795,11.429515,11.349347,11.401308,11.412288,11.378132,11.372524,11.363942,11.400532,11.392546,11.369928,11.410052,11.419455,11.422709,11.448059,11.433328,11.498442,11.634483,11.695325,11.771102,11.839768,11.9059,11.869633,11.870968,11.87516,11.870211,11.871248,11.868074,11.898057,11.847872,11.864901,11.849611,11.825994,11.82767,11.794135,11.652468,11.670751,11.513974,11.450555,11.360967,11.345696,11.34813,11.279284,11.34877,11.345634,11.358731,11.3119,11.329109,11.371027,11.350906,11.295033,11.376256,11.348491,11.318607,11.380448,11.38464,11.388093,11.391788,11.526748,11.564358,11.673806,11.752316,11.874564,11.895082,11.847494,11.875042,11.911651,11.828031,11.808568,11.886798,11.851487,11.991558,11.830266,11.865342,11.836098,11.810145,11.7499,11.730717,11.606276,11.515309,11.396837,11.282196,11.610847,11.325774,11.344019,11.321284,11.301759,11.282476,11.355676,11.329307,11.325034,11.322159,11.362302,11.370568,11.347751,11.389652,11.374841,11.393024,11.399451,11.415263,11.428596,11.516787,11.625578,11.829987,11.841805,11.888456,11.868434,11.917439,11.811462,11.894983,11.880731,11.957501,12.38151,11.884382,11.835756,11.893865,11.813679,11.82282,11.779765,11.725245,11.622286,11.5207,11.521718,11.292518,11.291562,11.360886,11.345137,11.859889,11.350447,11.315992,11.361445,11.345218,11.382945,11.334617,11.349049,11.339486,11.364817,11.296051,11.291518,11.421212,11.437918,11.461653,11.988124,11.671192,11.661889,11.803637,11.817213,11.900951,11.922811,11.890909,11.816492,11.85484,11.852443,11.878973,11.903466,11.827012,11.805295,11.871887,11.826994,11.829248,11.811462,11.670533,11.645121,11.521917,11.363761,11.380268,11.355198,11.308248,11.33394,11.354359,11.365078,11.342342,11.834197,11.320166,11.273173,11.355198,11.334337,11.307447,11.323159,11.347112,11.388255,11.493735,11.441433,11.457542,11.503094,11.620187,11.781181,11.825056,11.988962,11.878874,11.899175,11.878514,11.891089,11.889493,11.858473,11.862963,11.877377,11.846556,11.877855,11.910092,11.807351,11.821144,11.790962,11.699417,11.590888,11.465466,11.38995,11.334797,11.323438,11.308348,11.341802,11.330984,11.336474,11.314676,11.331903,11.386938,11.347373,11.415561,11.329866,11.35344,11.43662,11.433986,11.377933,11.479501,11.491437,11.462013,11.551521,11.581342,11.709956,11.834017,11.879352,11.984789,11.899374,11.937361,11.875899,11.847854,11.825596,11.867317,11.860311,11.905044,11.913247,11.864323,11.832142,11.800464,11.769704,11.734132,11.617653,11.541597,11.402786,11.305833,11.289264,11.347472,11.369468,11.331723,11.341504,11.295573,11.335536,11.343839,11.334337,11.362662,11.323078,11.349428,11.34805,11.367314,11.38995,11.393906,11.389391,11.46369,11.509981,11.606457,11.757905,11.811741,11.87616,11.839551,11.864162,11.938659,11.892549,11.874763,11.850648,11.877737,11.897399,11.910453,11.898256,11.846376,11.757725,11.791701,11.854002,11.698579,11.576753,11.527425,11.383603,11.405879,11.32709,11.451034,11.41702,11.414083,11.371984,11.41566,11.406239,11.372803,11.371866,11.370947,11.41145,11.435843,11.3958,11.393123,11.414027,11.397116,11.399514,11.393781,11.492375,11.527767,11.732313,11.833322,11.842662,11.861746,11.910596,11.875961,11.909236,11.909136,11.864342,11.960358,11.915942,11.894803,11.874322,11.819864,11.793477,11.819548,11.787869,11.705646,11.613822,12.115042,11.435582,11.400209,11.408494,11.393664,11.440874,11.38015,11.40001,11.389192,11.418175,11.463491,11.376617,11.34941,11.394899,11.377852,11.372884,11.40578,11.460337,11.458399,11.485208,12.055734,11.516967,11.630987,11.747844,11.814517,11.978343,11.996327,11.920234,11.914545,11.914347,11.93738,11.948441,11.942212,11.905143,11.966605,11.915862,11.878874,11.936523,11.895262,11.864801,11.730239,11.639712,11.586534,11.479818,11.401488,11.394502,11.451592,11.384541,11.419175,11.393005,11.957924,11.409574,11.427279,11.378771,11.404382,11.435763,11.400551,11.433806,11.429695,11.426261,11.430453,11.46808,11.469857,11.560464,11.658057,12.262081,11.852443,11.946025,11.896697,11.949999,11.987466,12.020603,11.947819,11.951055,11.950397,11.947143,12.201935,11.88586,11.902168,11.84378,12.370692,11.911651,11.693089,11.642687,11.593819,11.427739,11.378852,11.410791,11.427758,11.445742,11.387056,11.396458,11.391906,11.371145,11.364122,11.407158,11.436862,11.372443,11.432012,11.376275,11.354837,11.418896,11.508304,11.532617,11.45271,11.559905,11.631906,11.736865,11.836315,11.950856,11.920414,11.927021,11.932232,11.932791,12.188521,11.867975,11.902429,11.967543,11.917979,11.951893,11.907198,11.900672,11.898256,11.856536,11.717005,11.658976,11.591546,11.446003,11.386298,11.409593,11.42187,11.425062,11.402246,11.377635,11.442389,11.464988,11.423205,11.398216,11.378393,11.403066,11.435384,11.417778,11.376076,11.409574,11.446283,11.465305,11.513173,11.493872,11.633645,11.768326,11.81797,11.946683,11.999004,11.923289,11.99503,11.926841,11.874781,11.912129,11.849648,11.885618,11.866578,11.847313,11.78759,11.851487,11.795334,11.763277,11.740659,11.676421,11.484469,11.385261,11.318508,11.397657,11.36899,11.345578,11.36863,11.345398,11.298026,11.33815,11.330164,11.360687,11.337051,11.338989,11.328848,11.382026,11.347652,11.405482,11.397278,11.44696,11.378672,11.500119,12.268788,11.731518,11.816474,11.906441,11.946286,11.943112,11.987087,11.916222,11.879793,12.172511,11.835477,11.940417,11.873924,11.883165,11.797129,11.866199,11.782777,11.811723,11.683227,11.587174,11.474887,11.375201,11.325693,11.351645,11.362265,11.316173,11.376995,11.333481,11.320625,11.362743,11.342342,11.34374,11.3733,11.350528,11.352701,11.329506,11.305112,11.373822,12.024075,11.983075,11.393123,11.507565,11.573157,11.716545,11.842382,11.895002,11.888773,11.881749,11.881849,11.890512,11.983715,11.909055,11.942193,11.97425,12.479004,11.853244,11.839687,11.788248,11.82759,11.784615,11.64696,11.598253,11.528487,11.428397,11.328947,11.331723,11.319265,11.361625,11.312819,11.848891,11.36881,11.376436,11.318688,11.324737,11.31793,11.33276,11.356315,11.342361,11.31629,11.340926,11.420013,11.41145,11.423367,11.470577,11.641488,11.694207,11.769164,11.894064,11.902709,11.862485,11.89666,11.879631,11.847475,11.894225,11.857275,11.917737,11.891648,11.884401,11.809145,12.300783,11.893847,11.764314,11.661131,11.657877,11.48868,11.445643,11.345236,11.343821,11.378852,11.335915,11.356198,11.383261,11.347851,11.334319,11.992297,11.382026,11.340585,11.421572,11.409972,11.384541,11.356893,11.394384,11.458579,11.462212,11.450276,11.528227,11.619312,11.769885,11.824876,11.908478,11.912471,11.955986,11.986807,11.977703,11.883444,11.95393,11.915843,11.944826,11.955328,11.856238,11.920973,11.929257,11.863684,11.817871,11.767307,11.667317,11.506565,11.439296,11.407637,11.382243,11.414983,11.370667,11.690934,11.356794,11.358948,11.370748,11.311819,11.304237,11.334797,11.318489,11.345615,11.321843,11.311062,11.38043,11.369071,11.378473,11.396936,11.491375,11.548627,11.699759,11.801122,11.858771,11.842265,11.925922,11.907838,11.91267,11.882587,11.849549,11.870111,11.890611,11.855958,11.839669,11.874943,11.788167,11.808586,11.773095,11.665025,11.624938,11.543777,11.382026,11.331065,11.317849,11.312838,11.403724,11.313279,11.324016,11.329109,11.346075,11.312179,11.396657,11.332462,11.33889,11.348689,11.373723,11.326811,11.3539,11.394403,11.406221,11.449798,11.49471,11.563736,11.728562,11.846078,11.889493,11.899175,11.874483,11.864541,11.908298,12.356619,11.894163,11.929915,11.892909,11.904584,11.942094,11.792098,11.822423,11.847835,11.820287,12.250543,11.709558,11.562339,11.47852,11.392167,11.864801,11.385,11.407897,11.355359,11.409574,11.366376,11.391546,11.451114,11.380547,11.38482,11.455108,11.380249,11.348149,11.387534,11.41153,11.907838,11.494611,11.431931,11.589627,11.566413,11.698138,11.794514,11.889114,11.890971,11.91688,11.895082,11.863504,11.888556,11.884761,11.876458,11.882066,11.930853,11.857455,12.390533,11.873825,11.789006,11.785472,11.709298,11.583857,11.477843,11.476005,11.305093,11.349608,11.373102,11.347652,11.929717,11.319066,11.307528,11.372803,11.34392,11.390031,11.353341,11.371586,11.37558,11.36332,11.329425,11.4065,11.437539,11.417399,11.405761,11.518824,11.664783,11.758445,11.842482,11.890611,11.888357,11.993533,11.91139,11.932331,11.96858,11.918936,11.849549,11.885941,11.864919,11.861069,12.111409,11.849251,11.845258,11.826273,11.677321,11.581802,11.523737,11.397377,11.302758,11.338051,11.392428,11.347472,11.376455,11.31629,11.325333,11.692151,11.36432,11.290102,11.382845,11.331381,11.372282,11.31208,11.341864,11.425801,11.4163,11.436322,11.383224,11.469496,11.627515,11.727444,11.816492,11.865956,11.91121,11.940976,12.161811,11.957582,11.936045,11.927742,11.947962,11.917439,11.942771,11.923848,11.893865,11.911931,11.862945,11.808388,11.734952,11.643805,11.542678,11.465106,11.378411,11.385596,11.398414,11.424665,11.39552,11.408376,11.420852,11.391347,11.393185,11.38546,11.412847,11.408655,11.43267,11.375499,11.393583,11.427857,11.415561,11.440054,11.438657,11.541479,11.618132,11.792937,12.092244,11.944907,11.918458,11.972014,11.909695,11.924426,11.895082,11.957383,12.029564,11.975269,11.970797,11.883345,11.861485,11.879812,11.907956,11.841165,11.723351,11.618753,11.550285,11.486308,11.413604,11.3841,11.431372,11.36927,11.415822,11.433148,11.390409,11.432391,11.411928,11.35883,11.447581,11.384721,11.355098,11.393664,11.412946,11.408015,11.491537,11.497865,11.508484,11.512676,11.584957,11.711533,11.865658,11.892487,11.828391,11.903286,11.898138,12.021721,11.899852,11.901591,11.919296,11.926183,11.855579,11.870589,11.810046,11.861746,11.801743,11.757706,11.697101,11.711434,11.520898,11.393185,11.355378,11.299206,11.318029,11.370009,11.322997,11.315055,11.337231,11.382404,11.362283,11.41594,11.336691,11.33761,11.369351,11.309565,11.826354,11.90654,11.388534,11.415542,11.470018,11.503075,11.549546,11.7391,11.841265,11.836955,11.870788,11.941237,11.968841,11.87031,11.872303,11.876278,11.932412,11.864162,11.879054,11.841625,11.874061,11.821622,11.820603,11.777349,11.784435,11.647239,11.577132,11.424323,11.399234,11.386019,11.432148,11.920097,11.33312,11.444308,11.372543,11.397377,11.408674,11.346453,11.52619,11.431093,11.464087,11.387795,11.391446,11.449375,11.496548,11.496685,11.988385,11.522637,11.622864,11.757986,11.826155,11.930474,11.909695,11.949639,11.927878,11.988105,11.941752,11.952154,11.960737,11.928897,11.940417,12.407941,11.90718,11.958104,11.885661,11.849071,11.753154,11.634403,11.517408,11.436483,11.372505,11.412586,11.389391,11.382963,11.392546,11.424566,11.365177,11.34949,11.330543,11.299523,11.377995,11.382305,11.380349,11.368133,11.332282,11.394763,11.423547,11.43634,11.407817,11.497648,11.605258,11.695884,11.825795,11.906739,11.896678,11.886717,11.859429,11.860429,11.906062,11.860187,11.905665,11.930754,11.855101,11.877657,11.864901,11.784615,11.855318,11.807071,11.746348,11.594539,11.561861,11.425882,11.360309,11.347671,11.386758,11.395241,11.386416,11.382584,11.353043,11.441532,11.396558,11.369251,11.391229,11.361066,11.438557,11.411828,11.383063,11.403743,11.479619,11.45171,11.500976,11.507683,11.627795,11.790881,11.868732,11.894524,11.919377,11.925525,11.956986,11.953353,11.919538,11.940237,11.954589,11.959159,11.91716,11.902907,11.925264,11.867776,11.855039,11.846835,11.730058,11.694107,11.551602,11.432291,11.399632,11.389254,11.390329,11.413847,11.36909,11.366854,11.37558,11.39562,11.474868,11.431111,11.339629,11.386497,11.412847,11.356477,11.389751,11.467323,11.444805,11.474887,11.412487,11.501498,11.678539,11.778964,11.866137,11.914806,11.862945,11.959222,12.309409,11.950577,11.912328,12.007146,11.965568,11.904025,11.94351,11.884463,11.886239,11.904305,11.933052,11.794955,11.716104,11.597812,11.505131,11.408313,11.345056,11.325034,11.348807,11.327531,11.336772,11.346652,11.350726,11.346795,11.375517,11.326332,11.324935,11.376157,11.385298,11.335455,11.870248,11.360209,11.452313,11.453511,11.452449,11.489463,11.59326,11.69856,11.778945,11.899653,11.886779,11.94872,11.911092,11.879631,11.889791,12.445866,11.889574,11.896362,11.878694,11.903746,11.906801,11.868732,11.828031,11.841165,11.800085,11.644482,11.583398,11.466603,11.364898,11.40586,11.863702,11.429614,11.43734,11.352881,11.342802,11.442451,11.399613,11.394701,11.41163,11.381349,11.394222,11.405022,11.414822,11.420852,11.467323,11.467341,11.468062,11.605258,11.674148,11.75008,11.82867,11.930655,11.950956,11.954968,11.954427,11.935225,11.882426,11.933548,11.943951,12.015772,12.293561,11.923407,11.88622,11.863982,11.900032,11.839389,11.707882,11.637557,11.545733,11.461591,11.402606,11.384541,11.370288,11.42636,11.434185,11.394105,11.377654,11.372803,11.419374,11.393484,11.382765,11.391049,11.475986,11.39013,11.359209,11.408214,11.451773,11.45966,11.461013,11.470155,11.66205,11.786428,11.913887,11.914744,11.94872,11.882587,11.865261,11.857275,11.845376,11.901672,11.898616,11.860808,11.931015,11.856337,11.804277,11.830167,11.805873,11.781262,11.694306,11.601147,11.531319,11.430354,11.400551,11.311484,11.361165,11.358272,11.359389,11.317949,11.310503,11.359768,11.36917,11.340846,11.31711,11.398334,11.377834,11.369729,11.329326,11.341603,11.418275,11.458778,11.455604,11.481675,11.614101,11.775213,11.877216,11.931033,11.925904,11.911931,11.967164,11.903988,11.946764,11.925444,11.971996,11.928897,11.874141,11.804972,11.901789,11.837334,11.801221,11.763656,11.693089,11.577592,11.523115,11.388074,11.295132,11.301181,11.326954,11.340603,11.365637,11.293257,11.349068,11.405898,11.330164,11.316253,11.36514,11.368711,11.357036,11.302957,11.309683,11.346714,11.396936,11.451332,11.428975,11.592583,11.620827,11.718601,11.858933,11.875042,11.893667,12.518669,11.894505,11.8865,11.979622,11.890512,11.89153,11.97974,11.915123,11.906981,11.922072,11.911633,11.81843,11.81294,11.747466,11.644382,12.117395,11.415263,11.416958,11.372425,11.391329,11.38582,11.399812,11.367034,11.377554,11.459498,11.384541,11.435284,11.399812,11.413604,11.41027,11.816455,11.310223,11.378871,11.447978,11.401408,11.476166,11.54787,11.679315,11.818411,11.877315,11.914564,11.950956,11.933269,11.970077,11.949478,11.962053,11.918836,11.986528,11.931574,11.911111,11.859429,11.819647,11.805873,11.82859,11.799265,11.699877,11.639731,11.524792,11.408456,11.343081,11.815356,11.359389,11.429416,11.391887,11.383603,11.401749,11.417101,11.418175,11.338809,11.376995,11.3958,11.389733,11.3</t>
+  </si>
+  <si>
+    <t>12.623727,12.716309,12.695728,12.504255,12.362786,12.256529,12.07801,12.135262,11.968084,12.004575,12.070086,12.005432,12.015113,12.023913,11.995191,11.998284,12.050903,12.046394,12.040662,12.00691,11.989422,12.048108,12.04278,12.102305,12.110012,12.142889,12.144485,12.338212,12.56953,12.667782,12.706428,12.766574,12.699144,12.782143,12.735393,13.487809,12.77312,12.690337,12.655945,12.702516,12.798252,12.660715,12.662652,12.586975,12.580609,12.488344,12.471657,12.160873,12.033856,12.105199,12.030862,11.985807,11.975269,11.972573,12.02641,12.008984,11.989981,12.011201,12.034396,12.036532,12.043699,12.046692,12.056212,11.971735,11.984013,12.076234,12.113545,12.057834,12.193732,12.3245,12.424708,12.622907,12.764556,13.420559,12.749546,12.707825,13.07634,12.781485,12.867738,12.837476,12.754756,12.718184,12.733356,12.764916,12.70541,12.735032,12.627856,12.572865,12.349173,12.268347,12.116638,12.082941,12.128394,12.086357,11.938001,11.948161,12.000041,11.9898,11.987745,12.009245,12.023398,12.108353,12.009164,11.978163,11.989043,12.05394,12.652412,12.094741,12.046872,12.133964,12.269925,12.33448,12.472396,12.721438,12.725214,12.776833,12.729064,12.731101,12.73643,12.770785,12.664789,13.270067,12.793781,12.813722,12.737349,12.760904,12.632489,12.702994,12.619994,12.461597,12.365282,12.229043,12.010443,12.048288,12.069031,11.985211,12.498945,12.107316,12.027888,11.973989,12.047115,12.040743,12.059945,12.046891,11.976287,12.002755,11.953912,12.025652,12.013076,12.789229,12.160873,12.142528,12.259405,12.402351,12.628378,12.736672,12.791626,12.763419,12.770424,12.753638,12.832048,12.768667,12.739286,12.824323,12.744795,12.817995,13.173194,12.721239,12.68473,12.750024,12.727829,12.571964,12.385062,12.313818,12.101647,12.147397,12.108335,12.060367,12.077992,12.06436,12.067652,12.128456,12.058889,12.082283,12.043681,12.015331,12.014113,12.256411,12.056032,12.12622,12.071546,12.082625,12.126301,12.197545,12.287611,12.394085,12.592365,12.689921,12.721718,12.818715,12.790427,12.805996,12.776554,12.770207,12.807655,12.843146,12.726369,12.786515,12.828335,12.74631,12.862708,12.617597,12.572108,12.509167,12.28827,12.242637,12.118135,11.980479,11.988683,11.962134,11.955446,12.033657,12.050704,12.050921,12.045972,12.056275,12.007028,12.105919,12.032359,11.953372,11.987826,12.037011,12.050704,12.144404,12.044575,12.047729,12.242339,12.346018,12.515073,12.714694,12.674408,12.737827,12.73733,12.7421,12.67329,12.751061,12.78246,12.754477,12.768909,12.628577,12.738926,12.723574,12.598954,12.681656,12.630272,12.519886,12.32963,12.249903,12.07965,12.106857,12.031701,11.97974,11.97004,12.065398,12.104162,12.064317,12.060845,12.023597,12.128555,12.220678,12.00645,12.087313,12.010822,12.085537,12.098653,12.072502,12.131251,12.212952,12.268347,12.355899,12.508707,12.765096,12.795079,12.812523,12.746869,13.273961,12.717886,12.789788,12.786894,12.776256,12.751322,12.83955,12.787092,12.677861,12.640594,12.673831,12.623547,12.587353,12.371089,12.222634,12.73697,12.095939,11.962774,12.054436,12.098734,12.023876,12.072502,12.098212,11.972754,11.969499,12.09402,11.961737,12.019703,12.100069,11.989142,12.64327,12.134145,12.045854,12.153527,12.067192,12.179939,12.358414,12.522618,12.593427,12.755477,12.723873,12.681836,12.764456,12.725872,12.797513,12.846201,12.743137,12.727009,12.817516,12.64273,12.687624,12.86241,12.691996,12.579591,12.516371,12.348136,12.203432,12.128357,11.977125,11.968245,12.623745,11.991098,12.077352,12.127916,12.033477,12.077812,12.036371,12.007469,12.049288,12.017169,11.992415,12.080886,12.071465,12.091766,12.150713,12.16822,12.046711,12.185807,12.354601,12.470142,12.589434,12.813902,12.772939,12.842587,12.885425,12.686785,12.828316,12.730741,12.709862,12.740305,12.937665,12.702597,12.774138,12.719563,12.787912,12.675868,12.549788,12.403749,12.262479,12.121128,12.060864,12.040426,12.091505,12.052381,12.138697,12.302404,12.173548,12.050884,11.944168,12.020181,12.117178,12.019405,11.976647,12.028248,11.987745,12.134262,12.149434,12.093182,12.131431,12.165984,12.353564,12.489623,12.556377,12.746111,12.822565,12.725171,12.715532,12.787092,12.816138,12.801867,12.76286,12.697026,12.791744,12.696485,12.700081,12.589372,12.738765,12.696566,12.555079,12.414666,12.239842,12.07316,12.074719,11.975107,12.03847,12.090009,11.969562,11.977504,12.076116,12.069788,12.057132,12.090847,12.035036,12.122867,12.094263,12.067335,12.182671,12.191956,12.089729,12.173449,12.20437,12.34069,12.404227,12.541025,12.628856,12.800867,12.782981,12.763258,12.793961,12.797532,12.735212,12.770288,12.855063,12.723736,12.752061,12.666944,12.693014,12.626242,12.637159,12.635203,12.586099,12.275154,12.354862,12.082265,12.004972,11.97507,12.033918,11.995949,12.076414,12.071403,11.997806,12.020982,12.019287,12.107416,12.161811,11.996408,11.987646,12.032719,12.024714,12.090909,12.148857,12.029285,12.105,12.231459,12.437221,12.540106,12.677004,12.751961,12.758308,12.970542,12.846779,12.778709,12.827217,12.880854,12.799668,12.72581,12.781224,12.797874,12.739305,12.719662,12.697765,12.729903,12.610872,12.33969,12.322165,12.14141,12.122606,12.078352,12.095759,12.07352,12.088512,12.101827,12.102944,12.114645,12.019982,12.060106,12.036253,12.055256,12.116719,12.693275,12.064975,12.09512,12.084302,12.127419,12.1168,12.31847,12.333002,12.536635,12.61674,12.780826,12.782441,12.774678,12.79919,12.897063,12.888698,12.819094,12.763879,12.658759,12.760662,12.797215,12.916526,12.647021,12.747471,12.635744,12.560109,12.443829,12.283239,12.109534,12.112347,12.688642,12.099392,12.07352,11.986826,12.061864,12.078631,12.057032,12.112167,12.060665,12.107136,12.050785,12.072384,12.021361,12.186503,12.113564,12.558135,12.051443,12.244693,12.173728,12.365661,12.489145,12.577833,12.745733,12.753936,12.827316,12.83185,12.764556,12.675327,12.78382,12.75334,13.221621,12.761401,12.745174,12.692275,12.648679,12.608673,12.602146,12.539727,12.281246,12.206388,12.125879,12.00509,12.0436,12.060106,11.985491,12.05897,12.016827,11.959439,12.035495,12.007189,12.027329,12.046152,12.031061,11.925065,11.962693,12.085817,12.074061,12.04745,12.029763,12.069987,12.268149,12.424888,12.469204,12.661075,12.751105,12.730424,12.779367,12.734554,12.760544,12.746291,12.757731,12.709583,12.787254,12.808772,12.831111,12.786912,12.55937,12.682972,12.655405,12.484773,12.288568,12.159917,12.070086,12.017908,12.093244,12.093343,12.103963,12.091785,12.003215,11.971915,12.061783,12.066832,12.106037,12.04827,12.07965,12.057293,12.072322,12.061224,12.140013,12.070645,12.176064,12.08999,12.244873,12.354564,12.524357,12.667981,12.71665,12.778411,12.772579,12.718967,12.796197,12.752881,12.782342,12.781665,12.675625,12.68994,12.653269,12.764015,12.615262,12.646562,12.677103,12.488803,12.347335,12.241339,12.1674,12.136281,11.990521,12.016592,12.092145,12.038228,11.988304,12.045295,12.046593,12.013275,12.085059,12.052399,12.040346,12.09484,12.054219,12.053021,12.103603,12.053418,12.15075,12.132188,12.173548,12.373666,12.508167,12.595321,12.76332,13.298057,12.730803,12.8055,12.602326,12.681277,12.68894,12.866881,12.644227,12.725792,12.69992,12.680078,12.66395,12.711738,12.600612,12.470738,12.384845,12.166462,12.095958,12.077514,12.006829,12.039886,12.061622,11.984093,11.966624,12.031782,12.011039,12.002935,12.040103,12.080209,12.031341,12.606761,11.954508,12.014312,12.107714,12.132468,12.006388,12.091586,12.235272,12.420435,12.485891,12.619094,12.832626,12.756091,12.753179,12.749266,13.254678,12.815958,12.723835,12.775535,12.713415,12.757749,12.713775,12.714234,12.673731,12.617579,12.69012,12.556954,12.35552,12.29384,12.138256,12.645046,12.064298,12.010065,11.992856,12.082662,12.148596,12.059268,12.090928,12.04278,12.045214,12.155446,12.167959,11.976368,12.008785,12.026509,12.128158,12.056492,12.045133,12.166562,12.187981,12.273278,12.546236,12.654188,12.739665,12.738106,12.718426,12.657442,12.770406,12.755594,12.711837,13.047096,12.696467,12.748887,12.807276,12.665826,12.665087,12.635942,12.653989,12.470142,12.403649,12.236986,12.084221,12.055536,11.972754,12.005152,12.031881,12.043817,11.987664,12.005991,12.021001,12.018548,12.100808,12.048549,11.979461,12.032098,12.036154,12.010182,12.064938,12.094877,12.126599,12.12568,12.198663,12.37071,12.428142,12.549428,12.723096,12.756091,12.684748,12.745372,12.707366,12.68491,12.845003,12.829173,12.771244,12.756352,12.764456,12.6786,12.715489,12.622888,12.665844,12.450716,12.303956,12.16355,12.093524,12.01725,12.059367,11.99008,12.018386,11.997048,12.066813,11.94836,12.037371,12.103603,12.088214,12.014852,12.052859,11.958898,12.012797,12.043916,12.079768,12.115402,12.076936,12.005072,12.196526,12.391272,12.574858,12.591309,12.74695,12.722836,12.778591,12.850393,12.706248,12.711278,12.743677,12.69461,12.749105,12.771623,12.711539,12.713272,12.771822,12.704832,12.592346,12.642072,12.37692,12.24591,12.18908,12.046494,12.079867,12.092983,12.059827,12.144565,12.093362,12.080669,12.092424,12.054536,12.065056,12.059647,12.046313,11.989223,12.005152,12.108074,12.080047,12.125301,12.097355,12.057293,12.182392,12.317271,12.459262,12.617957,13.276016,12.745733,12.707285,12.739845,12.808394,12.830409,12.763438,12.702876,12.775157,12.641594,12.720761,12.755731,12.621671,12.684549,12.656144,13.09656,12.362109,12.171592,12.102106,12.000339,12.095039,12.018368,12.00755,11.99639,12.015113,12.069509,12.072502,12.02777,12.145224,12.156042,12.476948,12.096977,12.04791,12.033558,12.119631,12.091865,12.849952,12.10105,12.272881,12.305037,12.516712,12.687785,12.771902,12.729046,12.750583,12.712117,12.678023,12.709502,12.788751,12.732138,12.688282,12.68345,12.723376,12.737069,12.713694,12.629397,12.655566,12.477048,12.362885,12.190577,12.629875,12.11488,11.977405,11.963892,11.997905,11.96455,12.079569,12.098094,11.954868,11.973511,12.091766,12.010182,12.006469,12.008984,12.770685,12.042122,12.084121,12.033719,12.084302,12.225869,12.288729,12.383286,12.553682,12.651853,12.75683,12.78931,12.795899,12.855442,12.838693,12.762581,13.03937,12.70046,12.774219,12.802264,12.842947,12.687524,12.734635,12.655386,12.675868,12.546515,12.335498,12.291344,12.128357,12.041283,12.075458,12.309111,11.939318,11.98623,12.069509,11.97974,12.107136,12.089251,11.99721,11.99457,12.00645,12.049307,11.988403,12.016709,12.028726,12.183149,12.138976,12.078532,12.25679,12.474533,12.528568,12.612747,12.717048,12.678581,12.756749,12.662652,12.783559,12.743019,12.673669,12.725233,12.772101,12.70531,12.712937,12.758209,12.610133,12.710701,12.644668,12.50695,12.312483,12.219541,12.115141,12.013834,12.150037,11.976107,12.08378,12.073421,12.726531,12.093642,12.123326,12.031223,12.133126,12.045376,12.034477,12.043699,12.034117,12.046593,12.227105,12.124165,12.104242,12.208363,12.346478,12.363407,12.598395,12.672334,12.814921,12.795557,12.777771,12.740125,12.799407,12.854622,12.867919,12.797892,12.822466,12.764239,12.750204,12.67321,12.792104,12.702255,12.634085,12.506093,12.473334,12.204469,12.138914,12.113303,12.394346,12.041203,12.203134,12.052723,12.103684,12.116259,12.089412,11.983553,12.086736,12.046431,12.040283,11.991937,11.9479,12.06949,12.099392,12.029366,12.137318,12.261622,12.203693,12.367916,12.551564,12.836818,12.777032,12.718923,12.725891,12.740143,12.746111,12.724593,12.684947,12.701317,12.759966,12.752601,12.738827,12.65389,12.672912,12.664888,12.661715,12.54913,12.408319,12.240681,12.105099,12.014275,12.066633,12.025994,12.012058,12.029186,12.000979,12.026012,12.079967,11.990819,12.051561,12.542342,12.041184,11.968282,12.110968,12.035452,12.088251,12.045376,12.209238,12.037551,12.201575,12.414089,12.497411,12.631291,12.724574,12.679817,12.811927,12.722537,12.793501,12.786596,12.708366,12.742019,12.825378,12.66944,12.746571,12.730679,13.41433,12.71483,12.739305,12.464491,12.346198,12.876041,12.198023,12.047351,12.07462,12.056473,12.167959,12.101125,12.031502,12.034694,12.158737,12.038209,12.127338,12.090089,12.065776,12.093461,12.647841,11.971654,12.073061,12.090108,12.061324,12.060585,12.312502,12.284736,12.492977,12.664528,12.753557,12.726748,12.821069,12.758606,12.726549,13.272545,12.74713,12.69489,13.522164,12.688462,12.796874,12.712576,12.667043,12.713235,12.625683,12.478923,12.352645,12.210617,12.104441,12.081445,11.959799,11.958402,12.054797,11.96373,12.010021,12.037091,12.023615,11.985528,12.029745,12.037309,12.147397,11.992018,11.978504,12.10536,12.137958,12.169717,12.255591,12.225013,12.275713,12.47493,12.568251,12.67447,12.873868,12.773182,12.751663,12.753116,12.773318,12.690617,12.782143,12.769865,12.772082,12.770884,12.804879,12.742199,12.658082,12.694511,12.655703,12.506869,12.305795,12.184149,12.153607,12.045295,12.052281,12.065516,11.947043,12.003494,12.138697,11.975809,12.090847,12.002277,12.00545,12.060088,12.057591,12.007587,12.082382,12.064236,12.09402,12.069869,12.234893,12.088332,12.29294,12.364823,12.483655,12.707807,13.190899,12.835483,12.83552,12.86626,12.795476,12.828397,12.768306,12.705689,12.849195,12.766115,12.756035,12.712576,12.7732,12.643848,12.71026,12.49743,12.452275,12.311465,12.112347,12.052921,12.081327,12.009605,12.178218,12.057069,12.050027,12.045953,12.119694,12.063659,12.169816,12.071167,11.980578,12.045593,12.07444,12.087854,12.198402,12.1782,12.125742,12.219181,12.671694,12.42441,12.99847,12.697305,12.751682,12.819653,12.768549,12.825658,12.791067,12.838215,12.774318,12.844363,12.869217,12.827235,12.840532,12.695647,12.722637,12.663671,12.558091,12.473694,12.359594,12.250002,12.041942,12.013573,12.049686,12.032819,12.059206,12.027391,12.102864,11.992955,12.045755,12.004873,12.546615,12.044898,12.091766,11.997445,12.010002,12.030006,12.076675,12.033856,12.130133,12.116619,12.269446,12.315936,12.466428,12.701597,12.789247,13.306676,12.804301,12.85702,12.796278,12.729046,12.724773,12.703553,12.692356,12.788012,12.800146,12.700379,12.757588,12.693474,12.626124,12.432353,12.828894,12.136958,12.130512,12.101007,12.038327,12.066435,12.038408,11.95393,11.94323,12.064478,12.035613,12.004115,11.98605,12.047351,12.84073,12.062081,12.013257,12.084519,12.064541,12.114781,12.020802,12.104621,12.259144,12.377417,12.526872,12.723916,12.770983,12.755712,12.834483,12.668502,13.102112,12.783739,12.743497,12.799848,12.746111,12.743379,12.733797,12.645723,12.66277,12.552322,12.621969,12.505453,12.322003,12.138075,12.069211,12.01122,12.135641,12.022659,12.045394,12.025913,11.990639,11.972356,12.724674,12.073322,12.136976,12.103783,12.038489,12.127717,12.115241,12.142727,12.139436,12.144926,12.080507,12.147639,12.402289,12.498268,12.565059,12.710341,12.745453,12.847636,12.818112,12.803121,12.741559,12.850133,12.779808,12.754675,12.801326,12.697405,12.740206,12.751899,12.667124,12.698305,12.65892,12.463553,12.348055,12.173728,12.078451,12.059187,12.04314,11.960619,12.032819,12.076756,12.040004,12.085158,12.019324,11.965388,12.099131,12.028987,12.009083,11.958122,11.976548,12.060665,12.14087,12.092865,12.091226,12.13656,12.200277,12.350986,12.547354,12.66872,12.714551,12.740162,12.767232,12.711378,12.74164,12.734753,12.72627,12.773778,12.692474,12.764835,12.896504,12.689083,12.61125,12.7205,12.63303,12.599793,12.320668,12.19403,12.785118,12.11688,12.047171,12.083941,12.052182,12.056293,12.082625,12.082743,12.061243,12.037669,12.030962,12.069329,12.091685,12.048152,12.071664,12.073638,12.071204,12.112148,12.077775,12.073539,12.224274,12.924289,12.498169,12.599811,12.807195,12.745832,12.78767,12.784217,12.691878,12.80432,12.779088,12.767909,12.71116,12.780106,12.667503,12.756433,13.217249,12.623727,13.400798,12.466428,12.344143,12.192452,12.070086,12.045854,12.023236,11.989422,12.051064,12.001538,12.031521,12.027788,12.008046,12.614685,12.072664,12.072601,12.029745,12.065957,12.050406,12.05312,12.075414,12.035415,12.097355,12.136299,12.290126,12.365121,12.455169,12.703335,12.761463,12.752421,12.741721,12.68445,12.697883,12.812045,12.706888,12.7108,12.726071,12.675209,12.732039,12.73697,12.645046,12.661174,12.593185,13.017951,12.35131,12.154346,12.025391,12.071366,12.022578,11.976107,11.982715,12.059268,12.017927,12.064261,12.015393,12.038868,12.044736,12.077253,12.058529,12.063261,12.011896,12.029006,12.06885,12.022839,12.053039,12.140572,12.192552,12.362587,12.460218,12.619833,12.781801,12.755775,12.726251,12.969524,12.750763,12.797414,12.700777,12.763699,12.657641,12.68545,12.769648,12.645922,12.600811,12.701199,12.591607,12.445469,12.317054,12.161712,12.27665,12.081408,12.013356,11.922469,11.954607,12.049406,12.073502,12.013735,12.010201,12.011561,11.96273,12.092163,11.994732,12.012319,12.019846,12.054418,12.018783,12.09438,12.072943,12.115321,12.206046,12.366022,12.497728,12.74246,12.795241,12.712179,12.658082,12.708105,12.746391,12.744596,12.769567,12.625242,12.655287,12.791825,12.687245,12.726792,12.655188,12.629235,12.596899,12.544199,12.274315,12.152191,12.022218,11.95924,11.972735,12.011418,11.997247,12.029564,12.036272,12.030403,11.958799,12.030682,12.037868,12.030484,11.989242,12.0113,11.967344,12.051263,12.031322,12.033477,12.050505,12.130151,12.195427,12.343783,12.492517,12.660876,12.656622,12.732418,12.813362,12.745696,12.671595,12.728524,12.656386,12.764456,12.723016,12.680376,12.735312,12.713793,12.641134,12.679718,12.624385,12.506472,12.387919,12.228142,12.000041,12.061684,11.995669,12.011598,12.042798,12.100727,12.04809,12.022497,12.020001,12.03144,12.009164,12.040165,11.999122,12.018287,12.023038,12.022199,12.130611,12.141311,12.032359,12.203233,12.547652,12.442314,12.582025,12.64904,12.794619,12.874346,12.72114,12.835799,12.793402,12.788651,12.809133,12.794719,12.769406,12.788949,12.771722,12.786056,12.613766,12.664925,12.665105,12.484034,12.281103,12.109832,12.010263,12.077333,12.030682,12.009984,12.056473,12.010642,12.011102,12.07344,12.566276,12.067074,12.091505,12.047611,12.000979,12.029645,11.94944,12.118476,12.092704,12.089828,12.163587,12.158458,12.256672,12.471657,12.527034,12.74749,12.770145,12.894467,12.762618,12.76817,12.785136,12.766232,12.82133,12.896026,12.752179,12.782801,12.744255,12.813641,12.741919,12.720563,13.298373,12.502938,12.341628,12.233154,12.102205,12.12632,12.072844,12.086295,12.100709,12.096237,12.139454,12.112825,12.075638,12.07829,12.112365,12.630533,11.967543,11.957141,12.029825,12.055095,12.024453,12.131909,12.224671,12.13153,12.245351,12.340429,12.522662,12.725152,12.718265,12.773498,13.244816,12.73166,12.641215,12.786813,12.793141,12.730921,12.739224,12.78482,12.682215,12.777113,12.650275,12.689841,12.619435,12.468024,12.265814,12.248586,12.044916,12.099591,12.088431,12.045773,12.085717,12.078352,12.075098,12.096977,12.03244,11.988223,12.016809,12.034775,12.008586,12.206525,12.075955,12.04691,12.095101,12.138597,12.092344,12.226987,12.324059,12.42405,12.618994,12.7109,12.796414,12.787453,12.770306,12.797135,12.783919,12.753079,12.790247,12.946267,12.825559,12.800407,12.77833,12.736312,12.641811,12.743317,12.6376,12.516315,12.318532,12.263957,12.072142,12.142808,12.080786,12.191254,12.087332,12.0533,12.076793,12.076576,12.017486,12.134685,12.054679,12.183888,12.097256,12.133766,12.030304,12.098212,12.234353,12.205109,12.169636,12.133946,12.32047,12.480681,12.53402,12.678203,12.837314,12.873967,12.795278,12.825819,12.819752,12.81987,12.796215,12.824341,12.791384,12.798892,12.855063,12.764177,12.741342,12.706347,12.682215,12.543721,12.393986,12.229124,12.093561,11.977585,12.097094,12.064398,12.039426,12.071645,12.04332,12.074918,12.03783,12.001898,12.048549,12.034595,12.041103,11.997166,12.032241,12.113284,12.121469,12.172133,12.155203,12.599631,12.271782,12.422851,12.462895,12.681277,12.765295,12.784379,12.748869,12.750862,12.702895,12.735753,12.749266,12.727208,12.78382,12.842947,12.825099,12.702435,12.648959,12.751142,12.742398,12.441736,12.27683,12.174765,12.077613,12.094362,12.0123,11.955067,12.011797,12.032999,11.961035,12.610791,11.999023,12.003215,12.086015,12.053101,12.024714,12.008226,12.022559,12.10518,12.11552,12.0631,12.018026,12.136939,12.256529,12.340988,13.080072,12.624286,12.75929,12.755874,12.864385,12.743876,12.755793,12.73212,12.686767,12.721879,12.824521,12.792222,12.797054,12.757389,12.609952,13.225074,12.64822,12.540187,12.270881,12.187205,12.040563,12.012977,12.023876,11.971077,11.985888,11.955545,12.019964,12.056691,12.013716,12.007667,12.060647,12.029384,11.983472,12.00691,12.09438,12.078352,12.068031,12.032738,12.065019,12.079849,12.148198,12.346478,12.470639,12.654927,12.79901,13.123848,12.653548,12.791465,12.788769,12.80532,12.822006,12.755631,12.764357,12.812586,12.762202,12.733877,12.696927,12.660237,12.593564,12.526872,12.397141,12.184429,12.092406,11.992018,12.029006,12.074539,12.009804,12.054716,12.051921,11.976765,12.008624,12.019305,12.053958,12.061504,12.003215,11.959141,12.038309,12.080488,12.008524,12.112645,12.117657,12.031521,12.166562,12.321886,12.561805,12.660597,12.762941,12.801326,12.814902,12.807114,12.637222,12.780385,12.743776,12.683972,12.749266,12.742938,12.681295,12.747391,12.629036,12.649157,12.576337,12.508248,12.316116,12.254194,12.046953,12.105081,12.017908,12.043637,12.009443,11.964333,12.030484,12.027149,12.022578,11.995191,12.140833,12.090909,12.026789,12.018206,11.995371,12.015033,12.092163,12.124804,12.091288,12.073502,12.21407,12.366022,12.537492,12.646642,12.771524,12.756253,12.759507,12.733039,12.829533,12.856361,12.790906,12.797712,12.815479,12.781404,12.778609,12.717308,12.724413,12.718824,12.692933,12.542243,12.414107,12.235011,12.035514,12.096598,12.125103,12.100069,12.149335,12.124823,12.104342,12.103404,12.140013,12.097076,12.140752,12.07929,12.044718,12.004134,12.060386,12.161811,12.157638,12.072303,12.650816,12.179001,12.284835,12.433831,12.513775,12.703174,12.810828,12.81602,12.666565,12.716309,12.775796,12.749744,12.730201,12.786732,12.71601,13.300249,12.715091,12.702155,12.71583,12.649617,12.662112,12.528667,12.278128,12.232974,12.050686,12.080128,12.022479,12.103485,12.050244,12.033856,12.556396,11.986348,11.980821,12.053878,12.007487,12.044618,11.971456,11.938119,12.027888,12.055455,12.023317,12.137939,12.072701,12.08999,12.288928,12.397998,12.556495,12.717967,12.846139,12.714514,12.751881,12.725531,12.747589,12.84119,12.760625,12.725251,12.794439,12.79855,12.732598,12.751421,13.222199,12.670216,12.702056,12.459901,12.330847,12.288648,12.166202,12.0113,12.128555,11.997309,11.979144,12.02631,12.088891,12.03647,12.008145,11.99072,12.034297,12.037731,12.01689,12.060386,12.124084,12.029906,12.12568,12.176064,12.138498,12.083482,12.297132,12.371909,12.564202,12.718426,12.995234,12.808313,12.807655,12.71675,12.771524,12.681277,12.735473,12.733337,12.730164,12.700361,12.758308,12.788869,12.593464,12.646444,12.657163,12.537212,12.303901,12.195806,12.026211,12.09602,12.091226,11.996228,11.989583,11.946745,12.025913,12.030186,12.026851,12.054039,12.06428,12.071005,12.077234,12.032061,12.013095,12.106795,12.081246,12.030024,12.154067,12.20894,12.29194,12.446965,12.597116,12.633868,12.79919,12.888381,12.801507,12.689499,12.775796,12.716489,12.742776,12.790148,12.649338,12.752421,12.758948,12.719681,12.689381,12.621212,12.728884,12.506292,12.347236,12.176424,12.004413,12.120532,12.031322,12.036172,12.126599,12.079669,12.17884,12.077054,12.003395,12.109714,12.110192,12.113881,12.081327,12.09997,12.109732,12.12622,12.092207,12.097175,12.226708,12.176144,12.32899,12.457486,12.489543,12.719364,12.824062,12.728325,12.773697,12.820528,12.753297,12.777753,12.808512,12.681656,12.789571,12.802444,12.772082,12.716731,12.770046,12.700839,12.664447,12.820491,12.341566,12.248325,12.139734,12.084519,12.174648,12.064857,12.027049,12.025075,12.023236,12.040805,12.006568,12.001221,12.109372,11.983615,12.092325,12.039426,12.032179,12.067652,12.061143,12.443891,12.117017,12.051803,12.207226,12.400774,12.533083,12.73661,12.76414,12.739982,12.718445,12.645723,12.795656,12.731039,12.670856,12.678321,12.780566,12.698945,12.821547,12.750943,12.693654,12.693474,12.635185,12.489002,12.369474,12.206407,12.01158,12.052462,12.040923,12.001501,12.065994,12.588993,12.04881,12.044736,12.029564,11.99611,12.090568,12.053021,11.98038,12.070167,12.072583,12.006351,12.051543,12.032837,12.085059,12.080867,12.304559,12.368176,12.618994,12.613865,12.77887,12.752818,12.740882,12.682773,12.79955,12.703093,12.800848,13.489188,12.764456,12.784379,12.821447,13.190303,12.778448,12.752079,12.707546,12.508428,12.412313,12.191334,12.137877,12.076973,12.096796,12.12586,12.057771,12.064199,12.106379,12.143267,12.636402,11.952452,12.050443,11.992036,12.000861,12.026248,11.988422,12.10554,12.059728,12.050127,12.084419,12.088891,12.220019,12.414666,12.486766,13.135666,12.724295,12.674489,12.790906,13.49787,12.733536,12.770604,12.804338,12.674489,12.719544,12.78949,12.719842,12.688282,12.678103,12.630334,12.627298,12.552303,12.296852,12.22523,12.1469,12.013834,12.04891,12.002457,11.99978,12.046612,12.076694,12.00088,12.057672,12.139932,12.095958,12.087034,12.10967,12.013753,12.026391,12.045674,12.150794,12.191055,12.12155,12.107695,12.296716,12.435526,12.586577,12.813225,12.764618,12.758029,12.772641,12.659678,12.812865,12.801587,12.752359,12.744074,12.687624,12.707447,12.719941,12.73148,12.661814,12.736529,12.719743,12.429757,12.327655,12.230918,12.056194,12.05248,12.076775,12.015331,12.060187,12.070446,12.048251,12.018107,12.059069,12.023118,12.06785,12.033477,12.02274,12.119892,12.055933,12.056554,12.079929,12.087736,12.097715,12.8464,12.292461,12.348813,12.555638,12.595582,12.788192,12.815119,12.794278,12.718445,12.707627,12.763717,12.768189,12.752638,12.883649,12.809512,12.765754,12.620392,12.66323,12.69479,12.59031,12.432154,12.333443,12.171673,12.068931,12.082761,11.972754,12.056393,12.151751,12.075079,12.038147,12.005351,12.014852,12.000681,12.036613,11.959898,11.986528,12.007649,12.055455,12.796315,12.583503,12.143006,12.181553,12.222056,12.322662,12.413791,12.563761,12.670198,12.80853,12.78803,12.83049,12.847717,12.801246,12.745472,12.864304,12.757172,12.764556,12.806636,12.722736,12.77879,12.783279,12.735032,12.749906,12.606338,12.370971,12.238364,12.186006,12.04809,12.087971,12.058032,12.573163,12.081966,12.079768,12.040283,12.109453,12.065795,12.077433,12.117178,12.082283,12.080867,12.186186,12.099771,12.109173,12.167841,12.142609,12.67357,12.254374,12.306037,12.503137,12.667863,12.728325,12.77284,12.703273,12.711278,12.738727,12.73697,12.775616,12.739125,12.721898,12.697405,13.326797,12.733536,12.629136,12.60586,12.70028,12.457684,12.388496,12.244612,12.078253,12.096535,12.075738,12.039228,11.999842,12.008506,12.005233,12.822385,12.028006,12.045593,12.080768,12.045314,11.975169,12.07334,12.07911,12.01122,12.093983,12.045953,12.090729,12.170375,12.342268,12.390173,12.821187,12.697206,12.788192,12.84704,12.707645,12.750862,12.907943,12.795855,12.791906,12.791645,12.745714,12.729704,12.800948,12.732499,12.660218,12.70577,12.705031,12.507329,12.40768,12.247108,12.18872,12.104603,12.039985,12.4611,12.139734,11.969301,12.06318,12.078451,12.002358,12.050984,12.151949,12.086456,12.138417,12.050145,12.053958,12.142448,12.163351,12.07352,12.172574,12.167779,12.320507,12.480122,12.594601,12.687425,12.892331,12.763419,12.822565,12.889058,12.819212,12.800606,12.774579,12.75362,12.816616,12.846562,12.793601,12.736529,12.77366,12.812784,12.696548,12.558991,12.358215,12.182851,12.161612,12.066714,12.077613,12.062243,11.972375,12.022839,12.067994,12.008866,12.010363,11.99008,12.071465,12.05815,12.064118,12.007767,12.148676,12.015213,12.03783,12.121488,12.113726,12.119911,12.211896,12.405407,12.520265,12.658821,12.717805,12.689959,12.737169,12.716849,12.759047,12.792222,12.794539,12.727649,12.773498,12.71108,12.794241,12.75747,12.65261,13.084723,12.725611,12.530803,12.431614,12.291424,12.104603,12.090071,12.137039,12.051803,12.092605,12.08935,12.052182,12.115918,12.056312,12.078371,12.084699,12.033297,12.014356,12.135182,12.068472,12.621851,12.152111,12.122507,12.127437,12.171573,12.31947,12.419479,12.584043,12.734473,12.808592,12.838395,12.916787,12.770586,12.722078,12.813045,13.319252,12.790067,12.698342,13.525319,12.724314,12.666124,12.674768,12.711676,12.678302,12.473676,12.272042,12.233315,12.093182,12.123904,11.999122,12.527711,12.024814,12.020964,12.147478,12.028528,11.982435,12.00142,12.082643,12.036352,12.07947,12.032701,11.979821,12.101466,12.138336,12.040184,12.104621,12.099591,12.253536,12.41289,12.487108,12.654728,12.829813,12.694411,12.750322,12.722817,12.80432,12.720302,12.780727,12.811604,12.780628,13.265658,12.74128,12.634185,12.746968,12.628956,12.649797,12.469204,12.247208,12.190018,12.025491,12.043898,12.078253,12.059548,11.934486,12.108714,12.059548,12.05366,12.031322,12.064199,11.989981,12.076116,12.009723,11.97553,12.112906,12.089512,12.051263,12.038507,12.140653,12.096995,12.304478,12.538032,12.485891,12.739864,12.772741,13.458466,12.785894,12.779727,12.733418,12.734536,12.828235,12.772741,12.847419,12.837377,12.769027,12.670396,12.751303,12.670297,12.76853,12.50795,12.443972,12.202593,12.10097,12.093884,12.078569,12.176461,12.124444,12.144926,12.100411,12.096436,12.154446,12.177244,12.1157,12.144106,12.02823,12.116917,12.069627,12.131729,12.137498,12.104,12.136299,12.200737,12.381789,12.849555,12.577635,12.777194,12.774039,12.792961,12.828434,12.827956,12.804779,12.818175,12.858237,12.905447,12.738088,12.792825,12.8669,12.728108,12.693113,12.672713,12.680159,12.520904,12.474054,12.24142,12.087754,12.120668,12.125463,12.119315,12.154383,12.108273,12.143187,12.1167,12.049667,12.063802,12.109012,12.080128,12.122389,12.073899,12.045872,12.187882,12.146422,12.103143,12.134306,12.150713,12.248009,12.411853,12.578554,12.644407,12.825459,12.738467,12.766972,12.837358,12.815579,12.774399,12.744155,12.759209,12.782702,12.753918,12.722438,12.64804,12.657423,12.634147,12.658578,12.495312,12.390533,12.283339,12.150912,12.093461,12.023975,12.086754,11.971275,12.002836,12.046152,12.048649,12.066733,12.070148,12.045314,12.006469,12.014194,12.684469,12.463913,12.035135,12.087413,12.043556,12.066435,12.168121,12.242358,12.388459,12.469602,12.742758,12.760264,12.775598,12.783224,12.705888,12.768449,12.790067,12.685748,12.679519,12.77879,12.780448,12.789129,12.682954,12.693176,12.664969,12.572406,12.471738,12.357917,12.210698,12.034297,12.097833,12.656306,12.00088,12.060206,12.029527,11.97992,12.051822,11.99996,12.363724,11.957545,12.091748,12.145422,12.133784,12.084699,12.118035,12.135182,12.067236,12.134325,12.22605,12.324879,12.466348,12.600153,12.775318,12.734554,12.781025,12.754278,12.827198,12.819131,12.77312,12.882829,12.851449,13.367381,12.764835,12.792483,12.73615,12.704453,12.733337,12.665149,12.591328,12.451437,12.231477,12.054896,12.129636,12.065994,12.166264,12.07911,12.554998,12.055275,12.022118,12.095759,12.083482,11.937163,12.029186,11.997725,12.011841,11.995831,12.104162,12.141013,12.12586,12.162252,12.129195,12.7215,12.391831,12.601351,12.699162,12.698703,12.714731,12.754675,12.812225,12.870595,12.780845,12.784497,12.684469,12.769747,12.688822,12.704932,12.740802,12.734455,12.703994,12.583106,12.517867,12.34554,12.210779,12.085897,12.07947,12.139752,12.201358,12.094859,12.081904,12.104062,12.106397,12.052443,12.165444,12.144205,12.102268,12.074421,12.038625,12.083121,12.239861,12.206605,12.176604,12.158638,12.098833,12.3147,12.432371,12.57438,12.777131,12.874986,12.765953,12.801488,12.709602,12.743857,12.822466,12.899119,12.701118,12.755874,12.897063,12.752638,12.732877,12.670577,12.720681,12.729642,12.501522,12.369692,12.240122,12.129592,12.08835,12.113663,12.121469,12.027608,12.096697,12.080147,12.06867,12.104261,12.118035,12.159476,12.062143,12.105,12.083103,12.087934,12.171592,12.139355,12.118594,12.156781,12.182212,12.396023,12.416523,12.544478,12.719383,12.788949,12.816895,12.776094,12.749527,12.82536,12.886083,12.745074,12.771045,12.80504,12.762438,12.809151,12.771263,12.637159,12.826857,12.628198,12.406382,12.318352,12.239066,12.058069,12.051543,12.036371,11.960538,12.121469,12.149596,12.007947,12.013076,12.034378,12.092027,12.006152,12.014753,12.000681,12.650915,11.967643,12.068211,12.063839,12.069148,12.077514,12.124364,12.277849,12.483494,12.6581,12.811784,12.762382,12.736132,12.687804,12.804959,12.774256,12.758128,12.754036,12.770505,12.651573,12.73148,12.726288,12.700361,12.695548,12.729064,12.636203,12.609952,12.38115,12.170456,12.109832,12.648301,12.067391,12.117638,11.983354,12.060945,12.040463,12.132207,12.03162,12.148316,12.071366,12.054138,12.059709,12.066975,12.048288,12.095039,12.66287,12.126239,12.247667,12.195408,12.275595,12.421354,12.544577,12.71529,12.821168,12.796675,12.759705,12.844823,12.719283,12.82151,12.782162,13.317557,12.748446,12.823745,12.88794,12.830868,12.740802,12.699081,12.610015,12.497088,12.352328,12.249164,12.202792,12.10582,12.200196,12.157681,12.046792,12.104981,12.100907,12.078271,12.062702,12.063659,12.072204,12.120911,12.041283,12.046792,12.068031,12.075495,12.173648,12.119134,12.1158,12.534436,12.368655,12.576796,12.56953,12.679799,12.738069,12.724413,12.756091,12.787832,12.690418,12.789788,12.690797,12.812964,12.</t>
+  </si>
+  <si>
+    <t>9.900027,9.878725,9.892022,9.915415,9.901803,9.888389,9.920464,9.870422,9.914,9.894555,9.921626,9.898847,9.91775,9.924718,9.926774,9.958334,9.966998,9.998657,10.008519,10.008538,10.084333,10.145175,10.136294,10.136331,10.125793,10.129047,10.130047,10.135673,10.118725,10.113198,10.131742,10.154919,10.08601,10.056946,10.06936,10.073732,10.015344,10.034229,9.99095,9.965141,9.974922,9.948174,9.939629,9.92819,9.943902,9.954142,9.947516,9.935978,9.947833,9.941467,9.974903,9.935779,10.428634,9.937313,9.953503,9.966538,9.983585,10.034148,10.013847,10.039558,10.035825,10.058642,10.088463,10.118409,10.141803,10.111341,10.097108,10.673645,10.075328,10.088923,10.061635,10.07567,10.079086,10.05281,10.08134,10.015226,9.998135,10.000371,10.010096,9.968314,9.932164,9.927712,10.428932,9.905833,9.862157,9.884594,9.902082,9.915695,9.888805,9.90851,9.880384,9.902921,9.897449,9.908112,9.891761,9.855971,9.910447,9.953962,9.944281,9.96506,9.968593,9.988615,10.002309,10.009376,10.057325,10.069261,10.10184,10.071938,10.091736,10.069,10.101399,10.108665,10.677613,10.062933,10.048022,10.08116,10.048581,10.008358,9.988336,10.020455,9.999856,9.94456,9.930587,9.941946,9.922861,9.898251,9.878906,9.898729,9.893158,9.875732,9.907771,9.870801,9.878806,9.8925,9.953664,9.900126,9.872298,9.874353,9.902461,9.909267,9.938772,9.957676,10.120104,9.981349,9.98143,10.018058,10.025088,10.066007,10.080737,10.117769,10.061616,10.079862,10.099225,10.103318,10.080079,10.093493,10.12106,10.126451,10.098126,10.064231,10.060977,10.063212,10.008159,9.969252,9.927233,9.902262,9.905951,9.897809,9.887289,9.88234,9.893798,9.900884,9.880104,9.904119,9.883998,9.906274,9.885134,9.900064,9.877508,9.850202,9.921247,9.925557,9.928351,9.930388,9.945218,9.984125,9.986199,10.010692,10.058064,10.049239,10.098865,10.103877,10.098884,10.081539,10.086289,10.09104,10.072975,10.077465,10.069919,10.098685,10.064051,10.013027,9.99123,10.023529,10.019735,9.973785,9.934419,9.931245,9.925718,9.907889,9.883737,9.871081,9.901523,9.87649,9.920986,9.883458,9.859704,9.888289,9.921284,9.890525,9.880321,9.902921,9.912602,9.9334,9.944802,9.940169,9.979213,10.029578,10.037123,10.054152,10.070658,10.143417,10.083594,10.070199,10.061039,10.092816,10.095251,10.076906,10.068125,10.055946,10.071099,10.052313,10.042054,10.009935,9.992348,10.001632,10.09096,9.96093,9.91408,9.923023,9.917931,9.907311,9.868168,9.877508,9.893717,9.899107,9.884576,9.907392,9.873199,9.888848,9.896592,10.365134,9.877869,9.860082,9.904958,9.979753,9.986082,10.043569,10.026982,10.052015,10.057605,10.068125,10.094295,10.118247,10.079024,10.082377,10.084811,10.089183,10.088705,10.118887,10.066386,10.061896,10.071037,10.052015,10.055468,10.000495,10.024647,10.002011,10.010891,9.961048,9.926792,10.461051,9.923681,9.909069,9.891003,9.87739,9.888966,9.902181,9.877769,9.90238,9.881402,9.902299,9.882899,9.907212,9.893779,9.857648,9.931065,9.920526,9.928432,9.98171,9.967935,9.985044,10.00229,10.012667,10.042073,10.065709,10.078384,10.071416,10.090401,10.059561,10.099803,10.649829,10.082594,10.058424,10.051196,10.094034,10.059759,9.988317,9.976859,10.029839,10.009177,9.968935,9.933841,9.925656,9.917272,9.876192,10.412146,9.876092,9.880943,9.871603,9.917272,9.925079,9.933003,9.970189,9.963184,9.942126,9.929929,9.936834,9.943243,9.972028,9.966817,10.501554,10.051394,10.031652,10.04347,10.064231,10.045805,10.062653,10.094592,10.070677,10.089481,10.073894,10.070578,10.097207,10.069901,10.061977,10.047084,10.090581,10.050419,10.007618,9.99131,10.016623,10.004886,9.961688,9.971947,9.945218,9.918589,9.892301,9.879347,9.882899,9.898449,9.905355,9.915695,9.899288,9.892897,9.910826,9.907112,9.903119,9.89771,9.889705,9.901902,9.926414,9.939592,9.972667,9.970649,9.999135,9.993465,10.013568,10.088165,10.119464,10.154558,10.122042,10.131463,10.122619,10.135474,10.13789,10.113496,10.115453,10.122141,10.133158,10.102678,10.100443,10.053233,10.064492,10.056207,10.01794,9.987876,9.926134,9.926774,9.913341,9.905256,9.981349,9.89707,9.91272,9.902181,9.889786,9.916272,9.895655,9.912143,9.878725,9.915875,9.886532,9.906355,9.927134,9.942126,9.956459,9.940089,9.98656,9.999036,10.00732,10.035167,10.072615,10.131643,10.079402,10.072795,10.089283,10.090761,10.081539,10.076067,10.07449,10.083495,10.06479,10.066466,10.010953,10.001272,10.025485,10.006581,9.978635,9.952646,9.948075,9.890065,9.918129,9.896232,9.918011,9.904796,9.912702,9.899747,9.895096,9.935238,9.951546,10.500374,9.936617,9.942324,9.952205,9.956099,9.994304,9.988777,9.995304,10.013369,10.041874,10.058443,10.065448,10.081278,10.114875,10.123395,10.147094,10.126271,10.142262,10.131742,10.141343,10.076707,10.120104,10.134518,10.143858,10.094934,10.054928,10.060039,10.065647,10.061896,10.013487,10.542914,9.997018,9.964464,9.94959,9.938772,9.930668,9.936456,9.959849,9.948913,9.943684,9.942504,9.93971,9.964861,9.934158,9.958794,10.488438,9.96021,9.969333,9.981809,10.018778,10.020374,10.039899,10.058542,10.062653,10.078303,10.115714,10.143939,10.133357,10.16827,10.036204,10.582517,10.092835,10.079421,10.063293,10.086966,10.090419,10.050177,10.01145,10.025963,10.031255,10.008277,9.967016,9.967097,9.924141,9.913639,9.932425,9.88773,9.893059,9.884675,9.904417,9.901064,9.889624,9.888389,9.910565,9.909367,9.89771,9.895915,9.91336,9.906392,9.910267,10.253288,9.956819,9.964023,9.975462,10.020995,10.013928,10.04896,10.069721,10.097828,10.064988,10.063492,10.123998,10.138368,10.132941,10.166954,10.112379,10.1315,10.142181,10.099884,10.071758,10.050717,10.106808,10.052195,10.014226,9.986821,9.977915,9.975841,9.962626,9.935617,9.938393,9.967898,9.952168,9.944479,9.941865,9.978238,9.946336,9.959471,9.927774,9.93376,9.937772,9.948174,9.968854,9.979014,10.009736,10.030155,10.046643,10.085749,10.064889,10.086488,10.119744,10.142163,10.131382,10.13204,10.124774,10.147373,10.137412,10.120501,10.128028,10.141442,10.13771,10.102796,10.071298,10.055487,10.061256,10.044849,10.013748,9.984721,9.952403,9.96121,9.949789,9.933363,9.935897,9.956099,9.95526,9.949752,9.941026,9.936735,9.949292,9.970351,9.92937,9.925755,9.936915,9.955658,10.003209,9.992329,9.977157,9.985839,9.995763,10.004445,10.009196,10.041893,10.068802,10.100064,10.062933,10.069342,10.078843,10.095729,10.125613,10.073093,10.080899,10.081259,10.099704,10.061995,10.025765,10.027379,10.009376,10.01281,9.984703,9.953124,9.928432,9.926855,9.903678,9.887631,9.895934,9.926476,9.919129,9.893239,9.894257,9.889326,10.449413,9.908771,9.899828,9.886072,10.062933,9.95069,9.97091,9.993627,9.998477,10.031832,10.042253,10.05445,10.065926,10.089264,10.106411,10.68029,10.129128,10.117589,10.123458,10.14869,10.14284,10.116751,10.132761,10.138449,10.177853,10.106709,10.056027,10.051177,10.068224,10.050457,10.5295,9.987659,9.969432,9.965482,9.96157,9.934698,9.935717,9.955279,9.97037,9.950609,9.946597,9.934518,10.084892,9.969612,9.944082,9.915496,9.942504,9.963166,9.966998,9.989615,10.047904,10.026342,10.041694,10.049221,10.061995,10.080502,10.109584,10.141803,10.133537,10.116589,10.648333,10.147094,10.129984,10.113757,10.119545,10.14302,10.141604,10.105473,10.065808,10.039819,10.067882,10.066466,10.015984,9.994285,9.984324,9.99059,9.949671,9.944541,9.907473,9.961048,9.90933,9.905336,9.888308,9.893897,9.908591,9.910205,9.898648,9.890146,9.900784,9.909926,10.07998,9.933021,9.964923,9.9861,9.990454,10.015263,9.997819,10.03359,10.074832,10.101281,10.088084,10.081458,10.077248,10.089364,10.076527,10.064889,10.094953,10.097207,10.086687,10.062536,10.018698,10.002768,10.013928,10.025622,9.999415,9.944479,9.934959,9.91821,10.076626,9.946255,9.941467,9.957018,9.962184,9.948951,9.946237,9.94574,9.947535,9.95454,9.946255,9.946038,9.950789,9.959812,9.97091,9.98692,10.012431,10.029298,10.051394,10.046824,10.058822,10.077365,10.111602,10.140505,10.141225,10.130245,10.125613,10.13807,10.137511,10.11739,10.118707,10.135953,10.141604,10.105411,10.042793,10.048103,10.078763,9.99744,10.175617,9.930587,9.930109,9.930606,9.91408,9.890003,9.887109,9.888488,9.916713,9.897809,9.88152,9.895015,9.907591,9.912341,9.922942,9.880023,9.893897,9.906752,9.915974,9.948653,9.966159,9.973344,10.009854,10.064728,10.016102,10.037142,10.076589,10.107709,10.091059,10.077266,10.082396,10.097306,10.096189,10.085451,10.076788,10.074111,10.097567,10.059977,10.109863,10.014046,10.032472,10.015524,9.959651,9.95077,9.928333,9.935058,9.906373,9.888289,9.89286,9.907212,9.910764,9.890804,9.91418,10.397651,9.908889,9.935717,9.913323,9.891922,9.878185,9.910286,9.932823,9.937474,9.958154,9.974804,9.985541,10.010134,10.00229,10.050475,10.105311,10.101399,10.079204,10.097468,10.08455,10.097288,10.113695,10.084433,10.31521,10.089624,10.104933,10.063175,10.016344,10.010214,10.02397,10.579784,10.015046,9.99141,9.975183,9.962464,9.956577,9.932624,9.933841,9.943983,9.963302,9.937393,9.925936,9.938232,9.953025,9.962464,9.970531,9.938151,9.933201,9.988255,9.960309,9.989534,10.006662,10.019815,10.04832,10.053133,10.065268,10.077564,10.116633,10.12701,10.091438,10.619026,10.262871,10.087786,10.100064,10.077067,10.081638,10.083514,10.096369,10.071956,10.030994,9.992627,10.019517,10.048004,9.973146,9.952925,10.449873,9.923303,9.917154,9.90366,9.894655,9.908808,9.916415,9.901362,9.919626,9.863256,9.910485,9.911404,9.893779,9.893978,9.90202,10.34156,9.920924,9.946976,9.97037,9.974624,10.000713,10.011413,10.055568,9.997278,10.081837,10.105392,10.094214,10.103256,10.082396,10.092015,10.079024,10.073254,10.073173,10.116949,10.097667,10.078384,10.044967,9.980114,10.028081,10.00778,9.968755,9.938952,9.929208,9.924259,9.906112,9.896412,9.890624,9.905138,9.909646,9.905417,9.92003,9.87639,9.910006,9.924079,9.900225,9.896052,9.900045,9.912422,9.936158,9.949969,9.961868,9.975599,10.126513,10.056406,10.083874,10.067125,10.108944,10.149528,10.165097,10.123358,10.123458,10.144895,10.137052,10.118446,10.115291,10.135555,10.138909,10.098126,10.077906,10.090283,10.05884,10.061635,10.021231,9.98043,9.970351,9.968674,9.966979,9.946994,9.936375,9.940908,9.902163,9.881104,9.872938,9.919607,9.901523,9.898449,9.879167,9.89853,9.892978,9.91254,10.158452,9.951429,9.962986,9.974344,10.005762,10.037142,10.015903,10.027622,10.08016,10.103815,10.094232,10.076148,10.080241,10.111081,10.06497,10.09114,10.085811,10.09535,10.092357,10.068125,10.015586,10.015245,10.023529,10.015443,9.972965,9.947355,9.925097,9.924917,9.887271,9.88765,9.889805,9.928929,9.951267,9.957496,10.42538,9.874055,9.89332,9.918868,9.887091,9.879582,9.90284,9.912422,9.921744,9.965041,9.958353,9.969631,9.997341,9.991329,10.042153,10.062194,10.064392,10.096189,10.093673,10.072795,10.055748,10.099821,10.090301,10.074074,10.066187,10.084731,10.081079,10.061157,10.019815,10.02782,10.575412,10.009556,9.965041,9.969612,9.936717,9.922961,9.911782,9.895915,9.895394,9.88106,9.921744,9.906013,10.162203,9.935238,9.952124,10.540995,9.945777,9.946535,9.941107,9.951789,9.97604,9.992869,10.007501,10.030317,10.081179,10.047463,10.062157,10.082675,10.117968,10.137828,10.64424,10.112459,10.144877,10.133996,10.133878,10.118626,10.124954,10.126035,10.120042,10.09663,10.051655,10.048581,10.066069,10.043191,10.011972,10.036285,9.969333,9.968674,9.950131,9.932065,10.030074,9.953422,9.98107,9.952366,9.937834,9.945777,9.964203,9.96103,9.949311,9.934518,10.234564,9.965203,9.968792,9.987199,10.023032,10.016182,10.039098,10.052494,10.099983,10.087668,10.128966,10.146634,10.125035,10.127171,10.127091,10.140685,10.141784,10.123358,10.11749,10.137449,10.145057,10.106609,10.067386,10.061318,10.072795,10.050817,10.013649,9.99095,9.977238,9.974164,9.961048,9.950727,9.941946,9.962725,9.968476,9.956117,9.950888,9.952745,9.974822,9.914037,9.899089,9.899604,9.896313,9.915856,9.922762,9.951149,9.941107,9.975841,10.004967,10.00283,10.021014,10.041613,10.073913,10.099343,10.132562,10.140343,10.130724,10.159949,10.141163,10.126811,10.126053,10.143299,10.14833,10.110404,10.025287,10.058921,10.164457,10.050159,10.017921,9.993248,9.974363,9.972487,9.947796,9.916235,9.971928,9.956359,9.959073,9.956658,9.941287,9.933264,9.956676,9.965041,9.957415,9.943622,9.972866,9.97137,9.976418,9.984206,10.016505,10.029758,10.046246,10.056648,10.055387,10.071695,10.120862,10.148212,10.129345,10.122539,10.132878,10.130922,10.140026,10.129984,10.076049,10.134257,10.25894,10.094754,10.052214,10.055207,10.07595,10.051096,10.014307,9.993087,9.967196,9.960371,9.957415,9.942983,9.942244,9.947174,9.973885,10.484805,9.926116,9.979132,9.951609,9.964663,9.941287,9.94374,9.943442,9.937853,9.985721,9.980691,10.015984,10.015623,10.043551,10.05399,10.594037,10.082576,10.123377,10.128388,10.138909,10.12773,10.086128,10.139027,10.141983,10.123638,10.130724,10.148069,10.115272,10.106988,10.072515,10.569463,10.087227,10.018319,9.972506,9.948274,9.91821,9.925656,9.924718,9.8914,9.903579,9.898629,9.920526,9.903219,9.901722,9.877049,9.941206,9.924439,9.956018,9.927792,9.948913,9.968494,9.978077,10.016083,10.018102,10.025566,10.046606,10.059741,10.068044,10.085271,10.12755,10.594533,10.137331,10.091401,10.075968,10.079582,10.075887,10.072037,10.07036,10.040694,10.086966,10.043451,10.00678,10.020995,10.015027,9.997161,9.989913,9.941666,9.942765,9.916894,9.905895,9.874217,9.884278,9.894916,9.882855,9.910367,9.890922,9.92324,9.888749,9.917192,9.898946,10.010494,9.881303,9.905976,9.919508,9.942324,9.964681,9.956974,10.00706,9.985342,10.019499,10.043371,10.080421,10.105392,10.083532,10.123439,10.096369,10.146851,10.14284,10.13853,10.111621,10.066106,10.07988,10.018499,10.029416,10.007122,10.01812,9.979753,9.973624,9.931866,9.89268,9.914298,9.902939,9.8925,9.857226,9.891202,9.904579,9.887668,9.889308,9.911224,9.894655,9.901803,9.894537,9.903318,9.912621,9.903299,9.931425,9.93953,9.950627,9.95023,10.006401,10.010196,10.006581,10.030435,10.087327,10.100561,10.077906,10.071838,10.103616,10.091916,10.08978,10.079024,10.071416,10.077285,10.046463,10.053872,10.007159,9.989156,10.010854,10.005246,9.972487,9.902461,9.92837,9.932723,9.884756,9.886451,9.878707,9.902921,9.916154,9.846029,9.903219,9.879402,9.922843,9.903958,9.898791,9.879645,9.861759,9.968954,9.978176,9.994844,10.123619,10.0183,10.042973,10.053512,10.065268,10.085109,10.108385,10.147473,10.131661,10.131481,10.137989,10.146175,10.087066,10.062455,10.061238,10.20075,10.061815,10.05866,10.002948,10.009637,9.992987,10.009836,9.972984,9.93989,9.906256,9.921464,9.904995,9.882358,9.881961,9.90384,10.40937,9.888488,9.908032,9.893239,9.923601,9.929668,9.899629,9.894456,9.900126,9.919707,9.931084,9.950348,9.973028,9.977058,10.001073,10.050618,10.05335,10.034689,10.070839,10.09681,10.081557,10.084731,10.084271,10.091699,10.123377,10.06936,10.055766,10.068783,10.112099,10.051475,10.557365,10.02215,10.014605,10.00257,9.962085,9.952565,9.91354,9.911963,9.900126,9.892959,9.897033,9.872838,9.903299,9.913261,9.894177,9.919129,9.951727,9.902281,9.895853,9.883377,9.930208,9.921843,9.92919,9.943082,9.973326,9.973903,9.978635,10.028839,10.010935,10.031633,10.623957,10.111279,10.084333,10.05445,10.073074,10.105491,10.09653,10.074968,10.083234,10.089742,10.097468,10.046824,10.042153,10.009097,10.03962,10.577666,9.991851,9.954279,9.904417,9.928991,9.914397,9.926594,9.951329,9.941585,9.951609,9.95536,9.936276,9.921383,9.955161,9.960651,10.442129,9.946895,9.949609,9.973543,9.969053,9.991211,10.013288,10.024069,10.051177,10.05435,10.051475,10.064411,10.116589,10.137431,10.138188,10.124395,10.159408,10.139648,10.145237,10.103976,10.13304,10.133239,10.137431,10.09589,10.050997,10.007699,10.077347,10.048184,10.016443,9.943821,9.935735,9.906554,9.912782,9.878266,9.874254,9.900685,9.905995,9.921346,9.886749,9.917633,9.894655,9.911323,9.887091,9.90805,9.877887,9.907373,9.916875,9.935419,9.947796,9.947634,9.985442,9.997539,10.010494,10.025106,10.071199,10.08996,10.062933,10.073093,10.096648,10.080781,10.08052,10.061256,10.064392,10.09068,10.062076,10.049121,10.010314,10.020095,10.01199,10.003967,9.974723,9.938971,9.910926,9.908149,9.88773,9.867727,9.898251,9.900424,9.929587,9.901542,9.921545,9.886432,9.89304,9.92901,9.898629,9.899207,9.841539,9.919607,9.92406,9.923601,9.931525,9.968873,9.985342,10.003489,10.02343,10.071056,10.055946,10.082756,10.083874,10.095593,10.056307,10.094034,10.09086,10.067783,10.049059,10.058741,10.089842,10.032031,10.019039,9.968991,9.99241,10.006321,9.948932,9.946597,9.915993,9.899766,9.889146,9.868845,9.873596,10.254947,9.868864,9.912882,9.858604,9.898828,9.892562,9.914676,9.876589,9.838465,9.868944,9.899648,9.922023,9.911963,9.944281,9.971947,10.405097,9.996521,9.998576,10.036744,10.036862,10.053034,10.081439,10.062896,10.02325,10.146733,10.143777,10.121681,10.126911,10.133419,10.140387,10.558086,10.015686,10.014226,10.005464,10.000352,9.945479,9.960589,9.920508,9.915974,9.898008,9.8935,9.881862,9.89917,9.910944,9.88719,9.923303,9.888227,9.899089,9.915155,9.883917,9.886811,9.895195,9.90184,9.919229,9.931245,9.949392,9.943163,9.968035,10.015605,10.005383,10.560781,10.051096,10.116192,10.082756,10.068404,10.110602,10.108746,10.101002,10.07,10.084911,10.115092,10.093835,10.045669,10.043551,10.033112,10.044488,10.014984,9.978257,9.953484,9.901803,9.931506,9.921626,9.905516,9.915776,9.910926,9.916713,9.905454,9.906293,9.922582,9.916974,10.450432,9.908907,9.89186,9.902343,9.914857,9.945759,9.939791,9.977257,9.961787,10.005743,10.052972,10.097784,10.107168,10.115335,10.136232,10.634179,10.131102,10.121961,10.139927,10.115372,10.124855,10.128128,10.140765,10.136213,10.087165,10.063591,10.06487,10.066286,10.058921,10.022492,10.130003,9.97594,9.973245,9.956695,9.943461,9.94492,9.952006,9.960849,9.956198,9.967115,9.978157,9.954242,9.958775,9.903579,9.939629,9.954521,9.963464,9.972866,9.985361,10.005644,10.023591,10.050879,10.046066,10.061256,10.100741,10.123458,10.144777,10.125134,10.136971,10.127351,10.158651,10.136114,10.159589,10.125352,10.131562,10.120744,10.096269,10.069062,10.079502,10.047382,10.050159,10.014984,9.977598,9.975742,9.964023,9.946578,9.934661,9.933003,9.939691,9.972127,9.962427,9.944361,9.965122,9.952105,9.960471,9.88683,9.90256,9.896052,9.923284,9.936654,9.949193,9.934003,9.978635,10.006041,10.009277,10.018139,10.072497,10.078421,10.103517,10.082675,10.087345,10.077825,10.093456,10.079663,10.087569,10.079303,10.084234,10.106572,10.061734,10.014406,10.010836,10.021691,10.02279,9.953664,9.945299,9.954503,9.931606,9.906734,9.89707,9.907491,9.912882,9.891283,9.916136,9.890544,9.941387,9.966575,9.969053,9.967637,9.962824,9.952447,9.963147,9.98089,9.992329,10.024665,10.059281,10.047364,10.053251,10.06487,10.086631,10.12206,10.146292,10.145616,10.128966,10.114993,10.147671,10.140424,10.158191,10.123638,10.128649,10.736542,10.096269,10.062175,10.042712,10.064032,10.045047,10.036185,9.987199,9.985622,9.971289,9.959191,9.945678,9.938971,9.950491,9.959893,9.972587,9.941946,9.936474,9.94923,10.002191,9.959533,9.943883,9.941585,9.961669,9.974723,9.978455,10.01281,10.030776,10.042532,10.057344,10.566569,10.08565,10.125395,10.148671,10.141461,10.130165,10.129867,10.144417,10.13853,10.12234,10.11685,10.131121,10.13871,10.10038,10.061355,10.575673,10.062355,10.046525,10.030776,9.980393,9.969233,9.980393,9.968016,9.949031,9.93404,9.964184,9.97155,9.952105,9.93953,9.951664,10.427913,9.976779,9.977157,9.973524,9.953764,9.986541,9.996241,10.014388,10.014506,10.031174,10.059039,10.062355,10.075788,10.08547,10.131904,10.176617,10.151105,10.150727,10.128109,10.155055,10.147653,10.128308,10.134816,10.140666,10.161365,10.105771,10.071416,10.048482,10.102399,10.047283,10.048419,9.993447,9.974624,9.968053,9.958136,9.936437,9.941765,9.960011,9.961048,9.956477,9.943442,9.937294,9.987957,9.971748,9.974903,9.944082,9.92937,9.962545,9.981268,9.988957,9.998738,10.049537,10.037502,10.04886,10.061896,10.076446,10.121123,10.143939,10.137809,10.129885,10.137331,10.144237,10.148727,10.12224,10.131823,10.135673,10.1325,10.164178,10.057623,10.045526,10.066268,10.051736,10.028479,10.004246,9.976977,9.918949,9.906671,9.894934,9.874894,9.910826,9.912143,9.881502,9.910485,9.888885,9.914478,9.895114,9.907112,9.881781,9.86715,9.905814,9.927134,9.930326,9.944821,9.95508,9.988317,10.002029,10.00293,10.048022,10.094953,10.095151,10.080998,10.08034,10.081837,10.09563,10.079141,10.073732,10.07028,10.066727,10.087227,10.046066,10.040675,10.007979,10.036744,10.003489,9.961427,9.930587,9.927712,9.92991,9.907951,10.125991,9.894059,9.906013,9.895872,9.938412,9.930506,9.89735,9.895474,9.928171,9.90841,9.901722,9.892518,9.922501,9.930208,9.947516,9.99113,9.987678,10.013729,10.00257,10.044849,10.042135,10.089165,10.109764,10.090941,10.303672,10.118129,10.150764,10.144678,10.127631,10.131382,10.689512,10.14356,10.115633,10.030137,10.007699,10.018139,9.976238,9.97512,9.938313,9.901163,9.89222,9.90366,9.892022,9.866907,9.891102,10.483389,9.891202,9.886153,9.909168,9.905914,9.911422,9.880663,9.909069,9.889065,9.903597,9.928333,9.941585,9.945597,9.938971,10.02864,10.510435,10.018958,10.25199,10.073832,10.09489,10.098108,10.078204,10.08529,10.102138,10.102039,10.094971,10.127451,10.078682,10.092997,10.100443,10.029696,10.041135,10.005265,9.994385,9.95508,9.966078,9.920508,9.912161,9.908528,9.883278,9.880303,9.868646,9.90833,9.902082,9.87803,10.477502,9.914639,9.914279,9.880204,9.884557,9.925836,9.901144,9.928531,9.936735,9.962085,9.979095,9.973624,10.02774,10.031012,10.041315,10.076546,10.114894,10.079322,10.067764,10.072173,10.129227,10.086966,10.079123,10.082197,10.096189,10.09653,10.04365,10.042514,10.010295,10.013307,10.005184,9.98692,9.948013,9.915875,9.935338,9.906355,9.887469,9.874813,9.910286,9.935599,9.901703,9.906013,9.920607,9.919229,9.914658,9.914,9.924656,9.906392,10.181206,9.977338,10.005383,10.03313,10.025765,10.053332,10.062355,10.075571,10.090221,10.129245,10.135096,10.140144,10.185398,10.138368,10.139548,10.130724,10.124197,10.124215,10.138648,10.140964,10.102778,10.06012,10.089003,10.070578,10.053729,10.012171,10.020554,9.973245,9.974642,9.962346,9.939052,9.938971,9.963644,9.959073,9.955738,9.943821,9.947336,9.986721,10.087966,9.951267,9.967296,9.948733,9.962085,9.98143,9.981268,10.012891,10.021933,10.04868,10.050835,10.058064,10.08583,10.123917,10.145156,10.121942,10.140865,10.134735,10.136493,10.148348,10.123557,10.131481,10.137313,10.141505,10.106969,10.068783,10.056307,10.099362,10.056524,10.020635,10.009277,9.975661,9.970152,10.327326,9.927532,9.932146,9.946616,9.968612,9.957676,9.94528,9.977598,9.958154,9.964284,9.959632,9.956378,9.967078,9.971767,9.985703,10.427336,9.945516,9.975499,10.009935,10.015263,10.02828,10.063635,10.073552,10.102039,10.076247,10.096828,10.078843,10.094592,10.093114,10.08062,10.624038,10.068205,10.093754,10.056424,10.017958,10.008618,10.035285,10.00247,9.968215,9.931885,9.947174,9.948454,9.906491,10.138151,9.899405,9.937735,9.915875,9.903038,9.893779,9.900505,9.906715,9.913062,9.900523,9.893537,9.931146,9.91775,9.935897,9.966817,10.015543,10.01299,10.603917,10.067684,10.069522,10.085811,10.126712,10.160346,10.135853,10.115453,10.123178,10.143498,10.145616,10.150547,10.128668,10.132419,10.170289,10.115912,10.051537,10.052754,10.062355,10.046743,10.01776,10.071838,9.973686,9.970711,9.954161,9.960669,9.894338,9.862678,9.904237,9.901542,10.433223,9.885594,9.9139,9.910186,9.894636,9.881601,9.91867,9.906932,9.915037,9.935158,9.969053,9.986199,9.971189,10.016822,10.004066,10.48293,10.07046,10.111099,10.06397,10.061337,10.052276,10.099784,10.087885,10.079204,10.065529,10.072876,10.087246,10.031435,10.030435,10.013469,10.108286,9.992528,9.988957,9.946038,9.919309,9.923222,9.910845,9.888948,9.875832,9.908311,9.923619,9.905417,9.901821,9.917235,9.918309,9.927811,9.900586,9.92434,9.900685,9.9139,9.937095,9.952565,9.957496,9.952205,10.011612,10.013189,10.025187,10.072037,10.092897,10.087823,10.080719,10.090382,10.112279,10.108168,10.093177,10.084694,10.082054,10.357347,10.063833,10.078843,10.001073,9.993645,10.002489,10.003886,9.961986,9.92534,9.921067,9.912143,9.904237,9.893158,9.877049,9.920185,9.913161,9.888469,9.917893,9.885973,9.912863,9.880762,9.903678,9.882278,9.884476,9.898946,9.927594,9.938909,9.934599,9.95526,9.995322,10.002452,10.016903,10.05984,10.072894,10.091059,10.09535,10.094133,10.078744,10.308323,10.100262,10.083514,10.103057,10.114776,10.145255,10.107267,10.052791,10.063113,10.068621,10.046985,10.029317,10.027541,9.969513,10.318961,9.895015,9.889426,9.881321,9.875714,9.913838,9.889705,9.884215,9.880284,9.907851,9.909727,9.901244,9.880961,9.917614,9.905237,10.411326,9.947255,9.951727,9.98097,9.968295,10.005662,10.009637,10.037719,10.05435,10.099722,10.099902,10.066628,10.088643,10.094773,10.095692,10.117769,10.081557,10.092816,10.086488,10.042551,10.038421,10.030137,10.018102,9.994186,9.979213,9.940809,9.896971,9.916813,9.921824,9.897052,10.454984,9.911764,9.925457,9.908591,9.905256,9.91867,9.928252,9.90769,9.896474,9.916515,9.915217,9.915695,9.942604,9.952646,9.971829,9.983585,10.008655,10.225423,10.066647,10.083352,10.119644,10.147212,10.157893,10.121681,10.130065,10.144417,10.12819,10.105293,10.125432,10.13917,10.690531,10.101759,10.057903,10.04301,10.076229,10.052115,10.023908,9.986821,9.972866,9.961508,9.984802,9.956179,9.944821,9.957838,9.97091,10.51834,9.883576,9.87749,9.888966,9.90823,9.885333,9.873614,9.895357,9.911863,9.950509,10.162843,9.975002,9.980592,10.020834,10.007501,10.527544,10.050997,10.094195,10.091699,10.082377,10.075608,10.083973,10.092736,10.088103,10.091519,10.075887,10.083414,10.088364,10.015822,10.010134,10.01327,10.030994,9.993347,9.975381,9.946057,9.935158,9.922663,9.909087,9.915217,9.890444,9.902281,9.921744,9.920446,9.940089,9.931164,9.95087,9.955639,9.939052,9.88188,9.909628,9.906454,9.93504,9.951807,10.000452,9.962228,10.00796,10.010575,10.018238,10.04419,10.079862,10.100542,10.081278,10.076049,10.083594,10.108646,10.086091,10.087625,10.114676,10.097604,10.084613,10.048581,10.015785,10.000253,10.012171,9.999576,9.959732,9.956117,9.925737,9.918011,9.910267,9.903281,9.896232,9.907671,9.912341,9.910385,9.909926,10.105113,9.911323,9.919968,9.908609,9.901623,9.909826,9.921464,9.93386,9.945498,9.980592,9.976779,10.003147,10.013469,10.045606,10.008618,10.075608,10.104094,10.077943,10.086848,10.09096,10.098505,10.105212,10.079024,10.086588,10.07962,10.104374,10.055387,10.03844,9.985603,10.019716,10.032851,9.974065,9.95554,9.934959,9.92855,9.901722,9.900865,9.900846,10.0486,9.951348,9.943361,9.870702,9.883837,9.916154,9.901703,9.899288,9.873316,9.906752,10.45109,9.928053,9.944479,9.962526,9.956738,9.964843,10.022132,10.024728,10.040855,10.05966,10.099704,10.074372,10.058064,10.068522,10.093816,10.107808,10.072155,10.054369,10.080818,10.082377,10.025268,10.026224,10.015245,10.014965,9.985324,9.982368,9.937934,9.918949,9.905616,9.912242,10.443203,9.873497,9.899846,9.919508,9.909187,9.921843,9.90338,9.899685,9.922582,9.888507,9.907572,9.90138,9.863796,9.941225,9.932363,10.484165,9.923681,10.022989,9.993528,9.992248,10.025106,10.084892,10.081061,10.07046,10.064591,10.084532,10.060679,10.095114,10.061896,10.087587,10.588087,10.04329,10.074111,9.987758,9.989174,9.996241,10.01317,10.016344,9.996521,9.979275,9.961228,9.953664,9.945678,9.938754,9.947174,9.996124,9.948951,9.948553,9.944361,9.971767,9.966258,9.938673,9.935518,9.941206,9.9647,9.98638,9.998676,10.018499,10.021753,10.054531,10.449953,10.047103,10.094592,10.127109,10.142262,10.130264,10.127308,10.13286,10.11164,10.140883,10.1314,10.124395,10.139207,10.132897,10.059561,10.069441,10.049239,10.071118,10.058163,10.017921,9.988994,9.969413,9.970513,9.948472,9.94977,9.94859,9.951969,9.958434,9.955062,9.878725,9.890301,9.901803,9.921924,9.89799,9.874434,9.88701,9.918191,9.935158,9.927432,9.947615,9.96506,9.990391,10.000713,10.071956,10.042992,10.076409,10.094313,10.086209,10.073894,10.03313,10.08619,10.076626,10.07018,10.06936,10.089562,10.093655,10.050419,10.012053,10.026703,10.013649,9.999694,9.956397,9.956577,9.95069,9.934959,9.913,9.880384,9.890463,9.871838,9.925575,9.908628,9.898368,9.866131,9.917272,9.920048,9.904498,9.927675,9.899964,9.869323,9.935536,9.93486,9.949509,9.942765,9.958993,10.031633,10.016723,10.036682,10.073434,10.097549,10.077086,10.095071,10.116769,10.133077,10.133139,10.135915,10.128848,10.142343,10.19572,10.053512,10.006283,9.990634,10.036744,9.993745,9.961626,10.001371,9.946597,9.916136,9.896071,9.899027,9.877229,9.896133,9.885414,9.915856,9.890742,9.888326,9.889506,9.926774,9.904219,9.884135,10.445041,9.914776,9.957875,9.930227,9.945417,9.966619,9.984045,9.9968,10.045308,10.040297,10.08565,10.107448,10.079141,10.082377,10.088444,10.62328,10.103616,10.092518,10.089742,10.113794,10.111938,10.105591,10.065647,10.057785,10.066684,10.055027,10.0183,9.992789,9.976481,9.966637,10.467317,9.946715,9.934878,9.965321,9.961147,9.951987,9.932282,9.938313,9.970469,9.970829,9.945498,9.950168,9.938015,9.972587,10.029038,10.023169,10.022591,10.029596,10.002768,10.015903,10.022871,10.038241,10.080502,10.112857,10.086948,10.080359,10.083892,10.087029,10.098884,10.08519,10.625994,10.102896,10.054549,10.052313,10.022852,10.018996,10.021293,10.020437,9.96688,9.947336,9.932363,9.923321,9.913099,9.903597,9.928531,9.951565,9.92955,9.909528,9.894555,9.905814,9.915217,9.923023,9.909429,9.894375,9.89753,9.917074,9.989174,9.984324,10.01812,10.03395,10.187615,10.073832,10.07988,10.097586,10.125693,10.135195,10.126271,10.128687,10.129705,10.144877,10.139865,10.13222,10.115931,10.152882,10.139927,10.131543,10.065529,10.047724,10.05994,10.041234,10.021014,9.976319,9.976499,9.958632,9.957614,9.942126,9.938331,9.921744,9.969873,9.953683,9.93943,9.942883,9.961427,9.916515,9.944541,9.941964,9.944839,9.963265,9.988038,9.989093,10.008935,10.035645,10.04393,10.056424,10.066448,10.122979,10.113037,10.147392,10.1227,10.127929,10.125756,10.146175,10.129388,10.130823,10.128767,10.148311,10.136691,10.086668,10.050475,10.053791,10.075987,10.0485,10.023051,9.993447,9.986839,9.932841,9.948932,9.954602,9.943343,9.964284,9.963365,9.920129,9.882458,9.883656,9.917732,9.923122,9.895754,9.903759,9.893978,9.945641,9.938331,9.941126,9.967556,9.990932,10.011413,10.014866,10.0183,10.038142,10.091239,10.109205,10.083135,10.112577,10.085992,10.097567,10.099964,10.084153,10.078943,10.108385,10.088885,10.04942,10.027442,10.012332,10.023169,10.021672,10.055946,9.954242,9.947075,9.922861,9.914937,9.899884,9.899666,9.904678,9.951528,9.913279,9.900846,9.897232,9.911503,9.915415,9.891003,10.363954,9.895574,9.917552,9.942045,9.962427,9.963923,9.988516,10.001272,10.058461,10.024007,10.041054,10.087426,10.103535,10.094971,10.078384,10.109683,10.108367,10.106411,10.089382,10.084793,10.095332,10.134176,10.066106,10.017958,10.007681,10.031913,10.00778,9.975499,9.991329,9.987199,10.51349,9.964942,9.935518,9.934419,9.957577,9.963247,9.958893,9.956179,9.9442,9.959551,9.964104,9.945957,9.952484,9.941585,9.963625,10.008097,9.992789,10.010953,10.030975,10.047581,10.056424,10.066466,10.079303,10.127929,10.147771,10.132518,10.126532,10.11182,10.14841,10.147311,10.624678,10.12773,10.1325,10.142361,10.095512,10.07046,10.00842,10.019356,10.005662,9.964364,9.971189,9.930686,9.922203,9.916055,9.891202,10.494207,9.884296,9.91775,9.905373,9.871162,9.904399,9.919868,9.914117,9.907013,9.898251,9.924141,9.910926,9.92434,9.954124,9.962508,10.465125,9.968376,10.026224,10.019995,10.039756,10.073552,10.113037,10.061157,10.083495,10.081557,10.108466,10.091059,10.06451,10.069243,10.091022,10.086687,10.063572,10.019418,10.036744,9.983305,10.008836,9.971189,9.953304,9.942026,9.93422,9.910926,9.904877,9.994186,9.910348,9.895375,9.909447,9.883656,9.884613,9.896872,9.923439,9.890426,9.875254,9.887848,9.913161,9.948274,9.940188,9.960371,9.974102,9.993943,9.99131,10.035726,10.051158,10.085749,10.07621,10.076968,10.073534,10.048382,10.082495,10.090022,10.068205,10.112279,10.093754,10.095593,10.057046,10.014127,10.004905,10.026963,9.984603,9.967737,9.942784,9.943045,9.935077,9.918831,9.899505,9.917769,9.956558,9.964961,9.954322,9.948814,9.942585,9.906535,9.899865,9.878446,9.907032,9.889885,9.896033,9.925656,9.945759,9.951509,9.937195,10.004544,10.004246,10.024728,10.040197,10.083396,10.09763,10.079781,10.083992,10.103815,10.108764,10.075428,10.076707,10.075111,10.091717,10.068423,10.071596,10.008997,9.99644,10.006662,10.058704,9.97594,9.935456,9.91921,9.927792,9.911845,9.894735,9.904299,9.901921,9.918651,9.892618,9.951267,9.901424,9.919968,9.910485,10.447159,9.893518,9.876471,9.916235,9.942902,9.956595,9.950609,9.981368,10.010016,10.019337,10.084072,10.080601,10.12306,10.143461,10.145336,10.16809,10.125215,10.144038,10.140045,10.135214,10.134474,10.135493,10.139567,10.088507,10.055207,10.057704,10.063231,10.056145,10.026783,9.989255,10.476502,9.973605,9.954621,9.938772,9.963464,9.951286,9.969314,9.951925,9.948833,9.942802,9.945318,9.972866,9.961886,9.949112,9.941865,10.496182,10.010854,9.998216,10.026143,10.032211,10.049879,10.058083,10.070199,10.09553,10.121222,10.149186,10.151403,10.111441,10.102318,10.093754,10.594055,10.066547,10.077545,10.083315,10.057605,10.091978,10.009177,10.00211,10.00724,10.003706,9.952267,9.924979,9.923141,9.919328,9.902442,9.911323,9.877626,9.904138,</t>
+  </si>
+  <si>
+    <t>-0.125446,-0.093527,-0.087113,-0.130768,-0.09433,-0.082933,-0.130472,-0.093824,-0.086575,-0.127984</t>
+  </si>
+  <si>
+    <t>-5.547451,-5.541592,-5.530503,-5.533288,-5.539128,-5.541863,-5.53498,-5.535226,-5.527713,-5.54663,-5.540221,-5.53493,-5.531911,-5.541345,-5.545216,-5.540795,-5.535776,-5.54048,-5.539962,-5.547722,-5.54132,-5.533269,-5.525237,-5.538826,-5.540505,-5.53911,-5.529664,-5.542462,-5.542438,-5.538289,-5.531331,-5.538289,-5.542166,-5.546864,-5.536579,-5.52967,-5.539357,-5.541351,-5.536054,-5.532164,-5.533004,-5.539116,-5.539956,-5.532998,-5.532461,-5.539647,-5.545802,-5.541623,-5.536579,-5.53301,-5.536041,-5.552186,-5.541907,-5.539116,-5.53577,-5.543864,-5.549124,-5.53356,-5.5419,-5.536054,-5.545796,-5.539382,-5.540511,-5.534652,-5.537134,-5.543296,-5.541363,-5.542728,-5.5333,-5.53911,-5.545228,-5.541048,-5.532448,-5.53385,-5.541876,-5.547432,-5.535782,-5.533282,-5.545488,-5.533251,-5.54245,-5.529948,-5.531596,-5.530528,-5.542746,-5.543012,-5.531615,-5.539141,-5.543543,-5.541635,-5.535214,-5.527417,-5.539937,-5.54161,-5.542752,-5.531874,-5.537171,-5.532436,-5.542734,-5.541073,-5.534399,-5.545809,-5.545778,-5.530497,-5.534696,-5.535751,-5.537999,-5.542999,-5.538542,-5.529374,-5.533547,-5.538542,-5.547167,-5.537412,-5.532448,-5.540511,-5.541567,-5.539937,-5.536579,-5.533294,-5.545772,-5.542999,-5.538807,-5.539116,-5.531355,-5.546074,-5.539672,-5.537999,-5.52967,-5.537727,-5.539653,-5.536356,-5.539388,-5.537999,-5.538264,-5.545253,-5.541888,-5.534961,-5.534405,-5.541326,-5.536881,-5.539666,-5.532726,-5.537196,-5.540215,-5.537159,-5.538863,-5.530769,-5.54216,-5.539956,-5.540758,-5.530479,-5.537437,-5.548568,-5.54829,-5.532757,-5.543574,-5.535776,-5.542722,-5.539406,-5.541888,-5.526046,-5.53272,-5.537431,-5.537165,-5.532708,-5.533831,-5.537147,-5.537721,-5.540511,-5.536362,-5.541851,-5.543283,-5.544129,-5.537437,-5.528559,-5.544129,-5.542184,-5.54245,-5.528571,-5.533004,-5.539388,-5.544407,-5.535776,-5.526336,-5.536048,-5.543555,-5.536869,-5.538838,-5.534103,-5.548574,-5.548568,-5.543845,-5.540783,-5.535751,-5.543592,-5.545222,-5.529682,-5.53385,-5.536332,-5.550235,-5.543024,-5.541061,-5.539122,-5.546309,-5.546068,-5.536332,-5.531893,-5.546309,-5.537721,-5.542147,-5.533294,-5.534381,-5.540215,-5.550519,-5.545784,-5.534381,-5.543265,-5.542456,-5.546043,-5.543246,-5.531318,-5.536597,-5.537992,-5.538567,-5.537986,-5.538289,-5.539394,-5.549087,-5.542722,-5.533263,-5.54329,-5.541345,-5.540196,-5.533844,-5.532146,-5.541876,-5.541345,-5.537171,-5.534677,-5.53414,-5.541616,-5.546346,-5.531899,-5.532158,-5.543012,-5.536017,-5.543012,-5.535473,-5.537443,-5.5369,-5.537986,-5.544944,-5.533257,-5.529935,-5.541061,-5.544654,-5.536041,-5.529917,-5.527435,-5.539357,-5.538554,-5.540221,-5.530763,-5.533263,-5.544117,-5.531621,-5.534412,-5.536572,-5.537165,-5.54466,-5.536325,-5.541913,-5.541055,-5.538283,-5.546599,-5.53853,-5.527978,-5.536603,-5.545228,-5.536616,-5.534134,-5.538276,-5.54358,-5.544117,-5.538838,-5.530769,-5.543845,-5.539974,-5.540758,-5.534109,-5.53075,-5.541882,-5.544654,-5.545809,-5.531337,-5.536887,-5.532417,-5.545815,-5.533831,-5.541357,-5.536023,-5.548828,-5.545506,-5.536634,-5.531078,-5.54103,-5.532998,-5.5419,-5.541061,-5.531893,-5.539943,-5.543561,-5.531343,-5.539419,-5.53969,-5.54387,-5.539672,-5.53272,-5.531584,-5.539962,-5.538857,-5.541635,-5.537992,-5.539104,-5.540802,-5.548006,-5.53356,-5.528256,-5.539666,-5.54579,-5.543549,-5.530491,-5.530238,-5.540783,-5.541332,-5.543246,-5.538283,-5.537715,-5.540783,-5.539678,-5.536338,-5.534936,-5.539925,-5.549099,-5.549667,-5.538011,-5.535782,-5.538844,-5.545512,-5.531886,-5.529108,-5.537443,-5.534942,-5.543555,-5.541048,-5.534078,-5.533831,-5.533813,-5.542728,-5.533294,-5.534936,-5.544673,-5.549371,-5.542728,-5.534967,-5.537702,-5.539098,-5.544666,-5.544389,-5.531053,-5.544938,-5.542722,-5.5394,-5.537733,-5.536893,-5.542431,-5.542722,-5.543561,-5.533535,-5.537721,-5.537986,-5.544389,-5.537999,-5.526608,-5.537147,-5.551884,-5.54829,-5.527157,-5.538573,-5.54495,-5.537418,-5.543018,-5.533566,-5.536035,-5.541876,-5.53995,-5.542172,-5.531609,-5.53577,-5.548821,-5.534128,-5.53882,-5.533276,-5.53856,-5.541604,-5.545481,-5.533263,-5.536048,-5.542172,-5.540795,-5.537992,-5.526867,-5.547729,-5.538838,-5.530503,-5.542468,-5.528262,-5.540234,-5.538844,-5.546056,-5.533319,-5.535764,-5.539116,-5.543851,-5.538832,-5.533819,-5.536035,-5.538851,-5.539919,-5.534658,-5.534097,-5.541604,-5.542722,-5.546605,-5.529108,-5.538573,-5.543006,-5.545222,-5.537974,-5.532448,-5.536362,-5.542154,-5.540252,-5.534949,-5.530497,-5.541351,-5.552452,-5.542172,-5.532979,-5.534374,-5.540758,-5.544926,-5.539672,-5.526879,-5.541907,-5.54992,-5.536628,-5.538258,-5.540777,-5.54048,-5.541882,-5.541061,-5.530516,-5.534134,-5.543012,-5.543283,-5.539085,-5.533004,-5.541616,-5.538826,-5.543845,-5.528571,-5.538548,-5.540783,-5.544944,-5.542709,-5.529127,-5.539684,-5.541907,-5.545228,-5.534658,-5.53856,-5.540518,-5.548556,-5.532461,-5.527701,-5.53409,-5.539104,-5.540783,-5.546914,-5.535492,-5.538276,-5.544389,-5.544685,-5.534103,-5.532998,-5.542438,-5.545506,-5.540505,-5.537418,-5.537721,-5.536924,-5.53522,-5.537455,-5.525182,-5.531047,-5.543296,-5.54329,-5.537165,-5.536344,-5.544389,-5.542722,-5.541882,-5.531621,-5.5419,-5.537739,-5.537165,-5.529133,-5.532726,-5.541326,-5.545506,-5.543006,-5.540499,-5.531899,-5.53827,-5.540777,-5.541598,-5.531349,-5.532973,-5.545518,-5.54466,-5.538863,-5.530238,-5.542734,-5.542166,-5.53577,-5.537999,-5.541604,-5.54132,-5.540493,-5.536301,-5.536023,-5.533819,-5.54466,-5.543024,-5.537418,-5.530522,-5.53911,-5.542715,-5.541882,-5.540771,-5.536881,-5.538017,-5.549377,-5.535782,-5.53577,-5.542438,-5.544938,-5.550785,-5.532177,-5.531078,-5.538005,-5.54187,-5.539369,-5.532701,-5.542166,-5.53856,-5.546648,-5.539659,-5.531874,-5.535504,-5.543018,-5.551871,-5.535776,-5.532714,-5.543845,-5.541888,-5.53911,-5.537999,-5.528528,-5.543567,-5.544685,-5.535486,-5.538011,-5.538289,-5.54437,-5.539672,-5.530503,-5.535517,-5.540518,-5.540795,-5.547735,-5.536332,-5.537449,-5.537159,-5.545204,-5.536035,-5.525774,-5.538579,-5.549118,-5.541048,-5.541048,-5.531053,-5.538276,-5.54687,-5.540764,-5.532424,-5.540758,-5.547432,-5.535813,-5.544401,-5.531596,-5.533831,-5.540215,-5.54329,-5.541055,-5.529645,-5.540209,-5.53853,-5.53769,-5.526571,-5.524385,-5.543555,-5.544932,-5.534646,-5.532726,-5.536325,-5.544697,-5.544926,-5.528806,-5.543839,-5.54216,-5.542734,-5.538005,-5.539641,-5.539672,-5.541894,-5.53882,-5.533825,-5.53664,-5.539388,-5.542734,-5.535776,-5.536622,-5.539666,-5.540511,-5.551334,-5.535196,-5.532992,-5.535764,-5.542703,-5.539684,-5.532189,-5.528534,-5.541882,-5.546327,-5.538264,-5.538838,-5.52996,-5.536887,-5.542981,-5.543283,-5.5369,-5.533269,-5.537733,-5.545488,-5.53522,-5.534936,-5.543574,-5.537999,-5.5419,-5.540795,-5.543833,-5.542722,-5.544957,-5.53911,-5.537165,-5.533245,-5.545802,-5.544117,-5.533547,-5.536616,-5.548013,-5.550217,-5.537424,-5.530787,-5.531602,-5.543821,-5.539937,-5.540777,-5.530201,-5.5394,-5.541326,-5.542987,-5.537165,-5.53159,-5.541604,-5.545753,-5.542715,-5.532967,-5.533288,-5.537999,-5.542734,-5.546605,-5.531312,-5.54024,-5.542425,-5.544963,-5.537992,-5.527738,-5.533837,-5.539388,-5.531041,-5.531325,-5.533004,-5.536066,-5.542999,-5.538554,-5.533813,-5.530195,-5.542141,-5.541314,-5.535757,-5.534671,-5.543555,-5.548272,-5.541629,-5.530781,-5.528009,-5.54329,-5.542975,-5.535208,-5.53356,-5.537437,-5.540221,-5.544685,-5.529948,-5.536066,-5.53522,-5.545506,-5.542172,-5.531047,-5.536912,-5.550223,-5.542987,-5.53827,-5.535226,-5.535196,-5.547185,-5.541073,-5.542166,-5.532424,-5.542722,-5.537702,-5.546333,-5.533035,-5.532158,-5.540499,-5.546895,-5.540493,-5.533844,-5.536066,-5.544142,-5.540227,-5.539672,-5.532442,-5.539666,-5.543018,-5.538542,-5.539666,-5.530226,-5.547451,-5.544135,-5.540215,-5.531609,-5.53217,-5.542172,-5.545518,-5.538295,-5.531065,-5.541073,-5.5394,-5.543006,-5.540783,-5.531041,-5.544419,-5.539135,-5.534097,-5.530787,-5.536066,-5.53827,-5.537733,-5.540221,-5.537455,-5.531306,-5.547185,-5.53995,-5.53214,-5.527441,-5.543277,-5.544975,-5.536066,-5.53719,-5.53798,-5.543012,-5.542178,-5.535208,-5.536609,-5.539135,-5.541888,-5.537739,-5.533547,-5.532979,-5.537159,-5.546914,-5.538258,-5.531065,-5.538005,-5.538011,-5.543845,-5.537449,-5.53911,-5.543543,-5.547469,-5.533844,-5.537968,-5.532152,-5.545494,-5.539122,-5.536622,-5.533263,-5.543851,-5.542154,-5.540215,-5.532177,-5.534387,-5.546624,-5.537424,-5.540493,-5.530781,-5.542697,-5.544395,-5.542178,-5.539116,-5.526071,-5.53911,-5.540777,-5.551865,-5.547457,-5.531047,-5.542993,-5.532751,-5.537437,-5.535214,-5.533257,-5.546877,-5.549673,-5.537992,-5.532732,-5.539412,-5.535757,-5.546352,-5.531343,-5.535239,-5.534103,-5.547438,-5.545222,-5.529948,-5.532417,-5.538258,-5.536869,-5.533294,-5.537715,-5.539116,-5.539666,-5.540227,-5.53243,-5.543271,-5.544957,-5.543314,-5.54358,-5.530503,-5.541339,-5.541616,-5.537449,-5.535504,-5.532726,-5.543851,-5.534665,-5.531615,-5.538289,-5.541623,-5.545228,-5.544135,-5.541616,-5.533819,-5.537745,-5.543833,-5.541604,-5.538542,-5.53606,-5.538807,-5.541592,-5.53882,-5.531071,-5.540511,-5.53214,-5.549957,-5.538826,-5.529423,-5.535214,-5.542975,-5.54634,-5.526898,-5.537702,-5.536869,-5.542468,-5.544117,-5.534658,-5.535208,-5.544382,-5.537696,-5.537739,-5.531028,-5.541339,-5.540209,-5.546889,-5.536072,-5.535208,-5.53551,-5.542993,-5.54466,-5.538276,-5.538276,-5.542166,-5.543839,-5.535788,-5.533844,-5.534368,-5.543277,-5.547161,-5.536875,-5.536616,-5.540771,-5.538548,-5.542431,-5.535788,-5.537196,-5.539122,-5.542962,-5.536912,-5.525521,-5.537171,-5.546599,-5.538567,-5.530491,-5.52967,-5.54634,-5.549118,-5.539937,-5.531874,-5.539128,-5.53911,-5.543018,-5.531343,-5.528837,-5.537431,-5.55134,-5.537999,-5.535523,-5.530497,-5.53272,-5.533844,-5.53548,-5.533257,-5.53356,-5.541876,-5.540771,-5.540215,-5.530757,-5.539116,-5.537443,-5.538832,-5.533288,-5.534671,-5.538838,-5.540196,-5.535239,-5.534967,-5.532732,-5.537443,-5.547451,-5.536591,-5.530516,-5.537165,-5.550248,-5.53301,-5.539666,-5.540783,-5.536313,-5.544117,-5.539647,-5.534103,-5.533269,-5.548846,-5.547179,-5.541048,-5.531337,-5.539104,-5.544963,-5.529386,-5.532695,-5.534955,-5.541332,-5.544957,-5.534936,-5.530769,-5.533837,-5.537999,-5.53911,-5.536893,-5.541894,-5.546605,-5.540474,-5.536066,-5.533276,-5.53493,-5.543259,-5.547192,-5.543271,-5.527738,-5.537727,-5.542703,-5.53911,-5.543845,-5.53272,-5.536041,-5.546346,-5.541314,-5.526324,-5.53606,-5.547192,-5.548006,-5.534405,-5.536325,-5.531886,-5.545778,-5.540777,-5.536338,-5.531899,-5.543839,-5.548865,-5.539641,-5.536054,-5.537165,-5.539394,-5.537715,-5.541351,-5.525509,-5.53159,-5.539394,-5.544117,-5.533016,-5.532448,-5.548815,-5.536319,-5.539943,-5.52299,-5.539388,-5.537437,-5.543271,-5.533547,-5.527454,-5.537727,-5.551631,-5.539104,-5.534121,-5.531355,-5.541339,-5.547173,-5.546914,-5.539098,-5.530769,-5.544938,-5.541882,-5.543277,-5.537177,-5.537721,-5.541339,-5.539943,-5.53214,-5.537992,-5.544395,-5.541042,-5.535492,-5.534665,-5.528015,-5.539653,-5.545518,-5.540474,-5.526305,-5.543839,-5.551618,-5.536609,-5.532745,-5.535504,-5.535233,-5.540783,-5.539943,-5.532164,-5.537992,-5.544648,-5.543283,-5.531621,-5.531868,-5.537727,-5.54634,-5.532448,-5.54216,-5.535214,-5.549698,-5.539382,-5.536072,-5.538832,-5.534387,-5.541339,-5.541086,-5.534665,-5.528034,-5.53664,-5.541616,-5.543839,-5.528269,-5.537177,-5.54274,-5.544401,-5.54274,-5.527441,-5.541332,-5.545772,-5.547994,-5.541048,-5.531065,-5.541857,-5.54466,-5.536066,-5.536585,-5.529411,-5.540771,-5.540196,-5.53606,-5.537171,-5.542709,-5.548574,-5.543302,-5.539635,-5.533844,-5.538017,-5.538573,-5.537739,-5.531886,-5.531312,-5.542444,-5.54913,-5.537721,-5.534381,-5.535226,-5.540493,-5.544376,-5.533837,-5.531615,-5.538283,-5.537733,-5.538567,-5.53075,-5.530522,-5.544376,-5.542456,-5.543277,-5.531034,-5.536054,-5.549118,-5.542166,-5.53243,-5.529108,-5.539388,-5.540209,-5.543555,-5.533269,-5.538542,-5.537153,-5.542431,-5.538542,-5.53606,-5.536881,-5.546062,-5.537455,-5.537177,-5.532448,-5.532992,-5.536616,-5.543018,-5.533572,-5.537992,-5.54776,-5.542191,-5.536881,-5.536603,-5.544679,-5.546333,-5.539678,-5.528262,-5.535239,-5.540789,-5.539104,-5.537177,-5.524367,-5.539666,-5.539412,-5.541894,-5.536893,-5.539116,-5.540789,-5.546605,-5.538283,-5.52604,-5.534381,-5.542975,-5.540221,-5.537177,-5.533578,-5.52717,-5.54634,-5.553828,-5.539672,-5.539406,-5.531312,-5.541882,-5.543302,-5.54103,-5.532152,-5.538567,-5.542438,-5.533541,-5.537715,-5.537721,-5.543265,-5.546346,-5.536622,-5.526602,-5.536887,-5.543296,-5.542147,-5.53385,-5.533541,-5.548858,-5.534387,-5.533837,-5.532177,-5.532436,-5.546617,-5.53606,-5.531905,-5.534084,-5.536893,-5.550791,-5.546889,-5.541623,-5.534399,-5.537974,-5.548266,-5.539956,-5.540511,-5.537196,-5.539956,-5.542734,-5.538536,-5.526614,-5.537171,-5.543567,-5.542172,-5.539375,-5.531337,-5.549383,-5.549124,-5.540499,-5.534374,-5.536869,-5.53856,-5.547161,-5.536616,-5.527997,-5.540493,-5.543574,-5.539659,-5.538258,-5.534387,-5.536325,-5.542444,-5.541351,-5.531047,-5.532177,-5.547426,-5.541332,-5.532424,-5.531065,-5.535745,-5.534097,-5.536628,-5.538289,-5.539375,-5.538826,-5.538567,-5.544944,-5.529386,-5.534374,-5.535782,-5.538838,-5.538295,-5.534658,-5.542975,-5.546617,-5.52909,-5.533572,-5.54132,-5.55076,-5.536881,-5.532738,-5.538283,-5.536597,-5.545512,-5.537184,-5.53243,-5.529423,-5.534967,-5.54884,-5.540221,-5.536338,-5.534671,-5.542715,-5.541882,-5.540258,-5.525472,-5.536912,-5.542981,-5.543018,-5.538801,-5.532183,-5.539659,-5.538283,-5.537992,-5.539672,-5.529398,-5.544938,-5.546068,-5.531874,-5.53409,-5.540246,-5.544957,-5.538851,-5.540487,-5.529676,-5.530775,-5.541894,-5.542438,-5.529639,-5.537449,-5.537424,-5.536048,-5.537147,-5.533269,-5.53798,-5.548013,-5.534665,-5.530781,-5.536591,-5.54634,-5.542166,-5.538832,-5.533522,-5.541055,-5.543561,-5.545784,-5.537424,-5.53188,-5.543271,-5.539122,-5.542715,-5.536338,-5.525466,-5.536319,-5.544352,-5.542444,-5.527447,-5.535776,-5.538844,-5.53856,-5.539122,-5.539666,-5.536054,-5.543561,-5.533825,-5.534677,-5.541332,-5.548581,-5.542154,-5.537715,-5.531615,-5.532461,-5.548846,-5.544092,-5.531893,-5.532732,-5.539666,-5.53882,-5.539672,-5.537171,-5.533288,-5.541048,-5.546901,-5.541888,-5.540789,-5.528262,-5.542166,-5.535776,-5.530491,-5.536628,-5.527738,-5.535776,-5.541067,-5.527163,-5.539116,-5.547173,-5.544673,-5.5252,-5.538276,-5.532442,-5.528571,-5.546062,-5.531337,-5.527182,-5.536325,-5.544395,-5.539931,-5.540474,-5.537715,-5.547154,-5.540771,-5.541616,-5.52746,-5.540505,-5.540493,-5.544969,-5.527182,-5.535239,-5.533553,-5.540802,-5.536035,-5.532701,-5.526318,-5.543827,-5.547192,-5.533547,-5.536622,-5.536609,-5.544382,-5.537424,-5.534936,-5.539925,-5.539369,-5.545488,-5.539912,-5.528559,-5.536863,-5.540518,-5.548006,-5.535486,-5.534955,-5.524132,-5.548284,-5.541882,-5.540203,-5.535751,-5.532436,-5.538542,-5.53714,-5.534121,-5.527985,-5.539419,-5.545525,-5.536048,-5.531615,-5.537449,-5.54187,-5.539703,-5.539684,-5.532448,-5.538832,-5.536924,-5.544395,-5.535764,-5.537986,-5.539412,-5.543277,-5.538542,-5.523545,-5.534658,-5.54353,-5.535486,-5.538838,-5.533831,-5.543543,-5.542135,-5.532454,-5.522977,-5.542999,-5.54274,-5.542734,-5.534103,-5.525774,-5.540764,-5.538838,-5.54245,-5.536609,-5.535214,-5.538567,-5.54216,-5.538838,-5.53356,-5.533819,-5.540777,-5.538814,-5.528244,-5.534084,-5.539653,-5.545494,-5.537147,-5.537184,-5.528824,-5.535776,-5.543561,-5.538295,-5.530485,-5.539406,-5.543283,-5.540511,-5.532708,-5.529096,-5.53969,-5.540252,-5.538814,-5.530516,-5.540777,-5.537196,-5.543271,-5.53577,-5.5252,-5.538814,-5.547148,-5.542166,-5.537165,-5.529966,-5.542166,-5.546062,-5.540758,-5.536628,-5.535498,-5.551334,-5.543006,-5.534942,-5.531053,-5.541326,-5.543018,-5.535764,-5.537449,-5.528812,-5.532732,-5.545759,-5.545772,-5.537443,-5.527423,-5.546346,-5.542166,-5.538863,-5.534665,-5.53714,-5.536054,-5.543845,-5.542987,-5.530787,-5.544679,-5.540783,-5.543265,-5.528824,-5.535757,-5.543024,-5.54216,-5.535214,-5.534103,-5.543277,-5.540215,-5.540499,-5.530213,-5.532992,-5.543024,-5.542722,-5.535233,-5.537696,-5.538536,-5.545216,-5.540505,-5.536869,-5.533288,-5.533553,-5.543851,-5.543302,-5.541073,-5.532424,-5.534368,-5.537153,-5.53385,-5.533541,-5.534399,-5.538258,-5.54466,-5.543845,-5.53577,-5.539956,-5.539968,-5.536609,-5.53551,-5.530794,-5.542135,-5.540221,-5.540505,-5.536369,-5.532424,-5.538844,-5.540518,-5.541061,-5.525219,-5.536622,-5.546315,-5.540524,-5.542456,-5.534393,-5.538283,-5.539382,-5.543277,-5.533251,-5.535504,-5.535776,-5.539085,-5.541351,-5.536634,-5.539388,-5.544123,-5.534689,-5.53051,-5.531053,-5.540524,-5.545759,-5.537184,-5.53522,-5.538258,-5.543271,-5.532738,-5.536863,-5.53551,-5.53714,-5.536622,-5.5419,-5.532992,-5.532998,-5.539388,-5.539962,-5.530775,-5.527738,-5.533541,-5.539937,-5.54245,-5.533282,-5.534103,-5.543271,-5.541079,-5.540802,-5.5394,-5.534646,-5.535214,-5.545506,-5.538283,-5.530201,-5.531596,-5.544666,-5.547173,-5.540505,-5.535764,-5.537727,-5.539678,-5.538289,-5.529114,-5.537727,-5.539931,-5.550513,-5.53606,-5.536863,-5.53719,-5.54495,-5.541036,-5.529658,-5.528812,-5.531331,-5.541604,-5.542444,-5.532695,-5.526052,-5.539931,-5.541339,-5.534097,-5.526058,-5.534936,-5.534955,-5.537702,-5.534368,-5.530787,-5.539116,-5.54048,-5.545228,-5.531911,-5.533004,-5.536918,-5.54495,-5.540221,-5.526886,-5.533276,-5.539394,-5.54132,-5.536591,-5.53051,-5.536023,-5.542154,-5.542178,-5.542154,-5.538863,-5.539128,-5.535486,-5.54137,-5.535757,-5.537437,-5.53522,-5.541326,-5.532714,-5.528287,-5.542178,-5.549402,-5.543012,-5.529954,-5.531318,-5.543845,-5.547469,-5.54274,-5.539382,-5.533276,-5.547185,-5.536603,-5.539666,-5.541623,-5.531621,-5.542166,-5.53522,-5.522163,-5.538005,-5.541061,-5.546593,-5.534362,-5.534677,-5.547185,-5.539394,-5.534381,-5.538838,-5.530522,-5.537184,-5.543814,-5.528565,-5.531325,-5.535498,-5.545222,-5.542715,-5.53356,-5.529942,-5.530769,-5.544142,-5.537159,-5.536887,-5.534942,-5.544685,-5.532164,-5.540246,-5.5369,-5.53606,-5.544642,-5.545253,-5.538554,-5.532998,-5.534689,-5.541876,-5.534109,-5.536048,-5.537147,-5.543814,-5.547167,-5.538005,-5.530497,-5.535523,-5.545512,-5.545506,-5.530781,-5.539666,-5.534955,-5.547722,-5.540789,-5.537715,-5.531053,-5.546605,-5.541598,-5.536887,-5.532708,-5.539962,-5.549402,-5.543277,-5.53414,-5.530497,-5.538542,-5.541326,-5.547994,-5.534121,-5.527688,-5.544117,-5.541339,-5.535226,-5.529664,-5.535776,-5.55047,-5.54495,-5.535239,-5.539696,-5.538567,-5.541888,-5.534109,-5.531596,-5.529386,-5.540215,-5.54495,-5.534393,-5.522737,-5.532461,-5.539388,-5.538801,-5.534924,-5.541326,-5.534912,-5.551921,-5.54274,-5.534109,-5.532726,-5.540227,-5.547698,-5.538579,-5.530232,-5.533269,-5.548013,-5.536863,-5.539091,-5.542154,-5.536319,-5.544969,-5.535492,-5.53356,-5.543851,-5.5394,-5.537999,-5.53995,-5.52938,-5.536622,-5.53301,-5.542728,-5.532695,-5.533819,-5.539116,-5.544907,-5.537147,-5.532985,-5.534677,-5.54245,-5.538832,-5.536622,-5.531886,-5.536628,-5.546611,-5.531337,-5.534677,-5.530763,-5.537437,-5.547747,-5.536881,-5.537184,-5.531893,-5.533566,-5.53577,-5.529639,-5.526034,-5.536066,-5.548562,-5.53856,-5.524675,-5.534949,-5.542456,-5.543821,-5.53882,-5.536319,-5.534683,-5.547457,-5.539104,-5.538264,-5.538276,-5.536887,-5.536054,-5.53827,-5.537455,-5.530503,-5.542135,-5.543549,-5.532998,-5.531325,-5.534121,-5.536332,-5.542999,-5.537153,-5.538276,-5.538517,-5.539394,-5.542715,-5.531868,-5.531596,-5.54024,-5.534393,-5.536338,-5.538276,-5.530219,-5.544944,-5.529923,-5.539653,-5.533553,-5.525503,-5.540215,-5.544685,-5.529929,-5.526589,-5.539943,-5.538832,-5.537986,-5.527972,-5.534652,-5.543271,-5.543018,-5.536319,-5.534955,-5.53577,-5.544957,-5.542444,-5.531615,-5.52967,-5.539931,-5.543845,-5.535498,-5.531646,-5.53522,-5.537727,-5.539684,-5.537171,-5.529658,-5.527713,-5.547729,-5.537443,-5.536344,-5.533282,-5.54608,-5.538844,-5.53856,-5.52967,-5.533819,-5.541339,-5.538295,-5.545241,-5.531325,-5.536628,-5.533004,-5.544086,-5.530503,-5.532436,-5.537721,-5.543561,-5.532992,-5.533831,-5.536332,-5.543018,-5.542999,-5.532127,-5.532708,-5.540499,-5.546068,-5.543277,-5.533269,-5.528256,-5.54161,-5.544697,-5.537159,-5.530528,-5.536622,-5.53719,-5.544685,-5.541616,-5.53856,-5.537721,-5.542697,-5.539116,-5.534393,-5.538838,-5.543555,-5.541635,-5.537165,-5.529658,-5.533831,-5.546056,-5.545241,-5.532738,-5.528553,-5.541894,-5.541623,-5.538542,-5.529639,-5.531325,-5.539394,-5.540215,-5.538283,-5.532454,-5.529367,-5.547741,-5.544382,-5.530195,-5.538554,-5.539931,-5.542999,-5.532164,-5.531331,-5.534634,-5.537449,-5.544395,-5.535214,-5.531355,-5.53522,-5.545234,-5.540511,-5.530485,-5.532177,-5.543833,-5.53522,-5.5399,-5.530479,-5.537739,-5.541623,-5.543845,-5.535208,-5.530497,-5.536881,-5.54245,-5.538258,-5.534103,-5.534677,-5.539647,-5.543833,-5.540505,-5.533276,-5.544092,-5.53577,-5.542709,-5.538554,-5.534393,-5.545204,-5.545204,-5.536338,-5.527157,-5.530769,-5.54466,-5.541061,-5.535226,-5.529392,-5.532732,-5.534924,-5.541314,-5.53243,-5.53493,-5.536332,-5.538307,-5.540227,-5.526608,-5.538838,-5.533831,-5.546333,-5.543277,-5.531065,-5.536325,-5.540227,-5.543524,-5.540771,-5.529954,-5.53522,-5.537708,-5.54216,-5.527731,-5.53635,-5.544666,-5.542728,-5.535801,-5.531355,-5.54492,-5.54161,-5.541888,-5.534955,-5.527707,-5.53911,-5.539357,-5.537177,-5.535523,-5.53577,-5.539659,-5.548544,-5.540474,-5.53356,-5.54048,-5.547204,-5.540802,-5.533819,-5.524089,-5.538814,-5.542728,-5.540499,-5.530503,-5.536325,-5.530757,-5.544389,-5.539382,-5.528546,-5.534381,-5.53827,-5.546062,-5.533004,-5.530787,-5.534671,-5.539696,-5.537758,-5.531053,-5.532473,-5.538838,-5.542419,-5.534671,-5.53243,-5.536628,-5.552458,-5.544401,-5.531893,-5.531065,-5.542987,-5.543839,-5.540752,-5.526361,-5.530232,-5.544376,-5.54053,-5.537431,-5.529077,-5.533282,-5.549136,-5.542722,-5.538548,-5.53159,-5.54161,-5.547192,-5.546358,-5.534949,-5.535757,-5.538301,-5.543561,-5.535214,-5.526052,-5.534628,-5.544135,-5.537159,-5.536622,-5.524947,-5.539672,-5.545216,-5.536338,-5.529121,-5.542987,-5.547179,-5.540227,-5.540789,-5.537986,-5.540487,-5.541326,-5.551618,-5.534374,-5.527139,-5.53577,-5.545759,-5.534918,-5.527985,-5.529627,-5.541925,-5.541598,-5.53356,-5.52883,-5.530232,-5.533825,-5.546062,-5.535782,-5.531078,-5.536881,-5.541048,-5.541882,-5.521595,-5.542172,-5.541332,-5.543821,-5.532442,-5.534121,-5.544697,-5.540493,-5.539925,-5.533831,-5.53217,-5.539937,-5.538264,-5.545469,-5.522409,-5.534683,-5.539388,-5.538554,-5.536054,-5.535504,-5.531856,-5.535498,-5.541592,-5.541616,-5.541086,-5.539962,-5.537764,-5.544105,-5.530497,-5.537424,-5.543555,-5.544092,-5.536029,-5.537184,-5.533288,-5.548821,-5.538542,-5.530491,-5.52825,-5.54634,-5.544389,-5.543827,-5.532417,-5.532152,-5.550217,-5.550495,-5.529639,-5.530497,-5.533819,-5.543833,-5.546068,-5.537721,-5.536881,-5.544389,-5.542154,-5.536622,-5.53301,-5.542468,-5.532726,-5.541876,-5.540487,-5.534961,-5.537147,-5.546333,-5.543296,-5.536054,-5.531596,-5.540487,-5.548284,-5.541907,-5.537696,-5.536906,-5.535757,-5.538548,-5.536628,-5.541882,-5.536863,-5.540493,-5.542691,-5.530787,-5.54048,-5.538258,-5.546605,-5.532714,-5.528577,-5.536622,-5.546883,-5.539425,-5.531615,-5.524965,-5.541629,-5.538005,-5.542419,-5.532164,-5.536048,-5.547735,-5.544389,-5.540493,-5.53911,-5.538548,-5.547469,-5.540499,-5.529973,-5.533547,-5.538554,-5.534374,-5.532164,-5.533263,-5.526052,-5.542191,-5.532701,-5.53853,-5.53301,-5.533276,-5.537992,-5.540499,-5.534942,-5.533004,-5.542728,-5.544987,-5.536332,-5.52883,-5.534418,-5.542438,-5.546049,-5.535782,-5.533813,-5.536048,-5.54687,-5.540783,-5.526886,-5.531627,-5.55134,-5.543821,-5.535788,-5.531609,-5.540789,-5.544117,-5.543845,-5.533831,-5.531362,-5.540258,-5.542475,-5.544407,-5.534134,-5.537412,-5.541623,-5.544389,-5.531337,-5.530491,-5.547198,-5.535764,-5.548013,-5.536066,-5.530473,-5.54466,-5.542438,-5.538023,-5.536616,-5.532152,-5.539672,-5.538826,-5.534942,-5.528015,-5.5394,-5.539943,-5.539684,-5.538289,-5.533831,-5.539641,-5.544666,-5.545778,-5.536066,-5.536344,-5.541048,-5.543555,-5.539931,-5.530207,-5.534115,-5.540764,-5.547173,-5.53827,-5.535233,-5.542475,-5.542475,-5.541073,-5.529096,-5.535776,-5.539085,-5.553285,-5.538289,-5.532714,-5.533547,-5.542431,-5.535233,-5.53635,-5.53606,-5.53577,-5.541357,-5.535776,-5.536072,-5.536603,-5.53856,-5.541326,-5.531355,-5.534393,-5.540487,-5.544685,-5.544654,-5.535788,-5.532992,-5.538844,-5.539684,-5.541604,-5.539666,-5.533837,-5.542166,-5.538542,-5.535504,-5.529114,-5.539641,-5.541055,-5.54634,-5.542734,-5.530794,-5.543549,-5.543296,-5.538591,-5.532417,-5.53356,-5.543814,-5.542438,-5.53911,-5.528577,-5.539672,-5.543283,-5.538017,-5.536344,-5.541332,-5.540499,-5.544932,-5.539684,-5.53464,-5.537715,-5.541314,-5.543549,-5.535776,-5.533547,-5.53856,-5.539968,-5.542172,-5.530226,-5.534134,-5.539098,-5.541913,-5.541913,-5.532424,-5.529935,-5.542431,-5.540511,-5.532146,-5.531337,-5.538567,-5.547179,-5.54103,-5.528546,-5.539943,-5.547735,-5.546037,-5.532424,-5.532732,-5.533294,-5.544092,-5.543814,-5.540493,-5.539382,-5.537159,-5.543283,-5.539369,-5.537974,-5.528281,-5.544963,-5.546617,-5.528275,-5.526898,-5.533553,-5.540808,-5.543839,-5.53522,-5.541598,-5.540246,-5.53856,-5.540795,-5.532454,-5.536881,-5.535757,-5.54884,-5.542456,-5.53551,-5.540789,-5.532985,-5.546043,-5.541598,-5.530232,-5.534942,-5.541623,-5.540499,-5.534381,-5.534109,-5.545228,-5.551631,-5.534097,-5.528843,-5.527182,-5.545204,-5.540511,-5.535239,-5.528009,-5.540203,-5.540764,-5.540505,-5.528824,-5.532998,-5.540487,-5.542722,-5.532152,-5.534677,-5.535498,-5.538295,-5.542734,-5.52412,-5.529942,-5.536875,-5.539122,-5.544957,-5.531059,-5.532732,-5.546895,-5.547185,-5.539943,-5.536887,-5.533844,-5.540209,-5.535782,-5.531041,-5.534121,-5.537702,-5.54053,-5.539098,-5.532979,-5.536344,-5.546346,-5.544673,-5.540493,-5.528534,-5.537443,-5.538554,-5.540209,-5.535214,-5.528022,-5.532454,-5.550495,-5.547457,-5.538579,-5.529096,-5.544111,-5.53827,-5.538832,-5.52741,-5.535239,-5.543018,-5.539116,-5.528009,-5.532726,-5.538536,-5.549402,-5.531312,-5.532998,-5.538844,-5.54216,-5.552433,-5.535233,-5.530497,-5.537165,-5.540209,-5.539968,-5.533825,-5.533547,-5.537134,-5.544376,-5.540221,-5.53827,-5.539943,-5.544957,-5.546895,-5.533288,-5.532454,-5.539369,-5.543567,-5.547173,-5.533251,-5.536863,-5.543296,-5.54608,-5.542728,-5.535486,-5.538573,-5.553298,-5.542722,-5.536344,-5.532436,-5.544944,-5.538838,-5.532417,-5.539388,-5.530219,-5.541598,-5.545802,-5.535782,-5.534381,-5.540221,-5.545778,-5.542728,-5.539135,-5.531602,-5.535776,-5.542993,-5.546895,-5.533572,-5.531071,-5.545506,-5.545778,-5.532177,-5.535226,-5.538264,-5.54048,-5.532714,-5.544926,-5.535214,-5.538567,-5.544135,-5.532158,-5.535226,-5.529392,-5.540246,-5.537153,-5.537733,-5.52909,-5.537424,-5.549099,-5.534942,-5.534109,-5.530781,-5.539937,-5.543296,-5.548587,-5.52854,-5.531602,-5.536616,-5.54521,-5.537437,-5.530503,-5.536603,-5.542709,-5.546624,-5.532454,-5.534381,-5.542431,-5.534387,-5.536609,-5.531337,-5.528553,-5.539116,-5.54245,-5.539659,-5.528009,-5.53385,-5.532745,-5.546333,-5.540518,-5.53217,-5.536906,-5.546877,-5.538832,-5.530781,-5.529676,-5.534658,-5.551612,-5.539919,-5.531059,-5.539672,-5.53827,-5.537992,-5.534128,-5.532992,-5.53522,-5.541345,-5.534924,-5.532985,-5.533004,-5.544938,-5.542987,-5.536072,-5.534405,-5.529664,-5.543851,-5.541042,-5.530497,-5.527157,-5.547438,-5.54048,-5.538826,-5.539375,-5.531065,-5.543574,-5.542184,-5.538283,-5.528818,-5.536338,-5.548834,-5.536325,-5.534671,-5.529651,-5.543012,-5.542975,-5.533813,-5.529948,-5.524095,-5.539678,-5.532973,-5.538276,-5.531312,-5.527991,-5.539666,-5.537443,-5.529367,-5.535529,-5.540221,-5.541604,-5.535492,-5.542178,-5.534128,-5.540499,-5.546043,-5.532442,-5.527163,-5.537437,-5.543259,-5.542184,-5.533813,-5.53356,-5.538276,-5.540227,-5.536048,-5.531874,-5.539653,-5.546321,-5.542709,-5.533276,-5.534399,-5.53522,-5.546333,-5.536628,-5.528287,-5.532448,-5.545216,-5.541623,-5.54466,-5.527151,-5.537702,-5.5455,-5.538838,-5.537986,-5.526595,-5.53551,-5.54634,-5.539672,-5.533566,-5.532732,-5.540221,-5.546611,-5.540487,-5.52775,-5.538295,-5.542135,-5.541061,-5.53522,-5.538005,-5.528281,-5.540511,-5.542154,-5.531893,-5.538573,-5.540771,-5.538567,-5.543839,-5.534665,-5.533553,-5.548006,-5.533257,-5.546068,-5.530522,-5.539122,-5.543283,-5.539937,-5.530479,-5.525503,-5.549124,-5.54437,-5.532708,-5.532152,-5.539394,-5.53911,-5.53853,-5.532177,-5.534121,-5.534683,-5.548266,-5.543024,-5.533547,-5.530787,-5.544123,-5.536319,-5.535486,-5.533269,-5.539672,-5.548587,-5.539653,-5.529664,-5.540246,-5.529645,-5.533263,-5.542154,-5.534405,-5.536319,-5.537153,-5.539375,-5.53998,-5.534658,-5.53995,-5.54274,-5.542993,-5.539141,-5.537455,-5.541079,-5.554112,-5.538844,-5.527966,-5.541061,-5.544944,-5.543555,-5.539122,-5.534936,-5.538826,-5.540783,-5.546889,-5.537733,-5.533263,-5.539943,-5.544685,-5.534362,-5.52854,-5.5369,-5.547432,-5.546056,-5.537992,-5.526071,-5.544389,-5.547463,-5.54579,-5.524397,-5.53051,-5.543586,-5.544969,-5.541332,-5.53301,-5.534356,-5.545247,-5.542999,-5.53356,-5.532127,-5.536572,-5.547161,-5.539122,-5.527713,-5.534128,-5.537992,-5.54245,-5.542178,-5.531893,-5.533578,-5.539375,-5.544129,-5.539116,-5.536887,-5.532985,-5.546901,-5.542184,-5.54053,-5.533578,-5.540209,-5.538536,-5.542438,-5.539104,-5.533862,-5.548284,-5.544666,-5.534109,-5.527176,-5.546346,-5.548303,-5.541616,-5.529948,-5.534399,-5.539635,-5.544666,-5.542172,-5.534393,-5.536893,-5.544685,-5.543277,-5.532985,-5.522718,-5.538017,-5.540221,-5.53882,-5.534405,-5.530503,-5.542734,-5.541604,-5.538005,-5.529133,-5.542987,-5.540234,-5.548,-5.530219,-5.526608,-5.544389,-5.541876,-5.542734,-5.530516,-5.52746,-5.543018,-5.537424,-5.542728,-5.529121,-5.542135,-5.544111,-5.545228,-5.535782,-5.536035,-5.540505,-5.539956,-5.539375,-5.537418,-5.535745,-5.529948,-5.554952,-5.532424,-5.536893,-5.538548,-5.545228,-5.538844,-5.526311,-5.529108,-5.534942,-5.543283,-5.531893,-5.525472,-5.537739,-5.543567,-5.53911,-5.540487,-5.530775,-5.540795,-5.537159,-5.533294,-5.530769,-5.533535,-5.540511,-5.537999,-5.541363,-5.532436,-5.534955,-5.544926,-5.547729,-5.539116,-5.52746,-5.540771,-5.542431,-5.540789,-5.543555,-5.532695,-5.53995,-5.547173,-5.533269,-5.530497,-5.534399,-5.548284,-5.536319,-5.537159,-5.526583,-5.537721,-5.547994,-5.537702,-5.52996,-5.53051,-5.5394,-5.540764,-5.540518,-5.535492,-5.534918,-5.543851,-5.537147,-5.539116,-5.523268,-5.536066,-5.537437,-5.536875,-5.528269,-5.524083,-5.534918,-5.541876,-5.536603,-5.528806,-5.537733,-5.541604,-5.545518,-5.53217,-5.532701,-5.542993,-5.543018,-5.535788,-5.536338,-5.530485,-5.534405,-5.54103,-5.535245,-5.537449,-5.535776,-5.546068,-5.538857,-5.533837,-5.536332,-5.53272,-5.547167,-5.538838,-5.533541,-5.534109,-5.536035,-5.546901,-5.535467,-5.535788,-5.53359,-5.539419,-5.538826,-5.539678,-5.537745,-5.53856,-5.546327,-5.54161,-5.537727,-5.538295,-5.539659,-5.543814,-5.537715,-5.531349,-5.535782,-5.549939,-5.546889,-5.535764,-5.531041,-5.536881,-5.537159,-5.536048,-5.532164,-5.534134,-5.542184,-5.552452,-5.536319,-5.529948,-5.539116,-5.540518,-5.539956,-5.535523,-5.531596,-5.534665,-5.542431,-5.538536,-5.533547,-5.538542,-5.542178,-5.539135,-5.541042,-5.53301,-5.530781,-5.54245,-5.548284,-5.535788,-5.534393,-5.537177,-5.551056,-5.531886,-5.531596,-5.534115,-5.544926,-5.5394,-5.53214,-5.532158,-5.536356,-5.546901,-5.539937,-5.536072,-5.533831,-5.53272,-5.54329,-5.53827,-5.538542,-5.535214,-5.545494,-5.550772,-5.541919,-5.529966,-5.540499,-5.542734,-5.543283,-5.528837,-5.526898,-5.541042,-5.539388,-5.534103,-5.536616,-5.532732,-5.537455,-5.54024,-5.537437,-5.535776,-5.537159,-5.537184,-5.537739,-5.537165,-5.532967,-5.547457,-5.536603,-5.546086,-5.529102,-5.532448,-5.536906,-5.541635,-5.52633,-5.524385,-5.538832,-5.544666,-5.535233,-5.538579,-5.539937,-5.54024,-5.538826,-5.539684,-5.527738,-5.534399,-5.545494,-5.538536,-5.533535,-5.526058,-5.536066,-5.539357,-5.540752,-5.539672,-5.531034,-5.539678,-5.547457,-5.53301,-5.519397,-5.539678,-5.549957,-5.541048,-5.536041,-5.532998,-5.532164,-5.539098,-5.539653,-5.52938,-5.53551,-5.542987,-5.539937,-5.546062,-5.535486,-5.529398,-5.541919,-5.539678,-5.542734,-5.533541,-5.536591,-5.536609,-5.539672,-5.534399,-5.529386,-5.537147,-5.544382,-5.529676,-5.532998,-5.538011,-5.534683,-5.549112,-5.531609,-5.532164,-5.541913,-5.541888,-5.536362,-5.531325,-5.539666,-5.545537,-5.548865,-5.536048,-5.533819,-5.537708,-5.538844,-5.538017,-5.537461,-5.531034,-5.536869,-5.534671,-5.540499,-5.536356,-5.529108,-5.540518,-5.539104,-5.538005,-5.539406,-5.531602,-5.541332,-5.5369,-5.543827,-5.532714,-5.531899,-5.545475,-5.543283,-5.528269,-5.532448,-5.541332,-5.544944,-5.53214,-5.53301,-5.535492,-5.542166,-5.53719,-5.533868,-5.537147,-5.535245,-5.546605,-5.532424,-5.528262,-5.535202,-5.539956,-5.541345,-5.542444,-5.529966,-5.539672,-5.544932,-5.541339,-5.531911,-5.533239,-5.541919,-5.539098,-5.538289,-5.537999,-5.537999,-5.546611,-5.546327,-5.540215,-5.535208,-5.534387,-5.543845,-5.540493,-5.53522,-5.533269,-5.538301,-5.53911,-5.534393,-5.53</t>
+  </si>
+  <si>
+    <t>-7.9971,-8.002638,-8.006243,-7.981239,-7.999304,-7.98014,-7.99847,-8.039286,-8.083201,-8.129635,-8.14352,-8.190769,-8.23774,-8.336096,-8.412245,-8.507854,-8.551491,-8.843263,-8.552874,-8.522023,-8.542286,-8.523702,-8.537878,-8.499247,-8.555936,-8.520344,-8.448368,-8.406935,-8.405299,-8.400311,-8.329187,-8.219082,-8.361088,-8.07573,-7.992068,-7.981251,-7.990129,-7.999032,-8.012324,-8.016239,-8.588442,-8.004286,-8.01543,-8.005694,-7.998174,-7.995402,-8.004879,-8.017393,-7.99818,-8.062382,-8.096024,-8.15604,-8.136012,-8.190485,-8.283593,-8.366404,-8.475336,-8.541767,-8.522276,-8.562598,-8.560351,-8.549256,-8.562604,-8.561203,-8.555066,-8.542008,-8.53313,-8.542045,-8.470594,-8.420283,-8.414221,-8.40588,-8.314994,-8.206611,-8.169913,-8.073211,-8.008756,-8.005391,-8.293583,-8.025697,-8.002341,-8.019029,-8.00457,-8.030692,-7.99568,-8.00846,-8.025703,-8.015411,-8.016251,-8.017084,-8.021536,-8.089881,-8.136877,-8.149373,-8.161325,-8.200783,-8.315284,-8.378054,-8.477287,-8.531753,-8.565648,-8.53037,-8.57844,-8.542854,-8.548966,-8.549799,-8.549799,-8.550083,-8.575958,-8.524807,-8.474786,-8.418944,-8.424759,-8.399465,-8.311092,-8.217428,-8.126295,-8.05101,-7.986221,-7.977893,-7.980665,-8.11436,-8.001545,-7.977917,-7.9829,-7.995414,-7.970935,-7.985709,-7.998767,-8.004854,-8.001773,-8.003755,-7.999872,-8.064062,-8.097117,-8.129635,-8.729867,-8.223009,-8.295521,-8.371386,-8.478929,-8.512546,-8.537013,-8.53092,-8.543434,-8.535056,-8.51922,-8.526184,-8.550645,-8.530345,-8.539532,-8.503946,-8.410325,-8.393075,-8.952196,-8.386666,-8.291354,-8.221348,-8.111823,-8.044021,-8.031254,-7.997384,-8.008472,-8.029043,-8.022931,-7.985122,-8.989721,-8.000156,-8.015677,-7.990981,-8.031525,-8.010435,-7.984029,-8.010707,-8.05043,-8.106853,-8.140223,-8.162146,-8.154089,-8.225238,-8.327761,-8.418641,-8.519226,-8.537285,-8.54231,-8.579835,-8.554566,-8.543675,-8.563154,-8.540637,-8.545367,-8.557307,-8.873287,-8.517547,-8.42863,-8.439225,-9.382109,-8.380283,-8.265535,-8.220237,-8.121843,-8.055696,-8.01125,-8.018776,-8.004292,-8.029605,-8.007916,-8.004558,-8.004329,-8.006521,-8.01543,-9.000031,-8.010417,-7.994315,-7.98932,-8.000699,-8.012905,-8.059616,-8.123807,-8.13466,-8.146594,-8.212439,-8.300263,-8.410016,-8.523418,-8.56011,-9.482725,-8.55343,-8.513676,-8.533969,-8.540082,-8.53008,-8.541187,-8.544515,-8.548169,-8.47115,-8.407256,-8.415591,-8.419777,-8.346678,-8.254675,-8.172142,-8.091554,-8.00683,-8.006509,-7.971793,-7.995692,-8.003453,-7.981801,-8.009287,-7.983468,-8.012361,-7.986234,-7.99263,-7.89649,-7.850908,-7.891217,-7.882314,-7.96318,-7.967076,-7.999285,-7.969033,-8.023215,-8.139624,-8.314969,-8.226614,-8.376128,-8.363891,-8.913572,-8.450042,-8.419215,-8.496735,-8.399175,-8.359995,-8.370281,-8.383913,-8.389469,-8.297194,-8.26969,-8.281087,-8.322767,-8.265535,-8.127696,-8.081867,-7.937324,-7.929292,-7.885908,-7.839492,-7.93788,-7.883426,-7.920358,-7.86562,-7.865083,-7.857026,-7.935675,-7.902583,-7.900688,-7.87369,-7.862879,-7.937898,-7.957352,-8.00599,-7.992914,-8.037125,-8.02737,-8.156596,-8.764892,-8.330021,-8.402805,-8.383357,-8.383345,-8.423914,-8.504255,-8.390865,-8.434205,-8.441441,-8.383623,-8.416412,-8.418629,-8.38695,-8.296935,-8.360563,-8.289681,-8.20411,-8.155195,-8.065142,-7.984844,-7.87648,-7.899799,-7.960099,-7.938435,-7.857292,-7.939016,-7.88203,-7.876739,-7.919562,-7.893693,-7.836165,-7.928174,-7.90259,-7.963983,-7.926205,-7.917018,-7.926507,-7.943714,-8.994153,-8.118231,-8.164647,-8.302479,-8.314987,-8.398366,-8.392229,-8.437268,-8.470323,-8.403361,-8.455042,-8.401428,-8.450035,-8.402231,-8.378072,-8.415036,-8.405028,-8.359156,-8.31692,-8.309962,-8.282482,-8.052936,-8.062932,-7.96147,-7.924019,-7.840912,-7.938997,-7.912869,-7.906183,-7.902299,-8.892716,-7.9276,-7.879524,-7.960982,-7.958735,-7.936497,-7.902583,-8.40725,-7.971799,-7.95734,-8.015127,-7.976244,-8.024592,-8.113545,-8.152694,-9.284833,-8.39389,-8.480337,-8.463099,-8.433069,-8.472274,-8.4823,-8.390284,-8.400854,-8.378616,-8.395291,-8.516189,-8.394495,-8.372781,-8.291928,-9.17758,-8.31579,-8.165783,-8.045701,-8.082664,-7.961779,-7.896484,-7.897317,-7.839252,-7.906491,-7.886469,-7.863126,-7.924001,-7.910356,-7.976238,-8.419734,-7.909541,-7.893409,-7.929835,-7.861453,-7.866478,-7.932348,-7.977078,-8.076823,-8.001526,-8.075983,-8.170753,-8.21857,-8.323582,-8.424494,-9.046144,-8.403089,-8.458691,-8.399767,-8.416425,-8.424469,-8.416715,-8.364163,-8.442818,-8.415301,-8.335837,-8.356383,-8.288304,-8.239647,-8.13855,-8.060999,-8.002885,-7.913696,-7.902293,-7.844783,-7.840888,-7.846444,-7.874813,-7.891761,-7.919518,-7.862601,-7.850352,-7.942059,-7.939269,-7.958723,-7.938429,-7.899842,-7.9215,-7.958167,-7.981214,-8.047651,-8.007651,-8.122708,-8.223836,-8.268831,-8.29386,-8.430316,-8.430575,-8.409467,-8.398644,-8.413078,-8.456444,-8.475595,-8.39752,-8.371392,-8.406966,-8.359483,-8.301109,-8.326088,-8.296064,-8.231059,-8.191886,-8.045719,-7.978998,-7.990432,-7.851433,-8.392803,-7.992895,-7.994031,-7.988481,-8.007892,-7.985968,-7.990129,-8.020937,-8.010102,-7.993445,-7.985135,-7.978998,-7.992611,-8.028173,-8.098765,-8.114651,-8.128536,-8.161838,-8.253588,-8.306387,-8.41001,-8.507008,-8.552565,-8.53258,-8.544261,-8.542854,-8.571198,-8.544805,-8.540088,-8.537316,-8.550349,-8.52619,-8.460587,-8.429217,-8.395563,-8.412813,-8.318019,-8.244123,-8.558153,-8.086856,-8.008744,-7.999859,-8.003181,-7.851457,-7.924538,-7.895934,-7.85397,-7.885914,-7.942047,-7.91453,-7.850334,-7.963705,-7.878678,-7.854513,-7.919827,-7.877554,-7.980436,-8.110724,-8.989455,-8.047645,-8.100457,-8.222725,-8.248291,-8.447547,-8.369738,-8.43281,-8.393063,-8.391686,-8.492024,-8.431415,-8.351679,-8.396958,-8.409207,-9.449071,-8.396958,-8.274672,-8.29862,-8.292749,-8.155219,-8.083201,-8.084047,-7.906467,-7.920389,-7.844209,-7.826478,-7.939003,-7.894236,-7.864534,-8.869953,-7.92205,-7.934811,-7.900101,-7.912863,-7.898132,-7.95095,-7.900953,-7.861743,-7.927038,-7.997056,-7.931786,-8.077126,-8.032106,-8.106859,-8.27553,-8.253014,-8.458666,-8.400298,-8.404206,-8.452844,-8.437527,-8.409201,-8.463383,-8.496185,-8.507286,-8.437558,-8.497037,-8.447529,-8.418925,-9.394043,-8.425611,-8.308894,-8.245525,-8.122411,-8.084343,-8.031544,-8.014294,-7.982622,-7.990154,-7.968731,-8.001001,-7.978164,-7.960093,-7.990413,-8.008182,-7.990407,-7.976769,-8.003181,-7.988752,-7.993729,-8.052949,-8.0985,-8.136846,-8.147681,-8.195492,-8.286371,-8.376683,-8.458376,-8.525357,-8.826297,-8.550633,-8.538674,-8.527012,-8.545651,-8.559517,-8.553689,-8.559523,-8.548429,-8.546768,-8.432798,-8.417258,-8.42003,-8.407238,-8.308573,-8.404744,-8.128264,-8.05072,-8.007083,-8.036816,-8.006237,-7.988475,-7.998767,-8.024573,-7.994568,-7.984863,-8.00849,-8.027617,-8.021838,-7.992383,-8.00181,-8.004274,-8.027951,-8.10489,-8.143514,-8.13408,-8.144903,-8.214686,-8.344425,-8.386685,-8.489801,-8.551182,-8.538989,-8.556764,-8.527018,-8.548719,-8.551726,-8.584818,-8.560912,-8.532556,-8.547274,-8.528382,-8.441145,-8.425587,-8.419444,-8.354735,-8.282482,-8.217168,-8.123529,-8.040428,-7.996501,-8.010682,-8.007916,-7.998989,-8.00181,-8.020134,-8.013189,-8.030432,-8.004854,-8.03681,-8.001224,-8.016813,-8.006527,-8.010676,-8.01209,-8.088517,-8.151867,-8.1563,-8.153256,-8.251094,-8.310283,-8.423926,-8.505594,-8.556492,-8.567864,-8.53897,-8.532284,-8.574001,-8.568982,-8.507033,-8.538427,-8.541211,-8.545897,-8.482275,-8.424488,-8.406114,-8.414221,-8.378906,-8.27971,-8.194664,-8.103766,-8.034606,-8.018492,-7.987635,-8.093795,-7.976226,-7.992908,-8.004298,-7.976244,-7.985968,-7.984567,-7.996797,-7.986789,-7.987629,-7.968181,-7.990401,-8.045417,-8.079348,-8.112101,-8.743505,-8.166882,-8.275808,-8.345005,-8.416431,-8.514769,-8.537297,-8.548972,-8.579823,-8.56842,-8.565944,-8.534525,-8.549793,-8.558128,-8.56479,-8.5634,-8.491999,-8.435335,-8.400014,-8.446177,-8.371121,-8.275228,-8.181607,-8.074045,-8.021814,-7.997921,-8.027123,-8.004311,-7.994834,-8.01819,-8.976119,-8.011238,-7.982918,-8.000989,-8.012355,-8.006521,-8.009318,-7.983721,-8.005971,-8.04988,-8.095178,-8.168265,-8.144359,-8.192436,-8.269702,-8.312209,-8.396384,-8.493141,-8.540088,-8.522566,-8.533414,-8.538409,-8.554806,-8.538989,-8.457858,-8.544521,-8.471996,-8.524233,-8.473651,-8.400576,-9.372082,-8.407232,-8.331392,-8.249143,-8.155763,-8.034057,-8.0057,-8.008744,-8.01209,-7.990092,-8.008725,-8.020406,-7.991247,-7.992932,-8.006823,-8.971934,-7.994297,-7.975133,-7.965662,-7.987073,-7.971249,-8.020418,-8.092122,-8.120195,-8.134333,-8.162424,-8.272758,-8.342505,-8.42279,-8.524505,-9.492702,-8.503958,-8.523949,-8.516423,-8.540909,-8.513972,-8.535927,-8.522029,-8.514787,-8.491178,-8.448906,-8.369725,-8.403916,-8.366435,-8.27524,-8.188571,-8.114922,-8.041533,-7.984023,-7.979004,-7.979029,-7.987067,-7.989006,-7.990432,-7.982906,-7.971799,-7.97596,-8.00486,-8.033785,-7.996816,-8.000131,-8.008453,-7.997063,-8.090745,-8.13992,-8.13687,-8.13379,-8.192164,-8.291922,-8.366959,-8.450887,-8.517016,-8.548398,-8.540897,-8.545897,-8.524505,-8.544255,-8.529512,-8.527049,-8.519807,-8.55343,-8.508681,-8.451468,-8.409473,-8.401972,-8.396409,-8.300794,-8.202172,-8.104346,-8.020412,-8.00791,-7.995371,-7.986499,-7.984283,-7.984869,-7.986221,-7.988746,-7.970107,-8.10852,-7.991228,-7.975701,-7.980967,-7.955951,-7.98653,-8.02403,-8.07239,-8.103494,-8.115194,-8.127974,-8.209395,-8.309135,-8.380844,-8.449758,-8.524221,-8.503143,-8.490641,-8.50005,-8.492283,-8.544799,-8.52453,-8.510354,-8.502841,-8.536772,-8.471162,-8.421425,-8.37004,-8.402805,-8.371701,-8.278864,-8.19159,-8.085436,-8.016245,-7.949851,-7.920667,-7.977355,-7.970385,-7.99734,-7.990685,-7.967335,-7.940645,-7.98482,-7.972324,-7.976812,-7.985388,-7.970404,-7.984005,-8.015146,-8.092381,-8.120485,-9.08478,-8.082695,-8.215236,-8.291101,-8.388611,-8.479503,-8.528388,-8.504785,-8.505607,-8.514201,-8.497531,-8.527845,-8.52035,-8.520344,-8.51341,-8.515621,-8.45561,-8.414745,-8.378375,-8.385296,-8.334701,-8.26246,-8.162974,-8.10518,-8.003743,-7.999588,-8.003187,-7.988166,-8.004292,-7.997075,-8.988041,-7.986252,-8.002082,-7.991518,-8.003496,-7.997631,-7.96539,-7.967064,-7.966767,-8.016776,-8.058499,-8.123535,-8.120732,-8.132129,-8.222144,-9.281789,-8.356402,-8.500334,-8.518677,-8.484498,-8.500896,-8.529518,-8.5112,-8.51007,-8.510095,-8.51036,-8.497006,-8.501729,-8.468958,-8.388352,-9.329847,-8.396705,-8.318871,-8.260237,-8.151873,-8.060962,-7.991228,-8.008194,-7.980399,-7.989036,-7.999038,-7.97901,-7.986252,-7.973731,-7.97262,-7.987092,-7.968169,-7.967613,-7.926242,-7.902059,-7.946504,-7.893427,-8.026518,-7.990148,-7.948752,-8.057388,-8.187447,-8.311641,-8.324452,-8.374183,-9.000846,-8.499229,-8.475601,-8.408646,-8.433637,-8.382802,-8.443658,-8.360835,-8.388056,-8.372226,-8.420049,-8.271357,-8.30861,-8.303029,-8.18578,-8.119355,-8.082941,-7.935404,-7.81839,-7.95011,-7.907868,-7.868689,-7.927069,-7.949295,-7.944535,-7.86646,-7.916759,-7.906226,-7.956772,-7.902874,-7.919259,-7.918419,-7.969002,-7.902306,-7.980393,-8.009034,-8.048213,-8.033748,-8.11796,-8.274122,-8.380869,-8.392816,-8.425284,-8.355278,-8.374189,-8.400848,-8.436959,-8.45198,-8.422524,-8.342233,-8.457006,-8.470057,-8.379708,-8.310839,-8.298318,-8.288563,-8.23327,-8.124912,-8.030951,-7.880641,-7.883969,-7.902565,-7.888408,-7.945103,-7.878437,-7.886198,-7.925069,-7.879265,-7.955944,-7.940658,-7.844777,-7.838128,-7.918969,-7.912313,-7.940954,-7.887321,-7.991821,-7.992093,-8.105748,-8.196307,-8.245778,-8.226343,-8.288872,-8.355828,-8.437533,-8.473922,-8.405843,-8.348895,-8.397255,-8.425852,-8.31913,-8.386401,-8.490623,-8.409738,-8.300257,-8.32581,-8.29165,-8.252995,-8.171031,-8.05043,-8.017078,-7.983455,-7.865645,-7.877567,-7.859508,-7.881203,-7.863694,-7.929292,-7.916771,-7.96039,-7.920932,-7.914271,-7.912307,-7.901478,-7.830077,-7.886457,-7.910375,-7.987598,-7.993438,-9.09088,-8.106853,-8.190509,-8.263009,-8.369447,-8.445065,-8.503662,-8.523671,-8.508397,-8.515905,-8.527567,-8.525091,-8.517016,-8.520906,-8.518677,-9.509939,-8.500914,-8.439478,-8.379745,-8.371114,-8.352766,-8.271931,-8.195232,-8.076873,-7.970928,-7.98098,-7.965668,-7.962884,-7.972639,-7.980961,-8.913288,-7.961501,-7.992086,-7.97901,-7.982066,-7.999853,-7.997624,-7.962044,-7.97709,-7.987073,-8.069334,-8.106569,-8.121306,-8.141544,-8.233023,-8.332781,-8.41085,-8.428637,-8.522282,-8.540372,-8.507835,-8.518115,-8.524801,-8.517306,-8.539526,-8.518979,-8.511731,-8.522566,-8.463661,-8.444497,-9.360698,-8.384178,-8.335263,-8.263312,-8.167975,-8.067396,-8.002613,-7.976491,-7.960945,-7.968453,-7.970397,-7.980128,-7.999279,-7.967045,-7.996816,-7.965384,-7.962625,-7.969583,-7.980405,-7.973176,-7.985974,-8.038496,-8.061259,-8.133265,-8.116583,-8.126579,-8.219922,-8.303597,-8.373911,-8.358902,-8.754872,-8.460858,-8.404472,-8.491184,-8.446961,-8.362514,-8.466433,-8.429748,-8.414202,-8.446448,-8.390291,-8.299701,-8.299151,-8.351673,-8.223571,-8.335281,-8.05514,-8.012633,-7.96707,-7.982338,-7.889007,-7.902028,-7.8815,-7.925674,-8.243018,-7.986499,-7.995976,-7.957883,-7.997649,-8.010145,-7.980949,-7.965137,-8.012355,-8.05014,-8.088492,-8.130758,-8.122979,-8.141847,-8.244698,-8.299145,-8.408917,-8.514787,-8.488122,-8.543138,-8.531463,-8.478658,-8.509533,-8.543416,-8.508113,-8.534507,-8.535914,-8.538711,-8.472582,-8.390019,-8.347209,-8.385839,-8.32778,-8.22078,-8.139649,-8.059592,-7.978448,-7.947881,-8.552022,-7.972886,-8.000415,-7.996803,-8.005126,-7.982369,-8.008447,-7.984844,-8.008472,-8.004298,-7.971231,-7.973151,-7.997353,-8.028204,-8.120176,-8.118528,-8.125473,-8.190231,-8.27524,-8.352506,-8.418882,-8.514256,-8.537841,-8.54867,-8.55509,-8.538433,-8.528691,-8.533679,-8.528981,-8.52787,-8.535081,-8.535365,-8.451165,-8.408349,-8.391951,-8.335269,-8.311931,-8.23022,-8.146847,-8.056548,-7.989567,-7.992074,-8.091826,-7.9829,-7.980671,-7.980955,-7.989296,-7.989006,-7.95955,-7.978473,-7.991234,-7.94706,-7.990969,-7.980683,-7.930107,-7.980949,-8.09879,-8.74266,-8.111854,-8.14631,-8.257465,-8.354167,-8.390007,-8.488406,-8.503668,-8.489801,-8.521764,-8.524801,-8.503946,-8.511731,-8.512021,-8.517288,-8.557307,-8.478942,-8.407831,-8.37222,-8.921635,-8.374467,-8.28163,-8.206321,-8.107131,-8.050158,-7.976226,-7.971521,-7.975108,-8.013788,-7.986252,-8.997259,-8.003446,-7.989833,-8.00236,-8.003477,-8.003187,-7.999026,-8.020147,-8.003465,-8.009034,-8.066562,-8.11825,-8.131549,-8.107946,-8.216063,-8.30719,-8.357779,-8.451974,-8.520609,-8.555646,-8.542317,-8.560647,-8.532278,-8.528703,-8.538977,-8.539804,-8.546206,-8.851592,-8.49479,-8.443664,-9.387104,-8.399996,-8.365027,-8.296095,-8.203283,-8.120201,-7.985425,-8.004564,-8.021517,-7.999588,-7.972064,-7.972361,-8.004595,-8.001829,-7.991802,-8.961919,-7.955148,-7.990426,-7.987635,-7.969299,-7.960118,-8.011275,-8.076286,-8.107118,-8.098821,-8.115737,-8.192189,-8.271641,-8.358057,-8.460056,-9.461579,-8.523406,-8.527302,-8.517016,-8.513139,-8.529524,-8.527592,-8.504495,-8.50702,-8.488116,-8.480899,-8.432254,-8.386382,-8.393618,-8.363064,-8.27303,-8.154083,-8.071007,-8.002366,-7.987079,-7.966218,-7.976226,-7.982906,-7.972083,-7.981782,-7.991796,-7.966786,-7.970095,-7.975127,-7.989012,-7.983474,-7.966255,-7.995698,-7.999847,-8.055733,-8.255527,-8.118269,-8.122411,-8.21105,-8.288563,-8.395538,-8.457821,-8.521177,-9.111698,-8.497827,-8.489771,-8.505069,-8.518417,-8.531753,-8.508687,-8.508656,-8.51814,-8.471181,-8.391105,-8.360292,-8.386413,-8.330293,-8.256656,-8.17826,-8.080169,-7.996519,-7.96068,-7.96205,-7.979856,-7.982078,-7.949585,-7.997612,-7.978732,-7.974855,-7.96039,-7.998464,-7.969848,-7.940386,-7.960112,-7.972657,-8.003496,-8.056814,-8.088239,-8.1213,-8.135204,-8.221348,-8.879665,-8.353346,-8.484788,-8.519504,-8.537581,-8.50536,-8.510885,-8.523406,-8.528969,-8.516713,-8.502001,-8.513398,-8.500044,-8.428383,-8.385006,-8.362205,-8.361119,-8.324174,-8.239129,-8.146872,-8.055702,-8.011534,-7.987641,-7.991253,-7.977355,-7.955376,-7.990697,-7.960093,-7.958729,-7.986814,-7.984844,-7.962631,-7.977343,-7.981529,-7.964841,-7.964563,-8.016523,-8.07431,-9.101419,-8.108526,-8.151317,-8.244407,-8.337213,-8.411683,-8.480596,-8.515608,-8.502285,-8.515614,-8.52064,-8.512849,-8.534531,-8.534513,-8.529518,-8.531191,-8.506718,-8.454493,-8.392803,-8.367478,-8.395582,-8.315549,-8.203549,-8.17187,-8.065976,-7.978751,-7.98235,-7.983202,-7.980418,-7.989296,-8.969989,-7.989561,-7.98929,-7.975972,-7.943992,-7.997624,-7.993469,-7.977899,-8.547577,-7.948159,-8.033754,-8.092134,-8.117954,-8.107668,-8.218835,-9.252037,-8.351383,-8.407818,-8.510064,-8.526999,-8.540088,-8.479472,-8.515324,-8.542854,-8.513972,-8.531759,-8.51951,-8.522844,-8.488937,-8.437552,-9.356216,-8.373072,-8.353327,-8.28192,-8.224663,-8.107933,-8.037366,-7.989271,-7.993457,-7.984283,-7.985956,-7.983739,-7.968737,-7.985956,-7.971787,-7.982332,-8.502575,-7.965965,-7.978164,-7.987098,-7.950129,-8.00068,-8.086312,-8.109088,-8.092925,-8.117441,-8.1644,-8.279129,-8.3642,-8.452005,-9.090571,-8.52703,-8.533142,-8.510064,-8.503964,-8.520041,-8.468125,-8.522844,-8.51091,-8.525869,-8.488956,-8.430588,-8.384456,-8.368311,-8.3586,-8.281642,-8.219953,-8.127431,-8.032099,-7.978738,-7.978979,-7.988999,-7.97596,-7.964816,-7.993463,-8.007367,-7.985974,-8.002076,-7.976503,-7.964545,-7.997359,-7.963458,-7.967088,-7.979306,-8.066544,-8.106575,-8.061537,-8.084047,-8.076274,-8.268597,-8.336374,-8.272752,-8.404731,-8.386673,-8.430297,-8.431693,-8.49258,-8.391105,-8.375572,-8.443108,-8.446436,-8.363909,-8.443621,-8.330268,-8.315809,-8.360563,-8.278321,-8.234128,-8.065154,-8.037082,-7.95095,-7.863404,-8.498976,-8.010423,-7.975411,-8.006268,-7.990426,-7.98235,-7.96957,-7.965409,-8.00039,-7.997063,-7.979856,-7.958179,-7.95955,-8.033476,-8.052381,-8.129332,-8.120479,-8.119608,-8.228257,-8.340294,-8.388636,-8.463649,-8.510916,-8.497821,-8.509799,-8.512589,-8.531735,-8.505884,-8.522023,-8.50978,-8.526481,-8.538143,-8.44004,-8.411702,-8.381678,-8.36336,-8.328323,-8.243,-8.743512,-8.082688,-8.024864,-8.003761,-8.017949,-8.026543,-7.989858,-7.979547,-8.033198,-8.022635,-7.994303,-8.003761,-7.994574,-8.02516,-7.98903,-8.025148,-8.009867,-8.017338,-8.102395,-9.105598,-8.135185,-8.155176,-8.26217,-8.338035,-8.423383,-8.516195,-8.562024,-8.555646,-8.541749,-8.554516,-8.525369,-8.544521,-8.542317,-8.550886,-9.52772,-8.506428,-8.463389,-8.393359,-8.389173,-8.377239,-8.330256,-8.251896,-8.175482,-8.069328,-7.980961,-7.998192,-7.985968,-7.97596,-7.971774,-8.920252,-7.990148,-7.984023,-7.994568,-7.987351,-7.973725,-7.989012,-7.980368,-7.996538,-7.969842,-8.025148,-8.104649,-8.11186,-8.112687,-8.134068,-8.271066,-8.349463,-8.409763,-8.504792,-8.542292,-8.566197,-8.544545,-8.521455,-8.518948,-8.527586,-8.525906,-8.525906,-9.079187,-8.533685,-8.451992,-9.378207,-8.418369,-8.408905,-8.323872,-8.266065,-8.167147,-8.086294,-8.014028,-8.012615,-8.007638,-8.004873,-8.004323,-7.997896,-7.996513,-7.961791,-7.9854,-7.998458,-7.979257,-8.020153,-7.996254,-8.015689,-8.005965,-8.072396,-8.10739,-8.155491,-8.127128,-8.169672,-8.265251,-8.383913,-8.437842,-8.813801,-8.544508,-8.555337,-8.547293,-8.539236,-9.229539,-8.528419,-8.539526,-8.509231,-8.528425,-8.507551,-8.468687,-8.406966,-8.397526,-8.388327,-8.429791,-8.237196,-8.13187,-8.074619,-7.976497,-7.9915,-7.990401,-7.962359,-7.967607,-7.983461,-7.999588,-7.975127,-7.95984,-7.981794,-7.98456,-7.983461,-7.98569,-8.004873,-7.993759,-8.035137,-8.102099,-8.112138,-8.114348,-8.186299,-8.284958,-8.347234,-8.437533,-8.495889,-8.551466,-8.532587,-8.538958,-8.534803,-8.502569,-8.514509,-8.542841,-8.528123,-8.513139,-8.478948,-8.450288,-8.400014,-8.369151,-8.366682,-8.302504,-8.214952,-8.103501,-8.016541,-8.005175,-7.995704,-7.973725,-7.999872,-7.978461,-7.977362,-7.957327,-7.989876,-7.973731,-7.974553,-7.961773,-7.975954,-8.000693,-7.98206,-8.000137,-8.054319,-8.112403,-8.121856,-8.123232,-8.214396,-8.740727,-8.378603,-8.456709,-8.516164,-8.54315,-8.535365,-8.529234,-8.557603,-8.547589,-8.531197,-8.552287,-8.532877,-8.533673,-8.485924,-8.427525,-8.4103,-8.413091,-8.367774,-8.289137,-8.224947,-8.118787,-8.026543,-8.005126,-8.112434,-7.99179,-7.99121,-7.981776,-7.965415,-7.983153,-7.994278,-7.977349,-7.99513,-7.970675,-7.999007,-7.988191,-7.984851,-7.986258,-8.048769,-8.719335,-8.124084,-8.131011,-8.198529,-8.328885,-8.393347,-8.461735,-8.521455,-8.518967,-8.529524,-8.534821,-8.54202,-8.518979,-8.550929,-8.532852,-8.691268,-8.535933,-8.470323,-8.411955,-8.385598,-8.368064,-8.342245,-8.246365,-8.19272,-8.093505,-8.028469,-7.979856,-7.991809,-8.012077,-8.001557,-7.999581,-8.015152,-8.015973,-8.005694,-8.000396,-8.014306,-8.017906,-8.008756,-7.980115,-7.983715,-8.015171,-8.062389,-8.119621,-8.125727,-8.147977,-9.205653,-8.324168,-8.385574,-8.460611,-8.524807,-8.539514,-8.562042,-8.515046,-8.521202,-8.539217,-8.558146,-8.508416,-8.514238,-8.524542,-8.469761,-8.427809,-8.397532,-8.37417,-8.346931,-8.230232,-8.163264,-8.087942,-7.997081,-7.985116,-7.998192,-7.993192,-7.990679,-7.981492,-7.995414,-7.991512,-8.981917,-7.965397,-7.982628,-7.991265,-7.987913,-7.972632,-7.981523,-8.03736,-8.074329,-8.119645,-8.134086,-8.162998,-8.234103,-8.323619,-8.406404,-9.469352,-8.50089,-8.535655,-8.554251,-8.527024,-8.527573,-8.519807,-8.520054,-8.518948,-8.523406,-8.51175,-8.460346,-8.410596,-8.399737,-8.391945,-8.328323,-8.235215,-8.145489,-8.075737,-7.98043,-7.981788,-7.985678,-7.974275,-7.99818,-7.99237,-7.964563,-7.994037,-7.987604,-7.982881,-8.000415,-8.494518,-7.983214,-8.024592,-7.983208,-8.050152,-8.108224,-8.139062,-8.126856,-8.182144,-8.293867,-8.356408,-8.428939,-8.503396,-8.539791,-8.5401,-8.533432,-8.552034,-8.547027,-8.5487,-8.538958,-8.544805,-8.557023,-8.537575,-8.437249,-8.406139,-8.395859,-8.39026,-8.332762,-8.237462,-8.14323,-8.052905,-7.977343,-7.98569,-7.96289,-7.97651,-7.967885,-7.955099,-7.972639,-7.983171,-7.932873,-7.977096,-7.965656,-7.985678,-7.990419,-7.976522,-7.980399,-8.043212,-8.104612,-8.126301,-8.125733,-8.185786,-8.243833,-8.332194,-8.448399,-8.501458,-8.526487,-8.525061,-8.538143,-8.512836,-8.510046,-8.498945,-8.555912,-8.522017,-8.500606,-8.502557,-8.418079,-8.396113,-8.400589,-8.367496,-8.287724,-8.197436,-8.128838,-8.030976,-7.97538,-7.99513,-7.986499,-7.954833,-7.97233,-7.98319,-8.000156,-7.989302,-7.988462,-7.972083,-7.988475,-7.963964,-7.983739,-7.961223,-7.979578,-8.059048,-8.116015,-8.144341,-8.085744,-8.184928,-8.263571,-8.364724,-8.435033,-8.497568,-8.518442,-8.541508,-8.510342,-8.500865,-8.498105,-8.502279,-8.52895,-8.491153,-8.524517,-8.494784,-8.40057,-8.379165,-8.369725,-8.376646,-8.283846,-8.192176,-8.122152,-8.034569,-7.986246,-7.987894,-7.986252,-7.99597,-8.973891,-8.002094,-8.018486,-8.006805,-8.012355,-7.992321,-8.009855,-8.012374,-8.008478,-7.993167,-8.021264,-8.081552,-8.144927,-8.125443,-8.142692,-9.184791,-8.301109,-8.377807,-8.448912,-8.522838,-8.515898,-8.525369,-8.520356,-8.514781,-8.533704,-8.528956,-8.523394,-8.507564,-8.508681,-8.435885,-9.368199,-8.413091,-8.376109,-8.35334,-8.266924,-8.193541,-8.111008,-7.994303,-7.966212,-8.000421,-7.957056,-7.982622,-7.981239,-7.986795,-7.999563,-8.004879,-7.982344,-7.997347,-7.985672,-7.980992,-7.990666,-7.980399,-8.009034,-8.077941,-8.122146,-8.131851,-8.142421,-8.202999,-8.310264,-8.383055,-9.503265,-8.547305,-8.548416,-8.536204,-8.506175,-8.540637,-8.540372,-8.54315,-8.543138,-8.525925,-8.532031,-8.465581,-8.428112,-8.421135,-8.36139,-8.378048,-8.273061,-8.201332,-8.082954,-8.017072,-7.994278,-8.006539,-8.007391,-7.998458,-8.013195,-7.991512,-8.012615,-7.991247,-8.006262,-8.009312,-8.170759,-8.031568,-7.991259,-7.988468,-8.054319,-8.119614,-8.134358,-8.145181,-8.177698,-8.244148,-8.35221,-8.42726,-8.515627,-8.548126,-8.568438,-8.568142,-8.567574,-8.534809,-8.538983,-8.567852,-8.545922,-8.536754,-8.497297,-8.45645,-8.442528,-8.396403,-8.393087,-8.350845,-8.26467,-8.151299,-8.079354,-8.029599,-8.025117,-8.007626,-7.993463,-7.998742,-7.976806,-7.997921,-8.013213,-7.997093,-7.992901,-8.001224,-8.023474,-8.022629,-7.981535,-8.014288,-8.045429,-8.114348,-8.141569,-8.146866,-8.166894,-8.26246,-8.357229,-8.432532,-8.490048,-8.539532,-8.524807,-8.544539,-8.521177,-8.515355,-8.517856,-8.513386,-8.524505,-8.523684,-8.50423,-8.456147,-8.41085,-8.37501,-8.397242,-8.31692,-8.231887,-8.160492,-8.056567,-7.962902,-7.969027,-8.003477,-7.992086,-7.97375,-7.964001,-7.964545,-7.96899,-7.98456,-7.98737,-8.004008,-7.990413,-7.990105,-7.982924,-7.987073,-8.029321,-8.336374,-8.133253,-8.136599,-8.17576,-8.278018,-8.347203,-8.458098,-8.534828,-8.545928,-8.543416,-8.558998,-8.537878,-8.51646,-8.530636,-8.545101,-8.722934,-8.491147,-8.510323,-8.458654,-8.389222,-8.387506,-8.395866,-8.306937,-8.204654,-8.143254,-8.031266,-7.974596,-7.966193,-7.979306,-7.978195,-8.948856,-7.972077,-8.000427,-7.986783,-7.930668,-7.964014,-7.989827,-7.987339,-7.998495,-7.984573,-8.003743,-8.072952,-8.140186,-8.133524,-8.140451,-8.191046,-8.25607,-8.363632,-8.434205,-8.510885,-8.524239,-8.545058,-8.528141,-8.507027,-8.538674,-8.506489,-8.539261,-8.533976,-8.530068,-8.505625,-9.410713,-8.399761,-8.395291,-8.358625,-8.30777,-8.206037,-8.123547,-8.001248,-8.009861,-8.00265,-8.024049,-8.014893,-7.98958,-8.008182,-8.01985,-8.042089,-8.007904,-7.97709,-7.967619,-7.977627,-7.978751,-7.986505,-8.02792,-8.071841,-8.110193,-8.123226,-8.135741,-8.203549,-8.29775,-8.388333,-9.444916,-8.5148,-8.536451,-8.507539,-8.534809,-8.510891,-8.535908,-8.52314,-8.535643,-8.51033,-8.533698,-8.473416,-8.418641,-8.400836,-8.383061,-9.350128,-8.28581,-8.175476,-8.097672,-8.030976,-7.971811,-7.983177,-7.987357,-7.986536,-7.977059,-7.98766,-7.975404,-7.978195,-7.985153,-7.988444,-8.778771,-7.989592,-7.975417,-7.992914,-8.008756,-8.082657,-8.124331,-8.119627,-8.118775,-8.216045,-8.326378,-8.396952,-8.472798,-8.518133,-8.525598,-8.519523,-8.53008,-8.508397,-8.522307,-8.5234,-8.521183,-8.539254,-8.507014,-8.466155,-8.412819,-8.379159,-8.396964,-8.352759,-8.26246,-8.215489,-8.09879,-8.004582,-7.974843,-7.983437,-7.991241,-7.977602,-7.990395,-7.987907,-8.010151,-8.000977,-7.972898,-7.977349,-8.005434,-7.972071,-8.00344,-7.963168,-8.028784,-8.096005,-8.137136,-8.120744,-8.147724,-8.215779,-8.304128,-8.41585,-8.507848,-8.498667,-8.514781,-8.496735,-8.518695,-8.503946,-8.513145,-8.532833,-8.548725,-8.520387,-8.510323,-8.451702,-8.412251,-8.367515,-8.389198,-8.328045,-8.247439,-8.155188,-8.079336,-7.98151,-7.98845,-7.987894,-8.003477,-7.974559,-7.958463,-7.98958,-7.936466,-7.981794,-7.986264,-7.968477,-8.014874,-8.005669,-8.0021,-7.966236,-8.027105,-8.106841,-8.114348,-8.137408,-8.149928,-8.244105,-8.328866,-8.417264,-8.492283,-8.517812,-8.515652,-8.535939,-8.483399,-8.512281,-8.543687,-8.520084,-8.557591,-8.522572,-8.51759,-8.437811,-8.391396,-8.411146,-8.405268,-8.313018,-8.259145,-8.152429,-8.044064,-7.990401,-7.998199,-7.984289,-8.026802,-9.023628,-8.017381,-8.018492,-7.985943,-8.010429,-8.009836,-7.987086,-8.019881,-8.004033,-8.006262,-8.014572,-8.065167,-8.139359,-8.154904,-8.142118,-8.204932,-8.26246,-8.374183,-8.45645,-8.527296,-8.551213,-8.55204,-8.554263,-8.55259,-8.567883,-8.555918,-8.552022,-8.540903,-8.680964,-8.500902,-9.41906,-8.428933,-8.414177,-8.420845,-8.333626,-8.248025,-8.148811,-8.064901,-7.982875,-8.008219,-8.015134,-8.022635,-7.997921,-8.02127,-8.01459,-9.001093,-7.999581,-7.990987,-8.008484,-7.982344,-8.010966,-7.989024,-7.966218,-8.066568,-8.082133,-8.131036,-8.141038,-8.189917,-8.255829,-8.357229,-9.404866,-8.506465,-8.544261,-8.528123,-8.527308,-8.547848,-8.550658,-8.527876,-8.546749,-8.515917,-8.566753,-8.521165,-8.431705,-8.38671,-8.406985,-8.385537,-8.304973,-8.177723,-8.11073,-8.016523,-7.985703,-8.009287,-8.004292,-8.001792,-7.994846,-7.988462,-7.980393,-7.987931,-7.848691,-7.853427,-8.349463,-7.88842,-7.947338,-7.874529,-7.871189,-7.857267,-8.077947,-8.0082,-7.962909,-8.064321,-8.203536,-8.239691,-8.319741,-8.398625,-9.003044,-8.571217,-8.561209,-8.538711,-8.554522,-8.538415,-8.567043,-8.591486,-8.528691,-8.506162,-8.415881,-8.407503,-8.35334,-8.379758,-8.294416,-8.18215,-8.129641,-8.03071,-8.000717,-7.965952,-7.996791,-7.990673,-7.989283,-7.985962,-8.016529,-7.998192,-7.980399,-7.985135,-8.006496,-8.019857,-7.99542,-7.97041,-8.000433,-8.074601,-8.114626,-8.136562,-8.109928,-8.20579,-8.852709,-8.390315,-8.473941,-8.532025,-8.540915,-8.522572,-8.547293,-8.537026,-8.529549,-8.56287,-8.537013,-8.507564,-8.541465,-8.477552,-8.423907,-8.402509,-8.405843,-8.371664,-8.254403,-8.172982,-8.081583,-8.004305,-7.990673,-7.961513,-8.005694,-8.004311,-7.959297,-7.984585,-8.019035,-7.957358,-7.985375,-7.984283,-7.997353,-8.008744,-8.004027,-8.012374,-8.013763,-8.084047,-8.133796,-8.142421,-8.134333,-8.214359,-8.343622,-8.418635,-8.493672,-8.516195,-8.530623,-8.55117,-8.556473,-8.537859,-8.546743,-8.567315,-8.536735,-8.535075,-8.406972,-8.349185,-8.308616,-8.309443,-8.247445,-8.189663,-8.14936,-8.021536,-7.975404,-7.917024,-7.916481,-7.85313,-7.886747,-8.891889,-7.951499,-7.853705,-7.84813,-7.84032,-7.927322,-7.832281,-7.885124,-7.903726,-8.554257,-7.979288,-8.028204,-8.086831,-8.134901,-8.111298,-9.14479,-8.242148,-8.312469,-8.405855,-8.477275,-8.500334,-8.537007,-8.555084,-8.527839,-8.525635,-8.519257,-8.514509,-8.523696,-8.524814,-8.503396,-9.423209,-8.377245,-8.378079,-8.380857,-8.316648,-8.223262,-8.15462,-8.07431,-7.98151,-7.981788,-7.986789,-7.991247,-7.963439,-7.980961,-7.950968,-8.022116,-8.007095,-8.580379,-8.000983,-7.997896,-8.007077,-8.028222,-8.003218,-8.05519,-8.101864,-8.154633,-8.141019,-8.173266,-8.267479,-8.361384,-9.42879,-8.512855,-8.519239,-8.542298,-8.530648,-8.515361,-8.507872,-8.495926,-8.498939,-8.545613,-8.501421,-8.517849,-8.442553,-8.400595,-8.406676,-8.400033,-8.291378,-8.209945,-8.132962,-8.051004,-7.994297,-7.974003,-7.987894,-7.991506,-7.984295,-7.978738,-8.001218,-7.978732,-7.978195,-8.003199,-8.116015,-7.978726,-7.989833,-7.987604,-7.969299,-8.047645,-8.102692,-8.132123,-8.119083,-8.173821,-8.263855,-8.369447,-8.414733,-8.513139,-8.542317,-8.552559,-8.527882,-8.522603,-8.534223,-8.528401,-8.517596,-8.55146,-8.546459,-8.512003,-8.426723,-8.383617,-8.384481,-8.36307,-8.267467,-8.204962,-8.123226,-8.047664,-8.009589,-8.534272,-8.019597,-8.013467,-8.016535,-8.007651,-7.982912,-7.99902,-7.9626,-7.976238,-7.986511,-7.99789,-7.999322,-8.02763,-7.999859,-8.069902,-8.117139,-8.135463,-8.131592,-8.185484,-8.312469,-8.380844,-8.483115,-8.541465,-8.526715,-8.541755,-8.576483,-8.521196,-8.535359,-8.53897,-8.528413,-8.553417,-8.540915,-8.453363,-8.416171,-8.423673,-8.383647,-8.367237,-8.269696,-8.736004,-8.083213,-8.019307,-7.972879,-7.960933,-7.990419,-7.99455,-7.977355,-7.995414,-7.991809,-7.982628,-7.99876,-7.965088,-7.989006,-7.971515,-7.979553,-8.009843,-8.012071,-8.366114,-8.116595,-8.116015,-8.100735,-8.187441,-8.282457,-8.383073,-8.466446,-8.517288,-8.491437,-8.536742,-8.492024,-8.524239,-8.494512,-8.530074,-8.768763,-8.54065,-8.52035,-8.476435,-8.40475,-8.401138,-8.344449,-8.355822,-8.248859,-8.171568,-8.086547,-8.007916,-7.967897,-7.997365,-7.968434,-8.931365,-7.96402,-7.994297,-7.983184,-7.999038,-7.993192,-7.989024,-7.994297,-8.010139,-7.957624,-7.990673,-8.020141,-8.054325,-8.125486,-8.135753,-8.154923,-8.203567,-8.289712,-8.368058,-8.478688,-8.527851,-8.505353,-8.509768,-8.497852,-8.505619,-8.510644,-8.513386,-8.514528,-8.845511,-8.530907,-9.418232,-8.390291,-8.397242,-8.406133,-8.332774,-8.261077,-8.189651,-8.083219,-8.021536,-7.989567,-7.99095,-7.983486,-8.014868,-7.99066,-7.994013,-7.969854,-8.004595,-7.987363,-7.992901,-7.989265,-7.994037,-7.983733,-7.983159,-8.01848,-8.118509,-8.13182,-8.127369,-8.145471,-8.237987,-8.327502,-9.399044,-8.498371,-8.525906,-8.532852,-8.553973,-8.528685,-8.842152,-8.525079,-8.554238,-8.528691,-8.53092,-8.542588,-8.451708,-8.383055,-8.41477,-9.368736,-8.323291,-8.213853,-8.139359,-8.059598,-8.014856,-7.952635,-7.948425,-7.97204,-7.999588,-7.966236,-7.97901,-7.976497,-7.982653,-8.005971,-8.769349,-7.970688,-7.996241,-7.967632,-7.961773,-8.034853,-8.080447,-8.090177,-8.1421,-8.147391,-8.251903,-8.340547,-8.429205,-8.498414,-8.526993,-8.520622,-8.565654,-8.522307,-8.510632,-8.511737,-8.539236,-8.535093,-8.511441,-8.528388,-8.44948,-8.375837,-8.352778,-8.389723,-8.305825,-8.220521,-8.139661,-8.067383,-7.982338,-7.971521,-7.985696,-7.99179,-7.979572,-7.962322,-7.973731,-7.96594,-7.996507,-7.975386,-8.000131,-7.962075,-7.969317,-7.974837,-7.976497,-8.035674,-8.094061,-8.113243,-8.123807,-8.176328,-8.827983,-8.353327,-8.460883,-8.543403,-8.54399,-8.511447,-8.539236,-8.520091,-8.536174,-8.523962,-8.503952,-8.522572,-8.527579,-8.472274,-8.416962,-8.403892,-8.3753,-8.384746,-8.294151,-8.180767,-8.10965,-8.046565,-7.964563,-7.9854,-7.992617,-7.980689,-8.014028,-7.950672,-7.984567,-7.966786,-7.987092,-7.975386,-7.990123,-7.968434,-7.994568,-8.002644,-7.995136,-8.046244,-8.637611,-8.153509,-8.154349,-8.190787,-8.288613,-8.376665,-8.470866,-8.505347,-8.535636,-8.530345,-8.533389,-8.543959,-8.542885,-8.532315,-8.537859,-8.52314,-8.514837,-8.488659,-8.420882,-8.378085,-8.395038,-8.345277,-8.26275,-8.174087,-8.099339,-7.999859,-7.967354,-7.964835,-7.980134,-8.979188,-7.950925,-7.984301,-7.972904,-7.981819,-7.973472,-7.970972,-7.962637,-7.973484,-7.993457,-7.978732,-8.00762,-8.044861,</t>
+  </si>
+  <si>
+    <t>-8.985541,-9.023591,-9.326809,-8.974415,-8.963574,-8.959123,-8.927753,-8.94775,-8.899958,-9.204523,-8.803806,-8.839374,-8.743197,-8.648718,-8.518405,-8.407812,-8.318599,-8.280815,-8.300818,-8.326644,-8.324693,-8.308042,-8.314703,-8.324427,-8.339714,-8.313012,-8.332781,-8.309425,-8.322192,-8.323057,-8.30527,-8.358606,-8.414474,-8.461735,-8.477571,-8.503946,-8.551213,-8.737937,-8.802411,-9.938439,-8.944114,-8.926889,-8.95193,-8.94107,-8.981096,-8.954986,-8.80935,-8.811295,-8.856611,-8.846344,-8.76349,-8.755174,-8.732392,-8.772949,-9.639418,-8.522856,-8.421981,-8.322217,-8.193849,-8.251625,-8.21189,-8.161331,-8.284692,-8.157967,-8.232158,-8.202456,-8.268307,-8.243265,-8.259132,-9.182303,-8.228287,-8.233307,-8.182712,-8.174914,-8.273017,-8.301362,-8.37472,-8.416153,-9.143926,-8.542323,-8.755452,-8.805183,-8.741264,-8.767973,-8.907188,-8.815487,-8.848807,-8.793249,-8.841312,-8.806831,-8.877985,-8.758811,-8.75823,-8.672629,-8.756273,-8.75794,-8.578422,-8.520066,-8.358328,-9.227558,-8.237733,-8.230788,-8.197714,-8.202437,-8.264115,-8.204086,-8.236054,-8.193288,-8.1994,-8.261923,-8.219953,-8.1644,-8.19772,-8.2055,-8.22662,-8.276067,-8.963599,-8.336374,-8.342505,-8.464513,-8.555621,-8.660689,-8.72073,-8.770448,-8.821025,-8.766015,-8.826322,-8.835762,-8.882721,-8.883283,-8.816333,-8.824649,-8.86494,-8.836034,-8.71823,-8.682902,-8.696825,-8.696806,-8.620392,-8.491734,-8.353599,-8.27248,-8.234677,-8.2105,-8.171592,-8.169642,-8.17689,-8.196053,-8.222478,-8.178544,-8.292471,-8.180211,-8.183545,-8.237456,-8.268307,-8.208272,-8.204376,-8.261664,-8.303603,-8.309993,-8.414764,-8.353056,-8.523431,-8.679581,-8.784358,-8.882721,-8.87496,-8.827983,-8.789359,-8.868817,-8.84882,-8.874398,-8.807677,-8.770146,-8.807399,-8.805473,-8.750439,-8.744629,-8.726817,-8.781055,-8.588732,-8.516985,-8.288298,-8.24721,-8.219372,-8.175754,-8.162418,-8.210778,-8.211624,-8.281648,-8.255224,-8.209963,-8.82602,-8.220218,-8.196609,-8.217168,-8.198819,-8.258311,-8.206358,-8.191874,-8.219397,-8.302473,-8.342505,-8.50699,-8.552886,-8.60955,-8.78742,-8.746278,-8.878288,-8.815777,-8.87438,-8.844375,-8.831311,-8.717137,-8.81795,-8.907744,-8.905811,-8.734899,-9.456856,-8.749605,-8.749618,-8.655947,-8.509243,-8.442546,-8.333898,-8.239123,-8.289144,-8.259416,-8.271357,-8.184107,-8.880764,-8.197733,-8.249958,-9.190613,-8.187978,-8.227466,-8.278852,-8.190769,-8.16632,-8.27916,-8.23498,-8.263577,-8.371386,-8.383913,-8.278296,-8.455042,-8.580934,-8.748228,-9.723624,-8.809918,-8.811844,-8.843263,-8.866897,-8.900236,-8.756014,-8.763768,-8.769343,-8.935242,-8.949436,-8.788242,-8.710179,-8.664023,-8.736263,-8.570655,-8.528697,-8.481732,-8.33388,-8.243296,-8.275808,-8.224404,-8.219113,-8.266374,-8.226052,-8.182422,-8.212729,-8.19104,-8.236067,-8.243833,-9.238442,-8.186595,-8.241901,-8.185206,-8.224132,-8.351401,-8.301084,-8.364471,-8.352506,-8.438644,-8.547867,-8.693182,-8.834916,-8.817963,-8.802966,-8.770992,-8.851055,-8.740456,-8.903829,-8.854376,-8.779339,-8.811295,-8.788785,-8.776554,-8.762373,-8.720137,-8.661535,-8.64568,-9.134498,-8.376665,-9.124781,-8.223842,-8.154917,-8.172438,-8.179643,-8.274135,-8.242728,-8.248285,-8.206895,-8.245531,-8.254952,-8.193541,-8.21105,-8.229683,-8.199406,-9.084749,-8.254662,-8.328626,-8.370546,-8.402509,-8.481701,-8.483387,-8.642365,-8.656262,-8.841856,-8.836879,-8.806035,-8.852135,-8.827983,-8.810184,-8.813814,-8.78881,-8.798799,-8.863279,-8.843535,-8.73096,-9.298175,-8.660152,-8.762132,-8.59372,-8.472545,-8.327206,-8.299713,-8.216613,-8.329428,-8.21773,-8.155763,-8.261657,-8.220514,-8.196628,-8.28276,-8.260799,-8.196584,-8.280241,-8.18436,-8.248575,-8.228287,-8.222163,-8.231911,-8.396143,-8.37417,-8.302195,-8.396403,-8.463686,-8.62927,-8.789087,-8.774072,-8.788803,-9.14952,-8.842973,-8.804343,-8.911633,-8.801873,-8.837972,-8.862427,-8.826279,-8.897445,-8.744858,-8.706851,-8.659874,-8.744629,-8.567302,-8.530364,-8.424735,-8.28555,-8.167141,-8.161301,-8.212717,-8.220761,-8.299985,-8.183261,-8.225781,-8.188262,-8.220224,-8.240246,-8.21857,-8.200196,-8.16298,-8.294157,-8.198301,-8.270789,-8.267992,-8.329181,-8.332213,-8.391383,-8.493956,-8.674302,-8.743777,-8.78103,-8.910763,-8.756545,-8.747926,-8.871904,-8.876596,-8.833262,-8.883851,-8.734047,-8.818259,-8.854642,-8.821593,-8.727651,-8.708777,-8.643457,-8.576779,-8.466168,-8.391964,-8.239382,-8.152429,-8.245235,-8.189108,-8.283322,-8.167431,-8.167407,-8.297194,-8.219675,-8.205765,-8.200499,-8.214964,-8.24721,-8.309165,-8.243302,-8.205765,-8.331929,-8.391427,-8.375553,-8.369182,-8.465056,-8.523647,-8.716291,-9.75337,-8.783253,-8.802133,-8.863007,-8.831891,-8.876047,-8.783821,-8.865218,-8.868021,-8.809937,-8.876602,-8.801886,-8.669011,-8.743512,-8.720162,-8.679297,-8.573736,-8.460315,-8.366663,-8.284161,-8.244685,-8.296355,-8.175476,-8.170753,-8.21134,-8.212427,-8.244395,-8.214396,-8.276364,-8.151577,-9.212555,-8.24605,-8.23301,-8.219638,-8.238857,-8.298312,-8.347789,-8.341937,-8.525351,-8.478651,-8.523955,-8.664294,-8.817975,-8.846869,-8.882196,-9.876194,-8.813233,-8.829897,-8.802997,-8.857735,-8.824921,-8.86799,-8.855759,-8.763781,-8.733485,-8.688459,-8.68097,-8.659009,-8.62012,-8.423642,-9.2662,-8.229386,-8.20161,-8.285254,-8.250236,-8.20245,-8.238598,-8.176877,-8.195516,-8.302207,-8.283877,-8.311376,-8.218039,-8.164363,-8.195769,-8.30614,-8.277463,-8.225781,-8.44643,-8.41088,-8.505613,-8.592887,-8.713784,-8.815734,-8.95193,-8.917739,-8.929667,-8.907984,-8.954721,-8.931908,-8.970236,-8.969699,-8.962759,-8.952202,-8.952449,-8.8352,-8.822155,-8.757384,-8.805473,-8.711525,-8.65457,-8.507286,-8.428353,-8.32084,-8.28747,-8.316377,-8.294144,-8.352494,-8.321655,-8.290804,-8.328595,-8.295515,-8.265244,-8.279432,-8.309406,-8.320544,-8.337522,-8.321093,-8.354988,-8.433625,-8.487017,-8.516473,-8.55259,-8.650428,-8.737955,-8.824655,-8.936903,-8.968618,-8.952751,-8.960259,-8.973323,-8.936903,-8.926364,-8.980577,-8.93026,-8.981367,-8.946929,-8.83378,-8.818247,-8.826588,-8.793224,-8.710407,-8.625102,-8.517825,-8.383901,-8.359995,-8.347505,-8.307776,-8.301633,-8.333589,-8.324724,-8.332244,-8.329459,-8.328891,-8.343332,-8.329447,-8.330256,-8.347475,-8.323057,-8.341109,-8.382783,-8.431156,-8.476997,-8.481985,-8.531735,-8.613452,-8.741845,-8.698776,-8.808233,-8.855216,-8.769337,-8.799089,-8.81574,-8.777659,-8.819914,-8.858007,-8.891037,-8.87162,-8.858815,-9.118094,-8.690144,-8.722915,-8.700973,-8.558146,-8.523406,-8.381116,-8.34611,-8.273585,-8.175772,-8.237443,-8.261929,-8.200511,-8.301652,-8.356661,-8.368904,-8.344455,-8.353062,-8.36139,-8.35142,-8.347777,-8.354167,-8.383913,-8.35944,-8.495907,-8.474218,-8.521455,-8.581774,-8.666517,-8.812949,-9.852566,-8.957196,-8.982479,-8.971372,-8.997493,-8.998617,-8.966359,-8.965525,-8.911905,-8.956091,-8.954165,-8.934415,-8.851042,-8.805201,-8.832422,-9.791722,-8.671536,-8.570642,-8.47031,-8.383907,-8.34887,-8.331089,-8.325255,-8.341369,-8.337226,-8.33388,-8.309987,-8.327212,-8.306943,-8.355581,-9.273177,-8.321414,-8.329441,-8.331663,-8.390562,-8.439206,-8.477003,-8.469514,-8.463945,-8.57176,-8.675988,-8.798527,-8.887975,-8.934699,-8.939409,-8.97804,-8.951103,-8.962771,-8.974144,-8.968853,-8.930538,-8.989708,-8.991091,-8.943311,-8.875213,-8.843819,-8.842127,-8.785173,-8.672932,-8.54399,-9.457412,-8.382505,-8.335256,-8.340831,-8.338634,-8.333589,-8.326952,-8.333046,-8.277222,-8.328051,-8.328311,-8.355531,-8.325273,-8.336923,-8.31805,-8.33304,-8.355575,-8.406713,-8.457265,-8.464217,-8.454783,-8.588707,-8.65541,-8.799083,-8.853284,-8.948609,-8.983324,-8.934711,-8.931908,-8.998574,-8.925796,-8.962475,-8.947769,-8.944966,-8.965253,-8.846591,-8.814357,-8.8327,-8.844097,-8.785735,-8.685693,-8.581496,-8.456969,-8.366114,-8.319445,-8.325261,-8.321945,-8.303319,-8.34945,-8.306659,-8.296916,-8.335553,-8.331379,-8.313889,-8.322458,-8.344147,-8.302207,-8.325576,-8.351951,-8.445874,-8.435323,-8.472545,-8.495346,-8.613736,-8.703746,-8.829644,-8.922166,-8.972205,-8.98167,-8.95498,-8.953863,-8.992758,-8.926913,-8.961895,-8.951924,-8.962475,-8.986918,-8.896353,-8.828798,-8.813517,-8.841868,-8.767392,-8.642618,-8.504217,-8.442559,-8.291082,-8.312746,-8.351636,-8.299713,-8.309709,-8.308332,-8.32694,-8.324421,-8.334719,-8.357773,-8.363909,-8.313876,-8.313611,-8.345277,-8.297744,-8.3956,-8.401422,-8.4017,-8.44643,-8.49479,-8.60513,-8.707672,-8.834373,-8.909114,-8.901903,-8.935261,-8.946367,-8.93523,-8.972489,-8.904422,-8.934686,-8.961358,-8.884412,-8.930507,-9.557145,-8.790476,-8.824908,-8.784358,-8.721539,-8.574835,-8.471459,-8.403046,-8.318025,-8.277216,-8.335293,-8.295824,-8.31082,-8.282173,-8.29441,-9.31235,-8.304158,-8.317784,-8.330262,-8.286637,-8.289415,-8.284155,-8.336658,-8.374177,-8.435335,-8.449745,-8.473366,-8.545644,-8.631233,-8.754057,-9.770861,-8.90967,-8.890234,-8.944954,-8.906354,-8.93802,-8.926654,-8.951905,-8.925796,-8.895772,-8.95719,-8.948886,-8.85161,-8.780444,-8.79102,-8.800756,-8.702659,-8.561764,-8.480053,-8.373053,-8.312753,-8.327767,-8.292755,-8.301349,-8.349728,-8.319433,-8.339702,-8.32389,-8.331669,-8.287483,-9.339552,-8.306116,-8.331398,-8.293601,-8.315012,-8.361946,-8.430594,-8.488678,-8.439774,-8.527857,-8.62764,-8.738782,-8.871058,-8.934427,-8.969155,-8.988047,-8.969736,-8.961635,-8.945238,-8.939409,-8.955801,-8.938317,-8.96358,-8.951628,-8.819074,-8.813789,-8.846579,-8.79352,-8.70098,-8.607587,-9.289574,-8.361144,-8.352796,-8.336374,-8.327792,-8.355013,-8.302732,-8.331392,-8.352512,-8.318896,-8.321674,-8.356402,-8.302504,-8.349432,-8.346388,-9.199806,-8.316926,-8.386666,-8.479503,-8.487554,-8.496173,-8.562024,-8.686545,-8.764614,-8.876325,-8.953332,-8.975545,-8.798515,-8.845233,-8.809912,-8.827433,-8.876621,-8.784062,-8.774647,-8.811875,-8.836065,-8.752155,-8.737393,-8.682643,-8.640395,-8.65762,-8.537038,-8.395582,-8.232449,-8.212729,-8.215489,-8.300541,-8.287761,-8.20579,-8.309141,-8.180748,-8.227985,-8.180199,-8.224657,-8.227442,-8.22441,-8.205512,-8.261089,-8.230794,-8.252162,-8.415863,-8.31279,-8.370306,-8.402811,-8.518948,-8.648187,-8.731269,-8.754902,-8.83412,-8.873003,-8.821865,-8.832453,-8.802145,-8.831298,-8.846573,-8.804646,-8.82965,-8.796323,-8.767652,-8.801849,-8.697627,-8.694861,-8.536482,-8.403342,-8.366132,-8.223583,-8.284427,-8.294978,-8.172154,-8.20466,-8.212464,-8.301374,-8.182156,-8.221897,-8.372269,-8.34611,-8.322229,-8.327471,-8.330274,-8.341943,-8.358606,-8.427828,-8.465624,-8.497562,-8.482257,-8.627053,-8.673172,-8.78408,-8.946077,-8.956635,-8.965525,-8.956616,-8.964432,-8.966383,-8.976928,-8.947195,-8.956906,-8.994166,-8.974168,-8.894957,-8.821315,-8.812419,-8.829125,-8.75573,-8.656528,-8.545373,-8.473669,-8.330546,-8.325557,-8.34277,-8.36307,-8.335837,-8.309715,-8.363897,-8.380011,-8.329434,-8.323328,-8.261633,-8.213575,-8.214384,-8.251649,-8.233838,-8.234968,-8.263843,-8.366132,-8.372794,-8.403324,-8.555918,-8.590417,-9.643895,-8.795459,-8.839392,-8.87246,-8.765151,-8.868552,-8.815468,-8.84827,-8.802985,-8.790995,-8.820191,-8.856642,-8.828786,-8.712926,-8.787112,-8.762959,-8.725144,-8.513133,-8.411411,-8.330842,-8.166869,-8.211359,-8.228837,-8.209395,-8.189923,-8.25499,-8.215501,-8.228016,-8.192411,-8.23748,-9.213444,-8.232757,-8.221064,-8.258286,-8.251353,-8.370849,-8.289403,-8.283309,-8.365027,-8.450597,-8.536204,-8.590936,-8.673185,-8.831335,-8.816586,-9.81506,-8.852709,-8.826872,-8.803528,-8.837157,-8.820506,-8.837417,-8.83549,-8.847696,-8.796829,-8.735461,-8.782136,-8.765435,-8.632919,-9.041131,-9.334027,-8.261083,-8.182693,-8.312191,-8.177964,-8.15383,-8.232467,-8.225799,-8.217187,-8.243302,-8.26856,-8.198819,-8.226633,-8.199968,-8.219385,-8.253002,-8.145489,-8.243827,-8.282772,-8.30777,-8.331669,-8.406411,-8.597332,-8.727095,-8.830755,-8.792674,-8.77882,-8.82271,-8.840757,-8.850209,-8.86715,-8.798799,-8.786593,-8.87354,-8.812703,-8.802145,-8.783796,-8.708493,-8.68013,-8.665399,-8.617607,-8.420302,-8.362489,-8.276364,-8.286643,-8.226052,-8.213272,-8.274974,-8.171043,-8.199665,-8.224676,-8.20411,-8.188818,-8.246902,-8.258033,-8.195492,-8.229405,-8.274159,-8.311394,-8.279173,-8.34193,-8.319439,-8.372775,-8.436163,-8.543416,-8.666819,-8.800176,-8.776838,-8.831842,-8.778802,-8.824359,-8.840213,-8.79962,-8.849406,-8.878547,-9.369841,-8.978583,-8.851604,-8.735708,-8.645149,-8.807158,-8.708759,-8.562308,-8.497556,-8.371639,-8.258595,-8.228855,-8.166326,-8.180205,-8.204117,-8.248575,-8.213001,-8.253563,-8.208562,-8.231059,-8.187441,-8.221336,-8.238839,-8.248587,-8.194948,-8.244667,-8.336936,-8.394458,-8.284136,-8.370571,-8.420586,-8.49145,-8.735436,-8.744327,-8.776307,-8.862446,-8.821025,-8.748747,-9.435198,-8.817975,-8.840781,-8.819901,-8.812412,-8.741283,-9.244283,-8.667931,-8.704882,-8.662072,-8.657096,-8.668758,-8.527561,-8.456993,-8.317784,-8.238277,-8.199097,-8.154941,-8.23882,-8.25857,-8.21523,-8.191898,-8.216878,-8.316932,-8.206623,-8.22467,-8.223546,-8.249668,-8.221329,-8.258848,-8.316389,-8.359724,-8.378616,-8.357779,-8.468668,-8.63482,-9.603869,-8.766861,-8.959956,-8.874127,-8.807979,-8.775178,-8.805177,-8.783796,-8.936884,-8.81353,-8.809356,-8.973891,-8.879912,-8.696825,-8.727404,-9.661101,-8.607877,-8.59924,-8.485893,-8.250507,-8.253847,-8.224682,-8.233832,-8.207185,-8.212149,-8.196072,-8.188527,-8.249958,-8.196591,-8.246877,-9.227582,-8.17852,-8.222435,-8.188268,-8.251359,-8.264985,-8.322192,-8.323878,-8.291638,-8.411702,-9.130597,-8.560351,-8.715704,-8.793236,-8.852981,-8.961351,-8.901335,-8.80964,-8.857142,-8.850474,-8.841874,-8.822149,-8.856315,-8.850505,-8.832434,-8.737387,-8.707907,-8.697349,-8.574279,-8.512836,-9.397926,-8.324705,-8.182983,-8.216878,-8.200233,-8.17605,-8.265522,-8.223558,-8.219101,-8.232702,-8.220798,-8.196887,-8.240475,-8.248569,-8.204394,-8.21552,-8.165202,-8.330817,-9.021917,-8.451412,-8.475626,-8.524795,-8.642087,-8.750741,-8.814073,-8.95887,-8.998333,-8.992746,-8.925784,-8.971372,-8.956067,-8.918857,-8.960246,-8.993042,-8.956363,-8.924716,-8.889672,-8.817123,-8.796305,-8.8266,-8.746,-8.639586,-8.472014,-8.38971,-8.351667,-8.357791,-8.341085,-8.299151,-8.343307,-8.363644,-8.332762,-8.313043,-8.310271,-8.32778,-8.328311,-8.338035,-8.346962,-8.309437,-8.352222,-8.396705,-8.470076,-8.463118,-8.467532,-8.538717,-8.644285,-8.727101,-8.826044,-8.932192,-8.965834,-8.924685,-8.881066,-8.84769,-8.80104,-8.860476,-8.870484,-8.853271,-8.811869,-8.806004,-8.752408,-8.719884,-8.727947,-8.711833,-8.564555,-8.450875,-8.353327,-8.341381,-8.303041,-8.245772,-8.221329,-8.282778,-8.23577,-8.253835,-8.246087,-8.188243,-8.887425,-8.34277,-8.328613,-8.338349,-8.384178,-8.347783,-8.354463,-8.417542,-8.443923,-8.477806,-8.494222,-8.595931,-8.684557,-8.781018,-8.869089,-8.959431,-9.010533,-8.999154,-8.971366,-8.982195,-8.993598,-8.967766,-8.97528,-8.970544,-8.975558,-9.59467,-8.852722,-8.822445,-8.813814,-8.805195,-8.710969,-8.575668,-8.444769,-8.362199,-8.314444,-8.332237,-8.33191,-8.316648,-9.089756,-8.358322,-9.305398,-8.337479,-8.304961,-8.312765,-8.33751,-8.31471,-8.335275,-8.316654,-8.347215,-8.424759,-8.43478,-8.484498,-8.466977,-8.568142,-8.676525,-9.729743,-8.882455,-8.968032,-8.966099,-8.956363,-8.970514,-8.982775,-8.973884,-8.959999,-8.967445,-8.981664,-8.964142,-8.928043,-8.877738,-8.859081,-8.849659,-8.78713,-8.691799,-8.582317,-8.476169,-8.372528,-8.354704,-8.342474,-8.327181,-8.350549,-8.331929,-8.347215,-8.331379,-8.312487,-8.326378,-9.308467,-8.321396,-8.330533,-8.30556,-8.355569,-8.371954,-8.461142,-8.456722,-8.468378,-8.485628,-8.599018,-8.715735,-8.821297,-8.873818,-8.988331,-8.987486,-8.918566,-8.909404,-8.946077,-8.978027,-8.957758,-8.950257,-8.954406,-8.951918,-8.917727,-8.823285,-8.863267,-8.814369,-8.786025,-9.03529,-9.311776,-8.47173,-8.357501,-8.340276,-8.353068,-8.373349,-8.346104,-8.340813,-8.371411,-8.360532,-8.350833,-8.314419,-8.350284,-8.341122,-8.373337,-9.133375,-8.314975,-8.387512,-8.418913,-8.457277,-8.452826,-8.527265,-8.587892,-8.715711,-8.816296,-8.905521,-8.956369,-8.968865,-8.959166,-8.920486,-8.987214,-8.94383,-8.958308,-8.934415,-8.968877,-8.933834,-8.904144,-9.486849,-8.797416,-8.809362,-8.787402,-8.628171,-8.521758,-8.43891,-8.314994,-8.332484,-8.327767,-8.309715,-8.352766,-8.308875,-8.332472,-8.341122,-8.332497,-8.307208,-8.324458,-8.356396,-8.336658,-8.331941,-8.330262,-8.415597,-8.468372,-8.46865,-8.454215,-8.5148,-8.629825,-8.743221,-8.834101,-8.916368,-8.966087,-8.969976,-8.96663,-8.954134,-8.9625,-8.923302,-8.99332,-8.945244,-8.966389,-8.920801,-8.879405,-8.819105,-8.801034,-8.826853,-8.74658,-8.638765,-8.516744,-8.411702,-8.33083,-8.330299,-8.350018,-8.344739,-8.338874,-8.34916,-8.333608,-8.329706,-8.341955,-8.335831,-8.356087,-8.357501,-8.320538,-8.322513,-8.32581,-8.399737,-8.443392,-8.458098,-8.356951,-8.411146,-8.526499,-8.602623,-8.77682,-8.780993,-8.857432,-8.892185,-8.77769,-9.412398,-8.979163,-8.974718,-8.964988,-8.967482,-8.923845,-8.974699,-8.881072,-8.808239,-8.83462,-8.816049,-8.733491,-8.555115,-8.485066,-8.405009,-8.31805,-8.329175,-8.34945,-8.338621,-8.318877,-8.327218,-8.364712,-8.305264,-8.301664,-8.341949,-8.342221,-8.343042,-8.354729,-8.35,-8.352512,-8.405596,-8.43615,-8.492005,-8.473934,-8.545651,-8.647328,-9.740862,-8.863569,-9.596059,-8.981083,-8.987486,-8.975514,-8.976632,-8.947182,-8.998333,-8.971112,-8.976934,-8.940237,-8.913294,-8.836879,-8.838806,-8.802985,-8.797972,-8.715445,-8.605383,-8.448103,-8.371108,-8.350833,-8.3439,-8.298318,-8.336096,-8.321933,-8.326354,-8.342467,-8.326384,-8.33554,-9.290692,-8.310264,-8.333608,-8.346394,-8.32807,-8.303306,-8.428921,-8.457555,-8.460895,-8.448634,-8.557591,-8.697936,-8.792965,-8.879387,-8.954165,-9.941495,-8.914961,-8.983318,-8.951652,-8.951912,-8.950257,-8.948868,-8.950535,-8.978595,-8.880208,-8.730966,-8.729034,-8.741851,-8.668456,-8.587065,-9.420733,-8.350839,-8.207722,-8.172722,-8.228812,-8.164079,-8.172975,-8.227201,-8.202419,-8.17271,-8.246068,-8.228831,-8.198264,-8.286637,-8.194936,-8.239975,-8.249668,-8.251365,-8.884943,-8.331367,-8.303584,-8.34361,-8.486733,-8.490623,-8.604821,-8.795175,-8.848246,-8.787686,-8.835188,-8.822698,-8.831576,-8.798515,-8.790995,-8.824655,-8.89326,-8.738468,-8.746537,-8.742085,-8.685131,-8.742388,-8.624281,-8.533155,-8.482819,-8.309412,-8.287477,-8.267195,-8.259429,-8.247754,-8.26217,-8.26664,-8.194652,-8.288878,-8.271073,-8.172142,-8.202752,-8.192726,-8.469786,-8.362502,-8.353865,-8.408639,-8.475317,-8.437249,-8.512849,-8.521461,-8.61039,-8.714056,-8.807121,-8.886894,-8.924117,-8.954708,-8.971106,-8.897452,-8.961642,-8.979138,-8.954974,-8.946917,-8.955807,-8.966365,-8.882147,-8.836318,-8.828847,-8.821297,-8.754069,-8.660133,-8.5259,-8.409726,-8.319433,-8.310573,-8.378893,-8.338047,-8.312456,-8.320803,-8.326656,-8.317772,-8.331657,-8.323606,-8.335553,-8.336942,-8.321624,-8.311067,-8.347197,-8.355859,-8.432008,-8.488381,-8.479485,-8.487289,-8.63014,-8.625948,-8.737103,-8.829372,-8.806862,-8.871052,-8.901329,-8.799645,-8.792409,-8.8966,-8.886629,-8.918863,-8.895223,-9.286778,-8.73793,-8.771566,-8.757113,-8.738776,-8.63345,-8.597345,-8.481967,-8.298059,-8.269708,-8.25996,-8.301942,-8.276073,-8.242185,-8.365564,-8.342505,-8.304128,-8.348308,-8.351376,-8.350549,-8.347221,-8.348333,-8.340554,-8.329453,-8.383092,-8.460889,-8.470897,-8.417536,-8.547287,-8.648736,-9.746122,-8.847443,-8.961364,-8.95469,-8.937187,-8.989153,-8.947479,-8.953313,-8.968593,-8.945509,-8.922752,-8.969705,-8.955239,-8.88661,-8.824106,-9.815331,-8.803818,-8.740746,-8.615681,-8.49842,-8.384191,-8.299997,-8.342239,-8.32026,-8.336954,-8.314975,-8.35166,-8.347215,-8.335553,-8.350006,-9.240103,-8.337213,-8.380851,-8.341677,-8.3261,-8.349413,-8.399483,-8.468119,-8.498939,-8.490616,-8.5812,-8.653428,-8.772109,-8.886907,-8.973594,-8.983874,-8.995833,-8.975274,-8.964432,-8.990819,-9.011669,-8.973032,-8.96805,-8.981664,-8.954437,-8.913578,-8.837997,-8.855222,-8.842158,-8.729052,-9.566863,-8.500908,-8.398335,-8.315839,-8.314154,-8.343906,-8.335287,-8.330268,-8.335849,-8.324434,-8.353618,-8.334719,-8.327236,-8.335534,-8.350852,-8.341369,-8.333318,-8.382808,-8.416696,-8.47228,-8.483127,-8.479195,-8.573705,-8.65457,-8.765991,-8.868268,-8.961074,-8.969433,-8.966661,-8.986936,-8.977206,-8.952764,-8.948868,-8.962203,-8.972211,-8.958018,-8.924141,-8.862143,-8.84243,-8.816018,-8.794916,-8.685446,-8.607877,-8.496741,-8.389469,-8.355556,-8.322483,-8.349987,-8.319976,-8.348882,-8.313858,-8.340276,-8.328298,-8.334738,-8.345838,-8.323606,-8.350308,-8.33191,-8.315543,-8.350845,-8.400607,-8.487536,-8.488104,-8.478942,-8.56482,-8.669845,-8.77937,-8.883258,-8.969458,-8.965544,-8.956622,-8.943602,-8.93802,-8.964124,-8.966926,-8.964414,-8.96471,-8.95164,-8.923845,-8.866916,-8.828261,-8.828255,-8.760465,-8.674024,-8.558449,-8.468668,-8.361662,-8.212161,-8.351691,-8.348592,-8.311654,-8.316926,-8.365274,-8.335553,-8.351117,-8.323051,-8.334157,-8.360014,-8.341393,-8.31471,-8.300263,-8.367496,-8.439762,-8.481164,-8.456141,-8.463945,-8.557856,-8.705999,-8.794064,-8.887709,-8.969976,-8.954406,-8.956919,-8.908577,-8.978885,-8.953863,-8.970822,-8.936921,-9.011397,-9.655551,-8.856043,-8.840183,-8.836009,-8.843547,-8.744036,-8.628473,-8.532593,-8.427241,-8.346944,-8.333596,-8.371695,-8.333305,-8.326922,-8.322217,-9.353196,-8.3322,-8.290823,-8.36086,-8.33943,-8.343881,-8.343894,-8.340535,-8.315827,-8.386129,-8.473083,-8.478096,-8.466452,-8.504255,-8.623176,-9.687809,-8.811875,-8.93857,-8.959419,-8.974681,-8.981083,-8.977749,-8.955536,-8.950819,-8.94775,-8.934662,-8.967748,-8.933587,-8.894976,-8.834373,-8.844368,-8.805189,-8.722107,-8.646248,-8.535075,-8.422561,-8.346388,-8.298596,-8.352772,-8.35166,-8.313605,-8.342498,-8.295805,-8.34611,-8.31303,-9.326809,-8.315537,-8.348333,-8.355297,-8.340825,-8.330002,-8.374479,-8.458673,-8.433082,-8.4681,-8.541742,-8.618447,-8.744049,-8.83186,-8.934162,-9.015836,-8.95109,-8.961901,-8.962463,-8.964154,-8.983047,-8.927185,-8.980546,-8.92495,-8.937174,-8.864113,-8.833268,-8.815759,-8.807387,-8.720718,-9.309825,-8.498957,-8.414468,-8.312734,-8.356964,-8.33196,-8.316395,-8.326088,-8.319439,-8.316932,-8.32389,-8.312222,-8.309709,-8.333336,-8.348043,-9.123077,-8.353074,-8.316661,-8.399453,-8.478682,-8.49061,-8.476447,-8.548435,-8.63348,-8.74908,-8.823556,-8.969402,-8.978848,-8.809628,-8.788519,-8.825476,-8.771837,-8.859655,-8.835213,-8.866045,-8.82242,-8.780191,-8.692904,-8.734059,-8.774072,-8.665967,-8.606791,-8.602883,-8.38503,-8.249952,-8.206339,-8.20716,-8.166295,-8.206611,-8.229405,-8.24884,-8.235789,-8.218292,-8.170506,-8.253841,-8.20161,-8.219681,-8.168265,-8.154108,-8.217434,-8.273023,-8.340023,-8.292761,-8.371695,-8.416141,-8.483949,-8.681285,-8.716272,-8.842701,-8.753785,-8.83049,-8.822686,-8.83441,-8.891877,-8.872725,-8.773795,-8.80993,-8.808233,-8.762373,-8.749618,-8.766009,-8.646785,-8.695158,-8.557869,-8.543434,-8.397211,-8.315278,-8.154923,-8.181057,-8.281679,-8.229683,-8.239975,-8.254415,-8.260799,-8.222181,-8.207994,-8.227448,-8.205796,-8.199665,-8.213575,-8.22383,-8.192139,-8.263034,-8.305511,-8.435885,-8.401965,-8.395279,-8.480608,-8.646236,-8.772955,-8.842448,-8.828236,-8.793502,-8.811869,-8.751569,-8.779901,-8.875781,-8.80188,-8.763774,-8.854654,-8.78492,-8.766577,-8.650675,-8.762947,-8.619274,-8.537316,-8.50841,-8.345845,-8.216063,-8.185484,-8.229411,-8.207704,-8.312215,-8.222978,-8.280241,-8.302763,-8.253304,-8.237462,-8.190787,-8.213538,-8.209642,-8.181884,-8.210247,-8.222731,-8.300534,-8.35555,-8.324415,-8.349722,-8.478386,-9.472964,-8.679328,-8.762416,-8.785198,-8.784333,-8.81937,-8.771004,-8.831058,-8.838806,-8.829909,-8.826044,-8.787414,-8.861063,-8.825736,-8.69128,-8.749902,-8.804639,-8.659565,-8.630387,-8.471446,-8.344153,-8.300806,-8.178526,-8.1791,-8.266362,-8.201591,-8.182156,-8.158504,-8.186589,-8.233838,-9.262045,-8.214952,-8.181316,-8.284964,-8.233294,-8.278018,-8.284124,-8.237474,-8.265238,-8.343048,-8.310839,-8.484788,-8.582317,-8.655972,-8.767374,-9.811152,-8.799071,-8.88106,-8.986955,-8.720421,-8.864674,-8.865508,-8.786846,-8.849647,-8.861865,-8.711253,-8.752661,-8.678735,-8.698751,-8.627331,-9.624953,-8.543416,-8.446695,-8.33388,-8.326082,-8.309987,-8.359168,-8.344702,-8.29691,-8.324452,-8.327206,-8.317482,-8.283581,-8.331953,-8.309172,-8.331392,-8.325279,-8.3211,-8.412801,-8.430044,-8.444763,-8.472533,-8.486714,-8.611254,-8.743777,-8.832156,-8.968303,-8.98304,-8.953029,-8.978311,-8.956622,-8.956091,-8.953566,-8.974724,-8.944447,-8.983862,-8.88327,-8.90302,-8.817438,-8.843825,-8.812147,-8.743752,-8.639284,-8.45616,-8.29691,-8.211328,-8.195763,-8.26217,-8.233264,-8.184372,-8.215532,-8.223003,-8.262744,-8.238573,-8.167135,-8.223552,-8.230529,-8.220774,-8.174099,-8.229652,-8.254422,-8.404503,-8.332213,-8.371695,-8.452814,-8.567599,-8.647335,-8.690132,-8.765725,-8.919665,-8.859118,-8.824649,-8.809085,-8.938848,-8.781296,-8.865218,-8.903854,-8.843282,-8.731812,-8.749889,-8.690428,-8.720446,-8.69262,-8.564555,-8.505644,-8.366114,-8.294151,-8.249976,-8.19272,-8.184403,-8.170481,-8.189392,-8.230782,-8.208012,-8.22107,-8.179903,-8.256638,-8.23606,-8.214989,-8.298843,-8.158245,-8.214118,-8.237999,-8.362767,-8.309159,-8.344715,-8.556189,-8.619836,-8.693472,-8.716007,-8.814641,-8.843807,-8.807979,-8.875201,-8.924376,-8.95556,-8.985837,-8.959987,-8.928574,-9.385128,-8.93247,-8.878269,-8.806313,-8.840195,-8.776573,-8.701548,-8.606519,-8.477559,-8.36862,-8.326354,-8.318889,-8.32891,-8.341683,-8.291638,-8.336399,-8.347759,-8.34945,-8.344721,-8.364181,-8.325551,-8.310783,-8.329731,-8.321915,-8.343622,-8.418907,-8.476163,-8.486739,-8.473657,-8.567883,-9.662503,-8.797397,-8.865471,-8.963339,-8.944676,-8.953603,-8.959154,-8.956931,-8.942225,-8.946349,-8.86686,-8.797978,-8.846622,-8.786291,-8.801577,-9.711659,-8.70987,-8.645093,-8.571519,-8.451721,-8.358896,-8.233017,-8.172142,-8.225231,-8.206345,-8.251359,-8.265541,-8.261349,-8.239968,-8.243012,-9.261508,-8.232442,-8.263565,-8.22717,-8.191886,-8.253286,-8.221323,-8.237733,-8.424747,-8.313037,-8.403626,-9.134486,-8.562888,-8.660658,-8.757119,-8.82242,-8.824346,-8.889382,-8.799089,-8.767936,-8.825476,-8.790742,-8.861359,-8.746284,-8.803534,-8.752143,-8.800453,-8.791878,-8.731528,-8.651224,-9.584415,-8.526197,-8.37698,-8.286378,-8.282717,-8.172179,-8.198542,-8.263312,-8.238283,-8.239962,-8.239938,-8.233603,-8.227164,-8.229102,-8.229664,-8.234424,-8.205747,-8.194942,-8.215785,-8.874108,-8.336108,-8.363348,-8.378338,-8.435317,-8.552003,-8.642352,-8.774344,-8.771603,-8.839633,-8.782148,-8.848264,-8.778505,-8.863551,-8.812443,-8.844091,-8.909108,-8.814104,-8.795737,-8.804917,-8.724873,-8.737393,-8.610909,-8.525913,-8.412245,-8.31721,-8.220792,-8.199122,-8.160492,-8.303572,-8.210494,-8.189645,-8.236875,-8.253008,-8.211865,-8.303584,-8.169104,-8.233856,-8.253835,-8.202153,-8.14657,-8.231319,-8.278858,-8.334157,-8.359464,-8.378931,-8.438373,-8.615107,-8.734319,-8.861878,-8.837404,-8.911331,-8.790174,-8.808529,-8.850777,-8.832447,-8.786587,-8.876053,-8.796582,-8.881319,-8.756298,-8.719884,-8.695417,-8.646804,-8.574804,-8.440836,-8.470329,-8.271616,-8.229658,-8.257447,-8.229405,-8.251643,-8.242728,-8.236326,-8.226904,-8.211877,-8.866613,-8.347215,-8.360582,-8.319439,-8.335275,-8.341671,-8.313592,-8.394452,-8.423642,-8.456709,-8.45587,-8.524246,-8.609285,-8.738227,-8.874676,-8.944416,-8.935792,-8.931655,-8.97665,-8.94191,-8.974434,-8.956919,-8.955554,-8.969983,-9.649457,-8.914393,-8.877751,-8.831298,-8.816043,-8.816012,-8.695979,-8.58788,-8.512867,-8.396705,-8.35584,-8.311654,-8.345832,-8.329694,-8.996395,-9.341515,-8.323563,-8.345548,-8.364984,-8.342221,-8.309968,-8.361384,-8.354747,-8.364169,-8.346962,-8.440867,-8.491184,-8.475879,-8.500328,-8.547855,-9.59801,-8.771584,-8.881893,-8.971662,-9.013867,-8.974724,-8.973304,-8.954443,-8.954702,-9.001679,-8.985522,-8.947726,-8.963309,-8.92829,-8.882986,-8.844387,-8.869922,-8.844097,-8.679019,-8.641513,-8.532309,-8.392797,-8.363613,-8.325261,-8.348623,-8.356124,-8.362773,-8.302732,-8.379177,-8.344986,-9.345127,-8.358069,-8.347221,-8.356951,-8.380011,-8.357532,-8.343301,-8.41532,-8.491987,-8.485887,-8.465637,-8.598999,-8.693491,-8.766559,-8.916344,-8.934964,-8.958876,-8.933297,-8.983053,-8.970248,-8.961111,-8.972471,-8.997209,-8.971625,-8.98054,-8.915214,-8.828798,-8.80409,-8.837701,-8.735689,-10.03235,-8.601777,-8.483671,-8.319426,-8.352235,-8.333602,-8.331669,-8.341677,-8.343344,-8.307492,-8.33638,-8.305832,-8.344449,-8.325532,-8.316086,-9.075025,-8.349456,-8.326644,-8.351944,-8.438928,-8.477546,-8.4798,-8.486974,-8.587874,-8.682371,-8.781821,-8.879683,-8.91606,-8.929976,-8.920783,-8.906626,-8.944694,-8.893272,-8.944676,-8.964124,-8.925537,-8.945824,-8.883276,-9.469352,-8.79883,-8.811301,-8.743505,-8.62259,-8.514509,-8.462821,-8.350852,-8.335553,-8.311123,-8.330015,-8.31637,-8.296954,-8.295515,-8.33638,-8.298299,-8.335275,-8.339177,-8.339992,-8.309968,-8.311666,-8.311104,-8.386673,-8.375269,-8.461704,-8.434483,-8.456438,-8.566234,-8.727379,-8.787427,-8.872466,-8.907435,-8.939138,-8.946923,-8.947201,-8.956641,-8.941663,-8.945552,-8.979997,-8.93915,-8.959135,-8.867681,-8.779629,-8.78074,-8.79962,-8.717939,-8.646822,-8.560388,-8.453937,-8.32055,-8.282223,-8.328045,-8.345277,-8.342208,-8.337479,-8.335565,-8.323884,-8.309153,-8.322495,-8.300818,-8.326391,-8.319717,-8.326915,-8.314994,-8.360285,-8.426167,-8.487838,-8.478386,-8.503674,-8.637642,-8.702931,-8.782938,-8.942719,-8.924401,-8.939434,-8.945812,-9.555237,-8.94525,-8.966075,-8.937483,-8.96221,-8.973878,-8.945781,-8.865786,-8.840207,-8.779888,-8.76767,-8.736591,-8.623985,-8.536717,-8.441725,-8.341974,-8.346135,-8.328619,-8.321655,-8.331645,-8.313333,-8.306381,-8.34832,-8.283606,-8.315296,-8.306918,-8.317229,-8.313308,-8.343319,-8.338337,-8.358334,-8.390025,-8.432254,-8.422543,-8.519245,-9.560504,-8.75544,-8.85492,-9.208419,-8.966075,-8.961098,-8.915788,-8.928031,-8.96692,-8.976941,-8.954147,-8.94275,-8.965241,-8.913004,-8.851314,-8.781018,-8.771307,-8.786025,-8.705456,-8.578718,-8.479232,-8.402515,-8.315821,-8.283556,-8.279136,-8.357501,-8.307764,-8.322205,-8.293601,-8.323872,-9.285098,-8.353074,-8.348055,-8.320822,-8.315296,-8.340547,-8.339708,-8.359174,-8.45253,-8.459512,-8.452252,-8.532599,-8.633203,-8.703776,-8.879103,-9.905909,-8.971656,-8.886332,-8.947226,-8.942484,-8.915794,-8.975817,-8.931612,-8.994703,-8.900761,-8.890234,-8.854111,-8.806016,-8.807411,-8.781845,-9.679987,-8.594548,-8.445318,-8.375837,-8.299701,-8.330268,-8.269961,-8.340288,-8.310802,-8.303874,-8.327206,-8.306381,-8.321396,-8.275542,-8.280259,-8.315253,-8.342245,-8.315815,-8.331953,-9.043613,-8.410016,-8.442806,-8.440342,-8.546762,-8.65123,-8.736294,-8.82547,-8.914942,-8.918585,-8.937187,-8.981392,-8.974706,-8.902724,-8.892753,-8.922462,-8.933841,-8.917177,-8.899946,-8.869681,-8.819636,-8.785198,-8.746265,-8.714605,-8.503711,-8.451992,-8.330848,-8.308048,-8.292206,-8.296626,-8.290261,-8.278018,-8.310561,-8.30498,-8.357519,-8.319414,-8.327774,-8.287736,-8.940243,-8.314722,-8.313586,-8.304152,-8.363595,-8.472552,-8.475324,-8.49479,-8.597326,-8.679031,-8.804615,-8.923864,-8.963037,-8.971643,-8.992764,-8.953048,-8.925784,-8.975545,-8.921919,-8.916097,-8.933316,-8.934964,-8.855506,-8.849641,-8.802423,-8.798268,-8.761002,-8.643192,-8.534235,-8.432835,-8.338022,-8.328601,-8.352241,-8.298559,-8.328329,-8.320272,-8.310264,-8.282766,-8.344196,-8.322804,-8.302461,-8.335837,-8.328576,-8.348339,-8.331922,-8.344709,-8.443942,-8.434199,-8.432841,-8.483942,-8.568975,-8.667647,-8.791298,-8.864662,-8.958851,-8.937465,-8.942484,-8.958579,-8.950257,-8.979694,-8.961395,-8.964426,-9.405168,-8.931365,-8.879109,-8.804096,-8.81269,-8.803769,-8.762941,-8.601765,-8.54094,-8.442553,-8.322779,-8.34335,-8.29746,-8.334435,-8.955536,-8.339183,-8.332497,-8.310839,-8.366404,-8.366391,-8.322489,-8.342776,-8.341381,-8.366379,-8.342535,-8.37251,-8.463112,-8.490073,-8.485893,-8.52285,-9.594133,-8.711012,-8.863538,-8.954715,-8.968593,-8.9939,-8.988862,-9.021115,-8.986405,-8.949689,-8.985547,-8.996104,-9.01002,-8.969686,-8.930538,-9.850905,-8.820741,-8.853561,-8.734047,-8.639568,-8.503131,-8.43615,-8.978324,-8.374183,-8.348333,-8.341937,-8.362773,-8.330836,-8.363045,-8.359736,-9.305979,-8.350833,-8.353352,-8.38056,-8.360551,-8.346388,-8.353068,-8.389457,-8.450616,-8.488962,-8.455617,-8.552837,-8.633727,-8.732115,-8.856309,-8.994431,-8.983874,-8.981361,-8.9797,-8.953011,-8.973594,-8.987226,-8.988591,-8.99582,-8.970273,-8.941095,-8.904681,-8.829952,-8.850777,-8.822155,-9.675295,-8.609273,-8.517559,-8.462278,-8.367503,-8.35029,-8.346925,-8.325279,-8.344999,-8.336102,-8.357519,-8.318321,-8.365576,-8.334472,-8.355291,-8.354167,-8.348314,-8.368361,-8.321112,-8.425037,-8.445899,-8.514793,-8.504798,-8.560919,-8.65762,-8.765435,-8.862421,-8.968063,-8.979997,-8.961098,-9.010576,-8.926876,-8.943293,-8.962741,-8.993598,-9.001655,-8.965247,-8.939706,-8.877436,-8.848548,-8.874948,-8.830755,-8.72349,-8.611483,-8.528401,-8.37806,-8.342233,-8.340566,-8.301355,-8.313598,-8.302473,-8.312777,-8.33693,-8.306937,-8.324452,-8.336102,-8.335287,-8.326107,-8.348055,-8.337763,-8.340825,-8.398107,-8.46781,-8.463661,-8.469489,-8.521467,-8.655422,-8.709321,-8.863001,-8.938057,-8.954128,-8.937174,-8.932982,-8.930247,-8.961907,-8.966365,-8.949127,-8.977218,-8.941626</t>
+  </si>
+  <si>
+    <t>-13.015553,-12.640687,-12.909671,-12.810203,-12.584831,-12.735462,-12.879116,-12.776833,-12.93165,-12.892989,-12.589524,-13.469335,-12.608471,-12.640921,-12.881339,-12.803795,-12.678465,-12.990549,-12.788798,-12.757379,-12.462279,-13.279568,-13.491042,-13.879516,-13.699733,-14.15799,-15.224803,-14.460042,-14.470328,-14.478662,-14.424734,-14.156866,-13.955955,-14.165757,-14.170733,-14.157965,-14.399742,-13.611927,-14.132393,-14.122669,-15.584383,-13.858112,-12.558981,-12.773209,-12.675415,-12.747952,-12.526192,-12.680712,-12.729054,-12.522592,-12.508127,-12.512837,-12.763782,-12.321107,-12.283848,-12.4631,-12.591493,-12.58146,-12.476449,-12.835485,-12.640662,-12.906627,-12.538959,-12.862157,-13.463778,-14.08378,-14.440032,-14.525905,-14.455899,-14.544513,-14.144914,-14.809083,-14.092139,-14.21216,-13.808109,-14.511452,-14.429994,-14.240788,-15.019416,-13.853673,-14.064838,-13.853642,-13.536322,-13.326508,-12.500613,-12.726535,-12.676532,-12.292485,-12.48587,-12.285527,-12.524235,-12.268024,-12.247181,-12.494785,-12.511436,-12.429774,-12.548146,-12.73377,-12.311902,-12.508973,-12.562334,-12.846314,-12.626493,-12.921617,-12.990006,-12.854674,-13.488517,-13.842282,-13.964852,-14.43505,-14.264947,-14.219958,-14.179648,-14.171863,-14.499771,-14.057652,-14.497845,-14.221618,-14.177413,-14.299718,-14.327482,-14.117965,-14.11018,-13.960425,-13.663862,-13.278704,-12.86186,-12.682657,-12.476998,-12.696523,-12.682076,-12.820754,-12.748205,-12.694591,-12.706531,-12.254417,-12.780464,-12.480048,-12.454482,-12.703481,-12.740975,-12.266363,-12.577904,-12.814636,-12.632636,-12.898576,-12.973034,-13.454616,-13.807584,-13.930124,-13.85479,-14.103499,-13.83115,-14.047656,-14.294662,-14.035698,-14.119366,-14.351085,-14.383615,-14.147982,-14.117409,-13.944861,-13.987615,-13.799237,-13.794218,-13.660269,-13.267331,-12.833818,-12.777117,-12.440337,-12.510362,-12.566192,-11.955649,-12.161351,-12.407517,-12.365541,-12.600069,-12.66374,-12.271648,-12.255812,-12.654843,-12.214663,-12.646509,-12.38084,-12.642934,-12.672371,-12.288317,-12.65459,-13.030821,-13.075576,-14.518676,-13.699448,-14.279986,-14.08628,-13.629412,-13.915621,-14.017102,-14.105981,-14.16714,-13.898983,-14.091022,-13.376239,-14.054034,-14.027054,-14.030135,-14.98081,-13.802009,-13.446269,-13.453487,-12.90688,-12.663209,-12.571199,-12.048492,-12.678755,-12.705685,-12.732659,-12.663166,-12.550362,-12.619547,-12.186621,-13.664146,-12.121042,-12.506719,-12.572304,-12.446727,-12.38334,-12.646793,-12.585652,-12.105447,-12.474479,-12.704827,-13.343746,-13.800614,-13.943997,-13.833113,-14.051811,-14.312758,-14.228027,-14.11907,-14.326093,-14.246067,-13.869546,-14.300527,-14.062072,-13.853981,-13.904231,-14.038217,-14.037093,-14.171036,-13.794767,-14.167152,-12.709285,-12.420013,-12.283317,-12.423081,-12.227721,-12.364707,-12.000978,-12.431416,-12.642594,-12.193283,-12.552017,-12.540651,-12.387489,-12.678446,-12.472812,-12.37277,-12.585406,-12.626499,-12.370838,-12.53841,-12.592586,-12.633451,-12.996637,-13.731991,-13.678908,-13.853673,-14.077131,-13.855877,-14.28274,-14.396111,-13.696102,-14.480595,-14.08683,-13.832261,-14.38861,-14.160207,-14.041822,-13.743073,-13.776165,-13.927037,-13.092523,-13.285939,-12.660943,-12.345284,-12.811302,-12.628438,-12.426687,-12.221324,-12.344438,-12.450333,-12.328874,-12.480881,-12.211601,-12.391928,-12.323601,-12.468095,-12.360558,-12.395299,-12.607329,-12.211076,-12.722373,-12.770431,-12.776025,-12.946906,-13.352395,-13.78058,-14.274702,-14.054046,-14.068481,-14.12993,-14.390289,-14.030956,-14.338601,-13.833404,-14.049861,-14.166022,-14.202726,-13.792835,-13.837015,-13.714439,-14.020139,-13.828403,-13.396273,-12.823261,-12.581751,-12.428928,-12.288293,-12.401411,-12.352224,-12.308043,-12.424193,-12.643168,-12.587066,-12.419173,-12.258269,-12.145176,-12.436127,-12.413104,-12.285249,-12.46423,-12.255534,-12.568711,-12.579824,-12.740988,-11.928169,-12.861052,-13.157843,-13.491308,-13.850345,-14.242727,-13.888419,-14.059337,-14.076544,-13.902903,-14.081588,-14.146019,-13.952029,-14.157126,-13.704443,-13.81866,-14.010403,-13.920104,-14.010693,-13.397391,-13.337084,-13.262324,-12.870782,-12.110176,-12.383889,-12.439226,-12.413073,-12.014851,-12.659288,-12.695992,-12.177428,-12.234944,-12.169637,-12.455031,-12.674557,-12.189362,-12.275253,-12.39252,-12.418093,-12.291929,-12.701808,-12.516208,-12.685108,-12.993562,-13.829212,-13.812795,-14.345282,-13.910658,-13.582416,-14.0735,-14.085434,-14.068783,-13.935372,-13.882313,-14.321938,-14.22912,-13.90257,-14.002365,-13.778085,-13.974854,-14.049039,-13.864792,-13.43849,-12.665123,-12.80435,-12.489494,-12.210767,-12.578157,-12.6376,-12.181015,-12.507015,-12.356101,-12.117399,-12.42005,-13.497402,-12.392218,-12.613991,-12.179651,-12.478381,-12.624826,-12.462539,-12.307469,-12.699604,-12.808493,-12.679551,-13.068649,-13.233974,-13.534957,-14.355827,-14.336095,-13.856457,-14.323593,-14.146038,-13.865909,-14.351678,-14.307207,-14.065166,-13.96818,-14.01236,-14.045144,-14.328871,-14.279665,-13.96676,-13.827563,-13.77698,-12.903843,-12.446443,-12.670969,-12.128833,-12.386402,-12.139631,-12.448382,-12.704296,-12.42836,-12.39278,-12.558716,-12.4003,-12.411678,-12.581466,-13.552158,-12.507009,-12.60594,-12.465058,-12.768758,-12.725442,-12.324459,-12.792682,-13.390433,-13.556084,-14.095152,-14.027363,-13.762515,-14.160188,-14.216025,-15.324876,-14.073222,-13.843134,-13.840065,-14.207437,-14.078779,-13.900915,-14.050157,-14.342503,-14.05793,-14.242196,-13.629992,-12.929934,-13.164505,-12.28189,-12.678193,-12.482011,-12.269691,-12.512307,-12.520339,-12.62732,-12.494754,-12.673458,-12.741821,-12.738222,-12.643428,-12.342209,-12.680397,-12.451432,-12.713755,-12.561451,-12.610113,-12.692084,-12.533971,-12.918265,-12.973892,-13.447942,-14.142944,-14.432259,-14.136289,-14.331631,-14.221353,-14.234423,-14.373336,-14.02598,-14.45835,-14.128257,-14.197701,-13.963179,-14.455041,-14.067944,-14.338348,-13.925111,-13.750556,-13.470459,-12.633994,-12.447839,-12.747088,-12.645971,-12.75599,-12.735715,-12.580084,-12.506454,-12.661505,-12.535384,-12.502836,-12.539546,-12.062945,-12.562031,-12.698493,-12.716792,-12.370282,-12.623974,-12.741,-12.363046,-12.690677,-13.203672,-13.396526,-13.991801,-14.197695,-13.815326,-14.332773,-14.262743,-14.027647,-13.980651,-14.290538,-14.194373,-14.271343,-14.469772,-14.429191,-14.378071,-14.296057,-13.92595,-14.336095,-13.980935,-13.783945,-13.301794,-12.600383,-12.392255,-12.757398,-12.236327,-12.435028,-12.230783,-12.554789,-12.437257,-12.695998,-12.64457,-12.787687,-12.747396,-12.683163,-12.443912,-12.6832,-12.301653,-12.772116,-12.617331,-12.792707,-12.446135,-12.941078,-12.896879,-14.198812,-13.580218,-13.75807,-13.729454,-13.977348,-13.959296,-14.149637,-14.026517,-14.243313,-14.105426,-13.820889,-13.946225,-14.114619,-13.724194,-13.529932,-13.614699,-13.840615,-13.561351,-13.342634,-13.138118,-12.450296,-12.532014,-12.417821,-12.540089,-12.116572,-12.515634,-12.247434,-12.107681,-12.669,-12.306919,-13.340949,-12.600383,-12.434231,-12.343055,-12.371665,-12.151566,-12.224955,-12.579262,-12.222732,-12.685682,-12.817396,-12.94498,-13.316803,-13.755298,-14.00818,-14.953868,-14.072648,-13.763892,-13.721125,-14.040427,-14.105728,-13.975397,-14.247746,-14.024578,-13.922036,-13.841985,-13.737258,-13.950393,-14.122688,-13.668301,-14.366396,-12.984147,-12.712112,-12.728208,-12.395286,-12.476733,-12.187992,-12.679317,-12.684318,-12.077398,-12.357224,-12.617034,-12.434725,-12.41863,-12.50036,-12.389168,-12.496186,-12.604551,-12.550085,-12.743754,-12.534261,-12.447802,-12.98803,-13.220897,-13.590238,-13.801732,-14.116582,-14.133239,-13.757804,-14.369724,-14.652347,-14.200504,-14.055127,-14.002636,-14.218828,-14.072117,-13.987881,-14.083521,-13.942898,-13.856994,-13.830051,-13.499914,-13.261756,-13.160622,-12.674316,-12.610651,-12.574811,-12.443918,-12.520314,-12.358607,-12.179675,-12.405584,-12.199938,-12.080455,-12.529223,-12.222461,-12.443924,-12.771839,-12.74681,-12.509775,-12.682089,-12.871609,-12.579818,-12.813259,-12.67263,-13.310406,-13.598289,-14.193262,-14.439464,-14.474501,-14.209382,-14.337212,-14.220772,-14.201868,-14.471976,-14.185748,-13.993468,-14.41225,-14.419196,-14.337749,-14.268596,-14.283857,-13.990918,-13.409028,-13.200079,-13.136154,-12.781563,-12.462514,-12.458662,-12.675952,-12.681515,-12.730968,-12.532273,-12.510646,-12.410845,-12.772672,-12.714872,-12.775728,-12.717953,-12.768777,-12.534767,-12.485913,-12.759349,-12.688442,-12.603699,-12.438349,-12.947758,-13.07615,-13.752235,-14.277208,-14.190767,-14.047076,-14.462271,-13.969032,-14.469494,-14.215222,-13.931482,-14.179654,-14.420578,-14.301089,-14.261613,-14.138524,-13.835892,-13.882295,-13.704727,-13.508842,-13.13671,-13.027506,-12.341666,-12.722089,-12.700431,-12.459193,-12.477572,-12.197734,-12.486981,-12.261091,-12.752947,-12.478671,-12.769073,-12.476436,-12.717947,-12.486407,-12.669315,-12.546491,-12.394447,-12.692671,-12.608996,-12.398602,-12.973583,-14.533974,-13.932624,-14.337225,-13.997629,-14.457529,-13.947331,-14.438612,-14.141012,-13.946491,-14.164096,-14.414997,-14.161299,-14.113482,-14.208838,-14.078785,-15.293444,-14.060171,-13.85479,-13.105593,-13.138636,-12.569526,-12.314723,-12.767924,-12.659017,-12.775191,-12.469503,-12.449771,-12.460582,-12.636766,-12.412802,-13.517417,-12.68959,-12.491451,-12.450339,-12.254417,-12.438362,-12.580374,-12.766572,-12.907726,-12.638452,-12.959957,-13.253699,-13.290391,-13.810585,-14.224687,-14.06653,-14.450868,-14.440045,-14.201893,-14.309158,-14.200788,-14.462555,-13.915368,-13.828952,-14.255778,-14.374441,-13.817549,-14.03513,-13.843967,-13.907034,-15.71669,-13.162004,-12.556468,-12.545615,-12.555086,-11.852292,-12.592314,-12.533415,-12.322755,-12.287225,-12.332195,-12.091278,-12.485888,-12.497563,-12.304123,-12.754879,-12.778772,-12.523957,-12.605958,-12.447264,-12.638155,-12.836035,-12.852982,-12.845191,-13.777802,-13.516893,-14.041001,-14.027338,-14.247178,-13.950942,-14.552583,-14.494208,-14.192441,-14.168554,-14.009866,-14.045138,-13.756137,-13.902039,-13.939551,-14.171844,-13.736134,-13.704431,-12.872695,-12.814933,-12.51201,-12.626771,-12.444486,-12.536187,-12.524784,-11.810612,-12.533687,-12.782668,-11.820904,-12.295257,-12.679026,-12.485629,-12.318039,-12.237741,-12.551752,-12.308037,-12.384457,-12.672093,-12.188535,-12.641786,-12.874369,-13.444343,-13.1492,-13.658892,-14.289408,-14.196867,-14.261909,-14.239967,-14.224668,-14.464215,-13.820617,-14.066264,-14.97413,-14.062937,-14.2647,-13.795891,-13.94872,-13.948423,-14.288006,-13.691663,-13.378517,-13.083343,-12.658474,-12.705173,-12.540367,-12.721552,-12.56063,-12.292188,-12.074015,-12.298869,-12.744581,-12.336128,-12.485061,-12.555086,-12.521431,-12.58151,-12.515628,-12.729869,-12.154924,-12.179101,-12.649583,-12.649028,-12.682922,-13.269264,-13.473255,-13.824476,-14.049873,-14.239381,-14.256612,-13.774758,-15.617444,-14.072383,-14.27719,-13.832576,-14.234127,-14.319685,-14.229397,-13.979571,-13.924246,-13.882313,-14.068191,-13.460463,-13.329015,-12.90914,-12.686219,-12.467256,-12.677631,-12.717947,-12.521759,-12.299986,-12.403899,-12.755725,-12.48035,-12.524259,-12.496711,-12.457272,-12.4981,-12.468367,-12.494198,-12.558697,-12.580923,-12.592295,-12.795472,-12.833541,-12.749341,-13.82839,-13.854204,-14.062955,-14.388653,-14.52146,-14.186304,-14.231614,-14.191595,-14.383906,-14.176314,-14.436717,-14.425888,-14.227718,-14.444453,-14.03629,-14.279159,-14.271639,-14.170776,-13.39268,-13.343746,-13.005533,-12.231598,-12.564254,-12.192721,-12.400306,-11.910938,-12.156591,-12.411407,-12.455297,-12.388335,-13.336497,-12.680977,-12.69874,-12.195752,-12.371949,-12.365553,-12.594568,-12.49702,-12.797423,-12.538126,-12.532298,-14.517286,-13.35542,-13.512688,-13.912849,-14.385282,-14.30638,-14.278307,-14.351375,-14.029561,-14.011508,-14.044304,-14.117971,-14.239949,-14.372237,-14.149094,-14.23438,-13.826427,-14.044045,-13.799762,-14.215494,-13.051127,-12.650923,-12.670408,-12.627314,-12.577312,-12.632364,-12.637044,-12.115177,-12.346389,-12.591221,-12.642329,-12.617602,-12.679841,-12.380309,-13.24868,-12.436423,-12.63429,-12.413913,-14.578692,-12.795182,-12.697647,-12.692356,-13.032235,-13.299559,-13.550238,-14.376392,-14.223273,-13.997074,-14.239671,-15.453231,-13.764503,-14.436414,-14.318882,-14.299706,-14.006779,-14.467556,-13.855883,-14.128794,-13.763367,-13.850623,-13.855895,-13.320692,-13.137562,-12.724571,-12.698758,-12.503675,-12.302752,-12.655936,-12.714885,-12.312501,-12.752959,-12.658202,-12.61178,-12.487277,-12.73403,-12.666531,-12.431712,-12.444474,-12.50562,-12.797948,-12.824095,-12.609823,-12.860218,-12.534261,-13.308727,-13.664146,-14.073766,-14.499759,-14.50258,-14.390011,-14.188835,-14.209635,-14.202134,-13.819512,-14.207986,-14.26136,-14.400569,-14.213012,-14.137394,-14.267466,-14.235232,-14.19136,-13.532148,-13.282062,-12.973867,-12.846598,-12.696245,-12.205217,-12.12295,-12.408912,-12.445313,-12.45697,-12.555363,-12.243544,-13.888141,-12.672896,-12.478665,-12.64402,-12.358052,-12.491723,-12.701814,-12.624832,-12.614021,-12.267752,-12.587319,-12.864108,-12.803258,-13.593838,-14.009854,-14.009292,-13.947046,-14.126837,-13.664708,-14.328328,-13.841442,-13.828403,-13.832842,-13.836725,-13.838361,-14.159342,-13.821463,-13.886746,-13.617737,-14.234133,-13.476855,-13.450202,-13.169493,-12.269413,-12.406967,-12.506744,-12.536743,-12.412524,-13.859525,-12.38029,-12.442554,-11.899528,-12.667358,-12.607619,-12.361941,-12.54091,-12.411147,-12.394459,-12.209366,-12.217176,-12.521734,-12.261091,-12.810209,-12.583411,-14.068499,-13.203123,-13.334293,-13.955375,-14.338898,-14.099073,-13.885894,-14.204381,-14.087947,-13.882023,-14.269682,-14.065178,-14.080156,-14.345257,-13.969847,-14.023757,-14.225242,-13.868119,-13.169253,-13.041681,-13.029729,-12.530606,-12.172409,-12.082362,-12.44477,-12.310778,-12.422797,-12.518122,-12.588431,-12.182719,-13.341776,-12.653201,-12.460341,-12.418389,-12.391422,-12.565921,-12.228542,-12.4581,-12.499206,-12.684009,-12.465582,-12.749878,-13.316241,-13.653033,-14.104604,-15.23591,-14.087392,-14.337768,-14.087392,-14.023479,-14.12517,-14.268571,-14.001797,-14.136838,-14.163522,-14.122688,-13.997889,-14.231879,-13.739202,-13.896217,-16.032089,-13.207568,-12.759892,-12.483968,-12.369177,-12.489797,-12.640409,-12.445301,-12.649843,-12.249971,-12.389168,-12.645687,-12.176323,-12.306635,-12.381957,-12.498119,-12.496174,-12.620677,-12.029316,-12.386112,-12.46754,-12.528951,-12.572292,-13.143933,-12.958031,-13.421833,-13.748358,-13.673586,-14.092948,-14.34446,-14.632893,-13.802016,-14.152415,-14.145735,-14.184365,-14.276109,-13.935649,-13.85061,-15.769211,-14.027369,-13.982898,-14.054053,-13.542434,-12.806036,-12.661246,-12.41558,-12.485067,-12.361916,-12.338598,-12.674297,-12.710983,-12.638452,-12.488679,-11.935948,-12.634006,-12.393595,-12.61675,-12.214675,-12.161043,-12.390576,-12.414197,-12.506157,-12.416136,-12.674859,-12.684855,-12.666802,-13.359575,-13.519936,-14.11213,-13.975082,-14.161602,-13.913714,-13.918431,-14.123219,-13.961253,-14.092127,-14.229126,-13.865619,-14.10295,-13.857815,-13.689447,-13.587756,-14.055158,-13.573001,-13.357347,-13.155621,-12.300264,-12.590962,-12.773246,-12.474775,-12.523407,-12.249379,-12.2933,-12.303567,-12.454766,-12.649009,-12.666802,-12.482579,-12.295269,-12.202438,-12.684293,-12.356119,-12.605384,-12.717934,-12.539805,-12.742939,-12.416963,-13.166709,-13.397106,-13.883974,-14.255229,-13.698603,-14.098245,-13.876201,-15.757536,-13.707796,-13.831163,-13.731429,-14.364729,-14.093214,-13.954813,-14.25718,-14.223835,-13.98901,-13.803374,-13.749729,-13.65972,-13.03668,-12.666784,-12.685688,-12.373326,-12.623702,-12.638717,-12.200222,-12.672884,-12.431416,-12.602878,-12.243822,-12.163549,-12.266363,-12.257473,-12.233018,-12.381963,-12.398096,-12.434213,-12.445344,-12.760479,-12.765146,-12.669012,-14.167961,-13.644136,-13.755032,-15.722796,-13.980404,-14.171029,-14.054898,-13.750587,-14.165195,-14.002068,-14.544791,-14.171573,-14.391962,-14.007347,-14.066561,-14.588434,-14.123781,-14.041273,-13.557152,-13.365663,-13.223145,-12.915777,-12.726547,-12.049869,-12.532298,-12.293886,-12.559839,-12.749607,-12.493927,-12.72572,-13.441275,-12.692893,-12.699586,-12.591493,-12.768227,-12.636482,-12.679292,-12.513973,-12.414493,-12.693171,-12.673488,-13.051115,-13.025037,-13.689996,-13.848097,-14.558398,-14.12517,-14.405601,-13.922036,-14.450596,-14.40862,-14.184933,-14.448645,-14.241054,-14.24966,-14.236071,-14.003451,-13.681927,-14.140203,-13.987881,-14.785746,-13.281229,-12.440862,-12.232752,-12.274395,-12.605106,-12.359725,-12.538157,-12.649034,-12.014598,-12.659579,-12.381414,-12.365571,-11.998762,-12.276636,-12.620424,-12.682101,-12.665938,-12.050147,-14.461999,-12.803542,-12.86717,-12.897175,-12.983591,-13.319834,-13.83812,-14.053201,-14.136301,-14.421412,-14.033197,-14.771552,-14.196892,-13.715007,-14.318882,-14.338311,-14.057646,-14.211882,-14.332502,-14.020954,-13.690836,-14.183013,-14.279128,-13.454616,-13.350407,-13.022758,-13.042243,-12.753749,-12.543417,-12.214922,-12.749063,-12.782674,-12.699845,-12.644305,-12.484783,-12.701518,-12.442264,-12.470065,-13.315105,-12.390026,-12.754607,-12.630963,-12.861866,-12.807413,-12.851322,-12.179107,-13.058085,-13.378492,-13.427118,-14.138518,-14.325556,-14.3828,-14.250796,-14.477804,-13.998191,-13.778919,-14.415855,-14.021529,-13.904261,-14.412806,-14.106852,-14.39834,-14.264706,-14.104308,-14.082934,-13.614415,-13.250353,-12.849642,-12.491729,-12.766017,-12.697925,-12.697085,-12.533983,-12.721818,-12.838801,-12.277192,-12.719324,-12.726553,-12.419186,-12.742081,-12.031811,-12.625419,-12.55866,-12.559537,-12.782958,-12.720157,-12.655374,-12.624258,-12.972182,-13.552473,-13.867866,-14.077396,-14.447818,-14.450312,-14.393049,-14.269682,-14.161849,-14.51173,-14.389468,-14.386412,-14.460314,-14.321926,-14.30638,-13.888969,-14.071247,-14.101585,-14.065703,-13.556053,-13.325705,-12.790175,-12.246891,-12.758509,-12.457544,-12.499477,-12.494767,-12.884667,-12.755169,-12.461446,-12.417796,-12.532582,-12.722917,-12.204655,-12.521178,-12.527575,-12.777679,-12.547319,-12.605687,-12.767671,-12.630654,-12.761287,-13.558011,-13.661374,-14.069611,-14.164374,-14.433914,-14.177432,-14.506994,-14.211351,-13.936736,-14.227428,-13.903132,-14.193274,-14.222705,-14.192706,-13.871447,-14.300255,-13.811165,-14.354734,-13.781142,-13.410177,-13.118658,-13.016362,-12.396416,-12.50007,-12.273037,-12.728498,-12.750983,-12.271907,-12.822996,-12.786848,-13.713056,-12.658461,-12.211588,-12.758491,-12.438652,-12.425057,-12.75988,-12.742926,-12.747637,-12.62151,-12.855761,-12.784329,-13.280111,-13.472409,-14.02877,-14.408644,-14.483373,-14.294427,-13.984843,-14.458381,-14.393648,-14.390845,-14.187989,-14.397229,-14.188248,-14.238022,-14.111278,-14.11239,-14.114069,-14.427252,-14.856894,-13.176192,-13.000804,-12.680971,-12.434182,-12.73211,-12.675409,-12.747396,-12.761547,-12.745155,-12.688473,-12.820477,-12.682935,-12.451173,-12.512282,-13.280395,-12.573724,-12.367794,-12.532588,-12.427526,-12.523129,-12.461156,-12.555351,-12.742655,-13.187293,-13.473255,-13.590806,-14.147136,-14.012348,-14.045162,-14.962165,-14.246351,-14.124077,-13.670555,-13.951486,-14.039606,-14.018756,-14.18631,-13.772263,-14.031796,-13.707536,-14.141599,-13.633598,-13.133919,-12.828237,-12.547843,-12.302468,-12.417537,-12.277754,-12.486166,-12.227159,-12.466157,-12.356113,-12.278847,-12.53231,-12.583726,-12.370856,-12.232999,-12.330275,-12.379173,-12.323577,-12.242445,-12.381698,-12.450049,-12.325268,-12.771283,-13.197307,-13.460216,-13.92453,-14.122114,-13.889277,-14.017929,-14.194114,-13.803361,-14.082934,-14.047082,-14.099894,-14.030141,-13.828662,-14.025968,-13.857019,-13.865347,-13.785303,-13.890339,-13.533303,-13.173963,-12.662351,-12.607335,-12.451975,-12.374993,-12.59261,-12.506731,-12.562031,-12.428354,-12.479505,-12.194659,-12.102668,-12.198284,-12.553696,-12.479782,-12.513967,-12.523129,-12.101575,-12.56121,-12.720145,-12.567032,-12.636507,-12.804104,-12.977454,-13.374319,-14.129615,-13.984016,-14.070975,-14.067697,-14.1374,-14.198818,-14.155471,-14.074587,-13.738085,-14.328581,-13.741666,-14.01625,-14.044853,-14.061276,-13.968174,-13.727793,-13.408207,-13.280654,-12.69682,-12.597871,-12.367201,-12.438374,-12.310537,-12.688738,-12.239957,-12.399213,-12.273537,-12.501718,-12.389477,-12.401689,-12.229116,-12.601229,-12.413351,-12.354718,-12.561198,-12.547874,-12.193548,-12.574255,-12.351946,-13.707518,-13.175871,-13.472681,-13.948991,-14.138789,-14.288025,-14.139339,-14.166881,-13.958715,-14.169085,-13.960969,-14.103771,-14.11907,-14.027641,-13.70974,-13.766417,-14.01875,-13.698072,-13.705567,-13.576884,-12.882456,-12.664573,-12.535348,-12.376944,-12.278841,-12.252175,-12.164642,-12.502002,-12.673458,-12.226085,-13.350148,-12.369171,-12.443937,-12.239686,-12.258603,-12.167426,-12.277742,-12.452272,-12.280785,-12.473102,-12.478375,-12.611762,-13.001113,-13.147564,-13.489375,-14.806015,-13.819222,-13.939545,-14.220229,-14.01265,-13.928975,-13.940095,-13.945954,-14.000105,-14.273862,-14.124608,-13.940934,-13.976762,-14.132387,-13.62054,-14.521725,-13.406262,-12.815766,-12.785736,-12.555339,-12.391409,-12.567557,-12.343327,-12.511738,-12.479202,-12.27329,-12.276655,-12.412814,-12.583695,-12.52287,-12.346951,-12.483369,-12.256596,-12.249138,-12.160203,-12.541182,-12.558123,-12.044053,-12.43225,-13.130863,-13.058351,-13.637734,-14.118489,-14.134344,-14.039309,-14.617063,-14.104611,-14.121848,-14.224681,-14.062653,-13.904255,-14.045706,-13.876176,-13.699152,-14.081539,-14.005705,-13.978737,-13.596338,-13.293447,-13.169215,-12.52145,-12.486722,-12.48921,-12.580917,-12.442832,-12.217731,-12.456723,-12.212187,-12.336962,-12.440584,-12.300789,-12.38084,-12.462563,-12.570107,-12.350816,-12.373875,-12.532847,-12.763226,-12.629012,-12.832985,-12.755997,-12.931632,-13.395186,-13.734745,-14.134634,-14.090756,-14.258569,-14.220211,-14.230515,-14.314153,-14.087929,-14.354197,-14.333872,-14.246919,-14.300521,-14.019022,-13.985417,-14.154909,-14.139382,-13.846461,-13.388488,-13.071446,-12.779902,-12.454778,-12.598432,-12.557592,-12.541207,-12.775173,-12.362762,-12.483678,-12.459754,-12.410857,-12.273309,-12.397812,-12.421396,-12.568977,-12.47059,-12.510343,-12.570952,-12.52203,-12.529785,-12.562846,-12.926075,-13.153355,-13.603839,-14.022337,-14.187989,-14.264712,-14.142932,-14.021257,-14.013459,-13.873398,-14.250518,-14.14295,-13.989863,-14.214383,-14.38222,-13.977046,-13.761434,-14.160207,-13.688873,-13.504372,-13.407392,-12.91992,-12.59203,-12.557049,-12.515042,-12.554801,-12.590419,-12.546479,-12.393891,-12.652905,-12.348599,-12.37724,-12.368628,-12.640656,-12.585646,-12.515344,-12.353038,-12.176854,-12.672637,-12.714866,-12.751854,-12.362775,-13.878979,-13.353747,-13.730874,-13.964019,-14.355561,-14.112124,-14.2733,-14.199948,-13.915109,-13.889253,-14.13908,-14.017096,-14.088213,-14.275504,-14.29831,-14.856869,-14.060443,-13.984831,-14.053775,-13.722224,-13.157004,-12.948017,-12.626233,-12.493137,-12.666814,-12.33945,-12.762985,-12.442251,-12.510615,-12.636803,-13.395711,-12.403911,-12.292769,-12.335011,-12.638742,-12.440325,-12.493945,-12.445585,-12.654837,-12.646243,-12.547868,-12.71599,-13.178402,-13.155324,-13.668894,-13.990702,-14.129911,-14.302459,-14.273596,-13.989869,-13.975397,-14.103228,-14.377756,-14.25384,-14.110445,-14.11376,-14.164096,-14.209369,-14.174925,-14.008724,-15.114753,-13.7064,-13.351525,-12.909115,-12.215768,-12.200191,-12.378074,-12.425304,-12.609836,-12.712674,-12.701265,-12.411141,-12.692634,-12.545639,-12.668457,-12.480616,-12.373344,-12.278013,-12.507281,-12.376407,-12.524784,-12.748242,-12.842153,-12.936058,-13.315111,-13.447658,-13.767516,-14.328044,-14.219136,-14.196577,-14.632621,-14.397803,-13.977651,-14.065993,-14.257464,-14.399748,-14.450046,-14.258884,-14.221606,-14.121854,-13.629177,-14.124608,-13.677784,-13.407386,-12.822718,-13.059166,-12.371665,-12.535891,-12.564248,-12.453099,-12.630944,-12.356082,-12.47864,-12.727936,-12.231623,-12.286082,-12.471985,-12.565099,-12.362762,-12.5412,-12.403936,-12.491149,-12.564797,-12.671241,-12.725726,-12.722657,-12.844067,-13.071125,-13.875343,-14.193286,-14.298564,-14.307769,-14.17466,-14.104629,-14.27301,-14.106555,-14.010699,-14.145186,-14.346936,-13.952887,-14.289963,-14.118224,-14.156305,-14.095998,-13.654428,-13.474083,-13.125048,-12.8941,-12.452549,-12.619825,-12.634,-12.709884,-12.346074,-12.648138,-12.657912,-12.570656,-12.582035,-12.682904,-12.515066,-12.341098,-12.667345,-12.567588,-12.450055,-12.775463,-12.643206,-12.665425,-12.598155,-12.924939,-13.042768,-13.709172,-13.668036,-14.193552,-14.296366,-14.197423,-14.4239,-14.138808,-14.300249,-14.232441,-14.272201,-14.252179,-14.3083,-14.244949,-14.15436,-14.079322,-14.085132,-14.080989,-13.906762,-13.434341,-13.253983,-12.610404,-12.63429,-12.620103,-12.587054,-12.537305,-12.768499,-12.585646,-12.321391,-12.525914,-12.707908,-12.466996,-12.680403,-12.436429,-12.546214,-12.599,-12.321082,-12.671791,-12.637334,-12.76075,-12.29609,-13.383783,-13.20287,-13.496327,-14.043761,-14.179914,-14.357784,-14.223014,-14.094078,-14.133208,-13.924814,-14.094059,-14.477002,-13.926772,-13.895359,-14.170745,-14.233843,-13.923962,-14.184093,-14.132146,-13.72946,-13.34737,-13.121176,-12.373881,-12.557024,-12.695702,-12.520882,-12.36998,-12.586498,-12.187708,-12.326904,-13.48661,-12.100458,-12.202994,-12.043226,-12.262196,-12.324706,-12.152418,-12.536471,-12.345821,-12.461736,-12.40556,-12.351674,-14.449478,-13.105038,-13.41348,-13.729744,-13.863977,-13.806164,-13.783376,-14.030129,-14.039025,-14.175462,-13.99708,-13.877288,-13.691101,-14.408379,-14.189662,-13.905928,-13.668882,-13.860056,-14.719056,-13.348765,-13.144779,-12.390563,-12.068767,-12.434769,-11.946253,-12.255528,-12.412783,-12.557845,-12.343611,-12.181602,-12.333337,-12.216058,-12.737938,-13.449893,-12.291905,-12.377246,-12.137409,-12.034854,-14.156045,-12.323861,-12.309142,-12.703759,-12.712927,-13.229263,-13.418246,-13.950405,-13.932322,-14.166047,-14.920232,-13.964,-14.113797,-13.835898,-13.986232,-14.033172,-13.921487,-13.906478,-13.651372,-13.738375,-14.091547,-14.203004,-13.546867,-13.428235,-12.96134,-12.677341,-12.039022,-12.044905,-12.474226,-12.184929,-12.263869,-12.515103,-12.456451,-12.095185,-12.338579,-12.137681,-12.425001,-12.486444,-12.372208,-12.155183,-12.589542,-12.548412,-12.544818,-12.387514,-12.660388,-12.19716,-12.572595,-13.12924,-13.261491,-13.865631,-14.113797,-13.421277,-14.111019,-14.460314,-13.937847,-14.149624,-14.14242,-14.15854,-14.097924,-13.844794,-14.020399,-13.902304,-13.619416,-13.981509,-13.710561,-13.417369,-12.976361,-12.749051,-12.247465,-12.087141,-12.631778,-12.007078,-12.064328,-12.432262,-12.376931,-12.499761,-13.761675,-12.097402,-12.303036,-11.91066,-12.4956,-12.429755,-12.175761,-12.170205,-12.291102,-12.483678,-12.203815,-12.642329,-13.132277,-13.184786,-13.542428,-14.013743,-13.997907,-14.101826,-14.096819,-13.491882,-13.81616,-13.774758,-13.810875,-14.193274,-14.106278,-13.916208,-13.944534,-13.66527,-13.76115,-13.500451,-13.801423,-13.415455,-12.851865,-12.484765,-12.456729,-12.052931,-12.410301,-12.23829,-13.960117,-12.385828,-12.328602,-12.20355,-12.403918,-12.349458,-12.305802,-12.419457,-12.461452,-12.237735,-12.072089,-12.715977,-12.484481,-12.126,-12.488099,-13.604679,-12.752663,-13.184496,-13.863699,-13.205345,-14.218297,-13.907015,-14.041291,-13.852259,-14.010131,-13.922579,-14.178562,-13.738072,-13.891753,-13.564395,-13.924833,-13.733078,-13.889277,-13.719458,-13.502143,-13.21118,-13.084763,-12.373338,-12.540077,-12.633185,-12.446987,-12.089901,-12.453099,-12.316927,-12.705698,-13.3718,-12.190498,-12.142675,-12.435022,-12.55398,-12.132988,-12.084857,-12.516449,-12.503379,-12.089351,-12.588974,-12.616769,-12.25246,-12.841579,-13.391531,-14.521713,-14.301928,-13.963191,-13.712229,-13.948164,-13.711389,-14.03374,-14.004032,-14.216327,-13.720008,-14.07684,-13.826711,-13.768923,-13.556887,-14.014021,-15.10335,-15.0364,-13.332089,-12.506731,-12.307494,-12.288861,-12.487833,-12.400003,-11.999861,-12.11822,-12.272759,-11.859516,-12.264955,-12.447814,-12.226912,-12.452833,-12.436695,-12.413357,-12.399732,-11.858417,-12.098248,-12.572033,-12.401701,-12.430033,-12.646774,-13.038638,-13.198109,-13.831169,-14.172703,-13.793409,-14.481441,-14.177963,-14.159639,-13.80756,-14.397507,-13.72946,-14.292482,-13.775851,-13.977904,-15.117272,-13.530191,-13.614422,-13.904533,-13.151459,-13.039983,-12.834621,-12.596228,-12.093482,-12.525624,-12.120178,-12.407523,-12.585646,-11.999558,-11.999015,-12.465595,-12.163259,-12.491451,-12.566742,-12.066285,-12.236648,-12.476436,-12.417543,-12.443085,-12.491173,-12.102119,-12.604804,-12.771845,-13.120615,-13.424624,-13.903138,-13.946225,-13.999309,-14.145216,-13.837281,-14.035154,-13.818383,-13.66138,-14.155768,-14.066536,-13.757545,-14.038772,-13.798935,-13.854228,-13.739196,-13.48685,-13.541884,-13.074181,-12.612324,-12.421711,-12.60623,-12.259146,-12.187973,-12.475319,-12.079053,-12.258275,-12.642915,-12.411672,-12.528427,-12.297196,-12.266338,-12.330263,-12.151306,-12.109898,-12.310543,-12.246903,-12.397805,-12.240254,-12.532588,-12.38,-13.278722,-13.601345,-13.586886,-14.248549,-14.168264,-13.957604,-15.716684,-14.031536,-13.78337,-14.18021,-13.924259,-13.952054,-13.860334,-13.890376,-13.641624,-13.6055,-13.68665,-13.27206,-13.183416,-13.040817,-12.547856,-12.258831,-12.388075,-12.535631,-12.548146,-12.198524,-11.883408,-12.492007,-12.178286,-12.541497,-12.330553,-12.387791,-12.259417,-12.528402,-12.35473,-12.201327,-12.383358,-12.349167,-12.518406,-12.306105,-13.400453,-12.817137,-13.302368,-13.305122,-15.500196,-13.616632,-13.633851,-14.026245,-14.047379,-14.513119,-14.473396,-14.299428,-14.273028,-14.301904,-14.017373,-14.909384,-14.18134,-13.710296,-13.911466,-13.588578,-12.868818,-13.147576,-12.766566,-12.560926,-12.305814,-12.565081,-12.089345,-12.273025,-12.556759,-12.594246,-13.051115,-12.083517,-12.325534,-12.527871,-12.294967,-12.087413,-12.319446,-12.733209,-12.395021,-12.708482,-12.922148,-12.441992,-12.811592,-13.393501,-13.540501,-13.659152,-13.75752,-14.141024,-14.184081,-13.834219,-13.945133,-14.09572,-14.171332,-13.717804,-14.285253,-14.114649,-13.688619,-14.022609,-13.827551,-13.815598,-14.85745,-13.883406,-13.223126,-13.044731,-12.526476,-12.463946,-12.16826,-12.132124,-12.265511,-12.185744,-12.284428,-12.287453,-12.233839,-12.221349,-12.337227,-12.357496,-11.972627,-12.645675,-12.455889,-12.302474,-13.937607,-12.477276,-12.901917,-12.672599,-12.840215,-13.30122,-13.582465,-13.865082,-13.915387,-13.947578,-14.37946,-14.035957,-14.192434,-14.281623,-14.182964,-14.328594,-14.021263,-14.128794,-14.050435,-13.639444,-13.95816,-13.958462,-14.252729,-13.695868,-13.289841,-13.310653,-12.722404,-12.684861,-12.77989,-12.506194,-12.625937,-12.355829,-12.37695,-12.393595,-12.377506,-12.600383,-12.380278,-12.473102,-14.038186,-12.53423,-12.49589,-12.337493,-12.449228,-12.77713,-12.629833,-12.502836,-12.992488,-13.412912,-13.560215,-13.751704,-14.056275,-14.454467,-14.096832,-14.095986,-14.153526,-13.856179,-14.205486,-14.108772,-14.059868,-14.007057,-14.227428,-14.139067,-14.094899,-13.916486,-14.005989,-13.694164,-13.52745,-12.983313,-12.499508,-12.534496,-12.68349,-12.733486,-12.364454,-12.273049,-12.363892,-12.726819,-12.735987,-12.737932,-12.611521,-12.657078,-12.703185,-12.624579,-12.31221,-12.360848,-12.784625,-12.842715,-12.834084,-12.758769,-12.533699,-13.114225,-13.938996,-14.181056,-14.387511,-14.311109,-14.003482,-14.154372,-14.339997,-14.217729,-14.314992,-14.366396,-14.513656,-14.14881,-14.310825,-14.251605,-14.340559,-14.133227,-14.010971,-13.48159,-13.214267,-13.086424,-12.63789,-12.380852,-12.543151,-12.627907,-14.363359,-12.333603,-12.664857,-12.596488,-12.494779,-12.703481,-12.505639,-12.672087,-12.670969,-12.711828,-12.590962,-12.548424,-12.784612,-12.876894,-12.849932,-13.326786,-13.146428,-13.339004,-13.908985,-14.012354,-14.278857,-14.338311,-14.341411,-14.290266,-14.238572,-14.131023,-14.369718,-14.402798,-14.346115,-14.221347,-14.342491,-14.221631,-14.174382,-14.141592,-14.09209,-13.592177,-13.390704,-12.855199,-14.550916,-12.665969,-12.749335,-12.76685,-12.620356,-12.820754,-12.720441,-13.594665,-12.806573,-12.778223,-12.537311,-12.707093,-12.729572,-12.603977,-12.593987,-12.712094,-12.884407,-12.868281,-12.765165,-12.94998,-13.281506,-13.427957,-13.868126,-14.478101,-14.356104,-14.360284,-14.429469,-14.303305,-14.256884,-14.231892,-14.45222,-14.386122,-14.27885,-14.363062,-14.440619,-14.108204,-14.136857,-15.10364,-13.970662,-13.585799,-13.060839,-12.790756,-12.640396,-12.694856,-12.57207,-12.468101,-12.777111,-12.62485,-12.649293,-12.715724,-12.732097,-12.688176,-13.721403,-12.683453,-12.750996,-12.763492,-12.726553,-12.656813,-12.47059,-12.787687,-12.547603,-12.930236,-13.341226,-13.606365,-13.890907,-14.133239,-14.295557,-15.247331,-14.525362,-14.308318,-14.244388,-14.224946,-14.406138,-14.35445,-14.4756,-14.483126</t>
+  </si>
+  <si>
+    <t>-8.050701,-8.03376,-8.026524,-8.054054,-8.017918,-8.029296,-8.090727,-8.11407,-8.160183,-8.178242,-8.196868,-9.179803,-8.395026,-8.477256,-8.541712,-8.578706,-8.576779,-8.5954,-8.585114,-8.602327,-8.61428,-8.586219,-8.593986,-8.580947,-8.564518,-8.506193,-8.670135,-8.437268,-8.457537,-8.382783,-8.302775,-8.203011,-8.129925,-8.051257,-8.034606,-8.034304,-8.028469,-8.043756,-8.035446,-8.60458,-8.046281,-8.055159,-8.031254,-8.04462,-8.050961,-8.050708,-8.032667,-8.042626,-8.082355,-8.157701,-8.170475,-8.161319,-8.211618,-8.330533,-8.406966,-8.510348,-8.591757,-8.598425,-8.607334,-8.606754,-8.592887,-8.614545,-8.613718,-8.592325,-8.615947,-8.582607,-8.598197,-8.557017,-8.483942,-8.461735,-8.446164,-8.383641,-8.30719,-8.21744,-8.125467,-8.044324,-8.070186,-8.370015,-8.058505,-8.058215,-8.03736,-8.03263,-8.062913,-8.06458,-8.032951,-8.04099,-8.059042,-8.056838,-8.057079,-8.061802,-8.10768,-8.166017,-8.190756,-8.205771,-8.243296,-8.347771,-8.423383,-8.489493,-8.564827,-8.609322,-8.619009,-8.61039,-8.62317,-8.584534,-8.603179,-8.62543,-8.625133,-8.612594,-8.580657,-8.551738,-8.476972,-8.461723,-8.445312,-8.35944,-8.303041,-8.217989,-8.097413,-8.023197,-8.034581,-8.050695,-8.043478,-8.049578,-8.038477,-8.047349,-8.030982,-8.020956,-8.048497,-8.051541,-8.041527,-8.028735,-8.017084,-8.044583,-8.11712,-8.153237,-8.177149,-8.171321,-8.233578,-8.340554,-8.419203,-8.495599,-8.576471,-8.606235,-8.570933,-8.610094,-8.603691,-9.491053,-8.589263,-8.600394,-8.585096,-8.607877,-8.552034,-8.508694,-8.464513,-8.452246,-8.44919,-8.361113,-8.287489,-8.17797,-8.094592,-8.061827,-9.024727,-8.050967,-8.02487,-8.026247,-8.02374,-8.042107,-8.015942,-8.031278,-8.012065,-8.029296,-8.048769,-8.047645,-8.020171,-8.053788,-8.110187,-9.107259,-8.176044,-8.185484,-8.256076,-8.327483,-8.44672,-8.51646,-8.577878,-8.595085,-8.580916,-8.577298,-8.571494,-8.597857,-8.592319,-8.590072,-8.60592,-8.598444,-8.534531,-8.506168,-8.454481,-8.447831,-8.42392,-8.332762,-8.238011,-8.139883,-8.054325,-8.025987,-8.040163,-8.051282,-8.074045,-9.045292,-8.055721,-8.049071,-8.057394,-8.046812,-8.036545,-8.037637,-8.03681,-8.045435,-8.065136,-8.073489,-8.137716,-8.188287,-8.187422,-8.202153,-8.310289,-8.385845,-8.45532,-8.549546,-8.575909,-8.621781,-8.6354,-8.610396,-8.59038,-8.589288,-8.619848,-8.596764,-8.610378,-8.58207,-8.545354,-9.002482,-8.451134,-8.458117,-8.398613,-8.300812,-8.220243,-8.142149,-8.05485,-8.04291,-8.035149,-8.041515,-8.019869,-8.04044,-8.018776,-8.057653,-8.613458,-8.034884,-8.034847,-8.05322,-8.039064,-8.030142,-8.027617,-8.065161,-8.124368,-8.164097,-8.167975,-8.209642,-8.287501,-8.376683,-8.489795,-8.555362,-8.570105,-8.559807,-8.620404,-8.636783,-8.615675,-8.597048,-8.626232,-8.62567,-8.585948,-8.59677,-8.556202,-8.489795,-8.476719,-8.46142,-8.385024,-8.320569,-8.245531,-8.12464,-8.064889,-8.032951,-8.059042,-8.056011,-8.052115,-8.045713,-8.054017,-8.068223,-8.055727,-8.036538,-8.067939,-8.058493,-8.047658,-8.077416,-8.05072,-8.122399,-8.159362,-8.194096,-8.18023,-8.235517,-8.315549,-8.376128,-8.500069,-8.575656,-8.611773,-8.618157,-8.605667,-8.602864,-8.608161,-8.625405,-8.62067,-8.613705,-8.612069,-8.599271,-8.550929,-8.503952,-8.488128,-8.48088,-8.388377,-8.297454,-8.204672,-8.137148,-8.056542,-8.055986,-8.045398,-8.055431,-8.033205,-8.036254,-8.057647,-8.061821,-8.031519,-8.048479,-8.041539,-8.045694,-8.04044,-8.018492,-8.034859,-8.084892,-8.125751,-8.189651,-8.152694,-8.247741,-8.326965,-8.416406,-8.500044,-8.565648,-8.591757,-8.597604,-8.60011,-8.593702,-8.805454,-8.582638,-8.613162,-8.585071,-8.592603,-8.554251,-8.503952,-8.44614,-8.459778,-8.443929,-8.359186,-8.283852,-8.177698,-8.089597,-8.026518,-8.04517,-8.049071,-8.020721,-8.034291,-8.036551,-8.043206,-8.044305,-8.016251,-8.032908,-8.039588,-8.050417,-8.028204,-8.041811,-8.01459,-8.079898,-9.140327,-8.1816,-8.170469,-8.268023,-8.307227,-8.421969,-8.498963,-8.554831,-8.583194,-8.6101,-8.599826,-8.595665,-8.598728,-8.589004,-8.584836,-8.603438,-8.594826,-8.570389,-8.484782,-8.449788,-8.474212,-8.434199,-8.344455,-8.246871,-8.169388,-8.074354,-8.032927,-8.029037,-8.031513,-8.009299,-9.054738,-8.042663,-8.02821,-8.032359,-8.040971,-8.026524,-8.04433,-8.035705,-8.056826,-8.040984,-8.050701,-8.127418,-8.185508,-8.183823,-8.19133,-9.254,-8.312777,-8.43336,-8.51283,-8.585083,-8.596215,-8.60011,-8.578996,-8.594282,-8.597054,-8.586225,-8.600925,-8.57121,-8.572612,-8.535075,-9.445478,-8.4656,-8.446411,-8.382221,-8.317469,-8.274129,-8.177711,-8.065432,-8.020709,-8.013442,-8.003749,-8.048207,-8.008182,-8.038483,-8.024857,-8.027389,-8.032649,-8.010985,-8.013744,-8.048213,-8.044571,-8.034044,-8.063494,-8.131592,-8.180779,-8.162159,-8.196868,-8.267189,-8.357501,-8.431125,-8.516473,-8.584552,-8.59009,-8.584009,-8.599549,-8.592325,-8.585929,-8.616193,-8.591782,-8.586509,-8.587028,-8.536198,-8.472552,-8.445306,-8.434187,-8.41001,-8.329743,-8.226602,-8.142174,-8.074601,-8.03376,-8.032902,-8.042101,-8.046824,-8.045139,-8.054319,-8.065438,-8.072952,-8.029864,-8.052393,-8.050998,-8.073792,-8.027932,-8.036014,-8.079379,-8.153812,-8.20716,-8.208006,-8.226343,-8.293033,-8.386426,-8.476713,-8.562048,-8.609563,-8.584558,-8.593708,-8.595357,-8.587615,-8.585058,-8.590399,-8.587059,-8.579261,-8.619293,-8.535927,-8.481744,-8.428674,-8.464476,-8.385302,-8.306634,-8.220496,-8.124615,-8.049004,-8.045991,-8.039335,-8.018498,-8.057931,-8.041829,-8.026271,-8.030951,-8.030698,-8.053196,-8.058493,-8.067667,-8.05322,-8.038477,-8.0371,-8.091566,-8.144366,-8.185762,-8.159918,-8.229399,-8.315543,-8.376689,-8.471199,-8.550664,-8.573433,-8.628171,-8.577316,-8.602895,-9.212858,-8.609841,-8.623448,-8.623176,-8.62346,-8.637327,-8.552065,-8.503143,-8.466977,-8.444226,-8.369157,-8.28915,-8.20524,-8.122096,-8.057388,-8.078502,-8.031538,-8.059907,-8.03597,-8.032346,-8.03957,-8.059604,-8.042644,-8.045151,-8.036248,-8.031229,-8.049337,-8.053196,-8.02098,-8.097938,-9.162812,-8.183527,-8.177452,-8.247445,-8.311067,-8.39168,-8.48648,-8.569821,-8.588158,-8.610106,-8.60066,-8.601765,-8.586485,-8.6065,-8.577057,-9.56577,-8.588423,-8.596505,-8.53342,-8.475033,-8.463945,-8.450609,-8.360841,-8.309974,-8.20303,-8.128246,-8.062926,-8.074613,-8.058771,-8.050436,-9.001661,-8.040712,-8.055708,-8.05043,-8.053504,-8.037928,-8.032087,-8.087393,-8.052381,-8.047102,-8.017943,-8.079916,-8.150478,-8.189108,-8.157689,-8.258824,-8.316661,-8.421425,-8.483677,-8.572877,-8.607297,-8.589565,-8.580113,-8.592325,-8.57815,-8.597054,-8.644328,-8.603154,-8.606186,-8.584274,-9.300959,-8.496994,-8.472002,-8.438095,-8.358612,-8.303868,-8.201048,-8.114922,-8.057666,-8.064315,-8.065148,-8.078496,-8.045435,-8.085991,-8.054603,-8.051825,-8.056264,-8.045713,-8.042947,-8.043774,-8.048522,-8.059042,-8.065438,-8.129067,-8.204654,-8.200221,-8.182718,-8.273845,-8.368052,-8.463371,-8.528147,-8.604568,-8.602605,-8.62764,-8.618465,-8.589522,-8.609254,-8.602876,-8.61457,-8.591498,-8.604834,-8.576748,-8.51007,-8.486171,-8.464482,-8.432279,-8.361656,-8.254415,-8.182434,-8.099068,-8.054597,-8.047935,-8.041002,-8.049584,-8.063778,-8.068772,-8.075465,-8.073761,-8.066272,-8.070168,-8.059042,-8.071847,-8.079317,-8.040156,-8.061561,-8.126307,-8.223824,-8.180217,-8.196597,-8.297188,-8.368904,-8.470897,-8.557585,-8.608186,-8.606476,-8.617904,-8.597882,-8.596758,-8.62706,-8.593461,-8.609001,-8.600394,-8.586762,-8.593708,-8.518677,-8.472564,-8.474484,-8.421401,-8.337207,-8.25996,-8.167987,-8.067667,-8.06463,-8.056795,-8.065438,-8.060999,-8.052387,-8.067927,-8.05322,-8.064321,-8.040132,-8.081293,-8.059623,-8.060987,-8.078786,-8.079879,-8.076817,-8.141878,-8.189089,-8.206049,-8.210204,-8.297762,-8.381128,-8.466452,-8.548139,-8.603185,-8.594004,-8.625658,-8.628986,-9.50742,-8.604259,-8.620676,-8.631801,-8.606791,-8.602333,-8.556751,-8.476719,-8.477015,-8.478942,-8.423086,-8.32694,-8.269393,-8.148514,-8.072119,-9.010551,-8.054054,-8.04683,-8.065161,-8.050701,-8.052097,-8.058209,-8.054319,-8.061271,-8.052702,-8.042657,-8.061567,-8.040977,-8.048769,-8.10184,-9.098955,-8.181625,-8.194374,-8.219687,-8.323044,-8.426149,-8.48785,-8.562314,-8.624837,-8.610106,-8.597906,-8.595918,-8.610686,-8.603981,-8.607612,-8.621497,-8.620651,-8.623466,-8.56482,-8.481998,-8.47199,-8.456703,-8.39389,-8.304449,-8.232442,-8.153275,-8.07515,-8.052634,-8.035396,-8.044855,-9.041952,-8.041533,-8.084034,-8.070723,-8.074619,-8.059055,-8.370837,-8.049874,-8.065963,-8.050146,-8.049071,-8.079077,-8.171574,-8.210235,-8.180773,-8.233288,-8.33859,-8.399446,-8.488369,-8.609297,-8.574285,-8.610952,-8.623732,-8.600364,-8.601771,-8.612045,-8.622059,-8.613446,-8.614286,-8.594566,-9.019442,-8.494228,-8.467014,-8.452011,-8.364724,-8.306375,-8.22107,-8.132117,-8.039323,-8.057382,-8.075169,-8.048485,-8.057647,-8.067383,-8.380283,-8.644581,-8.064895,-8.035711,-8.061543,-8.046522,-8.087381,-8.060413,-8.055437,-8.10463,-8.152435,-8.186879,-8.200795,-8.237746,-8.353599,-8.431995,-8.498105,-8.592609,-8.615366,-8.611798,-8.597073,-8.594554,-8.599555,-8.616761,-8.62317,-8.612884,-8.603167,-8.57121,-8.523116,-8.463933,-8.440626,-8.430334,-8.339152,-8.278031,-8.200215,-8.097401,-8.059363,-8.05348,-8.050714,-8.021536,-8.04709,-8.025135,-8.039335,-8.048503,-8.026802,-8.016251,-8.029852,-8.050442,-8.041811,-8.020968,-8.030426,-8.085714,-8.15104,-8.173247,-8.177427,-8.258293,-8.346672,-8.420573,-8.479219,-8.575088,-8.580373,-8.595375,-8.606507,-8.586762,-8.60621,-8.557572,-8.593696,-8.590387,-8.58149,-8.553152,-8.520066,-8.469218,-8.469483,-8.417808,-8.353618,-8.237462,-8.672925,-8.092412,-8.046799,-8.048738,-8.088794,-8.052936,-8.036551,-8.053764,-8.044071,-8.055974,-8.049609,-8.047102,-8.043496,-8.045978,-8.048775,-8.018776,-8.066834,-8.088245,-8.161319,-8.183792,-8.159374,-8.234986,-8.36946,-8.435033,-8.523394,-8.586201,-8.5979,-8.575106,-8.598709,-8.777709,-8.59009,-8.597876,-8.584824,-8.622614,-8.604284,-8.528962,-8.462266,-8.46255,-9.010273,-8.413912,-8.341115,-8.247464,-8.209124,-8.082096,-8.067636,-8.048769,-8.055955,-8.073773,-8.052943,-8.067081,-8.061271,-8.080447,-8.068192,-8.03405,-8.069606,-8.065173,-8.05961,-8.03405,-8.062092,-9.201479,-8.19885,-8.199387,-8.200505,-8.316951,-8.370553,-8.45282,-8.557048,-8.622349,-8.602599,-8.60705,-8.634264,-8.622627,-8.61289,-8.597629,-8.601216,-8.604549,-8.608982,-8.552571,-8.51617,-8.48535,-8.488418,-8.400311,-8.30969,-8.24437,-8.163239,-8.073483,-8.063765,-8.065722,-8.050417,-9.044471,-8.062673,-8.056276,-8.082688,-8.057925,-8.044879,-8.043515,-8.065704,-8.062401,-8.070723,-8.060147,-8.078756,-8.158257,-8.182428,-8.177674,-9.202022,-8.284698,-8.374454,-8.479219,-8.517584,-8.581484,-8.598153,-8.603154,-8.61649,-8.58341,-9.157558,-8.578459,-8.598444,-8.601734,-8.603136,-9.490164,-8.465594,-8.451986,-8.447251,-8.369713,-8.302467,-8.224126,-8.14991,-8.043762,-8.030963,-8.042632,-8.05819,-8.055437,-8.041521,-8.047108,-8.043478,-8.029883,-8.03794,-8.034878,-8.030167,-8.05351,-8.035409,-8.021258,-8.083775,-8.131036,-8.189947,-8.187151,-8.252711,-8.306103,-8.372491,-8.48172,-8.570649,-8.564796,-9.141185,-8.604803,-8.608989,-8.565104,-8.606494,-8.580107,-8.594838,-8.587324,-8.581484,-8.517294,-8.479775,-8.458129,-8.433662,-8.376387,-8.296651,-8.199943,-8.145199,-8.051245,-8.040416,-8.044052,-8.044589,-8.048213,-8.044021,-8.043212,-8.027395,-8.030136,-8.039045,-8.047658,-8.02266,-8.048182,-8.026006,-8.034878,-8.086831,-8.132697,-8.167166,-8.180483,-8.246889,-8.33554,-8.404774,-8.484801,-8.59177,-8.595394,-8.589004,-8.60371,-8.598184,-8.577619,-8.582577,-8.569537,-8.606803,-8.587324,-8.550639,-8.514238,-8.468113,-8.451159,-8.441441,-8.363638,-8.268294,-8.17576,-8.111033,-8.050417,-8.034606,-8.017924,-8.022369,-8.05209,-8.045163,-8.007101,-8.060141,-8.040724,-8.027667,-8.025401,-8.029593,-8.0407,-8.039033,-8.051251,-8.095462,-8.160479,-8.74211,-8.167962,-8.225793,-8.33417,-8.423907,-8.51312,-8.59982,-8.571513,-8.546188,-8.607896,-8.60676,-8.59761,-8.572038,-8.596486,-8.624571,-8.627881,-8.580928,-8.530889,-8.472564,-8.46781,-8.44451,-8.366114,-8.261089,-8.183811,-8.101846,-8.179106,-8.040724,-8.027346,-8.038496,-8.030686,-8.047658,-8.031278,-8.029864,-8.017091,-8.040712,-8.027376,-8.019869,-8.028475,-8.60955,-8.048232,-8.825736,-8.184107,-8.181082,-8.178828,-8.261651,-8.355247,-8.4367,-8.523968,-8.586491,-8.595634,-8.606482,-8.590671,-8.598999,-8.585664,-8.589559,-8.617885,-8.605951,-8.582323,-8.540045,-8.470625,-8.456431,-8.448128,-8.406404,-8.330546,-8.25828,-8.173815,-8.083503,-8.025425,-8.030155,-8.069322,-9.047496,-8.054579,-8.038767,-8.042095,-8.049602,-8.05322,-8.033198,-8.043774,-8.049584,-8.022913,-8.032087,-8.072946,-8.113527,-8.168265,-8.198819,-8.180205,-8.285272,-8.374195,-8.441694,-8.524252,-8.577878,-8.595103,-8.597042,-8.623726,-8.597332,-8.596752,-8.589257,-8.605395,-8.586491,-8.598431,-9.530196,-8.492833,-8.482294,-8.444207,-8.392266,-8.310277,-8.243271,-8.142427,-8.058209,-8.039298,-8.033476,-8.053757,-8.043484,-8.015405,-8.337788,-9.023313,-8.072674,-8.034872,-8.044046,-8.060709,-8.051794,-8.064031,-8.054579,-8.069063,-8.137124,-8.184663,-8.209655,-8.215211,-8.33112,-8.381987,-9.424344,-8.555665,-8.620398,-8.602339,-8.621515,-8.602061,-8.593455,-8.577032,-8.578681,-8.579255,-8.600098,-8.582577,-8.519492,-8.467829,-8.445572,-8.444201,-8.395872,-8.290804,-8.210784,-8.142946,-8.061246,-8.045435,-8.597629,-8.059332,-8.066846,-8.050436,-8.053776,-8.042095,-8.078527,-8.050436,-8.09127,-8.056517,-8.03739,-8.056511,-8.06905,-8.090443,-8.16882,-8.199659,-8.191602,-8.222453,-8.326644,-8.377801,-8.498395,-8.567018,-8.633419,-8.633456,-8.621793,-8.615088,-8.590387,-8.611483,-8.617916,-8.618712,-8.611217,-8.600098,-8.55372,-8.482819,-8.484233,-8.473928,-8.378313,-8.292768,-8.226596,-8.162418,-8.069347,-8.032062,-8.047923,-8.060147,-8.06792,-8.067112,-8.06266,-8.086529,-8.048763,-8.055147,-8.070458,-8.048201,-8.074323,-8.072409,-8.039335,-8.083806,-8.178273,-8.192145,-8.206043,-8.253872,-8.332762,-8.412554,-8.53037,-8.573433,-8.613477,-8.596777,-8.608982,-8.653194,-8.621238,-8.582595,-8.609847,-8.607303,-8.603179,-8.589263,-8.543125,-8.465322,-8.798799,-8.45921,-8.376943,-8.28276,-8.213575,-8.132147,-8.055424,-8.05264,-8.072662,-8.055715,-8.044886,-8.050967,-8.063778,-8.051553,-8.059882,-8.074057,-8.044879,-8.046812,-8.065463,-8.068476,-8.052103,-9.091158,-8.171592,-8.206321,-8.177124,-8.228559,-8.344727,-8.425858,-8.515337,-8.6101,-8.608989,-8.62204,-8.601228,-8.623448,-8.628726,-8.617613,-8.61649,-8.615385,-8.928031,-8.604543,-8.522844,-8.476441,-8.464766,-8.450881,-8.371682,-8.294984,-8.202709,-8.099055,-8.065445,-8.041811,-8.056252,-9.033617,-8.05377,-8.0549,-8.059308,-8.056554,-8.081571,-8.024598,-8.030173,-8.041261,-8.062666,-8.044311,-8.029068,-8.114651,-8.153534,-8.170197,-9.169233,-8.264973,-8.357513,-8.41945,-8.510873,-8.571217,-8.576477,-8.593436,-8.59845,-8.575656,-8.593967,-8.599542,-8.564814,-8.59816,-8.575094,-9.516033,-8.508959,-8.461457,-8.440311,-8.439175,-8.321945,-8.250532,-8.169055,-8.094894,-8.043478,-8.007385,-8.047102,-8.046522,-8.025969,-8.016504,-8.081855,-8.026531,-8.032396,-8.039311,-8.059042,-7.989549,-7.966526,-8.026247,-7.961198,-8.117126,-8.104359,-8.132401,-8.171321,-8.266362,-8.268016,-8.991943,-8.428106,-8.550367,-8.846863,-8.603994,-8.580095,-8.607883,-8.580644,-8.577304,-8.580632,-8.587898,-8.581768,-8.532568,-8.474225,-8.44893,-8.480331,-8.407806,-8.306634,-8.225787,-8.14715,-8.075175,-8.043478,-8.039866,-8.026247,-8.05072,-8.04291,-8.041274,-8.037366,-8.028753,-8.032637,-8.036545,-8.054591,-8.02432,-8.049028,-8.042391,-8.063488,-8.101562,-8.153528,-8.196609,-8.212155,-8.267757,-8.368052,-8.449474,-8.531463,-8.583163,-8.59845,-8.614298,-8.599271,-8.609285,-8.590115,-8.595091,-8.60066,-8.600388,-8.583429,-8.556739,-8.455042,-8.449758,-8.444491,-8.399453,-8.293311,-8.21744,-8.143242,-8.067377,-8.047096,-8.001816,-8.030432,-8.051263,-8.023474,-8.038786,-8.042095,-8.041237,-8.044324,-8.049596,-8.019875,-8.035717,-8.02098,-8.0346,-8.076564,-8.124356,-8.154361,-8.193837,-8.230479,-8.293292,-8.379727,-8.489215,-8.543119,-8.584256,-8.567864,-8.599524,-8.605395,-8.573989,-8.595363,-8.599265,-8.585929,-8.598431,-8.607093,-8.50949,-8.468106,-8.466717,-8.455308,-8.36557,-8.284414,-8.213001,-8.132975,-8.082954,-8.018758,-8.045151,-8.060722,-8.022104,-8.02958,-8.049874,-8.038767,-8.061283,-8.033205,-8.046256,-8.043206,-8.052375,-8.054048,-8.050979,-9.069463,-8.142964,-8.19104,-8.199097,-8.211334,-8.328873,-8.414486,-8.512558,-8.585108,-8.597592,-8.58065,-8.606198,-8.627078,-8.613736,-8.602333,-9.597492,-8.577039,-8.584812,-8.563147,-8.515874,-8.4656,-8.454777,-8.446726,-8.369466,-8.292206,-8.192158,-8.151311,-8.020141,-8.020412,-8.030994,-8.974718,-8.042095,-8.017381,-8.038236,-8.048238,-8.038496,-8.023209,-8.067643,-8.05072,-8.052375,-8.05209,-8.054035,-8.101272,-8.181582,-8.203549,-8.214933,-8.280537,-8.36725,-8.411411,-8.508132,-8.575081,-8.606741,-8.604012,-8.607334,-8.622614,-8.615681,-8.613193,-8.621787,-8.60208,-8.599258,-9.551885,-8.536754,-8.468637,-8.498692,-8.457814,-8.355569,-8.273295,-8.180483,-8.112687,-8.068741,-8.045719,-8.032087,-8.070155,-8.060715,-8.046256,-8.082127,-8.069359,-8.044052,-8.059616,-8.05987,-8.012658,-8.053776,-8.044873,-8.034588,-8.109607,-8.137426,-8.158541,-8.169092,-8.259404,-8.339177,-8.733473,-8.473107,-8.57481,-8.587047,-8.562579,-8.608464,-8.596764,-8.604259,-8.579261,-8.587621,-8.605945,-8.602315,-8.545644,-8.48785,-8.445615,-8.487566,-8.414745,-8.349166,-8.243877,-8.15688,-8.087658,-8.031007,-8.015961,-8.049572,-8.038496,-8.039588,-8.043212,-8.03765,-8.042126,-8.057098,-8.050152,-8.036538,-8.036822,-8.057098,-8.024036,-8.065167,-8.092702,-8.154398,-8.187151,-8.165474,-8.256644,-8.345011,-8.410294,-8.505366,-8.603185,-8.600956,-8.562332,-8.596227,-8.593449,-8.579267,-8.578693,-8.568142,-8.585948,-8.616761,-8.53647,-8.494481,-8.480343,-8.463383,-8.400021,-8.3464,-8.229658,-8.154077,-8.081021,-8.026821,-8.02182,-8.038477,-8.045688,-8.035149,-8.030457,-8.036841,-8.062629,-8.05819,-8.041564,-8.034347,-8.057406,-8.038471,-8.059302,-8.064864,-8.11909,-8.196362,-8.171599,-8.228855,-8.2922,-8.393878,-8.443652,-8.545385,-8.576211,-8.594832,-8.63482,-8.617058,-8.619571,-8.593992,-8.608174,-8.588707,-8.631505,-8.614273,-8.556467,-8.506168,-8.461982,-8.450054,-8.390852,-8.282439,-8.254138,-8.146835,-8.186305,-8.052696,-8.031815,-8.029858,-8.031815,-8.060703,-8.039625,-8.025129,-8.038199,-8.032099,-8.039033,-8.056807,-8.025444,-8.033174,-8.019548,-8.829082,-8.132975,-8.173815,-8.183804,-8.211068,-8.273295,-8.394446,-8.473101,-8.540921,-8.579249,-8.610939,-8.589812,-8.586491,-8.584521,-8.614823,-8.598166,-8.603747,-8.60316,-8.596246,-8.5198,-8.471428,-8.448381,-8.467545,-8.385024,-8.311919,-8.22383,-8.130178,-8.038471,-8.033766,-8.033754,-9.009193,-8.029568,-8.06045,-8.042064,-8.041811,-8.023474,-8.065988,-8.028741,-8.032649,-8.042651,-8.066809,-8.050714,-8.078212,-8.130184,-8.195776,-8.218286,-8.253854,-8.327786,-8.389463,-8.48785,-8.590634,-8.637617,-8.591195,-8.602043,-8.59122,-8.614557,-8.609557,-8.609544,-8.598172,-8.608161,-9.610531,-8.509805,-8.48117,-8.469236,-8.47173,-8.397242,-8.321624,-8.228578,-8.132394,-8.065463,-8.049041,-8.055715,-8.066297,-8.054603,-8.051276,-9.014731,-8.052115,-8.053214,-8.064895,-8.050695,-8.040712,-8.02821,-8.054041,-8.065963,-8.107686,-8.140458,-8.189651,-8.205777,-8.259392,-8.320001,-9.37099,-8.482004,-8.598999,-8.593714,-8.582046,-8.578168,-8.598981,-8.590084,-8.608995,-8.572563,-8.591739,-8.604549,-8.576489,-8.496451,-8.480053,-8.42976,-8.472829,-8.345283,-8.234937,-8.173266,-8.109625,-8.045731,-8.065735,-8.033211,-8.039891,-8.049034,-8.06571,-8.042397,-8.049572,-8.032371,-8.024042,-8.029599,-8.03739,-8.02432,-8.066821,-8.031235,-8.096005,-8.174655,-8.19075,-8.197436,-8.250229,-8.326668,-8.429501,-8.528956,-8.599814,-8.59869,-8.624831,-8.62401,-8.604266,-8.64042,-8.598166,-8.615656,-8.611501,-8.598715,-8.582601,-8.503693,-8.465908,-8.468421,-8.461173,-8.363348,-8.286631,-8.193553,-8.096567,-8.044027,-8.049312,-8.051819,-8.061283,-8.051269,-8.042107,-8.053226,-8.068513,-8.04596,-8.069322,-8.048485,-8.055461,-8.03042,-8.061265,-8.042928,-8.090998,-8.157683,-8.186076,-8.203826,-8.27106,-8.344147,-8.434236,-8.505915,-8.579829,-8.590658,-8.611495,-8.591782,-8.621238,-8.573976,-8.59845,-8.574538,-8.578724,-8.591214,-8.587868,-8.476719,-8.466452,-8.456715,-8.400854,-8.326934,-8.254125,-8.171562,-8.075743,-8.047664,-8.01514,-8.036267,-8.058196,-8.055177,-8.065154,-8.025697,-8.044608,-8.02266,-8.060147,-8.048781,-8.039323,-8.049041,-8.042675,-9.02945,-8.115459,-8.179637,-8.206636,-8.190213,-8.291922,-8.352216,-8.451696,-8.528691,-8.586781,-8.573408,-8.600104,-8.604821,-8.600938,-8.593177,-8.600944,-8.56758,-8.580385,-8.609816,-8.537032,-8.475052,-8.468668,-8.448381,-8.4017,-8.313598,-8.224114,-8.134629,-8.069316,-8.051276,-8.044602,-9.001371,-8.032637,-8.029043,-8.039323,-8.024882,-8.029883,-8.049306,-8.024592,-8.048775,-8.05711,-8.021227,-8.037921,-8.083225,-8.120182,-8.170234,-9.18034,-8.214643,-8.286921,-8.37472,-8.447553,-8.556196,-8.585941,-8.614545,-8.602895,-8.580379,-8.584546,-8.581484,-8.594301,-8.570926,-8.583706,-9.565492,-8.533142,-8.47228,-8.439484,-8.432248,-8.408374,-8.308597,-8.220502,-8.138791,-8.072958,-8.042107,-8.024845,-8.030142,-8.064624,-8.021536,-8.061561,-8.046546,-8.055721,-8.041811,-8.069606,-8.067957,-8.03902,-8.067964,-8.063488,-8.101019,-8.165733,-8.176618,-8.218273,-8.239394,-8.315018,-8.986121,-8.498111,-8.557029,-8.633178,-8.635407,-8.628158,-8.61707,-8.614261,-8.603154,-8.59064,-8.593955,-8.617897,-8.595363,-8.538952,-8.474472,-8.472002,-8.463383,-8.412504,-8.293336,-8.214378,-8.130746,-8.087658,-8.040163,-8.065445,-8.043225,-8.067964,-8.062098,-8.065988,-8.057931,-8.044898,-8.048497,-8.045126,-8.044324,-8.058215,-8.05072,-8.04044,-8.11186,-8.176612,-8.199931,-8.216051,-8.247457,-8.347487,-8.403922,-8.556492,-8.573711,-8.59177,-8.588429,-8.576471,-8.59064,-8.607044,-8.555356,-8.582311,-8.58178,-8.577903,-8.578693,-8.510354,-8.438367,-8.462537,-8.440336,-8.348061,-8.283877,-8.21857,-8.114058,-8.049849,-8.036267,-8.030142,-8.06713,-8.058518,-8.052097,-8.028475,-8.049059,-8.045417,-8.022369,-8.039897,-8.035995,-8.044015,-8.0057,-8.041805,-8.099636,-8.138562,-8.148274,-8.195208,-8.218848,-8.31997,-8.413072,-8.490907,-8.569531,-8.609532,-8.602031,-8.600364,-8.614261,-8.608137,-8.602889,-8.625652,-8.616224,-8.602345,-8.569235,-8.520906,-8.474509,-8.681242,-8.445337,-8.366682,-8.29554,-8.188268,-8.122695,-8.051813,-8.060438,-8.04875,-8.041805,-8.02127,-8.021536,-8.035143,-8.044046,-8.032359,-8.044867,-8.024302,-8.02182,-8.02766,-8.033235,-9.027783,-8.127696,-8.157954,-8.174649,-8.176618,-8.249408,-8.33388,-8.417789,-8.502007,-8.597888,-8.606229,-8.557881,-8.585923,-8.560912,-8.579527,-9.584113,-8.570933,-8.598715,-8.59177,-8.559511,-8.501742,-8.476157,-8.448665,-8.438644,-8.337504,-8.25912,-8.166042,-8.070415,-8.057091,-8.036273,-8.987776,-7.967323,-8.033754,-8.041545,-8.042373,-7.994044,-8.022641,-8.03794,-7.991809,-8.024598,-8.032958,-8.039595,-8.003459,-8.120195,-8.096833,-8.118503,-8.112385,-8.202684,-8.308332,-8.356377,-8.530629,-8.558727,-8.569543,-8.503687,-8.575921,-8.532599,-9.149507,-8.596239,-8.607636,-8.590646,-9.551051,-8.55869,-8.484517,-8.434483,-8.440842,-8.411973,-8.313314,-8.245494,-8.139908,-8.056258,-8.034588,-8.040724,-8.021808,-8.034026,-8.032661,-8.035421,-8.038205,-8.03347,-8.031544,-8.042669,-8.01793,-8.037378,-8.035137,-8.038767,-8.053183,-8.11436,-8.161603,-8.165209,-8.217452,-8.258867,-8.648174,-8.459228,-8.531747,-8.597598,-9.150606,-8.603735,-8.607346,-8.618737,-8.608742,-8.616212,-8.632332,-8.606235,-8.586485,-8.523955,-8.454474,-8.463939,-8.480318,-8.371954,-8.321106,-8.237196,-8.126319,-8.074891,-8.04375,-8.009299,-8.024314,-8.018498,-8.026247,-8.03405,-8.030716,-8.025709,-8.048201,-8.039595,-8.025697,-8.050732,-8.041533,-8.031538,-8.067105,-8.114052,-8.162961,-8.16356,-8.175186,-8.313889,-8.37364,-8.460593,-8.542292,-8.606766,-8.601234,-8.598987,-8.595912,-8.579835,-8.586479,-8.582021,-8.577594,-8.570371,-8.575372,-8.523962,-8.501168,-8.464519,-8.454752,-8.387216,-8.284149,-8.208821,-8.117392,-8.061259,-8.0285,-8.038489,-8.045151,-8.021801,-8.031562,-8.049294,-8.038187,-8.050152,-8.024864,-8.034878,-8.04796,-8.05072,-8.031538,-8.045435,-8.104908,-8.116287,-8.768213,-8.19217,-8.221607,-8.328879,-8.400292,-8.500334,-8.599561,-8.587306,-8.589275,-8.62204,-8.610662,-8.64013,-8.627331,-8.593998,-8.604556,-8.609841,-8.58567,-8.52787,-8.461426,-8.4762,-8.486443,-8.408892,-8.284686,-8.213279,-8.253298,-8.033482,-8.030976,-8.021517,-8.023468,-8.029031,-8.038508,-8.02905,-8.039348,-8.036014,-8.009577,-8.022653,-8.03042,-8.027376,-8.569556,-8.805195,-8.065173,-8.157683,-8.17797,-8.19188,-8.239654,-8.327786,-8.384185,-8.496469,-8.57205,-8.579274,-8.581225,-8.592054,-8.573161,-8.600394,-8.605673,-8.584842,-8.576471,-8.605692,-8.551756,-8.520047,-8.446689,-8.44756,-8.433088,-8.35668,-8.259126,-8.160195,-8.086559,-8.025395,-7.940386,-8.934977,-8.019307,-7.995112,-8.029605,-7.981504,-8.001539,-7.957346,-8.037366,-8.013769,-7.961501,-8.01209,-7.958994,-8.002372,-8.021246,-8.13353,-8.098771,-8.095715,-8.162714,-8.339714,-8.386111,-8.418913,-8.520622,-8.598413,-8.598993,-8.563703,-8.578965,-8.469471,-8.50949,-8.582046,-8.539261,-9.583001,-8.587337,-8.441157,-8.423636,-8.410294,-8.421685,-8.277216,-8.216359,-8.100438,-8.082645,-8.032099,-7.982078,-7.955957,-7.997371,-7.997365,-9.526603,-8.034575,-7.965403,-8.005113,-7.94456,-8.030988,-7.979572,-7.989024,-8.015702,-8.003193,-8.057091,-8.132388,-8.182965,-8.129369,-8.214933,-9.175055,-8.374448,-8.497031,-8.522566,-8.526456,-8.549793,-8.522295,-8.538131,-8.600629,-8.561727,-8.511169,-8.56203,-8.559529,-8.536488,-8.453098,-8.462531,-8.382802,-8.350284,-8.339998,-8.187984,-8.150774,-8.034316,-7.958723,-8.493938,-7.95345,-7.917043,-7.98929,-7.935669,-7.940929,-8.011509,-7.991265,-8.024296,-8.022382,-8.02595,-8.024283,-8.045429,-8.025703,-8.002076,-8.093764,-8.101827,-8.192991,-8.238011,-8.290249,-8.40391,-8.506193,-8.451165,-8.586225,-8.560085,-8.507261,-8.500637,-8.54812,-8.460043,-8.577335,-8.558998,-8.521776,-8.522838,-8.495049,-8.428939,-8.457259,-8.337485,-8.249118,-8.138809,-8.132987,-8.041533,-8.009861,-7.941491,-8.019066,-8.023746,-8.052658,-8.000119,-7.962902,-8.028772,-7.928705,-8.042076,-8.023197,-7.926217,-8.013189,-7.962341,-8.006805,-8.149626,-8.166301,-8.074076,-8.113224,-8.253304,-8.323322,-8.447239,-8.427247,-8.498679,-8.53589,-8.556467,-8.558153,-8.572877,-8.539804,-8.571507,-8.626214,-8.514793,-8.595387,-8.505335,-8.404737,-8.879683,-8.428081,-8.344721,-8.294972,-8.149657,-8.041243,-8.043743,-7.962902,-8.0021,-8.026531,-7.934268,-7.989277,-8.025117,-8.020147,-7.935669,-7.962909,-8.027105,-8.019282,-8.042058,-7.990969,-8.866866,-8.022376,-8.086843,-8.102118,-8.144631,-8.191046,-8.268838,-8.35555,-8.412517,-8.538409,-8.522838,-8.503964,-8.538964,-8.53618,-8.57092,-8.552868,-8.566494,-8.527005,-9.235911,-8.572303,-8.50673,-8.453931,-8.437262,-8.433675,-8.376109,-8.282463,-8.193257,-8.116571,-8.052393,-8.027932,-9.021658,-8.028185,-8.039027,-8.032093,-8.010979,-8.036267,-8.03263,-8.022919,-8.023758,-8.042928,-8.041527,-8.00707,-8.05627,-8.09043,-8.15296,-9.15423,-8.174105,-8.224663,-8.315278,-8.388901,-8.488406,-8.574285,-8.591504,-8.579805,-8.587034,-8.596233,-8.59732,-8.600691,-8.596789,-8.583978,-9.547187,-8.516182,-8.465847,-8.456999,-8.38666,-8.420876,-8.326082,-8.181329,-8.095468,-8.033507,-8.020406,-8.005132,-7.994025,-7.95208,-8.004014,-8.036798,-8.010688,-8.025425,-7.991506,-7.961242,-7.970132,-8.041811,-8.043756,-8.018764,-8.000162,-8.039045,-8.134364,-8.172975,-8.175519,-8.252199,-8.83049,-8.419203,-8.431125,-8.571766,-9.075865,-8.604821,-8.586194,-8.619836,-8.615088,-8.631511,-8.59732,-8.608698,-8.590942,-8.590084,-8.519226,-8.47507,-8.456438,-8.448924,-8.367225,-8.28276,-8.19606,-8.108526,-8.02153,-8.032371,-8.027346,-8.045997,-8.039039,-8.028173,-8.031809,-8.044602,-8.029031,-8.038489,-8.046003,-8.003774,-8.022937,-8.058209,-8.052084,-8.093258,-8.139328,-8.154645,-8.17547,-8.242716,-8.913856,-8.451449,-8.521449,-8.570655,-8.609865,-8.633166,-8.584812,-8.614551,-8.61315,-8.622627,-8.612038,-8.619546,-8.588436,-8.583157,-8.510342,-8.472533,-8.479485,-8.437792,-8.345258,-8.283315,-8.148817,-8.060993,-8.02737,-8.057073,-8.032383,-8.035131,-8.057098,-8.071013,-8.067945,-8.03597,-8.054893,-8.053794,-8.054881,-8.067112,-8.047374,-8.047935,-8.079885,-8.132129,-8.190509,-8.180489,-8.207734,-8.291403,-8.367503,-8.456147,-8.527573,-8.617904,-8.60316,-8.613736,-8.595357,-8.596777,-8.592072,-8.602068,-8.592622,-8.590955,-8.59816,-8.545638,-8.465038,-8.483115,-8.478942,-8.398631,-8.318599,-8.222459,-8.170481,-8.085707,-8.070458,-8.058196,-8.05264,-8.067105,-8.071279,-8.069038,-8.039335,-8.049572,-8.06934,-8.051263,-8.069575,-8.030976,-8.364447,-8.997487,-8.089356,-8.149613,-8.199937,-8.194936,-8.220243,-8.29996,-8.380844,-8.463112,-8.552324,-8.623719,-8.607334,-8.624565,-8.602333,-8.605105,-9.603289,-8.60789,-8.582311,-8.594826,-8.593733,-8.553701,-8.509231,-8.44756,-8.450887,-8.422518,-8.321093,-8.233004,-8.145187,-8.07544,-8.056536,-8.998586,-8.046818,-8.057091,-8.043194,-8.056814,-8.046806,-8.046275,-8.213303,-8.065426,-8.071254,-8.050979,-8.053202,-8.074613,-8.086572,-8.162406,-8.177124,-8.184379,-8.251909,-8.314142,-8.376381,-8.480627,-8.55451,-8.600382,-8.639531,-8.650131,-8.600944,-8.616799,-8.620429,-8.60955,-8.59369,-9.585496,-8.595387,-8.559523,-8.483949,-8.469255,-8.476157,-8.396705,-8.2972,-8.188805,-8.11157,-8.041249,-8.051825,-8.045126,-8.041286,-8.04709,-8.059048,-8.037934,-8.029877,-8.019863,-8.025148,-8.040947,-8.04683,-8.042095,-8.023228,-8.037915,-8.087924,-8.140748,-8.178816,-8.179112,-8.227158,-8.612045,-8.430304,-8.509237,-8.559789,-8.593436,-8.580095,-8.572853,-8.585645,-8.56926,-8.580657,-8.593165,-8.605364,-8.558134,-8.576193,-8.494537,-8.476132,-8.449227,-8.459185,-8.36917,-8.29028,-8.154114,-8.105723,-8.011812,-8.007916,-8.044009,-8.037063,-8.02763,-8.040706,-8.055721,-8.043509,-8.058468,-8.04767,-8.060419,-8.043496,-8.054048,-8.044892,-8.051288,-8.110187,-8.161066,-8.199363,-8.178254,-8.267146,-8.352759,-8.412541,-8.513404,-8.575649,-8.619546,-8.6243,-8.617052,-8.601481,-8.589812,-8.64013,-8.618428,-8.593708,-8.585923,-8.576211,-8.501427,-8.463655,-8.484788,-8.440336,-8.397279,-8.268004,-8.202709,-8.099883,-8.056264,-8.041558,-8.054319,-8.057672,-8.075434,-8.050701,-8.049325,-8.056554,-8.047917,-8.047096,-8.062938,-8.045441,-8.017634,-8.019857,-8.051004,-8.112113,-8.146601,-8.154941,-8.160739,-8.268307,-8.328045,-8.427247,-8.518393,-8.575378,-8.582595,-8.590646,-8.585398,-8.5548,-8.559252,-8.603704,-8.574254,-8.590115,-8.578144,-8.554788,-8.491999,-8.454462,-8.452554,-8.42366,-8.328607,-8.229121,-8.154367,-8.067927,-8.042959,-8.031272,-8.046824,-8.021832,-8.028451,-8.017115,-8.05072,-8.012627,-8.028457,-8.032939,-8.050985,-8.029568,-8.024024,-8.149095,-8.05322,-8.113786,-8.172414,-8.171889,-8.164659,-8.260799,-8.359446,-8.455604,-8.525894,-8.577057,-8.598178,-8.586522,-8.587886,-8.592622,-8.595091,-8.578712,-8.576755,-8.595671,-8.607612,-8.578996,-8.511472,-8.459518,-8.472854,-8.416147,-8.339702,-8.234659,-8.170216,-8.080707,-8.062963,-9.0578,-8.058499,-8.038199,-8.035155,-8.056276,-8.054313,-8.051282,-8.058221,-8.061259,-8.053498,-8.042922,-8.052103,-8.062938,-8.086004,-8.143236,-9.161719,-8.16298,-8.189349,-8.277771,-8.350815,-8.44919,-8.520084,-8.594801,-8.620676,-8.596233,-8.573729,-8.576483,-8.58396,-8.604809,-8.583416,-9.533536,-8.577594,-8.557881,-8.488388,-8.454765,-8.480905,-8.391408,-8.308344,-8.22107,-8.122399,-8.084312,-8.048491,-8.02487,-8.014331,-8.036267,-8.051819,-8.041829,-8.02792,-8.024302,-8.05377,-8.014028,-8.035989,-8.043188,-8.030136,-8.029019,-8.07431,-8.135463,-8.166585,-8.19159,-8.220786,-9.318172,-8.393643,-8.480324,-8.596499,-8.574267,-8.60153,-8.571223,-8.590109,-8.580965,-8.580941,-8.588429,-8.602901,-8.592054,-8.573995,-8.521745,-8.454197,-8.457265,-8.443084,-8.390284,-8.297744,-8.20019,-8.130159,-8.072112,-8.043225,-8.037088,-8.039039,-8.036236,-8.040428,-8.039879,-8.030982,-8.057388,-8.037644,-8.032655,-8.053486,-8.043756,-8.040416,-8.039854,-8.076835,-8.135197,-8.159097,-8.152139,-8.209371,-8.304158,-8.386382,-8.502297,-8.578428,-8.598987,-8.587343,-8.608161,-8.563981,-8.561184,-8.595949,-8.580965,-8.59235,-8.573155,-8.552862,-8.527024,-8.467291,-8.437231,-8.433965,-8.355031,-8.282204,-8.192979,-8.112675,-8.039329,-8.053498,-8.040434,-8.020425,-8.038749,-8.009324,-8.051825,-8.056851,-8.030735,-8.021246,-8.039607,-8.040416,-8.034026,-8.019857,-8.028457,-8.078793,-8.130752,-8.163813,-8.198276,-8.242747,-8.333929,-8.405867,-8.501995,-8.561443,-8.600666,-8.613471,-8.597345,-8.595369,-8.619027,-8.583422,-8.624003,-8.590368,-8.625954,-8.568124,-8.548694,-8.475608,-8.467835,-8.428081,-8.384734,-8.284698,-8.194115,-8.116571,-8.050714,-8.050467,-8.046559,-8.052665,-8.076002,-8.047923,-8.079861,-8.051276,-8.056283,-8.052652,-8.067371,-8.039891,-8.050424,-8.40362,-8.047405,-8.121584,-8.152707,-8.151</t>
+  </si>
+  <si>
+    <t>-8.70127,-8.62204,-8.507595,-8.396113,-8.36499,-8.348629,-8.373065,-8.362236,-8.389741,-8.376671,-8.361119,-8.357791,-8.372232,-8.356964,-9.380967,-8.387518,-8.350821,-8.360569,-8.419178,-8.43031,-8.53647,-8.539822,-8.555072,-8.655688,-8.778505,-8.861303,-8.96584,-8.999414,-9.011403,-10.070999,-9.020257,-9.013891,-9.017194,-8.987763,-9.008082,-8.990813,-9.074457,-8.958857,-8.914424,-8.837972,-8.870799,-8.831866,-8.682353,-8.578434,-9.441848,-8.389463,-8.389179,-8.379739,-8.394748,-8.348055,-8.37722,-8.386975,-8.375306,-8.394476,-8.348351,-8.356408,-8.40612,-8.365274,-8.38082,-8.381703,-8.405571,-8.457561,-8.483127,-8.522029,-8.568963,-8.632598,-8.736257,-8.865218,-8.966087,-8.996938,-9.029721,-9.021109,-9.004167,-9.015861,-9.034179,-9.004717,-9.005569,-9.011101,-9.014453,-8.978324,-8.880233,-8.864952,-8.919418,-8.806559,-8.689045,-8.598147,-8.524252,-8.381684,-8.415313,-8.381412,-8.390031,-8.40446,-8.413924,-8.36917,-8.420864,-8.391155,-8.418388,-8.401126,-8.367793,-8.356396,-8.396971,-8.359989,-8.476731,-8.492265,-8.503365,-8.528691,-8.603975,-8.684576,-8.837417,-8.911652,-8.973039,-9.035031,-9.037223,-9.050027,-9.029709,-9.042779,-9.021664,-9.046409,-9.028079,-8.994987,-9.005285,-8.967223,-8.89108,-8.874108,-8.90633,-8.802398,-8.666511,-8.533988,-8.466433,-8.401422,-8.371411,-8.361131,-8.373905,-8.377788,-8.365274,-8.417524,-8.386685,-8.354754,-8.369744,-8.375837,-8.392248,-8.346931,-8.377517,-8.387531,-8.445053,-8.478966,-8.522035,-8.5087,-8.590961,-8.679581,-8.815468,-8.889111,-9.012206,-9.016102,-8.994178,-9.016941,-9.068629,-9.04891,-9.016108,-9.021399,-8.985257,-9.044465,-8.986671,-9.331261,-8.858828,-8.872163,-8.841856,-8.802942,-8.653996,-8.521183,-8.449498,-8.396137,-8.382524,-8.417536,-8.413072,-8.387537,-8.40504,-8.34582,-8.40228,-8.370275,-8.378054,-8.343603,-8.371121,-8.397823,-8.387815,-8.391982,-8.4681,-8.504792,-8.522844,-8.53676,-8.601765,-8.737091,-8.829094,-9.932845,-9.065042,-9.045588,-9.046662,-9.04865,-9.07334,-9.049447,-9.060578,-8.983602,-9.059158,-9.004427,-9.00694,-8.953856,-8.912176,-8.851308,-9.855906,-8.730423,-8.622898,-8.530105,-8.447825,-8.387253,-8.376714,-8.351123,-8.366682,-8.390889,-8.395859,-8.398335,-8.365539,-8.357501,-8.40199,-9.341528,-8.391124,-8.355587,-8.373053,-8.396421,-8.46865,-8.532549,-8.510657,-8.504785,-8.636222,-8.696831,-8.835194,-8.922765,-8.968908,-9.033617,-9.084187,-9.035309,-9.013046,-9.052793,-9.032783,-9.051682,-9.026424,-8.994444,-8.945238,-8.920239,-8.875226,-8.939971,-8.826334,-8.715402,-8.658997,-9.528813,-8.406423,-8.366669,-8.411411,-8.387222,-8.40475,-8.392248,-8.383339,-8.399761,-8.395279,-8.400873,-8.398619,-8.392507,-8.37364,-8.418073,-8.381406,-8.422234,-8.455326,-8.487548,-8.520368,-8.538396,-8.613736,-8.78242,-8.846048,-8.957196,-9.06474,-9.020578,-8.979422,-9.015552,-9.018614,-9.055571,-9.052781,-8.986399,-9.005841,-9.059442,-8.988881,-8.889129,-8.860223,-8.891605,-8.807961,-8.743215,-8.576779,-8.467582,-8.4042,-8.375269,-8.366663,-8.376973,-8.365033,-8.356099,-8.381406,-8.383901,-8.39836,-8.393896,-8.982207,-8.3586,-8.371127,-8.40057,-8.382783,-8.411671,-8.457586,-8.502026,-8.560672,-8.564567,-8.674024,-8.804386,-8.854957,-8.973316,-9.031962,-9.025579,-9.005822,-9.038649,-8.999716,-9.001105,-9.010835,-8.993882,-9.018355,-9.027233,-8.922758,-8.90273,-8.881332,-8.900224,-8.798243,-8.660127,-8.595387,-8.490616,-8.433681,-8.397792,-8.370003,-8.3586,-8.361668,-8.411121,-9.038334,-8.378937,-8.389457,-8.399212,-8.362261,-8.377776,-8.350833,-8.377776,-8.376387,-8.422543,-8.470601,-8.547305,-8.499198,-8.569803,-8.672617,-8.752124,-8.85884,-9.009996,-9.034753,-9.066425,-9.06169,-9.064468,-9.034988,-9.056701,-9.031666,-9.031962,-9.093942,-8.991085,-9.632485,-8.928556,-8.891889,-8.904953,-8.821309,-8.660979,-8.559548,-8.480047,-8.377245,-8.390568,-8.373627,-8.387234,-8.392538,-8.366385,-8.357501,-9.368458,-8.382511,-8.377233,-8.351957,-8.386969,-8.365564,-8.406151,-8.38616,-8.422802,-8.48172,-8.49897,-8.505619,-8.591745,-8.709889,-8.81019,-9.896216,-9.026147,-9.003618,-9.033049,-9.01194,-9.000834,-9.041686,-9.066123,-9.008038,-9.004735,-8.973045,-9.01194,-8.978608,-8.885764,-8.856062,-8.89492,-8.743796,-8.664881,-9.19954,-8.451449,-8.382561,-8.347771,-8.356674,-8.377523,-8.361094,-8.376677,-8.385296,-8.368626,-8.383351,-8.416165,-9.38519,-8.396964,-8.396674,-8.401984,-8.38808,-8.460049,-8.487252,-8.545058,-8.541483,-8.623454,-8.700696,-8.843245,-8.925247,-9.001661,-9.059479,-9.060017,-9.009446,-9.044199,-9.046953,-9.067246,-9.033629,-9.042236,-9.02748,-9.0203,-8.941083,-8.91246,-9.25037,-8.893284,-8.75936,-8.641827,-9.272022,-8.470903,-8.43168,-8.402533,-8.385018,-8.36194,-8.370559,-8.383079,-8.400323,-8.380851,-8.3875,-8.393353,-8.395285,-8.400323,-8.385024,-9.231472,-8.385006,-8.466989,-8.468668,-8.485881,-8.530901,-8.649279,-8.751853,-8.815481,-8.905527,-8.976904,-8.980521,-9.036395,-9.00752,-8.997247,-9.01946,-9.05554,-8.977225,-9.011082,-9.026696,-9.033919,-8.920511,-8.888296,-8.867453,-8.820488,-8.752421,-8.632616,-8.497556,-8.42363,-8.356951,-8.371689,-8.397551,-8.370849,-8.363916,-8.378356,-8.360841,-8.351938,-8.40141,-8.387512,-8.406139,-8.395014,-8.355285,-8.36557,-8.391945,-8.455302,-8.496722,-8.484504,-8.522566,-8.656528,-8.719878,-8.816043,-8.946355,-9.042217,-9.018874,-9.01917,-9.012237,-9.023905,-9.693063,-8.976657,-9.056133,-9.027764,-9.046965,-9.00639,-8.923851,-8.922178,-8.883023,-8.889938,-8.747123,-8.638759,-8.507848,-8.447541,-8.39865,-8.387555,-8.384753,-8.381962,-8.415863,-8.405299,-8.382234,-8.406991,-8.351963,-8.389729,-8.40946,-8.383647,-8.406127,-8.416956,-8.446164,-8.479787,-8.524258,-8.529234,-8.548416,-8.667906,-8.741005,-8.912726,-8.950806,-9.018633,-9.671659,-9.020294,-9.007508,-8.988325,-9.020028,-9.020553,-9.031666,-9.02945,-9.01031,-9.011119,-8.867718,-8.871608,-8.905786,-8.775159,-8.713753,-8.615971,-8.460056,-8.387259,-8.386117,-8.396958,-8.344455,-8.377795,-8.379727,-8.407263,-8.408065,-8.380011,-8.373053,-8.413912,-8.373349,-8.377239,-8.361119,-8.36917,-8.421697,-8.496173,-8.502847,-8.527845,-8.529265,-8.678186,-8.78434,-9.829784,-8.976928,-9.01165,-9.031394,-9.011669,-9.028894,-9.013052,-9.00944,-9.064733,-9.015268,-9.011101,-9.00247,-8.941922,-8.882721,-8.862446,-8.889388,-8.803794,-8.689867,-8.593165,-8.449486,-8.38529,-8.38558,-8.376961,-8.402521,-8.380301,-8.359742,-8.395298,-8.343622,-8.392513,-8.392217,-9.345701,-8.349722,-8.398891,-8.354173,-8.409195,-8.431131,-8.472836,-8.87496,-8.509774,-8.604846,-8.710969,-8.826001,-8.915245,-8.997506,-9.046965,-9.987355,-9.007761,-9.008322,-9.01833,-9.055294,-9.038933,-9.037525,-9.093102,-9.046971,-8.964426,-8.910232,-8.881906,-8.871885,-8.801861,-8.654268,-9.529943,-8.450035,-8.392235,-8.417233,-8.359724,-8.364465,-8.402527,-8.380875,-8.402256,-8.378893,-8.409207,-8.38666,-8.371682,-8.413356,-8.383913,-8.695151,-8.387216,-8.466717,-8.498093,-8.544261,-8.567883,-8.646785,-8.729627,-8.782938,-8.930247,-9.010002,-9.047508,-9.050854,-9.064999,-9.012218,-9.035006,-9.050861,-9.034444,-9.03529,-9.046156,-9.051972,-8.972458,-8.898569,-8.899094,-8.822414,-8.790464,-8.642352,-8.574279,-8.427815,-8.422531,-8.443096,-8.390309,-8.372516,-8.410047,-8.369738,-8.42613,-8.37698,-8.379184,-8.371398,-8.418647,-8.348049,-8.407244,-8.393081,-8.391136,-8.451702,-8.492012,-8.501711,-8.578712,-8.598153,-8.702369,-8.819654,-8.917455,-8.993332,-9.048916,-9.017793,-8.991943,-9.011959,-9.032234,-8.99303,-9.010551,-9.004742,-9.01528,-8.998315,-8.911615,-8.881603,-8.878288,-8.846313,-8.733775,-8.633178,-8.538137,-8.416122,-8.399193,-8.374454,-8.396143,-8.382246,-8.38695,-9.015842,-8.403892,-8.340276,-8.401675,-8.398638,-8.346116,-8.353611,-8.3956,-8.374714,-8.40057,-8.461439,-8.49813,-8.5234,-8.569253,-8.615959,-8.738208,-8.851598,-8.937458,-9.00944,-9.038334,-9.02777,-9.038352,-9.021102,-9.011934,-9.025566,-9.018349,-9.003031,-9.040581,-9.429074,-8.929667,-8.888271,-8.859365,-8.785753,-8.705406,-8.595091,-8.516448,-8.396711,-8.351099,-8.741277,-8.390556,-8.36194,-8.365842,-8.394464,-8.377233,-8.3875,-8.398897,-8.392525,-8.426426,-8.380838,-8.350024,-8.378912,-8.40475,-8.475632,-8.549262,-8.527024,-8.541736,-8.658466,-8.801287,-9.851455,-8.991091,-9.025029,-9.040291,-9.004705,-9.030561,-8.996672,-9.051978,-9.025307,-9.00752,-9.047255,-9.025825,-8.971668,-8.92579,-8.893556,-9.86618,-8.841028,-8.765991,-8.622065,-8.508373,-8.378344,-8.386123,-8.400298,-8.392488,-8.353889,-8.389488,-8.402552,-8.412535,-8.371127,-8.369447,-9.294014,-8.370046,-8.373658,-8.382783,-8.370559,-8.404194,-8.522881,-8.535643,-8.505637,-8.552584,-8.664294,-8.745432,-8.872731,-8.983627,-9.03863,-9.083372,-9.039464,-8.998068,-9.022757,-9.070586,-9.028628,-9.017503,-9.035006,-9.017787,-8.924135,-8.899927,-9.185087,-8.928043,-8.796014,-8.718242,-9.667775,-8.504261,-8.38111,-8.399181,-8.355853,-8.391124,-8.401972,-8.398082,-8.367503,-8.410028,-8.422833,-8.423389,-8.399737,-8.376949,-8.424475,-8.402793,-8.396693,-8.442824,-8.489505,-8.508107,-8.536742,-8.619003,-8.682649,-8.805491,-8.878856,-8.961666,-8.980244,-9.014169,-9.047811,-9.014706,-9.011125,-9.038636,-9.028894,-9.02945,-9.637214,-9.002223,-8.906342,-8.866866,-8.906626,-8.887987,-8.756569,-8.69625,-8.533698,-8.483103,-8.358057,-8.410035,-8.341381,-8.391667,-8.358075,-8.405861,-8.371652,-8.387815,-8.357779,-8.386123,-8.399749,-8.369731,-8.404762,-8.3672,-8.382795,-8.468946,-8.492549,-8.538693,-8.501452,-8.586479,-8.695973,-8.841319,-8.880776,-8.990295,-9.019985,-8.996104,-9.058899,-9.05141,-9.038612,-9.003877,-9.013885,-9.015842,-9.037253,-8.985837,-8.918319,-8.867162,-8.909139,-8.837694,-8.797663,-8.610081,-8.511743,-8.444226,-8.392241,-8.391414,-8.354155,-8.365262,-8.389192,-8.395032,-8.378369,-8.393649,-8.388901,-8.370009,-8.351413,-8.389179,-8.390575,-8.382518,-8.360551,-8.43978,-8.525079,-8.551763,-8.528956,-8.600141,-8.72378,-8.801589,-8.930778,-9.005847,-9.407959,-9.048323,-9.042804,-9.015287,-9.028635,-9.022245,-9.055294,-9.089497,-9.031407,-9.658607,-8.934155,-8.916362,-8.888851,-8.870762,-8.75652,-8.645402,-8.563431,-8.465612,-8.365564,-8.396693,-8.391143,-8.400008,-8.431693,-8.412825,-9.377349,-8.390303,-8.394452,-8.369194,-8.346406,-8.364743,-8.36641,-8.359705,-8.388358,-8.458123,-8.50089,-8.483677,-8.507842,-8.629017,-8.74713,-9.82395,-8.903582,-9.004705,-9.027789,-9.011082,-8.984423,-9.03195,-9.054151,-9.025017,-9.032765,-9.011101,-9.005279,-8.996672,-8.941891,-8.854389,-8.882184,-8.834101,-8.722397,-8.637074,-8.525363,-8.396403,-8.390871,-8.418647,-8.369731,-8.373633,-8.374454,-8.396421,-8.409757,-8.382518,-8.394446,-9.392358,-8.406682,-8.376943,-8.386685,-8.36307,-8.360032,-8.474793,-8.503409,-8.535328,-8.515639,-8.619564,-8.711247,-8.870496,-8.977484,-9.048626,-9.028641,-8.986337,-9.020016,-9.03111,-9.05835,-9.044718,-9.039754,-8.998901,-9.032808,-8.955523,-8.923018,-8.868008,-8.885252,-8.791557,-8.726564,-9.362655,-8.478942,-8.38892,-8.38111,-8.39752,-8.372238,-8.398372,-8.336676,-8.387222,-8.399471,-8.375566,-8.3753,-8.387228,-8.351951,-8.345301,-9.147575,-8.370571,-8.414764,-8.462019,-8.503094,-8.486733,-8.544237,-8.655688,-8.762941,-8.845474,-8.947195,-9.06724,-9.01002,-9.008335,-9.009742,-8.972477,-9.003902,-9.03805,-8.965544,-9.019429,-9.011959,-8.903558,-8.908305,-8.910232,-8.877183,-8.781314,-8.697102,-8.557307,-8.473928,-8.413616,-8.369725,-8.378622,-8.388642,-8.350012,-8.401416,-8.36862,-8.341122,-8.365564,-8.419468,-8.371102,-8.348611,-8.375584,-8.394489,-8.398897,-8.469508,-8.481732,-8.533414,-8.505897,-8.647372,-8.695435,-8.816314,-8.883289,-9.033092,-9.025548,-9.060869,-9.043353,-9.033913,-9.041143,-9.016386,-9.050268,-9.03947,-9.060319,-9.018046,-8.951356,-8.895785,-8.877726,-8.890241,-8.781018,-8.6882,-8.578977,-8.476972,-8.381684,-8.422531,-8.411164,-8.396674,-8.414468,-8.39781,-8.381641,-8.385845,-8.356371,-8.374448,-8.364743,-8.372226,-8.379159,-8.390581,-8.361397,-8.406392,-8.481176,-8.507576,-8.526474,-8.587318,-8.695429,-8.796311,-8.906626,-9.023053,-9.019176,-9.03445,-8.98359,-9.016663,-9.03166,-8.984991,-9.01165,-9.029178,-8.975521,-9.008032,-8.939965,-8.90996,-8.854389,-8.873015,-8.756551,-8.657639,-8.558986,-8.42308,-8.367243,-8.403651,-8.388908,-8.392556,-8.411411,-8.391371,-8.419499,-8.393637,-8.381709,-8.394476,-8.380844,-8.385296,-8.400589,-8.39168,-8.379171,-8.464217,-8.48811,-8.517306,-8.500618,-8.637586,-8.719044,-9.802267,-8.91856,-9.014719,-9.029993,-9.059442,-9.025301,-9.027239,-9.025282,-9.039729,-9.039748,-9.035278,-9.017497,-9.002501,-8.934415,-8.891623,-8.882159,-8.828267,-8.731837,-8.651508,-8.530605,-8.458944,-8.391136,-8.392785,-8.4042,-8.368595,-8.367787,-8.395557,-8.405028,-8.393637,-8.381696,-9.359012,-8.391957,-8.410312,-8.401688,-8.373331,-8.402249,-8.472811,-8.506749,-8.531759,-8.522838,-8.639858,-8.74487,-8.855772,-8.914121,-9.0086,-9.998184,-9.051398,-9.018374,-9.030302,-9.046107,-9.048348,-9.002217,-9.028332,-9.048922,-8.962475,-8.924388,-8.89163,-8.919387,-8.865742,-8.766287,-9.569937,-8.506489,-8.406423,-8.379443,-8.410572,-8.390007,-8.379708,-8.399761,-8.399193,-8.383345,-8.392241,-8.39752,-8.40446,-8.393377,-8.420611,-8.375844,-8.364465,-8.380548,-8.47838,-8.537884,-8.532556,-8.551732,-8.696269,-8.768516,-8.862143,-8.956912,-9.046119,-9.009452,-9.043903,-9.054997,-9.063622,-9.08002,-9.027221,-9.01165,-9.058899,-9.021109,-8.958326,-8.911053,-8.898013,-8.864119,-8.815191,-8.730725,-8.648452,-8.545107,-8.447269,-8.383888,-8.403892,-8.368342,-8.384469,-8.393347,-8.368071,-8.374738,-8.382234,-8.392235,-8.415881,-8.421135,-8.403385,-8.391155,-8.420308,-8.428346,-8.492833,-8.526444,-8.531197,-8.554257,-8.642877,-8.760169,-8.901076,-8.962753,-9.015805,-9.047508,-9.046669,-9.047243,-9.028073,-9.019436,-9.042791,-9.063616,-9.022776,-9.039204,-9.000815,-8.884684,-8.87801,-8.887166,-8.849647,-8.684594,-8.629301,-8.484782,-8.38474,-8.393637,-8.370559,-8.418357,-8.399187,-8.381968,-8.423914,-8.388914,-8.395853,-8.376146,-8.411992,-8.397798,-8.371392,-8.379715,-8.396687,-8.427538,-8.530654,-8.536488,-8.532012,-8.540069,-8.655682,-8.788779,-8.904959,-8.978033,-9.025295,-9.044718,-9.029468,-9.069179,-9.054744,-9.023078,-9.052256,-9.051941,-9.03111,-9.431846,-8.950782,-8.891617,-8.906638,-8.935792,-8.815715,-8.69985,-8.604549,-8.465063,-8.389432,-8.363891,-8.412251,-8.388074,-8.369157,-8.367774,-8.403929,-8.40725,-8.419184,-8.414474,-8.403089,-8.414492,-8.419468,-8.393063,-8.380289,-8.426698,-8.520084,-8.522856,-8.523671,-8.578996,-8.677389,-9.742541,-8.89718,-8.961376,-9.042248,-8.994709,-9.010823,-9.012212,-9.025863,-9.011947,-9.008076,-9.008329,-9.031678,-9.001389,-8.951628,-8.898847,-9.871193,-8.860235,-8.772387,-8.6643,-8.565074,-8.453629,-8.377819,-8.360835,-8.406707,-8.378887,-8.366682,-8.371386,-8.376121,-8.371114,-8.381931,-9.317363,-8.375837,-8.417246,-8.343603,-8.377239,-8.426426,-8.427544,-8.510885,-8.498124,-8.485881,-8.600678,-8.687088,-8.776851,-8.954418,-9.001661,-9.004143,-9.006396,-9.020004,-9.003606,-8.983312,-8.972205,-9.010841,-9.039723,-9.031962,-8.939669,-8.95109,-8.90912,-8.879387,-8.879677,-8.732386,-9.581915,-8.561166,-8.438076,-8.374461,-8.406972,-8.347203,-8.348888,-8.37225,-8.343894,-8.367509,-8.380591,-8.374436,-8.360279,-8.385574,-8.354155,-8.37835,-8.359149,-8.396964,-8.426723,-8.516201,-8.488104,-8.528117,-8.610952,-8.651212,-8.805757,-8.879411,-8.918326,-8.986664,-8.945522,-8.961642,-9.010008,-9.001111,-8.928574,-8.933569,-8.992233,-8.97165,-8.970544,-8.918313,-8.806047,-8.857432,-8.799058,-8.707901,-8.619842,-8.486745,-8.399737,-8.349438,-8.321371,-8.405299,-8.388346,-8.353068,-8.322748,-8.351969,-8.373609,-8.386679,-8.429205,-8.37109,-8.358316,-8.396119,-8.416141,-8.421716,-8.460031,-8.510638,-8.545367,-8.555381,-8.656793,-8.769084,-8.84188,-8.919128,-9.020269,-9.051416,-9.028054,-9.014453,-9.024702,-8.991962,-8.996679,-9.067505,-8.999988,-9.000543,-8.982763,-8.897445,-8.896908,-8.899403,-8.797965,-8.704036,-8.628418,-8.50702,-8.395328,-8.36278,-8.359186,-8.41448,-8.328064,-8.370022,-8.386691,-8.410294,-8.359736,-8.402256,-8.348611,-8.401978,-8.387778,-8.359736,-8.346388,-8.402811,-8.472008,-8.568969,-8.520091,-8.52314,-8.643729,-8.764065,-8.856062,-9.029999,-9.036408,-9.063641,-9.003346,-9.093917,-8.985812,-9.03776,-9.047496,-9.05083,-9.033623,-9.772806,-8.944114,-8.931377,-8.879374,-8.874935,-8.809085,-8.729911,-8.582033,-8.530074,-8.439182,-8.401694,-8.400582,-8.368904,-8.35973,-8.399193,-9.374608,-8.383363,-8.375282,-8.350852,-8.372226,-8.385296,-8.368608,-8.354729,-8.385827,-8.405021,-8.467014,-8.510089,-8.515053,-8.551207,-8.642612,-9.702534,-8.895507,-9.005575,-9.016398,-9.043897,-9.017503,-8.98777,-9.019732,-9.039198,-9.053336,-9.036679,-9.032765,-9.029734,-8.981664,-8.930784,-8.864928,-8.862464,-8.823785,-8.686804,-8.631517,-8.528123,-8.402552,-8.388056,-8.380283,-8.381956,-8.402515,-8.396952,-8.408078,-8.39723,-8.413912,-9.381819,-8.405318,-8.358341,-8.390297,-8.398644,-8.392809,-8.465859,-8.485332,-8.511182,-8.545367,-8.628442,-8.69764,-8.784346,-8.914689,-9.042248,-9.023331,-9.058066,-9.036111,-9.060875,-9.010848,-9.023615,-9.035574,-9.062795,-9.041662,-9.037235,-8.916881,-8.891352,-9.115038,-8.901619,-8.775727,-9.404347,-8.573995,-8.477571,-8.405299,-8.412831,-8.371386,-8.389192,-8.413628,-8.396119,-8.385561,-8.394742,-8.377801,-8.420573,-8.407516,-8.421123,-9.114205,-8.386957,-8.380307,-8.469495,-8.528413,-8.548139,-8.549818,-8.586806,-8.71405,-8.827421,-8.921622,-9.034728,-9.00944,-9.00944,-9.046953,-9.065561,-9.03082,-9.00555,-8.986343,-8.99971,-9.033598,-8.995808,-8.924135,-8.896871,-8.859396,-8.865761,-8.800744,-8.658497,-8.550904,-8.422543,-8.348327,-8.379196,-8.359761,-8.398082,-8.394211,-8.38558,-8.360292,-8.378918,-8.397823,-8.384166,-8.341122,-8.368898,-8.4078,-8.388352,-8.359724,-8.431149,-8.490913,-8.533124,-8.489783,-8.629838,-8.705425,-8.805448,-8.915782,-9.041131,-8.996956,-9.046946,-8.998883,-8.932458,-9.628318,-9.031944,-9.013607,-9.046959,-9.056392,-8.966087,-8.929976,-8.903835,-8.902465,-8.846869,-8.76157,-8.645137,-8.548997,-8.484239,-8.351938,-8.396403,-8.400298,-8.401434,-8.405596,-8.383907,-8.41974,-8.454518,-8.401947,-8.378338,-8.397255,-8.388364,-8.392507,-8.406972,-8.426963,-8.484801,-8.519251,-8.527573,-8.528691,-8.620132,-8.714031,-8.819636,-8.907466,-8.980268,-9.694169,-9.008631,-9.024449,-8.996679,-9.010557,-8.98304,-9.023331,-9.009446,-9.041939,-8.992202,-8.867175,-8.882184,-8.844943,-8.867428,-8.688724,-8.660139,-8.516738,-8.385012,-8.373343,-8.390019,-8.38779,-8.382246,-8.359705,-8.39418,-8.391124,-8.404762,-8.365564,-8.38808,-8.387549,-8.378634,-8.354451,-8.389451,-8.377245,-8.480324,-8.528969,-8.546218,-8.538693,-8.649563,-9.767502,-8.868261,-8.971921,-8.986942,-9.021961,-8.991369,-9.030011,-9.019182,-9.031401,-9.02167,-9.018071,-9.032215,-9.044736,-8.983868,-8.891617,-8.859951,-8.878282,-8.801565,-8.725694,-8.611767,-8.50063,-8.385314,-8.387228,-8.37614,-8.390031,-8.354186,-8.371676,-8.41088,-8.389729,-8.360563,-9.375151,-8.379184,-8.340294,-8.387518,-8.393631,-8.379727,-8.396415,-8.438095,-8.881054,-8.574273,-8.608161,-8.65065,-8.777116,-8.87717,-8.931075,-10.024021,-9.088614,-9.035846,-9.058634,-9.037519,-9.042507,-9.057535,-9.028628,-9.038618,-9.021652,-8.965537,-8.924944,-8.926339,-8.846894,-8.793817,-9.63222,-8.572847,-8.497266,-8.439515,-8.406966,-8.395316,-8.361662,-8.397205,-8.394192,-8.382808,-8.371966,-8.382234,-8.428661,-8.380838,-8.423383,-8.418073,-8.754878,-8.397792,-8.454215,-8.502279,-8.512034,-8.513386,-8.61983,-8.718223,-8.829638,-8.89826,-9.021096,-9.01362,-9.01888,-9.0228,-9.056405,-9.026924,-9.033617,-9.032493,-9.070333,-9.091411,-9.037494,-8.941935,-8.895519,-8.866335,-8.894377,-8.767973,-8.71129,-8.61649,-8.508126,-8.395853,-8.379177,-8.392791,-8.370843,-8.401706,-8.381116,-8.375578,-8.421685,-8.393075,-8.371664,-8.354451,-8.364459,-8.375029,-8.384746,-8.363088,-8.416122,-8.541755,-8.539242,-8.508403,-8.574267,-8.686236,-8.804639,-8.925784,-9.00084,-9.006106,-9.02222,-8.997203,-9.0086,-9.04139,-9.0203,-8.99666,-9.033605,-9.007224,-8.998895,-8.969976,-8.888567,-8.892976,-8.89271,-8.749056,-8.654558,-8.597338,-8.434483,-8.371664,-8.397804,-8.37672,-8.391964,-8.362242,-9.016941,-8.389716,-8.380011,-8.360866,-8.369768,-8.379424,-8.386407,-8.390297,-8.393056,-8.371664,-8.460871,-8.50368,-8.49203,-8.503952,-8.607606,-8.687113,-8.862989,-8.901329,-8.96747,-8.97415,-9.040587,-9.015552,-8.997753,-9.003599,-9.026955,-9.032209,-9.019732,-9.439606,-8.988325,-8.933019,-8.85521,-8.882171,-8.831588,-8.723483,-8.635697,-8.509792,-8.441713,-8.388908,-9.072253,-8.373886,-8.372528,-8.360538,-8.390581,-8.373905,-8.360841,-8.353321,-8.395304,-8.374714,-8.36583,-8.360563,-8.346122,-8.374726,-8.471453,-8.488406,-8.522332,-8.520634,-8.632363,-9.709696,-8.873262,-8.938045,-9.02945,-9.007804,-9.045866,-8.990826,-9.040853,-9.04444,-9.02945,-9.008347,-9.03308,-9.050324,-8.999975,-8.945552,-9.903137,-8.86657,-8.819383,-8.762953,-8.623195,-8.507008,-8.406972,-8.344986,-8.364984,-8.400323,-8.387802,-8.352506,-8.393921,-8.359186,-8.399743,-9.333761,-8.375535,-8.358902,-8.383925,-8.362502,-8.383901,-8.386994,-8.432279,-8.490882,-8.522301,-8.541193,-8.603735,-8.726817,-8.839923,-8.912726,-9.031666,-9.000562,-9.068623,-8.999444,-9.002501,-9.00555,-9.036679,-8.976941,-9.013607,-8.994981,-8.986374,-8.893556,-9.499913,-8.87133,-8.849351,-9.683624,-8.635666,-8.509243,-8.451165,-8.40057,-8.398384,-8.402546,-8.383055,-8.411689,-8.382789,-8.408078,-8.4139,-8.402521,-8.419172,-8.4189,-8.376955,-8.400274,-8.392254,-8.448121,-8.482856,-8.518405,-8.532827,-8.55843,-8.668758,-8.780716,-8.929963,-8.97415,-9.034173,-9.041137,-9.08557,-9.014712,-9.053349,-9.04807,-9.025832,-9.062511,-9.353487,-9.029709,-8.980534,-8.907182,-8.897186,-8.948874,-8.808529,-8.682378,-8.608155,-8.481979,-8.425019,-8.388926,-8.373899,-8.397792,-8.441114,-8.388895,-8.390013,-8.399465,-8.408362,-8.401965,-8.411683,-8.366422,-8.420845,-8.381968,-8.382808,-8.421679,-8.488949,-8.511157,-8.56929,-8.573705,-8.659565,-8.808535,-8.902459,-9.000266,-9.044465,-9.035259,-9.046959,-9.046385,-9.007205,-9.00723,-9.04862,-9.023609,-9.028326,-8.997481,-8.908583,-8.854667,-8.895501,-8.894383,-8.795187,-8.7171,-8.577014,-8.465581,-8.369176,-8.342505,-8.403336,-8.40725,-8.368651,-8.358631,-8.403935,-8.377245,-8.364447,-8.380307,-8.366416,-8.354729,-8.432804,-8.363632,-8.389488,-8.423926,-8.478392,-8.531481,-8.557591,-8.55038,-8.690694,-8.785735,-8.894667,-8.983034,-9.420708,-9.058072,-9.082273,-8.996092,-9.004149,-8.995839,-9.014743,-8.976669,-9.732533,-9.001667,-8.938286,-8.901891,-8.870231,-8.85329,-8.747117,-8.645686,-8.571501,-8.436694,-8.38837,-8.375004,-8.394742,-8.394464,-8.374195,-9.367662,-8.361144,-8.378616,-8.385302,-8.378066,-8.411973,-8.388901,-8.36223,-8.344455,-8.35305,-8.469508,-8.47449,-8.511441,-8.483362,-8.609026,-10.31388,-8.794916,-8.938564,-9.005847,-9.023924,-9.001099,-9.039186,-8.950529,-9.023603,-9.012231,-9.004995,-9.043619,-9.017787,-8.981386,-8.92608,-9.830908,-8.868552,-8.892729,-8.748235,-8.649304,-8.541168,-8.447807,-8.402774,-8.366947,-8.354723,-8.370849,-8.390556,-8.37309,-8.41698,-8.360008,-8.391673,-8.3403,-8.398076,-8.338609,-8.400879,-8.372528,-8.357211,-8.419493,-8.492005,-8.518671,-8.504792,-8.589831,-8.685705,-8.80714,-8.950257,-9.940384,-9.031672,-9.033358,-9.01278,-9.032493,-8.974706,-8.917739,-8.997796,-8.969723,-9.026665,-8.978027,-8.898557,-8.808523,-8.883245,-8.757378,-8.694028,-8.631221,-8.483955,-8.359458,-8.360001,-8.294966,-8.351667,-8.364193,-8.341393,-8.347505,-8.392797,-8.310252,-8.351111,-8.352228,-8.314716,-9.257081,-8.989153,-8.416171,-8.449214,-8.473688,-8.510632,-8.550633,-8.554819,-8.634851,-8.75878,-8.829094,-8.944441,-9.007217,-9.035012,-9.015564,-10.035165,-9.070846,-9.023628,-9.054454,-9.040019,-9.041674,-9.050589,-8.994425,-8.952492,-8.92858,-8.891889,-8.816604,-8.763225,-8.629004,-8.545095,-8.415579,-8.404194,-8.380857,-8.429205,-8.371652,-8.393884,-8.373362,-8.405836,-8.369176,-8.831588,-8.400311,-8.387512,-8.3814,-8.352482,-8.396674,-8.376097,-8.447257,-8.519504,-8.538118,-8.519269,-8.628467,-8.770726,-8.821315,-8.99474,-8.998883,-8.989998,-9.003315,-9.058911,-9.033364,-8.99779,-9.010564,-9.023603,-9.042514,-9.004711,-8.929445,-8.93026,-8.858519,-8.894396,-8.775184,-8.717649,-8.576211,-8.501168,-8.410584,-8.386975,-8.37919,-8.377517,-8.343616,-8.386407,-8.366953,-8.397835,-8.427556,-8.404453,-8.383339,-8.36528,-8.377504,-8.371114,-8.375837,-8.414196,-8.449202,-8.490635,-8.486992,-8.580107,-8.656225,-8.756267,-8.859106,-9.021942,-9.007798,-9.040303,-9.039186,-9.018071,-8.980546,-8.992789,-9.00944,-9.03892,-9.023344,-9.000537,-8.928611,-8.891611,-8.833552,-8.872435,-8.73848,-8.681248,-8.581225,-8.467822,-8.365317,-8.381135,-8.356377,-8.397816,-8.392519,-8.388624,-8.358612,-8.394464,-8.384154,-8.376671,-8.392816,-8.373905,-8.367787,-8.440608,-8.387784,-8.412239,-8.493666,-8.499507,-8.482862,-8.599839,-9.627194,-8.819068,-8.895525,-8.988869,-9.041699,-9.077563,-9.038624,-9.033055,-9.01775,-9.023053,-9.023905,-9.044736,-9.069759,-9.027511,-8.972495,-8.90244,-8.89329,-8.914695,-8.782123,-8.670129,-8.559529,-8.495346,-8.423339,-8.420845,-8.368336,-8.38474,-8.402793,-8.377196,-8.379159,-8.365576,-9.382658,-8.393902,-8.37722,-8.388358,-8.436175,-8.41448,-8.360279,-8.468353,-8.505069,-8.561468,-8.537834,-8.609834,-8.656521,-8.804053,-8.901928,-10.018193,-9.003902,-9.008884,-9.034191,-9.101968,-8.994715,-9.032808,-9.07279,-9.080014,-9.014719,-9.040556,-8.941614,-8.896062,-8.862723,-8.855475,-9.763082,-8.679309,-8.58341,-8.420876,-8.399737,-8.323038,-8.392532,-8.414202,-8.386401,-8.41364,-8.363045,-8.377511,-8.360261,-8.386123,-8.358612,-8.402527,-8.363879,-8.38195,-8.360551,-8.444226,-8.487838,-8.540075,-8.494234,-8.622898,-8.712383,-8.819099,-8.907176,-9.018318,-9.000284,-9.011107,-9.613309,-8.989159,-9.000543,-9.016386,-8.990819,-9.036951,-9.046699,-8.947503,-8.952757,-8.888283,-8.913294,-8.825742,-8.719631,-8.622898,-8.565648,-8.437008,-8.366959,-8.421691,-8.382758,-8.383629,-8.405589,-8.403348,-8.355834,-8.416993,-8.42337,-8.40475,-8.381684,-8.42613,-8.361113,-8.411418,-8.415005,-8.473934,-8.530642,-8.564549,-8.514244,-8.651798,-8.727373,-8.837985,-8.956363,-9.050002,-9.060862,-9.06474,-9.025869,-9.041662,-9.058362,-8.987751,-9.021374,-9.033629,-8.972187,-8.983571,-8.928025,-8.862155,-8.865496,-8.837157,-8.709321,-8.621775,-8.476435,-8.393093,-8.370565,-8.379455,-8.367194,-8.384728,-8.348055,-8.362496,-8.386685,-8.359458,-8.388889,-8.388895,-8.371411,-8.383092,-8.354982,-8.36223,-8.387821,-8.457271,-8.480312,-8.527005,-8.498118,-8.609822,-8.747117,-8.8727,-8.971372,-9.026128,-9.001957,-9.01333,-9.009162,-9.007508,-9.024159,-9.018602,-8.998049,-9.001365,-9.020547,-9.004408,-8.87049,-8.862995,-8.894655,-8.805738,-8.723792,-8.614008,-8.495617,-8.388099,-8.401681,-8.364996,-8.381085,-8.398631,-8.388617,-8.408343,-8.38224,-8.380264,-8.386111,-8.368046,-8.367521,-8.376683,-8.39807,-8.399724,-8.418937,-8.476169,-8.48309,-8.543663,-8.532006,-9.622199,-8.784914,-8.889672,-8.983602,-9.062801,-9.040563,-9.016114,-9.009712,-8.989721,-9.049725,-9.010582,-9.031413,-9.045594,-9.002525,-8.937205,-9.866186,-8.876609,-8.884394,-8.806041,-8.64902,-8.582898,-8.498389,-8.421691,-8.368879,-8.351099,-8.387241,-8.35526,-8.358057,-8.420833,-8.423092,-9.333743,-8.3753,-8.353865,-8.32999,-8.368064,-8.387518,-8.376967,-8.405855,-8.502575,-8.531741,-8.511472,-8.553701,-8.635956,-8.789359,-8.875213,-9.025011,-9.002766,-9.021942,-9.007489,-9.032234,-9.012218,-8.994153,-9.006384,-9.043903,-9.053892,-9.024473,-8.939984,-8.918011,-8.881603,-8.859674,-9.752833,-8.663751,-8.566771,-8.446998,-8.383067,-8.385827,-8.401972,-8.363366,-8.371374,-8.404478,-8.353895,-8.385006,-8.409195,-8.379745,-8.360285,-8.414764,-8.377782,-8.375294,-8.378054,-8.408911,-8.487005,-8.506181,-8.524505,-8.600944,-8.686798,-8.791038,-8.905237,-8.97665,-8.997234,-9.026128,-9.258439,-9.011409,-8.98777,-8.98777,-8.988887,-9.004729,-8.94275,-8.999982,-8.959722,-8.907694,-8.85855,-8.865508,-8.7135,-8.585077,-8.492851,-8.596486,-8.33054,-8.395316,-8.321649,-8.325539,-8.341381,-8.315006,-8.358328,-8.368342,-8.363613,-8.416962,-8.417252,-8.376128,-8.394186,-8.427241,-8.390562,-8.473922,-8.555893,-8.512324,-8.535346,-8.614008,-8.717094,-8.835756,-8.938576,-8.994419,-8.995845,-9.029159,-9.018627,-9.024733,-9.01667,-9.01833,-8.9975,-9.023344,-9.016676,-8.961358,-8.881881,-8.888277,-8.890197,-8.844356,-8.714056,-8.633456,-8.552886,-8.446992,-8.372226,-8.38474,-8.367509,-8.359464,-8.314154,-8.404194,-8.41419,-8.37225,-8.411689,-8.381406,-8.387765,-8.423667,-8.403651,-8.411967,-8.418098,-8.475867,-8.505335,-8.547033,-8.561196,-8.644303,-8.734356,-8.832181,-8.958604,-9.032759,-9.046422,-9.042242,-9.016126,-9.054195,-9.025301,-9.078884,-9.048916,-9.020275,-9.032808,-9.002198,-8.916066,-8.91301,-8.894686,-8.830199,-8.74821,-8.588442,-8.495617,-8.441139,-8.365836,-8.380851,-8.353346,-8.370287,-8.479787,-8.398928,-8.341683,-8.3753,-8.404206,-8.354729,-8.360292,-8.386685,-8.368348,-8.411411,-8.429192,-8.454758,-8.488363,-8.464223,-8.521998,-9.188699,-8.745172,-8.837713,-8.962753,-9.02669,-9.001389,-9.008903,-9.004995,-9.036117,-8.993308,-9.000574,-9.002494,-9.04418,-9.013885,-8.983837,-8.919128,-8.864113,-8.837447,-8.798793,-8.694861,-8.608989,-8.536192,-8.473366,-8.377239,-8.398872,-8.400866,-8.386105,-8.398885,-8.380554,-8.390309,-9.483534,-8.389185,-8.403916,-8.395014,-8.369188,-8.396705,-8.406954,-8.419752,-8.52285,-8.516182,-8.510342,-8.547021,-8.634024,-8.759082,-8.903854,-8.97833,-9.015009,-9.035821,-9.039741,-9.019145,-9.054997,-9.045835,-9.042785,-9.030833,-9.076976,-9.016398,-8.953869,-8.886592,-8.89994,-8.921332,-9.753938,-8.699597,-8.621781,-8.506452,-8.424469,-8.37556,-8.414468,-8.364434,-8.41001,-8.39447,-8.422796,-8.376955,-8.403348,-8.380814,-8.394717,-9.372366,-8.385024,-8.398909,-8.408368,-8.40809,-8.48953,-8.545076,-8.555066,-8.600413,-8.670129,-8.799645,-8.923864,-8.997759,-9.050015,-9.01888,-9.979823,-9.050854,-9.026406,-9.001408,-9.039451,-9.011088,-9.012792,-9.023078,-8.970563,-8.879683,-8.90273,-8.841596,-8.797953,-8.693194,-8.575619,-8.472286,-8.389476,-8.347252,-8.394186,-8.366379,-8.358057,-8.343054,-8.38863,-8.355853,-8.386703,-8.401675,-8.366663,-8.405855,-8.391976,-8.353902,-8.376418,-8.403632,-8.508687,-8.530926,-8.518955,-8.581225,-8.69459,-8.794909,-8.888561,-8.985528,-9.007754,-8.997524,-9.054707,-9.040859,-9.02364,-9.052231,-8.991641,-8.994153,-9.068327,-8.994178,-8.936076,-8.883258,-8.886623,-8.857747,-8.750735,-8.643186,-8.571476,-8.455067,-8.372541,-8.380295,-8.358341,-8.401144,-8.388611,-8.375022,-8.377813,-8.373078,-8.355569,-8.417252,-8.378066,-8.432538,-8.385561,-8.351401,-8.363619,-8.436447,-8.501458,-8.508403,-8.511743,-8.610939,-8.766015,-8.804633,-8.949442,-9.034457,-9.023615,-9.031123,-9.038056,-9.029166,-9.01725,-9.073655,-9.039192,-9.042501,-9.104234,-8.984979,-8.945231,-8.872416,-8.905472,-8.910238,-8.780191,-8.629856,-8.589843,-8.46476,-8.402243,-8.430581,-8.388914,-8.346122,-8.39447,-8.374732,-8.403379,-8.393921,-8.371133,-8.403645,-8.419765,-8.355846,-8.373621,-8.398922,-8.384185,-8.461723,-8.531469,-8.551732,-8.553991,-9.608006,-8.745722,-8.795718,-8.931908,-8.974144,-9.02861,-9.062233,-8.996654,-9.008594,-9.038605,-8.992777,-8.988301,-8.990566,-9.03863,-9.007754,-8.946658,-8.903545,-8.934125,-8.81966,-8.736294,-8.624287,-8.528962,-8.456431,-8.37556,-8.347215,-8.387802,-8.40307,-8.363885,-8.35305,-8.343073,-9.353184,-8.382227,-8.388358,-8.347777,-8.364453,-8.394791,-8.39639,-8.401978,-8.452264,-8.839077,-8.51646,-8.553677,-8.625411,-8.767374,-8.86189,-9.941217,-8.969983,-9.010545,-8.983874,-9.011366,-9.0639,-9.021102,-9.018312,-9.018892,-9.044742,-9.0147,-8.974712,-8.898001,-8.870521,-8.901625,-9.752827,-8.709901,-8.580379,-8.492555,-8.441707,-8.367237,-8.33083,-8.378313,-8.374461,-8.378931,-8.356414,-8.380301,-8.370312,-8.397798,-8.361131,-8.40278,-8.366651,-8.973341,-8.352506,-8.447844,-8.455049,-8.535346,-8.545916,-8.518411,-8.647063,-8.767114,-8.804096,-9.001395,-9.046107,-9.015842,-9.638301,-9.044477,-9.002198,-8.997512,-8.977484,-9.018065,-8.998043,-9.019707,-8.93886,-8.914961,-8.884665,-8.858846,-8.8241,-8.692355,-8.587898,-8.48314,-8.417258,-8.376121,-8.350815,-8.347789,-8.354741,-8.384178,-8.37196,-8.384728,-8.375022,-8.352512,-8.372516,-8.419184,-8.409738,-8.367515,-8.408646,-8.400033,-8.456715,-8.518967,-8.481436,-8.573421,-8.652335,-8.7521,-8.870496,-8.979978,-9.027801,-9.025004,-9.031407,-9.015003,-8.965828,-8.927173,-8.996944,-9.022522,-8.975582,-8.934112,-8.940249,-8.862149,-8.818524,-8.852709,-8.782685,-8.589269,-8.522585,-8.453128,-8.40086,-8.372775,-8.286371,-8.363613,-8.386123,-8.981373,-8.338331,-8.375553,-8.383079,-8.390575,-8.360557,-8.34527,-8.347512,-8.389451,-8.374473,-8.425865,-8.482529,-8.501736,-8.533401,-8.581478,-8.70461,-8.777937,-8.882431,-9.000821,-9.037778,-9.002494,-8.995555,-9.020553,-9.029474,-9.015003,-9.004167,-8.991678,-9.025023,-9.026937,-8.979694,-8.918301,-8.817963,-8.887722,-8.747673,-8.674296,-8.562283,-8.447541,-8.382808,-9.008606,-8.351975,-8.405</t>
+  </si>
+  <si>
+    <t>-13.957054,-14.091818,-13.235924,-13.439904,-12.690967,-13.634388,-12.437269,-12.539509,-12.568415,-12.426144,-12.607885,-12.748489,-12.338314,-12.5123,-12.540058,-12.523129,-12.578985,-12.638415,-12.381111,-12.550906,-13.442423,-12.896619,-12.646262,-12.661258,-12.864651,-13.427377,-13.193127,-13.734214,-13.970131,-13.99261,-14.150754,-14.085712,-14.055985,-14.63677,-14.084348,-15.320387,-14.118792,-14.26912,-13.987634,-14.352758,-13.809486,-15.645832,-13.916455,-13.788939,-13.48853,-13.294564,-12.70571,-12.498952,-12.379481,-12.62874,-13.408213,-13.018924,-12.264147,-12.411135,-12.473374,-12.522851,-12.335838,-12.284119,-12.500348,-12.739876,-12.464749,-12.612922,-12.583417,-12.314124,-12.592604,-13.599413,-12.931891,-13.049201,-13.18783,-13.648588,-14.059856,-14.23496,-13.964821,-13.925944,-14.28082,-14.215772,-14.119619,-14.549008,-14.358876,-15.209813,-15.321511,-14.290247,-13.759761,-14.132702,-13.979595,-13.708086,-13.595264,-13.238166,-12.706821,-12.841048,-12.268555,-12.366954,-12.669296,-12.914672,-12.209681,-13.488252,-12.454192,-12.601791,-12.755145,-12.472534,-12.394181,-12.550085,-12.505336,-12.623153,-12.498372,-12.617627,-12.680712,-12.773506,-12.513128,-13.047522,-13.547151,-13.805602,-14.132949,-13.994549,-13.926778,-14.335008,-14.283005,-14.112643,-14.079594,-14.42143,-14.106555,-14.103783,-14.225224,-13.834533,-13.986263,-14.329446,-13.748099,-13.700838,-13.427124,-13.085016,-12.832991,-12.593444,-12.326071,-12.673995,-12.500625,-12.468632,-12.807987,-12.744908,-12.35473,-12.532575,-12.502274,-12.539793,-12.917456,-12.483357,-12.35055,-12.57733,-12.598982,-12.73737,-12.803245,-12.585924,-12.564556,-12.939676,-13.396829,-13.995425,-14.119891,-15.838124,-14.182964,-14.304707,-13.864508,-14.110717,-14.072667,-14.148266,-13.992635,-14.304688,-14.038198,-14.307473,-13.964556,-14.020695,-13.785895,-13.723342,-13.324847,-13.266775,-12.905479,-12.607366,-12.730986,-12.660412,-12.342506,-12.528717,-12.166043,-12.516462,-12.635673,-12.455044,-12.379438,-12.762405,-12.54033,-12.765171,-12.383315,-12.216898,-12.403646,-12.668191,-12.352514,-12.552313,-12.850463,-14.963023,-13.557708,-14.1699,-14.169659,-14.43363,-13.965945,-14.136845,-14.039019,-14.007359,-13.78145,-14.355308,-14.059584,-13.821192,-14.068518,-14.274979,-14.039599,-14.131016,-13.769751,-13.687236,-13.574087,-12.765745,-12.745433,-12.756262,-12.446141,-12.283848,-12.622887,-12.696264,-12.305839,-12.732665,-12.527019,-12.49171,-12.518388,-12.924674,-12.344716,-12.397497,-12.623721,-12.575348,-12.640687,-12.477566,-12.671797,-12.866904,-12.934959,-13.479929,-13.44183,-13.746685,-14.166584,-14.518959,-14.361402,-14.266089,-14.207431,-14.011508,-15.17648,-14.094899,-13.867842,-14.417522,-14.267997,-14.01099,-13.959524,-13.986232,-13.905638,-13.645538,-13.019721,-12.954697,-12.762103,-12.73624,-12.488914,-13.45766,-12.199938,-12.477288,-12.602056,-12.327775,-12.49142,-12.716798,-12.21883,-12.577034,-12.900768,-13.40349,-12.152399,-12.542028,-12.357231,-12.918271,-13.743617,-12.360311,-12.914684,-13.298441,-13.6872,-14.212709,-14.156033,-13.945114,-14.291093,-14.337768,-14.047934,-14.21939,-14.040451,-13.792563,-14.181581,-14.550329,-14.046255,-14.347492,-14.19299,-14.109871,-14.184643,-13.517714,-13.026105,-12.973602,-12.422279,-12.373326,-12.506991,-12.415549,-12.451444,-12.696813,-13.501026,-12.566748,-12.612348,-13.158671,-12.406961,-12.716817,-12.532841,-12.522592,-12.917716,-12.718743,-12.262449,-12.926631,-12.590641,-12.812673,-12.974972,-13.524381,-13.869268,-14.262465,-13.827014,-14.417813,-14.117699,-14.224409,-14.052657,-14.290254,-13.862575,-14.213524,-14.229953,-14.078205,-14.142401,-14.355833,-14.179944,-14.313307,-13.599685,-13.460469,-13.193961,-12.939405,-12.582325,-12.648744,-12.457235,-12.453358,-12.479782,-12.746563,-12.732381,-12.357194,-12.327213,-12.350266,-12.608181,-12.540367,-12.074052,-12.595382,-12.629006,-12.643452,-12.766288,-12.575083,-12.506701,-12.811012,-12.853828,-13.352636,-13.659695,-14.235232,-13.755582,-14.490029,-14.443342,-14.296088,-14.201899,-14.087089,-14.172437,-14.453615,-13.989023,-14.374182,-13.938687,-13.96095,-14.201887,-14.314696,-13.73138,-13.536038,-12.977479,-12.519234,-12.561772,-13.95761,-12.78239,-12.659591,-12.257454,-12.355841,-12.754607,-12.813778,-12.638476,-12.349198,-12.609286,-12.639816,-12.755447,-12.657906,-12.181886,-12.475862,-12.777438,-12.637914,-12.714588,-12.639291,-13.100599,-13.836453,-13.965402,-14.145741,-14.349721,-14.065727,-13.913695,-14.273862,-13.976224,-14.442533,-14.062356,-14.353345,-14.054071,-14.387245,-14.031518,-14.069605,-14.179068,-13.945639,-14.075704,-14.000692,-12.9469,-13.553553,-12.464218,-12.348612,-12.475325,-12.349414,-12.431132,-12.908257,-12.580923,-12.503694,-12.559531,-12.746847,-12.566482,-12.59621,-12.643465,-12.447536,-13.204505,-12.420297,-12.379463,-12.883265,-12.654016,-12.989987,-13.507699,-13.629702,-13.773103,-14.200775,-14.26941,-14.134603,-14.239942,-14.281079,-13.855617,-15.554699,-14.534246,-14.480045,-14.137431,-13.915905,-13.984559,-14.269108,-13.988202,-14.425592,-13.43628,-13.054208,-12.975843,-12.728492,-12.742408,-12.818266,-12.130451,-12.334745,-13.008311,-12.524247,-12.231338,-12.366405,-12.822971,-12.381951,-12.654312,-12.277464,-12.40527,-12.53649,-12.71933,-12.511998,-12.826027,-13.796724,-12.555623,-13.222601,-13.25147,-13.810066,-13.890673,-14.564239,-13.94538,-14.228576,-14.336379,-14.138783,-14.356944,-14.133239,-14.149909,-14.873526,-13.951782,-14.441131,-14.498641,-14.110741,-14.044866,-13.95038,-13.662189,-13.51604,-13.024184,-12.38781,-12.58564,-12.775747,-12.565099,-12.856582,-12.569804,-13.28342,-12.487006,-12.658196,-12.812994,-12.362213,-12.457803,-12.599828,-12.77684,-12.409752,-12.33443,-12.893563,-12.854933,-12.545633,-13.058913,-13.12004,-14.489541,-13.783105,-14.4011,-14.065727,-14.182124,-14.28274,-14.424456,-15.201756,-14.176611,-14.212722,-14.19633,-14.08657,-13.87675,-14.637332,-14.268318,-14.251049,-14.05291,-13.862557,-13.425167,-13.546891,-13.196726,-12.658758,-12.307481,-12.432243,-12.825175,-12.708742,-12.549807,-12.501453,-12.623184,-12.537286,-12.586492,-12.535897,-12.367226,-12.553949,-12.362509,-12.493951,-12.77266,-12.708495,-12.498693,-12.584825,-12.592586,-13.247581,-13.397644,-13.78505,-13.599104,-14.117681,-14.064598,-14.064301,-14.269707,-13.928426,-14.591478,-14.387486,-14.087379,-14.253291,-14.507266,-13.872836,-14.141574,-13.899254,-13.92287,-13.72115,-13.380147,-12.974157,-12.8252,-12.547022,-12.756262,-12.598982,-12.617886,-12.259948,-12.355286,-12.609848,-12.476967,-12.365003,-12.554808,-12.530341,-12.51869,-12.287768,-12.334437,-12.470904,-12.623727,-12.715737,-12.682632,-12.720978,-13.069476,-14.825741,-13.580502,-13.675846,-13.933711,-13.991517,-14.038519,-14.171881,-13.937613,-14.468914,-14.175481,-14.716543,-14.003735,-14.239128,-14.440853,-13.969853,-14.059591,-14.197695,-14.091293,-14.173536,-13.329854,-13.024993,-12.897187,-12.496717,-12.513677,-12.662345,-12.516184,-12.48282,-12.553962,-12.26774,-12.473127,-12.861329,-12.340549,-12.371387,-12.457544,-12.442554,-12.829929,-12.75933,-12.5326,-12.486148,-12.244125,-12.680119,-12.435022,-13.207839,-13.106137,-13.925648,-13.794199,-14.384165,-14.130189,-14.227175,-14.486442,-14.469519,-15.23507,-14.233874,-14.307466,-14.188841,-14.192669,-13.921196,-14.264119,-13.978472,-14.125454,-13.727527,-13.651101,-13.192578,-12.71457,-12.559531,-12.65375,-12.328862,-12.346939,-12.569798,-12.754607,-12.373351,-12.340289,-12.342228,-12.556475,-12.328602,-12.406134,-12.380852,-12.374178,-12.453945,-12.745414,-12.423656,-13.443756,-12.762677,-12.742926,-13.105593,-13.557437,-13.834496,-14.280826,-14.191872,-14.247715,-14.073185,-13.94178,-14.289408,-14.134085,-14.107395,-14.258575,-15.105572,-14.118798,-14.32166,-14.304435,-14.305262,-14.406693,-13.800596,-13.234782,-12.638723,-12.899657,-12.553128,-12.383933,-12.386958,-12.593703,-12.214971,-13.569951,-12.498119,-12.616219,-12.469207,-12.408906,-12.499224,-12.642316,-12.500644,-12.4403,-12.452833,-12.560086,-12.516455,-12.744025,-12.574546,-12.665975,-13.059734,-13.557449,-13.846165,-13.990684,-14.109074,-13.883962,-14.157132,-14.531196,-13.849493,-14.051274,-14.394197,-14.165745,-13.917856,-14.185483,-13.857,-14.069327,-13.959549,-14.126565,-13.741412,-13.381536,-13.093067,-12.735135,-12.584831,-12.505916,-12.760713,-12.429477,-12.25107,-12.29777,-12.46641,-12.533397,-12.515887,-12.299702,-12.446993,-12.459477,-12.191326,-12.600945,-12.487561,-12.497279,-12.682064,-12.520913,-12.332769,-12.93023,-13.302633,-13.706684,-13.888709,-14.061251,-13.987628,-14.161028,-14.064894,-14.134918,-14.058461,-14.353369,-14.275788,-14.316931,-14.294409,-14.286333,-14.379152,-14.264132,-13.843387,-14.101548,-13.790057,-13.355988,-12.818513,-12.339981,-12.606761,-12.464218,-12.594821,-12.382235,-12.738191,-12.665697,-12.472547,-12.386705,-12.413635,-12.608996,-12.680409,-12.501724,-12.344988,-12.575638,-12.324719,-12.42836,-12.611762,-12.239686,-12.878542,-13.044478,-13.359575,-13.830045,-14.140203,-14.179648,-14.320833,-14.253284,-14.021806,-14.335539,-14.067913,-13.916764,-14.1577,-14.174357,-13.968989,-14.074624,-14.302496,-14.157422,-14.254402,-13.867292,-13.143656,-13.498525,-13.33622,-12.528964,-12.426144,-12.318039,-12.362491,-12.631241,-12.634828,-12.49618,-12.369757,-12.359175,-12.502836,-13.009157,-12.700987,-12.543404,-12.455321,-12.654004,-12.388032,-12.454216,-12.582059,-12.595111,-12.892458,-13.0853,-13.357081,-13.7967,-14.152113,-14.65707,-14.097671,-14.317487,-13.943163,-14.326383,-15.201163,-14.292464,-14.147402,-14.249957,-14.43476,-14.235522,-13.880362,-14.164893,-14.087651,-13.684465,-13.508817,-13.356495,-13.100333,-12.523697,-12.152702,-13.439614,-12.599544,-12.409733,-12.311926,-12.524222,-12.584251,-12.761559,-12.777957,-12.285805,-12.234956,-12.816865,-12.730702,-12.730708,-12.541169,-12.442523,-13.289816,-12.851309,-12.766542,-13.162542,-13.237573,-13.960407,-14.122416,-14.178006,-14.198571,-14.104864,-14.273837,-13.871478,-14.004581,-14.480027,-13.959289,-14.378886,-14.484509,-14.082662,-14.15741,-13.865909,-13.966519,-14.300799,-13.482115,-12.953851,-12.684595,-12.511992,-12.277723,-12.312192,-12.240803,-12.447536,-13.580484,-12.510065,-12.456445,-12.906072,-12.839628,-12.471725,-12.192443,-12.699302,-12.376956,-12.492562,-12.372233,-12.711267,-12.807968,-12.63789,-12.647046,-13.318179,-13.208401,-13.922055,-14.068512,-14.109902,-14.396704,-14.223545,-14.439168,-14.3347,-14.238288,-14.176308,-14.202708,-14.394753,-14.035685,-14.40252,-14.219377,-13.730016,-14.203807,-14.010946,-13.087541,-12.966088,-12.725979,-12.294146,-12.413376,-12.631778,-12.188251,-12.613163,-12.645663,-12.336097,-12.759892,-12.571749,-12.380018,-12.598167,-12.659548,-12.649009,-12.398361,-12.524494,-12.306358,-12.790725,-12.991907,-12.868003,-13.17342,-13.002773,-13.513287,-13.758934,-13.927877,-14.260514,-14.322191,-14.430043,-14.112137,-14.408891,-14.586471,-14.53453,-14.277474,-13.794224,-14.394735,-14.266929,-13.940644,-14.01846,-14.146025,-13.620793,-13.532982,-12.886618,-12.442541,-12.851019,-12.359465,-12.416432,-12.517554,-12.806869,-12.491179,-12.316088,-12.267721,-12.516165,-12.469762,-12.484209,-12.300005,-12.639835,-12.492581,-12.57428,-12.394459,-12.273012,-12.831009,-12.682638,-12.69322,-13.388488,-13.758952,-13.728089,-14.147976,-14.60758,-14.126034,-14.155181,-14.273874,-14.001772,-14.381942,-14.425314,-14.30304,-14.273578,-14.252741,-13.980984,-14.051534,-14.316684,-14.059868,-14.127133,-13.283167,-13.385432,-12.592326,-12.845222,-12.66153,-12.461446,-12.68846,-12.460606,-12.543948,-12.41282,-12.463656,-12.579818,-12.566489,-12.667074,-12.666796,-12.821582,-13.828359,-12.447524,-12.593987,-12.79546,-12.77879,-12.495069,-12.781834,-13.599129,-13.524919,-14.142389,-14.333897,-14.074599,-14.278289,-14.052645,-14.019034,-15.355134,-14.279406,-13.983473,-14.212722,-14.20188,-14.081255,-14.084342,-14.073476,-14.117668,-13.893716,-13.607198,-12.986653,-13.028908,-12.491414,-12.252175,-12.504213,-12.761003,-12.196592,-12.77019,-12.43893,-12.406696,-12.613997,-12.888538,-12.477004,-12.404479,-12.609552,-12.60565,-12.535119,-12.704031,-12.526729,-13.985146,-12.396694,-12.675989,-13.18423,-13.664159,-14.023486,-13.965661,-13.948695,-14.278023,-14.262199,-13.978749,-14.283845,-14.717932,-14.265509,-14.139913,-14.348615,-14.131844,-13.903434,-14.169091,-13.952572,-14.141833,-13.67918,-13.22951,-13.295379,-12.878548,-13.070859,-12.521456,-12.24828,-12.313865,-12.565353,-13.771973,-12.402522,-12.460032,-12.443387,-12.662369,-12.594568,-12.68625,-12.376431,-12.678175,-12.279131,-12.613169,-12.967483,-12.538959,-12.371665,-12.837708,-14.029024,-13.453511,-13.724163,-14.102376,-13.826186,-14.582328,-14.282771,-14.123231,-14.213814,-14.271065,-14.377238,-14.151841,-13.961778,-14.410324,-14.095992,-14.038772,-14.084613,-13.969304,-14.076563,-13.716421,-13.380962,-12.707087,-12.511467,-12.668728,-12.431422,-12.602038,-12.407258,-12.332486,-12.563414,-12.803511,-12.53176,-12.692109,-12.506448,-12.298035,-12.634006,-12.4981,-12.445591,-12.676779,-12.60536,-12.677631,-12.748483,-12.920519,-13.26593,-13.449881,-13.577996,-14.189076,-14.439187,-14.179093,-14.061535,-13.957048,-14.240257,-14.116563,-14.160484,-13.832261,-14.329439,-14.341108,-13.868694,-14.123799,-14.07184,-13.853401,-13.687484,-13.398212,-12.919117,-12.946356,-12.602618,-12.39725,-12.44811,-12.727955,-13.096715,-12.854359,-12.130988,-12.618998,-12.704877,-12.829633,-12.596759,-12.539268,-12.7324,-12.537823,-12.618732,-12.8313,-12.476733,-12.737648,-12.603143,-12.88079,-13.544391,-13.380702,-13.770856,-14.417813,-14.455313,-14.140444,-14.144926,-14.231898,-14.214092,-14.256056,-14.264712,-14.443941,-14.299162,-14.402261,-13.855605,-14.348912,-13.967914,-14.047095,-13.510756,-13.293187,-13.098086,-12.644835,-12.513683,-12.717638,-12.093543,-12.217435,-12.533113,-12.471719,-12.478362,-12.663468,-12.575922,-12.499212,-12.837943,-12.567316,-12.847704,-12.82186,-12.793497,-12.590357,-12.666518,-13.034186,-12.798485,-13.011398,-12.987518,-13.463532,-13.858957,-14.595652,-14.048761,-14.334181,-14.279394,-14.131837,-15.253697,-14.039593,-14.069061,-14.078501,-13.8484,-14.04933,-13.962061,-13.959271,-14.241319,-14.31193,-13.812548,-13.406837,-12.866324,-12.674581,-12.506182,-12.43475,-12.540336,-12.536175,-12.449203,-12.320817,-12.454476,-12.371393,-12.603433,-12.470046,-12.587301,-12.39194,-12.630666,-12.267752,-12.241346,-12.519234,-13.52356,-12.765177,-12.682095,-13.028049,-13.668882,-13.76583,-14.129059,-14.216599,-14.326105,-14.331637,-13.992925,-14.233293,-14.000969,-14.24411,-14.006779,-15.47826,-13.993147,-14.293044,-13.957332,-14.143537,-14.142123,-13.850073,-13.655564,-13.421296,-13.205351,-12.786002,-12.715131,-12.416136,-12.546183,-12.825768,-13.055573,-12.520067,-12.478134,-12.482271,-12.690998,-12.712378,-12.310272,-12.676267,-12.502268,-12.43922,-12.427817,-12.504799,-12.614546,-12.697906,-12.83772,-13.04888,-13.547182,-13.696417,-13.945676,-14.240751,-14.460338,-14.1841,-14.0593,-13.848412,-14.334168,-14.333625,-13.906756,-14.277455,-14.070432,-14.047095,-13.989288,-14.095189,-13.894821,-13.948473,-13.626646,-13.120053,-12.707087,-12.883815,-12.545096,-12.515091,-12.445882,-12.301097,-12.451975,-12.621226,-12.632302,-12.533427,-12.372776,-12.494513,-12.61233,-12.372221,-12.569526,-12.355551,-12.703475,-12.64152,-12.639859,-12.477239,-12.634556,-13.21731,-13.385722,-13.587188,-14.275788,-16.072664,-14.078767,-14.302472,-13.872003,-14.279388,-14.298298,-14.312727,-13.803676,-14.369699,-14.125194,-14.169363,-13.999858,-14.185495,-14.087126,-14.092936,-13.441312,-12.94832,-12.784619,-12.761281,-12.608459,-12.425298,-12.311926,-12.467274,-12.475899,-12.452259,-12.616226,-12.752379,-12.558987,-12.445597,-12.448931,-12.556456,-12.416957,-12.748773,-12.463959,-12.622072,-12.767412,-12.759898,-12.870775,-14.03821,-13.395699,-13.757823,-14.343905,-13.888401,-14.113223,-14.046798,-14.248839,-14.403903,-14.269676,-14.101838,-14.060992,-14.147964,-14.376935,-14.134066,-14.24858,-14.076822,-14.094041,-13.943459,-13.327051,-13.606642,-12.821014,-12.579837,-12.488673,-12.652892,-12.959402,-12.509775,-12.31555,-12.405591,-12.322502,-12.284416,-12.623702,-12.523154,-12.126302,-12.525352,-12.47893,-12.449765,-12.790768,-12.555067,-12.768801,-12.682632,-12.74989,-12.884957,-13.544953,-13.724447,-14.146056,-14.15657,-14.059875,-14.191607,-14.338608,-15.239793,-13.977323,-14.161028,-14.240492,-14.227428,-13.830063,-14.474761,-14.063227,-14.175752,-13.976496,-13.519103,-13.447127,-12.94188,-12.657331,-12.711841,-13.551059,-12.644576,-12.791583,-12.521209,-12.467009,-12.685404,-12.505898,-12.382494,-12.402775,-12.356125,-12.540361,-14.460567,-12.430021,-12.46115,-12.891612,-13.529086,-12.879956,-12.686528,-12.99973,-13.274832,-13.456024,-13.803096,-14.465858,-14.076532,-14.213833,-14.111291,-14.261915,-14.30746,-14.137129,-14.137412,-14.087379,-14.168233,-14.03124,-14.00652,-14.332786,-14.022072,-13.900347,-13.740289,-13.58525,-12.824082,-12.745451,-12.46423,-12.607903,-12.55119,-12.638742,-13.383487,-12.433632,-12.571755,-12.801572,-14.206313,-12.593172,-12.352798,-12.293874,-12.405016,-12.748205,-12.649849,-12.9266,-12.767116,-12.793491,-12.642878,-12.763201,-13.560486,-14.019874,-13.725292,-14.519521,-14.04068,-14.307763,-14.367211,-13.957906,-14.490609,-14.286901,-13.951757,-14.17382,-13.986263,-14.04152,-14.120206,-13.867021,-14.072673,-14.306942,-13.80588,-13.068649,-13.006941,-12.804326,-12.330275,-12.484493,-12.305252,-12.459513,-12.679304,-12.681799,-12.537576,-12.659857,-12.449475,-12.555351,-12.703185,-12.464193,-12.433355,-12.642909,-12.697369,-12.742951,-12.615398,-12.403325,-12.591752,-12.913277,-13.330694,-13.709444,-14.120762,-14.018435,-14.361667,-14.490887,-13.985405,-14.179111,-14.057096,-14.083514,-14.098517,-14.618433,-14.168535,-14.095152,-13.843405,-13.838942,-14.009292,-13.836447,-13.307616,-13.362384,-12.640662,-12.53536,-14.162127,-12.1863,-12.267462,-12.907177,-12.202414,-12.460045,-12.253015,-12.348871,-12.332498,-12.490877,-12.088475,-12.50838,-12.936916,-12.779902,-12.720435,-12.535891,-12.452265,-12.655418,-12.920228,-13.242037,-13.045577,-14.014842,-13.776419,-13.989838,-14.181858,-13.706098,-14.178271,-14.673461,-13.913708,-14.432235,-14.290544,-14.008458,-13.993159,-14.124318,-13.877596,-14.128244,-14.274133,-13.8509,-14.066264,-13.89092,-13.124214,-12.630401,-12.643724,-12.670414,-12.58372,-12.6051,-12.357508,-12.64541,-12.608996,-12.401683,-12.657887,-12.482838,-12.267178,-12.867985,-13.435434,-12.732912,-12.484215,-12.367232,-12.564815,-12.846889,-12.825465,-13.171173,-13.533815,-13.690262,-13.818111,-14.417806,-14.016799,-14.071821,-14.024017,-15.277312,-14.129084,-14.194657,-14.403372,-13.972341,-14.061801,-13.948158,-13.727231,-13.888716,-13.822278,-13.855895,-13.37656,-12.994167,-12.543404,-12.392805,-12.199098,-12.43504,-12.191041,-12.378055,-12.651793,-12.714045,-12.634278,-12.461131,-12.597309,-12.679014,-12.806314,-12.502539,-12.168272,-12.557598,-12.739864,-13.869539,-12.689016,-12.463372,-12.94109,-13.357637,-13.464927,-14.201065,-13.977614,-14.336922,-14.225767,-14.369718,-14.017898,-14.291383,-14.295514,-14.207993,-15.245911,-14.236337,-13.997623,-14.121867,-14.033475,-14.078199,-14.053756,-13.685841,-13.138939,-13.2673,-12.791027,-12.4581,-12.485302,-12.547288,-12.385877,-13.363755,-12.394484,-12.446968,-12.707926,-12.430854,-12.411981,-12.873838,-12.551177,-12.529791,-12.435874,-12.779624,-12.176335,-12.417815,-12.550375,-12.993334,-13.932328,-12.945245,-13.619694,-14.089892,-14.30496,-14.24774,-14.462826,-14.103203,-15.501023,-14.146284,-14.21826,-14.100999,-14.250802,-13.903391,-14.310806,-14.443101,-13.859785,-14.008477,-13.958184,-13.515479,-13.216748,-12.961612,-12.467805,-12.693486,-12.308605,-12.38392,-12.587048,-12.657078,-12.630092,-12.449185,-12.571199,-12.435861,-12.425853,-12.608156,-12.440029,-12.471744,-12.40004,-12.813506,-12.728486,-12.358045,-12.422526,-12.996106,-12.675693,-13.392939,-13.631097,-14.055695,-13.94425,-14.552033,-14.379145,-14.419479,-14.361093,-14.195762,-14.145186,-14.13519,-13.920079,-14.259403,-14.223835,-13.876183,-14.124633,-14.577043,-13.857574,-13.704165,-13.278728,-12.677063,-12.481727,-12.532575,-12.197147,-12.569804,-12.464199,-12.391113,-12.76072,-12.517554,-12.161308,-12.817976,-12.456149,-12.496168,-12.336375,-12.553418,-12.551764,-12.594821,-12.578978,-12.824644,-12.704031,-12.606495,-14.570931,-13.545774,-13.705814,-14.133498,-14.199917,-13.953461,-14.286926,-14.342213,-14.378892,-14.367798,-14.264971,-13.926197,-14.10324,-14.417535,-13.747512,-14.215241,-13.877862,-13.993166,-13.807831,-13.579706,-13.346505,-13.322334,-12.556475,-12.375845,-12.525074,-12.640674,-12.635667,-12.413073,-12.538681,-12.413364,-12.685423,-12.644842,-12.378623,-12.640933,-12.475059,-12.767116,-12.677625,-12.664857,-14.027079,-12.494217,-12.524537,-12.644274,-12.871566,-13.408788,-14.015429,-14.222162,-14.158515,-14.300799,-14.281616,-14.051546,-15.116395,-14.153526,-14.181056,-14.095733,-14.136875,-13.987356,-14.070136,-14.311924,-14.306639,-14.421684,-13.548849,-13.445442,-13.334571,-12.809074,-12.460575,-12.653497,-12.363874,-12.230227,-12.56205,-12.684027,-12.245798,-12.500082,-12.81408,-12.78268,-12.740444,-12.831312,-12.815198,-12.769882,-12.516486,-12.49589,-13.666381,-12.536193,-12.450024,-12.665129,-13.123924,-13.470452,-13.597758,-13.921764,-14.068222,-14.312764,-14.10821,-13.991227,-14.244672,-13.994876,-13.825612,-15.323456,-14.088799,-14.5801,-14.279709,-13.833132,-13.73225,-14.34443,-13.300102,-13.798922,-13.072248,-12.641804,-12.528686,-12.920241,-12.335023,-12.492587,-13.346518,-12.36446,-12.52592,-12.586208,-14.356938,-12.330281,-12.215484,-12.4631,-12.70989,-12.550912,-12.611503,-12.345272,-12.459767,-12.562587,-12.944127,-12.823539,-12.981949,-13.70277,-13.677198,-14.159083,-14.353616,-14.355549,-14.000673,-14.072377,-13.916208,-14.415022,-13.93899,-14.020405,-14.01457,-14.605092,-14.109902,-14.323031,-13.706104,-13.960117,-13.819235,-13.484677,-12.907164,-12.96999,-12.639575,-12.362503,-12.55732,-12.434756,-13.865915,-12.59926,-12.596222,-12.379179,-12.538113,-12.760164,-12.381945,-12.527309,-12.525074,-12.598982,-12.796886,-12.479764,-12.234944,-12.633735,-12.879653,-12.923291,-13.35847,-13.404311,-13.598845,-14.441706,-14.302737,-14.413059,-13.905898,-14.362772,-13.777258,-14.525356,-13.967062,-14.500043,-14.211888,-14.273596,-14.11657,-14.251895,-14.255217,-14.128781,-13.483807,-13.015288,-12.709309,-13.054171,-12.357237,-12.575657,-12.581781,-12.378642,-12.737932,-12.725417,-12.397497,-12.792132,-12.487555,-12.514511,-12.456711,-12.690152,-12.701518,-12.667617,-12.286935,-12.598155,-12.644292,-12.833541,-12.61012,-13.026944,-13.102809,-13.55577,-14.081292,-13.979836,-14.003488,-14.12964,-14.094035,-14.187971,-14.089052,-14.209091,-13.794767,-14.391388,-14.443657,-14.316931,-14.238004,-13.896458,-13.963747,-13.924796,-13.890105,-13.853419,-12.882154,-12.623424,-12.330535,-12.738475,-12.368911,-12.474201,-12.705969,-12.570922,-12.472565,-12.440319,-12.322459,-12.476171,-12.558703,-12.613157,-12.784347,-12.627363,-12.386939,-12.816581,-12.815173,-12.689016,-12.64762,-12.846321,-13.452943,-13.815036,-14.0568,-13.982343,-14.329976,-14.576476,-14.191058,-15.359851,-14.369459,-14.272998,-14.247728,-14.351128,-14.004309,-14.251895,-13.957054,-14.171869,-14.278844,-14.05125,-13.706653,-13.484887,-12.639291,-12.53649,-13.647464,-12.449777,-12.405294,-12.374462,-12.427817,-12.607335,-12.385013,-12.415889,-12.593413,-12.921914,-12.657338,-12.62482,-12.33335,-12.297183,-12.638168,-13.502427,-12.624554,-12.661227,-12.540632,-12.964699,-13.347086,-13.569963,-14.140462,-14.313035,-14.065437,-14.190761,-14.139339,-14.148507,-14.388919,-14.046533,-14.212987,-14.206326,-14.03374,-13.859519,-13.985405,-13.989579,-13.88732,-13.684983,-13.70666,-13.096981,-12.633445,-12.695696,-12.075466,-12.503922,-12.477264,-13.655811,-12.54146,-12.672081,-12.343321,-12.262202,-12.460335,-12.434207,-12.636223,-12.513109,-12.429762,-12.358885,-12.404745,-12.333331,-12.91048,-12.899422,-12.602594,-13.036119,-13.680285,-13.715593,-14.169931,-14.087929,-13.955968,-14.179377,-14.294711,-14.201041,-14.177994,-14.125194,-14.129072,-14.327501,-14.656496,-13.962333,-14.041804,-13.917597,-14.060159,-13.96095,-13.374016,-13.102235,-12.836325,-12.302752,-12.846598,-12.540361,-12.533113,-12.654843,-12.408091,-12.543688,-12.174637,-12.677069,-12.597889,-12.398083,-12.427002,-12.543966,-12.714891,-12.844635,-12.781001,-12.58535,-12.911912,-12.567878,-12.773796,-13.049757,-13.217304,-13.945682,-13.978743,-13.961531,-14.240776,-14.43171,-14.087935,-14.388888,-14.255241,-14.028172,-14.23078,-14.217716,-13.942058,-14.051805,-14.002883,-14.160188,-14.371428,-13.806455,-13.270393,-13.03668,-12.705432,-12.672908,-12.490865,-12.501447,-12.628172,-12.868831,-12.231332,-12.448376,-12.423927,-12.774907,-12.247736,-12.612336,-12.490902,-12.321656,-12.847444,-12.385569,-12.713193,-12.777932,-12.836609,-12.674841,-12.644848,-13.126696,-13.693596,-13.783339,-13.983164,-14.113804,-14.204128,-14.094584,-14.167418,-13.943163,-13.922024,-14.497264,-14.167986,-14.135468,-13.993437,-13.909824,-14.410601,-14.485361,-14.052361,-13.480207,-13.989838,-12.95358,-12.526729,-12.563692,-12.278569,-12.513683,-12.672075,-12.562006,-12.57704,-12.635667,-12.696264,-12.339153,-12.699048,-12.231907,-12.62595,-13.668869,-12.628154,-12.383099,-12.78518,-12.43588,-12.854384,-12.880191,-13.221484,-13.127005,-13.738079,-13.852271,-14.282197,-14.176845,-14.227434,-14.124349,-15.067233,-14.23467,-14.562597,-14.103783,-13.716143,-14.298866,-14.008736,-13.973156,-13.844202,-14.181321,-13.81921,-13.720279,-13.275394,-12.789329,-12.43475,-12.330825,-12.729862,-12.732925,-12.766838,-12.301949,-12.284434,-12.566476,-12.385032,-12.478924,-12.288589,-12.325812,-12.563161,-12.272735,-12.64707,-12.405035,-13.585521,-12.661246,-12.753224,-12.589258,-12.835226,-13.560221,-13.432397,-13.806152,-14.473087,-14.089071,-14.330261,-14.478644,-13.945972,-14.219118,-14.415855,-14.107963,-13.775604,-14.363877,-14.191848,-14.023208,-13.875658,-14.137394,-13.995116,-13.464062,-13.2034,-12.813235,-12.58038,-12.482548,-12.560086,-12.432824,-13.396279,-12.924674,-12.447845,-12.760201,-12.579843,-12.227455,-12.462829,-12.520635,-12.682095,-12.352199,-12.244971,-12.467817,-12.874653,-12.884389,-12.928322,-13.718044,-13.124492,-13.188404,-13.780074,-13.856185,-14.241875,-14.223545,-14.02598,-14.207147,-14.309701,-14.151026,-14.083181,-13.968995,-14.432531,-14.172443,-14.023757,-14.121033,-13.877312,-14.145747,-13.714155,-13.388753,-13.11365,-13.101136,-12.568711,-12.690973,-12.454507,-12.561766,-12.472818,-12.15995,-12.47614,-12.237445,-12.269407,-12.304981,-12.876894,-12.61872,-12.557864,-12.450895,-12.661536,-12.468114,-12.659029,-12.381692,-12.689602,-12.919142,-12.797967,-13.222589,-13.931204,-13.815333,-13.993159,-14.319987,-14.112939,-14.299965,-14.551212,-13.797268,-14.049305,-14.423628,-14.01291,-14.314393,-14.225804,-13.760595,-13.939274,-14.241313,-13.796434,-13.516868,-13.416023,-12.557574,-12.652077,-12.38221,-12.546461,-12.454235,-12.855464,-12.809061,-12.677921,-12.522864,-12.520919,-12.332189,-12.222714,-12.531458,-12.661233,-12.206884,-12.615948,-12.752101,-12.578707,-12.499224,-12.71431,-12.668191,-13.066414,-13.501044,-13.853413,-14.087676,-13.876195,-13.814227,-14.477545,-14.438909,-14.035975,-14.090145,-14.155724,-14.161034,-14.258279,-14.17992,-13.758638,-13.96676,-13.795903,-14.244678,-13.978163,-13.411547,-13.161449,-12.750174,-12.560358,-12.536477,-12.755725,-12.147954,-12.445857,-12.365849,-12.558981,-12.335276,-12.540645,-12.379734,-12.653467,-12.768801,-12.423637,-12.360027,-12.68817,-12.367788,-12.774895,-12.687923,-12.452253,-12.742093,-13.54436,-13.462939,-13.95038,-14.02209,-14.0857,-14.094078,-14.263866,-14.821579,-14.07768,-13.796138,-14.338608,-14.219686,-13.90039,-14.134369,-14.027943,-13.988461,-14.071272,-13.914535,-13.872021,-13.609414,-13.026957,-12.740704,-12.506719,-12.417506,-12.301653,-12.103514,-12.503138,-12.421692,-12.514511,-12.706513,-12.698752,-12.329973,-12.866305,-12.448079,-12.522567,-12.843252,-12.752113,-13.343715,-12.712372,-12.389187,-12.885482,-12.945276,-12.976652,-13.404052,-14.081848,-14.077384,-14.569814,-14.333878,-13.707481,-13.764478,-14.5801,-13.796459,-15.258142,-14.088756,-14.213259,-14.040989,-14.198824,-14.499203,-14.037914,-13.937033,-13.644433,-13.434878,-12.783236,-12.667086,-12.39223,-12.552863,-12.377228,-13.217304,-12.460038,-12.698764,-12.719879,-12.291633,-12.442807,-12.681274,-12.692362,-12.203297,-12.708488,-12.277211,-12.538132,-12.567304,-12.595382,-12.791015,-12.648466,-12.944961,-13.264565,-13.446825,-14.053201,-14.226644,-14.185452,-14.065721,-14.426691,-14.382523,-14.266916,-13.885376,-14.113791,-13.952634,-14.287481,-14.2591,-13.939533,-13.924259,-14.378374,-13.702233,-13.68752,-13.270931,-12.662888,-12.419476,-12.882129,-12.670704,-12.442264,-12.240476,-12.442819,-12.563408,-12.494223,-12.200216,-12.968854,-12.278865,-12.486994,-12.569823,-12.91106,-12.590919,-12.636779,-12.635945,-12.789891,-12.661795,-12.814908,-12.852982,-13.530191,-13.74834,-14.239967,-14.398599,-14.232454,-14.052083,-14.30136,-14.394191,-14.254976,-14.290562,-14.074081,-14.028178,-14.345566,-14.4442,-14.551743,-13.906743,-14.012626,-13.647483,-13.279265,-13.086133,-13.260379,-12.494229,-12.371677,-12.457544,-12.761849,-12.779908,-12.79325,-12.363034,-12.372227,-12.798541,-12.487271,-12.474769,-12.510331,-12.253003,-12.634006,-12.477548,-12.639304,-12.864373,-12.808234,-12.253003,-12.683484,-13.391562,-13.271492,-13.741987,-14.236337,-14.191866,-14.348332,-14.254118,-14.162423,-14.024035,-14.381677,-14.331112,-14.218556,-14.007347,-14.081563,-13.777851,-14.236899,-13.849505,-14.098233,-13.646365,-13.72557,-13.415153,-12.679298,-12.573694,-12.645416,-12.496717,-12.505626,-12.360824,-12.174644,-12.469484,-12.54396,-12.463409,-12.465298,-12.260807,-12.919679,-12.533125,-12.685126,-12.483968,-12.587313,-12.612311,-12.661499,-12.391668,-12.911634,-12.901886,-13.433242,-13.971798,-14.376367,-14.285247,-14.28358,-13.996506,-15.532164,-14.185766,-14.418121,-14.129047,-13.688619,-13.868113,-14.55483,-14.299984,-13.838411,-14.190483,-13.914553,-13.810591,-13.569389,-13.1745,-12.701808,-13.308702,-12.274976,-12.626524,-12.786008,-12.141854,-12.422229,-12.61291,-12.606767,-12.572613,-12.458946,-12.304431,-12.416697,-14.247444,-12.859378,-12.569835,-13.693318,-12.571483,-12.635686,-12.813506,-13.063611,-13.482133,-13.751143,-13.67776,-14.165751,-13.975125,-14.251611,-13.847554,-14.297465,-14.092133,-14.139339,-13.99816,-14.127127,-14.03208,-14.612346,-14.190199,-13.924549,-14.172419,-13.916788,-13.729731,-13.584132,-12.936089,-12.825724,-12.499804,-12.38087,-12.473127,-13.772794,-12.54259,-12.403072,-12.538144,-12.391409,-13.356266,-12.519493,-12.560938,-12.511195,-12.527593,-12.698764,-12.634828,-12.913845,-12.284675,-12.7496,-12.647632,-12.907455,-13.662751,-13.394359,-13.984843,-14.395012,-14.16743,-14.219099,-14.399735,-14.191872,-14.453924,-14.374459,-14.301083,-14.044026,-14.576747,-13.880344,-13.998166,-14.121861,-14.390542,-14.083786,-13.688891,-13.420728,-13.234245,-12.921611,-12.635408,-12.572329,-12.645965,-12.463391,-12.531773,-12.83606,-12.268326,-12.52784,-12.696789,-12.472837,-12.609842,-12.767665,-12.384723,-12.589536,-12.468916,-12.593981,-12.482295,-12.655689,-12.689565,-13.071952,-13.106421,-13.67111,-14.230503,-14.441687,-13.976515,-14.126269,-14.046823,-13.97181,-14.278332,-14.293587,-14.525072,-14.259403,-14.020417,-14.147136,-14.010983,-13.901477,-13.93568,-14.144889,-13.870638,-13.559116,-13.086152,-12.422803,-12.972744,-12.725991,-12.631222,-12.830787,-12.469478,-12.590666,-12.638427,-12.895483,-12.591493,-12.501163,-12.602044,-12.405584,-12.477541,-12.677921,-12.764078,-12.79354,-12.682638,-12.561482,-12.65706,-12.874665,-13.475472,-13.756965,-14.363322,-14.292205,-14.34167,-14.31887,-14.268867,-14.247191,-14.065987,-14.108241,-14.189372,-14.752135,-14.479206,-14.259693,-14.431161,-14.228008,-13.97344,-13.900619,-14.885763,-13.240363,-13.185385,-12.732943,-13.008892,-12.740451,-12.45505,-12.445326,-12.37445,-12.603995,-12.702635,-12.62598,-12.566754,-12.715693,-12.270808,-13.511583,-12.328577,-12.398058,-12.659585,-12.392502,-12.655411,-12.837677,-12.903003,-13.066402,-13.424333,-13.645266,-13.841436,-14.192441,-14.488954,-14.351394,-15.091138,-13.742839,-14.343874,-14.419757,-14.449466,-13.975965,-14.291661,-13.948738,-13.961512,-14.195472,-14.116835,-14.039896,-13.379622,-13.172012,-12.647052,-12.677619,-12.325262,-12.336097,-12.718502,-12.213014,-12.39307,-12.589246,-12.718478,-12.39031,-12.382253,-12.314155,-12.348309,-12.41587,-12.681799,-12.722096,-13.455734,-12.442264,-12.888266,-12.818797,-12.887994,-13.119485,-13.417116,-13.577162,-14.24219,-14.313597,-14.165751,-14.243276,-14.365248,-14.145192,-14.413614,-14.032364,-15.871185,-14.</t>
   </si>
 </sst>
 </file>
@@ -426,7 +462,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -457,22 +493,22 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>0.2393</v>
+        <v>0.2515</v>
       </c>
       <c r="C2">
-        <v>0.2465</v>
+        <v>0.2594</v>
       </c>
       <c r="D2">
-        <v>0.2313</v>
+        <v>0.2466</v>
       </c>
       <c r="E2">
-        <v>0.0049</v>
+        <v>0.0036</v>
       </c>
       <c r="F2">
         <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -480,22 +516,22 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>8.3785</v>
+        <v>8.4458</v>
       </c>
       <c r="C3">
-        <v>8.3981</v>
+        <v>8.4728</v>
       </c>
       <c r="D3">
-        <v>8.3554</v>
+        <v>8.417</v>
       </c>
       <c r="E3">
-        <v>0.0129</v>
+        <v>0.0109</v>
       </c>
       <c r="F3">
-        <v>10</v>
+        <v>6000</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -503,22 +539,22 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>0.2398</v>
+        <v>11.5345</v>
       </c>
       <c r="C4">
-        <v>0.2456</v>
+        <v>12.4969</v>
       </c>
       <c r="D4">
-        <v>0.236</v>
+        <v>11.1622</v>
       </c>
       <c r="E4">
-        <v>0.0031</v>
+        <v>0.251</v>
       </c>
       <c r="F4">
-        <v>10</v>
+        <v>6000</v>
       </c>
       <c r="G4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -526,22 +562,114 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>0.5613</v>
+        <v>12.2889</v>
       </c>
       <c r="C5">
-        <v>3.4334</v>
+        <v>13.7865</v>
       </c>
       <c r="D5">
-        <v>0.2377</v>
+        <v>11.7862</v>
       </c>
       <c r="E5">
-        <v>0.9574</v>
+        <v>0.3297</v>
       </c>
       <c r="F5">
+        <v>6000</v>
+      </c>
+      <c r="G5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G5" t="s">
+      <c r="B6">
+        <v>10.0009</v>
+      </c>
+      <c r="C6">
+        <v>10.9102</v>
+      </c>
+      <c r="D6">
+        <v>9.808</v>
+      </c>
+      <c r="E6">
+        <v>0.1141</v>
+      </c>
+      <c r="F6">
+        <v>6000</v>
+      </c>
+      <c r="G6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>11.6186</v>
+      </c>
+      <c r="C7">
+        <v>12.5187</v>
+      </c>
+      <c r="D7">
+        <v>11.2583</v>
+      </c>
+      <c r="E7">
+        <v>0.2541</v>
+      </c>
+      <c r="F7">
+        <v>6000</v>
+      </c>
+      <c r="G7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>12.3868</v>
+      </c>
+      <c r="C8">
+        <v>13.5615</v>
+      </c>
+      <c r="D8">
+        <v>11.9225</v>
+      </c>
+      <c r="E8">
+        <v>0.3325</v>
+      </c>
+      <c r="F8">
+        <v>6000</v>
+      </c>
+      <c r="G8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="1" t="s">
         <v>13</v>
+      </c>
+      <c r="B9">
+        <v>10.0159</v>
+      </c>
+      <c r="C9">
+        <v>10.7365</v>
+      </c>
+      <c r="D9">
+        <v>9.8385</v>
+      </c>
+      <c r="E9">
+        <v>0.1126</v>
+      </c>
+      <c r="F9">
+        <v>6000</v>
+      </c>
+      <c r="G9" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -551,7 +679,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -582,22 +710,22 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>-0.1002</v>
+        <v>-0.1053</v>
       </c>
       <c r="C2">
-        <v>-0.0857</v>
+        <v>-0.0829</v>
       </c>
       <c r="D2">
-        <v>-0.1302</v>
+        <v>-0.1308</v>
       </c>
       <c r="E2">
-        <v>0.0179</v>
+        <v>0.0194</v>
       </c>
       <c r="F2">
         <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -605,22 +733,22 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>-5.5106</v>
+        <v>-5.5377</v>
       </c>
       <c r="C3">
-        <v>-5.506</v>
+        <v>-5.5194</v>
       </c>
       <c r="D3">
-        <v>-5.5191</v>
+        <v>-5.555</v>
       </c>
       <c r="E3">
-        <v>0.004</v>
+        <v>0.0055</v>
       </c>
       <c r="F3">
-        <v>10</v>
+        <v>6000</v>
       </c>
       <c r="G3" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -628,22 +756,22 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>-0.4344</v>
+        <v>-8.2374</v>
       </c>
       <c r="C4">
-        <v>-0.0807</v>
+        <v>-7.8184</v>
       </c>
       <c r="D4">
-        <v>-3.4452</v>
+        <v>-10.0465</v>
       </c>
       <c r="E4">
-        <v>1.0038</v>
+        <v>0.2708</v>
       </c>
       <c r="F4">
-        <v>10</v>
+        <v>6000</v>
       </c>
       <c r="G4" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -651,22 +779,114 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>-0.101</v>
+        <v>-8.59</v>
       </c>
       <c r="C5">
-        <v>-0.083</v>
+        <v>-8.1274</v>
       </c>
       <c r="D5">
-        <v>-0.1319</v>
+        <v>-10.0323</v>
       </c>
       <c r="E5">
-        <v>0.018</v>
+        <v>0.3089</v>
       </c>
       <c r="F5">
+        <v>6000</v>
+      </c>
+      <c r="G5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G5" t="s">
-        <v>17</v>
+      <c r="B6">
+        <v>-13.1749</v>
+      </c>
+      <c r="C6">
+        <v>-11.7034</v>
+      </c>
+      <c r="D6">
+        <v>-16.0924</v>
+      </c>
+      <c r="E6">
+        <v>0.8015</v>
+      </c>
+      <c r="F6">
+        <v>6000</v>
+      </c>
+      <c r="G6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>-8.3119</v>
+      </c>
+      <c r="C7">
+        <v>-7.917</v>
+      </c>
+      <c r="D7">
+        <v>-9.6105</v>
+      </c>
+      <c r="E7">
+        <v>0.2716</v>
+      </c>
+      <c r="F7">
+        <v>6000</v>
+      </c>
+      <c r="G7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>-8.6921</v>
+      </c>
+      <c r="C8">
+        <v>-8.2752</v>
+      </c>
+      <c r="D8">
+        <v>-10.3139</v>
+      </c>
+      <c r="E8">
+        <v>0.3113</v>
+      </c>
+      <c r="F8">
+        <v>6000</v>
+      </c>
+      <c r="G8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>-13.285</v>
+      </c>
+      <c r="C9">
+        <v>-12.0621</v>
+      </c>
+      <c r="D9">
+        <v>-16.0727</v>
+      </c>
+      <c r="E9">
+        <v>0.7805</v>
+      </c>
+      <c r="F9">
+        <v>6000</v>
+      </c>
+      <c r="G9" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sync excel writer module
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -7,15 +7,64 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="3_3" sheetId="1" r:id="rId1"/>
-    <sheet name="1_8" sheetId="2" r:id="rId2"/>
+    <sheet name="Version" sheetId="1" r:id="rId1"/>
+    <sheet name="3_3" sheetId="2" r:id="rId2"/>
+    <sheet name="1_8" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="28">
+  <si>
+    <t>WLAN Version</t>
+  </si>
+  <si>
+    <t>BT Version</t>
+  </si>
+  <si>
+    <t>Hardware</t>
+  </si>
+  <si>
+    <t>DUT MAC address</t>
+  </si>
+  <si>
+    <t>DUT BD address</t>
+  </si>
+  <si>
+    <t>REF BD address</t>
+  </si>
+  <si>
+    <t>Test Engineer</t>
+  </si>
+  <si>
+    <t>Start Time</t>
+  </si>
+  <si>
+    <t>End Time</t>
+  </si>
+  <si>
+    <t>Run Time</t>
+  </si>
+  <si>
+    <t>xx.xx.xx.xx.xx.xx</t>
+  </si>
+  <si>
+    <t>Robin3 WIB module</t>
+  </si>
+  <si>
+    <t>00:50:43:22:0E:37</t>
+  </si>
+  <si>
+    <t>00:1B:DC:06:69:91</t>
+  </si>
+  <si>
+    <t>Alex Wang</t>
+  </si>
+  <si>
+    <t>Information</t>
+  </si>
   <si>
     <t>1.Average (mA)</t>
   </si>
@@ -41,26 +90,49 @@
     <t>BT Idle</t>
   </si>
   <si>
-    <t>0.579951,0.572253,0.583952,0.573646,0.609944,0.587851,0.6144,0.616812,0.572532,0.615508</t>
-  </si>
-  <si>
-    <t>9.842115,9.835627,9.826714,9.838406,9.849364,9.835899,9.827075,9.828379,9.844711,9.849085</t>
-  </si>
-  <si>
-    <t>0.005577,-0.006306,0.002814,-0.001336,-0.0058,0.0006,-0.001071,-0.003001,-0.000534,-0.002458</t>
-  </si>
-  <si>
-    <t>0.006175,-0.003858,-0.001607,-0.005239,-0.001077,0.002826,-0.001311,0.002241,-0.004148,-0.00247</t>
+    <t>0.61402,0.612172,0.601316,0.62601,0.647729,0.630277,0.607709,0.610684,0.609115,0.610121</t>
+  </si>
+  <si>
+    <t>9.885376,9.888637,9.906361,9.898759,9.895125,9.885845,9.892625,9.908128,9.905241,9.891783</t>
+  </si>
+  <si>
+    <t>-0.001367,-0.003549,-0.001885,-0.000787,-0.000238,0.001439,-0.004141,-0.009401,0.001149,-0.005504</t>
+  </si>
+  <si>
+    <t>0.00475,-0.002748,0.002006,-0.003278,-0.002729,-0.005202,-0.00802,0.002,-0.003007,-0.004665</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF464646"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF464646"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -74,20 +146,53 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF22798E"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDCE6F1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF2DA2BF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF2DA2BF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF2DA2BF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF2DA2BF"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -109,9 +214,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -408,79 +522,106 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:H4"/>
+  <dimension ref="B2:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="88.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:8">
-      <c r="C2" s="1" t="s">
+    <row r="2" spans="2:3">
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="2:3">
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="C3" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3">
+      <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
+      <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="C5" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3">
+      <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="C6" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3">
+      <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="C7" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3">
+      <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="2:8">
-      <c r="B3" s="1" t="s">
+      <c r="C8" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3">
+      <c r="B9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3">
-        <v>0.5927</v>
-      </c>
-      <c r="D3">
-        <v>0.6168</v>
-      </c>
-      <c r="E3">
-        <v>0.5723</v>
-      </c>
-      <c r="F3">
-        <v>0.0182</v>
-      </c>
-      <c r="G3">
-        <v>10</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="C9" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3">
+      <c r="B10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1.486771836083502e+18</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3">
+      <c r="B11" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="2:8">
-      <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4">
-        <v>9.8377</v>
-      </c>
-      <c r="D4">
-        <v>9.849399999999999</v>
-      </c>
-      <c r="E4">
-        <v>9.826700000000001</v>
-      </c>
-      <c r="F4">
-        <v>0.0081</v>
-      </c>
-      <c r="G4">
-        <v>10</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="C11" s="3">
+        <v>1.486771859481514e+18</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3">
+      <c r="B12" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="C12" s="3">
+        <v>23398012000</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:C2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -494,69 +635,148 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="2" spans="2:8">
-      <c r="C2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>5</v>
+      <c r="C2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="2:8">
-      <c r="B3" s="1" t="s">
-        <v>6</v>
+      <c r="B3" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="C3">
-        <v>-0.0012</v>
+        <v>0.6169</v>
       </c>
       <c r="D3">
-        <v>0.0056</v>
+        <v>0.6477000000000001</v>
       </c>
       <c r="E3">
-        <v>-0.0063</v>
+        <v>0.6012999999999999</v>
       </c>
       <c r="F3">
-        <v>0.0034</v>
+        <v>0.0131</v>
       </c>
       <c r="G3">
         <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="2:8">
-      <c r="B4" s="1" t="s">
-        <v>7</v>
+      <c r="B4" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="C4">
-        <v>-0.0008</v>
+        <v>9.895799999999999</v>
       </c>
       <c r="D4">
-        <v>0.0062</v>
+        <v>9.908099999999999</v>
       </c>
       <c r="E4">
-        <v>-0.0052</v>
+        <v>9.885400000000001</v>
       </c>
       <c r="F4">
-        <v>0.0034</v>
+        <v>0.008</v>
       </c>
       <c r="G4">
         <v>10</v>
       </c>
       <c r="H4" t="s">
-        <v>11</v>
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:H4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="2" spans="2:8">
+      <c r="C2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8">
+      <c r="B3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3">
+        <v>-0.0024</v>
+      </c>
+      <c r="D3">
+        <v>0.0014</v>
+      </c>
+      <c r="E3">
+        <v>-0.0094</v>
+      </c>
+      <c r="F3">
+        <v>0.0031</v>
+      </c>
+      <c r="G3">
+        <v>10</v>
+      </c>
+      <c r="H3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8">
+      <c r="B4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4">
+        <v>-0.0021</v>
+      </c>
+      <c r="D4">
+        <v>0.0047</v>
+      </c>
+      <c r="E4">
+        <v>-0.008</v>
+      </c>
+      <c r="F4">
+        <v>0.0037</v>
+      </c>
+      <c r="G4">
+        <v>10</v>
+      </c>
+      <c r="H4" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
restructure all folders complete
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -63,10 +63,10 @@
     <t>Alex Wang</t>
   </si>
   <si>
-    <t>23:56:43 03-01-2017 Wednesday Pacific Standard Time</t>
-  </si>
-  <si>
-    <t>23:57:36 03-01-2017 Wednesday Pacific Standard Time</t>
+    <t>23:09:56 03-02-2017 Thursday Pacific Standard Time</t>
+  </si>
+  <si>
+    <t>23:10:50 03-02-2017 Thursday Pacific Standard Time</t>
   </si>
   <si>
     <t>0:0:53 0 days</t>
@@ -102,22 +102,22 @@
     <t>BT Page Scan</t>
   </si>
   <si>
-    <t>-0.56944,-0.559134,-0.559976,-0.56944,-0.568516,-0.561641,-0.583923,-0.570275,-0.570017,-0.563319,-0.563957,-0.55607,-0.562571,-0.568142,-0.569922,-0.56573,-0.56359,-0.569915,-0.597476,-0.568237,-0.566009,-0.592748,-0.564616,-0.576783,-0.562666,-0.566477,-0.563882,-0.559881,-0.570839,-0.575017,-0.558584,-0.568699,-0.569073,-0.553101,-0.584766,-0.568332,-0.564705,-0.557938,-0.560065,-0.569364,-0.559046,-0.584861,-0.574738,-0.559691,-0.566756,-0.571199,-0.557096,-0.57715,-0.567035,-0.560078,-0.570377,-0.578278,-0.559046,-0.569263,-0.568692,-0.560527,-0.568434,-0.562857,-0.561375,-0.5702,-0.5648,-0.556457,-0.556722,-0.564983,-0.573067,-0.565268,-0.571389,-0.565458,-0.59552,-0.569636,-0.566851,-0.561634,-0.563509,-0.560717,-0.567877,-0.556722,-0.578353,-0.559046,-0.566756,-0.566382,-0.55645,-0.560717,-0.56944,-0.557564,-0.570655,-0.555526,-0.560527,-0.562204,-0.559229,-0.572972,-0.559799,-0.562945,-0.570472,-0.564059,-0.596926,-0.562299,-0.567116,-0.567768,-0.55664,-0.55162</t>
-  </si>
-  <si>
-    <t>-9.728567,-9.747494,-9.738676,-9.72763,-9.727997,-9.734783,-9.742582,-9.738303,-9.728656,-9.721787,-9.73979,-9.745082,-9.733941,-9.717704,-9.724288,-9.749356,-9.742848,-9.730966,-9.722793,-9.728282,-9.74388,-9.737385,-9.72104,-9.729586,-9.738683,-9.748703,-9.736081,-9.725864,-9.738113,-9.740171,-9.740993,-9.730789,-9.727548,-9.731156,-9.738316,-9.737202,-9.728751,-9.734036,-9.738126,-9.738398,-9.732358,-9.721509,-9.734505,-9.735898,-9.735898,-9.727351,-9.717976,-9.734688,-9.740259,-9.734315,-9.714546,-9.72744,-9.735612,-9.744804,-9.729016,-9.718337,-9.728377,-9.74119,-9.738208,-9.728289,-9.719736,-9.730599,-9.737759,-9.735993,-9.719179,-9.728744,-9.742209,-9.740259,-9.737107,-9.728561,-9.731896,-9.737093,-9.739974,-9.721787,-9.716597,-9.737284,-9.733574,-9.727718,-9.72085,-9.728934,-9.738683,-9.740986,-9.733574,-9.728744,-9.735239,-9.743329,-9.740809,-9.730137,-9.715008,-9.740266,-9.737752,-9.73636,-9.726142,-9.732087,-9.742399,-9.738119,-9.730143,-9.722888,-9.730599,-9.744437</t>
-  </si>
-  <si>
-    <t>-0.572048,-0.566111,-0.569073,-0.563964,-0.595166,-0.563882,-0.570649,-0.561559,-0.570839,-0.568522,-0.567123,-0.568054,-0.565635,-0.560058,-10.281401,-0.566668,-0.563407,-0.561919,-0.571111,-0.569351,-0.566382,-0.567598,-0.56323,-0.594419,-0.5648,-0.571308,-0.570934,-0.565262,-0.597945,-0.5634,-0.592001,-0.566111,-0.56573,-0.562666,-0.56535,-0.571484,-0.562666,-0.581702,-0.564711,-0.562768,-0.582904,-0.572137,-0.590146,-0.5648,-0.560907,-0.587272,-0.570751,-0.568047,-0.563509,-0.568801,-0.574086,-0.557096,-9.146671,-0.567402,-0.57037,-0.561559,-0.560907,-0.571213,-0.563686,-0.552272,-0.564983,-0.564066,-0.561179,-0.561926,-0.563774,-0.571491,-0.586899,-0.570377,-0.568991,-0.556539,-0.559603,-0.591729,-0.564256,-0.549861,-0.565186,-0.56592,-0.564623,-0.571668,-0.561274,-0.577802,-0.566477,-0.561002,-0.565825,-0.560717,-0.559976,-0.564623,-0.573067,-0.564256,-0.593672,-0.57177,-7.824211,-0.560166,-0.563964,-0.5766,-0.55412,-0.56342,-0.566104,-0.55895,-0.563869,-0.562571</t>
-  </si>
-  <si>
-    <t>0.000859,0.002543,0.001717,-0.001613,0.003092,-0.001095,-0.003543,0.003665,0.003381,0.002265,-0.00244,0.003344,0.004195,-0.001064,0.000588,0.001686,0.004183,0.009751,0.003381,-0.001897,0.000619,-0.001323,-0.004135,2.1e-05,0.000607,0.003388,0.001143,0.001969,0.003079,-0.003858,0.004467,0.006976,-0.005504,-0.000793,0.003085,0.000329,0.000341,0.001988,0.00364,0.004738,0.004497,0.00948,0.000588,0.000323,0.002512,-0.001354,-0.00022,-0.000522,-0.001354,-0.003852,-0.004413,0.005842,0.00089,0.000594,0.000304,0.002012,0.001408,0.003085,-0.000781,-0.003013,-0.002458,-0.003568,-0.004665,0.003344,-0.001071,0.009202,0.002524,-0.000812,0.005614,-0.000207,-0.002476,-0.002181,0.004467,-0.002723,-0.004672,0.000563,-0.001342,0.001698,0.001162,0.005324,0.002808,2.1e-05,-0.000516,0.003653,0.00311,0.003079,0.004195,0.001162,-0.001885,-0.003568,0.005046,-0.001058,0.000853,0.001433,0.001168,0.00644,-0.000238,0.003653,-0.00662,-0.000503</t>
-  </si>
-  <si>
-    <t>-0.002458,-0.000799,-0.003556,0.002247,0.004208,-0.001071,0.002814,-0.005245,-0.000232,0.000588,0.001162,0.006693,0.00446,-0.0072,4.5e-05,-0.001632,0.005595,3.9e-05,-0.002193,-0.001903,-0.000244,0.001131,0.002247,0.002808,-0.000793,0.000613,0.003893,5.2e-05,0.002537,0.000311,-0.00244,0.00562,-0.000522,-0.004678,-0.000812,3.9e-05,-0.000251,-0.000812,-0.004665,0.005311,-0.002174,0.003357,-0.00522,-0.000263,0.000872,-0.000516,-0.001095,0.001994,0.007248,0.00446,0.001155,-0.006602,-0.001897,-0.003019,0.00837,0.001704,0.007556,-0.002218,0.002537,0.003936,-0.003297,0.003092,0.001975,0.004479,0.00229,-0.00329,0.003949,3.3e-05,0.000594,0.002543,0.000853,-0.002181,-0.001644,0.001975,0.003363,-0.001348,0.003104,0.002537,0.006415,0.006409,0.002789,0.00393,0.003351,-0.002181,-0.000522,0.008074,-0.00329,0.000847,-0.000244,-0.004388,0.003659,0.001445,0.000576,-0.000251,-0.003303,0.004769,0.005601,0.001421,-0.000226,0.006674</t>
-  </si>
-  <si>
-    <t>-0.000509,-0.003543,0.000335,-0.000263,-0.002174,0.001421,0.008388,0.000853,0.005885,0.000304,-0.001336,0.001155,0.003616,0.001698,-0.002199,-0.000522,-0.004986,0.000329,0.008641,-0.001342,-0.002452,5.8e-05,-0.00136,0.00504,0.003073,-0.000793,-0.002174,0.006415,-0.00247,-0.000244,0.00504,-0.000516,0.001982,0.003653,0.006409,-0.003568,-0.004943,0.001149,-0.001903,0.000311,-0.001071,0.000613,0.003067,-0.001897,0.001433,2.7e-05,-0.000251,-0.002187,0.001137,4.5e-05,-0.003574,0.005848,0.005028,0.004738,-0.004955,0.001704,-0.003833,-0.002729,0.003943,-0.001619,0.000619,-0.004968,0.001988,0.000607,-0.000226,-0.00276,-0.001891,-0.001089,0.001445,0.001963,-0.00329,-0.003019,-0.001354,-0.003562,3.9e-05,0.00253,-0.005245,-0.002483,0.007241,0.006995,-0.006885,-0.000257,-0.00247,-0.00165,0.002241,0.003659,0.006686,0.001433,0.003388,-0.001613,0.005848,0.001969,0.004473,0.002814,-0.003549,0.002524,0.000329,0.005281,-0.001903,0.000878</t>
+    <t>0.0,0.003628,0.028967,-0.004178,0.026087,0.003709,-0.002235,0.022004,0.005102,0.024226,-0.007982,0.029429,0.002595,0.022371,-0.000279,0.026746,-0.002697,0.025713,-0.00195,0.040381,0.00157,0.025441,0.009654,0.033879,0.002228,-0.001773,0.012989,-0.003716,0.025815,0.00409,0.033791,-0.006596,0.0064,0.029715,-0.00716,0.033981,0.00269,0.006406,0.03481,-0.001494,0.033417,0.002867,-9.5e-05,0.028587,0.007609,0.0,0.029056,-0.002975,0.031651,0.001108,0.03324,0.000374,0.024314,-0.003893,0.033519,-0.004742,0.029626,-0.000924,0.010014,0.006324,0.003166,-0.00214,-0.005,-0.010856,-0.001678,0.017643,0.03017,-0.000374,0.024511,0.007976,0.008825,-0.000469,0.001209,0.035727,0.007432,0.019402,0.003064,0.021345,0.000177,0.047901,-0.00659,0.029157,-0.001855,0.035557,0.009457,-0.008084,0.003804,-0.009572,0.027663,-0.005476,0.029898,0.005102,0.005285,0.003519,0.028967,-0.004273,0.017921,0.004178,0.034069,-0.003152</t>
+  </si>
+  <si>
+    <t>0.0,-0.013091,-0.006128,0.007989,0.012357,0.011053,0.010679,0.011426,0.030829,0.026828,0.016712,0.009293,0.026359,0.040204,0.028872,0.02163,0.026087,0.036766,0.0404,0.033424,0.022194,0.039185,0.051617,0.05663,0.029443,0.032677,0.040666,0.050047,0.042248,0.028594,0.035469,0.046882,0.054877,0.039463,0.030544,0.040014,0.045591,0.050971,0.026644,0.046325,0.043166,0.047541,0.044198,0.026644,0.040197,0.048186,0.052833,0.031759,0.029905,0.036678,0.051624,0.040279,0.037146,0.030544,0.037133,0.061739,0.04159,0.030544,0.034443,0.050686,0.047534,0.045964,0.021726,0.043077,0.052453,0.042248,0.028791,0.036576,0.047629,0.052187,0.040109,0.029531,0.039457,0.054864,0.049661,0.024517,0.035007,0.043825,0.050598,0.036399,0.029993,0.030639,0.042615,0.043356,0.035652,0.03193,0.045027,0.051624,0.049851,0.029891,0.034633,0.04252,0.048471,0.040489,0.024144,0.030448,0.043268,0.049022,0.046141,0.029898</t>
+  </si>
+  <si>
+    <t>0.0,0.032582,0.007602,0.036855,0.000924,0.015319,0.018193,0.03036,0.006868,0.042153,0.011046,0.001203,0.037507,0.038159,-8.532837,0.015781,0.008539,0.030645,0.008172,0.009654,0.040564,-0.004083,0.033791,0.015509,0.035279,0.002317,0.001671,0.034721,0.009015,0.001304,0.04661,0.008077,0.012629,0.031753,-0.000747,0.034348,0.00966,0.009565,0.035931,0.03788,0.005951,0.038342,0.003437,0.031019,0.00928,0.032215,0.005109,0.038995,0.00966,0.008635,0.036943,0.0118,-7.341299,0.033886,0.005115,0.004837,0.029429,0.013825,0.002595,0.012439,0.008077,0.033417,0.007609,0.036868,0.006678,0.002323,0.035177,0.0168,0.006501,0.032955,0.00269,0.007153,0.006216,0.007439,0.044742,0.014756,0.003532,0.002127,0.042602,0.006773,0.010958,0.005292,0.03676,0.017086,0.006318,0.019782,0.03964,0.002684,0.001481,0.039185,-6.119939,0.039552,0.00428,0.043261,0.005666,0.005,0.011793,0.041773,-0.001386,0.030822</t>
+  </si>
+  <si>
+    <t>0.0,0.001986,0.003361,0.004717,-0.004144,-0.002177,-0.002732,-0.000247,-0.005266,-0.000506,-0.002183,-0.003848,-0.002466,-0.00024,-0.003552,-0.00053,0.00029,0.00394,0.00365,-0.000814,0.005309,-0.003058,0.000561,-0.00053,0.001696,0.003077,0.00558,4.9e-05,-0.003835,1.8e-05,0.001979,-0.001375,0.003095,-0.000795,-0.004162,0.002528,-0.000253,0.003342,-0.001634,-0.001091,0.003632,0.004495,-0.0055,-0.007739,0.000308,-0.003028,-0.001369,3.7e-05,-0.004964,-0.005235,-0.000802,0.005032,-0.001363,-0.002725,-0.001073,-0.004125,-0.001381,0.003897,0.003663,-0.001357,-0.005513,-0.004958,0.010853,0.003632,0.000327,-0.00304,-0.00246,0.004736,-0.000228,3.1e-05,-0.002183,-0.006351,-0.000216,0.000339,-0.002744,0.002799,0.001424,-0.000802,0.000857,0.001406,-0.004951,-0.000795,-0.000499,-0.001394,-0.001603,-0.003021,0.00251,0.00251,0.002528,0.000302,-0.004415,-0.001918,0.001424,-0.000518,0.001443,0.000302,0.002263,-0.001073,-0.001387,-0.001104</t>
+  </si>
+  <si>
+    <t>0.0,0.005019,0.004452,0.006382,-0.001394,0.006394,0.0,0.004175,0.006388,0.001406,0.000561,-0.00135,0.001665,-0.000814,0.004736,0.007208,0.001653,0.007782,0.002232,0.004181,-0.002207,-0.002479,-0.001665,0.006962,0.006413,-0.004156,0.002485,-0.000561,0.004181,0.006382,-0.000845,-0.000277,0.000284,0.005556,0.004156,-0.001363,0.010569,0.002769,-0.001659,0.005284,0.000284,-0.000536,-0.001671,0.003058,0.002226,0.003885,0.000302,-0.003891,-0.00164,0.00751,0.000302,0.000271,0.001135,-0.001955,0.000839,-0.000555,0.0014,0.00193,0.00193,0.003077,-0.006672,0.007498,0.001949,0.000845,0.003897,-0.003065,0.003644,0.003601,0.004193,-0.000277,-0.001128,0.007239,0.00333,-0.001387,0.00891,0.004964,0.003077,0.001961,0.000845,0.000277,0.003866,0.001116,0.001646,-0.000555,0.00275,-0.00082,0.003872,0.000826,-0.003879,-0.001104,0.006413,-3.1e-05,0.002479,2.5e-05,0.000536,0.001973,-0.000808,0.006962,-0.000271,0.002522</t>
+  </si>
+  <si>
+    <t>0.0,0.000265,0.000567,-0.002263,0.000795,-0.000851,0.000253,0.00164,1.2e-05,-0.002547,-0.004199,-0.003903,0.006925,0.005556,0.000555,-0.001671,0.003872,-0.006142,0.000271,0.001924,-0.002812,0.006629,0.00275,-0.003354,-0.003058,0.005802,-0.005297,-0.002522,0.000265,-0.002781,-0.003626,0.005568,-0.004162,-0.000839,0.000247,0.000543,0.003866,0.000795,0.00304,-0.003922,0.000536,0.000259,-0.000592,0.003052,0.001375,-0.001979,-0.001683,-0.004193,0.003305,-0.004742,-0.000851,-0.002775,-0.003613,0.007467,-1.2e-05,0.003866,0.003576,0.000247,0.003589,-0.004723,-0.002503,0.000549,-0.003089,0.003305,0.002485,-0.003058,0.00193,-0.000857,0.000253,0.003046,0.000518,-0.000302,0.004452,0.011648,-0.00169,-1.2e-05,0.00053,0.004421,0.001085,-0.004452,0.002473,1.2e-05,0.000253,0.001659,0.003311,0.001665,0.005241,-0.005858,0.000814,0.003028,0.001091,-0.00029,0.000555,-0.008892,-0.001967,0.00497,-1.2e-05,-0.001135,0.001375,-0.000561</t>
   </si>
 </sst>
 </file>
@@ -677,19 +677,19 @@
         <v>25</v>
       </c>
       <c r="C3">
-        <v>-0.5669999999999999</v>
+        <v>0.011</v>
       </c>
       <c r="D3">
-        <v>-0.552</v>
+        <v>0.048</v>
       </c>
       <c r="E3">
-        <v>-0.597</v>
+        <v>-0.011</v>
       </c>
       <c r="F3">
-        <v>0.008999999999999999</v>
+        <v>0.015</v>
       </c>
       <c r="G3">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H3" t="s">
         <v>28</v>
@@ -700,19 +700,19 @@
         <v>26</v>
       </c>
       <c r="C4">
-        <v>-9.733000000000001</v>
+        <v>0.036</v>
       </c>
       <c r="D4">
-        <v>-9.715</v>
+        <v>0.062</v>
       </c>
       <c r="E4">
-        <v>-9.749000000000001</v>
+        <v>-0.013</v>
       </c>
       <c r="F4">
-        <v>0.008</v>
+        <v>0.014</v>
       </c>
       <c r="G4">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H4" t="s">
         <v>29</v>
@@ -723,19 +723,19 @@
         <v>27</v>
       </c>
       <c r="C5">
-        <v>-0.824</v>
+        <v>-0.202</v>
       </c>
       <c r="D5">
-        <v>-0.55</v>
+        <v>0.047</v>
       </c>
       <c r="E5">
-        <v>-10.281</v>
+        <v>-8.532999999999999</v>
       </c>
       <c r="F5">
-        <v>1.463</v>
+        <v>1.265</v>
       </c>
       <c r="G5">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H5" t="s">
         <v>30</v>
@@ -779,19 +779,19 @@
         <v>25</v>
       </c>
       <c r="C3">
-        <v>0.001</v>
+        <v>-0</v>
       </c>
       <c r="D3">
-        <v>0.01</v>
+        <v>0.011</v>
       </c>
       <c r="E3">
-        <v>-0.007</v>
+        <v>-0.008</v>
       </c>
       <c r="F3">
         <v>0.003</v>
       </c>
       <c r="G3">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H3" t="s">
         <v>31</v>
@@ -802,10 +802,10 @@
         <v>26</v>
       </c>
       <c r="C4">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="D4">
-        <v>0.008</v>
+        <v>0.011</v>
       </c>
       <c r="E4">
         <v>-0.007</v>
@@ -814,7 +814,7 @@
         <v>0.003</v>
       </c>
       <c r="G4">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H4" t="s">
         <v>32</v>
@@ -825,19 +825,19 @@
         <v>27</v>
       </c>
       <c r="C5">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>0.008999999999999999</v>
+        <v>0.012</v>
       </c>
       <c r="E5">
-        <v>-0.007</v>
+        <v>-0.008999999999999999</v>
       </c>
       <c r="F5">
         <v>0.003</v>
       </c>
       <c r="G5">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H5" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
Update logging and  Decorator
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -63,13 +63,13 @@
     <t>Alex Wang</t>
   </si>
   <si>
-    <t>19:21:11 03-05-2017 Sunday Pacific Standard Time</t>
-  </si>
-  <si>
-    <t>19:22:13 03-05-2017 Sunday Pacific Standard Time</t>
-  </si>
-  <si>
-    <t>0:1:2 0 days</t>
+    <t>23:27:46 03-05-2017 Sunday Pacific Standard Time</t>
+  </si>
+  <si>
+    <t>23:28:48 03-05-2017 Sunday Pacific Standard Time</t>
+  </si>
+  <si>
+    <t>0:1:1 0 days</t>
   </si>
   <si>
     <t>Information</t>
@@ -102,22 +102,22 @@
     <t>BT ACL Sniff 1.28s interval Master @ 0dBm at Pin</t>
   </si>
   <si>
-    <t>-0.595635,-0.595615,-0.593862,-0.592374,-0.605472,-0.601749,-0.598964,-0.588475,-0.59497,-0.595533,-0.596647,-0.56963,-0.603801,-0.593577,-0.62181,-0.596736,-0.596097,-0.588298,-0.603047,-0.592279,-0.600452,-0.599901,-0.5934,-0.596185,-0.599066,-0.597938,-0.59516,-0.590621,-0.605839,-0.586247,-0.590235,-0.597204,-0.563876,-0.599243,-0.603699,-0.602116,-0.592191,-0.591172,-0.598502,-0.604541,-0.597388,-0.593869,-0.594704,-0.602211,-0.600914,-0.597755,-0.599901,-0.598047,-0.60713,-0.601097,-0.595432,-0.598964,-0.599066,-0.594039,-0.603801,-0.5959,-0.583373,-0.598692,-0.593033,-0.604351,-0.60213,-0.598509,-0.598686,-0.569813,-0.600825,-0.599623,-0.60073,-0.595628,-0.604915,-0.600072,-0.598699,-0.596552,-0.593217,-0.60092,-0.598692,-0.595812,-0.593951,-0.599059,-0.601661,-0.596926,-0.601566,-0.603699,-0.596919,-0.591172,-0.593951,-0.598142,-0.599148,-0.62514,-0.603326,-0.597381,-0.601933,-0.588013,-0.597952,-0.589589,-0.599901,-0.599433,-0.59359,-0.56499,-0.580955,-0.599515</t>
-  </si>
-  <si>
-    <t>-9.802087,-9.814906,-9.818703,-9.806353,-9.800972,-9.804226,-9.819172,-9.821862,-9.802732,-9.794281,-9.807556,-9.824172,-9.806733,-9.803201,-9.80672,-9.812582,-9.827793,-9.810714,-9.805986,-9.806169,-9.824458,-9.813221,-9.797168,-9.806733,-9.812576,-9.81676,-9.810531,-9.796054,-9.807841,-9.812854,-9.825483,-9.803568,-9.801625,-9.805898,-9.82371,-9.823072,-9.804416,-9.805701,-9.810626,-9.825572,-9.82121,-9.807936,-9.807372,-9.815653,-9.81369,-9.81174,-9.800143,-9.8071,-9.824553,-9.821122,-9.801808,-9.79744,-9.820191,-9.821482,-9.819736,-9.805334,-9.807657,-9.815266,-9.822983,-9.80905,-9.798099,-9.812019,-9.824267,-9.822134,-9.806536,-9.8071,-9.815728,-9.817963,-9.808316,-9.805252,-9.812297,-9.823615,-9.814899,-9.811462,-9.803486,-9.815001,-9.82799,-9.816197,-9.811829,-9.813405,-9.815735,-9.823812,-9.816373,-9.799396,-9.813228,-9.825293,-9.81797,-9.805979,-9.800599,-9.810905,-9.82604,-9.813588,-9.805891,-9.801991,-9.819267,-9.826122,-9.81424,-9.800334,-9.81369,-9.821951</t>
-  </si>
-  <si>
-    <t>-0.603142,-0.60287,-0.600078,-0.610377,-0.595527,-0.619575,-0.598135,-0.600825,-0.591906,-3.706386,-0.592558,-0.597762,-0.599521,-0.603794,-0.60232,-0.603984,-0.599895,-0.605377,-0.627184,-0.600363,-0.6116,-9.683071,-0.593026,-0.594875,-5.110253,-0.626349,-0.598414,-0.597204,-0.598781,-0.592836,-0.593584,-0.600553,-0.607605,-0.600275,-0.632109,-0.604541,-0.62645,-0.592843,-0.602959,-5.553909,-0.593393,-0.600268,-0.605465,-0.597021,-0.600357,-0.604269,-0.594236,-0.600072,-0.601661,-0.599249,-0.591919,-0.598794,-0.597762,-0.596824,-5.414751,-0.600268,-0.601009,-0.598047,-0.598033,-10.002522,-0.599426,-0.631654,-0.5959,-0.596736,-0.607232,-0.605927,-0.602782,-0.593774,-0.595533,-5.450573,-0.606389,-0.588665,-0.605642,-0.636104,-0.600363,-0.606294,-0.607789,-0.601287,-0.599338,-0.588386,-0.600642,-0.595907,-0.597571,-0.595989,-5.088433,-0.596736,-0.601756,-0.603047,-0.597123,-0.56518,-0.596818,-0.593584,-0.59768,-0.603604,-0.593312,-0.599066,-0.595995,-9.936414,-0.591634,-6.716669</t>
-  </si>
-  <si>
-    <t>-0.00247,0.002537,-0.001909,0.002808,0.000896,0.002253,-0.002168,0.00668,-0.001058,-0.006084,-0.001348,-0.000534,-0.001077,-0.001354,1.5e-05,-0.004407,-0.001336,0.000594,0.002265,-0.003821,-0.004382,-0.000238,0.001969,0.002802,0.004763,0.001408,-0.00244,-0.001638,0.002537,0.003363,0.004485,0.003665,0.003628,-0.001632,3.3e-05,0.004214,0.00533,0.005348,-0.000805,0.004226,-0.000509,0.00475,0.002259,0.004763,0.005583,-0.004407,0.000594,-0.000503,0.004504,0.004467,-0.000793,0.00475,0.001464,0.003936,-0.00165,0.004201,-0.000805,0.002518,0.00171,-0.003297,-0.000238,0.003363,-0.000805,0.009763,-0.000793,0.000872,0.001433,-0.007761,0.00089,-0.003845,-0.000214,0.005589,-0.000534,3.3e-05,0.002826,0.009745,-0.000775,2.7e-05,0.005305,-0.000251,0.005299,0.003918,0.003357,-0.002427,0.004744,0.006125,0.001692,-0.001083,0.001945,0.001402,-0.000522,-0.001613,0.001433,0.008074,-0.000799,-0.000781,-0.007181,0.005022,0.001433,-0.001077</t>
-  </si>
-  <si>
-    <t>-0.003839,-0.001619,0.0006,0.000317,-0.000232,0.000859,-0.003031,-0.002174,-0.003007,0.000872,0.001717,0.001433,0.000613,0.001149,-0.000503,-0.004129,0.000607,0.004467,-0.003309,-0.000528,-0.000787,0.005034,0.003949,0.005879,0.001698,-0.003284,-0.001656,0.004183,-0.001632,-0.004986,-0.002199,-0.002458,0.005601,0.002247,0.000607,0.005028,0.004769,-0.000528,-0.000509,0.003653,-0.002421,2.1e-05,0.002253,-0.003543,-0.002723,6.4e-05,0.000329,0.001439,0.001717,0.006964,-0.000232,0.001723,0.010288,0.001427,0.001143,-0.000781,0.007248,0.00422,-0.000534,0.003918,0.00504,0.002271,-0.002181,0.000576,0.006952,-0.000522,-0.001872,0.004485,0.001414,0.001994,0.001994,0.002808,-0.000787,0.001414,-0.001052,-0.001903,-0.001897,0.0006,0.004726,-0.001922,-0.000787,0.003665,0.001704,-0.000799,-0.000251,-0.001613,0.00057,0.006169,0.001421,0.001439,0.001421,0.00446,0.004226,-0.004413,-0.001626,0.001741,-0.002137,-0.002717,-0.001354,0.005052</t>
-  </si>
-  <si>
-    <t>-0.004955,-0.005812,-0.000787,0.003924,-0.002446,-0.001638,-0.00358,-0.008871,0.001414,-0.003272,-0.00522,-0.00498,0.003079,-0.002452,-0.003044,-0.000805,-0.001644,-0.001064,0.001723,0.005059,0.001149,0.000859,-0.001046,0.001421,-0.000251,0.004744,0.003369,0.003085,0.000896,-0.002168,0.008092,0.004183,3.3e-05,0.009215,-0.001095,0.003924,-0.001626,0.006421,-0.001058,0.000613,0.001155,-0.000799,0.005305,-0.009105,0.000872,-0.001909,-0.006053,0.00089,0.002543,-0.004135,-0.001632,0.002802,0.002259,-0.000226,-0.003007,0.004201,-0.002476,0.001433,0.000304,0.003344,0.002543,-0.003833,0.001975,-0.005233,-0.001903,0.002796,-0.002489,-0.001607,-0.007434,-0.000485,4.5e-05,-0.000516,0.003381,0.00755,0.002783,0.002814,-0.003007,0.000298,-0.00469,-0.007169,-0.001064,2.7e-05,0.005015,0.002259,0.006693,-0.000226,0.008086,0.008358,2.7e-05,0.000304,0.001421,0.004497,-0.003845,-0.001915,0.001427,0.005052,-0.002735,-0.007773,-0.00551,0.002006</t>
+    <t>-0.629141,-0.624487,-0.628027,-0.597395,-0.618176,-0.623387,-0.631179,-0.629881,-0.629508,-0.631274,-0.623006,-0.628393,-0.62338,-0.626811,-0.6284,-0.622646,-0.62821,-0.627191,-0.633686,-0.633027,-0.621247,-0.633407,-0.62107,-0.621342,-0.627564,-0.628122,-0.624582,-0.63109,-0.602782,-0.599433,-0.598312,-0.623291,-0.628767,-0.628027,-0.626817,-0.604453,-0.597388,-0.629331,-0.624215,-0.627191,-0.626729,-0.631933,-0.628862,-0.624956,-0.624501,-0.627653,-0.632857,-0.620785,-0.63592,-0.629324,-0.618088,-0.622177,-0.629419,-0.628951,-0.627191,-0.6334,-0.619575,-0.622558,-0.624969,-0.635642,-0.623658,-0.622829,-0.635907,-0.626906,-0.624406,-0.625982,-0.622918,-0.624963,-0.628122,-0.632571,-0.629691,-0.623013,-0.600357,-0.634344,-0.620785,-0.620886,-0.628393,-0.629698,-0.626627,-0.621715,-0.638794,-0.628387,-0.624596,-0.635452,-0.623475,-0.630261,-0.599154,-0.601199,-0.63266,-0.622924,-0.63285,-0.631831,-0.624677,-0.601566,-0.596742,-0.599249,-0.599901,-0.601376,-0.599426,-0.598128</t>
+  </si>
+  <si>
+    <t>-9.869865,-9.871618,-9.877746,-9.86549,-9.867338,-9.874688,-9.887026,-9.881183,-9.875612,-9.858357,-9.87032,-9.882772,-9.888058,-9.869491,-9.871801,-9.88657,-9.883316,-9.8771,-9.869206,-9.874872,-9.891217,-9.882379,-9.866604,-9.865402,-9.866896,-9.88619,-9.87441,-9.865218,-9.86475,-9.878493,-9.883031,-9.87672,-9.868181,-9.881278,-9.892052,-9.875796,-9.875517,-9.861876,-9.88407,-9.886013,-9.876638,-9.864301,-9.874308,-9.886937,-9.878398,-9.87403,-9.862521,-9.87867,-9.882209,-9.876822,-9.86801,-9.868839,-9.880252,-9.889729,-9.885823,-9.862712,-9.870592,-9.879607,-9.890748,-9.869668,-9.860762,-9.872821,-9.889818,-9.884804,-9.863269,-9.873017,-9.881272,-9.891128,-9.877195,-9.864281,-9.874226,-9.887596,-9.887412,-9.865782,-9.865775,-9.883683,-9.894091,-9.872555,-9.866142,-9.868751,-9.883405,-9.890653,-9.882297,-9.868561,-9.872637,-9.891299,-9.882386,-9.874682,-9.867623,-9.881924,-9.885823,-9.890647,-9.856027,-9.875524,-9.882215,-9.885279,-9.879519,-9.870225,-9.874587,-9.890565</t>
+  </si>
+  <si>
+    <t>-0.633319,-0.614283,-5.420498,-0.634059,-0.629603,-0.628393,-0.637306,-0.623937,-0.612524,-0.631267,-0.631084,-0.623203,-0.629242,-0.626817,-0.629508,-1.66741,-0.627646,-5.136143,-0.627007,-0.628482,-0.619113,-0.593679,-0.61912,-10.354458,-0.629698,-0.598964,-0.616512,-0.639731,-0.629324,-0.631457,-0.626729,-0.629698,-4.359852,-0.624311,-0.625798,-0.6309,-0.629236,-0.595533,-0.625343,-0.625526,-0.627273,-0.63535,-0.634901,-0.624589,-0.624963,-0.637673,-0.63499,-1.832675,-0.627931,-0.621709,-0.637028,-0.630255,-0.637857,-0.626824,-0.637402,-0.626349,-0.632938,-0.623563,-0.631736,-0.632021,-0.6259,-9.988316,-0.778889,-0.616879,-0.623753,-0.607225,-0.600819,-0.626729,-0.631185,-0.628584,-0.617993,-0.626729,-0.625153,-0.62376,-0.594698,-0.62162,-0.630812,-1.25569,-0.62357,-0.62997,-0.624399,-0.631274,-0.630356,-0.629983,-0.626349,-0.631749,-0.633971,-0.624786,-0.597293,-0.626817,-0.632673,-0.62857,-0.62088,-0.623658,-0.629521,-0.629976,-0.628407,-0.63249,-0.62626,-10.258656</t>
+  </si>
+  <si>
+    <t>-0.003278,0.003918,0.003628,-0.006349,0.002808,0.001982,0.000323,-0.000793,0.004479,-0.002181,-0.007465,-0.001638,0.001957,-0.004949,0.002259,-0.005214,-0.003593,-0.007459,-0.002729,0.002247,0.001969,-0.000244,-0.003013,-0.002446,0.005577,-0.003001,-0.001083,-0.010795,-0.003858,-0.007724,0.005034,5.2e-05,-0.000799,-0.000522,0.002265,6.4e-05,0.001717,-0.004154,0.000317,0.000607,-0.001077,0.003924,-0.000251,4.5e-05,0.000311,-0.001891,0.001427,0.003671,-0.003821,0.000317,-0.001095,-0.000812,-0.001336,0.000329,0.00253,-0.002729,-0.000251,5.2e-05,-0.000787,-0.006324,-0.004117,-0.001607,-0.00133,-0.000546,0.001667,3.3e-05,-0.000238,-0.002446,0.007809,0.001402,0.00504,-0.003019,-0.001367,0.001149,-0.006059,0.006421,-0.002199,-0.008026,0.003634,0.001162,-0.003025,0.001975,0.001433,-0.001626,-0.001348,-0.000226,-0.003025,0.001717,0.003375,0.005854,-0.002452,0.001692,0.000884,-0.006361,-0.003839,0.004473,-0.001897,0.00837,-0.000805,-0.004665</t>
+  </si>
+  <si>
+    <t>-0.003568,0.002524,0.0006,-0.00387,-0.000516,0.001667,-0.001064,0.007266,-0.009938,-0.003556,-0.003315,-0.001897,0.001704,0.000329,0.001975,-0.005523,0.000896,-0.005233,0.001994,0.001427,0.003098,-0.002742,-0.006065,0.004738,-0.001915,0.002839,-0.003007,-0.001897,0.000311,0.003092,0.002512,0.001661,0.000317,0.001433,-0.000805,0.005028,0.002808,0.003375,-0.00136,-0.000238,0.00118,0.002247,-0.00329,-0.000812,0.001427,-0.0044,-0.000516,-0.003297,0.001143,0.001149,-0.003278,0.000872,-0.000238,-0.001619,-0.002729,-0.003568,-0.002994,-0.003297,0.00446,-0.002748,-0.003303,0.000323,-0.003864,0.000311,-0.001613,-0.003858,-0.005782,0.00586,-0.003858,0.006421,0.002265,-0.005251,-0.005529,0.003067,-0.000793,-0.003019,-0.002168,-0.001064,-0.003556,0.007778,0.001723,0.001692,0.00475,-0.003019,-0.001909,0.004195,-0.002476,-0.003321,-0.00136,0.003344,-0.001613,0.000582,0.000872,-0.00247,-0.004419,0.001414,0.0006,-0.003574,0.001427,0.000335</t>
+  </si>
+  <si>
+    <t>-0.001619,-0.00133,-0.006602,-0.003013,-0.004678,0.003357,-0.001064,0.004479,-0.004092,0.000341,0.00253,-0.003556,-0.00136,-0.003007,-0.001064,0.003073,0.00253,-0.003303,-0.002717,3.9e-05,-0.003297,0.000317,-0.004961,0.000613,-0.002181,-0.003858,-0.002988,0.005879,0.002802,0.003092,-0.002711,-0.002168,0.002234,-0.000534,0.001975,0.001143,-0.006047,-0.005775,-0.005782,0.001168,0.00311,0.000853,-0.001915,-0.000509,0.003936,-0.000528,0.003634,-0.003025,-0.002156,0.000866,-0.005233,7e-05,-0.003007,-0.00358,-0.002754,-0.004986,-0.003007,-0.011054,-0.004678,-0.000793,0.001162,-0.004141,-0.003315,-0.002735,0.002284,0.00504,-0.005245,-0.001089,0.000335,-0.003833,2.7e-05,-0.00104,0.001131,0.004208,0.00533,-0.00247,-0.005233,-0.006059,0.00171,-0.004394,3.9e-05,0.000884,5.2e-05,0.000866,-0.006343,0.000866,-0.001336,-0.008291,-0.005486,0.001704,-0.004413,-0.001052,-0.007163,-0.000509,0.001414,-0.003568,-0.000207,-0.001632,-0.005202,0.004454</t>
   </si>
 </sst>
 </file>
@@ -677,16 +677,16 @@
         <v>25</v>
       </c>
       <c r="C3">
+        <v>-0.623</v>
+      </c>
+      <c r="D3">
         <v>-0.597</v>
       </c>
-      <c r="D3">
-        <v>-0.5639999999999999</v>
-      </c>
       <c r="E3">
-        <v>-0.625</v>
+        <v>-0.639</v>
       </c>
       <c r="F3">
-        <v>0.008999999999999999</v>
+        <v>0.011</v>
       </c>
       <c r="G3">
         <v>100</v>
@@ -700,16 +700,16 @@
         <v>26</v>
       </c>
       <c r="C4">
-        <v>-9.811999999999999</v>
+        <v>-9.877000000000001</v>
       </c>
       <c r="D4">
-        <v>-9.794</v>
+        <v>-9.856</v>
       </c>
       <c r="E4">
-        <v>-9.827999999999999</v>
+        <v>-9.894</v>
       </c>
       <c r="F4">
-        <v>0.008</v>
+        <v>0.008999999999999999</v>
       </c>
       <c r="G4">
         <v>100</v>
@@ -723,16 +723,16 @@
         <v>27</v>
       </c>
       <c r="C5">
-        <v>-1.208</v>
+        <v>-1.074</v>
       </c>
       <c r="D5">
-        <v>-0.5649999999999999</v>
+        <v>-0.594</v>
       </c>
       <c r="E5">
-        <v>-10.003</v>
+        <v>-10.354</v>
       </c>
       <c r="F5">
-        <v>1.949</v>
+        <v>1.776</v>
       </c>
       <c r="G5">
         <v>100</v>
@@ -779,16 +779,16 @@
         <v>25</v>
       </c>
       <c r="C3">
-        <v>0.001</v>
+        <v>-0.001</v>
       </c>
       <c r="D3">
-        <v>0.01</v>
+        <v>0.008</v>
       </c>
       <c r="E3">
-        <v>-0.008</v>
+        <v>-0.011</v>
       </c>
       <c r="F3">
-        <v>0.003</v>
+        <v>0.004</v>
       </c>
       <c r="G3">
         <v>100</v>
@@ -802,13 +802,13 @@
         <v>26</v>
       </c>
       <c r="C4">
-        <v>0.001</v>
+        <v>-0</v>
       </c>
       <c r="D4">
-        <v>0.01</v>
+        <v>0.008</v>
       </c>
       <c r="E4">
-        <v>-0.005</v>
+        <v>-0.01</v>
       </c>
       <c r="F4">
         <v>0.003</v>
@@ -825,16 +825,16 @@
         <v>27</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>-0.001</v>
       </c>
       <c r="D5">
-        <v>0.008999999999999999</v>
+        <v>0.006</v>
       </c>
       <c r="E5">
-        <v>-0.008999999999999999</v>
+        <v>-0.011</v>
       </c>
       <c r="F5">
-        <v>0.004</v>
+        <v>0.003</v>
       </c>
       <c r="G5">
         <v>100</v>

</xml_diff>

<commit_message>
Fix logging print extra line issue
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="31">
   <si>
     <t>WLAN Version</t>
   </si>
@@ -63,13 +63,13 @@
     <t>Alex Wang</t>
   </si>
   <si>
-    <t>23:27:46 03-05-2017 Sunday Pacific Standard Time</t>
-  </si>
-  <si>
-    <t>23:28:48 03-05-2017 Sunday Pacific Standard Time</t>
-  </si>
-  <si>
-    <t>0:1:1 0 days</t>
+    <t>22:04:37 03-07-2017 Tuesday Pacific Standard Time</t>
+  </si>
+  <si>
+    <t>22:05:11 03-07-2017 Tuesday Pacific Standard Time</t>
+  </si>
+  <si>
+    <t>0:0:34 0 days</t>
   </si>
   <si>
     <t>Information</t>
@@ -99,25 +99,16 @@
     <t>BT Idle</t>
   </si>
   <si>
-    <t>BT ACL Sniff 1.28s interval Master @ 0dBm at Pin</t>
-  </si>
-  <si>
-    <t>-0.629141,-0.624487,-0.628027,-0.597395,-0.618176,-0.623387,-0.631179,-0.629881,-0.629508,-0.631274,-0.623006,-0.628393,-0.62338,-0.626811,-0.6284,-0.622646,-0.62821,-0.627191,-0.633686,-0.633027,-0.621247,-0.633407,-0.62107,-0.621342,-0.627564,-0.628122,-0.624582,-0.63109,-0.602782,-0.599433,-0.598312,-0.623291,-0.628767,-0.628027,-0.626817,-0.604453,-0.597388,-0.629331,-0.624215,-0.627191,-0.626729,-0.631933,-0.628862,-0.624956,-0.624501,-0.627653,-0.632857,-0.620785,-0.63592,-0.629324,-0.618088,-0.622177,-0.629419,-0.628951,-0.627191,-0.6334,-0.619575,-0.622558,-0.624969,-0.635642,-0.623658,-0.622829,-0.635907,-0.626906,-0.624406,-0.625982,-0.622918,-0.624963,-0.628122,-0.632571,-0.629691,-0.623013,-0.600357,-0.634344,-0.620785,-0.620886,-0.628393,-0.629698,-0.626627,-0.621715,-0.638794,-0.628387,-0.624596,-0.635452,-0.623475,-0.630261,-0.599154,-0.601199,-0.63266,-0.622924,-0.63285,-0.631831,-0.624677,-0.601566,-0.596742,-0.599249,-0.599901,-0.601376,-0.599426,-0.598128</t>
-  </si>
-  <si>
-    <t>-9.869865,-9.871618,-9.877746,-9.86549,-9.867338,-9.874688,-9.887026,-9.881183,-9.875612,-9.858357,-9.87032,-9.882772,-9.888058,-9.869491,-9.871801,-9.88657,-9.883316,-9.8771,-9.869206,-9.874872,-9.891217,-9.882379,-9.866604,-9.865402,-9.866896,-9.88619,-9.87441,-9.865218,-9.86475,-9.878493,-9.883031,-9.87672,-9.868181,-9.881278,-9.892052,-9.875796,-9.875517,-9.861876,-9.88407,-9.886013,-9.876638,-9.864301,-9.874308,-9.886937,-9.878398,-9.87403,-9.862521,-9.87867,-9.882209,-9.876822,-9.86801,-9.868839,-9.880252,-9.889729,-9.885823,-9.862712,-9.870592,-9.879607,-9.890748,-9.869668,-9.860762,-9.872821,-9.889818,-9.884804,-9.863269,-9.873017,-9.881272,-9.891128,-9.877195,-9.864281,-9.874226,-9.887596,-9.887412,-9.865782,-9.865775,-9.883683,-9.894091,-9.872555,-9.866142,-9.868751,-9.883405,-9.890653,-9.882297,-9.868561,-9.872637,-9.891299,-9.882386,-9.874682,-9.867623,-9.881924,-9.885823,-9.890647,-9.856027,-9.875524,-9.882215,-9.885279,-9.879519,-9.870225,-9.874587,-9.890565</t>
-  </si>
-  <si>
-    <t>-0.633319,-0.614283,-5.420498,-0.634059,-0.629603,-0.628393,-0.637306,-0.623937,-0.612524,-0.631267,-0.631084,-0.623203,-0.629242,-0.626817,-0.629508,-1.66741,-0.627646,-5.136143,-0.627007,-0.628482,-0.619113,-0.593679,-0.61912,-10.354458,-0.629698,-0.598964,-0.616512,-0.639731,-0.629324,-0.631457,-0.626729,-0.629698,-4.359852,-0.624311,-0.625798,-0.6309,-0.629236,-0.595533,-0.625343,-0.625526,-0.627273,-0.63535,-0.634901,-0.624589,-0.624963,-0.637673,-0.63499,-1.832675,-0.627931,-0.621709,-0.637028,-0.630255,-0.637857,-0.626824,-0.637402,-0.626349,-0.632938,-0.623563,-0.631736,-0.632021,-0.6259,-9.988316,-0.778889,-0.616879,-0.623753,-0.607225,-0.600819,-0.626729,-0.631185,-0.628584,-0.617993,-0.626729,-0.625153,-0.62376,-0.594698,-0.62162,-0.630812,-1.25569,-0.62357,-0.62997,-0.624399,-0.631274,-0.630356,-0.629983,-0.626349,-0.631749,-0.633971,-0.624786,-0.597293,-0.626817,-0.632673,-0.62857,-0.62088,-0.623658,-0.629521,-0.629976,-0.628407,-0.63249,-0.62626,-10.258656</t>
-  </si>
-  <si>
-    <t>-0.003278,0.003918,0.003628,-0.006349,0.002808,0.001982,0.000323,-0.000793,0.004479,-0.002181,-0.007465,-0.001638,0.001957,-0.004949,0.002259,-0.005214,-0.003593,-0.007459,-0.002729,0.002247,0.001969,-0.000244,-0.003013,-0.002446,0.005577,-0.003001,-0.001083,-0.010795,-0.003858,-0.007724,0.005034,5.2e-05,-0.000799,-0.000522,0.002265,6.4e-05,0.001717,-0.004154,0.000317,0.000607,-0.001077,0.003924,-0.000251,4.5e-05,0.000311,-0.001891,0.001427,0.003671,-0.003821,0.000317,-0.001095,-0.000812,-0.001336,0.000329,0.00253,-0.002729,-0.000251,5.2e-05,-0.000787,-0.006324,-0.004117,-0.001607,-0.00133,-0.000546,0.001667,3.3e-05,-0.000238,-0.002446,0.007809,0.001402,0.00504,-0.003019,-0.001367,0.001149,-0.006059,0.006421,-0.002199,-0.008026,0.003634,0.001162,-0.003025,0.001975,0.001433,-0.001626,-0.001348,-0.000226,-0.003025,0.001717,0.003375,0.005854,-0.002452,0.001692,0.000884,-0.006361,-0.003839,0.004473,-0.001897,0.00837,-0.000805,-0.004665</t>
-  </si>
-  <si>
-    <t>-0.003568,0.002524,0.0006,-0.00387,-0.000516,0.001667,-0.001064,0.007266,-0.009938,-0.003556,-0.003315,-0.001897,0.001704,0.000329,0.001975,-0.005523,0.000896,-0.005233,0.001994,0.001427,0.003098,-0.002742,-0.006065,0.004738,-0.001915,0.002839,-0.003007,-0.001897,0.000311,0.003092,0.002512,0.001661,0.000317,0.001433,-0.000805,0.005028,0.002808,0.003375,-0.00136,-0.000238,0.00118,0.002247,-0.00329,-0.000812,0.001427,-0.0044,-0.000516,-0.003297,0.001143,0.001149,-0.003278,0.000872,-0.000238,-0.001619,-0.002729,-0.003568,-0.002994,-0.003297,0.00446,-0.002748,-0.003303,0.000323,-0.003864,0.000311,-0.001613,-0.003858,-0.005782,0.00586,-0.003858,0.006421,0.002265,-0.005251,-0.005529,0.003067,-0.000793,-0.003019,-0.002168,-0.001064,-0.003556,0.007778,0.001723,0.001692,0.00475,-0.003019,-0.001909,0.004195,-0.002476,-0.003321,-0.00136,0.003344,-0.001613,0.000582,0.000872,-0.00247,-0.004419,0.001414,0.0006,-0.003574,0.001427,0.000335</t>
-  </si>
-  <si>
-    <t>-0.001619,-0.00133,-0.006602,-0.003013,-0.004678,0.003357,-0.001064,0.004479,-0.004092,0.000341,0.00253,-0.003556,-0.00136,-0.003007,-0.001064,0.003073,0.00253,-0.003303,-0.002717,3.9e-05,-0.003297,0.000317,-0.004961,0.000613,-0.002181,-0.003858,-0.002988,0.005879,0.002802,0.003092,-0.002711,-0.002168,0.002234,-0.000534,0.001975,0.001143,-0.006047,-0.005775,-0.005782,0.001168,0.00311,0.000853,-0.001915,-0.000509,0.003936,-0.000528,0.003634,-0.003025,-0.002156,0.000866,-0.005233,7e-05,-0.003007,-0.00358,-0.002754,-0.004986,-0.003007,-0.011054,-0.004678,-0.000793,0.001162,-0.004141,-0.003315,-0.002735,0.002284,0.00504,-0.005245,-0.001089,0.000335,-0.003833,2.7e-05,-0.00104,0.001131,0.004208,0.00533,-0.00247,-0.005233,-0.006059,0.00171,-0.004394,3.9e-05,0.000884,5.2e-05,0.000866,-0.006343,0.000866,-0.001336,-0.008291,-0.005486,0.001704,-0.004413,-0.001052,-0.007163,-0.000509,0.001414,-0.003568,-0.000207,-0.001632,-0.005202,0.004454</t>
+    <t>0.587009,0.574672,0.604658,0.593782,0.613932,0.620433,0.586459,0.606221,0.607437,0.581628,0.618585,0.577919,0.61226,0.614407,0.575222,0.615147,0.61811,0.59027,0.616262,0.592118,0.617097,0.615324,0.581065,0.584971,0.620623,0.577641,0.592858,0.615147,0.586635,0.583395,0.611058,0.586268,0.578476,0.611622,0.58887,0.613646,0.578381,0.582838,0.616724,0.574393,0.594441,0.619312,0.620161,0.57438,0.583939,0.617743,0.577926,0.602797,0.612831,0.58209,0.617192,0.587301,0.584787,0.575969,0.61599,0.578741,0.581078,0.611336,0.586092,0.585997,0.613653,0.575494,0.589794,0.617743,0.575406,0.594244,0.608463,0.589427,0.615616,0.599733,0.584882,0.578653,0.613381,0.613286,0.5858,0.594624,0.615698,0.586547,0.610786,0.604101,0.586554,0.610881,0.600012,0.581363,0.612817,0.612362,0.583198,0.612722,0.614869,0.610412,0.579407,0.59044,0.582281,0.607804,0.581995,0.613279,0.588307,0.577919,0.615881,0.590446</t>
+  </si>
+  <si>
+    <t>9.824391,9.83664,9.837665,9.843515,9.827733,9.830247,9.845002,9.843046,9.835709,9.815288,9.837665,9.838311,9.84435,9.824479,9.818073,9.845186,9.844534,9.840356,9.8281,9.83274,9.840172,9.843046,9.832095,9.826246,9.83414,9.847319,9.839337,9.832095,9.825227,9.838127,9.845002,9.841103,9.830512,9.83414,9.841565,9.844629,9.834513,9.82346,9.835722,9.848243,9.845648,9.82717,9.828379,9.841375,9.849642,9.83181,9.819656,9.822251,9.852795,9.839982,9.840444,9.819099,9.842856,9.845845,9.840634,9.824391,9.824024,9.838311,9.849351,9.838039,9.821986,9.837475,9.842679,9.847503,9.826436,9.827081,9.83721,9.849908,9.83776,9.823365,9.82253,9.84361,9.85401,9.8256,9.829303,9.839432,9.846578,9.840077,9.830145,9.826062,9.839337,9.843148,9.832475,9.825043,9.83433,9.848617,9.853827,9.830152,9.828854,9.831069,9.842863,9.846762,9.836368,9.824486,9.834969,9.842489,9.836918,9.828385,9.836368,9.846015</t>
+  </si>
+  <si>
+    <t>0.001427,0.003375,0.00504,0.002253,0.005589,0.003659,-0.003284,0.000576,0.004479,0.001433,0.005034,-0.007175,0.00504,0.006421,0.008906,-0.003876,-0.003882,-0.003315,0.008111,0.004497,0.001445,0.003388,-0.000534,-0.002735,0.001155,-0.005276,5.2e-05,-0.002187,0.005577,0.00504,0.002271,0.001143,0.00282,0.001427,-0.001354,3.3e-05,-0.002446,-0.001071,0.001957,0.002537,0.003129,0.001445,-0.003025,-0.008001,0.001741,0.005022,0.007784,-0.004968,-0.003001,0.00253,0.003369,0.006125,-0.000799,-0.000775,-0.003284,0.001698,0.0006,-0.001354,0.003665,0.000884,-0.004684,-0.001632,0.00364,-0.006047,-0.000263,0.000859,0.001168,-0.004961,0.004214,-0.001071,-0.004696,-0.001373,0.001704,0.006144,0.009208,0.002265,0.00446,-0.004129,0.001698,0.001414,0.000866,0.003357,0.004485,-0.001077,0.001692,0.003351,-0.002742,0.0006,-0.001064,0.008092,0.00451,5.2e-05,-0.000824,0.002271,-0.001619,0.000866,0.006982,0.006674,0.002253,0.00057</t>
+  </si>
+  <si>
+    <t>3.9e-05,0.008099,-0.001342,-0.007434,0.001698,0.002019,0.002802,0.00282,0.001963,0.001396,0.001421,0.003924,0.002555,0.003085,0.000329,0.004473,-0.002483,-0.001052,0.00808,0.0006,0.0006,0.000329,0.002253,0.0006,2.1e-05,0.002814,0.004485,-0.000528,0.00475,-0.003321,0.000853,0.009196,0.000859,0.001938,0.002259,0.001427,-0.000509,0.004189,0.003665,0.000859,0.002518,0.002524,0.00089,3.9e-05,-0.000516,-0.003303,0.001149,-0.008852,-0.001903,0.003659,0.003129,0.001155,-0.003562,0.000576,-0.001656,0.004183,0.002808,0.001458,0.003394,0.001735,0.000317,-0.000824,-0.001323,0.000341,0.001433,-0.000528,0.004479,-0.004659,-0.006349,0.001692,0.004473,0.000594,-0.000522,-0.004943,4.5e-05,-0.002748,0.005583,0.001963,0.002543,-0.000491,0.002796,-0.002723,0.001439,5.2e-05,-0.001323,3.9e-05,0.00282,0.002814,0.006421,-0.000534,0.003647,0.003079,-0.003845,-0.001077,-0.001071,0.003918,0.000847,0.004491,0.005287,0.006409</t>
   </si>
 </sst>
 </file>
@@ -646,7 +637,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:H5"/>
+  <dimension ref="B2:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -677,22 +668,22 @@
         <v>25</v>
       </c>
       <c r="C3">
-        <v>-0.623</v>
+        <v>0.598</v>
       </c>
       <c r="D3">
-        <v>-0.597</v>
+        <v>0.621</v>
       </c>
       <c r="E3">
-        <v>-0.639</v>
+        <v>0.574</v>
       </c>
       <c r="F3">
-        <v>0.011</v>
+        <v>0.016</v>
       </c>
       <c r="G3">
         <v>100</v>
       </c>
       <c r="H3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="2:8">
@@ -700,13 +691,13 @@
         <v>26</v>
       </c>
       <c r="C4">
-        <v>-9.877000000000001</v>
+        <v>9.836</v>
       </c>
       <c r="D4">
-        <v>-9.856</v>
+        <v>9.853999999999999</v>
       </c>
       <c r="E4">
-        <v>-9.894</v>
+        <v>9.815</v>
       </c>
       <c r="F4">
         <v>0.008999999999999999</v>
@@ -715,30 +706,7 @@
         <v>100</v>
       </c>
       <c r="H4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8">
-      <c r="B5" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5">
-        <v>-1.074</v>
-      </c>
-      <c r="D5">
-        <v>-0.594</v>
-      </c>
-      <c r="E5">
-        <v>-10.354</v>
-      </c>
-      <c r="F5">
-        <v>1.776</v>
-      </c>
-      <c r="G5">
-        <v>100</v>
-      </c>
-      <c r="H5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -748,7 +716,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:H5"/>
+  <dimension ref="B2:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -779,13 +747,13 @@
         <v>25</v>
       </c>
       <c r="C3">
-        <v>-0.001</v>
+        <v>0.001</v>
       </c>
       <c r="D3">
-        <v>0.008</v>
+        <v>0.008999999999999999</v>
       </c>
       <c r="E3">
-        <v>-0.011</v>
+        <v>-0.008</v>
       </c>
       <c r="F3">
         <v>0.004</v>
@@ -794,7 +762,7 @@
         <v>100</v>
       </c>
       <c r="H3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="2:8">
@@ -802,13 +770,13 @@
         <v>26</v>
       </c>
       <c r="C4">
-        <v>-0</v>
+        <v>0.001</v>
       </c>
       <c r="D4">
-        <v>0.008</v>
+        <v>0.008999999999999999</v>
       </c>
       <c r="E4">
-        <v>-0.01</v>
+        <v>-0.008999999999999999</v>
       </c>
       <c r="F4">
         <v>0.003</v>
@@ -817,30 +785,7 @@
         <v>100</v>
       </c>
       <c r="H4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8">
-      <c r="B5" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5">
-        <v>-0.001</v>
-      </c>
-      <c r="D5">
-        <v>0.006</v>
-      </c>
-      <c r="E5">
-        <v>-0.011</v>
-      </c>
-      <c r="F5">
-        <v>0.003</v>
-      </c>
-      <c r="G5">
-        <v>100</v>
-      </c>
-      <c r="H5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update excel writer with format function
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="31">
   <si>
     <t>WLAN Version</t>
   </si>
@@ -63,13 +63,13 @@
     <t>Alex Wang</t>
   </si>
   <si>
-    <t>07:42:45 03-15-2017 Wednesday Pacific Daylight Time</t>
-  </si>
-  <si>
-    <t>07:43:04 03-15-2017 Wednesday Pacific Daylight Time</t>
-  </si>
-  <si>
-    <t>0:0:18 0 days</t>
+    <t>09:54:10 03-15-2017 Wednesday Pacific Daylight Time</t>
+  </si>
+  <si>
+    <t>09:54:45 03-15-2017 Wednesday Pacific Daylight Time</t>
+  </si>
+  <si>
+    <t>0:0:34 0 days</t>
   </si>
   <si>
     <t>Information</t>
@@ -96,10 +96,19 @@
     <t>Deep Sleep</t>
   </si>
   <si>
-    <t>0.58404,0.57847,0.575222,0.573456,0.57476,0.568436,0.580888,0.542077,0.547287,0.549604,0.581438,0.574665,0.584509,0.591004,0.573463,0.573001,0.570494,0.579203,0.587016,0.546547,0.574849,0.585623,0.585623,0.568082,0.565107,0.580419,0.543755,0.545236,0.573728,0.571886,0.555813,0.545983,0.543109,0.545147,0.55294,0.576051,0.57652,0.557485,0.589713,0.566404,0.575134,0.579767,0.577736,0.582749,0.576717,0.57726,0.573558,0.552858,0.569285,0.579584,0.575691,0.581628,0.571513,0.584964,0.572342,0.549407,0.568999,0.574387,0.573456,0.578938,0.573735,0.579305,0.575222,0.573463,0.575134,0.581628,0.579122,0.573551,0.576241,0.57726,0.573741,0.547199,0.572348,0.568075,0.57885,0.580236,0.576438,0.579217,0.569747,0.584414,0.547926,0.546343,0.577716,0.548034,0.542729,0.561853,0.579394,0.577817,0.569842,0.582097,0.577546,0.58154,0.571139,0.572899,0.588965,0.581166,0.57745,0.572994,0.577362,0.584781</t>
-  </si>
-  <si>
-    <t>0.00697,0.002543,-0.001891,-0.000214,-0.000528,-0.000534,-0.003852,0.00171,-0.00136,-0.003303,-0.004394,0.001414,0.003104,-0.002994,0.002253,0.007519,0.003936,0.005046,0.004479,0.000348,0.001149,-0.002464,-0.006071,-0.003852,0.00446,0.001433,0.003375,-0.002446,0.005589,0.000304,0.005052,-0.003574,0.002833,0.00475,-0.006065,0.003369,-0.00136,5.8e-05,0.002524,0.000859,-0.003543,-0.004141,-0.002156,0.00422,-0.00522,0.001982,-0.001613,0.001137,0.007821,0.001717,-0.001336,0.006995,0.008395,0.000311,0.003344,-0.004388,-0.001095,0.004177,0.00644,0.001433,-0.000257,0.003116,-0.001885,-0.006059,0.001988,-0.003019,4.5e-05,0.004214,0.001698,0.003912,0.001433,-0.004672,0.004195,-0.001342,0.001143,0.0006,0.003653,0.004454,-0.000812,0.006409,-0.003562,-0.000257,-0.003821,-0.00136,3.3e-05,0.001982,0.003369,2.7e-05,0.002808,-0.00244,0.007809,0.001975,-0.000787,0.002259,0.005299,-0.004955,-0.002174,0.001149,0.005903,-0.003839</t>
+    <t>BT Idle</t>
+  </si>
+  <si>
+    <t>0.574475,0.602885,0.567342,0.577349,0.576153,0.567892,0.56919,0.593048,0.571506,0.571886,0.565841,0.602512,0.572348,0.566771,0.574475,0.574108,0.595644,0.561302,0.566676,0.575684,0.578755,0.568911,0.571785,0.576798,0.572437,0.567613,0.600012,0.575494,0.571513,0.565657,0.572253,0.578008,0.586078,0.567151,0.574298,0.569196,0.568082,0.568347,0.602518,0.577172,0.575032,0.571411,0.605494,0.605487,0.567056,0.57188,0.574101,0.575868,0.592111,0.570019,0.561941,0.572158,0.581438,0.571791,0.596479,0.594991,0.572342,0.568442,0.580888,0.569101,0.593795,0.562498,0.568911,0.574672,0.566676,0.566683,0.596581,0.570019,0.572715,0.569006,0.613837,0.566778,0.564455,0.567233,0.601771,0.567063,0.559434,0.567518,0.599733,0.602138,0.567335,0.562777,0.577084,0.574577,0.559631,0.573931,0.575868,0.571785,0.566961,0.569835,0.569652,0.565575,0.592023,0.601411,0.573273,0.572899,0.562783,0.575589,0.576513,0.566683</t>
+  </si>
+  <si>
+    <t>9.840451,9.847224,9.848256,9.831905,9.82077,9.830329,9.83664,9.830892,9.810831,9.816497,9.813807,9.825125,9.812231,9.807129,9.797557,9.818447,9.813345,9.801266,9.785675,9.800627,9.81437,9.809439,9.783814,9.777326,9.797006,9.803222,9.799873,9.778813,9.781864,9.800716,9.793664,9.787815,9.773711,9.78289,9.79969,9.788555,9.772869,9.778617,9.792917,9.798202,9.784282,9.768141,9.790308,9.787536,9.789479,9.774812,9.780661,9.784758,9.797278,9.791341,9.772951,9.779547,9.788936,9.796361,9.780383,9.768691,9.777971,9.803229,9.79524,9.77825,9.774901,9.786415,9.798481,9.784561,9.772679,9.785125,9.803786,9.7945,9.781504,9.763868,9.787802,9.79524,9.78615,9.774072,9.777788,9.787346,9.790689,9.78734,9.77863,9.779364,9.788555,9.790593,9.783358,9.782618,9.787163,9.794214,9.787068,9.779642,9.78308,9.787713,9.790417,9.785865,9.771008,9.77806,9.794873,9.792733,9.787074,9.77435,9.787435,9.797842</t>
+  </si>
+  <si>
+    <t>0.00393,-0.006885,-0.000238,0.003918,-0.007157,-0.003537,-0.002162,0.000878,0.000311,-0.002205,-0.003278,-0.009956,-0.000793,-0.009679,-0.009679,-0.000503,-0.000793,0.002537,-0.002446,0.001162,-0.003019,0.004454,-0.004141,-0.003586,0.004756,0.003394,-0.003556,-0.007459,-0.004092,0.001137,0.001451,-0.006602,0.002814,0.000348,-0.009148,-0.00247,-0.003309,-0.002156,-0.004129,-0.003833,-0.001619,-0.002723,-0.002446,-0.003007,-0.001083,-0.001909,-0.007175,0.000576,5.2e-05,0.003647,-0.000818,-0.006084,-0.001903,-0.007169,-0.000238,0.001439,-0.003839,-0.002452,-0.002181,-0.004135,0.003375,0.000613,-0.006941,-0.005775,-0.001638,-0.003574,-0.002446,-0.003001,0.000576,-0.001626,0.000588,8e-06,-0.00633,0.002247,-0.001897,-0.004394,-0.00773,0.003067,-0.00054,-0.007989,-0.004672,-0.003303,0.005268,-0.006891,-0.00136,-0.005227,0.000588,-0.006071,0.003936,-0.005492,-0.005504,0.003079,-0.000528,-0.007187,-0.000516,3.3e-05,-0.002476,-0.004394,-0.004425,-0.003586</t>
+  </si>
+  <si>
+    <t>0.001445,-0.001077,-0.008316,-0.00276,-0.005245,0.00755,-0.007163,-0.001354,0.000323,0.002543,-0.003297,-0.003278,-0.000251,-0.010782,0.003369,-0.008556,0.002845,-0.002187,0.003079,-0.002464,0.000619,-0.004961,-0.003278,0.000317,-0.001903,-0.001922,-0.003013,-0.003858,-0.004702,0.001717,0.003388,0.000335,3.3e-05,-0.004141,0.00364,-0.001354,-0.003031,-0.007749,-0.004111,-0.001903,-0.001909,0.001988,-0.005516,-0.00329,-0.006367,-0.000775,-0.002742,-0.007194,-0.003556,-0.003827,-0.003272,0.00171,0.000859,-0.004129,-0.003253,-0.006614,-0.006374,0.000859,-0.001595,-0.007718,0.001427,-0.001891,-0.012188,-0.001909,-0.006904,-0.0072,0.002537,0.000582,-0.004659,0.000878,0.004473,-0.000214,4.5e-05,-0.007453,-0.004968,-0.005523,-0.000522,-0.007995,-0.007477,-0.001052,-0.00329,-0.00244,-0.006337,-0.007459,-0.002729,-0.002748,-0.004974,-0.003852,-0.000799,-0.0044,-0.005763,-0.002988,-0.006898,-0.003858,-0.009389,-0.00358,0.000582,0.000613,-0.007471,-0.001348</t>
   </si>
 </sst>
 </file>
@@ -616,7 +625,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:H3"/>
+  <dimension ref="B2:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -651,22 +660,45 @@
         <v>25</v>
       </c>
       <c r="C3" s="5">
-        <v>0.571</v>
+        <v>0.576</v>
       </c>
       <c r="D3" s="5">
-        <v>0.591</v>
+        <v>0.614</v>
       </c>
       <c r="E3" s="5">
-        <v>0.542</v>
+        <v>0.5590000000000001</v>
       </c>
       <c r="F3" s="5">
-        <v>0.013</v>
+        <v>0.012</v>
       </c>
       <c r="G3" s="5">
         <v>100</v>
       </c>
       <c r="H3" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8">
+      <c r="B4" s="2" t="s">
         <v>26</v>
+      </c>
+      <c r="C4" s="5">
+        <v>9.792999999999999</v>
+      </c>
+      <c r="D4" s="5">
+        <v>9.848000000000001</v>
+      </c>
+      <c r="E4" s="5">
+        <v>9.763999999999999</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0.017</v>
+      </c>
+      <c r="G4" s="5">
+        <v>100</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -676,7 +708,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:H3"/>
+  <dimension ref="B2:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -711,13 +743,13 @@
         <v>25</v>
       </c>
       <c r="C3" s="5">
-        <v>0.001</v>
+        <v>-0.002</v>
       </c>
       <c r="D3" s="5">
-        <v>0.008</v>
+        <v>0.005</v>
       </c>
       <c r="E3" s="5">
-        <v>-0.006</v>
+        <v>-0.01</v>
       </c>
       <c r="F3" s="5">
         <v>0.004</v>
@@ -726,7 +758,30 @@
         <v>100</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8">
+      <c r="B4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="5">
+        <v>-0.003</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0.008</v>
+      </c>
+      <c r="E4" s="5">
+        <v>-0.012</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0.004</v>
+      </c>
+      <c r="G4" s="5">
+        <v>100</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update excel col and row creator
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -63,13 +63,13 @@
     <t>Alex Wang</t>
   </si>
   <si>
-    <t>10:24:45 03-15-2017 Wednesday Pacific Daylight Time</t>
-  </si>
-  <si>
-    <t>10:25:20 03-15-2017 Wednesday Pacific Daylight Time</t>
-  </si>
-  <si>
-    <t>0:0:34 0 days</t>
+    <t>08:18:00 03-16-2017 Thursday Pacific Daylight Time</t>
+  </si>
+  <si>
+    <t>08:18:36 03-16-2017 Thursday Pacific Daylight Time</t>
+  </si>
+  <si>
+    <t>0:0:35 0 days</t>
   </si>
   <si>
     <t>Information</t>
@@ -99,16 +99,16 @@
     <t>BT Idle</t>
   </si>
   <si>
-    <t>0.602613,0.572437,0.573653,0.559441,0.577362,0.577641,0.570209,0.591928,0.58906,0.601866,0.597688,0.572906,0.570487,0.590725,0.601778,0.602145,0.598897,0.603544,0.605025,0.601391,0.571146,0.581812,0.570949,0.563239,0.584053,0.575874,0.575039,0.569461,0.585148,0.593238,0.609957,0.60688,0.579957,0.572158,0.580786,0.567797,0.5769,0.575039,0.573273,0.592036,0.596024,0.60883,0.603164,0.594808,0.602145,0.600841,0.595739,0.600854,0.575311,0.577919,0.569095,0.566588,0.568354,0.571968,0.558972,0.559821,0.570589,0.579115,0.568537,0.569747,0.574855,0.582749,0.587845,0.573273,0.603449,0.575969,0.5819,0.586452,0.605025,0.567151,0.596568,0.569183,0.576153,0.576336,0.56548,0.571886,0.599271,0.60243,0.602328,0.567974,0.571418,0.568259,0.568266,0.579951,0.567518,0.571601,0.568904,0.570861,0.565575,0.569557,0.568075,0.570766,0.562036,0.56938,0.56938,0.600759,0.591099,0.601037,0.58906,0.574285</t>
-  </si>
-  <si>
-    <t>9.796626,9.782788,9.769051,9.791708,9.80647,9.791708,9.784649,9.787163,9.79198,9.793847,9.785573,9.772869,9.791606,9.800342,9.795886,9.78094,9.773406,9.782244,9.79005,9.794404,9.769153,9.786884,9.789214,9.794411,9.781775,9.771938,9.798487,9.795519,9.788283,9.780947,9.776952,9.795227,9.797183,9.788087,9.775464,9.781775,9.797563,9.794316,9.786701,9.784194,9.794588,9.793664,9.789017,9.787353,9.772033,9.797754,9.795519,9.789296,9.779547,9.78753,9.804432,9.799133,9.790417,9.777319,9.793936,9.797006,9.794303,9.779452,9.790125,9.795994,9.796259,9.79236,9.775464,9.790308,9.792645,9.787998,9.784459,9.783909,9.797006,9.804153,9.788182,9.776585,9.781871,9.793936,9.799411,9.782985,9.784092,9.792265,9.791714,9.80257,9.777781,9.78308,9.794031,9.808338,9.783358,9.779832,9.789384,9.80666,9.796911,9.784751,9.779636,9.790322,9.79812,9.790043,9.783535,9.776307,9.792543,9.799418,9.788365,9.779649</t>
-  </si>
-  <si>
-    <t>-0.006885,0.001421,-0.003278,-0.001619,-0.001644,-0.001878,-0.002476,-0.001626,-0.002458,-0.002723,-0.006879,-0.00329,-0.002723,-0.003586,-0.005806,-0.003864,-0.005504,-0.003001,-0.002199,-0.001619,-0.000824,-0.012756,-0.003845,-0.006645,-0.006071,-0.001373,-0.009968,-0.001915,-0.005245,-0.006065,0.000317,-0.001897,-0.003845,-0.00995,-0.004647,0.004485,-0.006904,-0.002717,-0.004961,0.003616,-0.004407,-0.001607,-0.001089,0.000841,-0.006078,-0.001052,-0.00133,0.002,-0.000787,-0.013557,0.001982,0.002265,-0.00276,-0.004955,-0.001644,-0.006374,0.000588,-0.005498,-0.003864,-0.004696,-0.003284,-0.004672,-0.0058,-0.003007,0.002247,-0.006343,-0.006065,-0.004111,-0.001934,-0.003821,-0.003031,-0.001064,-0.002433,-0.002464,-0.009117,-0.005239,0.00615,0.000588,-0.000238,0.000588,0.000298,0.001131,-0.001083,-0.000793,-0.008014,0.001427,-0.000799,0.002284,-0.004943,0.005046,-0.004123,-0.002729,-0.002458,-0.000509,0.004744,-0.007169,-0.003845,-0.00133,-0.007157,-0.003839</t>
-  </si>
-  <si>
-    <t>-0.003568,-0.005245,-0.008563,-0.001915,-0.003001,-0.002711,-0.000787,-0.003562,-0.001342,-0.004955,-0.00022,-0.00691,0.006699,-0.007163,-0.005806,-0.004141,2e-06,-0.000805,-0.001619,-0.001903,0.005589,-0.002489,-0.003284,-0.00551,-0.006084,-0.001897,0.000292,-0.010234,-0.008014,-0.004943,-0.000509,0.004504,-0.002174,0.001975,0.000304,-0.007471,-0.008008,-0.006898,-0.00358,7e-05,0.004201,-0.014094,-0.003278,-0.004104,-0.001915,-0.003852,-0.001626,0.003893,-0.006059,-0.004992,-0.011633,-0.007187,-0.003044,-0.001336,0.001692,-0.001897,0.003092,0.000588,-0.006078,0.002253,0.000582,-0.002199,-0.002193,-0.001064,-0.003025,-0.003839,-0.005523,0.001451,0.001451,-0.004148,-0.003858,0.000311,-0.002452,-0.008008,-0.004104,-0.005794,-0.000251,-0.00133,-0.004394,-0.002748,0.001982,-0.004129,0.000588,-0.002754,-0.001083,-0.003876,0.000878,-0.001071,-0.005529,-0.000799,-0.000251,-0.003568,-0.009679,-0.0058,-0.003297,-0.004684,-0.006047,-0.003864,-0.003543,3.9e-05</t>
+    <t>0.569652,0.568823,0.57169,0.556466,0.567987,0.57188,0.544584,0.567892,0.567708,0.571601,0.575596,0.574387,0.567702,0.575583,0.568911,0.57978,0.563429,0.575399,0.568911,0.597226,0.568082,0.570589,0.571336,0.578001,0.596948,0.573836,0.573456,0.571424,0.57031,0.568911,0.565569,0.571791,0.568259,0.576153,0.57476,0.570297,0.576812,0.566309,0.572987,0.570576,0.576988,0.564455,0.57243,0.571044,0.569373,0.56334,0.575507,0.579869,0.566493,0.569835,0.566221,0.571778,0.573089,0.595277,0.566765,0.573836,0.568449,0.578843,0.56798,0.572715,0.565942,0.570576,0.566214,0.562043,0.56817,0.56101,0.573374,0.576425,0.562606,0.560467,0.57402,0.573368,0.573646,0.570202,0.575039,0.562036,0.564461,0.567987,0.575691,0.571968,0.576336,0.561859,0.572335,0.569278,0.57281,0.578001,0.566961,0.577729,0.581452,0.563144,0.572722,0.567423,0.574108,0.581825,0.574767,0.576982,0.573836,0.56724,0.574203,0.567335</t>
+  </si>
+  <si>
+    <t>9.776857,9.767393,9.748175,9.768413,9.774078,9.773134,9.762278,9.754948,9.765247,9.77361,9.771014,9.764506,9.756341,9.771476,9.772394,9.76721,9.751599,9.762278,9.772033,9.764785,9.756334,9.749194,9.761171,9.775743,9.765994,9.754479,9.760981,9.763025,9.76933,9.757075,9.757081,9.765355,9.770356,9.762944,9.752998,9.75579,9.758569,9.770166,9.771565,9.752169,9.754581,9.78289,9.774907,9.76488,9.751232,9.775559,9.779262,9.766001,9.761918,9.749846,9.765335,9.777319,9.77185,9.754853,9.757645,9.765899,9.770628,9.750036,9.757176,9.761531,9.773698,9.773793,9.755689,9.755043,9.768406,9.777414,9.769989,9.742971,9.761544,9.773053,9.764323,9.766083,9.749656,9.766463,9.775471,9.76414,9.748073,9.758094,9.766279,9.772862,9.76043,9.75272,9.756531,9.778528,9.770274,9.761266,9.753922,9.768684,9.77918,9.764038,9.759398,9.759866,9.771565,9.778161,9.760335,9.746972,9.769153,9.777135,9.768413,9.763025</t>
+  </si>
+  <si>
+    <t>0.002247,-0.002723,0.000853,0.00644,0.002271,-0.002199,0.003394,0.006397,0.001421,-0.00133,0.007821,-0.006614,-0.001909,-0.001101,0.000329,0.001433,0.004763,0.000594,-0.000491,-0.002742,0.006717,-0.000799,-0.000509,0.000859,-0.003845,-0.001626,0.002284,0.001686,0.003073,0.001421,-0.002723,-0.000775,-0.00305,-0.003309,-0.00133,-0.001909,-0.001897,-0.004123,-0.001632,-0.005245,0.003918,-0.000805,-0.001595,0.005866,0.004214,-0.003845,2.7e-05,-0.001064,0.000576,0.005034,3.9e-05,-0.003031,-0.001064,0.000872,0.000613,0.00171,0.001975,-0.006337,0.001421,0.001982,0.000884,-0.000238,0.004448,-0.004123,0.002789,0.001667,0.005318,0.004744,0.002833,0.000607,-0.000793,-0.006633,0.006699,0.004491,0.005324,-0.000522,-0.001632,0.00282,0.000323,0.002524,0.000304,-0.004665,0.001982,0.002808,-0.000522,-0.002742,0.000607,-0.004129,-0.006885,0.003357,-0.002723,0.004177,-0.00358,0.00311,-0.002705,-0.001077,-0.002717,-0.000522,-0.001909,0.002278</t>
+  </si>
+  <si>
+    <t>-0.000781,-0.002433,0.000607,0.002253,0.003085,-0.001064,-0.003031,-0.001613,-0.002168,0.003924,0.001155,0.00586,3.9e-05,-0.007736,-0.000781,0.001704,0.003634,0.000588,0.000896,0.000607,-0.00329,0.002253,-0.000509,-0.000503,-0.000805,0.002518,0.000298,0.001408,-0.001089,0.005022,0.001988,-0.001626,-0.005523,-0.003858,-0.004092,-0.000503,-0.00133,0.000341,-0.001058,-0.002181,0.002259,0.001427,0.001433,0.003357,0.006409,-0.005233,-0.001897,-0.00276,0.007796,-0.005504,-0.00133,0.002278,0.005305,0.001433,-0.003309,-0.000787,0.003918,0.002555,0.004479,0.004195,0.001994,-0.001632,0.003375,-0.004678,-0.001626,0.006138,-0.000781,-0.002994,-0.001064,-0.001348,0.003381,0.001125,0.000582,-0.000263,0.002241,0.00253,-0.001909,0.002006,-0.000787,0.005028,0.002808,-0.003272,-0.003864,0.002839,0.007001,-0.002446,3.9e-05,0.003634,0.004226,-0.006059,0.009486,-0.0058,0.001982,0.00089,-0.002181,0.000853,0.007537,-0.002458,0.001982,0.0006</t>
   </si>
 </sst>
 </file>
@@ -660,16 +660,16 @@
         <v>25</v>
       </c>
       <c r="C3" s="5">
-        <v>0.582</v>
+        <v>0.571</v>
       </c>
       <c r="D3" s="5">
-        <v>0.61</v>
+        <v>0.597</v>
       </c>
       <c r="E3" s="5">
-        <v>0.5590000000000001</v>
+        <v>0.545</v>
       </c>
       <c r="F3" s="5">
-        <v>0.014</v>
+        <v>0.007</v>
       </c>
       <c r="G3" s="5">
         <v>100</v>
@@ -683,13 +683,13 @@
         <v>26</v>
       </c>
       <c r="C4" s="5">
-        <v>9.789</v>
+        <v>9.763999999999999</v>
       </c>
       <c r="D4" s="5">
-        <v>9.808</v>
+        <v>9.782999999999999</v>
       </c>
       <c r="E4" s="5">
-        <v>9.769</v>
+        <v>9.743</v>
       </c>
       <c r="F4" s="5">
         <v>0.008999999999999999</v>
@@ -743,16 +743,16 @@
         <v>25</v>
       </c>
       <c r="C3" s="5">
-        <v>-0.003</v>
+        <v>0</v>
       </c>
       <c r="D3" s="5">
-        <v>0.006</v>
+        <v>0.008</v>
       </c>
       <c r="E3" s="5">
-        <v>-0.014</v>
+        <v>-0.007</v>
       </c>
       <c r="F3" s="5">
-        <v>0.004</v>
+        <v>0.003</v>
       </c>
       <c r="G3" s="5">
         <v>100</v>
@@ -766,16 +766,16 @@
         <v>26</v>
       </c>
       <c r="C4" s="5">
-        <v>-0.003</v>
+        <v>0</v>
       </c>
       <c r="D4" s="5">
-        <v>0.007</v>
+        <v>0.008999999999999999</v>
       </c>
       <c r="E4" s="5">
-        <v>-0.014</v>
+        <v>-0.008</v>
       </c>
       <c r="F4" s="5">
-        <v>0.004</v>
+        <v>0.003</v>
       </c>
       <c r="G4" s="5">
         <v>100</v>

</xml_diff>

<commit_message>
update excel array creator
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -63,10 +63,10 @@
     <t>Alex Wang</t>
   </si>
   <si>
-    <t>08:18:00 03-16-2017 Thursday Pacific Daylight Time</t>
-  </si>
-  <si>
-    <t>08:18:36 03-16-2017 Thursday Pacific Daylight Time</t>
+    <t>08:49:11 03-21-2017 Tuesday Pacific Daylight Time</t>
+  </si>
+  <si>
+    <t>08:49:46 03-21-2017 Tuesday Pacific Daylight Time</t>
   </si>
   <si>
     <t>0:0:35 0 days</t>
@@ -99,16 +99,16 @@
     <t>BT Idle</t>
   </si>
   <si>
-    <t>0.569652,0.568823,0.57169,0.556466,0.567987,0.57188,0.544584,0.567892,0.567708,0.571601,0.575596,0.574387,0.567702,0.575583,0.568911,0.57978,0.563429,0.575399,0.568911,0.597226,0.568082,0.570589,0.571336,0.578001,0.596948,0.573836,0.573456,0.571424,0.57031,0.568911,0.565569,0.571791,0.568259,0.576153,0.57476,0.570297,0.576812,0.566309,0.572987,0.570576,0.576988,0.564455,0.57243,0.571044,0.569373,0.56334,0.575507,0.579869,0.566493,0.569835,0.566221,0.571778,0.573089,0.595277,0.566765,0.573836,0.568449,0.578843,0.56798,0.572715,0.565942,0.570576,0.566214,0.562043,0.56817,0.56101,0.573374,0.576425,0.562606,0.560467,0.57402,0.573368,0.573646,0.570202,0.575039,0.562036,0.564461,0.567987,0.575691,0.571968,0.576336,0.561859,0.572335,0.569278,0.57281,0.578001,0.566961,0.577729,0.581452,0.563144,0.572722,0.567423,0.574108,0.581825,0.574767,0.576982,0.573836,0.56724,0.574203,0.567335</t>
-  </si>
-  <si>
-    <t>9.776857,9.767393,9.748175,9.768413,9.774078,9.773134,9.762278,9.754948,9.765247,9.77361,9.771014,9.764506,9.756341,9.771476,9.772394,9.76721,9.751599,9.762278,9.772033,9.764785,9.756334,9.749194,9.761171,9.775743,9.765994,9.754479,9.760981,9.763025,9.76933,9.757075,9.757081,9.765355,9.770356,9.762944,9.752998,9.75579,9.758569,9.770166,9.771565,9.752169,9.754581,9.78289,9.774907,9.76488,9.751232,9.775559,9.779262,9.766001,9.761918,9.749846,9.765335,9.777319,9.77185,9.754853,9.757645,9.765899,9.770628,9.750036,9.757176,9.761531,9.773698,9.773793,9.755689,9.755043,9.768406,9.777414,9.769989,9.742971,9.761544,9.773053,9.764323,9.766083,9.749656,9.766463,9.775471,9.76414,9.748073,9.758094,9.766279,9.772862,9.76043,9.75272,9.756531,9.778528,9.770274,9.761266,9.753922,9.768684,9.77918,9.764038,9.759398,9.759866,9.771565,9.778161,9.760335,9.746972,9.769153,9.777135,9.768413,9.763025</t>
-  </si>
-  <si>
-    <t>0.002247,-0.002723,0.000853,0.00644,0.002271,-0.002199,0.003394,0.006397,0.001421,-0.00133,0.007821,-0.006614,-0.001909,-0.001101,0.000329,0.001433,0.004763,0.000594,-0.000491,-0.002742,0.006717,-0.000799,-0.000509,0.000859,-0.003845,-0.001626,0.002284,0.001686,0.003073,0.001421,-0.002723,-0.000775,-0.00305,-0.003309,-0.00133,-0.001909,-0.001897,-0.004123,-0.001632,-0.005245,0.003918,-0.000805,-0.001595,0.005866,0.004214,-0.003845,2.7e-05,-0.001064,0.000576,0.005034,3.9e-05,-0.003031,-0.001064,0.000872,0.000613,0.00171,0.001975,-0.006337,0.001421,0.001982,0.000884,-0.000238,0.004448,-0.004123,0.002789,0.001667,0.005318,0.004744,0.002833,0.000607,-0.000793,-0.006633,0.006699,0.004491,0.005324,-0.000522,-0.001632,0.00282,0.000323,0.002524,0.000304,-0.004665,0.001982,0.002808,-0.000522,-0.002742,0.000607,-0.004129,-0.006885,0.003357,-0.002723,0.004177,-0.00358,0.00311,-0.002705,-0.001077,-0.002717,-0.000522,-0.001909,0.002278</t>
-  </si>
-  <si>
-    <t>-0.000781,-0.002433,0.000607,0.002253,0.003085,-0.001064,-0.003031,-0.001613,-0.002168,0.003924,0.001155,0.00586,3.9e-05,-0.007736,-0.000781,0.001704,0.003634,0.000588,0.000896,0.000607,-0.00329,0.002253,-0.000509,-0.000503,-0.000805,0.002518,0.000298,0.001408,-0.001089,0.005022,0.001988,-0.001626,-0.005523,-0.003858,-0.004092,-0.000503,-0.00133,0.000341,-0.001058,-0.002181,0.002259,0.001427,0.001433,0.003357,0.006409,-0.005233,-0.001897,-0.00276,0.007796,-0.005504,-0.00133,0.002278,0.005305,0.001433,-0.003309,-0.000787,0.003918,0.002555,0.004479,0.004195,0.001994,-0.001632,0.003375,-0.004678,-0.001626,0.006138,-0.000781,-0.002994,-0.001064,-0.001348,0.003381,0.001125,0.000582,-0.000263,0.002241,0.00253,-0.001909,0.002006,-0.000787,0.005028,0.002808,-0.003272,-0.003864,0.002839,0.007001,-0.002446,3.9e-05,0.003634,0.004226,-0.006059,0.009486,-0.0058,0.001982,0.00089,-0.002181,0.000853,0.007537,-0.002458,0.001982,0.0006</t>
+    <t>0.58442,0.60957,0.57188,0.583667,0.609672,0.580704,0.576336,0.602138,0.614027,0.574672,0.588123,0.609387,0.576513,0.575317,0.577355,0.608368,0.595277,0.572437,0.580229,0.612084,0.575596,0.600562,0.617464,0.591187,0.578761,0.573082,0.61811,0.610684,0.577267,0.576248,0.611248,0.615059,0.573361,0.583578,0.580046,0.584135,0.597682,0.577444,0.577552,0.614027,0.606411,0.576798,0.60724,0.586459,0.575678,0.613558,0.601398,0.575032,0.577641,0.608463,0.603347,0.580704,0.584692,0.580426,0.607437,0.608836,0.575507,0.582192,0.600936,0.567702,0.588769,0.611323,0.605576,0.579767,0.615052,0.57671,0.566221,0.606051,0.589801,0.580616,0.580698,0.607342,0.584971,0.576526,0.575956,0.607539,0.587206,0.574665,0.581255,0.608184,0.578938,0.571975,0.610039,0.611805,0.613286,0.569828,0.578748,0.615236,0.584135,0.579665,0.582552,0.579964,0.600474,0.572715,0.584977,0.613748,0.572063,0.578558,0.574101,0.614489</t>
+  </si>
+  <si>
+    <t>9.866544,9.869235,9.875084,9.867557,9.845002,9.854839,9.859017,9.864683,9.855206,9.842496,9.846857,9.856979,9.850661,9.835621,9.829778,9.84435,9.84685,9.834221,9.811578,9.824384,9.838304,9.846762,9.824669,9.814921,9.825322,9.832842,9.828949,9.818175,9.821694,9.824201,9.83757,9.825967,9.817985,9.82096,9.836178,9.8281,9.821232,9.817713,9.824309,9.83507,9.825777,9.822536,9.810091,9.824201,9.832006,9.828284,9.809717,9.826246,9.841558,9.827917,9.819472,9.817067,9.825322,9.832462,9.827917,9.818909,9.816232,9.833671,9.839615,9.822618,9.820953,9.824194,9.838311,9.836551,9.820953,9.81204,9.830607,9.83433,9.832937,9.816871,9.81825,9.836171,9.837387,9.822618,9.813623,9.828847,9.832652,9.83312,9.812699,9.822169,9.829873,9.834418,9.831164,9.81863,9.821137,9.834228,9.834235,9.828562,9.808141,9.82522,9.832475,9.836184,9.818155,9.817061,9.821979,9.838963,9.826531,9.821884,9.823277,9.838026</t>
+  </si>
+  <si>
+    <t>-0.001064,-0.004413,-0.000528,-0.001071,0.001704,-0.005523,-0.005245,-0.002754,0.000348,-0.000793,0.002814,-0.001354,-0.001077,0.001143,-0.002187,0.004201,-0.004117,0.000588,-0.001915,0.002814,0.002524,0.000853,0.002826,0.003085,3.3e-05,3.3e-05,-0.007194,-0.002205,0.000613,0.006452,-0.006337,4.5e-05,-0.004931,-0.003007,-0.003549,-0.003556,-0.001077,0.002265,7e-05,-0.002723,-0.003574,-0.004968,-0.001379,0.003653,-0.000799,-0.005794,0.006964,-0.001607,0.000878,-0.006078,-0.002483,-0.004431,-0.002193,-0.011048,-0.003574,-0.001632,-0.000522,-0.00022,0.001704,-0.001348,-0.001064,-0.005523,-0.001058,-0.000824,-0.007712,0.00475,-0.003013,0.006458,-0.000509,0.001686,-0.004135,3.3e-05,-0.003019,0.00118,0.003085,-0.001613,-0.006343,-0.003001,2.1e-05,-0.001626,-0.004931,-0.001089,-0.009944,-0.004394,-0.006633,-0.000232,-0.002181,0.000866,-0.004968,4.5e-05,-0.002193,0.011145,-0.000799,-0.000503,0.003079,0.000878,-0.002199,-0.003303,0.001414,0.007248</t>
+  </si>
+  <si>
+    <t>0.000872,0.000588,-0.003864,0.00118,-0.001058,-0.006071,-0.002717,0.003924,-0.008001,-0.001083,-0.005782,-0.001083,0.000329,-0.004943,-0.005806,-0.000226,-0.006891,-0.002187,0.000298,0.00253,0.002,-0.003007,0.000298,-0.00136,-0.006349,0.00533,0.004195,3.9e-05,-0.0058,0.001988,0.000329,-0.001083,-0.002717,0.001445,-0.010215,-0.003568,0.001162,0.00253,-0.001909,-0.001626,0.001143,0.002518,0.001717,-0.002168,-0.002174,-0.007181,0.001414,-0.00244,-0.003001,0.001988,2.7e-05,-0.000238,0.001125,0.002518,0.005589,0.000329,2.1e-05,-0.000793,0.000866,0.002802,0.000323,0.005854,-0.005794,0.003647,0.000329,0.004756,0.001982,0.00311,-0.005233,-0.003586,0.002259,-0.001354,4.5e-05,-0.003845,-0.001885,-0.001885,-0.005541,-0.004968,-0.000503,-0.002464,0.003653,-0.00633,0.008351,-0.000793,0.000872,-0.003013,-0.005788,-0.006626,0.001717,0.001723,0.000304,5.8e-05,-0.006916,-0.007724,-0.002211,-0.001077,0.002826,0.000619,0.001969,-0.000516</t>
   </si>
 </sst>
 </file>
@@ -660,16 +660,16 @@
         <v>25</v>
       </c>
       <c r="C3" s="5">
-        <v>0.571</v>
+        <v>0.59</v>
       </c>
       <c r="D3" s="5">
-        <v>0.597</v>
+        <v>0.618</v>
       </c>
       <c r="E3" s="5">
-        <v>0.545</v>
+        <v>0.5659999999999999</v>
       </c>
       <c r="F3" s="5">
-        <v>0.007</v>
+        <v>0.016</v>
       </c>
       <c r="G3" s="5">
         <v>100</v>
@@ -683,16 +683,16 @@
         <v>26</v>
       </c>
       <c r="C4" s="5">
-        <v>9.763999999999999</v>
+        <v>9.831</v>
       </c>
       <c r="D4" s="5">
-        <v>9.782999999999999</v>
+        <v>9.875</v>
       </c>
       <c r="E4" s="5">
-        <v>9.743</v>
+        <v>9.808</v>
       </c>
       <c r="F4" s="5">
-        <v>0.008999999999999999</v>
+        <v>0.014</v>
       </c>
       <c r="G4" s="5">
         <v>100</v>
@@ -743,16 +743,16 @@
         <v>25</v>
       </c>
       <c r="C3" s="5">
-        <v>0</v>
+        <v>-0.001</v>
       </c>
       <c r="D3" s="5">
-        <v>0.008</v>
+        <v>0.011</v>
       </c>
       <c r="E3" s="5">
-        <v>-0.007</v>
+        <v>-0.011</v>
       </c>
       <c r="F3" s="5">
-        <v>0.003</v>
+        <v>0.004</v>
       </c>
       <c r="G3" s="5">
         <v>100</v>
@@ -766,16 +766,16 @@
         <v>26</v>
       </c>
       <c r="C4" s="5">
-        <v>0</v>
+        <v>-0.001</v>
       </c>
       <c r="D4" s="5">
-        <v>0.008999999999999999</v>
+        <v>0.008</v>
       </c>
       <c r="E4" s="5">
-        <v>-0.008</v>
+        <v>-0.01</v>
       </c>
       <c r="F4" s="5">
-        <v>0.003</v>
+        <v>0.004</v>
       </c>
       <c r="G4" s="5">
         <v>100</v>

</xml_diff>

<commit_message>
Update work_flow excel writer comment and sequence
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -63,13 +63,13 @@
     <t>Alex Wang</t>
   </si>
   <si>
-    <t>08:49:11 03-21-2017 Tuesday Pacific Daylight Time</t>
-  </si>
-  <si>
-    <t>08:49:46 03-21-2017 Tuesday Pacific Daylight Time</t>
-  </si>
-  <si>
-    <t>0:0:35 0 days</t>
+    <t>21:36:18 03-21-2017 Tuesday Pacific Daylight Time</t>
+  </si>
+  <si>
+    <t>21:36:53 03-21-2017 Tuesday Pacific Daylight Time</t>
+  </si>
+  <si>
+    <t>0:0:34 0 days</t>
   </si>
   <si>
     <t>Information</t>
@@ -99,16 +99,16 @@
     <t>BT Idle</t>
   </si>
   <si>
-    <t>0.58442,0.60957,0.57188,0.583667,0.609672,0.580704,0.576336,0.602138,0.614027,0.574672,0.588123,0.609387,0.576513,0.575317,0.577355,0.608368,0.595277,0.572437,0.580229,0.612084,0.575596,0.600562,0.617464,0.591187,0.578761,0.573082,0.61811,0.610684,0.577267,0.576248,0.611248,0.615059,0.573361,0.583578,0.580046,0.584135,0.597682,0.577444,0.577552,0.614027,0.606411,0.576798,0.60724,0.586459,0.575678,0.613558,0.601398,0.575032,0.577641,0.608463,0.603347,0.580704,0.584692,0.580426,0.607437,0.608836,0.575507,0.582192,0.600936,0.567702,0.588769,0.611323,0.605576,0.579767,0.615052,0.57671,0.566221,0.606051,0.589801,0.580616,0.580698,0.607342,0.584971,0.576526,0.575956,0.607539,0.587206,0.574665,0.581255,0.608184,0.578938,0.571975,0.610039,0.611805,0.613286,0.569828,0.578748,0.615236,0.584135,0.579665,0.582552,0.579964,0.600474,0.572715,0.584977,0.613748,0.572063,0.578558,0.574101,0.614489</t>
-  </si>
-  <si>
-    <t>9.866544,9.869235,9.875084,9.867557,9.845002,9.854839,9.859017,9.864683,9.855206,9.842496,9.846857,9.856979,9.850661,9.835621,9.829778,9.84435,9.84685,9.834221,9.811578,9.824384,9.838304,9.846762,9.824669,9.814921,9.825322,9.832842,9.828949,9.818175,9.821694,9.824201,9.83757,9.825967,9.817985,9.82096,9.836178,9.8281,9.821232,9.817713,9.824309,9.83507,9.825777,9.822536,9.810091,9.824201,9.832006,9.828284,9.809717,9.826246,9.841558,9.827917,9.819472,9.817067,9.825322,9.832462,9.827917,9.818909,9.816232,9.833671,9.839615,9.822618,9.820953,9.824194,9.838311,9.836551,9.820953,9.81204,9.830607,9.83433,9.832937,9.816871,9.81825,9.836171,9.837387,9.822618,9.813623,9.828847,9.832652,9.83312,9.812699,9.822169,9.829873,9.834418,9.831164,9.81863,9.821137,9.834228,9.834235,9.828562,9.808141,9.82522,9.832475,9.836184,9.818155,9.817061,9.821979,9.838963,9.826531,9.821884,9.823277,9.838026</t>
-  </si>
-  <si>
-    <t>-0.001064,-0.004413,-0.000528,-0.001071,0.001704,-0.005523,-0.005245,-0.002754,0.000348,-0.000793,0.002814,-0.001354,-0.001077,0.001143,-0.002187,0.004201,-0.004117,0.000588,-0.001915,0.002814,0.002524,0.000853,0.002826,0.003085,3.3e-05,3.3e-05,-0.007194,-0.002205,0.000613,0.006452,-0.006337,4.5e-05,-0.004931,-0.003007,-0.003549,-0.003556,-0.001077,0.002265,7e-05,-0.002723,-0.003574,-0.004968,-0.001379,0.003653,-0.000799,-0.005794,0.006964,-0.001607,0.000878,-0.006078,-0.002483,-0.004431,-0.002193,-0.011048,-0.003574,-0.001632,-0.000522,-0.00022,0.001704,-0.001348,-0.001064,-0.005523,-0.001058,-0.000824,-0.007712,0.00475,-0.003013,0.006458,-0.000509,0.001686,-0.004135,3.3e-05,-0.003019,0.00118,0.003085,-0.001613,-0.006343,-0.003001,2.1e-05,-0.001626,-0.004931,-0.001089,-0.009944,-0.004394,-0.006633,-0.000232,-0.002181,0.000866,-0.004968,4.5e-05,-0.002193,0.011145,-0.000799,-0.000503,0.003079,0.000878,-0.002199,-0.003303,0.001414,0.007248</t>
-  </si>
-  <si>
-    <t>0.000872,0.000588,-0.003864,0.00118,-0.001058,-0.006071,-0.002717,0.003924,-0.008001,-0.001083,-0.005782,-0.001083,0.000329,-0.004943,-0.005806,-0.000226,-0.006891,-0.002187,0.000298,0.00253,0.002,-0.003007,0.000298,-0.00136,-0.006349,0.00533,0.004195,3.9e-05,-0.0058,0.001988,0.000329,-0.001083,-0.002717,0.001445,-0.010215,-0.003568,0.001162,0.00253,-0.001909,-0.001626,0.001143,0.002518,0.001717,-0.002168,-0.002174,-0.007181,0.001414,-0.00244,-0.003001,0.001988,2.7e-05,-0.000238,0.001125,0.002518,0.005589,0.000329,2.1e-05,-0.000793,0.000866,0.002802,0.000323,0.005854,-0.005794,0.003647,0.000329,0.004756,0.001982,0.00311,-0.005233,-0.003586,0.002259,-0.001354,4.5e-05,-0.003845,-0.001885,-0.001885,-0.005541,-0.004968,-0.000503,-0.002464,0.003653,-0.00633,0.008351,-0.000793,0.000872,-0.003013,-0.005788,-0.006626,0.001717,0.001723,0.000304,5.8e-05,-0.006916,-0.007724,-0.002211,-0.001077,0.002826,0.000619,0.001969,-0.000516</t>
+    <t>0.592485,0.565474,0.594074,0.566968,0.589244,0.593415,0.593327,0.593327,0.591846,0.566221,0.596024,0.572444,0.562695,0.590175,0.56919,0.59063,0.593409,0.563802,0.591187,0.56046,0.587655,0.5951,0.594726,0.563619,0.58794,0.594808,0.59546,0.589896,0.592131,0.554991,0.586635,0.558504,0.595739,0.563626,0.594448,0.561024,0.592953,0.569183,0.588136,0.567695,0.600379,0.564448,0.592396,0.591839,0.56724,0.592111,0.555256,0.593517,0.557124,0.604557,0.559543,0.592491,0.555643,0.596764,0.561112,0.598334,0.594346,0.565942,0.584509,0.562878,0.598062,0.559529,0.596846,0.569658,0.597315,0.556744,0.597593,0.569747,0.586173,0.558232,0.595182,0.600284,0.562416,0.592858,0.564828,0.594257,0.561207,0.592219,0.563986,0.597885,0.56046,0.588598,0.563619,0.593612,0.560745,0.593327,0.588497,0.605861,0.594991,0.566955,0.594529,0.562885,0.584135,0.564088,0.598252,0.566221,0.588028,0.563259,0.600113,0.565283</t>
+  </si>
+  <si>
+    <t>9.793752,9.802672,9.810648,9.800165,9.795709,9.791246,9.797183,9.807224,9.795607,9.782604,9.792448,9.810186,9.807584,9.797835,9.784934,9.795614,9.810464,9.800247,9.788739,9.797183,9.800994,9.809072,9.79988,9.786334,9.797842,9.805267,9.80509,9.789581,9.785865,9.796911,9.8113,9.801646,9.78558,9.786599,9.807387,9.809262,9.802482,9.779269,9.801735,9.810091,9.80916,9.790974,9.786612,9.79681,9.803318,9.796531,9.786137,9.79329,9.803026,9.807686,9.794962,9.788087,9.794676,9.811008,9.812034,9.789941,9.791429,9.805179,9.804527,9.808691,9.786707,9.795702,9.802102,9.8177,9.792353,9.788657,9.790125,9.811762,9.809819,9.793385,9.786796,9.79524,9.80935,9.803419,9.790505,9.79776,9.808882,9.808229,9.799703,9.794119,9.805444,9.805356,9.798222,9.791803,9.795512,9.802298,9.816687,9.79348,9.78846,9.794309,9.804602,9.803039,9.797747,9.791708,9.797835,9.810926,9.80397,9.793847,9.794139,9.804432</t>
+  </si>
+  <si>
+    <t>0.000613,-0.002742,-0.004129,-0.002187,0.001704,-0.001385,-0.005264,-0.001897,-0.00691,-0.001367,-0.003007,-0.002168,-0.00247,-0.00022,0.000311,0.005577,-0.002458,-0.001077,-0.005239,-0.005794,-0.013286,-0.006343,-0.004407,0.000298,-0.006608,-0.004672,-0.004678,0.000866,4.5e-05,-0.003013,-0.002452,-0.003013,-0.009395,-0.001613,0.00393,-0.002433,-0.002168,-0.00136,-0.002729,0.003104,0.000317,-0.004974,-0.005825,-0.002174,-0.003574,-0.000805,-0.002458,0.001686,-0.004123,-0.006626,-0.000793,-0.002187,0.003369,-0.002729,3.9e-05,-0.001626,0.003918,-0.000232,-0.003562,-0.000818,0.001162,-0.005788,-0.006078,-0.000787,-0.007459,-0.005794,-0.001891,-0.001891,0.001704,-0.00133,-0.003556,-0.003833,-0.003562,-0.003858,-0.004407,0.003085,-0.001613,3.3e-05,-0.00276,-0.010795,-0.001891,-0.005214,0.001439,-0.003303,0.001131,0.001433,-0.002181,-0.006639,-0.001626,0.003344,0.000576,-0.003852,-0.007169,-0.001613,0.006144,-0.002174,-0.000238,-0.005245,-0.005529,-0.006608</t>
+  </si>
+  <si>
+    <t>-0.000812,0.00393,-0.00498,-0.004702,-0.007181,0.000323,0.001421,0.000847,-0.007742,-0.000787,-0.00247,-0.0044,-0.003568,-0.002711,-0.002476,0.004756,-0.00638,0.004775,-0.001638,-0.001891,-0.001922,0.000329,3.3e-05,0.003659,0.004183,-0.000509,-0.007163,-0.001077,-0.006337,-0.003019,0.000853,-0.005523,0.000872,-0.00329,-0.000793,-0.001058,0.004485,-0.0044,-0.008291,-0.00329,-0.004117,-0.004659,-0.002168,-0.004955,-0.003593,-0.003821,0.002259,-0.000244,-0.003574,0.004195,-0.001607,-0.004918,-0.003833,0.003351,-0.006608,-0.002174,-0.001058,-0.003839,-0.004918,-0.004943,-0.005782,0.002259,-0.002729,-0.000805,-0.00609,2.1e-05,0.001445,0.002253,-0.000516,-0.000497,0.000884,-0.001077,-0.005782,-0.009142,-0.005486,-0.002476,-0.004129,0.001988,0.000563,-0.000793,-0.006916,0.004491,-0.003284,-0.004135,-0.000534,0.002247,-0.005775,-0.006361,0.001137,0.001975,-0.002458,0.005324,-0.000818,-0.003858,-0.004653,-0.004672,-0.00136,0.000884,-0.001077,0.003085</t>
   </si>
 </sst>
 </file>
@@ -660,13 +660,13 @@
         <v>25</v>
       </c>
       <c r="C3" s="5">
-        <v>0.59</v>
+        <v>0.581</v>
       </c>
       <c r="D3" s="5">
-        <v>0.618</v>
+        <v>0.606</v>
       </c>
       <c r="E3" s="5">
-        <v>0.5659999999999999</v>
+        <v>0.555</v>
       </c>
       <c r="F3" s="5">
         <v>0.016</v>
@@ -683,16 +683,16 @@
         <v>26</v>
       </c>
       <c r="C4" s="5">
-        <v>9.831</v>
+        <v>9.798999999999999</v>
       </c>
       <c r="D4" s="5">
-        <v>9.875</v>
+        <v>9.818</v>
       </c>
       <c r="E4" s="5">
-        <v>9.808</v>
+        <v>9.779</v>
       </c>
       <c r="F4" s="5">
-        <v>0.014</v>
+        <v>0.008</v>
       </c>
       <c r="G4" s="5">
         <v>100</v>
@@ -743,16 +743,16 @@
         <v>25</v>
       </c>
       <c r="C3" s="5">
-        <v>-0.001</v>
+        <v>-0.002</v>
       </c>
       <c r="D3" s="5">
-        <v>0.011</v>
+        <v>0.006</v>
       </c>
       <c r="E3" s="5">
-        <v>-0.011</v>
+        <v>-0.013</v>
       </c>
       <c r="F3" s="5">
-        <v>0.004</v>
+        <v>0.003</v>
       </c>
       <c r="G3" s="5">
         <v>100</v>
@@ -766,16 +766,16 @@
         <v>26</v>
       </c>
       <c r="C4" s="5">
-        <v>-0.001</v>
+        <v>-0.002</v>
       </c>
       <c r="D4" s="5">
-        <v>0.008</v>
+        <v>0.005</v>
       </c>
       <c r="E4" s="5">
-        <v>-0.01</v>
+        <v>-0.008999999999999999</v>
       </c>
       <c r="F4" s="5">
-        <v>0.004</v>
+        <v>0.003</v>
       </c>
       <c r="G4" s="5">
         <v>100</v>

</xml_diff>

<commit_message>
Update decorator starter and ender for main flow
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -63,13 +63,13 @@
     <t>Alex Wang</t>
   </si>
   <si>
-    <t>21:36:18 03-21-2017 Tuesday Pacific Daylight Time</t>
-  </si>
-  <si>
-    <t>21:36:53 03-21-2017 Tuesday Pacific Daylight Time</t>
-  </si>
-  <si>
-    <t>0:0:34 0 days</t>
+    <t>09:11:53 03-22-2017 Wednesday Pacific Daylight Time</t>
+  </si>
+  <si>
+    <t>09:12:28 03-22-2017 Wednesday Pacific Daylight Time</t>
+  </si>
+  <si>
+    <t>0:0:35 0 days</t>
   </si>
   <si>
     <t>Information</t>
@@ -99,16 +99,16 @@
     <t>BT Idle</t>
   </si>
   <si>
-    <t>0.592485,0.565474,0.594074,0.566968,0.589244,0.593415,0.593327,0.593327,0.591846,0.566221,0.596024,0.572444,0.562695,0.590175,0.56919,0.59063,0.593409,0.563802,0.591187,0.56046,0.587655,0.5951,0.594726,0.563619,0.58794,0.594808,0.59546,0.589896,0.592131,0.554991,0.586635,0.558504,0.595739,0.563626,0.594448,0.561024,0.592953,0.569183,0.588136,0.567695,0.600379,0.564448,0.592396,0.591839,0.56724,0.592111,0.555256,0.593517,0.557124,0.604557,0.559543,0.592491,0.555643,0.596764,0.561112,0.598334,0.594346,0.565942,0.584509,0.562878,0.598062,0.559529,0.596846,0.569658,0.597315,0.556744,0.597593,0.569747,0.586173,0.558232,0.595182,0.600284,0.562416,0.592858,0.564828,0.594257,0.561207,0.592219,0.563986,0.597885,0.56046,0.588598,0.563619,0.593612,0.560745,0.593327,0.588497,0.605861,0.594991,0.566955,0.594529,0.562885,0.584135,0.564088,0.598252,0.566221,0.588028,0.563259,0.600113,0.565283</t>
-  </si>
-  <si>
-    <t>9.793752,9.802672,9.810648,9.800165,9.795709,9.791246,9.797183,9.807224,9.795607,9.782604,9.792448,9.810186,9.807584,9.797835,9.784934,9.795614,9.810464,9.800247,9.788739,9.797183,9.800994,9.809072,9.79988,9.786334,9.797842,9.805267,9.80509,9.789581,9.785865,9.796911,9.8113,9.801646,9.78558,9.786599,9.807387,9.809262,9.802482,9.779269,9.801735,9.810091,9.80916,9.790974,9.786612,9.79681,9.803318,9.796531,9.786137,9.79329,9.803026,9.807686,9.794962,9.788087,9.794676,9.811008,9.812034,9.789941,9.791429,9.805179,9.804527,9.808691,9.786707,9.795702,9.802102,9.8177,9.792353,9.788657,9.790125,9.811762,9.809819,9.793385,9.786796,9.79524,9.80935,9.803419,9.790505,9.79776,9.808882,9.808229,9.799703,9.794119,9.805444,9.805356,9.798222,9.791803,9.795512,9.802298,9.816687,9.79348,9.78846,9.794309,9.804602,9.803039,9.797747,9.791708,9.797835,9.810926,9.80397,9.793847,9.794139,9.804432</t>
-  </si>
-  <si>
-    <t>0.000613,-0.002742,-0.004129,-0.002187,0.001704,-0.001385,-0.005264,-0.001897,-0.00691,-0.001367,-0.003007,-0.002168,-0.00247,-0.00022,0.000311,0.005577,-0.002458,-0.001077,-0.005239,-0.005794,-0.013286,-0.006343,-0.004407,0.000298,-0.006608,-0.004672,-0.004678,0.000866,4.5e-05,-0.003013,-0.002452,-0.003013,-0.009395,-0.001613,0.00393,-0.002433,-0.002168,-0.00136,-0.002729,0.003104,0.000317,-0.004974,-0.005825,-0.002174,-0.003574,-0.000805,-0.002458,0.001686,-0.004123,-0.006626,-0.000793,-0.002187,0.003369,-0.002729,3.9e-05,-0.001626,0.003918,-0.000232,-0.003562,-0.000818,0.001162,-0.005788,-0.006078,-0.000787,-0.007459,-0.005794,-0.001891,-0.001891,0.001704,-0.00133,-0.003556,-0.003833,-0.003562,-0.003858,-0.004407,0.003085,-0.001613,3.3e-05,-0.00276,-0.010795,-0.001891,-0.005214,0.001439,-0.003303,0.001131,0.001433,-0.002181,-0.006639,-0.001626,0.003344,0.000576,-0.003852,-0.007169,-0.001613,0.006144,-0.002174,-0.000238,-0.005245,-0.005529,-0.006608</t>
-  </si>
-  <si>
-    <t>-0.000812,0.00393,-0.00498,-0.004702,-0.007181,0.000323,0.001421,0.000847,-0.007742,-0.000787,-0.00247,-0.0044,-0.003568,-0.002711,-0.002476,0.004756,-0.00638,0.004775,-0.001638,-0.001891,-0.001922,0.000329,3.3e-05,0.003659,0.004183,-0.000509,-0.007163,-0.001077,-0.006337,-0.003019,0.000853,-0.005523,0.000872,-0.00329,-0.000793,-0.001058,0.004485,-0.0044,-0.008291,-0.00329,-0.004117,-0.004659,-0.002168,-0.004955,-0.003593,-0.003821,0.002259,-0.000244,-0.003574,0.004195,-0.001607,-0.004918,-0.003833,0.003351,-0.006608,-0.002174,-0.001058,-0.003839,-0.004918,-0.004943,-0.005782,0.002259,-0.002729,-0.000805,-0.00609,2.1e-05,0.001445,0.002253,-0.000516,-0.000497,0.000884,-0.001077,-0.005782,-0.009142,-0.005486,-0.002476,-0.004129,0.001988,0.000563,-0.000793,-0.006916,0.004491,-0.003284,-0.004135,-0.000534,0.002247,-0.005775,-0.006361,0.001137,0.001975,-0.002458,0.005324,-0.000818,-0.003858,-0.004653,-0.004672,-0.00136,0.000884,-0.001077,0.003085</t>
+    <t>0.601303,0.583211,0.597233,0.616622,0.603171,0.605304,0.581078,0.596391,0.598429,0.600202,0.577077,0.576703,0.602518,0.590073,0.60455,0.601303,0.575786,0.615888,0.603531,0.570392,0.608001,0.598422,0.573082,0.581452,0.60938,0.583015,0.603075,0.610596,0.583945,0.601588,0.609754,0.574292,0.611988,0.595739,0.569937,0.583388,0.606886,0.573925,0.609115,0.616058,0.574115,0.60298,0.608646,0.584686,0.59082,0.600392,0.598055,0.606044,0.595745,0.566955,0.572715,0.607253,0.581717,0.575589,0.605766,0.576805,0.600841,0.610589,0.606696,0.572906,0.603442,0.60762,0.607437,0.575684,0.602518,0.595745,0.574197,0.600936,0.607063,0.574013,0.603904,0.590168,0.584876,0.600385,0.60224,0.56817,0.611887,0.601499,0.582566,0.612084,0.580141,0.607811,0.573463,0.609672,0.607348,0.57709,0.602613,0.580704,0.599631,0.57188,0.598531,0.602233,0.585249,0.621921,0.575494,0.572532,0.598714,0.57902,0.607906,0.605949</t>
+  </si>
+  <si>
+    <t>9.83645,9.819934,9.825505,9.843508,9.832557,9.821782,9.817516,9.83005,9.831538,9.831721,9.819663,9.820675,9.840723,9.847407,9.827638,9.817142,9.82058,9.836273,9.835798,9.821511,9.818352,9.827733,9.838596,9.832557,9.822713,9.818637,9.838589,9.842869,9.826436,9.821144,9.833386,9.832835,9.835254,9.833487,9.823277,9.836653,9.841096,9.828847,9.819567,9.818542,9.839235,9.840641,9.832285,9.821055,9.836178,9.843888,9.833209,9.82717,9.827638,9.834316,9.842958,9.832835,9.814826,9.830063,9.839425,9.842027,9.828936,9.819928,9.832645,9.851395,9.831721,9.826062,9.818827,9.839989,9.846578,9.833304,9.812883,9.828936,9.836932,9.836545,9.820118,9.822992,9.832183,9.842217,9.831544,9.819656,9.818732,9.840824,9.845559,9.834038,9.822631,9.82522,9.842027,9.840729,9.824751,9.826334,9.831082,9.837564,9.836836,9.816402,9.836368,9.836456,9.842679,9.82774,9.810084,9.830702,9.841375,9.839242,9.830804,9.826436</t>
+  </si>
+  <si>
+    <t>-0.000263,-0.004974,-0.002982,-0.000251,0.001692,-0.001071,-0.000799,-0.001089,-0.000781,0.000311,-0.000799,-0.003013,-0.002735,-0.001885,0.000878,-0.003827,-0.004659,-0.005245,-0.001077,-0.005208,-0.005245,0.000317,-0.006904,-0.005208,-0.000768,-0.001607,0.003369,-0.001891,-0.000251,3.9e-05,0.001963,-0.000226,-0.003833,0.000866,0.001421,-0.003278,-0.001077,-0.001046,-0.003266,0.005318,-0.002193,-0.003852,-0.003852,-0.003845,-0.001934,0.002537,-0.002452,-0.001872,-0.00387,-0.00387,0.001149,0.001692,-0.008291,0.006427,0.005848,-0.00358,-0.000497,0.001717,-0.004111,-0.000244,-0.001922,0.000853,-0.000787,-0.003852,-0.004111,0.005614,-0.001897,0.001445,-0.005233,-0.004961,-0.003019,0.001969,-0.000787,-0.002181,-0.002464,-0.003297,0.004448,-0.001064,-0.00022,0.003943,-0.004123,0.001168,-0.008285,0.003955,-0.001897,-0.000238,-0.006065,-0.006645,0.006705,0.00311,-0.004672,-0.002199,-0.001909,-0.001071,0.001131,0.002253,0.000298,-0.003025,0.000582,-0.004968</t>
+  </si>
+  <si>
+    <t>-0.000214,0.000884,-0.004111,-0.005806,-0.001891,-0.002181,-0.000238,0.000311,-0.005492,-0.002729,0.003116,0.000329,0.003104,-0.001071,-0.005775,0.00393,0.005299,-0.01217,0.002506,-0.003019,0.000304,0.002259,0.003092,0.003943,-0.00136,-0.002458,0.000317,-0.002476,4.5e-05,-0.001342,-0.000793,0.005046,-0.001064,-0.006078,-0.001909,0.002549,0.000872,0.000607,0.00615,-0.000818,-0.002735,0.003369,0.001451,-0.002458,-0.007157,-0.001909,-0.00522,0.003098,-0.003858,-0.007736,-0.000509,-0.005523,0.000329,-0.004129,-0.003845,0.000594,-0.005535,-0.008581,0.001433,0.00282,-0.002458,-0.002994,0.001704,0.003085,0.003665,6.4e-05,0.003918,-0.004154,-0.00136,-0.003038,-0.002187,0.002518,-0.001613,-0.005257,-0.001589,5.8e-05,-0.000226,-0.001077,0.007285,-0.000793,4.5e-05,-0.0044,-0.005227,0.00253,5.2e-05,-0.004419,-0.009407,0.003936,-0.001342,-0.002199,4.5e-05,-0.001064,-0.000509,0.003924,-0.004129,8e-06,0.002228,-0.000226,-0.001354,0.001704</t>
   </si>
 </sst>
 </file>
@@ -660,16 +660,16 @@
         <v>25</v>
       </c>
       <c r="C3" s="5">
-        <v>0.581</v>
+        <v>0.594</v>
       </c>
       <c r="D3" s="5">
-        <v>0.606</v>
+        <v>0.622</v>
       </c>
       <c r="E3" s="5">
-        <v>0.555</v>
+        <v>0.5669999999999999</v>
       </c>
       <c r="F3" s="5">
-        <v>0.016</v>
+        <v>0.014</v>
       </c>
       <c r="G3" s="5">
         <v>100</v>
@@ -683,16 +683,16 @@
         <v>26</v>
       </c>
       <c r="C4" s="5">
-        <v>9.798999999999999</v>
+        <v>9.831</v>
       </c>
       <c r="D4" s="5">
-        <v>9.818</v>
+        <v>9.851000000000001</v>
       </c>
       <c r="E4" s="5">
-        <v>9.779</v>
+        <v>9.81</v>
       </c>
       <c r="F4" s="5">
-        <v>0.008</v>
+        <v>0.008999999999999999</v>
       </c>
       <c r="G4" s="5">
         <v>100</v>
@@ -743,13 +743,13 @@
         <v>25</v>
       </c>
       <c r="C3" s="5">
-        <v>-0.002</v>
+        <v>-0.001</v>
       </c>
       <c r="D3" s="5">
-        <v>0.006</v>
+        <v>0.007</v>
       </c>
       <c r="E3" s="5">
-        <v>-0.013</v>
+        <v>-0.008</v>
       </c>
       <c r="F3" s="5">
         <v>0.003</v>
@@ -766,13 +766,13 @@
         <v>26</v>
       </c>
       <c r="C4" s="5">
-        <v>-0.002</v>
+        <v>-0.001</v>
       </c>
       <c r="D4" s="5">
-        <v>0.005</v>
+        <v>0.007</v>
       </c>
       <c r="E4" s="5">
-        <v>-0.008999999999999999</v>
+        <v>-0.012</v>
       </c>
       <c r="F4" s="5">
         <v>0.003</v>

</xml_diff>

<commit_message>
Update decorator run time
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -63,13 +63,13 @@
     <t>Alex Wang</t>
   </si>
   <si>
-    <t>09:11:53 03-22-2017 Wednesday Pacific Daylight Time</t>
-  </si>
-  <si>
-    <t>09:12:28 03-22-2017 Wednesday Pacific Daylight Time</t>
-  </si>
-  <si>
-    <t>0:0:35 0 days</t>
+    <t>09:35:01 03-22-2017 Wednesday Pacific Daylight Time</t>
+  </si>
+  <si>
+    <t>09:35:36 03-22-2017 Wednesday Pacific Daylight Time</t>
+  </si>
+  <si>
+    <t>0:0:34 0 days</t>
   </si>
   <si>
     <t>Information</t>
@@ -99,16 +99,16 @@
     <t>BT Idle</t>
   </si>
   <si>
-    <t>0.601303,0.583211,0.597233,0.616622,0.603171,0.605304,0.581078,0.596391,0.598429,0.600202,0.577077,0.576703,0.602518,0.590073,0.60455,0.601303,0.575786,0.615888,0.603531,0.570392,0.608001,0.598422,0.573082,0.581452,0.60938,0.583015,0.603075,0.610596,0.583945,0.601588,0.609754,0.574292,0.611988,0.595739,0.569937,0.583388,0.606886,0.573925,0.609115,0.616058,0.574115,0.60298,0.608646,0.584686,0.59082,0.600392,0.598055,0.606044,0.595745,0.566955,0.572715,0.607253,0.581717,0.575589,0.605766,0.576805,0.600841,0.610589,0.606696,0.572906,0.603442,0.60762,0.607437,0.575684,0.602518,0.595745,0.574197,0.600936,0.607063,0.574013,0.603904,0.590168,0.584876,0.600385,0.60224,0.56817,0.611887,0.601499,0.582566,0.612084,0.580141,0.607811,0.573463,0.609672,0.607348,0.57709,0.602613,0.580704,0.599631,0.57188,0.598531,0.602233,0.585249,0.621921,0.575494,0.572532,0.598714,0.57902,0.607906,0.605949</t>
-  </si>
-  <si>
-    <t>9.83645,9.819934,9.825505,9.843508,9.832557,9.821782,9.817516,9.83005,9.831538,9.831721,9.819663,9.820675,9.840723,9.847407,9.827638,9.817142,9.82058,9.836273,9.835798,9.821511,9.818352,9.827733,9.838596,9.832557,9.822713,9.818637,9.838589,9.842869,9.826436,9.821144,9.833386,9.832835,9.835254,9.833487,9.823277,9.836653,9.841096,9.828847,9.819567,9.818542,9.839235,9.840641,9.832285,9.821055,9.836178,9.843888,9.833209,9.82717,9.827638,9.834316,9.842958,9.832835,9.814826,9.830063,9.839425,9.842027,9.828936,9.819928,9.832645,9.851395,9.831721,9.826062,9.818827,9.839989,9.846578,9.833304,9.812883,9.828936,9.836932,9.836545,9.820118,9.822992,9.832183,9.842217,9.831544,9.819656,9.818732,9.840824,9.845559,9.834038,9.822631,9.82522,9.842027,9.840729,9.824751,9.826334,9.831082,9.837564,9.836836,9.816402,9.836368,9.836456,9.842679,9.82774,9.810084,9.830702,9.841375,9.839242,9.830804,9.826436</t>
-  </si>
-  <si>
-    <t>-0.000263,-0.004974,-0.002982,-0.000251,0.001692,-0.001071,-0.000799,-0.001089,-0.000781,0.000311,-0.000799,-0.003013,-0.002735,-0.001885,0.000878,-0.003827,-0.004659,-0.005245,-0.001077,-0.005208,-0.005245,0.000317,-0.006904,-0.005208,-0.000768,-0.001607,0.003369,-0.001891,-0.000251,3.9e-05,0.001963,-0.000226,-0.003833,0.000866,0.001421,-0.003278,-0.001077,-0.001046,-0.003266,0.005318,-0.002193,-0.003852,-0.003852,-0.003845,-0.001934,0.002537,-0.002452,-0.001872,-0.00387,-0.00387,0.001149,0.001692,-0.008291,0.006427,0.005848,-0.00358,-0.000497,0.001717,-0.004111,-0.000244,-0.001922,0.000853,-0.000787,-0.003852,-0.004111,0.005614,-0.001897,0.001445,-0.005233,-0.004961,-0.003019,0.001969,-0.000787,-0.002181,-0.002464,-0.003297,0.004448,-0.001064,-0.00022,0.003943,-0.004123,0.001168,-0.008285,0.003955,-0.001897,-0.000238,-0.006065,-0.006645,0.006705,0.00311,-0.004672,-0.002199,-0.001909,-0.001071,0.001131,0.002253,0.000298,-0.003025,0.000582,-0.004968</t>
-  </si>
-  <si>
-    <t>-0.000214,0.000884,-0.004111,-0.005806,-0.001891,-0.002181,-0.000238,0.000311,-0.005492,-0.002729,0.003116,0.000329,0.003104,-0.001071,-0.005775,0.00393,0.005299,-0.01217,0.002506,-0.003019,0.000304,0.002259,0.003092,0.003943,-0.00136,-0.002458,0.000317,-0.002476,4.5e-05,-0.001342,-0.000793,0.005046,-0.001064,-0.006078,-0.001909,0.002549,0.000872,0.000607,0.00615,-0.000818,-0.002735,0.003369,0.001451,-0.002458,-0.007157,-0.001909,-0.00522,0.003098,-0.003858,-0.007736,-0.000509,-0.005523,0.000329,-0.004129,-0.003845,0.000594,-0.005535,-0.008581,0.001433,0.00282,-0.002458,-0.002994,0.001704,0.003085,0.003665,6.4e-05,0.003918,-0.004154,-0.00136,-0.003038,-0.002187,0.002518,-0.001613,-0.005257,-0.001589,5.8e-05,-0.000226,-0.001077,0.007285,-0.000793,4.5e-05,-0.0044,-0.005227,0.00253,5.2e-05,-0.004419,-0.009407,0.003936,-0.001342,-0.002199,4.5e-05,-0.001064,-0.000509,0.003924,-0.004129,8e-06,0.002228,-0.000226,-0.001354,0.001704</t>
+    <t>0.568721,0.572994,0.571051,0.573653,0.568816,0.570114,0.60046,0.565657,0.563993,0.579489,0.574672,0.563334,0.566683,0.571595,0.573639,0.563068,0.574006,0.571513,0.568075,0.566961,0.591194,0.573728,0.56919,0.589434,0.570304,0.569468,0.563809,0.57207,0.569828,0.579027,0.585351,0.569095,0.570671,0.57012,0.580609,0.566031,0.567892,0.573551,0.600005,0.568347,0.574944,0.567797,0.586934,0.568626,0.567879,0.565664,0.568911,0.590446,0.573273,0.573735,0.56743,0.565195,0.569557,0.572172,0.572253,0.558694,0.57745,0.592023,0.57671,0.564278,0.603823,0.566132,0.571506,0.573735,0.5715,0.565657,0.604468,0.561391,0.570766,0.569095,0.599815,0.572532,0.568816,0.597036,0.566316,0.566771,0.559346,0.594251,0.569095,0.573082,0.596764,0.574393,0.571975,0.564828,0.599828,0.575786,0.569747,0.572253,0.571323,0.570949,0.588598,0.572532,0.564461,0.603544,0.577552,0.568911,0.575317,0.57383,0.561853,0.562593</t>
+  </si>
+  <si>
+    <t>9.850566,9.843888,9.834602,9.830886,9.832006,9.846945,9.824853,9.810369,9.819099,9.838127,9.823739,9.812876,9.803684,9.814744,9.818453,9.813528,9.798019,9.800247,9.806381,9.810559,9.796728,9.780845,9.793657,9.804242,9.802285,9.777971,9.78168,9.787903,9.796538,9.782339,9.773426,9.783827,9.7906,9.787985,9.778528,9.762468,9.777224,9.784934,9.786606,9.775553,9.770362,9.782516,9.791714,9.773236,9.766089,9.768963,9.780947,9.788644,9.773046,9.766273,9.778712,9.784276,9.777129,9.775654,9.770913,9.787897,9.788922,9.779452,9.76219,9.77435,9.777883,9.783447,9.768318,9.766551,9.781035,9.788182,9.786701,9.773977,9.768318,9.777135,9.780947,9.776293,9.765431,9.764887,9.781775,9.788087,9.760899,9.773236,9.77649,9.791803,9.781694,9.765159,9.767659,9.784384,9.782238,9.776864,9.761354,9.77204,9.783535,9.787346,9.765254,9.76024,9.77825,9.785396,9.774812,9.760329,9.776673,9.79543,9.776952,9.776116</t>
+  </si>
+  <si>
+    <t>0.008074,-0.001619,-0.001354,0.00533,0.003092,0.003936,-0.003574,0.000853,0.00311,0.001439,-0.000509,-0.002495,-0.000787,-0.000257,0.002561,-0.004702,-0.000226,0.002802,0.002265,0.000841,0.003079,-0.002476,0.002253,0.001433,-0.003556,-0.004129,-0.010789,-0.003568,-0.003013,2.7e-05,0.002512,-0.004955,-0.000528,-0.001367,0.002228,-0.001046,-0.001891,0.001162,-0.003839,-0.002464,0.00253,-0.000226,-0.001903,0.001963,0.004208,0.001414,-0.003556,0.001975,0.000304,0.002228,-0.002187,-0.000818,0.002247,6.4e-05,-0.001595,-0.005251,-0.002994,-0.000232,0.001143,0.002278,-0.002464,0.001969,-0.000497,-0.001058,-0.003297,-0.002199,0.000594,0.000304,-0.004696,-0.002181,0.002826,-0.003882,-0.003309,-0.007995,-0.004407,-0.001613,-0.001607,-0.00247,-0.003007,-0.004653,0.003634,-0.003303,0.001698,-0.003007,0.004744,0.001439,0.005034,-0.00247,-0.000528,0.006125,0.001433,0.004214,0.00504,0.001149,-0.003852,-0.002735,0.005873,-0.004943,0.00475,0.001402</t>
+  </si>
+  <si>
+    <t>-0.002705,-0.00662,-0.000793,0.003061,-0.002181,-0.001348,0.000323,-0.005541,0.004177,-0.001613,-0.003562,0.00171,0.00475,-0.001632,0.001149,-0.000269,-0.003007,-0.002754,-0.004974,-0.002748,0.00282,0.002789,-0.005498,0.004473,-0.002181,-0.002735,-0.001607,-0.003876,-0.001058,-0.003284,-0.001095,-0.003864,0.001717,-0.000257,0.000329,-0.004937,-0.003284,-0.002476,-0.002187,0.00253,-0.001342,-0.007718,-0.001064,-0.004974,0.002814,-0.000516,-0.003309,-0.003852,-0.006361,-0.000263,0.000329,0.002012,0.000853,0.002808,0.002537,-0.001891,-0.001619,-0.00136,-0.003025,0.000317,0.003369,0.00171,-0.00215,-0.001582,-0.001613,0.007556,-0.001058,0.00504,0.001445,0.001704,-0.001638,0.001717,-0.003013,-0.004684,-0.005492,0.002537,0.00171,0.001994,-0.000534,0.001143,0.003098,0.003098,-0.003833,-0.000232,0.00311,-0.003001,-0.006904,0.000582,-0.000799,-0.005794,-0.001354,-0.007422,-0.005769,-0.004413,-0.005547,3.3e-05,-0.001891,2.7e-05,-0.002211,-0.004955</t>
   </si>
 </sst>
 </file>
@@ -660,16 +660,16 @@
         <v>25</v>
       </c>
       <c r="C3" s="5">
-        <v>0.594</v>
+        <v>0.574</v>
       </c>
       <c r="D3" s="5">
-        <v>0.622</v>
+        <v>0.604</v>
       </c>
       <c r="E3" s="5">
-        <v>0.5669999999999999</v>
+        <v>0.5590000000000001</v>
       </c>
       <c r="F3" s="5">
-        <v>0.014</v>
+        <v>0.011</v>
       </c>
       <c r="G3" s="5">
         <v>100</v>
@@ -683,16 +683,16 @@
         <v>26</v>
       </c>
       <c r="C4" s="5">
-        <v>9.831</v>
+        <v>9.787000000000001</v>
       </c>
       <c r="D4" s="5">
         <v>9.851000000000001</v>
       </c>
       <c r="E4" s="5">
-        <v>9.81</v>
+        <v>9.76</v>
       </c>
       <c r="F4" s="5">
-        <v>0.008999999999999999</v>
+        <v>0.021</v>
       </c>
       <c r="G4" s="5">
         <v>100</v>
@@ -743,13 +743,13 @@
         <v>25</v>
       </c>
       <c r="C3" s="5">
-        <v>-0.001</v>
+        <v>-0</v>
       </c>
       <c r="D3" s="5">
-        <v>0.007</v>
+        <v>0.008</v>
       </c>
       <c r="E3" s="5">
-        <v>-0.008</v>
+        <v>-0.011</v>
       </c>
       <c r="F3" s="5">
         <v>0.003</v>
@@ -769,10 +769,10 @@
         <v>-0.001</v>
       </c>
       <c r="D4" s="5">
-        <v>0.007</v>
+        <v>0.008</v>
       </c>
       <c r="E4" s="5">
-        <v>-0.012</v>
+        <v>-0.008</v>
       </c>
       <c r="F4" s="5">
         <v>0.003</v>

</xml_diff>

<commit_message>
Update test case init wrapper
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -63,13 +63,13 @@
     <t>Alex Wang</t>
   </si>
   <si>
-    <t>09:35:01 03-22-2017 Wednesday Pacific Daylight Time</t>
-  </si>
-  <si>
-    <t>09:35:36 03-22-2017 Wednesday Pacific Daylight Time</t>
-  </si>
-  <si>
-    <t>0:0:34 0 days</t>
+    <t>22:47:09 03-22-2017 Wednesday Pacific Daylight Time</t>
+  </si>
+  <si>
+    <t>22:47:44 03-22-2017 Wednesday Pacific Daylight Time</t>
+  </si>
+  <si>
+    <t>0:0:35 0 days</t>
   </si>
   <si>
     <t>Information</t>
@@ -99,16 +99,16 @@
     <t>BT Idle</t>
   </si>
   <si>
-    <t>0.568721,0.572994,0.571051,0.573653,0.568816,0.570114,0.60046,0.565657,0.563993,0.579489,0.574672,0.563334,0.566683,0.571595,0.573639,0.563068,0.574006,0.571513,0.568075,0.566961,0.591194,0.573728,0.56919,0.589434,0.570304,0.569468,0.563809,0.57207,0.569828,0.579027,0.585351,0.569095,0.570671,0.57012,0.580609,0.566031,0.567892,0.573551,0.600005,0.568347,0.574944,0.567797,0.586934,0.568626,0.567879,0.565664,0.568911,0.590446,0.573273,0.573735,0.56743,0.565195,0.569557,0.572172,0.572253,0.558694,0.57745,0.592023,0.57671,0.564278,0.603823,0.566132,0.571506,0.573735,0.5715,0.565657,0.604468,0.561391,0.570766,0.569095,0.599815,0.572532,0.568816,0.597036,0.566316,0.566771,0.559346,0.594251,0.569095,0.573082,0.596764,0.574393,0.571975,0.564828,0.599828,0.575786,0.569747,0.572253,0.571323,0.570949,0.588598,0.572532,0.564461,0.603544,0.577552,0.568911,0.575317,0.57383,0.561853,0.562593</t>
-  </si>
-  <si>
-    <t>9.850566,9.843888,9.834602,9.830886,9.832006,9.846945,9.824853,9.810369,9.819099,9.838127,9.823739,9.812876,9.803684,9.814744,9.818453,9.813528,9.798019,9.800247,9.806381,9.810559,9.796728,9.780845,9.793657,9.804242,9.802285,9.777971,9.78168,9.787903,9.796538,9.782339,9.773426,9.783827,9.7906,9.787985,9.778528,9.762468,9.777224,9.784934,9.786606,9.775553,9.770362,9.782516,9.791714,9.773236,9.766089,9.768963,9.780947,9.788644,9.773046,9.766273,9.778712,9.784276,9.777129,9.775654,9.770913,9.787897,9.788922,9.779452,9.76219,9.77435,9.777883,9.783447,9.768318,9.766551,9.781035,9.788182,9.786701,9.773977,9.768318,9.777135,9.780947,9.776293,9.765431,9.764887,9.781775,9.788087,9.760899,9.773236,9.77649,9.791803,9.781694,9.765159,9.767659,9.784384,9.782238,9.776864,9.761354,9.77204,9.783535,9.787346,9.765254,9.76024,9.77825,9.785396,9.774812,9.760329,9.776673,9.79543,9.776952,9.776116</t>
-  </si>
-  <si>
-    <t>0.008074,-0.001619,-0.001354,0.00533,0.003092,0.003936,-0.003574,0.000853,0.00311,0.001439,-0.000509,-0.002495,-0.000787,-0.000257,0.002561,-0.004702,-0.000226,0.002802,0.002265,0.000841,0.003079,-0.002476,0.002253,0.001433,-0.003556,-0.004129,-0.010789,-0.003568,-0.003013,2.7e-05,0.002512,-0.004955,-0.000528,-0.001367,0.002228,-0.001046,-0.001891,0.001162,-0.003839,-0.002464,0.00253,-0.000226,-0.001903,0.001963,0.004208,0.001414,-0.003556,0.001975,0.000304,0.002228,-0.002187,-0.000818,0.002247,6.4e-05,-0.001595,-0.005251,-0.002994,-0.000232,0.001143,0.002278,-0.002464,0.001969,-0.000497,-0.001058,-0.003297,-0.002199,0.000594,0.000304,-0.004696,-0.002181,0.002826,-0.003882,-0.003309,-0.007995,-0.004407,-0.001613,-0.001607,-0.00247,-0.003007,-0.004653,0.003634,-0.003303,0.001698,-0.003007,0.004744,0.001439,0.005034,-0.00247,-0.000528,0.006125,0.001433,0.004214,0.00504,0.001149,-0.003852,-0.002735,0.005873,-0.004943,0.00475,0.001402</t>
-  </si>
-  <si>
-    <t>-0.002705,-0.00662,-0.000793,0.003061,-0.002181,-0.001348,0.000323,-0.005541,0.004177,-0.001613,-0.003562,0.00171,0.00475,-0.001632,0.001149,-0.000269,-0.003007,-0.002754,-0.004974,-0.002748,0.00282,0.002789,-0.005498,0.004473,-0.002181,-0.002735,-0.001607,-0.003876,-0.001058,-0.003284,-0.001095,-0.003864,0.001717,-0.000257,0.000329,-0.004937,-0.003284,-0.002476,-0.002187,0.00253,-0.001342,-0.007718,-0.001064,-0.004974,0.002814,-0.000516,-0.003309,-0.003852,-0.006361,-0.000263,0.000329,0.002012,0.000853,0.002808,0.002537,-0.001891,-0.001619,-0.00136,-0.003025,0.000317,0.003369,0.00171,-0.00215,-0.001582,-0.001613,0.007556,-0.001058,0.00504,0.001445,0.001704,-0.001638,0.001717,-0.003013,-0.004684,-0.005492,0.002537,0.00171,0.001994,-0.000534,0.001143,0.003098,0.003098,-0.003833,-0.000232,0.00311,-0.003001,-0.006904,0.000582,-0.000799,-0.005794,-0.001354,-0.007422,-0.005769,-0.004413,-0.005547,3.3e-05,-0.001891,2.7e-05,-0.002211,-0.004955</t>
+    <t>0.565942,0.575229,0.600093,0.602512,0.56993,0.593524,0.602056,0.601866,0.5769,0.607253,0.596302,0.592301,0.561017,0.597872,0.601303,0.600562,0.596751,0.576703,0.607253,0.608184,0.565942,0.570772,0.600195,0.601486,0.601037,0.571513,0.599726,0.603442,0.58116,0.597416,0.592118,0.59974,0.592953,0.572437,0.595175,0.596486,0.58099,0.571241,0.597505,0.604101,0.570025,0.573449,0.608279,0.601316,0.565841,0.598524,0.598897,0.570861,0.601214,0.598626,0.599359,0.570677,0.596669,0.603171,0.603259,0.564176,0.599828,0.596479,0.561771,0.568911,0.598157,0.603809,0.574013,0.590161,0.600487,0.611703,0.56724,0.601493,0.600188,0.600854,0.578381,0.597878,0.576431,0.588959,0.597967,0.579033,0.600385,0.597505,0.570025,0.605677,0.600664,0.564271,0.564455,0.602328,0.594631,0.604373,0.569468,0.605386,0.602518,0.570494,0.603531,0.572077,0.59546,0.603164,0.596391,0.589054,0.564917,0.602695,0.590446,0.572627</t>
+  </si>
+  <si>
+    <t>9.825227,9.812129,9.822903,9.828664,9.835064,9.8177,9.814826,9.832095,9.839242,9.826429,9.80685,9.824758,9.837856,9.827088,9.81789,9.812604,9.830987,9.835064,9.831259,9.820675,9.815478,9.837665,9.834126,9.825036,9.813243,9.830057,9.827822,9.830702,9.817516,9.817238,9.824663,9.839058,9.823922,9.805166,9.825689,9.832557,9.840546,9.816592,9.814085,9.815851,9.837292,9.828556,9.812414,9.813066,9.825967,9.838216,9.824296,9.807034,9.818725,9.83933,9.827088,9.821979,9.8088,9.819384,9.832095,9.824486,9.810743,9.81399,9.832006,9.828195,9.824574,9.816123,9.819384,9.836456,9.825036,9.824663,9.81668,9.824296,9.838589,9.828936,9.806925,9.819377,9.829962,9.829506,9.825505,9.81789,9.818542,9.833481,9.828005,9.81575,9.821137,9.824574,9.829316,9.821599,9.811857,9.821137,9.823631,9.833107,9.828474,9.811116,9.817896,9.831905,9.831639,9.813712,9.819187,9.826069,9.838766,9.82522,9.816871,9.814832</t>
+  </si>
+  <si>
+    <t>-0.000762,-0.000263,-0.00802,0.001445,-0.006879,-0.001903,-0.000824,-0.004123,-0.002181,-0.003278,0.004201,0.000878,0.00253,-0.001632,-0.000263,0.000896,-0.003568,-0.000799,-0.003284,-0.001089,0.002567,-0.002489,-0.000509,-0.009117,-0.004955,-0.004413,0.003363,-0.004702,0.000866,-0.001342,0.001137,-0.001077,-0.002476,-0.002452,-0.003025,0.001982,0.002524,0.002278,-0.000793,-0.002458,-0.001656,-0.002452,0.003067,0.000594,-0.001928,-0.011078,-0.000799,0.003659,-0.005523,0.002512,-0.002168,-0.004388,-0.001354,0.000304,-0.004419,-0.002464,-0.000793,-0.004382,-0.004123,-0.001595,0.001969,-0.004123,-0.002187,-0.000812,0.000582,0.002555,-0.00773,-0.000522,-0.000516,-0.00276,-0.004123,0.00282,-0.000232,-0.005529,-0.005214,-0.00247,5.2e-05,0.001692,-0.001626,0.00446,0.001402,0.005564,0.003665,0.001427,0.001686,-0.002174,-0.000503,0.001988,-0.002754,-0.000516,-0.00215,3.9e-05,-0.002742,-0.010234,0.001698,-0.007194,-0.003019,-0.000781,0.001427,0.001427</t>
+  </si>
+  <si>
+    <t>-0.000522,-0.003284,0.003918,-0.00247,-0.003845,0.001704,-0.003278,-0.001626,0.001155,-0.002476,0.005601,-0.005233,-0.005239,-0.001089,0.000304,-0.004111,0.008074,-0.002723,-0.002181,0.000576,-0.004098,2.1e-05,-0.002181,-0.005214,5.2e-05,3.9e-05,-0.008852,-0.004986,-0.003833,0.004485,-0.002729,-0.001626,0.002561,-0.000805,-0.00022,-0.003297,-0.005794,-0.003593,-0.001626,0.004201,-0.004653,0.000304,-0.00387,0.002808,-0.003556,0.0006,-0.002211,0.004738,-0.004659,-0.006355,-0.001064,-0.002464,-0.0044,-0.001077,-0.00247,0.001692,0.002278,-0.002458,-0.001613,-0.003568,0.003079,-0.000509,-0.005529,0.001704,0.002808,0.000866,-0.000787,-0.001077,-0.001885,-0.001342,-0.00691,-0.00329,0.000311,-0.000232,-0.004955,0.004763,-0.005541,-0.008563,0.001131,-0.003882,-0.001613,-0.002748,0.005891,-0.004394,0.002537,-0.003019,0.00393,-0.001897,-0.004394,-0.000793,0.001704,-0.002446,-0.004123,-0.002193,0.001143,0.001433,0.00171,-0.001632,0.001963,0.00475</t>
   </si>
 </sst>
 </file>
@@ -660,16 +660,16 @@
         <v>25</v>
       </c>
       <c r="C3" s="5">
-        <v>0.574</v>
+        <v>0.59</v>
       </c>
       <c r="D3" s="5">
-        <v>0.604</v>
+        <v>0.612</v>
       </c>
       <c r="E3" s="5">
-        <v>0.5590000000000001</v>
+        <v>0.5610000000000001</v>
       </c>
       <c r="F3" s="5">
-        <v>0.011</v>
+        <v>0.014</v>
       </c>
       <c r="G3" s="5">
         <v>100</v>
@@ -683,16 +683,16 @@
         <v>26</v>
       </c>
       <c r="C4" s="5">
-        <v>9.787000000000001</v>
+        <v>9.824</v>
       </c>
       <c r="D4" s="5">
-        <v>9.851000000000001</v>
+        <v>9.840999999999999</v>
       </c>
       <c r="E4" s="5">
-        <v>9.76</v>
+        <v>9.805</v>
       </c>
       <c r="F4" s="5">
-        <v>0.021</v>
+        <v>0.008999999999999999</v>
       </c>
       <c r="G4" s="5">
         <v>100</v>
@@ -743,10 +743,10 @@
         <v>25</v>
       </c>
       <c r="C3" s="5">
-        <v>-0</v>
+        <v>-0.001</v>
       </c>
       <c r="D3" s="5">
-        <v>0.008</v>
+        <v>0.006</v>
       </c>
       <c r="E3" s="5">
         <v>-0.011</v>
@@ -772,7 +772,7 @@
         <v>0.008</v>
       </c>
       <c r="E4" s="5">
-        <v>-0.008</v>
+        <v>-0.008999999999999999</v>
       </c>
       <c r="F4" s="5">
         <v>0.003</v>

</xml_diff>

<commit_message>
Update main flow comments and some other code minor changes
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="28">
   <si>
     <t>WLAN Version</t>
   </si>
@@ -63,13 +63,13 @@
     <t>Alex Wang</t>
   </si>
   <si>
-    <t>22:47:09 03-22-2017 Wednesday Pacific Daylight Time</t>
-  </si>
-  <si>
-    <t>22:47:44 03-22-2017 Wednesday Pacific Daylight Time</t>
-  </si>
-  <si>
-    <t>0:0:35 0 days</t>
+    <t>23:03:07 03-26-2017 Sunday Pacific Daylight Time</t>
+  </si>
+  <si>
+    <t>23:03:24 03-26-2017 Sunday Pacific Daylight Time</t>
+  </si>
+  <si>
+    <t>0:0:16 0 days</t>
   </si>
   <si>
     <t>Information</t>
@@ -96,19 +96,10 @@
     <t>Deep Sleep</t>
   </si>
   <si>
-    <t>BT Idle</t>
-  </si>
-  <si>
-    <t>0.565942,0.575229,0.600093,0.602512,0.56993,0.593524,0.602056,0.601866,0.5769,0.607253,0.596302,0.592301,0.561017,0.597872,0.601303,0.600562,0.596751,0.576703,0.607253,0.608184,0.565942,0.570772,0.600195,0.601486,0.601037,0.571513,0.599726,0.603442,0.58116,0.597416,0.592118,0.59974,0.592953,0.572437,0.595175,0.596486,0.58099,0.571241,0.597505,0.604101,0.570025,0.573449,0.608279,0.601316,0.565841,0.598524,0.598897,0.570861,0.601214,0.598626,0.599359,0.570677,0.596669,0.603171,0.603259,0.564176,0.599828,0.596479,0.561771,0.568911,0.598157,0.603809,0.574013,0.590161,0.600487,0.611703,0.56724,0.601493,0.600188,0.600854,0.578381,0.597878,0.576431,0.588959,0.597967,0.579033,0.600385,0.597505,0.570025,0.605677,0.600664,0.564271,0.564455,0.602328,0.594631,0.604373,0.569468,0.605386,0.602518,0.570494,0.603531,0.572077,0.59546,0.603164,0.596391,0.589054,0.564917,0.602695,0.590446,0.572627</t>
-  </si>
-  <si>
-    <t>9.825227,9.812129,9.822903,9.828664,9.835064,9.8177,9.814826,9.832095,9.839242,9.826429,9.80685,9.824758,9.837856,9.827088,9.81789,9.812604,9.830987,9.835064,9.831259,9.820675,9.815478,9.837665,9.834126,9.825036,9.813243,9.830057,9.827822,9.830702,9.817516,9.817238,9.824663,9.839058,9.823922,9.805166,9.825689,9.832557,9.840546,9.816592,9.814085,9.815851,9.837292,9.828556,9.812414,9.813066,9.825967,9.838216,9.824296,9.807034,9.818725,9.83933,9.827088,9.821979,9.8088,9.819384,9.832095,9.824486,9.810743,9.81399,9.832006,9.828195,9.824574,9.816123,9.819384,9.836456,9.825036,9.824663,9.81668,9.824296,9.838589,9.828936,9.806925,9.819377,9.829962,9.829506,9.825505,9.81789,9.818542,9.833481,9.828005,9.81575,9.821137,9.824574,9.829316,9.821599,9.811857,9.821137,9.823631,9.833107,9.828474,9.811116,9.817896,9.831905,9.831639,9.813712,9.819187,9.826069,9.838766,9.82522,9.816871,9.814832</t>
-  </si>
-  <si>
-    <t>-0.000762,-0.000263,-0.00802,0.001445,-0.006879,-0.001903,-0.000824,-0.004123,-0.002181,-0.003278,0.004201,0.000878,0.00253,-0.001632,-0.000263,0.000896,-0.003568,-0.000799,-0.003284,-0.001089,0.002567,-0.002489,-0.000509,-0.009117,-0.004955,-0.004413,0.003363,-0.004702,0.000866,-0.001342,0.001137,-0.001077,-0.002476,-0.002452,-0.003025,0.001982,0.002524,0.002278,-0.000793,-0.002458,-0.001656,-0.002452,0.003067,0.000594,-0.001928,-0.011078,-0.000799,0.003659,-0.005523,0.002512,-0.002168,-0.004388,-0.001354,0.000304,-0.004419,-0.002464,-0.000793,-0.004382,-0.004123,-0.001595,0.001969,-0.004123,-0.002187,-0.000812,0.000582,0.002555,-0.00773,-0.000522,-0.000516,-0.00276,-0.004123,0.00282,-0.000232,-0.005529,-0.005214,-0.00247,5.2e-05,0.001692,-0.001626,0.00446,0.001402,0.005564,0.003665,0.001427,0.001686,-0.002174,-0.000503,0.001988,-0.002754,-0.000516,-0.00215,3.9e-05,-0.002742,-0.010234,0.001698,-0.007194,-0.003019,-0.000781,0.001427,0.001427</t>
-  </si>
-  <si>
-    <t>-0.000522,-0.003284,0.003918,-0.00247,-0.003845,0.001704,-0.003278,-0.001626,0.001155,-0.002476,0.005601,-0.005233,-0.005239,-0.001089,0.000304,-0.004111,0.008074,-0.002723,-0.002181,0.000576,-0.004098,2.1e-05,-0.002181,-0.005214,5.2e-05,3.9e-05,-0.008852,-0.004986,-0.003833,0.004485,-0.002729,-0.001626,0.002561,-0.000805,-0.00022,-0.003297,-0.005794,-0.003593,-0.001626,0.004201,-0.004653,0.000304,-0.00387,0.002808,-0.003556,0.0006,-0.002211,0.004738,-0.004659,-0.006355,-0.001064,-0.002464,-0.0044,-0.001077,-0.00247,0.001692,0.002278,-0.002458,-0.001613,-0.003568,0.003079,-0.000509,-0.005529,0.001704,0.002808,0.000866,-0.000787,-0.001077,-0.001885,-0.001342,-0.00691,-0.00329,0.000311,-0.000232,-0.004955,0.004763,-0.005541,-0.008563,0.001131,-0.003882,-0.001613,-0.002748,0.005891,-0.004394,0.002537,-0.003019,0.00393,-0.001897,-0.004394,-0.000793,0.001704,-0.002446,-0.004123,-0.002193,0.001143,0.001433,0.00171,-0.001632,0.001963,0.00475</t>
+    <t>0.558333,0.56298,0.565107,0.558422,0.555181,0.563442,0.578375,0.579489,0.556846,0.570025,0.573463,0.554339,0.581058,0.56027,0.567423,0.550528,0.56743,0.556751,0.561112,0.564733,0.600929,0.555263,0.564264,0.558055,0.567423,0.590453,0.562688,0.56334,0.56455,0.570019,0.566126,0.562315,0.562043,0.595644,0.567518,0.558048,0.561941,0.567695,0.590079,0.563993,0.57207,0.567512,0.562505,0.593877,0.561676,0.554434,0.556744,0.56222,0.568721,0.564828,0.572715,0.565113,0.58832,0.562872,0.552111,0.543381,0.568347,0.561112,0.559441,0.589054,0.565202,0.552471,0.5651,0.562973,0.574659,0.563245,0.568272,0.557953,0.568259,0.556295,0.573633,0.566024,0.557681,0.556187,0.568449,0.564455,0.559815,0.565936,0.565759,0.565657,0.558415,0.56046,0.560745,0.564373,0.562416,0.554978,0.557498,0.561751,0.567613,0.56919,0.569747,0.566398,0.586364,0.564821,0.556839,0.568266,0.556472,0.561669,0.582648,0.561764</t>
+  </si>
+  <si>
+    <t>-0.001903,0.001125,0.000317,-0.001878,-0.002452,0.002259,-0.002994,-0.002446,-0.001348,-0.004425,-0.005233,0.004467,-0.006602,-0.003562,-0.006078,-0.00884,-0.001891,0.001717,0.00168,-0.004129,-0.002742,-0.002187,0.000866,-0.002994,-0.006361,0.000878,-0.00662,-0.002735,-0.000485,-0.008822,-0.003864,0.000329,-0.000787,0.001143,-0.003562,-0.001348,-0.004111,0.004195,-0.001903,-0.002476,-0.000528,-0.008285,0.002006,-0.005208,-0.00329,-0.002735,-0.0044,-0.000805,-0.000509,2e-06,-0.002187,-0.005239,-0.00136,-0.001323,0.001704,-0.002994,-0.00469,-0.003038,-0.00022,-0.00133,-0.005239,0.001168,0.000329,0.000588,-0.006602,-0.003297,-0.006596,0.001698,0.003369,3.9e-05,0.003647,-0.007181,0.00639,-0.002988,0.001427,0.003659,0.001686,-0.004407,-0.005227,-0.00329,-0.003833,0.003079,-0.003007,-0.003586,3.9e-05,-0.006053,-0.001891,0.000619,0.000594,-0.002735,-0.000799,-0.003852,-0.000775,-0.002187,-0.009383,-0.003013,-0.002181,-0.006922,0.00057,-0.001909</t>
   </si>
 </sst>
 </file>
@@ -625,7 +616,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:H4"/>
+  <dimension ref="B2:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -660,45 +651,22 @@
         <v>25</v>
       </c>
       <c r="C3" s="5">
-        <v>0.59</v>
+        <v>0.5659999999999999</v>
       </c>
       <c r="D3" s="5">
-        <v>0.612</v>
+        <v>0.601</v>
       </c>
       <c r="E3" s="5">
-        <v>0.5610000000000001</v>
+        <v>0.543</v>
       </c>
       <c r="F3" s="5">
-        <v>0.014</v>
+        <v>0.01</v>
       </c>
       <c r="G3" s="5">
         <v>100</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8">
-      <c r="B4" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="C4" s="5">
-        <v>9.824</v>
-      </c>
-      <c r="D4" s="5">
-        <v>9.840999999999999</v>
-      </c>
-      <c r="E4" s="5">
-        <v>9.805</v>
-      </c>
-      <c r="F4" s="5">
-        <v>0.008999999999999999</v>
-      </c>
-      <c r="G4" s="5">
-        <v>100</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -708,7 +676,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:H4"/>
+  <dimension ref="B2:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -743,13 +711,13 @@
         <v>25</v>
       </c>
       <c r="C3" s="5">
-        <v>-0.001</v>
+        <v>-0.002</v>
       </c>
       <c r="D3" s="5">
         <v>0.006</v>
       </c>
       <c r="E3" s="5">
-        <v>-0.011</v>
+        <v>-0.008999999999999999</v>
       </c>
       <c r="F3" s="5">
         <v>0.003</v>
@@ -758,30 +726,7 @@
         <v>100</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8">
-      <c r="B4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="5">
-        <v>-0.001</v>
-      </c>
-      <c r="D4" s="5">
-        <v>0.008</v>
-      </c>
-      <c r="E4" s="5">
-        <v>-0.008999999999999999</v>
-      </c>
-      <c r="F4" s="5">
-        <v>0.003</v>
-      </c>
-      <c r="G4" s="5">
-        <v>100</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>